<commit_message>
Updated on 06.10.23 13:47
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 05.10.2023</t>
+          <t>Date - 06.10.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 04.10.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 05.10.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 05.10.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 05.10.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 05.10.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 05.10.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 05.10.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 05.10.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 05.10.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 05.10.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 05.10.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 05.10.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 05.10.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 05.10.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 05.10.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 05.10.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 06.10.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 06.10.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 06.10.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 06.10.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 06.10.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 06.10.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 06.10.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 06.10.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 06.10.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 06.10.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 06.10.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 06.10.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 06.10.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 06.10.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1122,29 +1122,29 @@
         <is>
           <t>DLV.R31KT6.WI.C.ZIP : last exported on 04.10.23
 DLV.KZ6KT6.WI.V.ZIP : last exported on 04.10.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 04.10.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 03.10.23
-DIT.E35KT6.WI.ZIP : last exported on 04.10.23
-DEL.K2PKT6.WI.ZIP : last exported on 04.10.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 05.10.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 05.10.23
+DIT.E35KT6.WI.ZIP : last exported on 05.10.23
+DEL.K2PKT6.WI.ZIP : last exported on 05.10.23
 DEL.R7AKT6.WI.ZIP : last exported on 23.09.23
 DEL.N5FKT6.WI.ZIP : last exported on 28.09.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 04.10.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 04.10.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 04.10.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 04.10.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 04.10.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 04.10.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 04.10.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 04.10.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 04.10.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 04.10.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 04.10.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 04.10.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 04.10.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 05.10.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 05.10.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 05.10.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 05.10.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 05.10.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 05.10.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 05.10.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 05.10.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 05.10.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 05.10.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 05.10.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 05.10.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 05.10.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 12.09.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 05.10.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 06.10.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 02.10.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 04.10.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 04.10.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 04.10.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 04.10.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 04.10.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 04.10.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 04.10.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 04.10.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 04.10.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 04.10.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 04.10.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 04.10.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 04.10.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 04.10.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 04.10.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 04.10.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 04.10.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 05.10.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 05.10.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 05.10.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 05.10.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 05.10.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 05.10.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 05.10.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 05.10.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 05.10.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 05.10.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 05.10.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 05.10.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 05.10.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 05.10.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 05.10.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 05.10.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 05.10.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1331,18 +1331,18 @@
       </c>
       <c r="C12" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.MANDANTN.TXT : last exported on 28.09.23</t>
+          <t>DEL.N3LKT6.MANDANTN.TXT : last exported on 05.10.23</t>
         </is>
       </c>
       <c r="D12" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 28.09.23
-DEL.N1LN3L.MC.F.GPL.DMP : last exported on 28.09.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 04.10.23
-DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 28.09.23
-DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 28.09.23
-DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 28.09.23
-DGI.KT6R11.MANDANT.TXT : last exported on 28.09.23</t>
+          <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 05.10.23
+DEL.N1LN3L.MC.F.GPL.DMP : last exported on 05.10.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 05.10.23
+DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 05.10.23
+DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 05.10.23
+DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 05.10.23
+DGI.KT6R11.MANDANT.TXT : last exported on 05.10.23</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 04.10.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 05.10.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 03.10.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 05.10.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1413,7 +1413,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 03.10.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 03.10.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 04.10.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 05.10.23
 DEL.KT6N5M.AU.GGO.ZIP : last exported on 03.10.23
 DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 03.10.23
 DEL.KT6KTZ.AU.GGO.ZIP : last exported on 03.10.23
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 04.10.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 04.10.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 05.10.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 05.10.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 04.10.23
-DHP.KUDKT6.ORGUNITS : last exported on 05.10.23
-DHS.R11KT6.HSB02ALL : last exported on 04.10.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 05.10.23
+DHP.KUDKT6.ORGUNITS : last exported on 06.10.23
+DHS.R11KT6.HSB02ALL : last exported on 05.10.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 04.10.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 04.10.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 04.10.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 04.10.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 04.10.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 04.10.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 04.10.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 04.10.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 04.10.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 04.10.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 05.10.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 05.10.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 05.10.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 05.10.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 05.10.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 05.10.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 05.10.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 05.10.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 05.10.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 05.10.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 04.10.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 05.10.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 04.10.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 04.10.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 04.10.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 04.10.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 04.10.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 04.10.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 04.10.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 04.10.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 04.10.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 04.10.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 04.10.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 04.10.23
-DEL.N1LKT6.MT.??????.G : last exported on 04.10.23
-DEL.N1LKT6.MT.??????.U : last exported on 04.10.23
-DEL.N1LKT6.MT.??????.AS : last exported on 04.10.23
-DVL.N1LN5X.VLM.DSP : last exported on 04.10.23
-DVL.N1LN5X.VLM.WT : last exported on 04.10.23
-DDS.N1LR11.DSP : last exported on 04.10.23
-DDS.N1LR11.WT : last exported on 04.10.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 04.10.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 04.10.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 04.10.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 04.10.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 04.10.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 04.10.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 04.10.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 04.10.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 04.10.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 04.10.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 04.10.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 05.10.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 05.10.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 05.10.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 05.10.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 05.10.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 05.10.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 05.10.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 05.10.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 05.10.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 05.10.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 05.10.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 05.10.23
+DEL.N1LKT6.MT.??????.G : last exported on 05.10.23
+DEL.N1LKT6.MT.??????.U : last exported on 05.10.23
+DEL.N1LKT6.MT.??????.AS : last exported on 05.10.23
+DVL.N1LN5X.VLM.DSP : last exported on 05.10.23
+DVL.N1LN5X.VLM.WT : last exported on 05.10.23
+DDS.N1LR11.DSP : last exported on 05.10.23
+DDS.N1LR11.WT : last exported on 05.10.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 05.10.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 05.10.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 05.10.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 05.10.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 05.10.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 05.10.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 05.10.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 05.10.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 05.10.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 05.10.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 05.10.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,22 +1710,22 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 05.10.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 05.10.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 06.10.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 06.10.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 04.10.23
-DEL.N1LN3L.EM.F.GPL.DMP : last exported on 04.10.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 04.10.23
-DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 04.10.23
-DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 04.10.23
-DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 04.10.23
-DEL.N1LK61.EM.F.CPD.DMP : last exported on 04.10.23
-DEL.N1LN0R.EM.F.CPL.DMP : last exported on 04.10.23
-DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 04.10.23
-DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 04.10.23</t>
+          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 05.10.23
+DEL.N1LN3L.EM.F.GPL.DMP : last exported on 05.10.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 05.10.23
+DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 05.10.23
+DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 05.10.23
+DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 05.10.23
+DEL.N1LK61.EM.F.CPD.DMP : last exported on 05.10.23
+DEL.N1LN0R.EM.F.CPL.DMP : last exported on 05.10.23
+DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 05.10.23
+DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 05.10.23</t>
         </is>
       </c>
       <c r="E21" s="11" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 05.10.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 05.10.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 05.10.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 05.10.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 05.10.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 05.10.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 05.10.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 05.10.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 06.10.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 06.10.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 06.10.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 06.10.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 06.10.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 06.10.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 06.10.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 06.10.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 01.10.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 04.10.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 05.10.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 01.10.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 01.10.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 04.10.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 04.10.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 04.10.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 04.10.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 04.10.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 04.10.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 04.10.23
-DEL.N1LKT6.EC.??????.G : last exported on 04.10.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 04.10.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 04.10.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 04.10.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 04.10.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 04.10.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 04.10.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 04.10.23
-DEL.N1LKT6.EC.??????.U : last exported on 04.10.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 04.10.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 04.10.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 04.10.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 04.10.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 04.10.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 04.10.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 04.10.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 04.10.23
-DEL.N1LKT6.EC.??????.AS : last exported on 04.10.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 04.10.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 04.10.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 04.10.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 04.10.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 04.10.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 04.10.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 04.10.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 04.10.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 05.10.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 05.10.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 05.10.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 05.10.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 05.10.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 05.10.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 05.10.23
+DEL.N1LKT6.EC.??????.G : last exported on 05.10.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 05.10.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 05.10.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 05.10.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 05.10.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 05.10.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 05.10.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 05.10.23
+DEL.N1LKT6.EC.??????.U : last exported on 05.10.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 05.10.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 05.10.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 05.10.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 05.10.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 05.10.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 05.10.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 05.10.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 05.10.23
+DEL.N1LKT6.EC.??????.AS : last exported on 05.10.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 05.10.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 05.10.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 05.10.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 05.10.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 05.10.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 05.10.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 05.10.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 05.10.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 09.10.23 15:18
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 06.10.2023</t>
+          <t>Date - 09.10.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 05.10.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 06.10.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 06.10.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 06.10.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 06.10.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 06.10.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 06.10.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 06.10.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 06.10.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 06.10.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 06.10.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 06.10.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 06.10.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 06.10.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 06.10.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 06.10.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 07.10.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 07.10.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 08.10.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 07.10.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 07.10.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 07.10.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 07.10.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 07.10.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 07.10.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 07.10.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 07.10.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 07.10.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 07.10.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 07.10.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1043,13 +1043,13 @@
       </c>
       <c r="C5" s="10" t="inlineStr">
         <is>
-          <t>DGQ.R11KT6.KDNR.TXT : last exported on 04.09.23</t>
+          <t>DGQ.R11KT6.KDNR.TXT : last exported on 06.10.23</t>
         </is>
       </c>
       <c r="D5" s="10" t="inlineStr">
         <is>
-          <t>DDS.N1LR11.KDNRTXT : last exported on 19.09.23
-DVL.N1LN5X.VLM.KDNRTXT : last exported on 19.09.23</t>
+          <t>DDS.N1LR11.KDNRTXT : last exported on 09.10.23
+DVL.N1LN5X.VLM.KDNRTXT : last exported on 09.10.23</t>
         </is>
       </c>
       <c r="E5" s="11" t="inlineStr">
@@ -1077,22 +1077,22 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 02.10.23
-DEH.N3LKT6.AP.COMPL.SNK : last exported on 02.10.23</t>
+          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 09.10.23
+DEH.N3LKT6.AP.COMPL.SNK : last exported on 09.10.23</t>
         </is>
       </c>
       <c r="D6" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 02.10.23
-DEL.N1LN3L.DN.F.GPL.DMP : last exported on 02.10.23
-DEL.N1LN3L.DN.F.GTR.DMP : last exported on 02.10.23
-DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 02.10.23
-DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 02.10.23
-DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 02.10.23
-DEL.N1LK61.DN.F.CPD.DMP : last exported on 02.10.23
-DEL.N1LN0R.DN.F.CPL.DMP : last exported on 02.10.23
-DEL.KT6E35.SN.F.GGO.ZIP : last exported on 02.10.23
-DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 02.10.23</t>
+          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 09.10.23
+DEL.N1LN3L.DN.F.GPL.DMP : last exported on 09.10.23
+DEL.N1LN3L.DN.F.GTR.DMP : last exported on 09.10.23
+DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 09.10.23
+DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 09.10.23
+DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 09.10.23
+DEL.N1LK61.DN.F.CPD.DMP : last exported on 09.10.23
+DEL.N1LN0R.DN.F.CPL.DMP : last exported on 09.10.23
+DEL.KT6E35.SN.F.GGO.ZIP : last exported on 09.10.23
+DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 09.10.23</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
@@ -1121,30 +1121,30 @@
       <c r="C7" s="10" t="inlineStr">
         <is>
           <t>DLV.R31KT6.WI.C.ZIP : last exported on 04.10.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 04.10.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 05.10.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 05.10.23
-DIT.E35KT6.WI.ZIP : last exported on 05.10.23
-DEL.K2PKT6.WI.ZIP : last exported on 05.10.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 07.10.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 06.10.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 08.10.23
+DIT.E35KT6.WI.ZIP : last exported on 06.10.23
+DEL.K2PKT6.WI.ZIP : last exported on 07.10.23
 DEL.R7AKT6.WI.ZIP : last exported on 23.09.23
 DEL.N5FKT6.WI.ZIP : last exported on 28.09.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 05.10.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 05.10.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 05.10.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 05.10.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 05.10.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 05.10.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 05.10.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 05.10.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 05.10.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 05.10.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 05.10.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 05.10.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 05.10.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 09.10.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 09.10.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 09.10.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 09.10.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 09.10.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 09.10.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 09.10.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 09.10.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 09.10.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 09.10.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 09.10.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 09.10.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 09.10.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 12.09.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 06.10.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 09.10.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 02.10.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 05.10.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 05.10.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 05.10.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 05.10.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 05.10.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 05.10.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 05.10.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 05.10.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 05.10.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 05.10.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 05.10.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 05.10.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 05.10.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 05.10.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 05.10.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 05.10.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 05.10.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 08.10.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 08.10.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 08.10.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 08.10.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 08.10.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 08.10.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 08.10.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 08.10.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 08.10.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 08.10.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 08.10.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 08.10.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 08.10.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 08.10.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 08.10.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 08.10.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 08.10.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1338,7 +1338,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 05.10.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 05.10.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 08.10.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 05.10.23
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 05.10.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 06.10.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 05.10.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 07.10.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1406,20 +1406,20 @@
           <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 07.08.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
 DLV.I5XKT6.AU.A.ZIP : last exported on 05.07.23
-DLV.R31KT6.AU.C.ZIP : last exported on 03.10.23</t>
+DLV.R31KT6.AU.C.ZIP : last exported on 06.10.23</t>
         </is>
       </c>
       <c r="D14" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 03.10.23
-DEL.N1LN3L.AU.D.GPL.DMP : last exported on 03.10.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 05.10.23
-DEL.KT6N5M.AU.GGO.ZIP : last exported on 03.10.23
-DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 03.10.23
-DEL.KT6KTZ.AU.GGO.ZIP : last exported on 03.10.23
-DEL.KT6KTZ.AU.IMG.GGO.ZIP : last exported on 03.10.23
-DEL.KT6E35.AU.GGO.ZIP : last exported on 03.10.23
-DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 03.10.23</t>
+          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 06.10.23
+DEL.N1LN3L.AU.D.GPL.DMP : last exported on 06.10.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 08.10.23
+DEL.KT6N5M.AU.GGO.ZIP : last exported on 06.10.23
+DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 06.10.23
+DEL.KT6KTZ.AU.GGO.ZIP : last exported on 06.10.23
+DEL.KT6KTZ.AU.IMG.GGO.ZIP : last exported on 06.10.23
+DEL.KT6E35.AU.GGO.ZIP : last exported on 06.10.23
+DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 06.10.23</t>
         </is>
       </c>
       <c r="E14" s="11" t="inlineStr">
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 05.10.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 05.10.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 08.10.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 08.10.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 05.10.23
-DHP.KUDKT6.ORGUNITS : last exported on 06.10.23
-DHS.R11KT6.HSB02ALL : last exported on 05.10.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 08.10.23
+DHP.KUDKT6.ORGUNITS : last exported on 09.10.23
+DHS.R11KT6.HSB02ALL : last exported on 06.10.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 05.10.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 05.10.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 05.10.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 05.10.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 05.10.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 05.10.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 05.10.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 05.10.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 05.10.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 05.10.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 06.10.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 06.10.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 08.10.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 06.10.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 06.10.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 06.10.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 06.10.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 06.10.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 06.10.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 06.10.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1620,7 +1620,7 @@
       </c>
       <c r="D19" s="16" t="inlineStr">
         <is>
-          <t>DEL.N1LE35.TRANS.ZIP : last exported on 01.10.23</t>
+          <t>DEL.N1LE35.TRANS.ZIP : last exported on 08.10.23</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 05.10.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 07.10.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 05.10.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 05.10.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 05.10.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 05.10.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 05.10.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 05.10.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 05.10.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 05.10.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 05.10.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 05.10.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 05.10.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 05.10.23
-DEL.N1LKT6.MT.??????.G : last exported on 05.10.23
-DEL.N1LKT6.MT.??????.U : last exported on 05.10.23
-DEL.N1LKT6.MT.??????.AS : last exported on 05.10.23
-DVL.N1LN5X.VLM.DSP : last exported on 05.10.23
-DVL.N1LN5X.VLM.WT : last exported on 05.10.23
-DDS.N1LR11.DSP : last exported on 05.10.23
-DDS.N1LR11.WT : last exported on 05.10.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 05.10.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 05.10.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 05.10.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 05.10.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 05.10.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 05.10.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 05.10.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 05.10.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 05.10.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 05.10.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 05.10.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 07.10.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 07.10.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 08.10.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 07.10.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 07.10.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 07.10.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 07.10.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 07.10.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 07.10.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 07.10.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 07.10.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 07.10.23
+DEL.N1LKT6.MT.??????.G : last exported on 07.10.23
+DEL.N1LKT6.MT.??????.U : last exported on 07.10.23
+DEL.N1LKT6.MT.??????.AS : last exported on 07.10.23
+DVL.N1LN5X.VLM.DSP : last exported on 07.10.23
+DVL.N1LN5X.VLM.WT : last exported on 07.10.23
+DDS.N1LR11.DSP : last exported on 07.10.23
+DDS.N1LR11.WT : last exported on 07.10.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 07.10.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 07.10.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 07.10.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 07.10.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 07.10.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 07.10.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 07.10.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 07.10.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 07.10.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 07.10.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 07.10.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,22 +1710,22 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 06.10.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 06.10.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 09.10.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 09.10.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 05.10.23
-DEL.N1LN3L.EM.F.GPL.DMP : last exported on 05.10.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 05.10.23
-DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 05.10.23
-DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 05.10.23
-DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 05.10.23
-DEL.N1LK61.EM.F.CPD.DMP : last exported on 05.10.23
-DEL.N1LN0R.EM.F.CPL.DMP : last exported on 05.10.23
-DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 05.10.23
-DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 05.10.23</t>
+          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 08.10.23
+DEL.N1LN3L.EM.F.GPL.DMP : last exported on 08.10.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 08.10.23
+DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 08.10.23
+DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 08.10.23
+DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 08.10.23
+DEL.N1LK61.EM.F.CPD.DMP : last exported on 08.10.23
+DEL.N1LN0R.EM.F.CPL.DMP : last exported on 08.10.23
+DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 08.10.23
+DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 08.10.23</t>
         </is>
       </c>
       <c r="E21" s="11" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 06.10.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 06.10.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 06.10.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 06.10.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 06.10.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 06.10.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 06.10.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 06.10.23
-DDC.R11KT6.ELFI.MD.TXT : last exported on 01.10.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 05.10.23
-DDC.R11KT6.ELFI.PK.TXT : last exported on 01.10.23
-DDC.R11KT6.ELFI.PR.TXT : last exported on 01.10.23</t>
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 09.10.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 09.10.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 09.10.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 09.10.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 09.10.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 09.10.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 09.10.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 09.10.23
+DDC.R11KT6.ELFI.MD.TXT : last exported on 08.10.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 06.10.23
+DDC.R11KT6.ELFI.PK.TXT : last exported on 08.10.23
+DDC.R11KT6.ELFI.PR.TXT : last exported on 08.10.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 05.10.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 05.10.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 05.10.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 05.10.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 05.10.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 05.10.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 05.10.23
-DEL.N1LKT6.EC.??????.G : last exported on 05.10.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 05.10.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 05.10.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 05.10.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 05.10.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 05.10.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 05.10.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 05.10.23
-DEL.N1LKT6.EC.??????.U : last exported on 05.10.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 05.10.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 05.10.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 05.10.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 05.10.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 05.10.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 05.10.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 05.10.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 05.10.23
-DEL.N1LKT6.EC.??????.AS : last exported on 05.10.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 05.10.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 05.10.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 05.10.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 05.10.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 05.10.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 05.10.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 05.10.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 05.10.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 08.10.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 08.10.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 08.10.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 08.10.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 08.10.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 08.10.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 08.10.23
+DEL.N1LKT6.EC.??????.G : last exported on 08.10.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 08.10.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 08.10.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 08.10.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 08.10.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 08.10.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 08.10.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 08.10.23
+DEL.N1LKT6.EC.??????.U : last exported on 08.10.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 08.10.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 08.10.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 08.10.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 08.10.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 08.10.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 08.10.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 08.10.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 08.10.23
+DEL.N1LKT6.EC.??????.AS : last exported on 08.10.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 08.10.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 08.10.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 08.10.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 08.10.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 08.10.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 08.10.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 08.10.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 08.10.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 10.10.23 11:56
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 09.10.2023</t>
+          <t>Date - 10.10.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 06.10.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 09.10.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 07.10.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 07.10.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 08.10.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 07.10.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 07.10.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 07.10.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 07.10.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 07.10.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 07.10.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 07.10.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 07.10.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 07.10.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 07.10.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 07.10.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 10.10.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 10.10.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 10.10.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 10.10.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 10.10.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 10.10.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 10.10.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 10.10.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 10.10.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 10.10.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 10.10.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 10.10.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 10.10.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 10.10.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1121,11 +1121,11 @@
       <c r="C7" s="10" t="inlineStr">
         <is>
           <t>DLV.R31KT6.WI.C.ZIP : last exported on 04.10.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 07.10.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 06.10.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 08.10.23
-DIT.E35KT6.WI.ZIP : last exported on 06.10.23
-DEL.K2PKT6.WI.ZIP : last exported on 07.10.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 09.10.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 09.10.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 09.10.23
+DIT.E35KT6.WI.ZIP : last exported on 09.10.23
+DEL.K2PKT6.WI.ZIP : last exported on 09.10.23
 DEL.R7AKT6.WI.ZIP : last exported on 23.09.23
 DEL.N5FKT6.WI.ZIP : last exported on 28.09.23</t>
         </is>
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 12.09.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 09.10.23
-DGV.N3LKT6.EPELS.??????.ZIP : last exported on 02.10.23</t>
+DEL.N3LKT6.HST.??????.ZIP : last exported on 10.10.23
+DGV.N3LKT6.EPELS.??????.ZIP : last exported on 09.10.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 08.10.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 08.10.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 08.10.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 08.10.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 08.10.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 08.10.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 08.10.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 08.10.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 08.10.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 08.10.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 08.10.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 08.10.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 08.10.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 08.10.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 08.10.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 08.10.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 08.10.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 09.10.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 09.10.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 09.10.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 09.10.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 09.10.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 09.10.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 09.10.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 09.10.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 09.10.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 09.10.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 09.10.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 09.10.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 09.10.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 09.10.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 09.10.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 09.10.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 09.10.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1298,12 +1298,12 @@
       </c>
       <c r="C11" s="14" t="inlineStr">
         <is>
-          <t>DEL.KT6KT6.APOSPRO.ZIP : last exported on 02.10.23</t>
+          <t>DEL.KT6KT6.APOSPRO.ZIP : last exported on 09.10.23</t>
         </is>
       </c>
       <c r="D11" s="15" t="inlineStr">
         <is>
-          <t>DEL.KT6N2O.XTIME.ZIP : last exported on 02.10.23</t>
+          <t>DEL.KT6N2O.XTIME.ZIP : last exported on 09.10.23</t>
         </is>
       </c>
       <c r="E11" s="11" t="inlineStr">
@@ -1338,7 +1338,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 05.10.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 08.10.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 09.10.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 05.10.23
@@ -1370,7 +1370,7 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 06.10.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 09.10.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
@@ -1406,20 +1406,20 @@
           <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 07.08.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
 DLV.I5XKT6.AU.A.ZIP : last exported on 05.07.23
-DLV.R31KT6.AU.C.ZIP : last exported on 06.10.23</t>
+DLV.R31KT6.AU.C.ZIP : last exported on 09.10.23</t>
         </is>
       </c>
       <c r="D14" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 06.10.23
-DEL.N1LN3L.AU.D.GPL.DMP : last exported on 06.10.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 08.10.23
-DEL.KT6N5M.AU.GGO.ZIP : last exported on 06.10.23
-DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 06.10.23
-DEL.KT6KTZ.AU.GGO.ZIP : last exported on 06.10.23
-DEL.KT6KTZ.AU.IMG.GGO.ZIP : last exported on 06.10.23
-DEL.KT6E35.AU.GGO.ZIP : last exported on 06.10.23
-DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 06.10.23</t>
+          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 09.10.23
+DEL.N1LN3L.AU.D.GPL.DMP : last exported on 09.10.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 09.10.23
+DEL.KT6N5M.AU.GGO.ZIP : last exported on 09.10.23
+DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 09.10.23
+DEL.KT6KTZ.AU.GGO.ZIP : last exported on 09.10.23
+DEL.KT6KTZ.AU.IMG.GGO.ZIP : last exported on 09.10.23
+DEL.KT6E35.AU.GGO.ZIP : last exported on 09.10.23
+DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 09.10.23</t>
         </is>
       </c>
       <c r="E14" s="11" t="inlineStr">
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 08.10.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 08.10.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 09.10.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 09.10.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 08.10.23
-DHP.KUDKT6.ORGUNITS : last exported on 09.10.23
-DHS.R11KT6.HSB02ALL : last exported on 06.10.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 09.10.23
+DHP.KUDKT6.ORGUNITS : last exported on 10.10.23
+DHS.R11KT6.HSB02ALL : last exported on 09.10.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 06.10.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 06.10.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 08.10.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 06.10.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 06.10.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 06.10.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 06.10.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 06.10.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 06.10.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 06.10.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 09.10.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 09.10.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 09.10.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 09.10.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 09.10.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 09.10.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 09.10.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 09.10.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 09.10.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 09.10.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 07.10.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 09.10.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 07.10.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 07.10.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 08.10.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 07.10.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 07.10.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 07.10.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 07.10.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 07.10.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 07.10.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 07.10.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 07.10.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 07.10.23
-DEL.N1LKT6.MT.??????.G : last exported on 07.10.23
-DEL.N1LKT6.MT.??????.U : last exported on 07.10.23
-DEL.N1LKT6.MT.??????.AS : last exported on 07.10.23
-DVL.N1LN5X.VLM.DSP : last exported on 07.10.23
-DVL.N1LN5X.VLM.WT : last exported on 07.10.23
-DDS.N1LR11.DSP : last exported on 07.10.23
-DDS.N1LR11.WT : last exported on 07.10.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 07.10.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 07.10.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 07.10.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 07.10.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 07.10.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 07.10.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 07.10.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 07.10.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 07.10.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 07.10.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 07.10.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 09.10.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 09.10.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 09.10.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 09.10.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 09.10.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 09.10.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 09.10.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 09.10.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 09.10.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 09.10.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 09.10.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 09.10.23
+DEL.N1LKT6.MT.??????.G : last exported on 09.10.23
+DEL.N1LKT6.MT.??????.U : last exported on 09.10.23
+DEL.N1LKT6.MT.??????.AS : last exported on 09.10.23
+DVL.N1LN5X.VLM.DSP : last exported on 09.10.23
+DVL.N1LN5X.VLM.WT : last exported on 09.10.23
+DDS.N1LR11.DSP : last exported on 09.10.23
+DDS.N1LR11.WT : last exported on 09.10.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 09.10.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 09.10.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 09.10.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 09.10.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 09.10.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 09.10.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 09.10.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 09.10.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 09.10.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 09.10.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 09.10.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,22 +1710,22 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 09.10.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 09.10.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 10.10.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 10.10.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 08.10.23
-DEL.N1LN3L.EM.F.GPL.DMP : last exported on 08.10.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 08.10.23
-DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 08.10.23
-DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 08.10.23
-DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 08.10.23
-DEL.N1LK61.EM.F.CPD.DMP : last exported on 08.10.23
-DEL.N1LN0R.EM.F.CPL.DMP : last exported on 08.10.23
-DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 08.10.23
-DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 08.10.23</t>
+          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 09.10.23
+DEL.N1LN3L.EM.F.GPL.DMP : last exported on 09.10.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 09.10.23
+DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 09.10.23
+DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 09.10.23
+DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 09.10.23
+DEL.N1LK61.EM.F.CPD.DMP : last exported on 09.10.23
+DEL.N1LN0R.EM.F.CPL.DMP : last exported on 09.10.23
+DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 09.10.23
+DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 09.10.23</t>
         </is>
       </c>
       <c r="E21" s="11" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 09.10.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 09.10.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 09.10.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 09.10.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 09.10.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 09.10.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 09.10.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 09.10.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 10.10.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 10.10.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 10.10.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 10.10.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 10.10.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 10.10.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 10.10.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 10.10.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 08.10.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 06.10.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 09.10.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 08.10.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 08.10.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 08.10.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 08.10.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 08.10.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 08.10.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 08.10.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 08.10.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 08.10.23
-DEL.N1LKT6.EC.??????.G : last exported on 08.10.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 08.10.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 08.10.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 08.10.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 08.10.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 08.10.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 08.10.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 08.10.23
-DEL.N1LKT6.EC.??????.U : last exported on 08.10.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 08.10.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 08.10.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 08.10.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 08.10.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 08.10.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 08.10.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 08.10.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 08.10.23
-DEL.N1LKT6.EC.??????.AS : last exported on 08.10.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 08.10.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 08.10.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 08.10.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 08.10.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 08.10.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 08.10.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 08.10.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 08.10.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 09.10.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 09.10.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 09.10.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 09.10.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 09.10.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 09.10.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 09.10.23
+DEL.N1LKT6.EC.??????.G : last exported on 09.10.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 09.10.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 09.10.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 09.10.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 09.10.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 09.10.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 09.10.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 09.10.23
+DEL.N1LKT6.EC.??????.U : last exported on 09.10.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 09.10.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 09.10.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 09.10.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 09.10.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 09.10.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 09.10.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 09.10.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 09.10.23
+DEL.N1LKT6.EC.??????.AS : last exported on 09.10.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 09.10.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 09.10.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 09.10.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 09.10.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 09.10.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 09.10.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 09.10.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 09.10.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 11.10.23 12:37
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 10.10.2023</t>
+          <t>Date - 11.10.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 09.10.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 10.10.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 10.10.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 10.10.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 10.10.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 10.10.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 10.10.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 10.10.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 10.10.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 10.10.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 10.10.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 10.10.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 10.10.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 10.10.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 10.10.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 10.10.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 11.10.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 11.10.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 11.10.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 11.10.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 11.10.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 11.10.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 11.10.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 11.10.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 11.10.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 11.10.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 11.10.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 11.10.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 11.10.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 11.10.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1121,30 +1121,30 @@
       <c r="C7" s="10" t="inlineStr">
         <is>
           <t>DLV.R31KT6.WI.C.ZIP : last exported on 04.10.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 09.10.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 09.10.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 09.10.23
-DIT.E35KT6.WI.ZIP : last exported on 09.10.23
-DEL.K2PKT6.WI.ZIP : last exported on 09.10.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 10.10.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 10.10.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 10.10.23
+DIT.E35KT6.WI.ZIP : last exported on 10.10.23
+DEL.K2PKT6.WI.ZIP : last exported on 10.10.23
 DEL.R7AKT6.WI.ZIP : last exported on 23.09.23
 DEL.N5FKT6.WI.ZIP : last exported on 28.09.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 09.10.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 09.10.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 09.10.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 09.10.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 09.10.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 09.10.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 09.10.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 09.10.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 09.10.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 09.10.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 09.10.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 09.10.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 09.10.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 10.10.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 10.10.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 10.10.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 10.10.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 10.10.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 10.10.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 10.10.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 10.10.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 10.10.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 10.10.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 10.10.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 10.10.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 10.10.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 12.09.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 10.10.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 11.10.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 09.10.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 09.10.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 09.10.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 09.10.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 09.10.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 09.10.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 09.10.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 09.10.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 09.10.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 09.10.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 09.10.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 09.10.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 09.10.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 09.10.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 09.10.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 09.10.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 09.10.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 09.10.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 10.10.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 10.10.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 10.10.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 10.10.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 10.10.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 10.10.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 10.10.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 10.10.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 10.10.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 10.10.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 10.10.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 10.10.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 10.10.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 10.10.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 10.10.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 10.10.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 10.10.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1338,7 +1338,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 05.10.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 09.10.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 10.10.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 05.10.23
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 09.10.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 10.10.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 07.10.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 10.10.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1413,7 +1413,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 09.10.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 09.10.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 09.10.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 10.10.23
 DEL.KT6N5M.AU.GGO.ZIP : last exported on 09.10.23
 DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 09.10.23
 DEL.KT6KTZ.AU.GGO.ZIP : last exported on 09.10.23
@@ -1455,8 +1455,8 @@
 DGQ.R11KT6.PKAT.US2.TXT : last exported on 04.10.23
 DGQ.R11KT6.BSITK.TXT : last exported on 04.10.23
 DGQ.R11KT6.BSITX.TXT : last exported on 04.10.23
-DGQ.R31KT6.BSIVMC.TXT : last exported on 12.09.23
-DGQ.R31KT6.PKATC.TXT : last exported on 12.09.23
+DGQ.R31KT6.BSIVMC.TXT : last exported on 10.10.23
+DGQ.R31KT6.PKATC.TXT : last exported on 10.10.23
 DEL.KMPKT6.APOS.DATA.ZIP : last exported on 04.10.23</t>
         </is>
       </c>
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 09.10.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 09.10.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 10.10.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 10.10.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 09.10.23
-DHP.KUDKT6.ORGUNITS : last exported on 10.10.23
-DHS.R11KT6.HSB02ALL : last exported on 09.10.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 10.10.23
+DHP.KUDKT6.ORGUNITS : last exported on 11.10.23
+DHS.R11KT6.HSB02ALL : last exported on 10.10.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 09.10.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 09.10.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 09.10.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 09.10.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 09.10.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 09.10.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 09.10.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 09.10.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 09.10.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 09.10.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 10.10.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 10.10.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 10.10.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 10.10.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 10.10.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 10.10.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 10.10.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 10.10.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 10.10.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 10.10.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 09.10.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 10.10.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 09.10.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 09.10.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 09.10.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 09.10.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 09.10.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 09.10.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 09.10.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 09.10.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 09.10.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 09.10.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 09.10.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 09.10.23
-DEL.N1LKT6.MT.??????.G : last exported on 09.10.23
-DEL.N1LKT6.MT.??????.U : last exported on 09.10.23
-DEL.N1LKT6.MT.??????.AS : last exported on 09.10.23
-DVL.N1LN5X.VLM.DSP : last exported on 09.10.23
-DVL.N1LN5X.VLM.WT : last exported on 09.10.23
-DDS.N1LR11.DSP : last exported on 09.10.23
-DDS.N1LR11.WT : last exported on 09.10.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 09.10.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 09.10.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 09.10.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 09.10.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 09.10.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 09.10.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 09.10.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 09.10.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 09.10.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 09.10.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 09.10.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 10.10.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 10.10.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 10.10.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 10.10.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 10.10.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 10.10.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 10.10.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 10.10.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 10.10.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 10.10.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 10.10.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 10.10.23
+DEL.N1LKT6.MT.??????.G : last exported on 10.10.23
+DEL.N1LKT6.MT.??????.U : last exported on 10.10.23
+DEL.N1LKT6.MT.??????.AS : last exported on 10.10.23
+DVL.N1LN5X.VLM.DSP : last exported on 10.10.23
+DVL.N1LN5X.VLM.WT : last exported on 10.10.23
+DDS.N1LR11.DSP : last exported on 10.10.23
+DDS.N1LR11.WT : last exported on 10.10.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 10.10.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 10.10.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 10.10.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 10.10.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 10.10.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 10.10.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 10.10.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 10.10.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 10.10.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 10.10.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 10.10.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,22 +1710,22 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 10.10.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 10.10.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 11.10.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 11.10.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 09.10.23
-DEL.N1LN3L.EM.F.GPL.DMP : last exported on 09.10.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 09.10.23
-DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 09.10.23
-DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 09.10.23
-DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 09.10.23
-DEL.N1LK61.EM.F.CPD.DMP : last exported on 09.10.23
-DEL.N1LN0R.EM.F.CPL.DMP : last exported on 09.10.23
-DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 09.10.23
-DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 09.10.23</t>
+          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 10.10.23
+DEL.N1LN3L.EM.F.GPL.DMP : last exported on 10.10.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 10.10.23
+DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 10.10.23
+DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 10.10.23
+DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 10.10.23
+DEL.N1LK61.EM.F.CPD.DMP : last exported on 10.10.23
+DEL.N1LN0R.EM.F.CPL.DMP : last exported on 10.10.23
+DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 10.10.23
+DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 10.10.23</t>
         </is>
       </c>
       <c r="E21" s="11" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 10.10.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 10.10.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 10.10.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 10.10.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 10.10.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 10.10.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 10.10.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 10.10.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 11.10.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 11.10.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 11.10.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 11.10.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 11.10.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 11.10.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 11.10.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 11.10.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 08.10.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 09.10.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 10.10.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 08.10.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 08.10.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 09.10.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 09.10.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 09.10.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 09.10.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 09.10.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 09.10.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 09.10.23
-DEL.N1LKT6.EC.??????.G : last exported on 09.10.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 09.10.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 09.10.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 09.10.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 09.10.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 09.10.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 09.10.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 09.10.23
-DEL.N1LKT6.EC.??????.U : last exported on 09.10.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 09.10.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 09.10.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 09.10.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 09.10.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 09.10.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 09.10.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 09.10.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 09.10.23
-DEL.N1LKT6.EC.??????.AS : last exported on 09.10.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 09.10.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 09.10.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 09.10.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 09.10.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 09.10.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 09.10.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 09.10.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 09.10.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 10.10.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 10.10.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 10.10.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 10.10.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 10.10.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 10.10.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 10.10.23
+DEL.N1LKT6.EC.??????.G : last exported on 10.10.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 10.10.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 10.10.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 10.10.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 10.10.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 10.10.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 10.10.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 10.10.23
+DEL.N1LKT6.EC.??????.U : last exported on 10.10.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 10.10.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 10.10.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 10.10.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 10.10.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 10.10.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 10.10.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 10.10.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 10.10.23
+DEL.N1LKT6.EC.??????.AS : last exported on 10.10.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 10.10.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 10.10.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 10.10.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 10.10.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 10.10.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 10.10.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 10.10.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 10.10.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 12.10.23 12:14
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 10.10.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 11.10.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 11.10.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 11.10.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 11.10.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 11.10.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 11.10.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 11.10.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 11.10.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 11.10.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 11.10.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 11.10.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 11.10.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 11.10.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 11.10.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 11.10.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 12.10.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 12.10.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 12.10.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 12.10.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 12.10.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 12.10.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 12.10.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 12.10.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 12.10.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 12.10.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 12.10.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 12.10.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 12.10.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 12.10.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1120,31 +1120,31 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 04.10.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 10.10.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 10.10.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 10.10.23
-DIT.E35KT6.WI.ZIP : last exported on 10.10.23
-DEL.K2PKT6.WI.ZIP : last exported on 10.10.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 11.10.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 11.10.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 11.10.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 11.10.23
+DIT.E35KT6.WI.ZIP : last exported on 11.10.23
+DEL.K2PKT6.WI.ZIP : last exported on 11.10.23
 DEL.R7AKT6.WI.ZIP : last exported on 23.09.23
 DEL.N5FKT6.WI.ZIP : last exported on 28.09.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 10.10.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 10.10.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 10.10.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 10.10.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 10.10.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 10.10.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 10.10.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 10.10.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 10.10.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 10.10.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 10.10.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 10.10.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 10.10.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 11.10.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 11.10.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 11.10.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 11.10.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 11.10.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 11.10.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 11.10.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 11.10.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 11.10.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 11.10.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 11.10.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 11.10.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 11.10.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 12.09.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 11.10.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 12.10.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 09.10.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 10.10.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 10.10.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 10.10.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 10.10.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 10.10.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 10.10.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 10.10.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 10.10.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 10.10.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 10.10.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 10.10.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 10.10.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 10.10.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 10.10.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 10.10.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 10.10.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 10.10.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 11.10.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 11.10.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 11.10.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 11.10.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 11.10.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 11.10.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 11.10.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 11.10.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 11.10.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 11.10.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 11.10.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 11.10.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 11.10.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 11.10.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 11.10.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 11.10.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 11.10.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1338,7 +1338,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 05.10.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 10.10.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 11.10.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 05.10.23
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 10.10.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 11.10.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 10.10.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 11.10.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1406,20 +1406,20 @@
           <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 07.08.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
 DLV.I5XKT6.AU.A.ZIP : last exported on 05.07.23
-DLV.R31KT6.AU.C.ZIP : last exported on 09.10.23</t>
+DLV.R31KT6.AU.C.ZIP : last exported on 11.10.23</t>
         </is>
       </c>
       <c r="D14" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 09.10.23
-DEL.N1LN3L.AU.D.GPL.DMP : last exported on 09.10.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 10.10.23
-DEL.KT6N5M.AU.GGO.ZIP : last exported on 09.10.23
-DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 09.10.23
-DEL.KT6KTZ.AU.GGO.ZIP : last exported on 09.10.23
-DEL.KT6KTZ.AU.IMG.GGO.ZIP : last exported on 09.10.23
-DEL.KT6E35.AU.GGO.ZIP : last exported on 09.10.23
-DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 09.10.23</t>
+          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 11.10.23
+DEL.N1LN3L.AU.D.GPL.DMP : last exported on 11.10.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 11.10.23
+DEL.KT6N5M.AU.GGO.ZIP : last exported on 11.10.23
+DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 11.10.23
+DEL.KT6KTZ.AU.GGO.ZIP : last exported on 11.10.23
+DEL.KT6KTZ.AU.IMG.GGO.ZIP : last exported on 11.10.23
+DEL.KT6E35.AU.GGO.ZIP : last exported on 11.10.23
+DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 11.10.23</t>
         </is>
       </c>
       <c r="E14" s="11" t="inlineStr">
@@ -1457,24 +1457,24 @@
 DGQ.R11KT6.BSITX.TXT : last exported on 04.10.23
 DGQ.R31KT6.BSIVMC.TXT : last exported on 10.10.23
 DGQ.R31KT6.PKATC.TXT : last exported on 10.10.23
-DEL.KMPKT6.APOS.DATA.ZIP : last exported on 04.10.23</t>
+DEL.KMPKT6.APOS.DATA.ZIP : last exported on 11.10.23</t>
         </is>
       </c>
       <c r="D15" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 04.10.23
-DEL.N1LN3L.AP.F.GPL.DMP : last exported on 04.10.23
-DEL.N1LN3L.AP.F.GTR.DMP : last exported on 04.10.23
-DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 04.10.23
-DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 04.10.23
-DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 04.10.23
-DEL.N1LK61.AP.F.CPD.DMP : last exported on 04.10.23
-DEL.N1LN0R.AP.F.CPL.DMP : last exported on 04.10.23
-DEL.N1LR31.AP.F.PPS.DMP : last exported on 04.10.23
-DEL.KT6E35.AP.F.DB.ZIP : last exported on 04.10.23
-DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 04.10.23
-DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 04.10.23
-DVL.KT6N5X.VLM.AP.ZIP : last exported on 04.10.23</t>
+          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 11.10.23
+DEL.N1LN3L.AP.F.GPL.DMP : last exported on 11.10.23
+DEL.N1LN3L.AP.F.GTR.DMP : last exported on 11.10.23
+DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 11.10.23
+DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 11.10.23
+DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 11.10.23
+DEL.N1LK61.AP.F.CPD.DMP : last exported on 11.10.23
+DEL.N1LN0R.AP.F.CPL.DMP : last exported on 11.10.23
+DEL.N1LR31.AP.F.PPS.DMP : last exported on 11.10.23
+DEL.KT6E35.AP.F.DB.ZIP : last exported on 11.10.23
+DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 11.10.23
+DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 11.10.23
+DVL.KT6N5X.VLM.AP.ZIP : last exported on 11.10.23</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 10.10.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 10.10.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 11.10.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 11.10.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 10.10.23
-DHP.KUDKT6.ORGUNITS : last exported on 11.10.23
-DHS.R11KT6.HSB02ALL : last exported on 10.10.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 11.10.23
+DHP.KUDKT6.ORGUNITS : last exported on 12.10.23
+DHS.R11KT6.HSB02ALL : last exported on 11.10.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 10.10.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 10.10.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 10.10.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 10.10.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 10.10.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 10.10.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 10.10.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 10.10.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 10.10.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 10.10.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 11.10.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 11.10.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 11.10.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 11.10.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 11.10.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 11.10.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 11.10.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 11.10.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 11.10.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 11.10.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 10.10.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 11.10.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 10.10.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 10.10.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 10.10.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 10.10.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 10.10.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 10.10.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 10.10.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 10.10.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 10.10.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 10.10.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 10.10.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 10.10.23
-DEL.N1LKT6.MT.??????.G : last exported on 10.10.23
-DEL.N1LKT6.MT.??????.U : last exported on 10.10.23
-DEL.N1LKT6.MT.??????.AS : last exported on 10.10.23
-DVL.N1LN5X.VLM.DSP : last exported on 10.10.23
-DVL.N1LN5X.VLM.WT : last exported on 10.10.23
-DDS.N1LR11.DSP : last exported on 10.10.23
-DDS.N1LR11.WT : last exported on 10.10.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 10.10.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 10.10.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 10.10.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 10.10.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 10.10.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 10.10.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 10.10.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 10.10.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 10.10.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 10.10.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 10.10.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 11.10.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 11.10.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 11.10.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 11.10.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 11.10.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 11.10.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 11.10.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 11.10.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 11.10.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 11.10.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 11.10.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 11.10.23
+DEL.N1LKT6.MT.??????.G : last exported on 11.10.23
+DEL.N1LKT6.MT.??????.U : last exported on 11.10.23
+DEL.N1LKT6.MT.??????.AS : last exported on 11.10.23
+DVL.N1LN5X.VLM.DSP : last exported on 11.10.23
+DVL.N1LN5X.VLM.WT : last exported on 11.10.23
+DDS.N1LR11.DSP : last exported on 11.10.23
+DDS.N1LR11.WT : last exported on 11.10.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 11.10.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 11.10.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 11.10.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 11.10.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 11.10.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 11.10.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 11.10.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 11.10.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 11.10.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 11.10.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 11.10.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,22 +1710,22 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 11.10.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 11.10.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 12.10.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 12.10.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 10.10.23
-DEL.N1LN3L.EM.F.GPL.DMP : last exported on 10.10.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 10.10.23
-DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 10.10.23
-DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 10.10.23
-DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 10.10.23
-DEL.N1LK61.EM.F.CPD.DMP : last exported on 10.10.23
-DEL.N1LN0R.EM.F.CPL.DMP : last exported on 10.10.23
-DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 10.10.23
-DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 10.10.23</t>
+          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 11.10.23
+DEL.N1LN3L.EM.F.GPL.DMP : last exported on 11.10.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 11.10.23
+DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 11.10.23
+DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 11.10.23
+DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 11.10.23
+DEL.N1LK61.EM.F.CPD.DMP : last exported on 11.10.23
+DEL.N1LN0R.EM.F.CPL.DMP : last exported on 11.10.23
+DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 11.10.23
+DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 11.10.23</t>
         </is>
       </c>
       <c r="E21" s="11" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 11.10.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 11.10.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 11.10.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 11.10.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 11.10.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 11.10.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 11.10.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 11.10.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 12.10.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 12.10.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 12.10.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 12.10.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 12.10.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 12.10.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 12.10.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 12.10.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 08.10.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 10.10.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 11.10.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 08.10.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 08.10.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 10.10.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 10.10.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 10.10.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 10.10.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 10.10.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 10.10.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 10.10.23
-DEL.N1LKT6.EC.??????.G : last exported on 10.10.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 10.10.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 10.10.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 10.10.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 10.10.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 10.10.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 10.10.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 10.10.23
-DEL.N1LKT6.EC.??????.U : last exported on 10.10.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 10.10.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 10.10.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 10.10.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 10.10.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 10.10.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 10.10.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 10.10.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 10.10.23
-DEL.N1LKT6.EC.??????.AS : last exported on 10.10.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 10.10.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 10.10.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 10.10.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 10.10.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 10.10.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 10.10.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 10.10.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 10.10.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 11.10.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 11.10.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 11.10.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 11.10.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 11.10.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 11.10.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 11.10.23
+DEL.N1LKT6.EC.??????.G : last exported on 11.10.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 11.10.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 11.10.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 11.10.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 11.10.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 11.10.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 11.10.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 11.10.23
+DEL.N1LKT6.EC.??????.U : last exported on 11.10.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 11.10.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 11.10.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 11.10.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 11.10.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 11.10.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 11.10.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 11.10.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 11.10.23
+DEL.N1LKT6.EC.??????.AS : last exported on 11.10.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 11.10.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 11.10.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 11.10.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 11.10.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 11.10.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 11.10.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 11.10.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 11.10.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 13.10.23 12:05
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 12.10.2023</t>
+          <t>Date - 13.10.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 11.10.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 12.10.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 12.10.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 12.10.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 12.10.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 12.10.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 12.10.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 12.10.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 12.10.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 12.10.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 12.10.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 12.10.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 12.10.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 12.10.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 12.10.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 12.10.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 13.10.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 13.10.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 13.10.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 13.10.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 13.10.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 13.10.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 13.10.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 13.10.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 13.10.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 13.10.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 13.10.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 13.10.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 13.10.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 13.10.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1121,30 +1121,30 @@
       <c r="C7" s="10" t="inlineStr">
         <is>
           <t>DLV.R31KT6.WI.C.ZIP : last exported on 11.10.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 11.10.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 12.10.23
 DLV.RPKKT6.WI.S.ZIP : last exported on 11.10.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 11.10.23
-DIT.E35KT6.WI.ZIP : last exported on 11.10.23
-DEL.K2PKT6.WI.ZIP : last exported on 11.10.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 12.10.23
+DIT.E35KT6.WI.ZIP : last exported on 12.10.23
+DEL.K2PKT6.WI.ZIP : last exported on 12.10.23
 DEL.R7AKT6.WI.ZIP : last exported on 23.09.23
-DEL.N5FKT6.WI.ZIP : last exported on 28.09.23</t>
+DEL.N5FKT6.WI.ZIP : last exported on 12.10.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 11.10.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 11.10.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 11.10.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 11.10.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 11.10.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 11.10.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 11.10.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 11.10.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 11.10.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 11.10.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 11.10.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 11.10.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 11.10.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 12.10.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 12.10.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 12.10.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 12.10.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 12.10.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 12.10.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 12.10.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 12.10.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 12.10.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 12.10.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 12.10.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 12.10.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 12.10.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 12.09.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 12.10.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 13.10.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 09.10.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 11.10.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 11.10.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 11.10.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 11.10.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 11.10.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 11.10.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 11.10.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 11.10.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 11.10.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 11.10.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 11.10.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 11.10.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 11.10.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 11.10.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 11.10.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 11.10.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 11.10.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 12.10.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 12.10.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 12.10.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 12.10.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 12.10.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 12.10.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 12.10.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 12.10.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 12.10.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 12.10.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 12.10.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 12.10.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 12.10.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 12.10.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 12.10.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 12.10.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 12.10.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1338,7 +1338,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 05.10.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 11.10.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 12.10.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 05.10.23
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 11.10.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 12.10.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 11.10.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 12.10.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1413,7 +1413,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 11.10.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 11.10.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 11.10.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 12.10.23
 DEL.KT6N5M.AU.GGO.ZIP : last exported on 11.10.23
 DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 11.10.23
 DEL.KT6KTZ.AU.GGO.ZIP : last exported on 11.10.23
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 11.10.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 11.10.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 12.10.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 12.10.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 11.10.23
-DHP.KUDKT6.ORGUNITS : last exported on 12.10.23
-DHS.R11KT6.HSB02ALL : last exported on 11.10.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 12.10.23
+DHP.KUDKT6.ORGUNITS : last exported on 13.10.23
+DHS.R11KT6.HSB02ALL : last exported on 12.10.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 11.10.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 11.10.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 11.10.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 11.10.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 11.10.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 11.10.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 11.10.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 11.10.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 11.10.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 11.10.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 12.10.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 12.10.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 12.10.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 12.10.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 12.10.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 12.10.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 12.10.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 12.10.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 12.10.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 12.10.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 11.10.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 12.10.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 11.10.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 11.10.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 11.10.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 11.10.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 11.10.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 11.10.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 11.10.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 11.10.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 11.10.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 11.10.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 11.10.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 11.10.23
-DEL.N1LKT6.MT.??????.G : last exported on 11.10.23
-DEL.N1LKT6.MT.??????.U : last exported on 11.10.23
-DEL.N1LKT6.MT.??????.AS : last exported on 11.10.23
-DVL.N1LN5X.VLM.DSP : last exported on 11.10.23
-DVL.N1LN5X.VLM.WT : last exported on 11.10.23
-DDS.N1LR11.DSP : last exported on 11.10.23
-DDS.N1LR11.WT : last exported on 11.10.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 11.10.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 11.10.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 11.10.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 11.10.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 11.10.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 11.10.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 11.10.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 11.10.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 11.10.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 11.10.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 11.10.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 12.10.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 12.10.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 12.10.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 12.10.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 12.10.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 12.10.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 12.10.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 12.10.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 12.10.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 12.10.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 12.10.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 12.10.23
+DEL.N1LKT6.MT.??????.G : last exported on 12.10.23
+DEL.N1LKT6.MT.??????.U : last exported on 12.10.23
+DEL.N1LKT6.MT.??????.AS : last exported on 12.10.23
+DVL.N1LN5X.VLM.DSP : last exported on 12.10.23
+DVL.N1LN5X.VLM.WT : last exported on 12.10.23
+DDS.N1LR11.DSP : last exported on 12.10.23
+DDS.N1LR11.WT : last exported on 12.10.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 12.10.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 12.10.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 12.10.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 12.10.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 12.10.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 12.10.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 12.10.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 12.10.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 12.10.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 12.10.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 12.10.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,22 +1710,22 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 12.10.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 12.10.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 13.10.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 13.10.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 11.10.23
-DEL.N1LN3L.EM.F.GPL.DMP : last exported on 11.10.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 11.10.23
-DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 11.10.23
-DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 11.10.23
-DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 11.10.23
-DEL.N1LK61.EM.F.CPD.DMP : last exported on 11.10.23
-DEL.N1LN0R.EM.F.CPL.DMP : last exported on 11.10.23
-DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 11.10.23
-DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 11.10.23</t>
+          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 12.10.23
+DEL.N1LN3L.EM.F.GPL.DMP : last exported on 12.10.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 12.10.23
+DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 12.10.23
+DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 12.10.23
+DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 12.10.23
+DEL.N1LK61.EM.F.CPD.DMP : last exported on 12.10.23
+DEL.N1LN0R.EM.F.CPL.DMP : last exported on 12.10.23
+DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 12.10.23
+DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 12.10.23</t>
         </is>
       </c>
       <c r="E21" s="11" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 12.10.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 12.10.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 12.10.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 12.10.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 12.10.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 12.10.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 12.10.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 12.10.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 13.10.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 13.10.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 13.10.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 13.10.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 13.10.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 13.10.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 13.10.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 13.10.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 08.10.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 11.10.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 12.10.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 08.10.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 08.10.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 11.10.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 11.10.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 11.10.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 11.10.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 11.10.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 11.10.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 11.10.23
-DEL.N1LKT6.EC.??????.G : last exported on 11.10.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 11.10.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 11.10.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 11.10.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 11.10.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 11.10.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 11.10.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 11.10.23
-DEL.N1LKT6.EC.??????.U : last exported on 11.10.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 11.10.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 11.10.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 11.10.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 11.10.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 11.10.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 11.10.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 11.10.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 11.10.23
-DEL.N1LKT6.EC.??????.AS : last exported on 11.10.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 11.10.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 11.10.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 11.10.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 11.10.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 11.10.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 11.10.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 11.10.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 11.10.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 12.10.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 12.10.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 12.10.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 12.10.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 12.10.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 12.10.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 12.10.23
+DEL.N1LKT6.EC.??????.G : last exported on 12.10.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 12.10.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 12.10.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 12.10.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 12.10.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 12.10.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 12.10.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 12.10.23
+DEL.N1LKT6.EC.??????.U : last exported on 12.10.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 12.10.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 12.10.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 12.10.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 12.10.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 12.10.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 12.10.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 12.10.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 12.10.23
+DEL.N1LKT6.EC.??????.AS : last exported on 12.10.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 12.10.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 12.10.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 12.10.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 12.10.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 12.10.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 12.10.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 12.10.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 12.10.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 16.10.23 13:06
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 13.10.2023</t>
+          <t>Date - 16.10.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 12.10.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 13.10.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 13.10.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 13.10.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 13.10.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 13.10.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 13.10.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 13.10.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 13.10.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 13.10.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 13.10.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 13.10.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 13.10.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 13.10.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 13.10.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 13.10.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 14.10.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 14.10.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 15.10.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 14.10.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 14.10.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 14.10.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 14.10.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 14.10.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 14.10.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 14.10.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 14.10.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 14.10.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 14.10.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 14.10.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1077,22 +1077,22 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 09.10.23
-DEH.N3LKT6.AP.COMPL.SNK : last exported on 09.10.23</t>
+          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 16.10.23
+DEH.N3LKT6.AP.COMPL.SNK : last exported on 16.10.23</t>
         </is>
       </c>
       <c r="D6" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 09.10.23
-DEL.N1LN3L.DN.F.GPL.DMP : last exported on 09.10.23
-DEL.N1LN3L.DN.F.GTR.DMP : last exported on 09.10.23
-DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 09.10.23
-DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 09.10.23
-DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 09.10.23
-DEL.N1LK61.DN.F.CPD.DMP : last exported on 09.10.23
-DEL.N1LN0R.DN.F.CPL.DMP : last exported on 09.10.23
-DEL.KT6E35.SN.F.GGO.ZIP : last exported on 09.10.23
-DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 09.10.23</t>
+          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 16.10.23
+DEL.N1LN3L.DN.F.GPL.DMP : last exported on 16.10.23
+DEL.N1LN3L.DN.F.GTR.DMP : last exported on 16.10.23
+DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 16.10.23
+DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 16.10.23
+DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 16.10.23
+DEL.N1LK61.DN.F.CPD.DMP : last exported on 16.10.23
+DEL.N1LN0R.DN.F.CPL.DMP : last exported on 16.10.23
+DEL.KT6E35.SN.F.GGO.ZIP : last exported on 16.10.23
+DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 16.10.23</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
@@ -1121,30 +1121,30 @@
       <c r="C7" s="10" t="inlineStr">
         <is>
           <t>DLV.R31KT6.WI.C.ZIP : last exported on 11.10.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 12.10.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 15.10.23
 DLV.RPKKT6.WI.S.ZIP : last exported on 11.10.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 12.10.23
-DIT.E35KT6.WI.ZIP : last exported on 12.10.23
-DEL.K2PKT6.WI.ZIP : last exported on 12.10.23
-DEL.R7AKT6.WI.ZIP : last exported on 23.09.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 14.10.23
+DIT.E35KT6.WI.ZIP : last exported on 13.10.23
+DEL.K2PKT6.WI.ZIP : last exported on 15.10.23
+DEL.R7AKT6.WI.ZIP : last exported on 14.10.23
 DEL.N5FKT6.WI.ZIP : last exported on 12.10.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 12.10.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 12.10.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 12.10.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 12.10.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 12.10.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 12.10.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 12.10.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 12.10.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 12.10.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 12.10.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 12.10.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 12.10.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 12.10.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 16.10.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 16.10.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 16.10.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 16.10.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 16.10.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 16.10.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 16.10.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 15.10.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 15.10.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 15.10.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 15.10.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 15.10.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 15.10.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 12.09.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 13.10.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 16.10.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 09.10.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 12.10.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 12.10.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 12.10.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 12.10.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 12.10.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 12.10.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 12.10.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 12.10.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 12.10.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 12.10.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 12.10.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 12.10.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 12.10.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 12.10.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 12.10.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 12.10.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 12.10.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 15.10.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 15.10.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 15.10.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 15.10.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 15.10.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 15.10.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 15.10.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 15.10.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 15.10.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 15.10.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 15.10.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 15.10.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 15.10.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 15.10.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 15.10.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 15.10.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 15.10.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1338,7 +1338,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 05.10.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 12.10.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 15.10.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 05.10.23
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 12.10.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 13.10.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 12.10.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 14.10.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1406,20 +1406,20 @@
           <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 07.08.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
 DLV.I5XKT6.AU.A.ZIP : last exported on 05.07.23
-DLV.R31KT6.AU.C.ZIP : last exported on 11.10.23</t>
+DLV.R31KT6.AU.C.ZIP : last exported on 13.10.23</t>
         </is>
       </c>
       <c r="D14" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 11.10.23
-DEL.N1LN3L.AU.D.GPL.DMP : last exported on 11.10.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 12.10.23
-DEL.KT6N5M.AU.GGO.ZIP : last exported on 11.10.23
-DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 11.10.23
-DEL.KT6KTZ.AU.GGO.ZIP : last exported on 11.10.23
-DEL.KT6KTZ.AU.IMG.GGO.ZIP : last exported on 11.10.23
-DEL.KT6E35.AU.GGO.ZIP : last exported on 11.10.23
-DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 11.10.23</t>
+          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 13.10.23
+DEL.N1LN3L.AU.D.GPL.DMP : last exported on 13.10.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 15.10.23
+DEL.KT6N5M.AU.GGO.ZIP : last exported on 13.10.23
+DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 13.10.23
+DEL.KT6KTZ.AU.GGO.ZIP : last exported on 13.10.23
+DEL.KT6KTZ.AU.IMG.GGO.ZIP : last exported on 13.10.23
+DEL.KT6E35.AU.GGO.ZIP : last exported on 13.10.23
+DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 13.10.23</t>
         </is>
       </c>
       <c r="E14" s="11" t="inlineStr">
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 12.10.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 12.10.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 15.10.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 15.10.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 12.10.23
-DHP.KUDKT6.ORGUNITS : last exported on 13.10.23
-DHS.R11KT6.HSB02ALL : last exported on 12.10.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 15.10.23
+DHP.KUDKT6.ORGUNITS : last exported on 16.10.23
+DHS.R11KT6.HSB02ALL : last exported on 13.10.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 12.10.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 12.10.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 12.10.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 12.10.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 12.10.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 12.10.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 12.10.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 12.10.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 12.10.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 12.10.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 13.10.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 13.10.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 15.10.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 13.10.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 13.10.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 13.10.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 13.10.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 13.10.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 13.10.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 13.10.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1620,7 +1620,7 @@
       </c>
       <c r="D19" s="16" t="inlineStr">
         <is>
-          <t>DEL.N1LE35.TRANS.ZIP : last exported on 08.10.23</t>
+          <t>DEL.N1LE35.TRANS.ZIP : last exported on 15.10.23</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 12.10.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 14.10.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 12.10.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 12.10.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 12.10.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 12.10.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 12.10.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 12.10.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 12.10.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 12.10.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 12.10.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 12.10.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 12.10.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 12.10.23
-DEL.N1LKT6.MT.??????.G : last exported on 12.10.23
-DEL.N1LKT6.MT.??????.U : last exported on 12.10.23
-DEL.N1LKT6.MT.??????.AS : last exported on 12.10.23
-DVL.N1LN5X.VLM.DSP : last exported on 12.10.23
-DVL.N1LN5X.VLM.WT : last exported on 12.10.23
-DDS.N1LR11.DSP : last exported on 12.10.23
-DDS.N1LR11.WT : last exported on 12.10.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 12.10.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 12.10.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 12.10.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 12.10.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 12.10.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 12.10.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 12.10.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 12.10.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 12.10.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 12.10.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 12.10.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 14.10.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 14.10.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 15.10.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 14.10.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 14.10.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 14.10.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 14.10.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 14.10.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 14.10.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 14.10.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 14.10.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 14.10.23
+DEL.N1LKT6.MT.??????.G : last exported on 14.10.23
+DEL.N1LKT6.MT.??????.U : last exported on 14.10.23
+DEL.N1LKT6.MT.??????.AS : last exported on 14.10.23
+DVL.N1LN5X.VLM.DSP : last exported on 14.10.23
+DVL.N1LN5X.VLM.WT : last exported on 14.10.23
+DDS.N1LR11.DSP : last exported on 14.10.23
+DDS.N1LR11.WT : last exported on 14.10.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 14.10.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 14.10.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 14.10.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 14.10.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 14.10.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 14.10.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 14.10.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 14.10.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 14.10.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 14.10.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 14.10.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,22 +1710,22 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 13.10.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 13.10.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 16.10.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 16.10.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 12.10.23
-DEL.N1LN3L.EM.F.GPL.DMP : last exported on 12.10.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 12.10.23
-DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 12.10.23
-DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 12.10.23
-DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 12.10.23
-DEL.N1LK61.EM.F.CPD.DMP : last exported on 12.10.23
-DEL.N1LN0R.EM.F.CPL.DMP : last exported on 12.10.23
-DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 12.10.23
-DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 12.10.23</t>
+          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 15.10.23
+DEL.N1LN3L.EM.F.GPL.DMP : last exported on 15.10.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 15.10.23
+DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 15.10.23
+DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 15.10.23
+DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 15.10.23
+DEL.N1LK61.EM.F.CPD.DMP : last exported on 15.10.23
+DEL.N1LN0R.EM.F.CPL.DMP : last exported on 15.10.23
+DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 15.10.23
+DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 15.10.23</t>
         </is>
       </c>
       <c r="E21" s="11" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 13.10.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 13.10.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 13.10.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 13.10.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 13.10.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 13.10.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 13.10.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 13.10.23
-DDC.R11KT6.ELFI.MD.TXT : last exported on 08.10.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 12.10.23
-DDC.R11KT6.ELFI.PK.TXT : last exported on 08.10.23
-DDC.R11KT6.ELFI.PR.TXT : last exported on 08.10.23</t>
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 16.10.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 16.10.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 16.10.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 16.10.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 16.10.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 16.10.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 16.10.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 16.10.23
+DDC.R11KT6.ELFI.MD.TXT : last exported on 15.10.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 13.10.23
+DDC.R11KT6.ELFI.PK.TXT : last exported on 15.10.23
+DDC.R11KT6.ELFI.PR.TXT : last exported on 15.10.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 12.10.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 12.10.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 12.10.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 12.10.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 12.10.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 12.10.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 12.10.23
-DEL.N1LKT6.EC.??????.G : last exported on 12.10.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 12.10.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 12.10.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 12.10.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 12.10.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 12.10.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 12.10.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 12.10.23
-DEL.N1LKT6.EC.??????.U : last exported on 12.10.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 12.10.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 12.10.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 12.10.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 12.10.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 12.10.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 12.10.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 12.10.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 12.10.23
-DEL.N1LKT6.EC.??????.AS : last exported on 12.10.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 12.10.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 12.10.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 12.10.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 12.10.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 12.10.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 12.10.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 12.10.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 12.10.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 15.10.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 15.10.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 15.10.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 15.10.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 15.10.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 15.10.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 15.10.23
+DEL.N1LKT6.EC.??????.G : last exported on 15.10.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 15.10.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 15.10.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 15.10.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 15.10.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 15.10.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 15.10.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 15.10.23
+DEL.N1LKT6.EC.??????.U : last exported on 15.10.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 15.10.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 15.10.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 15.10.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 15.10.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 15.10.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 15.10.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 15.10.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 15.10.23
+DEL.N1LKT6.EC.??????.AS : last exported on 15.10.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 15.10.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 15.10.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 15.10.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 15.10.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 15.10.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 15.10.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 15.10.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 15.10.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 17.10.23 11:58
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 16.10.2023</t>
+          <t>Date - 17.10.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 13.10.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 16.10.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 14.10.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 14.10.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 15.10.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 14.10.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 14.10.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 14.10.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 14.10.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 14.10.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 14.10.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 14.10.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 14.10.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 14.10.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 14.10.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 14.10.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 17.10.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 17.10.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 17.10.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 17.10.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 17.10.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 17.10.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 17.10.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 17.10.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 17.10.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 17.10.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 17.10.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 17.10.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 17.10.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 17.10.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1120,12 +1120,12 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 11.10.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 15.10.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 16.10.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 16.10.23
 DLV.RPKKT6.WI.S.ZIP : last exported on 11.10.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 14.10.23
-DIT.E35KT6.WI.ZIP : last exported on 13.10.23
-DEL.K2PKT6.WI.ZIP : last exported on 15.10.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 16.10.23
+DIT.E35KT6.WI.ZIP : last exported on 16.10.23
+DEL.K2PKT6.WI.ZIP : last exported on 16.10.23
 DEL.R7AKT6.WI.ZIP : last exported on 14.10.23
 DEL.N5FKT6.WI.ZIP : last exported on 12.10.23</t>
         </is>
@@ -1139,12 +1139,12 @@
 DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 16.10.23
 DEL.N1LK61.WI.D.CPD.DMP : last exported on 16.10.23
 DEL.N1LN0R.WI.D.CPL.DMP : last exported on 16.10.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 15.10.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 15.10.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 15.10.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 15.10.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 15.10.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 15.10.23</t>
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 16.10.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 16.10.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 16.10.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 16.10.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 16.10.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 16.10.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 12.09.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 16.10.23
-DGV.N3LKT6.EPELS.??????.ZIP : last exported on 09.10.23</t>
+DEL.N3LKT6.HST.??????.ZIP : last exported on 17.10.23
+DGV.N3LKT6.EPELS.??????.ZIP : last exported on 16.10.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 15.10.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 15.10.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 15.10.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 15.10.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 15.10.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 15.10.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 15.10.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 15.10.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 15.10.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 15.10.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 15.10.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 15.10.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 15.10.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 15.10.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 15.10.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 15.10.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 15.10.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 16.10.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 16.10.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 16.10.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 16.10.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 16.10.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 16.10.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 16.10.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 16.10.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 16.10.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 16.10.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 16.10.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 16.10.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 16.10.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 16.10.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 16.10.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 16.10.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 16.10.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1298,12 +1298,12 @@
       </c>
       <c r="C11" s="14" t="inlineStr">
         <is>
-          <t>DEL.KT6KT6.APOSPRO.ZIP : last exported on 09.10.23</t>
+          <t>DEL.KT6KT6.APOSPRO.ZIP : last exported on 16.10.23</t>
         </is>
       </c>
       <c r="D11" s="15" t="inlineStr">
         <is>
-          <t>DEL.KT6N2O.XTIME.ZIP : last exported on 09.10.23</t>
+          <t>DEL.KT6N2O.XTIME.ZIP : last exported on 16.10.23</t>
         </is>
       </c>
       <c r="E11" s="11" t="inlineStr">
@@ -1338,7 +1338,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 05.10.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 15.10.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 16.10.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 05.10.23
@@ -1370,7 +1370,7 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 13.10.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 16.10.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
@@ -1406,20 +1406,20 @@
           <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 07.08.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
 DLV.I5XKT6.AU.A.ZIP : last exported on 05.07.23
-DLV.R31KT6.AU.C.ZIP : last exported on 13.10.23</t>
+DLV.R31KT6.AU.C.ZIP : last exported on 16.10.23</t>
         </is>
       </c>
       <c r="D14" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 13.10.23
-DEL.N1LN3L.AU.D.GPL.DMP : last exported on 13.10.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 15.10.23
-DEL.KT6N5M.AU.GGO.ZIP : last exported on 13.10.23
-DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 13.10.23
-DEL.KT6KTZ.AU.GGO.ZIP : last exported on 13.10.23
-DEL.KT6KTZ.AU.IMG.GGO.ZIP : last exported on 13.10.23
-DEL.KT6E35.AU.GGO.ZIP : last exported on 13.10.23
-DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 13.10.23</t>
+          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 16.10.23
+DEL.N1LN3L.AU.D.GPL.DMP : last exported on 16.10.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 16.10.23
+DEL.KT6N5M.AU.GGO.ZIP : last exported on 16.10.23
+DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 16.10.23
+DEL.KT6KTZ.AU.GGO.ZIP : last exported on 16.10.23
+DEL.KT6KTZ.AU.IMG.GGO.ZIP : last exported on 16.10.23
+DEL.KT6E35.AU.GGO.ZIP : last exported on 16.10.23
+DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 16.10.23</t>
         </is>
       </c>
       <c r="E14" s="11" t="inlineStr">
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 15.10.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 15.10.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 16.10.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 16.10.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 15.10.23
-DHP.KUDKT6.ORGUNITS : last exported on 16.10.23
-DHS.R11KT6.HSB02ALL : last exported on 13.10.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 16.10.23
+DHP.KUDKT6.ORGUNITS : last exported on 17.10.23
+DHS.R11KT6.HSB02ALL : last exported on 16.10.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 13.10.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 13.10.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 15.10.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 13.10.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 13.10.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 13.10.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 13.10.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 13.10.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 13.10.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 13.10.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 16.10.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 16.10.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 16.10.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 16.10.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 16.10.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 16.10.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 16.10.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 16.10.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 16.10.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 16.10.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 14.10.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 16.10.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 14.10.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 14.10.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 15.10.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 14.10.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 14.10.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 14.10.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 14.10.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 14.10.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 14.10.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 14.10.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 14.10.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 14.10.23
-DEL.N1LKT6.MT.??????.G : last exported on 14.10.23
-DEL.N1LKT6.MT.??????.U : last exported on 14.10.23
-DEL.N1LKT6.MT.??????.AS : last exported on 14.10.23
-DVL.N1LN5X.VLM.DSP : last exported on 14.10.23
-DVL.N1LN5X.VLM.WT : last exported on 14.10.23
-DDS.N1LR11.DSP : last exported on 14.10.23
-DDS.N1LR11.WT : last exported on 14.10.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 14.10.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 14.10.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 14.10.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 14.10.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 14.10.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 14.10.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 14.10.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 14.10.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 14.10.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 14.10.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 14.10.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 16.10.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 16.10.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 16.10.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 16.10.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 16.10.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 16.10.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 16.10.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 16.10.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 16.10.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 16.10.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 16.10.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 16.10.23
+DEL.N1LKT6.MT.??????.G : last exported on 16.10.23
+DEL.N1LKT6.MT.??????.U : last exported on 16.10.23
+DEL.N1LKT6.MT.??????.AS : last exported on 16.10.23
+DVL.N1LN5X.VLM.DSP : last exported on 16.10.23
+DVL.N1LN5X.VLM.WT : last exported on 16.10.23
+DDS.N1LR11.DSP : last exported on 16.10.23
+DDS.N1LR11.WT : last exported on 16.10.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 16.10.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 16.10.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 16.10.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 16.10.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 16.10.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 16.10.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 16.10.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 16.10.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 16.10.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 16.10.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 16.10.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,22 +1710,22 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 16.10.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 16.10.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 17.10.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 17.10.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 15.10.23
-DEL.N1LN3L.EM.F.GPL.DMP : last exported on 15.10.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 15.10.23
-DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 15.10.23
-DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 15.10.23
-DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 15.10.23
-DEL.N1LK61.EM.F.CPD.DMP : last exported on 15.10.23
-DEL.N1LN0R.EM.F.CPL.DMP : last exported on 15.10.23
-DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 15.10.23
-DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 15.10.23</t>
+          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 16.10.23
+DEL.N1LN3L.EM.F.GPL.DMP : last exported on 16.10.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 16.10.23
+DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 16.10.23
+DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 16.10.23
+DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 16.10.23
+DEL.N1LK61.EM.F.CPD.DMP : last exported on 16.10.23
+DEL.N1LN0R.EM.F.CPL.DMP : last exported on 16.10.23
+DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 16.10.23
+DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 16.10.23</t>
         </is>
       </c>
       <c r="E21" s="11" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 16.10.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 16.10.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 16.10.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 16.10.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 16.10.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 16.10.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 16.10.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 16.10.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 17.10.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 17.10.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 17.10.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 17.10.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 17.10.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 17.10.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 17.10.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 17.10.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 15.10.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 13.10.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 16.10.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 15.10.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 15.10.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 15.10.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 15.10.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 15.10.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 15.10.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 15.10.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 15.10.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 15.10.23
-DEL.N1LKT6.EC.??????.G : last exported on 15.10.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 15.10.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 15.10.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 15.10.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 15.10.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 15.10.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 15.10.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 15.10.23
-DEL.N1LKT6.EC.??????.U : last exported on 15.10.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 15.10.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 15.10.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 15.10.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 15.10.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 15.10.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 15.10.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 15.10.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 15.10.23
-DEL.N1LKT6.EC.??????.AS : last exported on 15.10.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 15.10.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 15.10.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 15.10.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 15.10.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 15.10.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 15.10.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 15.10.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 15.10.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 16.10.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 16.10.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 16.10.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 16.10.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 16.10.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 16.10.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 16.10.23
+DEL.N1LKT6.EC.??????.G : last exported on 16.10.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 16.10.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 16.10.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 16.10.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 16.10.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 16.10.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 16.10.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 16.10.23
+DEL.N1LKT6.EC.??????.U : last exported on 16.10.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 16.10.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 16.10.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 16.10.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 16.10.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 16.10.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 16.10.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 16.10.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 16.10.23
+DEL.N1LKT6.EC.??????.AS : last exported on 16.10.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 16.10.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 16.10.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 16.10.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 16.10.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 16.10.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 16.10.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 16.10.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 16.10.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 18.10.23 13:02
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 17.10.2023</t>
+          <t>Date - 18.10.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 16.10.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 17.10.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 17.10.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 17.10.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 17.10.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 17.10.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 17.10.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 17.10.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 17.10.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 17.10.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 17.10.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 17.10.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 17.10.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 17.10.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 17.10.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 17.10.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 18.10.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 18.10.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 18.10.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 18.10.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 18.10.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 18.10.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 18.10.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 18.10.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 18.10.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 18.10.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 18.10.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 18.10.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 18.10.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 18.10.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1120,31 +1120,31 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 16.10.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 16.10.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 11.10.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 16.10.23
-DIT.E35KT6.WI.ZIP : last exported on 16.10.23
-DEL.K2PKT6.WI.ZIP : last exported on 16.10.23
-DEL.R7AKT6.WI.ZIP : last exported on 14.10.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 17.10.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 17.10.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 17.10.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 17.10.23
+DIT.E35KT6.WI.ZIP : last exported on 17.10.23
+DEL.K2PKT6.WI.ZIP : last exported on 17.10.23
+DEL.R7AKT6.WI.ZIP : last exported on 18.10.23
 DEL.N5FKT6.WI.ZIP : last exported on 12.10.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 16.10.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 16.10.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 16.10.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 16.10.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 16.10.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 16.10.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 16.10.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 16.10.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 16.10.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 16.10.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 16.10.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 16.10.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 16.10.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 17.10.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 17.10.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 17.10.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 17.10.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 17.10.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 17.10.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 17.10.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 17.10.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 17.10.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 17.10.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 17.10.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 17.10.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 17.10.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 12.09.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 17.10.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 18.10.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 16.10.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 16.10.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 16.10.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 16.10.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 16.10.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 16.10.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 16.10.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 16.10.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 16.10.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 16.10.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 16.10.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 16.10.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 16.10.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 16.10.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 16.10.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 16.10.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 16.10.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 16.10.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 17.10.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 17.10.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 17.10.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 17.10.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 17.10.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 17.10.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 17.10.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 17.10.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 17.10.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 17.10.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 17.10.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 17.10.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 17.10.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 17.10.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 17.10.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 17.10.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 17.10.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1338,7 +1338,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 05.10.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 16.10.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 17.10.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 05.10.23
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 16.10.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 17.10.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 14.10.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 17.10.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1413,7 +1413,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 16.10.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 16.10.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 16.10.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 17.10.23
 DEL.KT6N5M.AU.GGO.ZIP : last exported on 16.10.23
 DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 16.10.23
 DEL.KT6KTZ.AU.GGO.ZIP : last exported on 16.10.23
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 16.10.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 16.10.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 17.10.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 17.10.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 16.10.23
-DHP.KUDKT6.ORGUNITS : last exported on 17.10.23
-DHS.R11KT6.HSB02ALL : last exported on 16.10.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 17.10.23
+DHP.KUDKT6.ORGUNITS : last exported on 18.10.23
+DHS.R11KT6.HSB02ALL : last exported on 17.10.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 16.10.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 16.10.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 16.10.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 16.10.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 16.10.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 16.10.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 16.10.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 16.10.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 16.10.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 16.10.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 17.10.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 17.10.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 17.10.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 17.10.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 17.10.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 17.10.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 17.10.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 17.10.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 17.10.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 17.10.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1655,7 +1655,7 @@
         <is>
           <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 16.10.23
 DEL.N1LN3L.MT.F.GPL.DMP : last exported on 16.10.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 16.10.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 17.10.23
 DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 16.10.23
 DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 16.10.23
 DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 16.10.23
@@ -1710,22 +1710,22 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 17.10.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 17.10.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 18.10.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 18.10.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 16.10.23
-DEL.N1LN3L.EM.F.GPL.DMP : last exported on 16.10.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 16.10.23
-DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 16.10.23
-DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 16.10.23
-DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 16.10.23
-DEL.N1LK61.EM.F.CPD.DMP : last exported on 16.10.23
-DEL.N1LN0R.EM.F.CPL.DMP : last exported on 16.10.23
-DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 16.10.23
-DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 16.10.23</t>
+          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 17.10.23
+DEL.N1LN3L.EM.F.GPL.DMP : last exported on 17.10.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 17.10.23
+DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 17.10.23
+DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 17.10.23
+DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 17.10.23
+DEL.N1LK61.EM.F.CPD.DMP : last exported on 17.10.23
+DEL.N1LN0R.EM.F.CPL.DMP : last exported on 17.10.23
+DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 17.10.23
+DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 17.10.23</t>
         </is>
       </c>
       <c r="E21" s="11" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 17.10.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 17.10.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 17.10.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 17.10.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 17.10.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 17.10.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 17.10.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 17.10.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 18.10.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 18.10.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 18.10.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 18.10.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 18.10.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 18.10.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 18.10.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 18.10.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 15.10.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 16.10.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 17.10.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 15.10.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 15.10.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 16.10.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 16.10.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 16.10.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 16.10.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 16.10.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 16.10.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 16.10.23
-DEL.N1LKT6.EC.??????.G : last exported on 16.10.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 16.10.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 16.10.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 16.10.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 16.10.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 16.10.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 16.10.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 16.10.23
-DEL.N1LKT6.EC.??????.U : last exported on 16.10.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 16.10.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 16.10.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 16.10.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 16.10.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 16.10.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 16.10.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 16.10.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 16.10.23
-DEL.N1LKT6.EC.??????.AS : last exported on 16.10.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 16.10.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 16.10.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 16.10.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 16.10.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 16.10.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 16.10.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 16.10.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 16.10.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 17.10.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 17.10.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 17.10.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 17.10.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 17.10.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 17.10.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 17.10.23
+DEL.N1LKT6.EC.??????.G : last exported on 17.10.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 17.10.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 17.10.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 17.10.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 17.10.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 17.10.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 17.10.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 17.10.23
+DEL.N1LKT6.EC.??????.U : last exported on 17.10.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 17.10.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 17.10.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 17.10.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 17.10.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 17.10.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 17.10.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 17.10.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 17.10.23
+DEL.N1LKT6.EC.??????.AS : last exported on 17.10.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 17.10.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 17.10.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 17.10.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 17.10.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 17.10.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 17.10.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 17.10.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 17.10.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 19.10.23 12:53
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 18.10.2023</t>
+          <t>Date - 19.10.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 17.10.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 18.10.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 18.10.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 18.10.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 18.10.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 18.10.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 18.10.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 18.10.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 18.10.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 18.10.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 18.10.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 18.10.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 18.10.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 18.10.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 18.10.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 18.10.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 19.10.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 19.10.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 19.10.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 19.10.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 19.10.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 19.10.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 19.10.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 19.10.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 19.10.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 19.10.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 19.10.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 19.10.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 19.10.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 19.10.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1120,31 +1120,31 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 17.10.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 17.10.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 17.10.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 17.10.23
-DIT.E35KT6.WI.ZIP : last exported on 17.10.23
-DEL.K2PKT6.WI.ZIP : last exported on 17.10.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 18.10.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 18.10.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 18.10.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 18.10.23
+DIT.E35KT6.WI.ZIP : last exported on 18.10.23
+DEL.K2PKT6.WI.ZIP : last exported on 18.10.23
 DEL.R7AKT6.WI.ZIP : last exported on 18.10.23
 DEL.N5FKT6.WI.ZIP : last exported on 12.10.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 17.10.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 17.10.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 17.10.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 17.10.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 17.10.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 17.10.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 17.10.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 17.10.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 17.10.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 17.10.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 17.10.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 17.10.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 17.10.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 18.10.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 18.10.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 18.10.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 18.10.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 18.10.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 18.10.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 18.10.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 18.10.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 18.10.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 18.10.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 18.10.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 18.10.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 18.10.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 12.09.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 18.10.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 19.10.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 16.10.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 17.10.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 17.10.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 17.10.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 17.10.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 17.10.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 17.10.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 17.10.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 17.10.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 17.10.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 17.10.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 17.10.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 17.10.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 17.10.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 17.10.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 17.10.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 17.10.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 17.10.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 18.10.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 18.10.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 18.10.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 18.10.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 18.10.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 18.10.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 18.10.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 18.10.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 18.10.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 18.10.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 18.10.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 18.10.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 18.10.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 18.10.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 18.10.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 18.10.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 18.10.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1338,7 +1338,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 05.10.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 17.10.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 18.10.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 05.10.23
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 17.10.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 18.10.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 17.10.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 18.10.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1406,20 +1406,20 @@
           <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 07.08.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
 DLV.I5XKT6.AU.A.ZIP : last exported on 05.07.23
-DLV.R31KT6.AU.C.ZIP : last exported on 16.10.23</t>
+DLV.R31KT6.AU.C.ZIP : last exported on 18.10.23</t>
         </is>
       </c>
       <c r="D14" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 16.10.23
-DEL.N1LN3L.AU.D.GPL.DMP : last exported on 16.10.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 17.10.23
-DEL.KT6N5M.AU.GGO.ZIP : last exported on 16.10.23
-DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 16.10.23
-DEL.KT6KTZ.AU.GGO.ZIP : last exported on 16.10.23
-DEL.KT6KTZ.AU.IMG.GGO.ZIP : last exported on 16.10.23
-DEL.KT6E35.AU.GGO.ZIP : last exported on 16.10.23
-DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 16.10.23</t>
+          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 18.10.23
+DEL.N1LN3L.AU.D.GPL.DMP : last exported on 18.10.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 18.10.23
+DEL.KT6N5M.AU.GGO.ZIP : last exported on 18.10.23
+DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 18.10.23
+DEL.KT6KTZ.AU.GGO.ZIP : last exported on 18.10.23
+DEL.KT6KTZ.AU.IMG.GGO.ZIP : last exported on 18.10.23
+DEL.KT6E35.AU.GGO.ZIP : last exported on 18.10.23
+DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 18.10.23</t>
         </is>
       </c>
       <c r="E14" s="11" t="inlineStr">
@@ -1457,24 +1457,24 @@
 DGQ.R11KT6.BSITX.TXT : last exported on 04.10.23
 DGQ.R31KT6.BSIVMC.TXT : last exported on 10.10.23
 DGQ.R31KT6.PKATC.TXT : last exported on 10.10.23
-DEL.KMPKT6.APOS.DATA.ZIP : last exported on 11.10.23</t>
+DEL.KMPKT6.APOS.DATA.ZIP : last exported on 18.10.23</t>
         </is>
       </c>
       <c r="D15" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 11.10.23
-DEL.N1LN3L.AP.F.GPL.DMP : last exported on 11.10.23
-DEL.N1LN3L.AP.F.GTR.DMP : last exported on 11.10.23
-DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 11.10.23
-DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 11.10.23
-DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 11.10.23
-DEL.N1LK61.AP.F.CPD.DMP : last exported on 11.10.23
-DEL.N1LN0R.AP.F.CPL.DMP : last exported on 11.10.23
-DEL.N1LR31.AP.F.PPS.DMP : last exported on 11.10.23
-DEL.KT6E35.AP.F.DB.ZIP : last exported on 11.10.23
-DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 11.10.23
-DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 11.10.23
-DVL.KT6N5X.VLM.AP.ZIP : last exported on 11.10.23</t>
+          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 18.10.23
+DEL.N1LN3L.AP.F.GPL.DMP : last exported on 18.10.23
+DEL.N1LN3L.AP.F.GTR.DMP : last exported on 18.10.23
+DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 18.10.23
+DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 18.10.23
+DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 18.10.23
+DEL.N1LK61.AP.F.CPD.DMP : last exported on 18.10.23
+DEL.N1LN0R.AP.F.CPL.DMP : last exported on 18.10.23
+DEL.N1LR31.AP.F.PPS.DMP : last exported on 18.10.23
+DEL.KT6E35.AP.F.DB.ZIP : last exported on 18.10.23
+DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 18.10.23
+DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 18.10.23
+DVL.KT6N5X.VLM.AP.ZIP : last exported on 18.10.23</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 17.10.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 17.10.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 18.10.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 18.10.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 17.10.23
-DHP.KUDKT6.ORGUNITS : last exported on 18.10.23
-DHS.R11KT6.HSB02ALL : last exported on 17.10.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 18.10.23
+DHP.KUDKT6.ORGUNITS : last exported on 19.10.23
+DHS.R11KT6.HSB02ALL : last exported on 18.10.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 17.10.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 17.10.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 17.10.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 17.10.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 17.10.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 17.10.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 17.10.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 17.10.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 17.10.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 17.10.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 18.10.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 18.10.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 18.10.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 18.10.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 18.10.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 18.10.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 18.10.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 18.10.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 18.10.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 18.10.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1648,14 +1648,14 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 16.10.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 19.10.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 16.10.23
 DEL.N1LN3L.MT.F.GPL.DMP : last exported on 16.10.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 17.10.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 18.10.23
 DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 16.10.23
 DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 16.10.23
 DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 16.10.23
@@ -1710,22 +1710,22 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 18.10.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 18.10.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 19.10.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 19.10.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 17.10.23
-DEL.N1LN3L.EM.F.GPL.DMP : last exported on 17.10.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 17.10.23
-DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 17.10.23
-DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 17.10.23
-DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 17.10.23
-DEL.N1LK61.EM.F.CPD.DMP : last exported on 17.10.23
-DEL.N1LN0R.EM.F.CPL.DMP : last exported on 17.10.23
-DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 17.10.23
-DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 17.10.23</t>
+          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 18.10.23
+DEL.N1LN3L.EM.F.GPL.DMP : last exported on 18.10.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 18.10.23
+DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 18.10.23
+DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 18.10.23
+DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 18.10.23
+DEL.N1LK61.EM.F.CPD.DMP : last exported on 18.10.23
+DEL.N1LN0R.EM.F.CPL.DMP : last exported on 18.10.23
+DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 18.10.23
+DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 18.10.23</t>
         </is>
       </c>
       <c r="E21" s="11" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 18.10.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 18.10.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 18.10.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 18.10.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 18.10.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 18.10.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 18.10.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 18.10.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 19.10.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 19.10.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 19.10.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 19.10.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 19.10.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 19.10.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 19.10.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 19.10.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 15.10.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 17.10.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 18.10.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 15.10.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 15.10.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 17.10.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 17.10.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 17.10.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 17.10.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 17.10.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 17.10.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 17.10.23
-DEL.N1LKT6.EC.??????.G : last exported on 17.10.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 17.10.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 17.10.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 17.10.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 17.10.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 17.10.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 17.10.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 17.10.23
-DEL.N1LKT6.EC.??????.U : last exported on 17.10.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 17.10.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 17.10.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 17.10.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 17.10.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 17.10.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 17.10.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 17.10.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 17.10.23
-DEL.N1LKT6.EC.??????.AS : last exported on 17.10.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 17.10.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 17.10.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 17.10.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 17.10.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 17.10.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 17.10.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 17.10.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 17.10.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 18.10.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 18.10.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 18.10.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 18.10.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 18.10.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 18.10.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 18.10.23
+DEL.N1LKT6.EC.??????.G : last exported on 18.10.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 18.10.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 18.10.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 18.10.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 18.10.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 18.10.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 18.10.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 18.10.23
+DEL.N1LKT6.EC.??????.U : last exported on 18.10.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 18.10.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 18.10.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 18.10.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 18.10.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 18.10.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 18.10.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 18.10.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 18.10.23
+DEL.N1LKT6.EC.??????.AS : last exported on 18.10.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 18.10.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 18.10.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 18.10.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 18.10.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 18.10.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 18.10.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 18.10.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 18.10.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 20.10.23 13:32
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 19.10.2023</t>
+          <t>Date - 20.10.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 18.10.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 19.10.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 19.10.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 19.10.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 19.10.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 19.10.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 19.10.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 19.10.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 19.10.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 19.10.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 19.10.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 19.10.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 19.10.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 19.10.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 19.10.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 19.10.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 20.10.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 20.10.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 20.10.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 20.10.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 20.10.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 20.10.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 20.10.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 20.10.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 20.10.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 20.10.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 20.10.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 20.10.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 20.10.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 20.10.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1121,30 +1121,30 @@
       <c r="C7" s="10" t="inlineStr">
         <is>
           <t>DLV.R31KT6.WI.C.ZIP : last exported on 18.10.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 18.10.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 18.10.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 18.10.23
-DIT.E35KT6.WI.ZIP : last exported on 18.10.23
-DEL.K2PKT6.WI.ZIP : last exported on 18.10.23
-DEL.R7AKT6.WI.ZIP : last exported on 18.10.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 19.10.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 19.10.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 19.10.23
+DIT.E35KT6.WI.ZIP : last exported on 19.10.23
+DEL.K2PKT6.WI.ZIP : last exported on 19.10.23
+DEL.R7AKT6.WI.ZIP : last exported on 20.10.23
 DEL.N5FKT6.WI.ZIP : last exported on 12.10.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 18.10.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 18.10.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 18.10.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 18.10.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 18.10.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 18.10.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 18.10.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 18.10.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 18.10.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 18.10.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 18.10.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 18.10.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 18.10.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 19.10.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 19.10.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 19.10.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 19.10.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 19.10.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 19.10.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 19.10.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 19.10.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 19.10.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 19.10.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 19.10.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 19.10.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 19.10.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 12.09.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 19.10.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 20.10.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 16.10.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 18.10.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 18.10.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 18.10.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 18.10.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 18.10.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 18.10.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 18.10.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 18.10.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 18.10.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 18.10.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 18.10.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 18.10.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 18.10.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 18.10.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 18.10.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 18.10.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 18.10.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 19.10.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 19.10.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 19.10.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 19.10.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 19.10.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 19.10.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 19.10.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 19.10.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 19.10.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 19.10.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 19.10.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 19.10.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 19.10.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 19.10.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 19.10.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 19.10.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 19.10.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1338,7 +1338,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 05.10.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 18.10.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 19.10.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 05.10.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 05.10.23
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 18.10.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 19.10.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 18.10.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 19.10.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1413,7 +1413,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 18.10.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 18.10.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 18.10.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 19.10.23
 DEL.KT6N5M.AU.GGO.ZIP : last exported on 18.10.23
 DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 18.10.23
 DEL.KT6KTZ.AU.GGO.ZIP : last exported on 18.10.23
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 18.10.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 18.10.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 19.10.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 19.10.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 18.10.23
-DHP.KUDKT6.ORGUNITS : last exported on 19.10.23
-DHS.R11KT6.HSB02ALL : last exported on 18.10.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 19.10.23
+DHP.KUDKT6.ORGUNITS : last exported on 20.10.23
+DHS.R11KT6.HSB02ALL : last exported on 19.10.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 18.10.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 18.10.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 18.10.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 18.10.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 18.10.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 18.10.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 18.10.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 18.10.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 18.10.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 18.10.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 19.10.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 19.10.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 19.10.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 19.10.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 19.10.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 19.10.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 19.10.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 19.10.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 19.10.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 19.10.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1653,36 +1653,36 @@
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 16.10.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 16.10.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 18.10.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 16.10.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 16.10.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 16.10.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 16.10.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 16.10.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 16.10.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 16.10.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 16.10.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 16.10.23
-DEL.N1LKT6.MT.??????.G : last exported on 16.10.23
-DEL.N1LKT6.MT.??????.U : last exported on 16.10.23
-DEL.N1LKT6.MT.??????.AS : last exported on 16.10.23
-DVL.N1LN5X.VLM.DSP : last exported on 16.10.23
-DVL.N1LN5X.VLM.WT : last exported on 16.10.23
-DDS.N1LR11.DSP : last exported on 16.10.23
-DDS.N1LR11.WT : last exported on 16.10.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 16.10.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 16.10.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 16.10.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 16.10.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 16.10.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 16.10.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 16.10.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 16.10.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 16.10.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 16.10.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 16.10.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 19.10.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 19.10.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 19.10.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 19.10.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 19.10.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 19.10.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 19.10.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 19.10.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 19.10.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 19.10.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 19.10.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 19.10.23
+DEL.N1LKT6.MT.??????.G : last exported on 19.10.23
+DEL.N1LKT6.MT.??????.U : last exported on 19.10.23
+DEL.N1LKT6.MT.??????.AS : last exported on 19.10.23
+DVL.N1LN5X.VLM.DSP : last exported on 19.10.23
+DVL.N1LN5X.VLM.WT : last exported on 19.10.23
+DDS.N1LR11.DSP : last exported on 19.10.23
+DDS.N1LR11.WT : last exported on 19.10.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 19.10.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 19.10.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 19.10.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 19.10.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 19.10.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 19.10.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 19.10.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 19.10.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 19.10.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 19.10.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 19.10.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,22 +1710,22 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 19.10.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 19.10.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 20.10.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 20.10.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 18.10.23
-DEL.N1LN3L.EM.F.GPL.DMP : last exported on 18.10.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 18.10.23
-DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 18.10.23
-DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 18.10.23
-DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 18.10.23
-DEL.N1LK61.EM.F.CPD.DMP : last exported on 18.10.23
-DEL.N1LN0R.EM.F.CPL.DMP : last exported on 18.10.23
-DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 18.10.23
-DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 18.10.23</t>
+          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 19.10.23
+DEL.N1LN3L.EM.F.GPL.DMP : last exported on 19.10.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 19.10.23
+DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 19.10.23
+DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 19.10.23
+DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 19.10.23
+DEL.N1LK61.EM.F.CPD.DMP : last exported on 19.10.23
+DEL.N1LN0R.EM.F.CPL.DMP : last exported on 19.10.23
+DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 19.10.23
+DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 19.10.23</t>
         </is>
       </c>
       <c r="E21" s="11" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 19.10.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 19.10.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 19.10.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 19.10.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 19.10.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 19.10.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 19.10.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 19.10.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 20.10.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 20.10.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 20.10.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 20.10.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 20.10.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 20.10.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 20.10.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 20.10.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 15.10.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 18.10.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 19.10.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 15.10.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 15.10.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 18.10.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 18.10.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 18.10.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 18.10.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 18.10.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 18.10.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 18.10.23
-DEL.N1LKT6.EC.??????.G : last exported on 18.10.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 18.10.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 18.10.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 18.10.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 18.10.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 18.10.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 18.10.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 18.10.23
-DEL.N1LKT6.EC.??????.U : last exported on 18.10.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 18.10.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 18.10.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 18.10.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 18.10.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 18.10.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 18.10.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 18.10.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 18.10.23
-DEL.N1LKT6.EC.??????.AS : last exported on 18.10.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 18.10.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 18.10.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 18.10.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 18.10.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 18.10.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 18.10.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 18.10.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 18.10.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 19.10.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 19.10.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 19.10.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 19.10.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 19.10.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 19.10.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 19.10.23
+DEL.N1LKT6.EC.??????.G : last exported on 19.10.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 19.10.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 19.10.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 19.10.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 19.10.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 19.10.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 19.10.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 19.10.23
+DEL.N1LKT6.EC.??????.U : last exported on 19.10.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 19.10.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 19.10.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 19.10.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 19.10.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 19.10.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 19.10.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 19.10.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 19.10.23
+DEL.N1LKT6.EC.??????.AS : last exported on 19.10.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 19.10.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 19.10.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 19.10.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 19.10.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 19.10.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 19.10.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 19.10.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 19.10.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 23.10.23 13:46
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 20.10.2023</t>
+          <t>Date - 23.10.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 19.10.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 20.10.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 20.10.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 20.10.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 20.10.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 20.10.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 20.10.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 20.10.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 20.10.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 20.10.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 20.10.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 20.10.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 20.10.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 20.10.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 20.10.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 20.10.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 21.10.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 21.10.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 22.10.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 21.10.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 21.10.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 21.10.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 21.10.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 21.10.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 21.10.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 21.10.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 21.10.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 21.10.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 21.10.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 21.10.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1077,22 +1077,22 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 16.10.23
-DEH.N3LKT6.AP.COMPL.SNK : last exported on 16.10.23</t>
+          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 23.10.23
+DEH.N3LKT6.AP.COMPL.SNK : last exported on 23.10.23</t>
         </is>
       </c>
       <c r="D6" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 16.10.23
-DEL.N1LN3L.DN.F.GPL.DMP : last exported on 16.10.23
-DEL.N1LN3L.DN.F.GTR.DMP : last exported on 16.10.23
-DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 16.10.23
-DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 16.10.23
-DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 16.10.23
-DEL.N1LK61.DN.F.CPD.DMP : last exported on 16.10.23
-DEL.N1LN0R.DN.F.CPL.DMP : last exported on 16.10.23
-DEL.KT6E35.SN.F.GGO.ZIP : last exported on 16.10.23
-DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 16.10.23</t>
+          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 23.10.23
+DEL.N1LN3L.DN.F.GPL.DMP : last exported on 23.10.23
+DEL.N1LN3L.DN.F.GTR.DMP : last exported on 23.10.23
+DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 23.10.23
+DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 23.10.23
+DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 23.10.23
+DEL.N1LK61.DN.F.CPD.DMP : last exported on 23.10.23
+DEL.N1LN0R.DN.F.CPL.DMP : last exported on 23.10.23
+DEL.KT6E35.SN.F.GGO.ZIP : last exported on 23.10.23
+DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 23.10.23</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
@@ -1120,31 +1120,31 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 18.10.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 19.10.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 19.10.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 19.10.23
-DIT.E35KT6.WI.ZIP : last exported on 19.10.23
-DEL.K2PKT6.WI.ZIP : last exported on 19.10.23
-DEL.R7AKT6.WI.ZIP : last exported on 20.10.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 20.10.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 20.10.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 20.10.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 21.10.23
+DIT.E35KT6.WI.ZIP : last exported on 20.10.23
+DEL.K2PKT6.WI.ZIP : last exported on 21.10.23
+DEL.R7AKT6.WI.ZIP : last exported on 21.10.23
 DEL.N5FKT6.WI.ZIP : last exported on 12.10.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 19.10.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 19.10.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 19.10.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 19.10.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 19.10.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 19.10.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 19.10.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 19.10.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 19.10.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 19.10.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 19.10.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 19.10.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 19.10.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 22.10.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 22.10.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 23.10.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 22.10.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 22.10.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 22.10.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 22.10.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 22.10.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 22.10.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 22.10.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 22.10.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 22.10.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 22.10.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1247,30 +1247,30 @@
       </c>
       <c r="C10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 12.09.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 20.10.23
+          <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 21.10.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 23.10.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 16.10.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 19.10.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 19.10.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 19.10.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 19.10.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 19.10.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 19.10.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 19.10.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 19.10.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 19.10.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 19.10.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 19.10.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 19.10.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 19.10.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 19.10.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 19.10.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 19.10.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 19.10.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 22.10.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 22.10.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 22.10.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 22.10.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 22.10.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 22.10.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 22.10.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 22.10.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 22.10.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 22.10.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 22.10.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 22.10.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 22.10.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 22.10.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 22.10.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 22.10.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 22.10.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1331,18 +1331,18 @@
       </c>
       <c r="C12" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.MANDANTN.TXT : last exported on 05.10.23</t>
+          <t>DEL.N3LKT6.MANDANTN.TXT : last exported on 21.10.23</t>
         </is>
       </c>
       <c r="D12" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 05.10.23
-DEL.N1LN3L.MC.F.GPL.DMP : last exported on 05.10.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 19.10.23
-DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 05.10.23
-DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 05.10.23
-DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 05.10.23
-DGI.KT6R11.MANDANT.TXT : last exported on 05.10.23</t>
+          <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 21.10.23
+DEL.N1LN3L.MC.F.GPL.DMP : last exported on 21.10.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 22.10.23
+DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 21.10.23
+DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 21.10.23
+DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 21.10.23
+DGI.KT6R11.MANDANT.TXT : last exported on 21.10.23</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 19.10.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 20.10.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 19.10.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 21.10.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1406,20 +1406,20 @@
           <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 07.08.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
 DLV.I5XKT6.AU.A.ZIP : last exported on 05.07.23
-DLV.R31KT6.AU.C.ZIP : last exported on 18.10.23</t>
+DLV.R31KT6.AU.C.ZIP : last exported on 20.10.23</t>
         </is>
       </c>
       <c r="D14" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 18.10.23
-DEL.N1LN3L.AU.D.GPL.DMP : last exported on 18.10.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 19.10.23
-DEL.KT6N5M.AU.GGO.ZIP : last exported on 18.10.23
-DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 18.10.23
-DEL.KT6KTZ.AU.GGO.ZIP : last exported on 18.10.23
-DEL.KT6KTZ.AU.IMG.GGO.ZIP : last exported on 18.10.23
-DEL.KT6E35.AU.GGO.ZIP : last exported on 18.10.23
-DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 18.10.23</t>
+          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 20.10.23
+DEL.N1LN3L.AU.D.GPL.DMP : last exported on 20.10.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 22.10.23
+DEL.KT6N5M.AU.GGO.ZIP : last exported on 20.10.23
+DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 20.10.23
+DEL.KT6KTZ.AU.GGO.ZIP : last exported on 20.10.23
+DEL.KT6KTZ.AU.IMG.GGO.ZIP : last exported on 20.10.23
+DEL.KT6E35.AU.GGO.ZIP : last exported on 20.10.23
+DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 20.10.23</t>
         </is>
       </c>
       <c r="E14" s="11" t="inlineStr">
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 19.10.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 19.10.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 22.10.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 22.10.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 19.10.23
-DHP.KUDKT6.ORGUNITS : last exported on 20.10.23
-DHS.R11KT6.HSB02ALL : last exported on 19.10.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 22.10.23
+DHP.KUDKT6.ORGUNITS : last exported on 23.10.23
+DHS.R11KT6.HSB02ALL : last exported on 20.10.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 19.10.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 19.10.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 19.10.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 19.10.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 19.10.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 19.10.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 19.10.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 19.10.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 19.10.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 19.10.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 20.10.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 20.10.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 22.10.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 20.10.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 20.10.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 20.10.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 20.10.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 20.10.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 20.10.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 20.10.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1620,7 +1620,7 @@
       </c>
       <c r="D19" s="16" t="inlineStr">
         <is>
-          <t>DEL.N1LE35.TRANS.ZIP : last exported on 15.10.23</t>
+          <t>DEL.N1LE35.TRANS.ZIP : last exported on 22.10.23</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 19.10.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 21.10.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 19.10.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 19.10.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 19.10.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 19.10.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 19.10.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 19.10.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 19.10.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 19.10.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 19.10.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 19.10.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 19.10.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 19.10.23
-DEL.N1LKT6.MT.??????.G : last exported on 19.10.23
-DEL.N1LKT6.MT.??????.U : last exported on 19.10.23
-DEL.N1LKT6.MT.??????.AS : last exported on 19.10.23
-DVL.N1LN5X.VLM.DSP : last exported on 19.10.23
-DVL.N1LN5X.VLM.WT : last exported on 19.10.23
-DDS.N1LR11.DSP : last exported on 19.10.23
-DDS.N1LR11.WT : last exported on 19.10.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 19.10.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 19.10.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 19.10.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 19.10.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 19.10.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 19.10.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 19.10.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 19.10.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 19.10.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 19.10.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 19.10.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 21.10.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 21.10.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 22.10.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 21.10.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 21.10.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 21.10.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 21.10.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 21.10.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 21.10.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 21.10.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 21.10.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 21.10.23
+DEL.N1LKT6.MT.??????.G : last exported on 21.10.23
+DEL.N1LKT6.MT.??????.U : last exported on 21.10.23
+DEL.N1LKT6.MT.??????.AS : last exported on 21.10.23
+DVL.N1LN5X.VLM.DSP : last exported on 21.10.23
+DVL.N1LN5X.VLM.WT : last exported on 21.10.23
+DDS.N1LR11.DSP : last exported on 21.10.23
+DDS.N1LR11.WT : last exported on 21.10.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 21.10.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 21.10.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 21.10.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 21.10.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 21.10.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 21.10.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 21.10.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 21.10.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 21.10.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 21.10.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 21.10.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,22 +1710,22 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 20.10.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 20.10.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 23.10.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 23.10.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 19.10.23
-DEL.N1LN3L.EM.F.GPL.DMP : last exported on 19.10.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 19.10.23
-DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 19.10.23
-DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 19.10.23
-DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 19.10.23
-DEL.N1LK61.EM.F.CPD.DMP : last exported on 19.10.23
-DEL.N1LN0R.EM.F.CPL.DMP : last exported on 19.10.23
-DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 19.10.23
-DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 19.10.23</t>
+          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 22.10.23
+DEL.N1LN3L.EM.F.GPL.DMP : last exported on 22.10.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 22.10.23
+DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 22.10.23
+DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 22.10.23
+DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 22.10.23
+DEL.N1LK61.EM.F.CPD.DMP : last exported on 22.10.23
+DEL.N1LN0R.EM.F.CPL.DMP : last exported on 22.10.23
+DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 22.10.23
+DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 22.10.23</t>
         </is>
       </c>
       <c r="E21" s="11" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 20.10.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 20.10.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 20.10.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 20.10.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 20.10.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 20.10.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 20.10.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 20.10.23
-DDC.R11KT6.ELFI.MD.TXT : last exported on 15.10.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 19.10.23
-DDC.R11KT6.ELFI.PK.TXT : last exported on 15.10.23
-DDC.R11KT6.ELFI.PR.TXT : last exported on 15.10.23</t>
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 23.10.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 23.10.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 23.10.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 23.10.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 23.10.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 23.10.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 23.10.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 23.10.23
+DDC.R11KT6.ELFI.MD.TXT : last exported on 22.10.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 20.10.23
+DDC.R11KT6.ELFI.PK.TXT : last exported on 22.10.23
+DDC.R11KT6.ELFI.PR.TXT : last exported on 22.10.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 19.10.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 19.10.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 19.10.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 19.10.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 19.10.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 19.10.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 19.10.23
-DEL.N1LKT6.EC.??????.G : last exported on 19.10.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 19.10.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 19.10.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 19.10.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 19.10.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 19.10.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 19.10.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 19.10.23
-DEL.N1LKT6.EC.??????.U : last exported on 19.10.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 19.10.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 19.10.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 19.10.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 19.10.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 19.10.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 19.10.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 19.10.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 19.10.23
-DEL.N1LKT6.EC.??????.AS : last exported on 19.10.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 19.10.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 19.10.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 19.10.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 19.10.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 19.10.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 19.10.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 19.10.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 19.10.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 22.10.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 22.10.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 22.10.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 22.10.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 22.10.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 22.10.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 22.10.23
+DEL.N1LKT6.EC.??????.G : last exported on 22.10.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 22.10.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 22.10.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 22.10.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 22.10.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 22.10.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 22.10.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 22.10.23
+DEL.N1LKT6.EC.??????.U : last exported on 22.10.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 22.10.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 22.10.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 22.10.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 22.10.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 22.10.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 22.10.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 22.10.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 22.10.23
+DEL.N1LKT6.EC.??????.AS : last exported on 22.10.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 22.10.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 22.10.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 22.10.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 22.10.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 22.10.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 22.10.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 22.10.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 22.10.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 24.10.23 11:46
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 23.10.2023</t>
+          <t>Date - 24.10.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 20.10.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 23.10.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 21.10.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 21.10.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 22.10.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 21.10.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 21.10.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 21.10.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 21.10.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 21.10.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 21.10.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 21.10.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 21.10.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 21.10.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 21.10.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 21.10.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 24.10.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 24.10.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 24.10.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 24.10.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 24.10.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 24.10.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 24.10.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 24.10.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 24.10.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 24.10.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 24.10.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 24.10.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 24.10.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 24.10.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1120,12 +1120,12 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 20.10.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 20.10.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 20.10.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 23.10.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 23.10.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 23.10.23
 DLV.I5XKT6.WI.A.ZIP : last exported on 21.10.23
-DIT.E35KT6.WI.ZIP : last exported on 20.10.23
-DEL.K2PKT6.WI.ZIP : last exported on 21.10.23
+DIT.E35KT6.WI.ZIP : last exported on 23.10.23
+DEL.K2PKT6.WI.ZIP : last exported on 23.10.23
 DEL.R7AKT6.WI.ZIP : last exported on 21.10.23
 DEL.N5FKT6.WI.ZIP : last exported on 12.10.23</t>
         </is>
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 21.10.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 23.10.23
-DGV.N3LKT6.EPELS.??????.ZIP : last exported on 16.10.23</t>
+DEL.N3LKT6.HST.??????.ZIP : last exported on 24.10.23
+DGV.N3LKT6.EPELS.??????.ZIP : last exported on 23.10.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 22.10.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 22.10.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 22.10.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 22.10.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 22.10.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 22.10.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 22.10.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 22.10.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 22.10.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 22.10.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 22.10.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 22.10.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 22.10.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 22.10.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 22.10.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 22.10.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 22.10.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 23.10.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 23.10.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 23.10.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 23.10.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 23.10.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 23.10.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 23.10.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 23.10.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 23.10.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 23.10.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 23.10.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 23.10.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 23.10.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 23.10.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 23.10.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 23.10.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 23.10.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1298,12 +1298,12 @@
       </c>
       <c r="C11" s="14" t="inlineStr">
         <is>
-          <t>DEL.KT6KT6.APOSPRO.ZIP : last exported on 16.10.23</t>
+          <t>DEL.KT6KT6.APOSPRO.ZIP : last exported on 23.10.23</t>
         </is>
       </c>
       <c r="D11" s="15" t="inlineStr">
         <is>
-          <t>DEL.KT6N2O.XTIME.ZIP : last exported on 16.10.23</t>
+          <t>DEL.KT6N2O.XTIME.ZIP : last exported on 23.10.23</t>
         </is>
       </c>
       <c r="E11" s="11" t="inlineStr">
@@ -1338,7 +1338,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 21.10.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 21.10.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 22.10.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 23.10.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 21.10.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 21.10.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 21.10.23
@@ -1370,7 +1370,7 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 20.10.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 23.10.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
@@ -1406,20 +1406,20 @@
           <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 07.08.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
 DLV.I5XKT6.AU.A.ZIP : last exported on 05.07.23
-DLV.R31KT6.AU.C.ZIP : last exported on 20.10.23</t>
+DLV.R31KT6.AU.C.ZIP : last exported on 23.10.23</t>
         </is>
       </c>
       <c r="D14" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 20.10.23
-DEL.N1LN3L.AU.D.GPL.DMP : last exported on 20.10.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 22.10.23
-DEL.KT6N5M.AU.GGO.ZIP : last exported on 20.10.23
-DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 20.10.23
-DEL.KT6KTZ.AU.GGO.ZIP : last exported on 20.10.23
-DEL.KT6KTZ.AU.IMG.GGO.ZIP : last exported on 20.10.23
-DEL.KT6E35.AU.GGO.ZIP : last exported on 20.10.23
-DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 20.10.23</t>
+          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.10.23
+DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.10.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 23.10.23
+DEL.KT6N5M.AU.GGO.ZIP : last exported on 23.10.23
+DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 23.10.23
+DEL.KT6KTZ.AU.GGO.ZIP : last exported on 23.10.23
+DEL.KT6KTZ.AU.IMG.GGO.ZIP : last exported on 23.10.23
+DEL.KT6E35.AU.GGO.ZIP : last exported on 23.10.23
+DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 23.10.23</t>
         </is>
       </c>
       <c r="E14" s="11" t="inlineStr">
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 22.10.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 22.10.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 23.10.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 23.10.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 22.10.23
-DHP.KUDKT6.ORGUNITS : last exported on 23.10.23
-DHS.R11KT6.HSB02ALL : last exported on 20.10.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 23.10.23
+DHP.KUDKT6.ORGUNITS : last exported on 24.10.23
+DHS.R11KT6.HSB02ALL : last exported on 23.10.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 20.10.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 20.10.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 22.10.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 20.10.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 20.10.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 20.10.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 20.10.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 20.10.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 20.10.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 20.10.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 23.10.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 23.10.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 23.10.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 23.10.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 23.10.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 23.10.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 23.10.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 23.10.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 23.10.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 23.10.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 21.10.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 23.10.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 21.10.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 21.10.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 22.10.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 21.10.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 21.10.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 21.10.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 21.10.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 21.10.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 21.10.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 21.10.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 21.10.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 21.10.23
-DEL.N1LKT6.MT.??????.G : last exported on 21.10.23
-DEL.N1LKT6.MT.??????.U : last exported on 21.10.23
-DEL.N1LKT6.MT.??????.AS : last exported on 21.10.23
-DVL.N1LN5X.VLM.DSP : last exported on 21.10.23
-DVL.N1LN5X.VLM.WT : last exported on 21.10.23
-DDS.N1LR11.DSP : last exported on 21.10.23
-DDS.N1LR11.WT : last exported on 21.10.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 21.10.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 21.10.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 21.10.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 21.10.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 21.10.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 21.10.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 21.10.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 21.10.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 21.10.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 21.10.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 21.10.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 23.10.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 23.10.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 23.10.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 23.10.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 23.10.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 23.10.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 23.10.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 23.10.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 23.10.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 23.10.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 23.10.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 23.10.23
+DEL.N1LKT6.MT.??????.G : last exported on 23.10.23
+DEL.N1LKT6.MT.??????.U : last exported on 23.10.23
+DEL.N1LKT6.MT.??????.AS : last exported on 23.10.23
+DVL.N1LN5X.VLM.DSP : last exported on 23.10.23
+DVL.N1LN5X.VLM.WT : last exported on 23.10.23
+DDS.N1LR11.DSP : last exported on 23.10.23
+DDS.N1LR11.WT : last exported on 23.10.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 23.10.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 23.10.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 23.10.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 23.10.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 23.10.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 23.10.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 23.10.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 23.10.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 23.10.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 23.10.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 23.10.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,22 +1710,22 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 23.10.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 23.10.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 24.10.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 24.10.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 22.10.23
-DEL.N1LN3L.EM.F.GPL.DMP : last exported on 22.10.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 22.10.23
-DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 22.10.23
-DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 22.10.23
-DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 22.10.23
-DEL.N1LK61.EM.F.CPD.DMP : last exported on 22.10.23
-DEL.N1LN0R.EM.F.CPL.DMP : last exported on 22.10.23
-DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 22.10.23
-DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 22.10.23</t>
+          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 23.10.23
+DEL.N1LN3L.EM.F.GPL.DMP : last exported on 23.10.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 23.10.23
+DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 23.10.23
+DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 23.10.23
+DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 23.10.23
+DEL.N1LK61.EM.F.CPD.DMP : last exported on 23.10.23
+DEL.N1LN0R.EM.F.CPL.DMP : last exported on 23.10.23
+DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 23.10.23
+DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 23.10.23</t>
         </is>
       </c>
       <c r="E21" s="11" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 23.10.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 23.10.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 23.10.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 23.10.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 23.10.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 23.10.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 23.10.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 23.10.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 24.10.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 24.10.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 24.10.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 24.10.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 24.10.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 24.10.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 24.10.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 24.10.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 22.10.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 20.10.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 23.10.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 22.10.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 22.10.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 22.10.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 22.10.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 22.10.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 22.10.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 22.10.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 22.10.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 22.10.23
-DEL.N1LKT6.EC.??????.G : last exported on 22.10.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 22.10.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 22.10.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 22.10.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 22.10.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 22.10.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 22.10.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 22.10.23
-DEL.N1LKT6.EC.??????.U : last exported on 22.10.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 22.10.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 22.10.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 22.10.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 22.10.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 22.10.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 22.10.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 22.10.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 22.10.23
-DEL.N1LKT6.EC.??????.AS : last exported on 22.10.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 22.10.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 22.10.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 22.10.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 22.10.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 22.10.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 22.10.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 22.10.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 22.10.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 23.10.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 23.10.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 23.10.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 23.10.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 23.10.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 23.10.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 23.10.23
+DEL.N1LKT6.EC.??????.G : last exported on 23.10.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 23.10.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 23.10.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 23.10.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 23.10.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 23.10.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 23.10.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 23.10.23
+DEL.N1LKT6.EC.??????.U : last exported on 23.10.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 23.10.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 23.10.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 23.10.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 23.10.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 23.10.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 23.10.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 23.10.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 23.10.23
+DEL.N1LKT6.EC.??????.AS : last exported on 23.10.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 23.10.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 23.10.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 23.10.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 23.10.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 23.10.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 23.10.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 23.10.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 23.10.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 25.10.23 13:54
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 24.10.2023</t>
+          <t>Date - 25.10.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 23.10.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 24.10.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 24.10.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 24.10.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 24.10.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 24.10.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 24.10.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 24.10.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 24.10.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 24.10.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 24.10.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 24.10.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 24.10.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 24.10.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 24.10.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 24.10.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 25.10.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 25.10.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 25.10.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 25.10.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 25.10.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 25.10.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 25.10.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 25.10.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 25.10.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 25.10.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 25.10.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 25.10.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 25.10.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 25.10.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1121,30 +1121,30 @@
       <c r="C7" s="10" t="inlineStr">
         <is>
           <t>DLV.R31KT6.WI.C.ZIP : last exported on 23.10.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 23.10.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 23.10.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 21.10.23
-DIT.E35KT6.WI.ZIP : last exported on 23.10.23
-DEL.K2PKT6.WI.ZIP : last exported on 23.10.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 24.10.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 24.10.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 24.10.23
+DIT.E35KT6.WI.ZIP : last exported on 24.10.23
+DEL.K2PKT6.WI.ZIP : last exported on 24.10.23
 DEL.R7AKT6.WI.ZIP : last exported on 21.10.23
 DEL.N5FKT6.WI.ZIP : last exported on 12.10.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 22.10.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 22.10.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 23.10.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 22.10.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 22.10.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 22.10.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 22.10.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 22.10.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 22.10.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 22.10.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 22.10.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 22.10.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 22.10.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 24.10.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 24.10.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 24.10.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 24.10.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 24.10.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 24.10.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 24.10.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 24.10.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 24.10.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 24.10.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 24.10.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 24.10.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 24.10.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 21.10.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 24.10.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 25.10.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 23.10.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 23.10.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 23.10.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 23.10.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 23.10.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 23.10.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 23.10.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 23.10.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 23.10.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 23.10.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 23.10.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 23.10.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 23.10.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 23.10.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 23.10.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 23.10.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 23.10.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 23.10.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 24.10.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 24.10.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 24.10.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 24.10.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 24.10.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 24.10.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 24.10.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 24.10.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 24.10.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 24.10.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 24.10.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 24.10.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 24.10.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 24.10.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 24.10.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 24.10.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 24.10.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1338,7 +1338,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 21.10.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 21.10.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 23.10.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 24.10.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 21.10.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 21.10.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 21.10.23
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 23.10.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 24.10.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 21.10.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 24.10.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1406,20 +1406,20 @@
           <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 07.08.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
 DLV.I5XKT6.AU.A.ZIP : last exported on 05.07.23
-DLV.R31KT6.AU.C.ZIP : last exported on 23.10.23</t>
+DLV.R31KT6.AU.C.ZIP : last exported on 24.10.23</t>
         </is>
       </c>
       <c r="D14" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.10.23
-DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.10.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 23.10.23
-DEL.KT6N5M.AU.GGO.ZIP : last exported on 23.10.23
-DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 23.10.23
-DEL.KT6KTZ.AU.GGO.ZIP : last exported on 23.10.23
-DEL.KT6KTZ.AU.IMG.GGO.ZIP : last exported on 23.10.23
-DEL.KT6E35.AU.GGO.ZIP : last exported on 23.10.23
-DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 23.10.23</t>
+          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 24.10.23
+DEL.N1LN3L.AU.D.GPL.DMP : last exported on 24.10.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 24.10.23
+DEL.KT6N5M.AU.GGO.ZIP : last exported on 24.10.23
+DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 24.10.23
+DEL.KT6KTZ.AU.GGO.ZIP : last exported on 24.10.23
+DEL.KT6KTZ.AU.IMG.GGO.ZIP : last exported on 24.10.23
+DEL.KT6E35.AU.GGO.ZIP : last exported on 24.10.23
+DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 24.10.23</t>
         </is>
       </c>
       <c r="E14" s="11" t="inlineStr">
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 23.10.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 23.10.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 24.10.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 24.10.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 23.10.23
-DHP.KUDKT6.ORGUNITS : last exported on 24.10.23
-DHS.R11KT6.HSB02ALL : last exported on 23.10.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 24.10.23
+DHP.KUDKT6.ORGUNITS : last exported on 25.10.23
+DHS.R11KT6.HSB02ALL : last exported on 24.10.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 23.10.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 23.10.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 23.10.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 23.10.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 23.10.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 23.10.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 23.10.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 23.10.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 23.10.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 23.10.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 24.10.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 24.10.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 24.10.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 24.10.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 24.10.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 24.10.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 24.10.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 24.10.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 24.10.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 24.10.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 23.10.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 24.10.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 23.10.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 23.10.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 23.10.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 23.10.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 23.10.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 23.10.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 23.10.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 23.10.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 23.10.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 23.10.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 23.10.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 23.10.23
-DEL.N1LKT6.MT.??????.G : last exported on 23.10.23
-DEL.N1LKT6.MT.??????.U : last exported on 23.10.23
-DEL.N1LKT6.MT.??????.AS : last exported on 23.10.23
-DVL.N1LN5X.VLM.DSP : last exported on 23.10.23
-DVL.N1LN5X.VLM.WT : last exported on 23.10.23
-DDS.N1LR11.DSP : last exported on 23.10.23
-DDS.N1LR11.WT : last exported on 23.10.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 23.10.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 23.10.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 23.10.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 23.10.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 23.10.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 23.10.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 23.10.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 23.10.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 23.10.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 23.10.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 23.10.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 24.10.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 24.10.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 24.10.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 24.10.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 24.10.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 24.10.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 24.10.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 24.10.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 24.10.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 24.10.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 24.10.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 24.10.23
+DEL.N1LKT6.MT.??????.G : last exported on 24.10.23
+DEL.N1LKT6.MT.??????.U : last exported on 24.10.23
+DEL.N1LKT6.MT.??????.AS : last exported on 24.10.23
+DVL.N1LN5X.VLM.DSP : last exported on 24.10.23
+DVL.N1LN5X.VLM.WT : last exported on 24.10.23
+DDS.N1LR11.DSP : last exported on 24.10.23
+DDS.N1LR11.WT : last exported on 24.10.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 24.10.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 24.10.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 24.10.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 24.10.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 24.10.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 24.10.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 24.10.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 24.10.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 24.10.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 24.10.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 24.10.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,22 +1710,22 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 24.10.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 24.10.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 25.10.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 25.10.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 23.10.23
-DEL.N1LN3L.EM.F.GPL.DMP : last exported on 23.10.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 23.10.23
-DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 23.10.23
-DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 23.10.23
-DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 23.10.23
-DEL.N1LK61.EM.F.CPD.DMP : last exported on 23.10.23
-DEL.N1LN0R.EM.F.CPL.DMP : last exported on 23.10.23
-DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 23.10.23
-DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 23.10.23</t>
+          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 24.10.23
+DEL.N1LN3L.EM.F.GPL.DMP : last exported on 24.10.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 24.10.23
+DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 24.10.23
+DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 24.10.23
+DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 24.10.23
+DEL.N1LK61.EM.F.CPD.DMP : last exported on 24.10.23
+DEL.N1LN0R.EM.F.CPL.DMP : last exported on 24.10.23
+DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 24.10.23
+DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 24.10.23</t>
         </is>
       </c>
       <c r="E21" s="11" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 24.10.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 24.10.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 24.10.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 24.10.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 24.10.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 24.10.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 24.10.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 24.10.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 25.10.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 25.10.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 25.10.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 25.10.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 25.10.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 25.10.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 25.10.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 25.10.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 22.10.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 23.10.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 24.10.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 22.10.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 22.10.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 23.10.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 23.10.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 23.10.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 23.10.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 23.10.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 23.10.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 23.10.23
-DEL.N1LKT6.EC.??????.G : last exported on 23.10.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 23.10.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 23.10.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 23.10.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 23.10.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 23.10.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 23.10.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 23.10.23
-DEL.N1LKT6.EC.??????.U : last exported on 23.10.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 23.10.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 23.10.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 23.10.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 23.10.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 23.10.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 23.10.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 23.10.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 23.10.23
-DEL.N1LKT6.EC.??????.AS : last exported on 23.10.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 23.10.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 23.10.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 23.10.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 23.10.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 23.10.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 23.10.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 23.10.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 23.10.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 24.10.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 24.10.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 24.10.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 24.10.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 24.10.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 24.10.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 24.10.23
+DEL.N1LKT6.EC.??????.G : last exported on 24.10.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 24.10.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 24.10.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 24.10.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 24.10.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 24.10.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 24.10.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 24.10.23
+DEL.N1LKT6.EC.??????.U : last exported on 24.10.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 24.10.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 24.10.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 24.10.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 24.10.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 24.10.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 24.10.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 24.10.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 24.10.23
+DEL.N1LKT6.EC.??????.AS : last exported on 24.10.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 24.10.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 24.10.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 24.10.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 24.10.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 24.10.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 24.10.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 24.10.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 24.10.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 26.10.23 15:21
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 25.10.2023</t>
+          <t>Date - 26.10.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 24.10.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 25.10.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 25.10.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 25.10.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 25.10.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 25.10.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 25.10.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 25.10.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 25.10.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 25.10.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 25.10.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 25.10.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 25.10.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 25.10.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 25.10.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 25.10.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 26.10.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 26.10.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 26.10.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 26.10.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 26.10.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 26.10.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 26.10.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 26.10.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 26.10.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 26.10.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 26.10.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 26.10.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 26.10.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 26.10.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1121,30 +1121,30 @@
       <c r="C7" s="10" t="inlineStr">
         <is>
           <t>DLV.R31KT6.WI.C.ZIP : last exported on 23.10.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 24.10.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 24.10.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 24.10.23
-DIT.E35KT6.WI.ZIP : last exported on 24.10.23
-DEL.K2PKT6.WI.ZIP : last exported on 24.10.23
-DEL.R7AKT6.WI.ZIP : last exported on 21.10.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 25.10.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 25.10.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 25.10.23
+DIT.E35KT6.WI.ZIP : last exported on 25.10.23
+DEL.K2PKT6.WI.ZIP : last exported on 25.10.23
+DEL.R7AKT6.WI.ZIP : last exported on 26.10.23
 DEL.N5FKT6.WI.ZIP : last exported on 12.10.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 24.10.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 24.10.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 24.10.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 24.10.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 24.10.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 24.10.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 24.10.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 24.10.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 24.10.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 24.10.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 24.10.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 24.10.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 24.10.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 26.10.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 26.10.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 26.10.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 26.10.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 26.10.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 26.10.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 26.10.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 26.10.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 26.10.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 26.10.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 25.10.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 26.10.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 26.10.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1207,15 +1207,15 @@
       </c>
       <c r="C9" s="10" t="inlineStr">
         <is>
-          <t>ElsaPro-GUI_&lt;language&gt;.xml : last exported on 25.02.23</t>
+          <t>ElsaPro-GUI_&lt;language&gt;.xml : last exported on 25.10.23</t>
         </is>
       </c>
       <c r="D9" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TRANS.F.GPD.DMP : last exported on 25.02.23
-DEL.N1LN3L.TRANS.F.GPL.DMP : last exported on 25.02.23
+          <t>DEL.N1LN3L.TRANS.F.GPD.DMP : last exported on 25.10.23
+DEL.N1LN3L.TRANS.F.GPL.DMP : last exported on 25.10.23
 DEL.N1LN3L.TRANS.F.GTR.DMP : last exported on 25.02.23
-DEL.N1LKQQ.TRANS.F.UPD.DMP : last exported on 25.02.23
+DEL.N1LKQQ.TRANS.F.UPD.DMP : last exported on 25.10.23
 DEL.N1LN3L.TRANS.F.ASPD.DMP : last exported on 25.02.23
 DEL.N1LN3L.TRANS.F.ASPL.DMP : last exported on 25.02.23
 DEL.N1LK61.TRANS.D.CPD.DMP : last exported on 25.02.23
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 21.10.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 25.10.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 26.10.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 23.10.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 24.10.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 24.10.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 24.10.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 24.10.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 24.10.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 24.10.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 24.10.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 24.10.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 24.10.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 24.10.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 24.10.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 24.10.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 24.10.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 24.10.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 24.10.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 24.10.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 24.10.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 25.10.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 25.10.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 25.10.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 25.10.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 25.10.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 25.10.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 25.10.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 25.10.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 25.10.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 25.10.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 25.10.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 25.10.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 25.10.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 25.10.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 25.10.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 25.10.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 25.10.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1338,7 +1338,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 21.10.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 21.10.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 24.10.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 25.10.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 21.10.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 21.10.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 21.10.23
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 24.10.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 25.10.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 24.10.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 25.10.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1406,20 +1406,20 @@
           <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 07.08.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
 DLV.I5XKT6.AU.A.ZIP : last exported on 05.07.23
-DLV.R31KT6.AU.C.ZIP : last exported on 24.10.23</t>
+DLV.R31KT6.AU.C.ZIP : last exported on 25.10.23</t>
         </is>
       </c>
       <c r="D14" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 24.10.23
-DEL.N1LN3L.AU.D.GPL.DMP : last exported on 24.10.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 24.10.23
-DEL.KT6N5M.AU.GGO.ZIP : last exported on 24.10.23
-DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 24.10.23
-DEL.KT6KTZ.AU.GGO.ZIP : last exported on 24.10.23
-DEL.KT6KTZ.AU.IMG.GGO.ZIP : last exported on 24.10.23
-DEL.KT6E35.AU.GGO.ZIP : last exported on 24.10.23
-DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 24.10.23</t>
+          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 25.10.23
+DEL.N1LN3L.AU.D.GPL.DMP : last exported on 25.10.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 25.10.23
+DEL.KT6N5M.AU.GGO.ZIP : last exported on 25.10.23
+DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 25.10.23
+DEL.KT6KTZ.AU.GGO.ZIP : last exported on 25.10.23
+DEL.KT6KTZ.AU.IMG.GGO.ZIP : last exported on 25.10.23
+DEL.KT6E35.AU.GGO.ZIP : last exported on 25.10.23
+DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 25.10.23</t>
         </is>
       </c>
       <c r="E14" s="11" t="inlineStr">
@@ -1457,24 +1457,24 @@
 DGQ.R11KT6.BSITX.TXT : last exported on 04.10.23
 DGQ.R31KT6.BSIVMC.TXT : last exported on 10.10.23
 DGQ.R31KT6.PKATC.TXT : last exported on 10.10.23
-DEL.KMPKT6.APOS.DATA.ZIP : last exported on 18.10.23</t>
+DEL.KMPKT6.APOS.DATA.ZIP : last exported on 25.10.23</t>
         </is>
       </c>
       <c r="D15" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 18.10.23
-DEL.N1LN3L.AP.F.GPL.DMP : last exported on 18.10.23
-DEL.N1LN3L.AP.F.GTR.DMP : last exported on 18.10.23
-DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 18.10.23
-DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 18.10.23
-DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 18.10.23
-DEL.N1LK61.AP.F.CPD.DMP : last exported on 18.10.23
-DEL.N1LN0R.AP.F.CPL.DMP : last exported on 18.10.23
-DEL.N1LR31.AP.F.PPS.DMP : last exported on 18.10.23
-DEL.KT6E35.AP.F.DB.ZIP : last exported on 18.10.23
-DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 18.10.23
-DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 18.10.23
-DVL.KT6N5X.VLM.AP.ZIP : last exported on 18.10.23</t>
+          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 25.10.23
+DEL.N1LN3L.AP.F.GPL.DMP : last exported on 25.10.23
+DEL.N1LN3L.AP.F.GTR.DMP : last exported on 25.10.23
+DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 25.10.23
+DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 25.10.23
+DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 25.10.23
+DEL.N1LK61.AP.F.CPD.DMP : last exported on 25.10.23
+DEL.N1LN0R.AP.F.CPL.DMP : last exported on 25.10.23
+DEL.N1LR31.AP.F.PPS.DMP : last exported on 25.10.23
+DEL.KT6E35.AP.F.DB.ZIP : last exported on 25.10.23
+DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 25.10.23
+DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 25.10.23
+DVL.KT6N5X.VLM.AP.ZIP : last exported on 25.10.23</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 24.10.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 24.10.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 25.10.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 25.10.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 24.10.23
-DHP.KUDKT6.ORGUNITS : last exported on 25.10.23
-DHS.R11KT6.HSB02ALL : last exported on 24.10.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 26.10.23
+DHP.KUDKT6.ORGUNITS : last exported on 26.10.23
+DHS.R11KT6.HSB02ALL : last exported on 25.10.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 24.10.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 24.10.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 24.10.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 24.10.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 24.10.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 24.10.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 24.10.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 24.10.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 24.10.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 24.10.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 25.10.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 25.10.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 25.10.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 25.10.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 25.10.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 25.10.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 25.10.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 25.10.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 25.10.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 25.10.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 24.10.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 25.10.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 24.10.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 24.10.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 24.10.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 24.10.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 24.10.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 24.10.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 24.10.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 24.10.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 24.10.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 24.10.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 24.10.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 24.10.23
-DEL.N1LKT6.MT.??????.G : last exported on 24.10.23
-DEL.N1LKT6.MT.??????.U : last exported on 24.10.23
-DEL.N1LKT6.MT.??????.AS : last exported on 24.10.23
-DVL.N1LN5X.VLM.DSP : last exported on 24.10.23
-DVL.N1LN5X.VLM.WT : last exported on 24.10.23
-DDS.N1LR11.DSP : last exported on 24.10.23
-DDS.N1LR11.WT : last exported on 24.10.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 24.10.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 24.10.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 24.10.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 24.10.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 24.10.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 24.10.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 24.10.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 24.10.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 24.10.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 24.10.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 24.10.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 25.10.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 25.10.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 25.10.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 25.10.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 25.10.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 25.10.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 25.10.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 25.10.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 25.10.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 25.10.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 25.10.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 25.10.23
+DEL.N1LKT6.MT.??????.G : last exported on 25.10.23
+DEL.N1LKT6.MT.??????.U : last exported on 25.10.23
+DEL.N1LKT6.MT.??????.AS : last exported on 25.10.23
+DVL.N1LN5X.VLM.DSP : last exported on 25.10.23
+DVL.N1LN5X.VLM.WT : last exported on 25.10.23
+DDS.N1LR11.DSP : last exported on 25.10.23
+DDS.N1LR11.WT : last exported on 25.10.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 25.10.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 25.10.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 25.10.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 25.10.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 25.10.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 25.10.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 25.10.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 25.10.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 25.10.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 25.10.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 25.10.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,22 +1710,22 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 25.10.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 25.10.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 26.10.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 26.10.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 24.10.23
-DEL.N1LN3L.EM.F.GPL.DMP : last exported on 24.10.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 24.10.23
-DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 24.10.23
-DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 24.10.23
-DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 24.10.23
-DEL.N1LK61.EM.F.CPD.DMP : last exported on 24.10.23
-DEL.N1LN0R.EM.F.CPL.DMP : last exported on 24.10.23
-DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 24.10.23
-DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 24.10.23</t>
+          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 25.10.23
+DEL.N1LN3L.EM.F.GPL.DMP : last exported on 25.10.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 25.10.23
+DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 25.10.23
+DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 25.10.23
+DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 25.10.23
+DEL.N1LK61.EM.F.CPD.DMP : last exported on 25.10.23
+DEL.N1LN0R.EM.F.CPL.DMP : last exported on 25.10.23
+DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 25.10.23
+DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 25.10.23</t>
         </is>
       </c>
       <c r="E21" s="11" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 25.10.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 25.10.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 25.10.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 25.10.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 25.10.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 25.10.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 25.10.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 25.10.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 26.10.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 26.10.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 26.10.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 26.10.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 26.10.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 26.10.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 26.10.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 26.10.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 22.10.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 24.10.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 25.10.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 22.10.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 22.10.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 24.10.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 24.10.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 24.10.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 24.10.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 24.10.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 24.10.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 24.10.23
-DEL.N1LKT6.EC.??????.G : last exported on 24.10.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 24.10.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 24.10.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 24.10.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 24.10.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 24.10.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 24.10.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 24.10.23
-DEL.N1LKT6.EC.??????.U : last exported on 24.10.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 24.10.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 24.10.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 24.10.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 24.10.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 24.10.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 24.10.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 24.10.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 24.10.23
-DEL.N1LKT6.EC.??????.AS : last exported on 24.10.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 24.10.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 24.10.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 24.10.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 24.10.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 24.10.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 24.10.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 24.10.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 24.10.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 25.10.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 25.10.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 25.10.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 25.10.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 25.10.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 25.10.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 25.10.23
+DEL.N1LKT6.EC.??????.G : last exported on 25.10.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 25.10.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 25.10.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 25.10.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 25.10.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 25.10.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 25.10.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 25.10.23
+DEL.N1LKT6.EC.??????.U : last exported on 25.10.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 25.10.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 25.10.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 25.10.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 25.10.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 25.10.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 25.10.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 25.10.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 25.10.23
+DEL.N1LKT6.EC.??????.AS : last exported on 25.10.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 25.10.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 25.10.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 25.10.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 25.10.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 25.10.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 25.10.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 25.10.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 25.10.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 30.10.23 12:23
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 26.10.2023</t>
+          <t>Date - 30.10.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 25.10.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 27.10.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 26.10.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 26.10.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 26.10.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 26.10.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 26.10.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 26.10.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 26.10.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 26.10.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 26.10.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 26.10.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 26.10.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 26.10.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 26.10.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 26.10.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 27.10.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 27.10.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 29.10.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 27.10.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 27.10.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 27.10.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 27.10.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 27.10.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 27.10.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 27.10.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 27.10.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 27.10.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 27.10.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 27.10.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1077,22 +1077,22 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 23.10.23
-DEH.N3LKT6.AP.COMPL.SNK : last exported on 23.10.23</t>
+          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 30.10.23
+DEH.N3LKT6.AP.COMPL.SNK : last exported on 30.10.23</t>
         </is>
       </c>
       <c r="D6" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 23.10.23
-DEL.N1LN3L.DN.F.GPL.DMP : last exported on 23.10.23
-DEL.N1LN3L.DN.F.GTR.DMP : last exported on 23.10.23
-DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 23.10.23
-DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 23.10.23
-DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 23.10.23
-DEL.N1LK61.DN.F.CPD.DMP : last exported on 23.10.23
-DEL.N1LN0R.DN.F.CPL.DMP : last exported on 23.10.23
-DEL.KT6E35.SN.F.GGO.ZIP : last exported on 23.10.23
-DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 23.10.23</t>
+          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 30.10.23
+DEL.N1LN3L.DN.F.GPL.DMP : last exported on 30.10.23
+DEL.N1LN3L.DN.F.GTR.DMP : last exported on 30.10.23
+DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 30.10.23
+DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 30.10.23
+DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 30.10.23
+DEL.N1LK61.DN.F.CPD.DMP : last exported on 30.10.23
+DEL.N1LN0R.DN.F.CPL.DMP : last exported on 30.10.23
+DEL.KT6E35.SN.F.GGO.ZIP : last exported on 30.10.23
+DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 30.10.23</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
@@ -1121,30 +1121,30 @@
       <c r="C7" s="10" t="inlineStr">
         <is>
           <t>DLV.R31KT6.WI.C.ZIP : last exported on 23.10.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 25.10.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 25.10.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 25.10.23
-DIT.E35KT6.WI.ZIP : last exported on 25.10.23
-DEL.K2PKT6.WI.ZIP : last exported on 25.10.23
-DEL.R7AKT6.WI.ZIP : last exported on 26.10.23
-DEL.N5FKT6.WI.ZIP : last exported on 12.10.23</t>
+DLV.KZ6KT6.WI.V.ZIP : last exported on 27.10.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 27.10.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 29.10.23
+DIT.E35KT6.WI.ZIP : last exported on 27.10.23
+DEL.K2PKT6.WI.ZIP : last exported on 29.10.23
+DEL.R7AKT6.WI.ZIP : last exported on 30.10.23
+DEL.N5FKT6.WI.ZIP : last exported on 27.10.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 26.10.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 26.10.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 26.10.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 26.10.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 26.10.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 26.10.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 26.10.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 26.10.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 26.10.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 26.10.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 25.10.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 26.10.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 26.10.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 29.10.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 29.10.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 29.10.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 29.10.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 29.10.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 29.10.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 29.10.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 29.10.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 29.10.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 29.10.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 29.10.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 29.10.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 29.10.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 21.10.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 26.10.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 30.10.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 23.10.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 25.10.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 25.10.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 25.10.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 25.10.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 25.10.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 25.10.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 25.10.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 25.10.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 25.10.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 25.10.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 25.10.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 25.10.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 25.10.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 25.10.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 25.10.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 25.10.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 25.10.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 29.10.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 29.10.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 29.10.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 29.10.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 29.10.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 29.10.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 29.10.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 29.10.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 29.10.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 29.10.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 29.10.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 29.10.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 29.10.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 29.10.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 29.10.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 29.10.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 29.10.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1331,18 +1331,18 @@
       </c>
       <c r="C12" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.MANDANTN.TXT : last exported on 21.10.23</t>
+          <t>DEL.N3LKT6.MANDANTN.TXT : last exported on 28.10.23</t>
         </is>
       </c>
       <c r="D12" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 21.10.23
-DEL.N1LN3L.MC.F.GPL.DMP : last exported on 21.10.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 25.10.23
-DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 21.10.23
-DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 21.10.23
-DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 21.10.23
-DGI.KT6R11.MANDANT.TXT : last exported on 21.10.23</t>
+          <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 28.10.23
+DEL.N1LN3L.MC.F.GPL.DMP : last exported on 28.10.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 29.10.23
+DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 28.10.23
+DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 28.10.23
+DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 28.10.23
+DGI.KT6R11.MANDANT.TXT : last exported on 28.10.23</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 25.10.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 27.10.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 25.10.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 28.10.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1405,21 +1405,21 @@
         <is>
           <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 07.08.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
-DLV.I5XKT6.AU.A.ZIP : last exported on 05.07.23
-DLV.R31KT6.AU.C.ZIP : last exported on 25.10.23</t>
+DLV.I5XKT6.AU.A.ZIP : last exported on 26.10.23
+DLV.R31KT6.AU.C.ZIP : last exported on 26.10.23</t>
         </is>
       </c>
       <c r="D14" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 25.10.23
-DEL.N1LN3L.AU.D.GPL.DMP : last exported on 25.10.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 25.10.23
-DEL.KT6N5M.AU.GGO.ZIP : last exported on 25.10.23
-DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 25.10.23
-DEL.KT6KTZ.AU.GGO.ZIP : last exported on 25.10.23
-DEL.KT6KTZ.AU.IMG.GGO.ZIP : last exported on 25.10.23
-DEL.KT6E35.AU.GGO.ZIP : last exported on 25.10.23
-DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 25.10.23</t>
+          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 27.10.23
+DEL.N1LN3L.AU.D.GPL.DMP : last exported on 27.10.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 29.10.23
+DEL.KT6N5M.AU.GGO.ZIP : last exported on 27.10.23
+DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 27.10.23
+DEL.KT6KTZ.AU.GGO.ZIP : last exported on 27.10.23
+DEL.KT6KTZ.AU.IMG.GGO.ZIP : last exported on 27.10.23
+DEL.KT6E35.AU.GGO.ZIP : last exported on 27.10.23
+DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 27.10.23</t>
         </is>
       </c>
       <c r="E14" s="11" t="inlineStr">
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 25.10.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 25.10.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 29.10.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 29.10.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 26.10.23
-DHP.KUDKT6.ORGUNITS : last exported on 26.10.23
-DHS.R11KT6.HSB02ALL : last exported on 25.10.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 29.10.23
+DHP.KUDKT6.ORGUNITS : last exported on 30.10.23
+DHS.R11KT6.HSB02ALL : last exported on 27.10.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 25.10.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 25.10.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 25.10.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 25.10.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 25.10.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 25.10.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 25.10.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 25.10.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 25.10.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 25.10.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 27.10.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 27.10.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 29.10.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 27.10.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 27.10.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 27.10.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 27.10.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 27.10.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 27.10.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 27.10.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1620,7 +1620,7 @@
       </c>
       <c r="D19" s="16" t="inlineStr">
         <is>
-          <t>DEL.N1LE35.TRANS.ZIP : last exported on 22.10.23</t>
+          <t>DEL.N1LE35.TRANS.ZIP : last exported on 29.10.23</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 25.10.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 28.10.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 25.10.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 25.10.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 25.10.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 25.10.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 25.10.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 25.10.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 25.10.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 25.10.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 25.10.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 25.10.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 25.10.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 25.10.23
-DEL.N1LKT6.MT.??????.G : last exported on 25.10.23
-DEL.N1LKT6.MT.??????.U : last exported on 25.10.23
-DEL.N1LKT6.MT.??????.AS : last exported on 25.10.23
-DVL.N1LN5X.VLM.DSP : last exported on 25.10.23
-DVL.N1LN5X.VLM.WT : last exported on 25.10.23
-DDS.N1LR11.DSP : last exported on 25.10.23
-DDS.N1LR11.WT : last exported on 25.10.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 25.10.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 25.10.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 25.10.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 25.10.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 25.10.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 25.10.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 25.10.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 25.10.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 25.10.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 25.10.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 25.10.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 28.10.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 28.10.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 29.10.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 28.10.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 28.10.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 28.10.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 28.10.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 28.10.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 28.10.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 28.10.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 28.10.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 28.10.23
+DEL.N1LKT6.MT.??????.G : last exported on 28.10.23
+DEL.N1LKT6.MT.??????.U : last exported on 28.10.23
+DEL.N1LKT6.MT.??????.AS : last exported on 28.10.23
+DVL.N1LN5X.VLM.DSP : last exported on 28.10.23
+DVL.N1LN5X.VLM.WT : last exported on 28.10.23
+DDS.N1LR11.DSP : last exported on 28.10.23
+DDS.N1LR11.WT : last exported on 28.10.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 28.10.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 28.10.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 28.10.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 28.10.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 28.10.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 28.10.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 28.10.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 28.10.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 28.10.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 28.10.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 28.10.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,22 +1710,22 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 26.10.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 26.10.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 30.10.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 30.10.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 25.10.23
-DEL.N1LN3L.EM.F.GPL.DMP : last exported on 25.10.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 25.10.23
-DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 25.10.23
-DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 25.10.23
-DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 25.10.23
-DEL.N1LK61.EM.F.CPD.DMP : last exported on 25.10.23
-DEL.N1LN0R.EM.F.CPL.DMP : last exported on 25.10.23
-DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 25.10.23
-DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 25.10.23</t>
+          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 29.10.23
+DEL.N1LN3L.EM.F.GPL.DMP : last exported on 29.10.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 29.10.23
+DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 29.10.23
+DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 29.10.23
+DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 29.10.23
+DEL.N1LK61.EM.F.CPD.DMP : last exported on 29.10.23
+DEL.N1LN0R.EM.F.CPL.DMP : last exported on 29.10.23
+DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 29.10.23
+DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 29.10.23</t>
         </is>
       </c>
       <c r="E21" s="11" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 26.10.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 26.10.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 26.10.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 26.10.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 26.10.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 26.10.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 26.10.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 26.10.23
-DDC.R11KT6.ELFI.MD.TXT : last exported on 22.10.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 25.10.23
-DDC.R11KT6.ELFI.PK.TXT : last exported on 22.10.23
-DDC.R11KT6.ELFI.PR.TXT : last exported on 22.10.23</t>
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 30.10.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 30.10.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 30.10.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 30.10.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 30.10.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 30.10.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 30.10.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 30.10.23
+DDC.R11KT6.ELFI.MD.TXT : last exported on 29.10.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 27.10.23
+DDC.R11KT6.ELFI.PK.TXT : last exported on 29.10.23
+DDC.R11KT6.ELFI.PR.TXT : last exported on 29.10.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 25.10.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 25.10.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 25.10.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 25.10.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 25.10.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 25.10.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 25.10.23
-DEL.N1LKT6.EC.??????.G : last exported on 25.10.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 25.10.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 25.10.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 25.10.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 25.10.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 25.10.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 25.10.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 25.10.23
-DEL.N1LKT6.EC.??????.U : last exported on 25.10.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 25.10.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 25.10.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 25.10.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 25.10.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 25.10.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 25.10.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 25.10.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 25.10.23
-DEL.N1LKT6.EC.??????.AS : last exported on 25.10.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 25.10.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 25.10.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 25.10.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 25.10.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 25.10.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 25.10.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 25.10.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 25.10.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 29.10.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 29.10.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 29.10.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 29.10.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 29.10.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 29.10.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 29.10.23
+DEL.N1LKT6.EC.??????.G : last exported on 29.10.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 29.10.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 29.10.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 29.10.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 29.10.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 29.10.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 29.10.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 29.10.23
+DEL.N1LKT6.EC.??????.U : last exported on 29.10.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 29.10.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 29.10.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 29.10.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 29.10.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 29.10.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 29.10.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 29.10.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 29.10.23
+DEL.N1LKT6.EC.??????.AS : last exported on 29.10.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 29.10.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 29.10.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 29.10.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 29.10.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 29.10.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 29.10.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 29.10.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 29.10.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 31.10.23 12:07
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 30.10.2023</t>
+          <t>Date - 31.10.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 27.10.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 30.10.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 27.10.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 27.10.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 29.10.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 27.10.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 27.10.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 27.10.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 27.10.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 27.10.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 27.10.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 27.10.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 27.10.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 27.10.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 27.10.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 27.10.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 31.10.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 31.10.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 31.10.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 31.10.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 31.10.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 31.10.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 31.10.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 31.10.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 31.10.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 31.10.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 31.10.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 31.10.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 31.10.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 31.10.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1122,29 +1122,29 @@
         <is>
           <t>DLV.R31KT6.WI.C.ZIP : last exported on 23.10.23
 DLV.KZ6KT6.WI.V.ZIP : last exported on 27.10.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 27.10.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 29.10.23
-DIT.E35KT6.WI.ZIP : last exported on 27.10.23
-DEL.K2PKT6.WI.ZIP : last exported on 29.10.23
-DEL.R7AKT6.WI.ZIP : last exported on 30.10.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 30.10.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 30.10.23
+DIT.E35KT6.WI.ZIP : last exported on 30.10.23
+DEL.K2PKT6.WI.ZIP : last exported on 30.10.23
+DEL.R7AKT6.WI.ZIP : last exported on 31.10.23
 DEL.N5FKT6.WI.ZIP : last exported on 27.10.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 29.10.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 29.10.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 29.10.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 29.10.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 29.10.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 29.10.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 29.10.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 29.10.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 29.10.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 29.10.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 29.10.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 29.10.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 29.10.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 30.10.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 30.10.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 30.10.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 30.10.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 30.10.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 30.10.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 30.10.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 30.10.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 30.10.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 30.10.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 30.10.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 30.10.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 30.10.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 21.10.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 30.10.23
-DGV.N3LKT6.EPELS.??????.ZIP : last exported on 23.10.23</t>
+DEL.N3LKT6.HST.??????.ZIP : last exported on 31.10.23
+DGV.N3LKT6.EPELS.??????.ZIP : last exported on 30.10.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 29.10.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 29.10.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 29.10.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 29.10.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 29.10.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 29.10.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 29.10.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 29.10.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 29.10.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 29.10.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 29.10.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 29.10.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 29.10.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 29.10.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 29.10.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 29.10.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 29.10.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 30.10.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 30.10.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 30.10.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 30.10.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 30.10.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 30.10.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 30.10.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 30.10.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 30.10.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 30.10.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 30.10.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 30.10.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 30.10.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 30.10.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 30.10.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 30.10.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 30.10.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1298,12 +1298,12 @@
       </c>
       <c r="C11" s="14" t="inlineStr">
         <is>
-          <t>DEL.KT6KT6.APOSPRO.ZIP : last exported on 23.10.23</t>
+          <t>DEL.KT6KT6.APOSPRO.ZIP : last exported on 30.10.23</t>
         </is>
       </c>
       <c r="D11" s="15" t="inlineStr">
         <is>
-          <t>DEL.KT6N2O.XTIME.ZIP : last exported on 23.10.23</t>
+          <t>DEL.KT6N2O.XTIME.ZIP : last exported on 30.10.23</t>
         </is>
       </c>
       <c r="E11" s="11" t="inlineStr">
@@ -1338,7 +1338,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 28.10.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 28.10.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 29.10.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 30.10.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 28.10.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 28.10.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 28.10.23
@@ -1370,7 +1370,7 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 27.10.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 30.10.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
@@ -1413,7 +1413,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 27.10.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 27.10.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 29.10.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 30.10.23
 DEL.KT6N5M.AU.GGO.ZIP : last exported on 27.10.23
 DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 27.10.23
 DEL.KT6KTZ.AU.GGO.ZIP : last exported on 27.10.23
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 29.10.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 29.10.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 30.10.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 30.10.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 29.10.23
-DHP.KUDKT6.ORGUNITS : last exported on 30.10.23
-DHS.R11KT6.HSB02ALL : last exported on 27.10.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 30.10.23
+DHP.KUDKT6.ORGUNITS : last exported on 31.10.23
+DHS.R11KT6.HSB02ALL : last exported on 30.10.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 27.10.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 27.10.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 29.10.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 27.10.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 27.10.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 27.10.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 27.10.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 27.10.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 27.10.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 27.10.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 30.10.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 30.10.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 30.10.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 30.10.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 30.10.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 30.10.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 30.10.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 30.10.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 30.10.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 30.10.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 28.10.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 30.10.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 28.10.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 28.10.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 29.10.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 28.10.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 28.10.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 28.10.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 28.10.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 28.10.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 28.10.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 28.10.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 28.10.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 28.10.23
-DEL.N1LKT6.MT.??????.G : last exported on 28.10.23
-DEL.N1LKT6.MT.??????.U : last exported on 28.10.23
-DEL.N1LKT6.MT.??????.AS : last exported on 28.10.23
-DVL.N1LN5X.VLM.DSP : last exported on 28.10.23
-DVL.N1LN5X.VLM.WT : last exported on 28.10.23
-DDS.N1LR11.DSP : last exported on 28.10.23
-DDS.N1LR11.WT : last exported on 28.10.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 28.10.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 28.10.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 28.10.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 28.10.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 28.10.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 28.10.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 28.10.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 28.10.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 28.10.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 28.10.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 28.10.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 30.10.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 30.10.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 30.10.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 30.10.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 30.10.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 30.10.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 30.10.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 30.10.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 30.10.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 30.10.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 30.10.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 30.10.23
+DEL.N1LKT6.MT.??????.G : last exported on 30.10.23
+DEL.N1LKT6.MT.??????.U : last exported on 30.10.23
+DEL.N1LKT6.MT.??????.AS : last exported on 30.10.23
+DVL.N1LN5X.VLM.DSP : last exported on 30.10.23
+DVL.N1LN5X.VLM.WT : last exported on 30.10.23
+DDS.N1LR11.DSP : last exported on 30.10.23
+DDS.N1LR11.WT : last exported on 30.10.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 30.10.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 30.10.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 30.10.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 30.10.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 30.10.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 30.10.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 30.10.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 30.10.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 30.10.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 30.10.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 30.10.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,22 +1710,22 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 30.10.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 30.10.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 31.10.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 31.10.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 29.10.23
-DEL.N1LN3L.EM.F.GPL.DMP : last exported on 29.10.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 29.10.23
-DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 29.10.23
-DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 29.10.23
-DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 29.10.23
-DEL.N1LK61.EM.F.CPD.DMP : last exported on 29.10.23
-DEL.N1LN0R.EM.F.CPL.DMP : last exported on 29.10.23
-DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 29.10.23
-DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 29.10.23</t>
+          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 30.10.23
+DEL.N1LN3L.EM.F.GPL.DMP : last exported on 30.10.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 30.10.23
+DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 30.10.23
+DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 30.10.23
+DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 30.10.23
+DEL.N1LK61.EM.F.CPD.DMP : last exported on 30.10.23
+DEL.N1LN0R.EM.F.CPL.DMP : last exported on 30.10.23
+DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 30.10.23
+DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 30.10.23</t>
         </is>
       </c>
       <c r="E21" s="11" t="inlineStr">
@@ -1762,46 +1762,46 @@
 DKG.R11KT6.L520.P.EDCP.TGE : last exported on 30.10.23
 DKG.R11KT6.L520.P.EDCP.TMO : last exported on 30.10.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 29.10.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 27.10.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 30.10.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 29.10.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 29.10.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 29.10.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 29.10.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 29.10.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 29.10.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 29.10.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 29.10.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 29.10.23
-DEL.N1LKT6.EC.??????.G : last exported on 29.10.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 29.10.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 29.10.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 29.10.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 29.10.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 29.10.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 29.10.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 29.10.23
-DEL.N1LKT6.EC.??????.U : last exported on 29.10.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 29.10.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 29.10.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 29.10.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 29.10.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 29.10.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 29.10.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 29.10.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 29.10.23
-DEL.N1LKT6.EC.??????.AS : last exported on 29.10.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 29.10.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 29.10.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 29.10.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 29.10.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 29.10.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 29.10.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 29.10.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 29.10.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 30.10.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 30.10.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 30.10.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 30.10.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 30.10.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 30.10.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 30.10.23
+DEL.N1LKT6.EC.??????.G : last exported on 30.10.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 30.10.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 30.10.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 30.10.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 30.10.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 30.10.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 30.10.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 30.10.23
+DEL.N1LKT6.EC.??????.U : last exported on 30.10.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 30.10.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 30.10.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 30.10.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 30.10.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 30.10.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 30.10.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 30.10.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 30.10.23
+DEL.N1LKT6.EC.??????.AS : last exported on 30.10.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 30.10.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 30.10.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 30.10.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 30.10.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 30.10.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 30.10.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 30.10.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 30.10.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 01.11.23 12:19
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 31.10.2023</t>
+          <t>Date - 01.11.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 30.10.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 31.10.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 31.10.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 31.10.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 31.10.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 31.10.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 31.10.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 31.10.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 31.10.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 31.10.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 31.10.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 31.10.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 31.10.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 31.10.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 31.10.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 31.10.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 01.11.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 01.11.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 01.11.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 01.11.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 01.11.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 01.11.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 01.11.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 01.11.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 01.11.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 01.11.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 01.11.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 01.11.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 01.11.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 01.11.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1120,31 +1120,31 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 23.10.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 31.10.23
 DLV.KZ6KT6.WI.V.ZIP : last exported on 27.10.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 30.10.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 30.10.23
-DIT.E35KT6.WI.ZIP : last exported on 30.10.23
-DEL.K2PKT6.WI.ZIP : last exported on 30.10.23
-DEL.R7AKT6.WI.ZIP : last exported on 31.10.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 31.10.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 31.10.23
+DIT.E35KT6.WI.ZIP : last exported on 31.10.23
+DEL.K2PKT6.WI.ZIP : last exported on 31.10.23
+DEL.R7AKT6.WI.ZIP : last exported on 01.11.23
 DEL.N5FKT6.WI.ZIP : last exported on 27.10.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 30.10.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 30.10.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 30.10.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 30.10.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 30.10.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 30.10.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 30.10.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 30.10.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 30.10.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 30.10.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 30.10.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 30.10.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 30.10.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 31.10.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 31.10.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 31.10.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 31.10.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 31.10.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 31.10.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 31.10.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 31.10.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 31.10.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 31.10.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 31.10.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 31.10.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 31.10.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 21.10.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 31.10.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 01.11.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 30.10.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 30.10.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 30.10.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 30.10.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 30.10.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 30.10.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 30.10.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 30.10.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 30.10.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 30.10.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 30.10.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 30.10.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 30.10.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 30.10.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 30.10.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 30.10.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 30.10.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 30.10.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 31.10.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 31.10.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 31.10.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 31.10.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 31.10.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 31.10.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 31.10.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 31.10.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 31.10.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 31.10.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 31.10.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 31.10.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 31.10.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 31.10.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 31.10.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 31.10.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 31.10.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1338,7 +1338,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 28.10.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 28.10.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 30.10.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 31.10.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 28.10.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 28.10.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 28.10.23
@@ -1375,7 +1375,7 @@
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 28.10.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 31.10.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1413,7 +1413,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 27.10.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 27.10.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 30.10.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 31.10.23
 DEL.KT6N5M.AU.GGO.ZIP : last exported on 27.10.23
 DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 27.10.23
 DEL.KT6KTZ.AU.GGO.ZIP : last exported on 27.10.23
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 30.10.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 30.10.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 31.10.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 31.10.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 30.10.23
-DHP.KUDKT6.ORGUNITS : last exported on 31.10.23
-DHS.R11KT6.HSB02ALL : last exported on 30.10.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 31.10.23
+DHP.KUDKT6.ORGUNITS : last exported on 01.11.23
+DHS.R11KT6.HSB02ALL : last exported on 31.10.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 30.10.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 30.10.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 30.10.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 30.10.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 30.10.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 30.10.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 30.10.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 30.10.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 30.10.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 30.10.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 31.10.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 31.10.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 31.10.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 31.10.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 31.10.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 31.10.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 31.10.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 31.10.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 31.10.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 31.10.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 30.10.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 31.10.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 30.10.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 30.10.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 30.10.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 30.10.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 30.10.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 30.10.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 30.10.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 30.10.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 30.10.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 30.10.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 30.10.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 30.10.23
-DEL.N1LKT6.MT.??????.G : last exported on 30.10.23
-DEL.N1LKT6.MT.??????.U : last exported on 30.10.23
-DEL.N1LKT6.MT.??????.AS : last exported on 30.10.23
-DVL.N1LN5X.VLM.DSP : last exported on 30.10.23
-DVL.N1LN5X.VLM.WT : last exported on 30.10.23
-DDS.N1LR11.DSP : last exported on 30.10.23
-DDS.N1LR11.WT : last exported on 30.10.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 30.10.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 30.10.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 30.10.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 30.10.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 30.10.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 30.10.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 30.10.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 30.10.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 30.10.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 30.10.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 30.10.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 31.10.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 31.10.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 31.10.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 31.10.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 31.10.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 31.10.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 31.10.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 31.10.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 31.10.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 31.10.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 31.10.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 31.10.23
+DEL.N1LKT6.MT.??????.G : last exported on 31.10.23
+DEL.N1LKT6.MT.??????.U : last exported on 31.10.23
+DEL.N1LKT6.MT.??????.AS : last exported on 31.10.23
+DVL.N1LN5X.VLM.DSP : last exported on 31.10.23
+DVL.N1LN5X.VLM.WT : last exported on 31.10.23
+DDS.N1LR11.DSP : last exported on 31.10.23
+DDS.N1LR11.WT : last exported on 31.10.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 31.10.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 31.10.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 31.10.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 31.10.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 31.10.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 31.10.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 31.10.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 31.10.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 31.10.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 31.10.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 31.10.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,22 +1710,22 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 31.10.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 31.10.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 01.11.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 01.11.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 30.10.23
-DEL.N1LN3L.EM.F.GPL.DMP : last exported on 30.10.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 30.10.23
-DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 30.10.23
-DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 30.10.23
-DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 30.10.23
-DEL.N1LK61.EM.F.CPD.DMP : last exported on 30.10.23
-DEL.N1LN0R.EM.F.CPL.DMP : last exported on 30.10.23
-DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 30.10.23
-DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 30.10.23</t>
+          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 31.10.23
+DEL.N1LN3L.EM.F.GPL.DMP : last exported on 31.10.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 31.10.23
+DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 31.10.23
+DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 31.10.23
+DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 31.10.23
+DEL.N1LK61.EM.F.CPD.DMP : last exported on 31.10.23
+DEL.N1LN0R.EM.F.CPL.DMP : last exported on 31.10.23
+DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 31.10.23
+DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 31.10.23</t>
         </is>
       </c>
       <c r="E21" s="11" t="inlineStr">
@@ -1753,14 +1753,14 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 30.10.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 30.10.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 30.10.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 30.10.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 30.10.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 30.10.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 30.10.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 30.10.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 01.11.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 01.11.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 01.11.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 01.11.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 01.11.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 01.11.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 01.11.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 01.11.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 29.10.23
 DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 30.10.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 29.10.23
@@ -1769,39 +1769,39 @@
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 30.10.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 30.10.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 30.10.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 30.10.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 30.10.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 30.10.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 30.10.23
-DEL.N1LKT6.EC.??????.G : last exported on 30.10.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 30.10.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 30.10.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 30.10.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 30.10.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 30.10.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 30.10.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 30.10.23
-DEL.N1LKT6.EC.??????.U : last exported on 30.10.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 30.10.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 30.10.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 30.10.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 30.10.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 30.10.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 30.10.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 30.10.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 30.10.23
-DEL.N1LKT6.EC.??????.AS : last exported on 30.10.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 30.10.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 30.10.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 30.10.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 30.10.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 30.10.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 30.10.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 30.10.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 30.10.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 31.10.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 31.10.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 31.10.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 31.10.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 31.10.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 31.10.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 31.10.23
+DEL.N1LKT6.EC.??????.G : last exported on 31.10.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 31.10.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 31.10.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 31.10.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 31.10.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 31.10.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 31.10.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 31.10.23
+DEL.N1LKT6.EC.??????.U : last exported on 31.10.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 31.10.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 31.10.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 31.10.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 31.10.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 31.10.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 31.10.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 31.10.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 31.10.23
+DEL.N1LKT6.EC.??????.AS : last exported on 31.10.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 31.10.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 31.10.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 31.10.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 31.10.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 31.10.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 31.10.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 31.10.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 31.10.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 02.11.23 13:19
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 01.11.2023</t>
+          <t>Date - 02.11.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 31.10.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 01.11.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 01.11.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 01.11.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 01.11.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 01.11.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 01.11.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 01.11.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 01.11.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 01.11.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 01.11.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 01.11.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 01.11.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 01.11.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 01.11.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 01.11.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 02.11.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 02.11.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 02.11.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 02.11.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 02.11.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 02.11.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 02.11.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 02.11.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 02.11.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 02.11.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 02.11.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 02.11.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 02.11.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 02.11.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1121,30 +1121,30 @@
       <c r="C7" s="10" t="inlineStr">
         <is>
           <t>DLV.R31KT6.WI.C.ZIP : last exported on 31.10.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 27.10.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 01.11.23
 DLV.RPKKT6.WI.S.ZIP : last exported on 31.10.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 31.10.23
-DIT.E35KT6.WI.ZIP : last exported on 31.10.23
-DEL.K2PKT6.WI.ZIP : last exported on 31.10.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 01.11.23
+DIT.E35KT6.WI.ZIP : last exported on 01.11.23
+DEL.K2PKT6.WI.ZIP : last exported on 01.11.23
 DEL.R7AKT6.WI.ZIP : last exported on 01.11.23
 DEL.N5FKT6.WI.ZIP : last exported on 27.10.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 31.10.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 31.10.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 31.10.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 31.10.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 31.10.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 31.10.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 31.10.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 31.10.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 31.10.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 31.10.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 31.10.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 31.10.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 31.10.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 01.11.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 01.11.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 01.11.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 01.11.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 01.11.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 01.11.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 01.11.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 01.11.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 01.11.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 01.11.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 01.11.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 01.11.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 01.11.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 21.10.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 01.11.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 02.11.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 30.10.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 31.10.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 31.10.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 31.10.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 31.10.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 31.10.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 31.10.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 31.10.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 31.10.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 31.10.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 31.10.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 31.10.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 31.10.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 31.10.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 31.10.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 31.10.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 31.10.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 31.10.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 01.11.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 01.11.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 01.11.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 01.11.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 01.11.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 01.11.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 01.11.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 01.11.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 01.11.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 01.11.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 01.11.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 01.11.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 01.11.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 01.11.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 01.11.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 01.11.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 01.11.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1338,7 +1338,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 28.10.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 28.10.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 31.10.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 01.11.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 28.10.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 28.10.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 28.10.23
@@ -1370,7 +1370,7 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 30.10.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 01.11.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
@@ -1413,7 +1413,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 27.10.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 27.10.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 31.10.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 01.11.23
 DEL.KT6N5M.AU.GGO.ZIP : last exported on 27.10.23
 DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 27.10.23
 DEL.KT6KTZ.AU.GGO.ZIP : last exported on 27.10.23
@@ -1447,34 +1447,34 @@
       </c>
       <c r="C15" s="10" t="inlineStr">
         <is>
-          <t>DGQ.R11KT6.BSIVM.TXT : last exported on 04.10.23
-DGQ.R11KT6.BSIVM.C.TXT : last exported on 04.10.23
-DGQ.R11KT6.BSIVM.US2.TXT : last exported on 04.10.23
-DGQ.R11KT6.PKAT.TXT : last exported on 04.10.23
-DGQ.R11KT6.PKAT.C.TXT : last exported on 04.10.23
-DGQ.R11KT6.PKAT.US2.TXT : last exported on 04.10.23
-DGQ.R11KT6.BSITK.TXT : last exported on 04.10.23
-DGQ.R11KT6.BSITX.TXT : last exported on 04.10.23
+          <t>DGQ.R11KT6.BSIVM.TXT : last exported on 01.11.23
+DGQ.R11KT6.BSIVM.C.TXT : last exported on 01.11.23
+DGQ.R11KT6.BSIVM.US2.TXT : last exported on 01.11.23
+DGQ.R11KT6.PKAT.TXT : last exported on 01.11.23
+DGQ.R11KT6.PKAT.C.TXT : last exported on 01.11.23
+DGQ.R11KT6.PKAT.US2.TXT : last exported on 01.11.23
+DGQ.R11KT6.BSITK.TXT : last exported on 01.11.23
+DGQ.R11KT6.BSITX.TXT : last exported on 01.11.23
 DGQ.R31KT6.BSIVMC.TXT : last exported on 10.10.23
 DGQ.R31KT6.PKATC.TXT : last exported on 10.10.23
-DEL.KMPKT6.APOS.DATA.ZIP : last exported on 25.10.23</t>
+DEL.KMPKT6.APOS.DATA.ZIP : last exported on 01.11.23</t>
         </is>
       </c>
       <c r="D15" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 25.10.23
-DEL.N1LN3L.AP.F.GPL.DMP : last exported on 25.10.23
-DEL.N1LN3L.AP.F.GTR.DMP : last exported on 25.10.23
-DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 25.10.23
-DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 25.10.23
-DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 25.10.23
-DEL.N1LK61.AP.F.CPD.DMP : last exported on 25.10.23
-DEL.N1LN0R.AP.F.CPL.DMP : last exported on 25.10.23
-DEL.N1LR31.AP.F.PPS.DMP : last exported on 25.10.23
-DEL.KT6E35.AP.F.DB.ZIP : last exported on 25.10.23
-DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 25.10.23
-DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 25.10.23
-DVL.KT6N5X.VLM.AP.ZIP : last exported on 25.10.23</t>
+          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 01.11.23
+DEL.N1LN3L.AP.F.GPL.DMP : last exported on 01.11.23
+DEL.N1LN3L.AP.F.GTR.DMP : last exported on 01.11.23
+DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 01.11.23
+DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 01.11.23
+DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 01.11.23
+DEL.N1LK61.AP.F.CPD.DMP : last exported on 01.11.23
+DEL.N1LN0R.AP.F.CPL.DMP : last exported on 01.11.23
+DEL.N1LR31.AP.F.PPS.DMP : last exported on 01.11.23
+DEL.KT6E35.AP.F.DB.ZIP : last exported on 01.11.23
+DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 01.11.23
+DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 01.11.23
+DVL.KT6N5X.VLM.AP.ZIP : last exported on 01.11.23</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 31.10.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 31.10.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 01.11.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 01.11.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 31.10.23
-DHP.KUDKT6.ORGUNITS : last exported on 01.11.23
-DHS.R11KT6.HSB02ALL : last exported on 31.10.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 01.11.23
+DHP.KUDKT6.ORGUNITS : last exported on 02.11.23
+DHS.R11KT6.HSB02ALL : last exported on 01.11.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 31.10.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 31.10.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 31.10.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 31.10.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 31.10.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 31.10.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 31.10.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 31.10.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 31.10.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 31.10.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 01.11.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 01.11.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 01.11.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 01.11.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 01.11.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 01.11.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 01.11.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 01.11.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 01.11.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 01.11.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 31.10.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 01.11.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 31.10.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 31.10.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 31.10.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 31.10.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 31.10.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 31.10.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 31.10.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 31.10.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 31.10.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 31.10.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 31.10.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 31.10.23
-DEL.N1LKT6.MT.??????.G : last exported on 31.10.23
-DEL.N1LKT6.MT.??????.U : last exported on 31.10.23
-DEL.N1LKT6.MT.??????.AS : last exported on 31.10.23
-DVL.N1LN5X.VLM.DSP : last exported on 31.10.23
-DVL.N1LN5X.VLM.WT : last exported on 31.10.23
-DDS.N1LR11.DSP : last exported on 31.10.23
-DDS.N1LR11.WT : last exported on 31.10.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 31.10.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 31.10.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 31.10.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 31.10.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 31.10.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 31.10.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 31.10.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 31.10.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 31.10.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 31.10.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 31.10.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 01.11.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 01.11.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 01.11.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 01.11.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 01.11.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 01.11.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 01.11.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 01.11.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 01.11.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 01.11.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 01.11.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 01.11.23
+DEL.N1LKT6.MT.??????.G : last exported on 01.11.23
+DEL.N1LKT6.MT.??????.U : last exported on 01.11.23
+DEL.N1LKT6.MT.??????.AS : last exported on 01.11.23
+DVL.N1LN5X.VLM.DSP : last exported on 01.11.23
+DVL.N1LN5X.VLM.WT : last exported on 01.11.23
+DDS.N1LR11.DSP : last exported on 01.11.23
+DDS.N1LR11.WT : last exported on 01.11.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 01.11.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 01.11.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 01.11.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 01.11.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 01.11.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 01.11.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 01.11.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 01.11.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 01.11.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 01.11.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 01.11.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,22 +1710,22 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 01.11.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 01.11.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 02.11.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 02.11.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 31.10.23
-DEL.N1LN3L.EM.F.GPL.DMP : last exported on 31.10.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 31.10.23
-DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 31.10.23
-DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 31.10.23
-DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 31.10.23
-DEL.N1LK61.EM.F.CPD.DMP : last exported on 31.10.23
-DEL.N1LN0R.EM.F.CPL.DMP : last exported on 31.10.23
-DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 31.10.23
-DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 31.10.23</t>
+          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 01.11.23
+DEL.N1LN3L.EM.F.GPL.DMP : last exported on 01.11.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 01.11.23
+DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 01.11.23
+DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 01.11.23
+DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 01.11.23
+DEL.N1LK61.EM.F.CPD.DMP : last exported on 01.11.23
+DEL.N1LN0R.EM.F.CPL.DMP : last exported on 01.11.23
+DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 01.11.23
+DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 01.11.23</t>
         </is>
       </c>
       <c r="E21" s="11" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 01.11.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 01.11.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 01.11.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 01.11.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 01.11.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 01.11.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 01.11.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 01.11.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 02.11.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 02.11.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 02.11.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 02.11.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 02.11.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 02.11.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 02.11.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 02.11.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 29.10.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 30.10.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 01.11.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 29.10.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 29.10.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 31.10.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 31.10.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 31.10.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 31.10.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 31.10.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 31.10.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 31.10.23
-DEL.N1LKT6.EC.??????.G : last exported on 31.10.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 31.10.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 31.10.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 31.10.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 31.10.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 31.10.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 31.10.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 31.10.23
-DEL.N1LKT6.EC.??????.U : last exported on 31.10.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 31.10.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 31.10.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 31.10.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 31.10.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 31.10.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 31.10.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 31.10.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 31.10.23
-DEL.N1LKT6.EC.??????.AS : last exported on 31.10.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 31.10.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 31.10.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 31.10.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 31.10.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 31.10.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 31.10.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 31.10.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 31.10.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 01.11.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 01.11.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 01.11.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 01.11.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 01.11.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 01.11.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 01.11.23
+DEL.N1LKT6.EC.??????.G : last exported on 01.11.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 01.11.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 01.11.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 01.11.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 01.11.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 01.11.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 01.11.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 01.11.23
+DEL.N1LKT6.EC.??????.U : last exported on 01.11.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 01.11.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 01.11.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 01.11.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 01.11.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 01.11.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 01.11.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 01.11.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 01.11.23
+DEL.N1LKT6.EC.??????.AS : last exported on 01.11.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 01.11.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 01.11.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 01.11.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 01.11.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 01.11.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 01.11.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 01.11.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 01.11.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 03.11.23 13:07
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 02.11.2023</t>
+          <t>Date - 03.11.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 01.11.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 02.11.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 02.11.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 02.11.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 02.11.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 02.11.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 02.11.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 02.11.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 02.11.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 02.11.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 02.11.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 02.11.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 02.11.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 02.11.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 02.11.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 02.11.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 03.11.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 03.11.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 03.11.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 03.11.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 03.11.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 03.11.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 03.11.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 03.11.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 03.11.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 03.11.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 03.11.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 03.11.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 03.11.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 03.11.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1120,31 +1120,31 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 31.10.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 01.11.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 31.10.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 01.11.23
-DIT.E35KT6.WI.ZIP : last exported on 01.11.23
-DEL.K2PKT6.WI.ZIP : last exported on 01.11.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 02.11.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 02.11.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 02.11.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 02.11.23
+DIT.E35KT6.WI.ZIP : last exported on 02.11.23
+DEL.K2PKT6.WI.ZIP : last exported on 02.11.23
 DEL.R7AKT6.WI.ZIP : last exported on 01.11.23
 DEL.N5FKT6.WI.ZIP : last exported on 27.10.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 01.11.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 01.11.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 01.11.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 01.11.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 01.11.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 01.11.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 01.11.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 01.11.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 01.11.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 01.11.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 01.11.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 01.11.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 01.11.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 02.11.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 02.11.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 02.11.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 02.11.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 02.11.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 02.11.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 02.11.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 02.11.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 02.11.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 02.11.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 02.11.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 02.11.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 02.11.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 21.10.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 02.11.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 03.11.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 30.10.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 01.11.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 01.11.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 01.11.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 01.11.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 01.11.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 01.11.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 01.11.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 01.11.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 01.11.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 01.11.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 01.11.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 01.11.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 01.11.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 01.11.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 01.11.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 01.11.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 01.11.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 02.11.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 02.11.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 02.11.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 02.11.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 02.11.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 02.11.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 02.11.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 02.11.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 02.11.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 02.11.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 02.11.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 02.11.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 02.11.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 02.11.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 02.11.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 02.11.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 02.11.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 01.11.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 02.11.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 31.10.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 02.11.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 01.11.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 01.11.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 02.11.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 02.11.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 01.11.23
-DHP.KUDKT6.ORGUNITS : last exported on 02.11.23
-DHS.R11KT6.HSB02ALL : last exported on 01.11.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 02.11.23
+DHP.KUDKT6.ORGUNITS : last exported on 03.11.23
+DHS.R11KT6.HSB02ALL : last exported on 02.11.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 01.11.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 01.11.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 01.11.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 01.11.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 01.11.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 01.11.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 01.11.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 01.11.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 01.11.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 01.11.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 02.11.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 02.11.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 02.11.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 02.11.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 02.11.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 02.11.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 02.11.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 02.11.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 02.11.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 02.11.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 01.11.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 02.11.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 01.11.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 01.11.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 01.11.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 01.11.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 01.11.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 01.11.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 01.11.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 01.11.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 01.11.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 01.11.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 01.11.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 01.11.23
-DEL.N1LKT6.MT.??????.G : last exported on 01.11.23
-DEL.N1LKT6.MT.??????.U : last exported on 01.11.23
-DEL.N1LKT6.MT.??????.AS : last exported on 01.11.23
-DVL.N1LN5X.VLM.DSP : last exported on 01.11.23
-DVL.N1LN5X.VLM.WT : last exported on 01.11.23
-DDS.N1LR11.DSP : last exported on 01.11.23
-DDS.N1LR11.WT : last exported on 01.11.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 01.11.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 01.11.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 01.11.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 01.11.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 01.11.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 01.11.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 01.11.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 01.11.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 01.11.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 01.11.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 01.11.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 02.11.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 02.11.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 02.11.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 02.11.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 02.11.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 02.11.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 02.11.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 02.11.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 02.11.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 02.11.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 02.11.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 02.11.23
+DEL.N1LKT6.MT.??????.G : last exported on 02.11.23
+DEL.N1LKT6.MT.??????.U : last exported on 02.11.23
+DEL.N1LKT6.MT.??????.AS : last exported on 02.11.23
+DVL.N1LN5X.VLM.DSP : last exported on 02.11.23
+DVL.N1LN5X.VLM.WT : last exported on 02.11.23
+DDS.N1LR11.DSP : last exported on 02.11.23
+DDS.N1LR11.WT : last exported on 02.11.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 02.11.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 02.11.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 02.11.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 02.11.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 02.11.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 02.11.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 02.11.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 02.11.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 02.11.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 02.11.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 02.11.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,22 +1710,22 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 02.11.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 02.11.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 03.11.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 03.11.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 01.11.23
-DEL.N1LN3L.EM.F.GPL.DMP : last exported on 01.11.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 01.11.23
-DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 01.11.23
-DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 01.11.23
-DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 01.11.23
-DEL.N1LK61.EM.F.CPD.DMP : last exported on 01.11.23
-DEL.N1LN0R.EM.F.CPL.DMP : last exported on 01.11.23
-DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 01.11.23
-DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 01.11.23</t>
+          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 02.11.23
+DEL.N1LN3L.EM.F.GPL.DMP : last exported on 02.11.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 02.11.23
+DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 02.11.23
+DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 02.11.23
+DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 02.11.23
+DEL.N1LK61.EM.F.CPD.DMP : last exported on 02.11.23
+DEL.N1LN0R.EM.F.CPL.DMP : last exported on 02.11.23
+DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 02.11.23
+DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 02.11.23</t>
         </is>
       </c>
       <c r="E21" s="11" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 02.11.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 02.11.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 02.11.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 02.11.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 02.11.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 02.11.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 02.11.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 02.11.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 03.11.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 03.11.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 03.11.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 03.11.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 03.11.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 03.11.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 03.11.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 03.11.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 29.10.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 01.11.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 02.11.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 29.10.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 29.10.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 01.11.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 01.11.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 01.11.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 01.11.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 01.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 01.11.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 01.11.23
-DEL.N1LKT6.EC.??????.G : last exported on 01.11.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 01.11.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 01.11.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 01.11.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 01.11.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 01.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 01.11.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 01.11.23
-DEL.N1LKT6.EC.??????.U : last exported on 01.11.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 01.11.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 01.11.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 01.11.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 01.11.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 01.11.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 01.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 01.11.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 01.11.23
-DEL.N1LKT6.EC.??????.AS : last exported on 01.11.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 01.11.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 01.11.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 01.11.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 01.11.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 01.11.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 01.11.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 01.11.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 01.11.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 02.11.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 02.11.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 02.11.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 02.11.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 02.11.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 02.11.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 02.11.23
+DEL.N1LKT6.EC.??????.G : last exported on 02.11.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 02.11.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 02.11.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 02.11.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 02.11.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 02.11.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 02.11.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 02.11.23
+DEL.N1LKT6.EC.??????.U : last exported on 02.11.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 02.11.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 02.11.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 02.11.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 02.11.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 02.11.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 02.11.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 02.11.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 02.11.23
+DEL.N1LKT6.EC.??????.AS : last exported on 02.11.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 02.11.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 02.11.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 02.11.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 02.11.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 02.11.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 02.11.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 02.11.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 02.11.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 06.11.23 16:22
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 03.11.2023</t>
+          <t>Date - 06.11.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 02.11.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 03.11.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 03.11.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 03.11.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 03.11.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 03.11.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 03.11.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 03.11.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 03.11.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 03.11.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 03.11.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 03.11.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 03.11.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 03.11.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 03.11.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 03.11.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 05.11.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 05.11.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 05.11.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 05.11.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 05.11.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 05.11.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 05.11.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 05.11.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 05.11.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 05.11.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 05.11.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 05.11.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 05.11.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 05.11.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1043,13 +1043,13 @@
       </c>
       <c r="C5" s="10" t="inlineStr">
         <is>
-          <t>DGQ.R11KT6.KDNR.TXT : last exported on 06.10.23</t>
+          <t>DGQ.R11KT6.KDNR.TXT : last exported on 03.11.23</t>
         </is>
       </c>
       <c r="D5" s="10" t="inlineStr">
         <is>
-          <t>DDS.N1LR11.KDNRTXT : last exported on 09.10.23
-DVL.N1LN5X.VLM.KDNRTXT : last exported on 09.10.23</t>
+          <t>DDS.N1LR11.KDNRTXT : last exported on 06.11.23
+DVL.N1LN5X.VLM.KDNRTXT : last exported on 06.11.23</t>
         </is>
       </c>
       <c r="E5" s="11" t="inlineStr">
@@ -1077,22 +1077,22 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 30.10.23
-DEH.N3LKT6.AP.COMPL.SNK : last exported on 30.10.23</t>
+          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 06.11.23
+DEH.N3LKT6.AP.COMPL.SNK : last exported on 06.11.23</t>
         </is>
       </c>
       <c r="D6" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 30.10.23
-DEL.N1LN3L.DN.F.GPL.DMP : last exported on 30.10.23
-DEL.N1LN3L.DN.F.GTR.DMP : last exported on 30.10.23
-DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 30.10.23
-DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 30.10.23
-DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 30.10.23
-DEL.N1LK61.DN.F.CPD.DMP : last exported on 30.10.23
-DEL.N1LN0R.DN.F.CPL.DMP : last exported on 30.10.23
-DEL.KT6E35.SN.F.GGO.ZIP : last exported on 30.10.23
-DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 30.10.23</t>
+          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 06.11.23
+DEL.N1LN3L.DN.F.GPL.DMP : last exported on 06.11.23
+DEL.N1LN3L.DN.F.GTR.DMP : last exported on 06.11.23
+DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 06.11.23
+DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 06.11.23
+DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 06.11.23
+DEL.N1LK61.DN.F.CPD.DMP : last exported on 06.11.23
+DEL.N1LN0R.DN.F.CPL.DMP : last exported on 06.11.23
+DEL.KT6E35.SN.F.GGO.ZIP : last exported on 06.11.23
+DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 06.11.23</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
@@ -1120,31 +1120,31 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 02.11.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 02.11.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 02.11.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 02.11.23
-DIT.E35KT6.WI.ZIP : last exported on 02.11.23
-DEL.K2PKT6.WI.ZIP : last exported on 02.11.23
-DEL.R7AKT6.WI.ZIP : last exported on 01.11.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 03.11.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 05.11.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 03.11.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 05.11.23
+DIT.E35KT6.WI.ZIP : last exported on 03.11.23
+DEL.K2PKT6.WI.ZIP : last exported on 05.11.23
+DEL.R7AKT6.WI.ZIP : last exported on 04.11.23
 DEL.N5FKT6.WI.ZIP : last exported on 27.10.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 02.11.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 02.11.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 02.11.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 02.11.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 02.11.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 02.11.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 02.11.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 02.11.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 02.11.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 02.11.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 02.11.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 02.11.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 02.11.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 06.11.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 06.11.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 06.11.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 06.11.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 06.11.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 06.11.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 06.11.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 06.11.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 06.11.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 06.11.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 06.11.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 06.11.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 06.11.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1247,30 +1247,30 @@
       </c>
       <c r="C10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 21.10.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 03.11.23
+          <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 03.11.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 06.11.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 30.10.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 02.11.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 02.11.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 02.11.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 02.11.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 02.11.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 02.11.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 02.11.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 02.11.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 02.11.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 02.11.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 02.11.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 02.11.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 02.11.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 02.11.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 02.11.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 02.11.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 02.11.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 05.11.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 05.11.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 05.11.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 05.11.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 05.11.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 05.11.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 05.11.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 05.11.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 05.11.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 05.11.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 05.11.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 05.11.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 05.11.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 05.11.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 05.11.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 05.11.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 05.11.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1338,7 +1338,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 28.10.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 28.10.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 01.11.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 05.11.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 28.10.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 28.10.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 28.10.23
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 02.11.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 03.11.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 02.11.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 04.11.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1413,7 +1413,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 27.10.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 27.10.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 01.11.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 05.11.23
 DEL.KT6N5M.AU.GGO.ZIP : last exported on 27.10.23
 DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 27.10.23
 DEL.KT6KTZ.AU.GGO.ZIP : last exported on 27.10.23
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 02.11.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 02.11.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 05.11.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 05.11.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 02.11.23
-DHP.KUDKT6.ORGUNITS : last exported on 03.11.23
-DHS.R11KT6.HSB02ALL : last exported on 02.11.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 06.11.23
+DHP.KUDKT6.ORGUNITS : last exported on 06.11.23
+DHS.R11KT6.HSB02ALL : last exported on 03.11.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 02.11.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 02.11.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 02.11.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 02.11.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 02.11.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 02.11.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 02.11.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 02.11.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 02.11.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 02.11.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 04.11.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 04.11.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 05.11.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 04.11.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 04.11.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 04.11.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 04.11.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 04.11.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 04.11.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 04.11.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1620,7 +1620,7 @@
       </c>
       <c r="D19" s="16" t="inlineStr">
         <is>
-          <t>DEL.N1LE35.TRANS.ZIP : last exported on 29.10.23</t>
+          <t>DEL.N1LE35.TRANS.ZIP : last exported on 05.11.23</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 02.11.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 04.11.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 02.11.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 02.11.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 02.11.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 02.11.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 02.11.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 02.11.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 02.11.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 02.11.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 02.11.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 02.11.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 02.11.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 02.11.23
-DEL.N1LKT6.MT.??????.G : last exported on 02.11.23
-DEL.N1LKT6.MT.??????.U : last exported on 02.11.23
-DEL.N1LKT6.MT.??????.AS : last exported on 02.11.23
-DVL.N1LN5X.VLM.DSP : last exported on 02.11.23
-DVL.N1LN5X.VLM.WT : last exported on 02.11.23
-DDS.N1LR11.DSP : last exported on 02.11.23
-DDS.N1LR11.WT : last exported on 02.11.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 02.11.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 02.11.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 02.11.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 02.11.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 02.11.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 02.11.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 02.11.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 02.11.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 02.11.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 02.11.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 02.11.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 04.11.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 04.11.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 05.11.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 04.11.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 04.11.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 04.11.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 04.11.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 04.11.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 04.11.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 04.11.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 04.11.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 04.11.23
+DEL.N1LKT6.MT.??????.G : last exported on 04.11.23
+DEL.N1LKT6.MT.??????.U : last exported on 04.11.23
+DEL.N1LKT6.MT.??????.AS : last exported on 04.11.23
+DVL.N1LN5X.VLM.DSP : last exported on 04.11.23
+DVL.N1LN5X.VLM.WT : last exported on 04.11.23
+DDS.N1LR11.DSP : last exported on 04.11.23
+DDS.N1LR11.WT : last exported on 04.11.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 04.11.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 04.11.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 04.11.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 04.11.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 04.11.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 04.11.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 04.11.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 04.11.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 04.11.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 04.11.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 04.11.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,22 +1710,22 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 03.11.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 03.11.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 06.11.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 06.11.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 02.11.23
-DEL.N1LN3L.EM.F.GPL.DMP : last exported on 02.11.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 02.11.23
-DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 02.11.23
-DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 02.11.23
-DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 02.11.23
-DEL.N1LK61.EM.F.CPD.DMP : last exported on 02.11.23
-DEL.N1LN0R.EM.F.CPL.DMP : last exported on 02.11.23
-DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 02.11.23
-DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 02.11.23</t>
+          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 05.11.23
+DEL.N1LN3L.EM.F.GPL.DMP : last exported on 05.11.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 05.11.23
+DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 05.11.23
+DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 05.11.23
+DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 05.11.23
+DEL.N1LK61.EM.F.CPD.DMP : last exported on 05.11.23
+DEL.N1LN0R.EM.F.CPL.DMP : last exported on 05.11.23
+DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 05.11.23
+DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 05.11.23</t>
         </is>
       </c>
       <c r="E21" s="11" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 03.11.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 03.11.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 03.11.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 03.11.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 03.11.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 03.11.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 03.11.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 03.11.23
-DDC.R11KT6.ELFI.MD.TXT : last exported on 29.10.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 02.11.23
-DDC.R11KT6.ELFI.PK.TXT : last exported on 29.10.23
-DDC.R11KT6.ELFI.PR.TXT : last exported on 29.10.23</t>
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 06.11.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 06.11.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 06.11.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 06.11.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 06.11.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 06.11.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 06.11.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 06.11.23
+DDC.R11KT6.ELFI.MD.TXT : last exported on 05.11.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 03.11.23
+DDC.R11KT6.ELFI.PK.TXT : last exported on 05.11.23
+DDC.R11KT6.ELFI.PR.TXT : last exported on 05.11.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 02.11.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 02.11.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 02.11.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 02.11.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 02.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 02.11.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 02.11.23
-DEL.N1LKT6.EC.??????.G : last exported on 02.11.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 02.11.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 02.11.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 02.11.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 02.11.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 02.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 02.11.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 02.11.23
-DEL.N1LKT6.EC.??????.U : last exported on 02.11.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 02.11.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 02.11.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 02.11.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 02.11.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 02.11.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 02.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 02.11.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 02.11.23
-DEL.N1LKT6.EC.??????.AS : last exported on 02.11.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 02.11.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 02.11.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 02.11.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 02.11.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 02.11.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 02.11.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 02.11.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 02.11.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 05.11.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 05.11.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 05.11.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 05.11.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 05.11.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 05.11.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 05.11.23
+DEL.N1LKT6.EC.??????.G : last exported on 05.11.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 05.11.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 05.11.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 05.11.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 05.11.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 05.11.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 05.11.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 05.11.23
+DEL.N1LKT6.EC.??????.U : last exported on 05.11.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 05.11.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 05.11.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 05.11.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 05.11.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 05.11.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 05.11.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 05.11.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 05.11.23
+DEL.N1LKT6.EC.??????.AS : last exported on 05.11.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 05.11.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 05.11.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 05.11.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 05.11.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 05.11.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 05.11.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 05.11.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 05.11.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 07.11.23 12:19
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 06.11.2023</t>
+          <t>Date - 07.11.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -1002,14 +1002,14 @@
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 05.11.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 05.11.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 05.11.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 05.11.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 05.11.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 05.11.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 05.11.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 05.11.23
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 07.11.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 07.11.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 07.11.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 07.11.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 07.11.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 07.11.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 07.11.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 07.11.23
 DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 05.11.23
 DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 05.11.23
 DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 05.11.23
@@ -1254,14 +1254,14 @@
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 05.11.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 05.11.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 05.11.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 05.11.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 05.11.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 05.11.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 05.11.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 05.11.23
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 06.11.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 06.11.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 06.11.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 06.11.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 06.11.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 06.11.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 06.11.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 06.11.23
 DEL.KT6E35.TP.D.GGO.ZIP : last exported on 05.11.23
 DEL.KT6E35.TP.D.UGO.ZIP : last exported on 05.11.23
 DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 05.11.23
@@ -1338,7 +1338,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 28.10.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 28.10.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 05.11.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 06.11.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 28.10.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 28.10.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 28.10.23
@@ -1413,7 +1413,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 27.10.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 27.10.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 05.11.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 06.11.23
 DEL.KT6N5M.AU.GGO.ZIP : last exported on 27.10.23
 DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 27.10.23
 DEL.KT6KTZ.AU.GGO.ZIP : last exported on 27.10.23
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 05.11.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 05.11.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 06.11.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 06.11.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1545,7 +1545,7 @@
         <is>
           <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 04.11.23
 DEL.N1LN3L.DP.F.GPL.DMP : last exported on 04.11.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 05.11.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 06.11.23
 DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 04.11.23
 DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 04.11.23
 DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 04.11.23
@@ -1653,25 +1653,25 @@
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 04.11.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 04.11.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 05.11.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 04.11.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 04.11.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 04.11.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 04.11.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 04.11.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 04.11.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 04.11.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 04.11.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 04.11.23
-DEL.N1LKT6.MT.??????.G : last exported on 04.11.23
-DEL.N1LKT6.MT.??????.U : last exported on 04.11.23
-DEL.N1LKT6.MT.??????.AS : last exported on 04.11.23
-DVL.N1LN5X.VLM.DSP : last exported on 04.11.23
-DVL.N1LN5X.VLM.WT : last exported on 04.11.23
-DDS.N1LR11.DSP : last exported on 04.11.23
-DDS.N1LR11.WT : last exported on 04.11.23
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 06.11.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 06.11.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 06.11.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 06.11.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 06.11.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 06.11.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 06.11.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 06.11.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 06.11.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 06.11.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 06.11.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 06.11.23
+DEL.N1LKT6.MT.??????.G : last exported on 06.11.23
+DEL.N1LKT6.MT.??????.U : last exported on 06.11.23
+DEL.N1LKT6.MT.??????.AS : last exported on 06.11.23
+DVL.N1LN5X.VLM.DSP : last exported on 06.11.23
+DVL.N1LN5X.VLM.WT : last exported on 06.11.23
+DDS.N1LR11.DSP : last exported on 06.11.23
+DDS.N1LR11.WT : last exported on 06.11.23
 DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 04.11.23
 DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 04.11.23
 DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 04.11.23
@@ -1716,16 +1716,16 @@
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 05.11.23
-DEL.N1LN3L.EM.F.GPL.DMP : last exported on 05.11.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 05.11.23
-DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 05.11.23
-DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 05.11.23
-DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 05.11.23
-DEL.N1LK61.EM.F.CPD.DMP : last exported on 05.11.23
-DEL.N1LN0R.EM.F.CPL.DMP : last exported on 05.11.23
-DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 05.11.23
-DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 05.11.23</t>
+          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 06.11.23
+DEL.N1LN3L.EM.F.GPL.DMP : last exported on 06.11.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 06.11.23
+DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 06.11.23
+DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 06.11.23
+DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 06.11.23
+DEL.N1LK61.EM.F.CPD.DMP : last exported on 06.11.23
+DEL.N1LN0R.EM.F.CPL.DMP : last exported on 06.11.23
+DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 06.11.23
+DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 06.11.23</t>
         </is>
       </c>
       <c r="E21" s="11" t="inlineStr">
@@ -1769,38 +1769,38 @@
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 05.11.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 05.11.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 05.11.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 05.11.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 05.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 05.11.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 05.11.23
-DEL.N1LKT6.EC.??????.G : last exported on 05.11.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 05.11.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 05.11.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 05.11.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 05.11.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 05.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 05.11.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 05.11.23
-DEL.N1LKT6.EC.??????.U : last exported on 05.11.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 05.11.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 05.11.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 05.11.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 05.11.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 05.11.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 05.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 05.11.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 05.11.23
-DEL.N1LKT6.EC.??????.AS : last exported on 05.11.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 05.11.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 05.11.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 05.11.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 05.11.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 05.11.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 05.11.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 05.11.23
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 06.11.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 06.11.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 06.11.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 06.11.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 06.11.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 06.11.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 06.11.23
+DEL.N1LKT6.EC.??????.G : last exported on 06.11.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 06.11.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 06.11.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 06.11.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 06.11.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 06.11.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 06.11.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 06.11.23
+DEL.N1LKT6.EC.??????.U : last exported on 06.11.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 06.11.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 06.11.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 06.11.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 06.11.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 06.11.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 06.11.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 06.11.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 06.11.23
+DEL.N1LKT6.EC.??????.AS : last exported on 06.11.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 06.11.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 06.11.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 06.11.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 06.11.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 06.11.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 06.11.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 06.11.23
 DEL.KT6N5X.EL.F.AU.ZIP : last exported on 05.11.23</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Updated on 08.11.23 13:22
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 07.11.2023</t>
+          <t>Date - 08.11.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -1002,14 +1002,14 @@
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 07.11.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 07.11.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 07.11.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 07.11.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 07.11.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 07.11.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 07.11.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 07.11.23
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 08.11.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 08.11.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 08.11.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 08.11.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 08.11.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 08.11.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 08.11.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 08.11.23
 DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 05.11.23
 DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 05.11.23
 DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 05.11.23
@@ -1132,13 +1132,13 @@
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 06.11.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 06.11.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 06.11.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 06.11.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 06.11.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 06.11.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 06.11.23
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 07.11.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 07.11.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 07.11.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 07.11.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 07.11.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 07.11.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 07.11.23
 DEL.KT6KTZ.WI.GGO.ZIP : last exported on 06.11.23
 DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 06.11.23
 DEL.KT6E35.WI.GGO.ZIP : last exported on 06.11.23
@@ -1254,14 +1254,14 @@
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 06.11.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 06.11.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 06.11.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 06.11.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 06.11.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 06.11.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 06.11.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 06.11.23
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 07.11.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 07.11.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 07.11.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 07.11.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 07.11.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 07.11.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 07.11.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 07.11.23
 DEL.KT6E35.TP.D.GGO.ZIP : last exported on 05.11.23
 DEL.KT6E35.TP.D.UGO.ZIP : last exported on 05.11.23
 DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 05.11.23
@@ -1336,12 +1336,12 @@
       </c>
       <c r="D12" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 28.10.23
-DEL.N1LN3L.MC.F.GPL.DMP : last exported on 28.10.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 06.11.23
-DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 28.10.23
-DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 28.10.23
-DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 28.10.23
+          <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 07.11.23
+DEL.N1LN3L.MC.F.GPL.DMP : last exported on 07.11.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 07.11.23
+DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 07.11.23
+DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 07.11.23
+DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 07.11.23
 DGI.KT6R11.MANDANT.TXT : last exported on 28.10.23</t>
         </is>
       </c>
@@ -1413,7 +1413,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 27.10.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 27.10.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 06.11.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 07.11.23
 DEL.KT6N5M.AU.GGO.ZIP : last exported on 27.10.23
 DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 27.10.23
 DEL.KT6KTZ.AU.GGO.ZIP : last exported on 27.10.23
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 06.11.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 06.11.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 07.11.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 07.11.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1543,16 +1543,16 @@
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 04.11.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 04.11.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 06.11.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 04.11.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 04.11.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 04.11.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 04.11.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 04.11.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 04.11.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 04.11.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 07.11.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 07.11.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 07.11.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 07.11.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 07.11.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 07.11.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 07.11.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 07.11.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 07.11.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 07.11.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1653,25 +1653,25 @@
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 06.11.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 06.11.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 06.11.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 06.11.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 06.11.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 06.11.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 06.11.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 06.11.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 06.11.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 06.11.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 06.11.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 06.11.23
-DEL.N1LKT6.MT.??????.G : last exported on 06.11.23
-DEL.N1LKT6.MT.??????.U : last exported on 06.11.23
-DEL.N1LKT6.MT.??????.AS : last exported on 06.11.23
-DVL.N1LN5X.VLM.DSP : last exported on 06.11.23
-DVL.N1LN5X.VLM.WT : last exported on 06.11.23
-DDS.N1LR11.DSP : last exported on 06.11.23
-DDS.N1LR11.WT : last exported on 06.11.23
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 07.11.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 07.11.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 07.11.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 07.11.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 07.11.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 07.11.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 07.11.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 07.11.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 07.11.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 07.11.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 07.11.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 07.11.23
+DEL.N1LKT6.MT.??????.G : last exported on 07.11.23
+DEL.N1LKT6.MT.??????.U : last exported on 07.11.23
+DEL.N1LKT6.MT.??????.AS : last exported on 07.11.23
+DVL.N1LN5X.VLM.DSP : last exported on 07.11.23
+DVL.N1LN5X.VLM.WT : last exported on 07.11.23
+DDS.N1LR11.DSP : last exported on 07.11.23
+DDS.N1LR11.WT : last exported on 07.11.23
 DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 04.11.23
 DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 04.11.23
 DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 04.11.23
@@ -1716,16 +1716,16 @@
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 06.11.23
-DEL.N1LN3L.EM.F.GPL.DMP : last exported on 06.11.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 06.11.23
-DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 06.11.23
-DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 06.11.23
-DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 06.11.23
-DEL.N1LK61.EM.F.CPD.DMP : last exported on 06.11.23
-DEL.N1LN0R.EM.F.CPL.DMP : last exported on 06.11.23
-DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 06.11.23
-DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 06.11.23</t>
+          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 07.11.23
+DEL.N1LN3L.EM.F.GPL.DMP : last exported on 07.11.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 07.11.23
+DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 07.11.23
+DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 07.11.23
+DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 07.11.23
+DEL.N1LK61.EM.F.CPD.DMP : last exported on 07.11.23
+DEL.N1LN0R.EM.F.CPL.DMP : last exported on 07.11.23
+DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 07.11.23
+DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 07.11.23</t>
         </is>
       </c>
       <c r="E21" s="11" t="inlineStr">
@@ -1769,38 +1769,38 @@
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 06.11.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 06.11.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 06.11.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 06.11.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 06.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 06.11.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 06.11.23
-DEL.N1LKT6.EC.??????.G : last exported on 06.11.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 06.11.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 06.11.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 06.11.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 06.11.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 06.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 06.11.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 06.11.23
-DEL.N1LKT6.EC.??????.U : last exported on 06.11.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 06.11.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 06.11.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 06.11.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 06.11.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 06.11.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 06.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 06.11.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 06.11.23
-DEL.N1LKT6.EC.??????.AS : last exported on 06.11.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 06.11.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 06.11.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 06.11.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 06.11.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 06.11.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 06.11.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 06.11.23
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 07.11.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 07.11.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 07.11.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 07.11.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 07.11.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 07.11.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 07.11.23
+DEL.N1LKT6.EC.??????.G : last exported on 07.11.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 07.11.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 07.11.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 07.11.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 07.11.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 07.11.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 07.11.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 07.11.23
+DEL.N1LKT6.EC.??????.U : last exported on 07.11.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 07.11.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 07.11.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 07.11.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 07.11.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 07.11.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 07.11.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 07.11.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 07.11.23
+DEL.N1LKT6.EC.??????.AS : last exported on 07.11.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 07.11.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 07.11.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 07.11.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 07.11.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 07.11.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 07.11.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 07.11.23
 DEL.KT6N5X.EL.F.AU.ZIP : last exported on 05.11.23</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Updated on 09.11.23 12:04
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 08.11.2023</t>
+          <t>Date - 09.11.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 03.11.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 08.11.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 08.11.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 08.11.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 08.11.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 08.11.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 08.11.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 08.11.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 08.11.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 08.11.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 05.11.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 05.11.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 05.11.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 05.11.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 05.11.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 05.11.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 09.11.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 09.11.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 09.11.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 09.11.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 09.11.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 09.11.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 09.11.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 09.11.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 09.11.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 09.11.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 09.11.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 09.11.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 09.11.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 09.11.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1120,31 +1120,31 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 03.11.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 05.11.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 03.11.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 05.11.23
-DIT.E35KT6.WI.ZIP : last exported on 03.11.23
-DEL.K2PKT6.WI.ZIP : last exported on 05.11.23
-DEL.R7AKT6.WI.ZIP : last exported on 04.11.23
-DEL.N5FKT6.WI.ZIP : last exported on 27.10.23</t>
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 07.11.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 08.11.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 06.11.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 08.11.23
+DIT.E35KT6.WI.ZIP : last exported on 08.11.23
+DEL.K2PKT6.WI.ZIP : last exported on 08.11.23
+DEL.R7AKT6.WI.ZIP : last exported on 09.11.23
+DEL.N5FKT6.WI.ZIP : last exported on 08.11.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 07.11.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 07.11.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 07.11.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 07.11.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 07.11.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 07.11.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 07.11.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 06.11.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 06.11.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 06.11.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 06.11.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 06.11.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 06.11.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 08.11.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 08.11.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 08.11.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 08.11.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 08.11.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 08.11.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 08.11.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 08.11.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 08.11.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 08.11.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 08.11.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 08.11.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 08.11.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 03.11.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 06.11.23
-DGV.N3LKT6.EPELS.??????.ZIP : last exported on 30.10.23</t>
+DEL.N3LKT6.HST.??????.ZIP : last exported on 09.11.23
+DGV.N3LKT6.EPELS.??????.ZIP : last exported on 06.11.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 07.11.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 07.11.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 07.11.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 07.11.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 07.11.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 07.11.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 07.11.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 07.11.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 05.11.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 05.11.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 05.11.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 05.11.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 05.11.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 05.11.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 05.11.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 05.11.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 05.11.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 08.11.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 08.11.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 08.11.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 08.11.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 08.11.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 08.11.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 08.11.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 08.11.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 08.11.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 08.11.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 08.11.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 08.11.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 08.11.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 08.11.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 08.11.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 08.11.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 08.11.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1298,12 +1298,12 @@
       </c>
       <c r="C11" s="14" t="inlineStr">
         <is>
-          <t>DEL.KT6KT6.APOSPRO.ZIP : last exported on 30.10.23</t>
+          <t>DEL.KT6KT6.APOSPRO.ZIP : last exported on 06.11.23</t>
         </is>
       </c>
       <c r="D11" s="15" t="inlineStr">
         <is>
-          <t>DEL.KT6N2O.XTIME.ZIP : last exported on 30.10.23</t>
+          <t>DEL.KT6N2O.XTIME.ZIP : last exported on 06.11.23</t>
         </is>
       </c>
       <c r="E11" s="11" t="inlineStr">
@@ -1331,18 +1331,18 @@
       </c>
       <c r="C12" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.MANDANTN.TXT : last exported on 28.10.23</t>
+          <t>DEL.N3LKT6.MANDANTN.TXT : last exported on 07.11.23</t>
         </is>
       </c>
       <c r="D12" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 07.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 07.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 07.11.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 08.11.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 07.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 07.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 07.11.23
-DGI.KT6R11.MANDANT.TXT : last exported on 28.10.23</t>
+DGI.KT6R11.MANDANT.TXT : last exported on 07.11.23</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 03.11.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 08.11.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 04.11.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 08.11.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1405,21 +1405,21 @@
         <is>
           <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 07.08.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
-DLV.I5XKT6.AU.A.ZIP : last exported on 26.10.23
+DLV.I5XKT6.AU.A.ZIP : last exported on 07.11.23
 DLV.R31KT6.AU.C.ZIP : last exported on 26.10.23</t>
         </is>
       </c>
       <c r="D14" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 27.10.23
-DEL.N1LN3L.AU.D.GPL.DMP : last exported on 27.10.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 07.11.23
-DEL.KT6N5M.AU.GGO.ZIP : last exported on 27.10.23
-DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 27.10.23
-DEL.KT6KTZ.AU.GGO.ZIP : last exported on 27.10.23
-DEL.KT6KTZ.AU.IMG.GGO.ZIP : last exported on 27.10.23
-DEL.KT6E35.AU.GGO.ZIP : last exported on 27.10.23
-DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 27.10.23</t>
+          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 08.11.23
+DEL.N1LN3L.AU.D.GPL.DMP : last exported on 08.11.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 08.11.23
+DEL.KT6N5M.AU.GGO.ZIP : last exported on 08.11.23
+DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 08.11.23
+DEL.KT6KTZ.AU.GGO.ZIP : last exported on 08.11.23
+DEL.KT6KTZ.AU.IMG.GGO.ZIP : last exported on 08.11.23
+DEL.KT6E35.AU.GGO.ZIP : last exported on 08.11.23
+DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 08.11.23</t>
         </is>
       </c>
       <c r="E14" s="11" t="inlineStr">
@@ -1455,26 +1455,26 @@
 DGQ.R11KT6.PKAT.US2.TXT : last exported on 01.11.23
 DGQ.R11KT6.BSITK.TXT : last exported on 01.11.23
 DGQ.R11KT6.BSITX.TXT : last exported on 01.11.23
-DGQ.R31KT6.BSIVMC.TXT : last exported on 10.10.23
-DGQ.R31KT6.PKATC.TXT : last exported on 10.10.23
-DEL.KMPKT6.APOS.DATA.ZIP : last exported on 01.11.23</t>
+DGQ.R31KT6.BSIVMC.TXT : last exported on 07.11.23
+DGQ.R31KT6.PKATC.TXT : last exported on 07.11.23
+DEL.KMPKT6.APOS.DATA.ZIP : last exported on 08.11.23</t>
         </is>
       </c>
       <c r="D15" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 01.11.23
-DEL.N1LN3L.AP.F.GPL.DMP : last exported on 01.11.23
-DEL.N1LN3L.AP.F.GTR.DMP : last exported on 01.11.23
-DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 01.11.23
-DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 01.11.23
-DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 01.11.23
-DEL.N1LK61.AP.F.CPD.DMP : last exported on 01.11.23
-DEL.N1LN0R.AP.F.CPL.DMP : last exported on 01.11.23
-DEL.N1LR31.AP.F.PPS.DMP : last exported on 01.11.23
-DEL.KT6E35.AP.F.DB.ZIP : last exported on 01.11.23
-DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 01.11.23
-DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 01.11.23
-DVL.KT6N5X.VLM.AP.ZIP : last exported on 01.11.23</t>
+          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 08.11.23
+DEL.N1LN3L.AP.F.GPL.DMP : last exported on 08.11.23
+DEL.N1LN3L.AP.F.GTR.DMP : last exported on 08.11.23
+DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 08.11.23
+DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 08.11.23
+DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 08.11.23
+DEL.N1LK61.AP.F.CPD.DMP : last exported on 08.11.23
+DEL.N1LN0R.AP.F.CPL.DMP : last exported on 08.11.23
+DEL.N1LR31.AP.F.PPS.DMP : last exported on 08.11.23
+DEL.KT6E35.AP.F.DB.ZIP : last exported on 08.11.23
+DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 08.11.23
+DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 08.11.23
+DVL.KT6N5X.VLM.AP.ZIP : last exported on 08.11.23</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 07.11.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 07.11.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 08.11.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 08.11.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 06.11.23
-DHP.KUDKT6.ORGUNITS : last exported on 06.11.23
-DHS.R11KT6.HSB02ALL : last exported on 03.11.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 08.11.23
+DHP.KUDKT6.ORGUNITS : last exported on 09.11.23
+DHS.R11KT6.HSB02ALL : last exported on 08.11.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 07.11.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 07.11.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 07.11.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 07.11.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 07.11.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 07.11.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 07.11.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 07.11.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 07.11.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 07.11.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 08.11.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 08.11.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 08.11.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 08.11.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 08.11.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 08.11.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 08.11.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 08.11.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 08.11.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 08.11.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 04.11.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 08.11.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 07.11.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 07.11.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 07.11.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 07.11.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 07.11.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 07.11.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 07.11.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 07.11.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 07.11.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 07.11.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 07.11.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 07.11.23
-DEL.N1LKT6.MT.??????.G : last exported on 07.11.23
-DEL.N1LKT6.MT.??????.U : last exported on 07.11.23
-DEL.N1LKT6.MT.??????.AS : last exported on 07.11.23
-DVL.N1LN5X.VLM.DSP : last exported on 07.11.23
-DVL.N1LN5X.VLM.WT : last exported on 07.11.23
-DDS.N1LR11.DSP : last exported on 07.11.23
-DDS.N1LR11.WT : last exported on 07.11.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 04.11.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 04.11.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 04.11.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 04.11.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 04.11.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 04.11.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 04.11.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 04.11.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 04.11.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 04.11.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 04.11.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 08.11.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 08.11.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 08.11.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 08.11.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 08.11.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 08.11.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 08.11.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 08.11.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 08.11.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 08.11.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 08.11.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 08.11.23
+DEL.N1LKT6.MT.??????.G : last exported on 08.11.23
+DEL.N1LKT6.MT.??????.U : last exported on 08.11.23
+DEL.N1LKT6.MT.??????.AS : last exported on 08.11.23
+DVL.N1LN5X.VLM.DSP : last exported on 08.11.23
+DVL.N1LN5X.VLM.WT : last exported on 08.11.23
+DDS.N1LR11.DSP : last exported on 08.11.23
+DDS.N1LR11.WT : last exported on 08.11.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 08.11.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 08.11.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 08.11.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 08.11.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 08.11.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 08.11.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 08.11.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 08.11.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 08.11.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 08.11.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 08.11.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,22 +1710,22 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 06.11.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 06.11.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 09.11.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 09.11.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 07.11.23
-DEL.N1LN3L.EM.F.GPL.DMP : last exported on 07.11.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 07.11.23
-DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 07.11.23
-DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 07.11.23
-DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 07.11.23
-DEL.N1LK61.EM.F.CPD.DMP : last exported on 07.11.23
-DEL.N1LN0R.EM.F.CPL.DMP : last exported on 07.11.23
-DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 07.11.23
-DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 07.11.23</t>
+          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 08.11.23
+DEL.N1LN3L.EM.F.GPL.DMP : last exported on 08.11.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 08.11.23
+DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 08.11.23
+DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 08.11.23
+DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 08.11.23
+DEL.N1LK61.EM.F.CPD.DMP : last exported on 08.11.23
+DEL.N1LN0R.EM.F.CPL.DMP : last exported on 08.11.23
+DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 08.11.23
+DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 08.11.23</t>
         </is>
       </c>
       <c r="E21" s="11" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 06.11.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 06.11.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 06.11.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 06.11.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 06.11.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 06.11.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 06.11.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 06.11.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 09.11.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 09.11.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 09.11.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 09.11.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 09.11.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 09.11.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 09.11.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 09.11.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 05.11.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 03.11.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 08.11.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 05.11.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 05.11.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 07.11.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 07.11.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 07.11.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 07.11.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 07.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 07.11.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 07.11.23
-DEL.N1LKT6.EC.??????.G : last exported on 07.11.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 07.11.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 07.11.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 07.11.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 07.11.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 07.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 07.11.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 07.11.23
-DEL.N1LKT6.EC.??????.U : last exported on 07.11.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 07.11.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 07.11.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 07.11.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 07.11.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 07.11.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 07.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 07.11.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 07.11.23
-DEL.N1LKT6.EC.??????.AS : last exported on 07.11.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 07.11.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 07.11.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 07.11.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 07.11.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 07.11.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 07.11.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 07.11.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 05.11.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 08.11.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 08.11.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 08.11.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 08.11.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 08.11.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 08.11.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 08.11.23
+DEL.N1LKT6.EC.??????.G : last exported on 08.11.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 08.11.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 08.11.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 08.11.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 08.11.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 08.11.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 08.11.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 08.11.23
+DEL.N1LKT6.EC.??????.U : last exported on 08.11.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 08.11.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 08.11.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 08.11.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 08.11.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 08.11.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 08.11.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 08.11.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 08.11.23
+DEL.N1LKT6.EC.??????.AS : last exported on 08.11.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 08.11.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 08.11.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 08.11.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 08.11.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 08.11.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 08.11.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 08.11.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 08.11.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 10.11.23 11:54
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 09.11.2023</t>
+          <t>Date - 10.11.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 08.11.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 09.11.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 09.11.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 09.11.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 09.11.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 09.11.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 09.11.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 09.11.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 09.11.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 09.11.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 09.11.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 09.11.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 09.11.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 09.11.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 09.11.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 09.11.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 10.11.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 10.11.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 10.11.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 10.11.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 10.11.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 10.11.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 10.11.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 10.11.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 10.11.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 10.11.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 10.11.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 10.11.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 10.11.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 10.11.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1120,31 +1120,31 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 07.11.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 08.11.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 06.11.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 08.11.23
-DIT.E35KT6.WI.ZIP : last exported on 08.11.23
-DEL.K2PKT6.WI.ZIP : last exported on 08.11.23
-DEL.R7AKT6.WI.ZIP : last exported on 09.11.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 09.11.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 09.11.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 09.11.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 09.11.23
+DIT.E35KT6.WI.ZIP : last exported on 09.11.23
+DEL.K2PKT6.WI.ZIP : last exported on 09.11.23
+DEL.R7AKT6.WI.ZIP : last exported on 10.11.23
 DEL.N5FKT6.WI.ZIP : last exported on 08.11.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 08.11.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 08.11.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 08.11.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 08.11.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 08.11.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 08.11.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 08.11.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 08.11.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 08.11.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 08.11.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 08.11.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 08.11.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 08.11.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 09.11.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 09.11.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 09.11.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 09.11.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 09.11.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 09.11.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 09.11.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 09.11.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 09.11.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 09.11.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 09.11.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 09.11.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 09.11.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 03.11.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 09.11.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 10.11.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 06.11.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 08.11.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 08.11.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 08.11.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 08.11.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 08.11.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 08.11.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 08.11.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 08.11.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 08.11.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 08.11.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 08.11.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 08.11.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 08.11.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 08.11.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 08.11.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 08.11.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 08.11.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 09.11.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 09.11.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 09.11.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 09.11.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 09.11.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 09.11.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 09.11.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 09.11.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 09.11.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 09.11.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 09.11.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 09.11.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 09.11.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 09.11.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 09.11.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 09.11.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 09.11.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1338,7 +1338,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 07.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 07.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 08.11.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 09.11.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 07.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 07.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 07.11.23
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 08.11.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 09.11.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 08.11.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 09.11.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1405,7 +1405,7 @@
         <is>
           <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 07.08.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
-DLV.I5XKT6.AU.A.ZIP : last exported on 07.11.23
+DLV.I5XKT6.AU.A.ZIP : last exported on 09.11.23
 DLV.R31KT6.AU.C.ZIP : last exported on 26.10.23</t>
         </is>
       </c>
@@ -1413,7 +1413,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 08.11.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 08.11.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 08.11.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 09.11.23
 DEL.KT6N5M.AU.GGO.ZIP : last exported on 08.11.23
 DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 08.11.23
 DEL.KT6KTZ.AU.GGO.ZIP : last exported on 08.11.23
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 08.11.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 08.11.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 09.11.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 09.11.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 08.11.23
-DHP.KUDKT6.ORGUNITS : last exported on 09.11.23
-DHS.R11KT6.HSB02ALL : last exported on 08.11.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 09.11.23
+DHP.KUDKT6.ORGUNITS : last exported on 10.11.23
+DHS.R11KT6.HSB02ALL : last exported on 09.11.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 08.11.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 08.11.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 08.11.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 08.11.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 08.11.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 08.11.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 08.11.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 08.11.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 08.11.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 08.11.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 09.11.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 09.11.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 09.11.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 09.11.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 09.11.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 09.11.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 09.11.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 09.11.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 09.11.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 09.11.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 08.11.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 09.11.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 08.11.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 08.11.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 08.11.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 08.11.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 08.11.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 08.11.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 08.11.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 08.11.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 08.11.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 08.11.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 08.11.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 08.11.23
-DEL.N1LKT6.MT.??????.G : last exported on 08.11.23
-DEL.N1LKT6.MT.??????.U : last exported on 08.11.23
-DEL.N1LKT6.MT.??????.AS : last exported on 08.11.23
-DVL.N1LN5X.VLM.DSP : last exported on 08.11.23
-DVL.N1LN5X.VLM.WT : last exported on 08.11.23
-DDS.N1LR11.DSP : last exported on 08.11.23
-DDS.N1LR11.WT : last exported on 08.11.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 08.11.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 08.11.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 08.11.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 08.11.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 08.11.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 08.11.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 08.11.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 08.11.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 08.11.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 08.11.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 08.11.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 09.11.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 09.11.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 09.11.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 09.11.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 09.11.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 09.11.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 09.11.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 09.11.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 09.11.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 09.11.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 09.11.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 09.11.23
+DEL.N1LKT6.MT.??????.G : last exported on 09.11.23
+DEL.N1LKT6.MT.??????.U : last exported on 09.11.23
+DEL.N1LKT6.MT.??????.AS : last exported on 09.11.23
+DVL.N1LN5X.VLM.DSP : last exported on 09.11.23
+DVL.N1LN5X.VLM.WT : last exported on 09.11.23
+DDS.N1LR11.DSP : last exported on 09.11.23
+DDS.N1LR11.WT : last exported on 09.11.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 09.11.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 09.11.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 09.11.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 09.11.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 09.11.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 09.11.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 09.11.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 09.11.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 09.11.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 09.11.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 09.11.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,22 +1710,22 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 09.11.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 09.11.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 10.11.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 10.11.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 08.11.23
-DEL.N1LN3L.EM.F.GPL.DMP : last exported on 08.11.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 08.11.23
-DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 08.11.23
-DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 08.11.23
-DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 08.11.23
-DEL.N1LK61.EM.F.CPD.DMP : last exported on 08.11.23
-DEL.N1LN0R.EM.F.CPL.DMP : last exported on 08.11.23
-DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 08.11.23
-DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 08.11.23</t>
+          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 09.11.23
+DEL.N1LN3L.EM.F.GPL.DMP : last exported on 09.11.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 09.11.23
+DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 09.11.23
+DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 09.11.23
+DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 09.11.23
+DEL.N1LK61.EM.F.CPD.DMP : last exported on 09.11.23
+DEL.N1LN0R.EM.F.CPL.DMP : last exported on 09.11.23
+DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 09.11.23
+DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 09.11.23</t>
         </is>
       </c>
       <c r="E21" s="11" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 09.11.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 09.11.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 09.11.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 09.11.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 09.11.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 09.11.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 09.11.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 09.11.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 10.11.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 10.11.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 10.11.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 10.11.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 10.11.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 10.11.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 10.11.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 10.11.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 05.11.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 08.11.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 09.11.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 05.11.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 05.11.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 08.11.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 08.11.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 08.11.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 08.11.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 08.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 08.11.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 08.11.23
-DEL.N1LKT6.EC.??????.G : last exported on 08.11.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 08.11.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 08.11.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 08.11.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 08.11.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 08.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 08.11.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 08.11.23
-DEL.N1LKT6.EC.??????.U : last exported on 08.11.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 08.11.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 08.11.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 08.11.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 08.11.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 08.11.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 08.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 08.11.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 08.11.23
-DEL.N1LKT6.EC.??????.AS : last exported on 08.11.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 08.11.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 08.11.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 08.11.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 08.11.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 08.11.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 08.11.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 08.11.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 08.11.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 09.11.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 09.11.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 09.11.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 09.11.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 09.11.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 09.11.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 09.11.23
+DEL.N1LKT6.EC.??????.G : last exported on 09.11.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 09.11.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 09.11.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 09.11.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 09.11.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 09.11.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 09.11.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 09.11.23
+DEL.N1LKT6.EC.??????.U : last exported on 09.11.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 09.11.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 09.11.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 09.11.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 09.11.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 09.11.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 09.11.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 09.11.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 09.11.23
+DEL.N1LKT6.EC.??????.AS : last exported on 09.11.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 09.11.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 09.11.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 09.11.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 09.11.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 09.11.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 09.11.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 09.11.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 09.11.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 13.11.23 12:03
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 10.11.2023</t>
+          <t>Date - 13.11.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 09.11.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 10.11.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 10.11.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 10.11.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 10.11.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 10.11.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 10.11.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 10.11.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 10.11.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 10.11.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 10.11.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 10.11.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 10.11.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 10.11.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 10.11.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 10.11.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 11.11.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 11.11.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 12.11.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 11.11.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 11.11.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 11.11.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 11.11.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 11.11.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 11.11.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 11.11.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 11.11.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 11.11.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 11.11.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 11.11.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1077,22 +1077,22 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 06.11.23
-DEH.N3LKT6.AP.COMPL.SNK : last exported on 06.11.23</t>
+          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 13.11.23
+DEH.N3LKT6.AP.COMPL.SNK : last exported on 13.11.23</t>
         </is>
       </c>
       <c r="D6" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 06.11.23
-DEL.N1LN3L.DN.F.GPL.DMP : last exported on 06.11.23
-DEL.N1LN3L.DN.F.GTR.DMP : last exported on 06.11.23
-DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 06.11.23
-DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 06.11.23
-DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 06.11.23
-DEL.N1LK61.DN.F.CPD.DMP : last exported on 06.11.23
-DEL.N1LN0R.DN.F.CPL.DMP : last exported on 06.11.23
-DEL.KT6E35.SN.F.GGO.ZIP : last exported on 06.11.23
-DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 06.11.23</t>
+          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 13.11.23
+DEL.N1LN3L.DN.F.GPL.DMP : last exported on 13.11.23
+DEL.N1LN3L.DN.F.GTR.DMP : last exported on 13.11.23
+DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 13.11.23
+DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 13.11.23
+DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 13.11.23
+DEL.N1LK61.DN.F.CPD.DMP : last exported on 13.11.23
+DEL.N1LN0R.DN.F.CPL.DMP : last exported on 13.11.23
+DEL.KT6E35.SN.F.GGO.ZIP : last exported on 13.11.23
+DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 13.11.23</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
@@ -1120,31 +1120,31 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 09.11.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 09.11.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 10.11.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 12.11.23
 DLV.RPKKT6.WI.S.ZIP : last exported on 09.11.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 09.11.23
-DIT.E35KT6.WI.ZIP : last exported on 09.11.23
-DEL.K2PKT6.WI.ZIP : last exported on 09.11.23
-DEL.R7AKT6.WI.ZIP : last exported on 10.11.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 11.11.23
+DIT.E35KT6.WI.ZIP : last exported on 10.11.23
+DEL.K2PKT6.WI.ZIP : last exported on 12.11.23
+DEL.R7AKT6.WI.ZIP : last exported on 13.11.23
 DEL.N5FKT6.WI.ZIP : last exported on 08.11.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 09.11.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 09.11.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 09.11.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 09.11.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 09.11.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 09.11.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 09.11.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 09.11.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 09.11.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 09.11.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 09.11.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 09.11.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 09.11.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 12.11.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 12.11.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 12.11.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 12.11.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 12.11.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 12.11.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 12.11.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 12.11.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 12.11.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 12.11.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 12.11.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 12.11.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 12.11.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 03.11.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 10.11.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 13.11.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 06.11.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 09.11.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 09.11.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 09.11.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 09.11.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 09.11.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 09.11.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 09.11.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 09.11.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 09.11.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 09.11.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 09.11.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 09.11.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 09.11.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 09.11.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 09.11.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 09.11.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 09.11.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 12.11.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 12.11.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 12.11.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 12.11.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 12.11.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 12.11.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 12.11.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 12.11.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 12.11.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 12.11.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 12.11.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 12.11.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 12.11.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 12.11.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 12.11.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 12.11.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 12.11.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1331,18 +1331,18 @@
       </c>
       <c r="C12" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.MANDANTN.TXT : last exported on 07.11.23</t>
+          <t>DEL.N3LKT6.MANDANTN.TXT : last exported on 11.11.23</t>
         </is>
       </c>
       <c r="D12" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 07.11.23
-DEL.N1LN3L.MC.F.GPL.DMP : last exported on 07.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 09.11.23
-DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 07.11.23
-DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 07.11.23
-DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 07.11.23
-DGI.KT6R11.MANDANT.TXT : last exported on 07.11.23</t>
+          <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 11.11.23
+DEL.N1LN3L.MC.F.GPL.DMP : last exported on 11.11.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 12.11.23
+DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 11.11.23
+DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 11.11.23
+DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 11.11.23
+DGI.KT6R11.MANDANT.TXT : last exported on 11.11.23</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 09.11.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 10.11.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 09.11.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 11.11.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1411,15 +1411,15 @@
       </c>
       <c r="D14" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 08.11.23
-DEL.N1LN3L.AU.D.GPL.DMP : last exported on 08.11.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 09.11.23
-DEL.KT6N5M.AU.GGO.ZIP : last exported on 08.11.23
-DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 08.11.23
-DEL.KT6KTZ.AU.GGO.ZIP : last exported on 08.11.23
-DEL.KT6KTZ.AU.IMG.GGO.ZIP : last exported on 08.11.23
-DEL.KT6E35.AU.GGO.ZIP : last exported on 08.11.23
-DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 08.11.23</t>
+          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 10.11.23
+DEL.N1LN3L.AU.D.GPL.DMP : last exported on 10.11.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 12.11.23
+DEL.KT6N5M.AU.GGO.ZIP : last exported on 10.11.23
+DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 10.11.23
+DEL.KT6KTZ.AU.GGO.ZIP : last exported on 10.11.23
+DEL.KT6KTZ.AU.IMG.GGO.ZIP : last exported on 10.11.23
+DEL.KT6E35.AU.GGO.ZIP : last exported on 10.11.23
+DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 10.11.23</t>
         </is>
       </c>
       <c r="E14" s="11" t="inlineStr">
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 09.11.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 09.11.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 12.11.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 12.11.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 09.11.23
-DHP.KUDKT6.ORGUNITS : last exported on 10.11.23
-DHS.R11KT6.HSB02ALL : last exported on 09.11.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 12.11.23
+DHP.KUDKT6.ORGUNITS : last exported on 13.11.23
+DHS.R11KT6.HSB02ALL : last exported on 10.11.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 09.11.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 09.11.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 09.11.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 09.11.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 09.11.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 09.11.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 09.11.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 09.11.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 09.11.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 09.11.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 10.11.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 10.11.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 12.11.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 10.11.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 10.11.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 10.11.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 10.11.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 10.11.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 10.11.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 10.11.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1620,7 +1620,7 @@
       </c>
       <c r="D19" s="16" t="inlineStr">
         <is>
-          <t>DEL.N1LE35.TRANS.ZIP : last exported on 05.11.23</t>
+          <t>DEL.N1LE35.TRANS.ZIP : last exported on 12.11.23</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 09.11.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 11.11.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 09.11.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 09.11.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 09.11.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 09.11.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 09.11.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 09.11.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 09.11.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 09.11.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 09.11.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 09.11.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 09.11.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 09.11.23
-DEL.N1LKT6.MT.??????.G : last exported on 09.11.23
-DEL.N1LKT6.MT.??????.U : last exported on 09.11.23
-DEL.N1LKT6.MT.??????.AS : last exported on 09.11.23
-DVL.N1LN5X.VLM.DSP : last exported on 09.11.23
-DVL.N1LN5X.VLM.WT : last exported on 09.11.23
-DDS.N1LR11.DSP : last exported on 09.11.23
-DDS.N1LR11.WT : last exported on 09.11.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 09.11.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 09.11.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 09.11.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 09.11.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 09.11.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 09.11.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 09.11.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 09.11.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 09.11.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 09.11.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 09.11.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 11.11.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 11.11.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 12.11.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 11.11.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 11.11.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 11.11.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 11.11.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 11.11.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 11.11.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 11.11.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 11.11.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 11.11.23
+DEL.N1LKT6.MT.??????.G : last exported on 11.11.23
+DEL.N1LKT6.MT.??????.U : last exported on 11.11.23
+DEL.N1LKT6.MT.??????.AS : last exported on 11.11.23
+DVL.N1LN5X.VLM.DSP : last exported on 11.11.23
+DVL.N1LN5X.VLM.WT : last exported on 11.11.23
+DDS.N1LR11.DSP : last exported on 11.11.23
+DDS.N1LR11.WT : last exported on 11.11.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 11.11.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 11.11.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 11.11.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 11.11.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 11.11.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 11.11.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 11.11.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 11.11.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 11.11.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 11.11.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 11.11.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,22 +1710,22 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 10.11.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 10.11.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 13.11.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 13.11.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 09.11.23
-DEL.N1LN3L.EM.F.GPL.DMP : last exported on 09.11.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 09.11.23
-DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 09.11.23
-DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 09.11.23
-DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 09.11.23
-DEL.N1LK61.EM.F.CPD.DMP : last exported on 09.11.23
-DEL.N1LN0R.EM.F.CPL.DMP : last exported on 09.11.23
-DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 09.11.23
-DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 09.11.23</t>
+          <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 10.11.23
+DEL.N1LN3L.EM.F.GPL.DMP : last exported on 10.11.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 12.11.23
+DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 10.11.23
+DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 10.11.23
+DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 10.11.23
+DEL.N1LK61.EM.F.CPD.DMP : last exported on 10.11.23
+DEL.N1LN0R.EM.F.CPL.DMP : last exported on 10.11.23
+DEL.N1LN3L.EM.F.DISS.ZIP : last exported on 10.11.23
+DEL.N1LN3L.EM.F.DISSA.ZIP : last exported on 10.11.23</t>
         </is>
       </c>
       <c r="E21" s="11" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 10.11.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 10.11.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 10.11.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 10.11.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 10.11.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 10.11.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 10.11.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 10.11.23
-DDC.R11KT6.ELFI.MD.TXT : last exported on 05.11.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 09.11.23
-DDC.R11KT6.ELFI.PK.TXT : last exported on 05.11.23
-DDC.R11KT6.ELFI.PR.TXT : last exported on 05.11.23</t>
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 13.11.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 13.11.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 13.11.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 13.11.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 13.11.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 13.11.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 13.11.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 13.11.23
+DDC.R11KT6.ELFI.MD.TXT : last exported on 12.11.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 10.11.23
+DDC.R11KT6.ELFI.PK.TXT : last exported on 12.11.23
+DDC.R11KT6.ELFI.PR.TXT : last exported on 12.11.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 09.11.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 09.11.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 09.11.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 09.11.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 09.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 09.11.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 09.11.23
-DEL.N1LKT6.EC.??????.G : last exported on 09.11.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 09.11.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 09.11.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 09.11.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 09.11.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 09.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 09.11.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 09.11.23
-DEL.N1LKT6.EC.??????.U : last exported on 09.11.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 09.11.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 09.11.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 09.11.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 09.11.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 09.11.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 09.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 09.11.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 09.11.23
-DEL.N1LKT6.EC.??????.AS : last exported on 09.11.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 09.11.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 09.11.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 09.11.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 09.11.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 09.11.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 09.11.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 09.11.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 09.11.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 12.11.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 12.11.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 12.11.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 12.11.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 12.11.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 12.11.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 12.11.23
+DEL.N1LKT6.EC.??????.G : last exported on 12.11.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 12.11.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 12.11.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 12.11.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 12.11.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 12.11.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 12.11.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 12.11.23
+DEL.N1LKT6.EC.??????.U : last exported on 12.11.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 12.11.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 12.11.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 12.11.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 12.11.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 12.11.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 12.11.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 12.11.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 12.11.23
+DEL.N1LKT6.EC.??????.AS : last exported on 12.11.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 12.11.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 12.11.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 12.11.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 12.11.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 12.11.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 12.11.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 12.11.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 12.11.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 14.11.23 14:05
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 13.11.2023</t>
+          <t>Date - 14.11.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 10.11.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 13.11.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 11.11.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 11.11.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 12.11.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 11.11.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 11.11.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 11.11.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 11.11.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 11.11.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 11.11.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 11.11.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 11.11.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 11.11.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 11.11.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 11.11.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 14.11.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 14.11.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 14.11.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 14.11.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 14.11.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 14.11.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 14.11.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 14.11.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 14.11.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 14.11.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 14.11.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 14.11.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 14.11.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 14.11.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1120,31 +1120,31 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 10.11.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 12.11.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 13.11.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 13.11.23
 DLV.RPKKT6.WI.S.ZIP : last exported on 09.11.23
 DLV.I5XKT6.WI.A.ZIP : last exported on 11.11.23
-DIT.E35KT6.WI.ZIP : last exported on 10.11.23
-DEL.K2PKT6.WI.ZIP : last exported on 12.11.23
+DIT.E35KT6.WI.ZIP : last exported on 13.11.23
+DEL.K2PKT6.WI.ZIP : last exported on 13.11.23
 DEL.R7AKT6.WI.ZIP : last exported on 13.11.23
 DEL.N5FKT6.WI.ZIP : last exported on 08.11.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 12.11.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 12.11.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 12.11.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 12.11.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 12.11.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 12.11.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 12.11.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 12.11.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 12.11.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 12.11.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 12.11.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 12.11.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 12.11.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 13.11.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 13.11.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 13.11.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 13.11.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 13.11.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 13.11.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 13.11.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 13.11.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 13.11.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 13.11.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 13.11.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 13.11.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 13.11.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 03.11.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 13.11.23
-DGV.N3LKT6.EPELS.??????.ZIP : last exported on 06.11.23</t>
+DEL.N3LKT6.HST.??????.ZIP : last exported on 14.11.23
+DGV.N3LKT6.EPELS.??????.ZIP : last exported on 13.11.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 12.11.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 12.11.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 12.11.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 12.11.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 12.11.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 12.11.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 12.11.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 12.11.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 12.11.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 12.11.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 12.11.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 12.11.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 12.11.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 12.11.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 12.11.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 12.11.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 12.11.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 13.11.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 13.11.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 13.11.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 13.11.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 13.11.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 13.11.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 13.11.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 13.11.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 13.11.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 13.11.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 13.11.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 13.11.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 13.11.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 13.11.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 13.11.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 13.11.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 13.11.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1298,12 +1298,12 @@
       </c>
       <c r="C11" s="14" t="inlineStr">
         <is>
-          <t>DEL.KT6KT6.APOSPRO.ZIP : last exported on 06.11.23</t>
+          <t>DEL.KT6KT6.APOSPRO.ZIP : last exported on 13.11.23</t>
         </is>
       </c>
       <c r="D11" s="15" t="inlineStr">
         <is>
-          <t>DEL.KT6N2O.XTIME.ZIP : last exported on 06.11.23</t>
+          <t>DEL.KT6N2O.XTIME.ZIP : last exported on 13.11.23</t>
         </is>
       </c>
       <c r="E11" s="11" t="inlineStr">
@@ -1338,7 +1338,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 11.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 11.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 12.11.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 13.11.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 11.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 11.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 11.11.23
@@ -1370,7 +1370,7 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 10.11.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 13.11.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
@@ -1413,7 +1413,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 10.11.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 10.11.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 12.11.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 13.11.23
 DEL.KT6N5M.AU.GGO.ZIP : last exported on 10.11.23
 DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 10.11.23
 DEL.KT6KTZ.AU.GGO.ZIP : last exported on 10.11.23
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 12.11.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 12.11.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 13.11.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 13.11.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 12.11.23
-DHP.KUDKT6.ORGUNITS : last exported on 13.11.23
-DHS.R11KT6.HSB02ALL : last exported on 10.11.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 13.11.23
+DHP.KUDKT6.ORGUNITS : last exported on 14.11.23
+DHS.R11KT6.HSB02ALL : last exported on 13.11.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 10.11.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 10.11.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 12.11.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 10.11.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 10.11.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 10.11.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 10.11.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 10.11.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 10.11.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 10.11.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 13.11.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 13.11.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 13.11.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 13.11.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 13.11.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 13.11.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 13.11.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 13.11.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 13.11.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 13.11.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 11.11.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 13.11.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 11.11.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 11.11.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 12.11.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 11.11.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 11.11.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 11.11.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 11.11.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 11.11.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 11.11.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 11.11.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 11.11.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 11.11.23
-DEL.N1LKT6.MT.??????.G : last exported on 11.11.23
-DEL.N1LKT6.MT.??????.U : last exported on 11.11.23
-DEL.N1LKT6.MT.??????.AS : last exported on 11.11.23
-DVL.N1LN5X.VLM.DSP : last exported on 11.11.23
-DVL.N1LN5X.VLM.WT : last exported on 11.11.23
-DDS.N1LR11.DSP : last exported on 11.11.23
-DDS.N1LR11.WT : last exported on 11.11.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 11.11.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 11.11.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 11.11.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 11.11.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 11.11.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 11.11.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 11.11.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 11.11.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 11.11.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 11.11.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 11.11.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 13.11.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 13.11.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 13.11.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 13.11.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 13.11.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 13.11.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 13.11.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 13.11.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 13.11.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 13.11.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 13.11.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 13.11.23
+DEL.N1LKT6.MT.??????.G : last exported on 13.11.23
+DEL.N1LKT6.MT.??????.U : last exported on 13.11.23
+DEL.N1LKT6.MT.??????.AS : last exported on 13.11.23
+DVL.N1LN5X.VLM.DSP : last exported on 13.11.23
+DVL.N1LN5X.VLM.WT : last exported on 13.11.23
+DDS.N1LR11.DSP : last exported on 13.11.23
+DDS.N1LR11.WT : last exported on 13.11.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 13.11.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 13.11.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 13.11.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 13.11.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 13.11.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 13.11.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 13.11.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 13.11.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 13.11.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 13.11.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 13.11.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,15 +1710,15 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 13.11.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 13.11.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 14.11.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 14.11.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 10.11.23
 DEL.N1LN3L.EM.F.GPL.DMP : last exported on 10.11.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 12.11.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 13.11.23
 DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 10.11.23
 DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 10.11.23
 DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 10.11.23
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 13.11.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 13.11.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 13.11.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 13.11.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 13.11.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 13.11.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 13.11.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 13.11.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 14.11.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 14.11.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 14.11.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 14.11.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 14.11.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 14.11.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 14.11.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 14.11.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 12.11.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 10.11.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 13.11.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 12.11.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 12.11.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 12.11.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 12.11.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 12.11.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 12.11.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 12.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 12.11.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 12.11.23
-DEL.N1LKT6.EC.??????.G : last exported on 12.11.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 12.11.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 12.11.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 12.11.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 12.11.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 12.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 12.11.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 12.11.23
-DEL.N1LKT6.EC.??????.U : last exported on 12.11.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 12.11.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 12.11.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 12.11.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 12.11.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 12.11.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 12.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 12.11.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 12.11.23
-DEL.N1LKT6.EC.??????.AS : last exported on 12.11.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 12.11.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 12.11.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 12.11.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 12.11.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 12.11.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 12.11.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 12.11.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 12.11.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 13.11.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 13.11.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 13.11.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 13.11.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 13.11.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 13.11.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 13.11.23
+DEL.N1LKT6.EC.??????.G : last exported on 13.11.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 13.11.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 13.11.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 13.11.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 13.11.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 13.11.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 13.11.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 13.11.23
+DEL.N1LKT6.EC.??????.U : last exported on 13.11.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 13.11.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 13.11.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 13.11.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 13.11.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 13.11.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 13.11.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 13.11.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 13.11.23
+DEL.N1LKT6.EC.??????.AS : last exported on 13.11.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 13.11.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 13.11.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 13.11.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 13.11.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 13.11.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 13.11.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 13.11.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 13.11.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 15.11.23 11:24
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 14.11.2023</t>
+          <t>Date - 15.11.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -1004,7 +1004,7 @@
         <is>
           <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 14.11.23
 DEL.N1LN3L.WD.D.GPL.DMP : last exported on 14.11.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 14.11.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 15.11.23
 DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 14.11.23
 DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 14.11.23
 DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 14.11.23
@@ -1132,13 +1132,13 @@
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 13.11.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 13.11.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 13.11.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 13.11.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 13.11.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 13.11.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 13.11.23
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 14.11.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 14.11.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 14.11.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 14.11.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 14.11.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 14.11.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 14.11.23
 DEL.KT6KTZ.WI.GGO.ZIP : last exported on 13.11.23
 DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 13.11.23
 DEL.KT6E35.WI.GGO.ZIP : last exported on 13.11.23
@@ -1254,14 +1254,14 @@
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 13.11.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 13.11.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 13.11.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 13.11.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 13.11.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 13.11.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 13.11.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 13.11.23
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 14.11.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 14.11.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 14.11.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 14.11.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 14.11.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 14.11.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 14.11.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 14.11.23
 DEL.KT6E35.TP.D.GGO.ZIP : last exported on 13.11.23
 DEL.KT6E35.TP.D.UGO.ZIP : last exported on 13.11.23
 DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 13.11.23
@@ -1338,7 +1338,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 11.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 11.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 13.11.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 14.11.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 11.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 11.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 11.11.23
@@ -1413,7 +1413,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 10.11.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 10.11.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 13.11.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 14.11.23
 DEL.KT6N5M.AU.GGO.ZIP : last exported on 10.11.23
 DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 10.11.23
 DEL.KT6KTZ.AU.GGO.ZIP : last exported on 10.11.23
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 13.11.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 13.11.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 14.11.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 14.11.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1543,16 +1543,16 @@
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 13.11.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 13.11.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 13.11.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 13.11.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 13.11.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 13.11.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 13.11.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 13.11.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 13.11.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 13.11.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 14.11.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 14.11.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 14.11.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 14.11.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 14.11.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 14.11.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 14.11.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 14.11.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 14.11.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 14.11.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1653,25 +1653,25 @@
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 13.11.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 13.11.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 13.11.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 13.11.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 13.11.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 13.11.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 13.11.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 13.11.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 13.11.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 13.11.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 13.11.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 13.11.23
-DEL.N1LKT6.MT.??????.G : last exported on 13.11.23
-DEL.N1LKT6.MT.??????.U : last exported on 13.11.23
-DEL.N1LKT6.MT.??????.AS : last exported on 13.11.23
-DVL.N1LN5X.VLM.DSP : last exported on 13.11.23
-DVL.N1LN5X.VLM.WT : last exported on 13.11.23
-DDS.N1LR11.DSP : last exported on 13.11.23
-DDS.N1LR11.WT : last exported on 13.11.23
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 14.11.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 14.11.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 14.11.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 14.11.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 14.11.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 14.11.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 14.11.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 14.11.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 14.11.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 14.11.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 14.11.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 14.11.23
+DEL.N1LKT6.MT.??????.G : last exported on 14.11.23
+DEL.N1LKT6.MT.??????.U : last exported on 14.11.23
+DEL.N1LKT6.MT.??????.AS : last exported on 14.11.23
+DVL.N1LN5X.VLM.DSP : last exported on 14.11.23
+DVL.N1LN5X.VLM.WT : last exported on 14.11.23
+DDS.N1LR11.DSP : last exported on 14.11.23
+DDS.N1LR11.WT : last exported on 14.11.23
 DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 13.11.23
 DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 13.11.23
 DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 13.11.23
@@ -1718,7 +1718,7 @@
         <is>
           <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 10.11.23
 DEL.N1LN3L.EM.F.GPL.DMP : last exported on 10.11.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 13.11.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 14.11.23
 DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 10.11.23
 DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 10.11.23
 DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 10.11.23
@@ -1769,38 +1769,38 @@
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 13.11.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 13.11.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 13.11.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 13.11.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 13.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 13.11.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 13.11.23
-DEL.N1LKT6.EC.??????.G : last exported on 13.11.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 13.11.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 13.11.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 13.11.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 13.11.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 13.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 13.11.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 13.11.23
-DEL.N1LKT6.EC.??????.U : last exported on 13.11.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 13.11.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 13.11.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 13.11.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 13.11.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 13.11.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 13.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 13.11.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 13.11.23
-DEL.N1LKT6.EC.??????.AS : last exported on 13.11.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 13.11.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 13.11.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 13.11.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 13.11.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 13.11.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 13.11.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 13.11.23
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 14.11.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 14.11.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 14.11.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 14.11.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 14.11.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 14.11.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 14.11.23
+DEL.N1LKT6.EC.??????.G : last exported on 14.11.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 14.11.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 14.11.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 14.11.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 14.11.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 14.11.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 14.11.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 14.11.23
+DEL.N1LKT6.EC.??????.U : last exported on 14.11.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 14.11.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 14.11.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 14.11.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 14.11.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 14.11.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 14.11.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 14.11.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 14.11.23
+DEL.N1LKT6.EC.??????.AS : last exported on 14.11.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 14.11.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 14.11.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 14.11.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 14.11.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 14.11.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 14.11.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 14.11.23
 DEL.KT6N5X.EL.F.AU.ZIP : last exported on 13.11.23</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Updated on 15.11.23 12:05
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -1120,13 +1120,13 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 13.11.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 13.11.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 09.11.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 11.11.23
-DIT.E35KT6.WI.ZIP : last exported on 13.11.23
-DEL.K2PKT6.WI.ZIP : last exported on 13.11.23
-DEL.R7AKT6.WI.ZIP : last exported on 13.11.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 14.11.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 14.11.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 14.11.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 14.11.23
+DIT.E35KT6.WI.ZIP : last exported on 14.11.23
+DEL.K2PKT6.WI.ZIP : last exported on 14.11.23
+DEL.R7AKT6.WI.ZIP : last exported on 15.11.23
 DEL.N5FKT6.WI.ZIP : last exported on 08.11.23</t>
         </is>
       </c>
@@ -1139,12 +1139,12 @@
 DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 14.11.23
 DEL.N1LK61.WI.D.CPD.DMP : last exported on 14.11.23
 DEL.N1LN0R.WI.D.CPL.DMP : last exported on 14.11.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 13.11.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 13.11.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 13.11.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 13.11.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 13.11.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 13.11.23</t>
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 14.11.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 14.11.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 14.11.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 14.11.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 14.11.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 14.11.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1248,7 +1248,7 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 03.11.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 14.11.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 15.11.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 13.11.23</t>
         </is>
       </c>
@@ -1262,15 +1262,15 @@
 DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 14.11.23
 DEL.N1LK61.TP.D.CPD.DMP : last exported on 14.11.23
 DEL.N1LN0R.TP.D.CPL.DMP : last exported on 14.11.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 13.11.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 13.11.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 13.11.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 13.11.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 13.11.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 13.11.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 13.11.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 13.11.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 13.11.23</t>
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 14.11.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 14.11.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 14.11.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 14.11.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 14.11.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 14.11.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 14.11.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 14.11.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 14.11.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 13.11.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 14.11.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 11.11.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 14.11.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1536,9 +1536,9 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 13.11.23
-DHP.KUDKT6.ORGUNITS : last exported on 14.11.23
-DHS.R11KT6.HSB02ALL : last exported on 13.11.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 14.11.23
+DHP.KUDKT6.ORGUNITS : last exported on 15.11.23
+DHS.R11KT6.HSB02ALL : last exported on 14.11.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
@@ -1648,7 +1648,7 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 13.11.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 14.11.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
@@ -1672,17 +1672,17 @@
 DVL.N1LN5X.VLM.WT : last exported on 14.11.23
 DDS.N1LR11.DSP : last exported on 14.11.23
 DDS.N1LR11.WT : last exported on 14.11.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 13.11.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 13.11.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 13.11.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 13.11.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 13.11.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 13.11.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 13.11.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 13.11.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 13.11.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 13.11.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 13.11.23</t>
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 14.11.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 14.11.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 14.11.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 14.11.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 14.11.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 14.11.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 14.11.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 14.11.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 14.11.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 14.11.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 14.11.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,8 +1710,8 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 14.11.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 14.11.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 15.11.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 15.11.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
@@ -1753,16 +1753,16 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 14.11.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 14.11.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 14.11.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 14.11.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 14.11.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 14.11.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 14.11.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 14.11.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 15.11.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 15.11.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 15.11.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 15.11.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 15.11.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 15.11.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 15.11.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 15.11.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 12.11.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 13.11.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 14.11.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 12.11.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 12.11.23</t>
         </is>
@@ -1801,7 +1801,7 @@
 DGV.N1LN7K.EL.F.ZIP : last exported on 14.11.23
 DGV.N1LN5X.EL.F.ZIP : last exported on 14.11.23
 DEL.KT6KT6.EL.F.DRE.CSV : last exported on 14.11.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 13.11.23</t>
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 14.11.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 16.11.23 10:51
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 15.11.2023</t>
+          <t>Date - 16.11.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 13.11.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 15.11.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 14.11.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 14.11.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 15.11.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 14.11.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 14.11.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 14.11.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 14.11.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 14.11.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 14.11.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 14.11.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 14.11.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 14.11.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 14.11.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 14.11.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 16.11.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 16.11.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 16.11.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 16.11.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 16.11.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 16.11.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 16.11.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 16.11.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 16.11.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 16.11.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 16.11.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 16.11.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 16.11.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 16.11.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1120,31 +1120,31 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 14.11.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 14.11.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 15.11.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 15.11.23
 DLV.RPKKT6.WI.S.ZIP : last exported on 14.11.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 14.11.23
-DIT.E35KT6.WI.ZIP : last exported on 14.11.23
-DEL.K2PKT6.WI.ZIP : last exported on 14.11.23
-DEL.R7AKT6.WI.ZIP : last exported on 15.11.23
-DEL.N5FKT6.WI.ZIP : last exported on 08.11.23</t>
+DLV.I5XKT6.WI.A.ZIP : last exported on 15.11.23
+DIT.E35KT6.WI.ZIP : last exported on 15.11.23
+DEL.K2PKT6.WI.ZIP : last exported on 15.11.23
+DEL.R7AKT6.WI.ZIP : last exported on 16.11.23
+DEL.N5FKT6.WI.ZIP : last exported on 15.11.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 14.11.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 14.11.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 14.11.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 14.11.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 14.11.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 14.11.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 14.11.23
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 15.11.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 15.11.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 15.11.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 15.11.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 15.11.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 15.11.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 15.11.23
 DEL.KT6KTZ.WI.GGO.ZIP : last exported on 14.11.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 14.11.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 14.11.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 14.11.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 14.11.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 14.11.23</t>
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 15.11.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 15.11.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 15.11.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 15.11.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 15.11.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 03.11.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 15.11.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 16.11.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 13.11.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 14.11.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 14.11.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 14.11.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 14.11.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 14.11.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 14.11.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 14.11.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 14.11.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 14.11.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 14.11.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 14.11.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 14.11.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 14.11.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 14.11.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 14.11.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 14.11.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 14.11.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 15.11.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 15.11.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 15.11.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 15.11.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 15.11.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 15.11.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 15.11.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 15.11.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 15.11.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 15.11.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 15.11.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 15.11.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 15.11.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 15.11.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 15.11.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 15.11.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 15.11.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1331,18 +1331,18 @@
       </c>
       <c r="C12" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.MANDANTN.TXT : last exported on 11.11.23</t>
+          <t>DEL.N3LKT6.MANDANTN.TXT : last exported on 15.11.23</t>
         </is>
       </c>
       <c r="D12" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 11.11.23
-DEL.N1LN3L.MC.F.GPL.DMP : last exported on 11.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 14.11.23
-DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 11.11.23
-DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 11.11.23
-DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 11.11.23
-DGI.KT6R11.MANDANT.TXT : last exported on 11.11.23</t>
+          <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 15.11.23
+DEL.N1LN3L.MC.F.GPL.DMP : last exported on 15.11.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 15.11.23
+DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 15.11.23
+DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 15.11.23
+DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 15.11.23
+DGI.KT6R11.MANDANT.TXT : last exported on 15.11.23</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 14.11.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 15.11.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 14.11.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 15.11.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1413,7 +1413,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 10.11.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 10.11.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 14.11.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 15.11.23
 DEL.KT6N5M.AU.GGO.ZIP : last exported on 10.11.23
 DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 10.11.23
 DEL.KT6KTZ.AU.GGO.ZIP : last exported on 10.11.23
@@ -1457,24 +1457,24 @@
 DGQ.R11KT6.BSITX.TXT : last exported on 01.11.23
 DGQ.R31KT6.BSIVMC.TXT : last exported on 07.11.23
 DGQ.R31KT6.PKATC.TXT : last exported on 07.11.23
-DEL.KMPKT6.APOS.DATA.ZIP : last exported on 08.11.23</t>
+DEL.KMPKT6.APOS.DATA.ZIP : last exported on 15.11.23</t>
         </is>
       </c>
       <c r="D15" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 08.11.23
-DEL.N1LN3L.AP.F.GPL.DMP : last exported on 08.11.23
-DEL.N1LN3L.AP.F.GTR.DMP : last exported on 08.11.23
-DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 08.11.23
-DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 08.11.23
-DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 08.11.23
-DEL.N1LK61.AP.F.CPD.DMP : last exported on 08.11.23
-DEL.N1LN0R.AP.F.CPL.DMP : last exported on 08.11.23
-DEL.N1LR31.AP.F.PPS.DMP : last exported on 08.11.23
-DEL.KT6E35.AP.F.DB.ZIP : last exported on 08.11.23
-DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 08.11.23
-DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 08.11.23
-DVL.KT6N5X.VLM.AP.ZIP : last exported on 08.11.23</t>
+          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 15.11.23
+DEL.N1LN3L.AP.F.GPL.DMP : last exported on 15.11.23
+DEL.N1LN3L.AP.F.GTR.DMP : last exported on 15.11.23
+DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 15.11.23
+DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 15.11.23
+DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 15.11.23
+DEL.N1LK61.AP.F.CPD.DMP : last exported on 15.11.23
+DEL.N1LN0R.AP.F.CPL.DMP : last exported on 15.11.23
+DEL.N1LR31.AP.F.PPS.DMP : last exported on 15.11.23
+DEL.KT6E35.AP.F.DB.ZIP : last exported on 15.11.23
+DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 15.11.23
+DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 15.11.23
+DVL.KT6N5X.VLM.AP.ZIP : last exported on 15.11.23</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 14.11.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 14.11.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 15.11.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 15.11.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 14.11.23
-DHP.KUDKT6.ORGUNITS : last exported on 15.11.23
-DHS.R11KT6.HSB02ALL : last exported on 14.11.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 15.11.23
+DHP.KUDKT6.ORGUNITS : last exported on 16.11.23
+DHS.R11KT6.HSB02ALL : last exported on 15.11.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 14.11.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 14.11.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 14.11.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 14.11.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 14.11.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 14.11.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 14.11.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 14.11.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 14.11.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 14.11.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 15.11.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 15.11.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 15.11.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 15.11.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 15.11.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 15.11.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 15.11.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 15.11.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 15.11.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 15.11.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 14.11.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 15.11.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 14.11.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 14.11.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 14.11.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 14.11.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 14.11.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 14.11.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 14.11.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 14.11.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 14.11.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 14.11.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 14.11.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 14.11.23
-DEL.N1LKT6.MT.??????.G : last exported on 14.11.23
-DEL.N1LKT6.MT.??????.U : last exported on 14.11.23
-DEL.N1LKT6.MT.??????.AS : last exported on 14.11.23
-DVL.N1LN5X.VLM.DSP : last exported on 14.11.23
-DVL.N1LN5X.VLM.WT : last exported on 14.11.23
-DDS.N1LR11.DSP : last exported on 14.11.23
-DDS.N1LR11.WT : last exported on 14.11.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 14.11.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 14.11.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 14.11.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 14.11.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 14.11.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 14.11.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 14.11.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 14.11.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 14.11.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 14.11.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 14.11.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 15.11.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 15.11.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 15.11.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 15.11.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 15.11.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 15.11.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 15.11.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 15.11.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 15.11.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 15.11.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 15.11.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 15.11.23
+DEL.N1LKT6.MT.??????.G : last exported on 15.11.23
+DEL.N1LKT6.MT.??????.U : last exported on 15.11.23
+DEL.N1LKT6.MT.??????.AS : last exported on 15.11.23
+DVL.N1LN5X.VLM.DSP : last exported on 15.11.23
+DVL.N1LN5X.VLM.WT : last exported on 15.11.23
+DDS.N1LR11.DSP : last exported on 15.11.23
+DDS.N1LR11.WT : last exported on 15.11.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 15.11.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 15.11.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 15.11.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 15.11.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 15.11.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 15.11.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 15.11.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 15.11.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 15.11.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 15.11.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 15.11.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,15 +1710,15 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 15.11.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 15.11.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 16.11.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 16.11.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 10.11.23
 DEL.N1LN3L.EM.F.GPL.DMP : last exported on 10.11.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 14.11.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 15.11.23
 DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 10.11.23
 DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 10.11.23
 DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 10.11.23
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 15.11.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 15.11.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 15.11.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 15.11.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 15.11.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 15.11.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 15.11.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 15.11.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 16.11.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 16.11.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 16.11.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 16.11.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 16.11.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 16.11.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 16.11.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 16.11.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 12.11.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 14.11.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 15.11.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 12.11.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 12.11.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 14.11.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 14.11.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 14.11.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 14.11.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 14.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 14.11.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 14.11.23
-DEL.N1LKT6.EC.??????.G : last exported on 14.11.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 14.11.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 14.11.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 14.11.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 14.11.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 14.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 14.11.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 14.11.23
-DEL.N1LKT6.EC.??????.U : last exported on 14.11.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 14.11.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 14.11.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 14.11.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 14.11.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 14.11.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 14.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 14.11.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 14.11.23
-DEL.N1LKT6.EC.??????.AS : last exported on 14.11.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 14.11.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 14.11.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 14.11.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 14.11.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 14.11.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 14.11.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 14.11.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 14.11.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 15.11.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 15.11.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 15.11.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 15.11.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 15.11.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 15.11.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 15.11.23
+DEL.N1LKT6.EC.??????.G : last exported on 15.11.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 15.11.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 15.11.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 15.11.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 15.11.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 15.11.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 15.11.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 15.11.23
+DEL.N1LKT6.EC.??????.U : last exported on 15.11.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 15.11.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 15.11.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 15.11.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 15.11.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 15.11.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 15.11.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 15.11.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 15.11.23
+DEL.N1LKT6.EC.??????.AS : last exported on 15.11.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 15.11.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 15.11.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 15.11.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 15.11.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 15.11.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 15.11.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 15.11.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 15.11.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 21.11.23 14:10
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 16.11.2023</t>
+          <t>Date - 21.11.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 15.11.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 20.11.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 16.11.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 16.11.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 16.11.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 16.11.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 16.11.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 16.11.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 16.11.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 16.11.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 16.11.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 16.11.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 16.11.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 16.11.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 16.11.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 16.11.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 21.11.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 21.11.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 21.11.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 21.11.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 21.11.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 21.11.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 21.11.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 21.11.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 21.11.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 21.11.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 21.11.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 21.11.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 21.11.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 21.11.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1077,22 +1077,22 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 13.11.23
-DEH.N3LKT6.AP.COMPL.SNK : last exported on 13.11.23</t>
+          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 20.11.23
+DEH.N3LKT6.AP.COMPL.SNK : last exported on 20.11.23</t>
         </is>
       </c>
       <c r="D6" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 13.11.23
-DEL.N1LN3L.DN.F.GPL.DMP : last exported on 13.11.23
-DEL.N1LN3L.DN.F.GTR.DMP : last exported on 13.11.23
-DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 13.11.23
-DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 13.11.23
-DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 13.11.23
-DEL.N1LK61.DN.F.CPD.DMP : last exported on 13.11.23
-DEL.N1LN0R.DN.F.CPL.DMP : last exported on 13.11.23
-DEL.KT6E35.SN.F.GGO.ZIP : last exported on 13.11.23
-DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 13.11.23</t>
+          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 20.11.23
+DEL.N1LN3L.DN.F.GPL.DMP : last exported on 20.11.23
+DEL.N1LN3L.DN.F.GTR.DMP : last exported on 20.11.23
+DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 20.11.23
+DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 20.11.23
+DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 20.11.23
+DEL.N1LK61.DN.F.CPD.DMP : last exported on 20.11.23
+DEL.N1LN0R.DN.F.CPL.DMP : last exported on 20.11.23
+DEL.KT6E35.SN.F.GGO.ZIP : last exported on 20.11.23
+DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 20.11.23</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
@@ -1120,31 +1120,31 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 15.11.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 15.11.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 14.11.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 15.11.23
-DIT.E35KT6.WI.ZIP : last exported on 15.11.23
-DEL.K2PKT6.WI.ZIP : last exported on 15.11.23
-DEL.R7AKT6.WI.ZIP : last exported on 16.11.23
-DEL.N5FKT6.WI.ZIP : last exported on 15.11.23</t>
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 20.11.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 19.11.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 20.11.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 20.11.23
+DIT.E35KT6.WI.ZIP : last exported on 20.11.23
+DEL.K2PKT6.WI.ZIP : last exported on 20.11.23
+DEL.R7AKT6.WI.ZIP : last exported on 21.11.23
+DEL.N5FKT6.WI.ZIP : last exported on 20.11.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 15.11.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 15.11.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 15.11.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 15.11.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 15.11.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 15.11.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 15.11.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 14.11.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 15.11.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 15.11.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 15.11.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 15.11.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 15.11.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 20.11.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 20.11.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 20.11.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 20.11.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 20.11.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 20.11.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 20.11.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 20.11.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 20.11.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 20.11.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 20.11.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 20.11.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 20.11.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 03.11.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 16.11.23
-DGV.N3LKT6.EPELS.??????.ZIP : last exported on 13.11.23</t>
+DEL.N3LKT6.HST.??????.ZIP : last exported on 21.11.23
+DGV.N3LKT6.EPELS.??????.ZIP : last exported on 20.11.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 15.11.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 15.11.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 15.11.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 15.11.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 15.11.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 15.11.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 15.11.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 15.11.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 15.11.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 15.11.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 15.11.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 15.11.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 15.11.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 15.11.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 15.11.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 15.11.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 15.11.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 20.11.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 20.11.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 20.11.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 20.11.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 20.11.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 20.11.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 20.11.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 20.11.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 20.11.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 20.11.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 20.11.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 20.11.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 20.11.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 20.11.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 20.11.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 20.11.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 20.11.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1298,12 +1298,12 @@
       </c>
       <c r="C11" s="14" t="inlineStr">
         <is>
-          <t>DEL.KT6KT6.APOSPRO.ZIP : last exported on 13.11.23</t>
+          <t>DEL.KT6KT6.APOSPRO.ZIP : last exported on 20.11.23</t>
         </is>
       </c>
       <c r="D11" s="15" t="inlineStr">
         <is>
-          <t>DEL.KT6N2O.XTIME.ZIP : last exported on 13.11.23</t>
+          <t>DEL.KT6N2O.XTIME.ZIP : last exported on 20.11.23</t>
         </is>
       </c>
       <c r="E11" s="11" t="inlineStr">
@@ -1338,7 +1338,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 15.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 15.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 15.11.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 20.11.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 15.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 15.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 15.11.23
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 15.11.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 20.11.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 15.11.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 18.11.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1413,7 +1413,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 10.11.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 10.11.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 15.11.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 20.11.23
 DEL.KT6N5M.AU.GGO.ZIP : last exported on 10.11.23
 DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 10.11.23
 DEL.KT6KTZ.AU.GGO.ZIP : last exported on 10.11.23
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 15.11.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 15.11.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 20.11.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 20.11.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 15.11.23
-DHP.KUDKT6.ORGUNITS : last exported on 16.11.23
-DHS.R11KT6.HSB02ALL : last exported on 15.11.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 20.11.23
+DHP.KUDKT6.ORGUNITS : last exported on 21.11.23
+DHS.R11KT6.HSB02ALL : last exported on 17.11.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 15.11.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 15.11.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 15.11.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 15.11.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 15.11.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 15.11.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 15.11.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 15.11.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 15.11.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 15.11.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 20.11.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 20.11.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 20.11.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 20.11.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 20.11.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 20.11.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 20.11.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 20.11.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 20.11.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 20.11.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1615,12 +1615,12 @@
       </c>
       <c r="C19" s="16" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.TRANS.ZIP : last exported on 09.01.23</t>
+          <t>DIT.E35KT6.TRANS.ZIP : last exported on 20.11.23</t>
         </is>
       </c>
       <c r="D19" s="16" t="inlineStr">
         <is>
-          <t>DEL.N1LE35.TRANS.ZIP : last exported on 12.11.23</t>
+          <t>DEL.N1LE35.TRANS.ZIP : last exported on 19.11.23</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 15.11.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 20.11.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 15.11.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 15.11.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 15.11.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 15.11.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 15.11.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 15.11.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 15.11.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 15.11.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 15.11.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 15.11.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 15.11.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 15.11.23
-DEL.N1LKT6.MT.??????.G : last exported on 15.11.23
-DEL.N1LKT6.MT.??????.U : last exported on 15.11.23
-DEL.N1LKT6.MT.??????.AS : last exported on 15.11.23
-DVL.N1LN5X.VLM.DSP : last exported on 15.11.23
-DVL.N1LN5X.VLM.WT : last exported on 15.11.23
-DDS.N1LR11.DSP : last exported on 15.11.23
-DDS.N1LR11.WT : last exported on 15.11.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 15.11.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 15.11.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 15.11.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 15.11.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 15.11.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 15.11.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 15.11.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 15.11.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 15.11.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 15.11.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 15.11.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 20.11.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 20.11.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 20.11.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 20.11.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 20.11.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 20.11.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 20.11.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 20.11.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 20.11.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 20.11.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 20.11.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 20.11.23
+DEL.N1LKT6.MT.??????.G : last exported on 20.11.23
+DEL.N1LKT6.MT.??????.U : last exported on 20.11.23
+DEL.N1LKT6.MT.??????.AS : last exported on 20.11.23
+DVL.N1LN5X.VLM.DSP : last exported on 20.11.23
+DVL.N1LN5X.VLM.WT : last exported on 20.11.23
+DDS.N1LR11.DSP : last exported on 20.11.23
+DDS.N1LR11.WT : last exported on 20.11.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 20.11.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 20.11.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 20.11.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 20.11.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 20.11.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 20.11.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 20.11.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 20.11.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 20.11.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 20.11.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 20.11.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,15 +1710,15 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 16.11.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 16.11.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 21.11.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 21.11.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.EM.F.GPD.DMP : last exported on 10.11.23
 DEL.N1LN3L.EM.F.GPL.DMP : last exported on 10.11.23
-DEL.N1LN3L.EM.F.GTR.DMP : last exported on 15.11.23
+DEL.N1LN3L.EM.F.GTR.DMP : last exported on 19.11.23
 DEL.N1LKQQ.EM.F.UPD.DMP : last exported on 10.11.23
 DEL.N1LN3L.EM.F.ASPD.DMP : last exported on 10.11.23
 DEL.N1LN3L.EM.F.ASPL.DMP : last exported on 10.11.23
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 16.11.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 16.11.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 16.11.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 16.11.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 16.11.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 16.11.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 16.11.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 16.11.23
-DDC.R11KT6.ELFI.MD.TXT : last exported on 12.11.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 15.11.23
-DDC.R11KT6.ELFI.PK.TXT : last exported on 12.11.23
-DDC.R11KT6.ELFI.PR.TXT : last exported on 12.11.23</t>
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 21.11.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 21.11.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 21.11.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 21.11.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 21.11.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 21.11.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 21.11.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 21.11.23
+DDC.R11KT6.ELFI.MD.TXT : last exported on 19.11.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 20.11.23
+DDC.R11KT6.ELFI.PK.TXT : last exported on 19.11.23
+DDC.R11KT6.ELFI.PR.TXT : last exported on 19.11.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 15.11.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 15.11.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 15.11.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 15.11.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 15.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 15.11.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 15.11.23
-DEL.N1LKT6.EC.??????.G : last exported on 15.11.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 15.11.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 15.11.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 15.11.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 15.11.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 15.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 15.11.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 15.11.23
-DEL.N1LKT6.EC.??????.U : last exported on 15.11.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 15.11.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 15.11.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 15.11.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 15.11.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 15.11.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 15.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 15.11.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 15.11.23
-DEL.N1LKT6.EC.??????.AS : last exported on 15.11.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 15.11.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 15.11.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 15.11.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 15.11.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 15.11.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 15.11.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 15.11.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 15.11.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 20.11.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 20.11.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 20.11.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 20.11.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 20.11.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 20.11.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 20.11.23
+DEL.N1LKT6.EC.??????.G : last exported on 20.11.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 20.11.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 20.11.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 20.11.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 20.11.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 20.11.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 20.11.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 20.11.23
+DEL.N1LKT6.EC.??????.U : last exported on 20.11.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 20.11.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 20.11.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 20.11.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 20.11.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 20.11.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 20.11.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 20.11.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 20.11.23
+DEL.N1LKT6.EC.??????.AS : last exported on 20.11.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 20.11.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 20.11.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 20.11.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 20.11.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 20.11.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 20.11.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 20.11.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 20.11.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 22.11.23 09:38
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 21.11.2023</t>
+          <t>Date - 22.11.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,7 +997,7 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 20.11.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 21.11.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
@@ -1120,31 +1120,31 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 20.11.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 19.11.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 20.11.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 20.11.23
-DIT.E35KT6.WI.ZIP : last exported on 20.11.23
-DEL.K2PKT6.WI.ZIP : last exported on 20.11.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 21.11.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 21.11.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 21.11.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 21.11.23
+DIT.E35KT6.WI.ZIP : last exported on 21.11.23
+DEL.K2PKT6.WI.ZIP : last exported on 21.11.23
 DEL.R7AKT6.WI.ZIP : last exported on 21.11.23
 DEL.N5FKT6.WI.ZIP : last exported on 20.11.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 20.11.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 20.11.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 20.11.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 20.11.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 20.11.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 20.11.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 20.11.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 20.11.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 20.11.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 20.11.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 20.11.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 20.11.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 20.11.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 21.11.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 21.11.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 21.11.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 21.11.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 21.11.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 21.11.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 21.11.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 21.11.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 21.11.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 21.11.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 21.11.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 21.11.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 21.11.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 03.11.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 21.11.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 22.11.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 20.11.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 20.11.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 20.11.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 20.11.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 20.11.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 20.11.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 20.11.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 20.11.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 20.11.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 20.11.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 20.11.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 20.11.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 20.11.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 20.11.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 20.11.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 20.11.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 20.11.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 20.11.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 21.11.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 21.11.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 21.11.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 21.11.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 21.11.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 21.11.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 21.11.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 21.11.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 21.11.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 21.11.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 21.11.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 21.11.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 21.11.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 21.11.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 21.11.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 21.11.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 21.11.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1338,7 +1338,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 15.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 15.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 20.11.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 21.11.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 15.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 15.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 15.11.23
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 20.11.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 21.11.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 18.11.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 21.11.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1413,7 +1413,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 10.11.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 10.11.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 20.11.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 21.11.23
 DEL.KT6N5M.AU.GGO.ZIP : last exported on 10.11.23
 DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 10.11.23
 DEL.KT6KTZ.AU.GGO.ZIP : last exported on 10.11.23
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 20.11.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 20.11.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 21.11.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 21.11.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,8 +1536,8 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 20.11.23
-DHP.KUDKT6.ORGUNITS : last exported on 21.11.23
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 21.11.23
+DHP.KUDKT6.ORGUNITS : last exported on 22.11.23
 DHS.R11KT6.HSB02ALL : last exported on 17.11.23</t>
         </is>
       </c>
@@ -1545,7 +1545,7 @@
         <is>
           <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 20.11.23
 DEL.N1LN3L.DP.F.GPL.DMP : last exported on 20.11.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 20.11.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 21.11.23
 DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 20.11.23
 DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 20.11.23
 DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 20.11.23
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 20.11.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 21.11.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 20.11.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 20.11.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 20.11.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 20.11.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 20.11.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 20.11.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 20.11.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 20.11.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 20.11.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 20.11.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 20.11.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 20.11.23
-DEL.N1LKT6.MT.??????.G : last exported on 20.11.23
-DEL.N1LKT6.MT.??????.U : last exported on 20.11.23
-DEL.N1LKT6.MT.??????.AS : last exported on 20.11.23
-DVL.N1LN5X.VLM.DSP : last exported on 20.11.23
-DVL.N1LN5X.VLM.WT : last exported on 20.11.23
-DDS.N1LR11.DSP : last exported on 20.11.23
-DDS.N1LR11.WT : last exported on 20.11.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 20.11.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 20.11.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 20.11.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 20.11.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 20.11.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 20.11.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 20.11.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 20.11.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 20.11.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 20.11.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 20.11.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 21.11.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 21.11.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 21.11.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 21.11.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 21.11.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 21.11.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 21.11.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 21.11.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 21.11.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 21.11.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 21.11.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 21.11.23
+DEL.N1LKT6.MT.??????.G : last exported on 21.11.23
+DEL.N1LKT6.MT.??????.U : last exported on 21.11.23
+DEL.N1LKT6.MT.??????.AS : last exported on 21.11.23
+DVL.N1LN5X.VLM.DSP : last exported on 21.11.23
+DVL.N1LN5X.VLM.WT : last exported on 21.11.23
+DDS.N1LR11.DSP : last exported on 21.11.23
+DDS.N1LR11.WT : last exported on 21.11.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 21.11.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 21.11.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 21.11.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 21.11.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 21.11.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 21.11.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 21.11.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 21.11.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 21.11.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 21.11.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 21.11.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1711,7 +1711,7 @@
       <c r="C21" s="10" t="inlineStr">
         <is>
           <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 21.11.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 21.11.23</t>
+DHP.KUDKT6.DPO.EMAILS : last exported on 22.11.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
@@ -1762,46 +1762,46 @@
 DKG.R11KT6.L520.P.EDCP.TGE : last exported on 21.11.23
 DKG.R11KT6.L520.P.EDCP.TMO : last exported on 21.11.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 19.11.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 20.11.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 21.11.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 19.11.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 19.11.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 20.11.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 20.11.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 20.11.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 20.11.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 20.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 20.11.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 20.11.23
-DEL.N1LKT6.EC.??????.G : last exported on 20.11.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 20.11.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 20.11.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 20.11.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 20.11.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 20.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 20.11.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 20.11.23
-DEL.N1LKT6.EC.??????.U : last exported on 20.11.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 20.11.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 20.11.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 20.11.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 20.11.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 20.11.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 20.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 20.11.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 20.11.23
-DEL.N1LKT6.EC.??????.AS : last exported on 20.11.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 20.11.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 20.11.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 20.11.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 20.11.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 20.11.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 20.11.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 20.11.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 20.11.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 21.11.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 21.11.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 21.11.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 21.11.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 21.11.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 21.11.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 21.11.23
+DEL.N1LKT6.EC.??????.G : last exported on 21.11.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 21.11.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 21.11.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 21.11.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 21.11.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 21.11.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 21.11.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 21.11.23
+DEL.N1LKT6.EC.??????.U : last exported on 21.11.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 21.11.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 21.11.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 21.11.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 21.11.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 21.11.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 21.11.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 21.11.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 21.11.23
+DEL.N1LKT6.EC.??????.AS : last exported on 21.11.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 21.11.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 21.11.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 21.11.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 21.11.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 21.11.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 21.11.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 21.11.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 21.11.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 23.11.23 09:09
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 22.11.2023</t>
+          <t>Date - 23.11.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 21.11.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 22.11.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 21.11.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 21.11.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 21.11.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 21.11.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 21.11.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 21.11.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 21.11.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 21.11.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 21.11.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 21.11.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 21.11.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 21.11.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 21.11.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 21.11.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 23.11.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 23.11.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 23.11.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 23.11.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 23.11.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 23.11.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 23.11.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 23.11.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 23.11.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 23.11.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 23.11.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 23.11.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 23.11.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 23.11.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1120,31 +1120,31 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 21.11.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 21.11.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 21.11.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 21.11.23
-DIT.E35KT6.WI.ZIP : last exported on 21.11.23
-DEL.K2PKT6.WI.ZIP : last exported on 21.11.23
-DEL.R7AKT6.WI.ZIP : last exported on 21.11.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 22.11.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 22.11.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 22.11.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 22.11.23
+DIT.E35KT6.WI.ZIP : last exported on 22.11.23
+DEL.K2PKT6.WI.ZIP : last exported on 22.11.23
+DEL.R7AKT6.WI.ZIP : last exported on 23.11.23
 DEL.N5FKT6.WI.ZIP : last exported on 20.11.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 21.11.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 21.11.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 21.11.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 21.11.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 21.11.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 21.11.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 21.11.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 21.11.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 21.11.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 21.11.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 21.11.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 21.11.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 21.11.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 22.11.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 22.11.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 22.11.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 22.11.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 22.11.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 22.11.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 22.11.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 22.11.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 22.11.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 22.11.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 22.11.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 22.11.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 22.11.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 03.11.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 22.11.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 23.11.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 20.11.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 21.11.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 21.11.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 21.11.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 21.11.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 21.11.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 21.11.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 21.11.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 21.11.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 21.11.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 21.11.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 21.11.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 21.11.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 21.11.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 21.11.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 21.11.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 21.11.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 21.11.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 22.11.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 22.11.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 22.11.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 22.11.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 22.11.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 22.11.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 22.11.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 22.11.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 22.11.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 22.11.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 22.11.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 22.11.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 22.11.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 22.11.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 22.11.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 22.11.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 22.11.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1338,7 +1338,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 15.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 15.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 21.11.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 22.11.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 15.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 15.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 15.11.23
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 21.11.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 22.11.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 21.11.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 22.11.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1413,7 +1413,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 10.11.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 10.11.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 21.11.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 22.11.23
 DEL.KT6N5M.AU.GGO.ZIP : last exported on 10.11.23
 DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 10.11.23
 DEL.KT6KTZ.AU.GGO.ZIP : last exported on 10.11.23
@@ -1457,24 +1457,24 @@
 DGQ.R11KT6.BSITX.TXT : last exported on 01.11.23
 DGQ.R31KT6.BSIVMC.TXT : last exported on 07.11.23
 DGQ.R31KT6.PKATC.TXT : last exported on 07.11.23
-DEL.KMPKT6.APOS.DATA.ZIP : last exported on 15.11.23</t>
+DEL.KMPKT6.APOS.DATA.ZIP : last exported on 22.11.23</t>
         </is>
       </c>
       <c r="D15" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 15.11.23
-DEL.N1LN3L.AP.F.GPL.DMP : last exported on 15.11.23
-DEL.N1LN3L.AP.F.GTR.DMP : last exported on 15.11.23
-DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 15.11.23
-DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 15.11.23
-DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 15.11.23
-DEL.N1LK61.AP.F.CPD.DMP : last exported on 15.11.23
-DEL.N1LN0R.AP.F.CPL.DMP : last exported on 15.11.23
-DEL.N1LR31.AP.F.PPS.DMP : last exported on 15.11.23
-DEL.KT6E35.AP.F.DB.ZIP : last exported on 15.11.23
-DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 15.11.23
-DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 15.11.23
-DVL.KT6N5X.VLM.AP.ZIP : last exported on 15.11.23</t>
+          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 22.11.23
+DEL.N1LN3L.AP.F.GPL.DMP : last exported on 22.11.23
+DEL.N1LN3L.AP.F.GTR.DMP : last exported on 22.11.23
+DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 22.11.23
+DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 22.11.23
+DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 22.11.23
+DEL.N1LK61.AP.F.CPD.DMP : last exported on 22.11.23
+DEL.N1LN0R.AP.F.CPL.DMP : last exported on 22.11.23
+DEL.N1LR31.AP.F.PPS.DMP : last exported on 22.11.23
+DEL.KT6E35.AP.F.DB.ZIP : last exported on 22.11.23
+DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 22.11.23
+DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 22.11.23
+DVL.KT6N5X.VLM.AP.ZIP : last exported on 22.11.23</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 21.11.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 21.11.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 22.11.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 22.11.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,8 +1536,8 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 21.11.23
-DHP.KUDKT6.ORGUNITS : last exported on 22.11.23
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 22.11.23
+DHP.KUDKT6.ORGUNITS : last exported on 23.11.23
 DHS.R11KT6.HSB02ALL : last exported on 17.11.23</t>
         </is>
       </c>
@@ -1545,7 +1545,7 @@
         <is>
           <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 20.11.23
 DEL.N1LN3L.DP.F.GPL.DMP : last exported on 20.11.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 21.11.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 22.11.23
 DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 20.11.23
 DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 20.11.23
 DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 20.11.23
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 21.11.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 22.11.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 21.11.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 21.11.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 21.11.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 21.11.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 21.11.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 21.11.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 21.11.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 21.11.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 21.11.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 21.11.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 21.11.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 21.11.23
-DEL.N1LKT6.MT.??????.G : last exported on 21.11.23
-DEL.N1LKT6.MT.??????.U : last exported on 21.11.23
-DEL.N1LKT6.MT.??????.AS : last exported on 21.11.23
-DVL.N1LN5X.VLM.DSP : last exported on 21.11.23
-DVL.N1LN5X.VLM.WT : last exported on 21.11.23
-DDS.N1LR11.DSP : last exported on 21.11.23
-DDS.N1LR11.WT : last exported on 21.11.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 21.11.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 21.11.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 21.11.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 21.11.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 21.11.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 21.11.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 21.11.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 21.11.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 21.11.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 21.11.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 21.11.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 22.11.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 22.11.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 22.11.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 22.11.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 22.11.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 22.11.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 22.11.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 22.11.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 22.11.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 22.11.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 22.11.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 22.11.23
+DEL.N1LKT6.MT.??????.G : last exported on 22.11.23
+DEL.N1LKT6.MT.??????.U : last exported on 22.11.23
+DEL.N1LKT6.MT.??????.AS : last exported on 22.11.23
+DVL.N1LN5X.VLM.DSP : last exported on 22.11.23
+DVL.N1LN5X.VLM.WT : last exported on 22.11.23
+DDS.N1LR11.DSP : last exported on 22.11.23
+DDS.N1LR11.WT : last exported on 22.11.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 22.11.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 22.11.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 22.11.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 22.11.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 22.11.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 22.11.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 22.11.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 22.11.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 22.11.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 22.11.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 22.11.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,8 +1710,8 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 21.11.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 22.11.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 22.11.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 23.11.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 21.11.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 21.11.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 21.11.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 21.11.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 21.11.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 21.11.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 21.11.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 21.11.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 22.11.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 22.11.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 22.11.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 22.11.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 22.11.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 22.11.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 22.11.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 22.11.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 19.11.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 21.11.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 22.11.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 19.11.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 19.11.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 21.11.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 21.11.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 21.11.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 21.11.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 21.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 21.11.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 21.11.23
-DEL.N1LKT6.EC.??????.G : last exported on 21.11.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 21.11.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 21.11.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 21.11.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 21.11.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 21.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 21.11.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 21.11.23
-DEL.N1LKT6.EC.??????.U : last exported on 21.11.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 21.11.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 21.11.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 21.11.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 21.11.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 21.11.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 21.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 21.11.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 21.11.23
-DEL.N1LKT6.EC.??????.AS : last exported on 21.11.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 21.11.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 21.11.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 21.11.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 21.11.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 21.11.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 21.11.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 21.11.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 21.11.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 22.11.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 22.11.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 22.11.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 22.11.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 22.11.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 22.11.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 22.11.23
+DEL.N1LKT6.EC.??????.G : last exported on 22.11.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 22.11.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 22.11.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 22.11.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 22.11.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 22.11.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 22.11.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 22.11.23
+DEL.N1LKT6.EC.??????.U : last exported on 22.11.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 22.11.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 22.11.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 22.11.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 22.11.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 22.11.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 22.11.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 22.11.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 22.11.23
+DEL.N1LKT6.EC.??????.AS : last exported on 22.11.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 22.11.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 22.11.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 22.11.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 22.11.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 22.11.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 22.11.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 22.11.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 22.11.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 24.11.23 12:21
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 23.11.2023</t>
+          <t>Date - 24.11.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 22.11.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 23.11.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 23.11.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 23.11.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 23.11.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 23.11.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 23.11.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 23.11.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 23.11.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 23.11.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 23.11.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 23.11.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 23.11.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 23.11.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 23.11.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 23.11.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 24.11.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 24.11.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 24.11.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 24.11.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 24.11.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 24.11.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 24.11.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 24.11.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 24.11.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 24.11.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 24.11.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 24.11.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 24.11.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 24.11.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1120,31 +1120,31 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 22.11.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 22.11.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 22.11.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 22.11.23
-DIT.E35KT6.WI.ZIP : last exported on 22.11.23
-DEL.K2PKT6.WI.ZIP : last exported on 22.11.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 23.11.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 23.11.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 23.11.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 23.11.23
+DIT.E35KT6.WI.ZIP : last exported on 23.11.23
+DEL.K2PKT6.WI.ZIP : last exported on 23.11.23
 DEL.R7AKT6.WI.ZIP : last exported on 23.11.23
 DEL.N5FKT6.WI.ZIP : last exported on 20.11.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 22.11.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 22.11.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 22.11.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 22.11.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 22.11.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 22.11.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 22.11.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 22.11.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 22.11.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 22.11.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 22.11.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 22.11.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 22.11.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 23.11.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 23.11.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 23.11.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 23.11.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 23.11.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 23.11.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 23.11.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 23.11.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 23.11.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 23.11.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 23.11.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 23.11.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 23.11.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1247,30 +1247,30 @@
       </c>
       <c r="C10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 03.11.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 23.11.23
+          <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 23.11.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 24.11.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 20.11.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 22.11.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 22.11.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 22.11.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 22.11.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 22.11.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 22.11.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 22.11.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 22.11.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 22.11.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 22.11.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 22.11.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 22.11.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 22.11.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 22.11.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 22.11.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 22.11.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 22.11.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 23.11.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 23.11.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 23.11.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 23.11.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 23.11.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 23.11.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 23.11.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 23.11.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 23.11.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 23.11.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 23.11.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 23.11.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 23.11.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 23.11.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 23.11.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 23.11.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 23.11.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1331,7 +1331,7 @@
       </c>
       <c r="C12" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.MANDANTN.TXT : last exported on 15.11.23</t>
+          <t>DEL.N3LKT6.MANDANTN.TXT : last exported on 23.11.23</t>
         </is>
       </c>
       <c r="D12" s="10" t="inlineStr">
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 22.11.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 23.11.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 22.11.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 23.11.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 22.11.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 22.11.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 23.11.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 23.11.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,16 +1536,16 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 22.11.23
-DHP.KUDKT6.ORGUNITS : last exported on 23.11.23
-DHS.R11KT6.HSB02ALL : last exported on 17.11.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 23.11.23
+DHP.KUDKT6.ORGUNITS : last exported on 24.11.23
+DHS.R11KT6.HSB02ALL : last exported on 23.11.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 20.11.23
 DEL.N1LN3L.DP.F.GPL.DMP : last exported on 20.11.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 22.11.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 23.11.23
 DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 20.11.23
 DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 20.11.23
 DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 20.11.23
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 22.11.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 23.11.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 22.11.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 22.11.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 22.11.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 22.11.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 22.11.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 22.11.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 22.11.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 22.11.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 22.11.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 22.11.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 22.11.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 22.11.23
-DEL.N1LKT6.MT.??????.G : last exported on 22.11.23
-DEL.N1LKT6.MT.??????.U : last exported on 22.11.23
-DEL.N1LKT6.MT.??????.AS : last exported on 22.11.23
-DVL.N1LN5X.VLM.DSP : last exported on 22.11.23
-DVL.N1LN5X.VLM.WT : last exported on 22.11.23
-DDS.N1LR11.DSP : last exported on 22.11.23
-DDS.N1LR11.WT : last exported on 22.11.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 22.11.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 22.11.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 22.11.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 22.11.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 22.11.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 22.11.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 22.11.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 22.11.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 22.11.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 22.11.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 22.11.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 23.11.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 23.11.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 23.11.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 23.11.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 23.11.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 23.11.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 23.11.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 23.11.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 23.11.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 23.11.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 23.11.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 23.11.23
+DEL.N1LKT6.MT.??????.G : last exported on 23.11.23
+DEL.N1LKT6.MT.??????.U : last exported on 23.11.23
+DEL.N1LKT6.MT.??????.AS : last exported on 23.11.23
+DVL.N1LN5X.VLM.DSP : last exported on 23.11.23
+DVL.N1LN5X.VLM.WT : last exported on 23.11.23
+DDS.N1LR11.DSP : last exported on 23.11.23
+DDS.N1LR11.WT : last exported on 23.11.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 23.11.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 23.11.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 23.11.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 23.11.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 23.11.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 23.11.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 23.11.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 23.11.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 23.11.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 23.11.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 23.11.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,8 +1710,8 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 22.11.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 23.11.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 24.11.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 24.11.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 22.11.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 22.11.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 22.11.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 22.11.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 22.11.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 22.11.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 22.11.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 22.11.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 24.11.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 24.11.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 24.11.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 24.11.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 24.11.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 24.11.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 24.11.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 24.11.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 19.11.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 22.11.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 23.11.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 19.11.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 19.11.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 22.11.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 22.11.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 22.11.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 22.11.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 22.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 22.11.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 22.11.23
-DEL.N1LKT6.EC.??????.G : last exported on 22.11.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 22.11.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 22.11.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 22.11.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 22.11.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 22.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 22.11.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 22.11.23
-DEL.N1LKT6.EC.??????.U : last exported on 22.11.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 22.11.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 22.11.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 22.11.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 22.11.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 22.11.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 22.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 22.11.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 22.11.23
-DEL.N1LKT6.EC.??????.AS : last exported on 22.11.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 22.11.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 22.11.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 22.11.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 22.11.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 22.11.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 22.11.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 22.11.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 22.11.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 23.11.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 23.11.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 23.11.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 23.11.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 23.11.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 23.11.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 23.11.23
+DEL.N1LKT6.EC.??????.G : last exported on 23.11.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 23.11.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 23.11.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 23.11.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 23.11.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 23.11.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 23.11.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 23.11.23
+DEL.N1LKT6.EC.??????.U : last exported on 23.11.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 23.11.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 23.11.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 23.11.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 23.11.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 23.11.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 23.11.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 23.11.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 23.11.23
+DEL.N1LKT6.EC.??????.AS : last exported on 23.11.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 23.11.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 23.11.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 23.11.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 23.11.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 23.11.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 23.11.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 23.11.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 23.11.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 27.11.23 12:46
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 24.11.2023</t>
+          <t>Date - 27.11.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 23.11.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 24.11.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 24.11.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 24.11.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 24.11.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 24.11.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 24.11.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 24.11.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 24.11.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 24.11.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 24.11.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 24.11.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 24.11.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 24.11.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 24.11.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 24.11.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 25.11.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 25.11.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 26.11.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 25.11.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 25.11.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 25.11.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 25.11.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 25.11.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 25.11.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 25.11.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 25.11.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 25.11.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 25.11.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 25.11.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1077,22 +1077,22 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 20.11.23
-DEH.N3LKT6.AP.COMPL.SNK : last exported on 20.11.23</t>
+          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 27.11.23
+DEH.N3LKT6.AP.COMPL.SNK : last exported on 27.11.23</t>
         </is>
       </c>
       <c r="D6" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 20.11.23
-DEL.N1LN3L.DN.F.GPL.DMP : last exported on 20.11.23
-DEL.N1LN3L.DN.F.GTR.DMP : last exported on 20.11.23
-DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 20.11.23
-DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 20.11.23
-DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 20.11.23
-DEL.N1LK61.DN.F.CPD.DMP : last exported on 20.11.23
-DEL.N1LN0R.DN.F.CPL.DMP : last exported on 20.11.23
-DEL.KT6E35.SN.F.GGO.ZIP : last exported on 20.11.23
-DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 20.11.23</t>
+          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 27.11.23
+DEL.N1LN3L.DN.F.GPL.DMP : last exported on 27.11.23
+DEL.N1LN3L.DN.F.GTR.DMP : last exported on 27.11.23
+DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 27.11.23
+DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 27.11.23
+DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 27.11.23
+DEL.N1LK61.DN.F.CPD.DMP : last exported on 27.11.23
+DEL.N1LN0R.DN.F.CPL.DMP : last exported on 27.11.23
+DEL.KT6E35.SN.F.GGO.ZIP : last exported on 27.11.23
+DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 27.11.23</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
@@ -1120,31 +1120,31 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 23.11.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 23.11.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 24.11.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 26.11.23
 DLV.RPKKT6.WI.S.ZIP : last exported on 23.11.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 23.11.23
-DIT.E35KT6.WI.ZIP : last exported on 23.11.23
-DEL.K2PKT6.WI.ZIP : last exported on 23.11.23
-DEL.R7AKT6.WI.ZIP : last exported on 23.11.23
-DEL.N5FKT6.WI.ZIP : last exported on 20.11.23</t>
+DLV.I5XKT6.WI.A.ZIP : last exported on 26.11.23
+DIT.E35KT6.WI.ZIP : last exported on 24.11.23
+DEL.K2PKT6.WI.ZIP : last exported on 25.11.23
+DEL.R7AKT6.WI.ZIP : last exported on 25.11.23
+DEL.N5FKT6.WI.ZIP : last exported on 24.11.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 23.11.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 23.11.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 23.11.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 23.11.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 23.11.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 23.11.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 23.11.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 23.11.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 23.11.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 23.11.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 23.11.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 23.11.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 23.11.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 27.11.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 27.11.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 27.11.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 27.11.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 27.11.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 27.11.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 27.11.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 27.11.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 27.11.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 27.11.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 27.11.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 27.11.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 27.11.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1247,30 +1247,30 @@
       </c>
       <c r="C10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 23.11.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 24.11.23
+          <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 24.11.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 27.11.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 20.11.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 23.11.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 23.11.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 23.11.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 23.11.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 23.11.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 23.11.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 23.11.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 23.11.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 23.11.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 23.11.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 23.11.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 23.11.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 23.11.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 23.11.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 23.11.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 23.11.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 23.11.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 26.11.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 26.11.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 26.11.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 26.11.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 26.11.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 26.11.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 26.11.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 26.11.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 26.11.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 26.11.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 26.11.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 26.11.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 26.11.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 26.11.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 26.11.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 26.11.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 26.11.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1336,13 +1336,13 @@
       </c>
       <c r="D12" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 15.11.23
-DEL.N1LN3L.MC.F.GPL.DMP : last exported on 15.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 22.11.23
-DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 15.11.23
-DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 15.11.23
-DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 15.11.23
-DGI.KT6R11.MANDANT.TXT : last exported on 15.11.23</t>
+          <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 24.11.23
+DEL.N1LN3L.MC.F.GPL.DMP : last exported on 24.11.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 26.11.23
+DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 24.11.23
+DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 24.11.23
+DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 24.11.23
+DGI.KT6R11.MANDANT.TXT : last exported on 24.11.23</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 23.11.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 24.11.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 23.11.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 25.11.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1413,7 +1413,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 10.11.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 10.11.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 22.11.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 26.11.23
 DEL.KT6N5M.AU.GGO.ZIP : last exported on 10.11.23
 DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 10.11.23
 DEL.KT6KTZ.AU.GGO.ZIP : last exported on 10.11.23
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 23.11.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 23.11.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 26.11.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 26.11.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 23.11.23
-DHP.KUDKT6.ORGUNITS : last exported on 24.11.23
-DHS.R11KT6.HSB02ALL : last exported on 23.11.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 26.11.23
+DHP.KUDKT6.ORGUNITS : last exported on 27.11.23
+DHS.R11KT6.HSB02ALL : last exported on 24.11.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 20.11.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 20.11.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 23.11.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 20.11.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 20.11.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 20.11.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 20.11.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 20.11.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 20.11.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 20.11.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 24.11.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 24.11.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 26.11.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 24.11.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 24.11.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 24.11.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 24.11.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 24.11.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 24.11.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 24.11.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1620,7 +1620,7 @@
       </c>
       <c r="D19" s="16" t="inlineStr">
         <is>
-          <t>DEL.N1LE35.TRANS.ZIP : last exported on 19.11.23</t>
+          <t>DEL.N1LE35.TRANS.ZIP : last exported on 26.11.23</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 23.11.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 25.11.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 23.11.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 23.11.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 23.11.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 23.11.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 23.11.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 23.11.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 23.11.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 23.11.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 23.11.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 23.11.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 23.11.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 23.11.23
-DEL.N1LKT6.MT.??????.G : last exported on 23.11.23
-DEL.N1LKT6.MT.??????.U : last exported on 23.11.23
-DEL.N1LKT6.MT.??????.AS : last exported on 23.11.23
-DVL.N1LN5X.VLM.DSP : last exported on 23.11.23
-DVL.N1LN5X.VLM.WT : last exported on 23.11.23
-DDS.N1LR11.DSP : last exported on 23.11.23
-DDS.N1LR11.WT : last exported on 23.11.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 23.11.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 23.11.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 23.11.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 23.11.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 23.11.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 23.11.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 23.11.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 23.11.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 23.11.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 23.11.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 23.11.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 25.11.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 25.11.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 26.11.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 25.11.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 25.11.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 25.11.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 25.11.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 25.11.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 25.11.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 25.11.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 25.11.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 25.11.23
+DEL.N1LKT6.MT.??????.G : last exported on 25.11.23
+DEL.N1LKT6.MT.??????.U : last exported on 25.11.23
+DEL.N1LKT6.MT.??????.AS : last exported on 25.11.23
+DVL.N1LN5X.VLM.DSP : last exported on 25.11.23
+DVL.N1LN5X.VLM.WT : last exported on 25.11.23
+DDS.N1LR11.DSP : last exported on 25.11.23
+DDS.N1LR11.WT : last exported on 25.11.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 25.11.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 25.11.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 25.11.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 25.11.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 25.11.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 25.11.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 25.11.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 25.11.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 25.11.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 25.11.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 25.11.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,8 +1710,8 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 24.11.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 24.11.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 27.11.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 27.11.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 24.11.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 24.11.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 24.11.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 24.11.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 24.11.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 24.11.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 24.11.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 24.11.23
-DDC.R11KT6.ELFI.MD.TXT : last exported on 19.11.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 23.11.23
-DDC.R11KT6.ELFI.PK.TXT : last exported on 19.11.23
-DDC.R11KT6.ELFI.PR.TXT : last exported on 19.11.23</t>
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 27.11.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 27.11.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 27.11.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 27.11.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 27.11.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 27.11.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 27.11.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 27.11.23
+DDC.R11KT6.ELFI.MD.TXT : last exported on 26.11.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 24.11.23
+DDC.R11KT6.ELFI.PK.TXT : last exported on 26.11.23
+DDC.R11KT6.ELFI.PR.TXT : last exported on 26.11.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 23.11.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 23.11.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 23.11.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 23.11.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 23.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 23.11.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 23.11.23
-DEL.N1LKT6.EC.??????.G : last exported on 23.11.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 23.11.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 23.11.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 23.11.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 23.11.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 23.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 23.11.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 23.11.23
-DEL.N1LKT6.EC.??????.U : last exported on 23.11.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 23.11.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 23.11.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 23.11.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 23.11.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 23.11.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 23.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 23.11.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 23.11.23
-DEL.N1LKT6.EC.??????.AS : last exported on 23.11.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 23.11.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 23.11.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 23.11.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 23.11.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 23.11.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 23.11.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 23.11.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 23.11.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 26.11.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 26.11.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 26.11.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 26.11.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 26.11.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 26.11.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 26.11.23
+DEL.N1LKT6.EC.??????.G : last exported on 26.11.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 26.11.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 26.11.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 26.11.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 26.11.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 26.11.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 26.11.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 26.11.23
+DEL.N1LKT6.EC.??????.U : last exported on 26.11.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 26.11.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 26.11.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 26.11.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 26.11.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 26.11.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 26.11.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 26.11.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 26.11.23
+DEL.N1LKT6.EC.??????.AS : last exported on 26.11.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 26.11.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 26.11.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 26.11.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 26.11.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 26.11.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 26.11.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 26.11.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 26.11.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 28.11.23 11:54
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 27.11.2023</t>
+          <t>Date - 28.11.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 24.11.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 27.11.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 25.11.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 25.11.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 26.11.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 25.11.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 25.11.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 25.11.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 25.11.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 25.11.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 25.11.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 25.11.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 25.11.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 25.11.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 25.11.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 25.11.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 28.11.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 28.11.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 28.11.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 28.11.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 28.11.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 28.11.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 28.11.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 28.11.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 28.11.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 28.11.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 28.11.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 28.11.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 28.11.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 28.11.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1120,13 +1120,13 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 24.11.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 26.11.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 27.11.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 27.11.23
 DLV.RPKKT6.WI.S.ZIP : last exported on 23.11.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 26.11.23
-DIT.E35KT6.WI.ZIP : last exported on 24.11.23
-DEL.K2PKT6.WI.ZIP : last exported on 25.11.23
-DEL.R7AKT6.WI.ZIP : last exported on 25.11.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 27.11.23
+DIT.E35KT6.WI.ZIP : last exported on 27.11.23
+DEL.K2PKT6.WI.ZIP : last exported on 27.11.23
+DEL.R7AKT6.WI.ZIP : last exported on 28.11.23
 DEL.N5FKT6.WI.ZIP : last exported on 24.11.23</t>
         </is>
       </c>
@@ -1247,30 +1247,30 @@
       </c>
       <c r="C10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 24.11.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 27.11.23
-DGV.N3LKT6.EPELS.??????.ZIP : last exported on 20.11.23</t>
+          <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 27.11.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 28.11.23
+DGV.N3LKT6.EPELS.??????.ZIP : last exported on 27.11.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 26.11.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 26.11.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 26.11.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 26.11.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 26.11.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 26.11.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 26.11.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 26.11.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 26.11.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 26.11.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 26.11.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 26.11.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 26.11.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 26.11.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 26.11.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 26.11.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 26.11.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 27.11.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 27.11.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 27.11.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 27.11.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 27.11.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 27.11.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 27.11.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 27.11.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 27.11.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 27.11.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 27.11.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 27.11.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 27.11.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 27.11.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 27.11.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 27.11.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 27.11.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1298,12 +1298,12 @@
       </c>
       <c r="C11" s="14" t="inlineStr">
         <is>
-          <t>DEL.KT6KT6.APOSPRO.ZIP : last exported on 20.11.23</t>
+          <t>DEL.KT6KT6.APOSPRO.ZIP : last exported on 27.11.23</t>
         </is>
       </c>
       <c r="D11" s="15" t="inlineStr">
         <is>
-          <t>DEL.KT6N2O.XTIME.ZIP : last exported on 20.11.23</t>
+          <t>DEL.KT6N2O.XTIME.ZIP : last exported on 27.11.23</t>
         </is>
       </c>
       <c r="E11" s="11" t="inlineStr">
@@ -1338,7 +1338,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 24.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 24.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 26.11.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 27.11.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 24.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 24.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 24.11.23
@@ -1370,7 +1370,7 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 24.11.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 27.11.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
@@ -1413,7 +1413,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 10.11.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 10.11.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 26.11.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 27.11.23
 DEL.KT6N5M.AU.GGO.ZIP : last exported on 10.11.23
 DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 10.11.23
 DEL.KT6KTZ.AU.GGO.ZIP : last exported on 10.11.23
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 26.11.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 26.11.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 27.11.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 27.11.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 26.11.23
-DHP.KUDKT6.ORGUNITS : last exported on 27.11.23
-DHS.R11KT6.HSB02ALL : last exported on 24.11.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 27.11.23
+DHP.KUDKT6.ORGUNITS : last exported on 28.11.23
+DHS.R11KT6.HSB02ALL : last exported on 27.11.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 24.11.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 24.11.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 26.11.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 24.11.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 24.11.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 24.11.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 24.11.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 24.11.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 24.11.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 24.11.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 27.11.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 27.11.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 27.11.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 27.11.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 27.11.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 27.11.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 27.11.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 27.11.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 27.11.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 27.11.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 25.11.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 27.11.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 25.11.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 25.11.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 26.11.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 25.11.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 25.11.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 25.11.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 25.11.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 25.11.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 25.11.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 25.11.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 25.11.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 25.11.23
-DEL.N1LKT6.MT.??????.G : last exported on 25.11.23
-DEL.N1LKT6.MT.??????.U : last exported on 25.11.23
-DEL.N1LKT6.MT.??????.AS : last exported on 25.11.23
-DVL.N1LN5X.VLM.DSP : last exported on 25.11.23
-DVL.N1LN5X.VLM.WT : last exported on 25.11.23
-DDS.N1LR11.DSP : last exported on 25.11.23
-DDS.N1LR11.WT : last exported on 25.11.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 25.11.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 25.11.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 25.11.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 25.11.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 25.11.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 25.11.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 25.11.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 25.11.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 25.11.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 25.11.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 25.11.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 27.11.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 27.11.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 27.11.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 27.11.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 27.11.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 27.11.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 27.11.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 27.11.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 27.11.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 27.11.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 27.11.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 27.11.23
+DEL.N1LKT6.MT.??????.G : last exported on 27.11.23
+DEL.N1LKT6.MT.??????.U : last exported on 27.11.23
+DEL.N1LKT6.MT.??????.AS : last exported on 27.11.23
+DVL.N1LN5X.VLM.DSP : last exported on 27.11.23
+DVL.N1LN5X.VLM.WT : last exported on 27.11.23
+DDS.N1LR11.DSP : last exported on 27.11.23
+DDS.N1LR11.WT : last exported on 27.11.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 27.11.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 27.11.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 27.11.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 27.11.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 27.11.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 27.11.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 27.11.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 27.11.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 27.11.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 27.11.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 27.11.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,8 +1710,8 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 27.11.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 27.11.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 28.11.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 28.11.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 27.11.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 27.11.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 27.11.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 27.11.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 27.11.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 27.11.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 27.11.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 27.11.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 28.11.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 28.11.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 28.11.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 28.11.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 28.11.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 28.11.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 28.11.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 28.11.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 26.11.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 24.11.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 27.11.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 26.11.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 26.11.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 26.11.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 26.11.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 26.11.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 26.11.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 26.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 26.11.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 26.11.23
-DEL.N1LKT6.EC.??????.G : last exported on 26.11.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 26.11.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 26.11.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 26.11.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 26.11.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 26.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 26.11.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 26.11.23
-DEL.N1LKT6.EC.??????.U : last exported on 26.11.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 26.11.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 26.11.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 26.11.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 26.11.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 26.11.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 26.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 26.11.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 26.11.23
-DEL.N1LKT6.EC.??????.AS : last exported on 26.11.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 26.11.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 26.11.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 26.11.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 26.11.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 26.11.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 26.11.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 26.11.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 26.11.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 27.11.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 27.11.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 27.11.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 27.11.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 27.11.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 27.11.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 27.11.23
+DEL.N1LKT6.EC.??????.G : last exported on 27.11.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 27.11.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 27.11.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 27.11.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 27.11.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 27.11.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 27.11.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 27.11.23
+DEL.N1LKT6.EC.??????.U : last exported on 27.11.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 27.11.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 27.11.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 27.11.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 27.11.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 27.11.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 27.11.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 27.11.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 27.11.23
+DEL.N1LKT6.EC.??????.AS : last exported on 27.11.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 27.11.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 27.11.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 27.11.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 27.11.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 27.11.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 27.11.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 27.11.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 27.11.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 29.11.23 11:59
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 28.11.2023</t>
+          <t>Date - 29.11.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 27.11.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 28.11.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 28.11.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 28.11.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 28.11.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 28.11.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 28.11.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 28.11.23
-DEL.N1LK61.WD.D.CPD.DMP : last exported on 28.11.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 28.11.23
-DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 28.11.23
-DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 28.11.23
-DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 28.11.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 28.11.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 28.11.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 28.11.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 29.11.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 29.11.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 29.11.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 29.11.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 29.11.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 29.11.23
+DEL.N1LK61.WD.D.CPD.DMP : last exported on 29.11.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 29.11.23
+DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 29.11.23
+DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 29.11.23
+DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 29.11.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 29.11.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 29.11.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 29.11.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1120,31 +1120,31 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 27.11.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 27.11.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 23.11.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 27.11.23
-DIT.E35KT6.WI.ZIP : last exported on 27.11.23
-DEL.K2PKT6.WI.ZIP : last exported on 27.11.23
-DEL.R7AKT6.WI.ZIP : last exported on 28.11.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 28.11.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 28.11.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 28.11.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 28.11.23
+DIT.E35KT6.WI.ZIP : last exported on 28.11.23
+DEL.K2PKT6.WI.ZIP : last exported on 28.11.23
+DEL.R7AKT6.WI.ZIP : last exported on 29.11.23
 DEL.N5FKT6.WI.ZIP : last exported on 24.11.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 27.11.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 27.11.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 27.11.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 27.11.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 27.11.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 27.11.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 27.11.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 27.11.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 27.11.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 27.11.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 27.11.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 27.11.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 27.11.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 28.11.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 28.11.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 28.11.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 28.11.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 28.11.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 28.11.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 28.11.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 28.11.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 28.11.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 28.11.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 28.11.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 28.11.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 28.11.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1247,30 +1247,30 @@
       </c>
       <c r="C10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 27.11.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 28.11.23
+          <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 28.11.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 29.11.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 27.11.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 27.11.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 27.11.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 27.11.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 27.11.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 27.11.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 27.11.23
-DEL.N1LK61.TP.D.CPD.DMP : last exported on 27.11.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 27.11.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 27.11.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 27.11.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 27.11.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 27.11.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 27.11.23
-DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 27.11.23
-DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 27.11.23
-DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 27.11.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 27.11.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 28.11.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 28.11.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 28.11.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 28.11.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 28.11.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 28.11.23
+DEL.N1LK61.TP.D.CPD.DMP : last exported on 28.11.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 28.11.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 28.11.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 28.11.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 28.11.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 28.11.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 28.11.23
+DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 28.11.23
+DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 28.11.23
+DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 28.11.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 28.11.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1338,7 +1338,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 24.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 24.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 27.11.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 28.11.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 24.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 24.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 24.11.23
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 27.11.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 28.11.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 25.11.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 28.11.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1413,7 +1413,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 10.11.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 10.11.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 27.11.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 28.11.23
 DEL.KT6N5M.AU.GGO.ZIP : last exported on 10.11.23
 DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 10.11.23
 DEL.KT6KTZ.AU.GGO.ZIP : last exported on 10.11.23
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 27.11.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 27.11.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 28.11.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 28.11.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 27.11.23
-DHP.KUDKT6.ORGUNITS : last exported on 28.11.23
-DHS.R11KT6.HSB02ALL : last exported on 27.11.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 28.11.23
+DHP.KUDKT6.ORGUNITS : last exported on 29.11.23
+DHS.R11KT6.HSB02ALL : last exported on 28.11.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 27.11.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 27.11.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 27.11.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 27.11.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 27.11.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 27.11.23
-DEL.N1LK61.DP.F.CPD.DMP : last exported on 27.11.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 27.11.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 27.11.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 27.11.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 28.11.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 28.11.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 28.11.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 28.11.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 28.11.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 28.11.23
+DEL.N1LK61.DP.F.CPD.DMP : last exported on 28.11.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 28.11.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 28.11.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 28.11.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 27.11.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 28.11.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 27.11.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 27.11.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 27.11.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 27.11.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 27.11.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 27.11.23
-DEL.N1LK61.MT.F.CPD.DMP : last exported on 27.11.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 27.11.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 27.11.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 27.11.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 27.11.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 27.11.23
-DEL.N1LKT6.MT.??????.G : last exported on 27.11.23
-DEL.N1LKT6.MT.??????.U : last exported on 27.11.23
-DEL.N1LKT6.MT.??????.AS : last exported on 27.11.23
-DVL.N1LN5X.VLM.DSP : last exported on 27.11.23
-DVL.N1LN5X.VLM.WT : last exported on 27.11.23
-DDS.N1LR11.DSP : last exported on 27.11.23
-DDS.N1LR11.WT : last exported on 27.11.23
-DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 27.11.23
-DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 27.11.23
-DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 27.11.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 27.11.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 27.11.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 27.11.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 27.11.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 27.11.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 27.11.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 27.11.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 27.11.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 28.11.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 28.11.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 28.11.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 28.11.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 28.11.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 28.11.23
+DEL.N1LK61.MT.F.CPD.DMP : last exported on 28.11.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 28.11.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 28.11.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 28.11.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 28.11.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 28.11.23
+DEL.N1LKT6.MT.??????.G : last exported on 28.11.23
+DEL.N1LKT6.MT.??????.U : last exported on 28.11.23
+DEL.N1LKT6.MT.??????.AS : last exported on 28.11.23
+DVL.N1LN5X.VLM.DSP : last exported on 28.11.23
+DVL.N1LN5X.VLM.WT : last exported on 28.11.23
+DDS.N1LR11.DSP : last exported on 28.11.23
+DDS.N1LR11.WT : last exported on 28.11.23
+DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 28.11.23
+DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 28.11.23
+DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 28.11.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 28.11.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 28.11.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 28.11.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 28.11.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 28.11.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 28.11.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 28.11.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 28.11.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,8 +1710,8 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 28.11.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 28.11.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 29.11.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 29.11.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 28.11.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 28.11.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 28.11.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 28.11.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 28.11.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 28.11.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 28.11.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 28.11.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 29.11.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 29.11.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 29.11.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 29.11.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 29.11.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 29.11.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 29.11.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 29.11.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 26.11.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 27.11.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 28.11.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 26.11.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 26.11.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 27.11.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 27.11.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 27.11.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 27.11.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 27.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 27.11.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 27.11.23
-DEL.N1LKT6.EC.??????.G : last exported on 27.11.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 27.11.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 27.11.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 27.11.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 27.11.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 27.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 27.11.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 27.11.23
-DEL.N1LKT6.EC.??????.U : last exported on 27.11.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 27.11.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 27.11.23
-DEL.N1LK61.EL.F.CPD.DMP : last exported on 27.11.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 27.11.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 27.11.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 27.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 27.11.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 27.11.23
-DEL.N1LKT6.EC.??????.AS : last exported on 27.11.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 27.11.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 27.11.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 27.11.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 27.11.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 27.11.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 27.11.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 27.11.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 27.11.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 28.11.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 28.11.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 28.11.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 28.11.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 28.11.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 28.11.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 28.11.23
+DEL.N1LKT6.EC.??????.G : last exported on 28.11.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 28.11.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 28.11.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 28.11.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 28.11.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 28.11.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 28.11.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 28.11.23
+DEL.N1LKT6.EC.??????.U : last exported on 28.11.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 28.11.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 28.11.23
+DEL.N1LK61.EL.F.CPD.DMP : last exported on 28.11.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 28.11.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 28.11.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 28.11.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 28.11.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 28.11.23
+DEL.N1LKT6.EC.??????.AS : last exported on 28.11.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 28.11.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 28.11.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 28.11.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 28.11.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 28.11.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 28.11.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 28.11.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 28.11.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 30.11.23 12:15
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 29.11.2023</t>
+          <t>Date - 30.11.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 28.11.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 29.11.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 29.11.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 29.11.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 29.11.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 29.11.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 29.11.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 29.11.23
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 30.11.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 30.11.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 30.11.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 30.11.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 30.11.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 30.11.23
 DEL.N1LK61.WD.D.CPD.DMP : last exported on 29.11.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 29.11.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 30.11.23
 DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 29.11.23
 DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 29.11.23
 DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 29.11.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 29.11.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 29.11.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 29.11.23</t>
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 30.11.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 30.11.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 30.11.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1120,31 +1120,31 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 28.11.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 29.11.23
 DLV.KZ6KT6.WI.V.ZIP : last exported on 28.11.23
 DLV.RPKKT6.WI.S.ZIP : last exported on 28.11.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 28.11.23
-DIT.E35KT6.WI.ZIP : last exported on 28.11.23
-DEL.K2PKT6.WI.ZIP : last exported on 28.11.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 29.11.23
+DIT.E35KT6.WI.ZIP : last exported on 29.11.23
+DEL.K2PKT6.WI.ZIP : last exported on 29.11.23
 DEL.R7AKT6.WI.ZIP : last exported on 29.11.23
 DEL.N5FKT6.WI.ZIP : last exported on 24.11.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 28.11.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 28.11.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 28.11.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 28.11.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 28.11.23
-DEL.N1LK61.WI.D.CPD.DMP : last exported on 28.11.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 28.11.23
-DEL.KT6KTZ.WI.GGO.ZIP : last exported on 28.11.23
-DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 28.11.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 28.11.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 28.11.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 28.11.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 28.11.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 29.11.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 29.11.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 29.11.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 29.11.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 29.11.23
+DEL.N1LK61.WI.D.CPD.DMP : last exported on 29.11.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 29.11.23
+DEL.KT6KTZ.WI.GGO.ZIP : last exported on 29.11.23
+DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 29.11.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 29.11.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 29.11.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 29.11.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 29.11.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 28.11.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 29.11.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 30.11.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 27.11.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 28.11.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 28.11.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 28.11.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 28.11.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 28.11.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 28.11.23
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 29.11.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 29.11.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 29.11.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 29.11.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 29.11.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 29.11.23
 DEL.N1LK61.TP.D.CPD.DMP : last exported on 28.11.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 28.11.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 28.11.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 28.11.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 28.11.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 28.11.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 28.11.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 29.11.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 29.11.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 29.11.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 29.11.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 29.11.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 29.11.23
 DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 28.11.23
 DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 28.11.23
 DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 28.11.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 28.11.23</t>
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 29.11.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1338,7 +1338,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 24.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 24.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 28.11.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 29.11.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 24.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 24.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 24.11.23
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 28.11.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 29.11.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 28.11.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 29.11.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1413,7 +1413,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 10.11.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 10.11.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 28.11.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 29.11.23
 DEL.KT6N5M.AU.GGO.ZIP : last exported on 10.11.23
 DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 10.11.23
 DEL.KT6KTZ.AU.GGO.ZIP : last exported on 10.11.23
@@ -1457,24 +1457,24 @@
 DGQ.R11KT6.BSITX.TXT : last exported on 01.11.23
 DGQ.R31KT6.BSIVMC.TXT : last exported on 07.11.23
 DGQ.R31KT6.PKATC.TXT : last exported on 07.11.23
-DEL.KMPKT6.APOS.DATA.ZIP : last exported on 22.11.23</t>
+DEL.KMPKT6.APOS.DATA.ZIP : last exported on 29.11.23</t>
         </is>
       </c>
       <c r="D15" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 22.11.23
-DEL.N1LN3L.AP.F.GPL.DMP : last exported on 22.11.23
-DEL.N1LN3L.AP.F.GTR.DMP : last exported on 22.11.23
-DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 22.11.23
-DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 22.11.23
-DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 22.11.23
+          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 29.11.23
+DEL.N1LN3L.AP.F.GPL.DMP : last exported on 29.11.23
+DEL.N1LN3L.AP.F.GTR.DMP : last exported on 29.11.23
+DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 29.11.23
+DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 29.11.23
+DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 29.11.23
 DEL.N1LK61.AP.F.CPD.DMP : last exported on 22.11.23
-DEL.N1LN0R.AP.F.CPL.DMP : last exported on 22.11.23
-DEL.N1LR31.AP.F.PPS.DMP : last exported on 22.11.23
-DEL.KT6E35.AP.F.DB.ZIP : last exported on 22.11.23
-DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 22.11.23
-DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 22.11.23
-DVL.KT6N5X.VLM.AP.ZIP : last exported on 22.11.23</t>
+DEL.N1LN0R.AP.F.CPL.DMP : last exported on 29.11.23
+DEL.N1LR31.AP.F.PPS.DMP : last exported on 29.11.23
+DEL.KT6E35.AP.F.DB.ZIP : last exported on 29.11.23
+DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 29.11.23
+DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 29.11.23
+DVL.KT6N5X.VLM.AP.ZIP : last exported on 29.11.23</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 28.11.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 28.11.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 29.11.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 29.11.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 28.11.23
-DHP.KUDKT6.ORGUNITS : last exported on 29.11.23
-DHS.R11KT6.HSB02ALL : last exported on 28.11.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 29.11.23
+DHP.KUDKT6.ORGUNITS : last exported on 30.11.23
+DHS.R11KT6.HSB02ALL : last exported on 29.11.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 28.11.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 28.11.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 28.11.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 28.11.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 28.11.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 28.11.23
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 29.11.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 29.11.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 29.11.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 29.11.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 29.11.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 29.11.23
 DEL.N1LK61.DP.F.CPD.DMP : last exported on 28.11.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 28.11.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 28.11.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 28.11.23</t>
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 29.11.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 29.11.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 29.11.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 28.11.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 29.11.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 28.11.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 28.11.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 28.11.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 28.11.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 28.11.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 28.11.23
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 29.11.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 29.11.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 29.11.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 29.11.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 29.11.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 29.11.23
 DEL.N1LK61.MT.F.CPD.DMP : last exported on 28.11.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 28.11.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 28.11.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 28.11.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 28.11.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 28.11.23
-DEL.N1LKT6.MT.??????.G : last exported on 28.11.23
-DEL.N1LKT6.MT.??????.U : last exported on 28.11.23
-DEL.N1LKT6.MT.??????.AS : last exported on 28.11.23
-DVL.N1LN5X.VLM.DSP : last exported on 28.11.23
-DVL.N1LN5X.VLM.WT : last exported on 28.11.23
-DDS.N1LR11.DSP : last exported on 28.11.23
-DDS.N1LR11.WT : last exported on 28.11.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 29.11.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 29.11.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 29.11.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 29.11.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 29.11.23
+DEL.N1LKT6.MT.??????.G : last exported on 29.11.23
+DEL.N1LKT6.MT.??????.U : last exported on 29.11.23
+DEL.N1LKT6.MT.??????.AS : last exported on 29.11.23
+DVL.N1LN5X.VLM.DSP : last exported on 29.11.23
+DVL.N1LN5X.VLM.WT : last exported on 29.11.23
+DDS.N1LR11.DSP : last exported on 29.11.23
+DDS.N1LR11.WT : last exported on 29.11.23
 DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 28.11.23
 DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 28.11.23
 DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 28.11.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 28.11.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 28.11.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 28.11.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 28.11.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 28.11.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 28.11.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 28.11.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 28.11.23</t>
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 29.11.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 29.11.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 29.11.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 29.11.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 29.11.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 29.11.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 29.11.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 29.11.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,8 +1710,8 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 29.11.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 29.11.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 30.11.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 30.11.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 29.11.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 29.11.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 29.11.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 29.11.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 29.11.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 29.11.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 29.11.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 29.11.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 30.11.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 30.11.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 30.11.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 30.11.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 30.11.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 30.11.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 30.11.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 30.11.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 26.11.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 28.11.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 29.11.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 26.11.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 26.11.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 28.11.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 28.11.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 28.11.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 28.11.23
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 29.11.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 29.11.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 29.11.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 29.11.23
 DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 28.11.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 28.11.23
-DEL.N1LKT6.EC.??????.G : last exported on 28.11.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 28.11.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 28.11.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 28.11.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 28.11.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 29.11.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 29.11.23
+DEL.N1LKT6.EC.??????.G : last exported on 29.11.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 29.11.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 29.11.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 29.11.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 29.11.23
 DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 28.11.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 28.11.23
-DEL.N1LKT6.EC.??????.U : last exported on 28.11.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 28.11.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 28.11.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 29.11.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 29.11.23
+DEL.N1LKT6.EC.??????.U : last exported on 29.11.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 29.11.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 29.11.23
 DEL.N1LK61.EL.F.CPD.DMP : last exported on 28.11.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 28.11.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 28.11.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 29.11.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 29.11.23
 DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 28.11.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 28.11.23
-DEL.N1LKT6.EC.??????.AS : last exported on 28.11.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 28.11.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 28.11.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 28.11.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 28.11.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 29.11.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 29.11.23
+DEL.N1LKT6.EC.??????.AS : last exported on 29.11.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 29.11.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 29.11.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 29.11.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 29.11.23
 DGV.N1LN7K.EL.F.ZIP : last exported on 28.11.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 28.11.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 28.11.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 28.11.23</t>
+DGV.N1LN5X.EL.F.ZIP : last exported on 29.11.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 29.11.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 29.11.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 01.12.23 12:09
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -942,7 +942,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="34" t="inlineStr">
         <is>
-          <t>Date - 30.11.2023</t>
+          <t>Date - 01.12.2023</t>
         </is>
       </c>
       <c r="B2" s="27" t="n"/>
@@ -997,25 +997,25 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 29.11.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 30.11.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 30.11.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 30.11.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 30.11.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 30.11.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 30.11.23
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 01.12.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 01.12.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 01.12.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 01.12.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 01.12.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 01.12.23
 DEL.N1LK61.WD.D.CPD.DMP : last exported on 29.11.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 30.11.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 01.12.23
 DEL.KT6KTZ.SL.D.GGO.ZIP : last exported on 29.11.23
 DEL.KT6KTZ.SL.D.UGO.ZIP : last exported on 29.11.23
 DEL.KT6KTZ.SL.D.ASGO.ZIP : last exported on 29.11.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 30.11.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 30.11.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 30.11.23</t>
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 01.12.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 01.12.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 01.12.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1121,30 +1121,30 @@
       <c r="C7" s="10" t="inlineStr">
         <is>
           <t>DLV.R31KT6.WI.C.ZIP : last exported on 29.11.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 28.11.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 28.11.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 29.11.23
-DIT.E35KT6.WI.ZIP : last exported on 29.11.23
-DEL.K2PKT6.WI.ZIP : last exported on 29.11.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 30.11.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 30.11.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 30.11.23
+DIT.E35KT6.WI.ZIP : last exported on 30.11.23
+DEL.K2PKT6.WI.ZIP : last exported on 30.11.23
 DEL.R7AKT6.WI.ZIP : last exported on 29.11.23
 DEL.N5FKT6.WI.ZIP : last exported on 24.11.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 29.11.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 29.11.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 29.11.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 29.11.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 29.11.23
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 30.11.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 30.11.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 30.11.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 30.11.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 30.11.23
 DEL.N1LK61.WI.D.CPD.DMP : last exported on 29.11.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 29.11.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 30.11.23
 DEL.KT6KTZ.WI.GGO.ZIP : last exported on 29.11.23
 DEL.KT6KTZ.WI.IMG.GGO.ZIP : last exported on 29.11.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 29.11.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 29.11.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 29.11.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 29.11.23</t>
+DEL.KT6E35.WI.GGO.ZIP : last exported on 30.11.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 30.11.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 30.11.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 30.11.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1248,29 +1248,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 28.11.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 30.11.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 01.12.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 27.11.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 29.11.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 29.11.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 29.11.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 29.11.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 29.11.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 29.11.23
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 30.11.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 30.11.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 30.11.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 30.11.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 30.11.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 30.11.23
 DEL.N1LK61.TP.D.CPD.DMP : last exported on 28.11.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 29.11.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 29.11.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 29.11.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 29.11.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 29.11.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 29.11.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 30.11.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 30.11.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 30.11.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 30.11.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 30.11.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 30.11.23
 DEL.KT6KTZ.TP.D.GGO.ZIP : last exported on 28.11.23
 DEL.KT6KTZ.TP.D.UGO.ZIP : last exported on 28.11.23
 DEL.KT6KTZ.TP.D.ASGO.ZIP : last exported on 28.11.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 29.11.23</t>
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 30.11.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1331,18 +1331,18 @@
       </c>
       <c r="C12" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.MANDANTN.TXT : last exported on 23.11.23</t>
+          <t>DEL.N3LKT6.MANDANTN.TXT : last exported on 30.11.23</t>
         </is>
       </c>
       <c r="D12" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 24.11.23
-DEL.N1LN3L.MC.F.GPL.DMP : last exported on 24.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 29.11.23
-DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 24.11.23
-DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 24.11.23
-DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 24.11.23
-DGI.KT6R11.MANDANT.TXT : last exported on 24.11.23</t>
+          <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
+DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 30.11.23
+DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
+DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
+DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
+DGI.KT6R11.MANDANT.TXT : last exported on 30.11.23</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1370,12 +1370,12 @@
       </c>
       <c r="C13" s="16" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 29.11.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 30.11.23</t>
         </is>
       </c>
       <c r="D13" s="16" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 29.11.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 30.11.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1413,7 +1413,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 10.11.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 10.11.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 29.11.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 30.11.23
 DEL.KT6N5M.AU.GGO.ZIP : last exported on 10.11.23
 DEL.KT6N5M.AU.IMG.GGO.ZIP : last exported on 10.11.23
 DEL.KT6KTZ.AU.GGO.ZIP : last exported on 10.11.23
@@ -1507,8 +1507,8 @@
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 29.11.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 29.11.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 30.11.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 30.11.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1536,23 +1536,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 29.11.23
-DHP.KUDKT6.ORGUNITS : last exported on 30.11.23
-DHS.R11KT6.HSB02ALL : last exported on 29.11.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 30.11.23
+DHP.KUDKT6.ORGUNITS : last exported on 01.12.23
+DHS.R11KT6.HSB02ALL : last exported on 30.11.23</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 29.11.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 29.11.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 29.11.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 29.11.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 29.11.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 29.11.23
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 30.11.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 30.11.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 30.11.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 30.11.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 30.11.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 30.11.23
 DEL.N1LK61.DP.F.CPD.DMP : last exported on 28.11.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 29.11.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 29.11.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 29.11.23</t>
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 30.11.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 30.11.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 30.11.23</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1648,41 +1648,41 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 29.11.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 30.11.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 29.11.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 29.11.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 29.11.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 29.11.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 29.11.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 29.11.23
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 30.11.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 30.11.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 30.11.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 30.11.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 30.11.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 30.11.23
 DEL.N1LK61.MT.F.CPD.DMP : last exported on 28.11.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 29.11.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 29.11.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 29.11.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 29.11.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 29.11.23
-DEL.N1LKT6.MT.??????.G : last exported on 29.11.23
-DEL.N1LKT6.MT.??????.U : last exported on 29.11.23
-DEL.N1LKT6.MT.??????.AS : last exported on 29.11.23
-DVL.N1LN5X.VLM.DSP : last exported on 29.11.23
-DVL.N1LN5X.VLM.WT : last exported on 29.11.23
-DDS.N1LR11.DSP : last exported on 29.11.23
-DDS.N1LR11.WT : last exported on 29.11.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 30.11.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 30.11.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 30.11.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 30.11.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 30.11.23
+DEL.N1LKT6.MT.??????.G : last exported on 30.11.23
+DEL.N1LKT6.MT.??????.U : last exported on 30.11.23
+DEL.N1LKT6.MT.??????.AS : last exported on 30.11.23
+DVL.N1LN5X.VLM.DSP : last exported on 30.11.23
+DVL.N1LN5X.VLM.WT : last exported on 30.11.23
+DDS.N1LR11.DSP : last exported on 30.11.23
+DDS.N1LR11.WT : last exported on 30.11.23
 DEL.KT6KTZ.MT.F.GGO.ZIP : last exported on 28.11.23
 DEL.KT6KTZ.MT.F.UGO.ZIP : last exported on 28.11.23
 DEL.KT6KTZ.MT.F.ASGO.ZIP : last exported on 28.11.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 29.11.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 29.11.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 29.11.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 29.11.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 29.11.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 29.11.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 29.11.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 29.11.23</t>
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 30.11.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 30.11.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 30.11.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 30.11.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 30.11.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 30.11.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 30.11.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 30.11.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1710,8 +1710,8 @@
       </c>
       <c r="C21" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 30.11.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 30.11.23</t>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 01.12.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 01.12.23</t>
         </is>
       </c>
       <c r="D21" s="10" t="inlineStr">
@@ -1753,55 +1753,55 @@
       </c>
       <c r="C22" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 30.11.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 30.11.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 30.11.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 30.11.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 30.11.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 30.11.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 30.11.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 30.11.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 01.12.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 01.12.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 01.12.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 01.12.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 01.12.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 01.12.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 01.12.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 01.12.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 26.11.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 29.11.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 30.11.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 26.11.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 26.11.23</t>
         </is>
       </c>
       <c r="D22" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 29.11.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 29.11.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 29.11.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 29.11.23
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 30.11.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 30.11.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 30.11.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 30.11.23
 DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 29.11.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 29.11.23
-DEL.N1LKT6.EC.??????.G : last exported on 29.11.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 29.11.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 29.11.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 29.11.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 29.11.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 30.11.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 30.11.23
+DEL.N1LKT6.EC.??????.G : last exported on 30.11.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 30.11.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 30.11.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 30.11.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 30.11.23
 DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 29.11.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 29.11.23
-DEL.N1LKT6.EC.??????.U : last exported on 29.11.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 29.11.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 29.11.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 30.11.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 30.11.23
+DEL.N1LKT6.EC.??????.U : last exported on 30.11.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 30.11.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 30.11.23
 DEL.N1LK61.EL.F.CPD.DMP : last exported on 28.11.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 29.11.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 29.11.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 30.11.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 30.11.23
 DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 29.11.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 29.11.23
-DEL.N1LKT6.EC.??????.AS : last exported on 29.11.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 29.11.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 29.11.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 29.11.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 29.11.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 28.11.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 29.11.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 29.11.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 29.11.23</t>
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 30.11.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 30.11.23
+DEL.N1LKT6.EC.??????.AS : last exported on 30.11.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 30.11.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 30.11.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 30.11.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 30.11.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 30.11.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 30.11.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 30.11.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 30.11.23</t>
         </is>
       </c>
       <c r="E22" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 04.12.23 12:20
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -1121,17 +1121,17 @@
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 03.12.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 03.12.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 03.12.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 03.12.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 03.12.23
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 03.12.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 03.12.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 03.12.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 03.12.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 03.12.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 03.12.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 04.12.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 04.12.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 04.12.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 04.12.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 04.12.23
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 04.12.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 04.12.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 04.12.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 04.12.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 04.12.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 04.12.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1662,14 +1662,14 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 01.12.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 01.12.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 01.12.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 01.12.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 01.12.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 01.12.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 01.12.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 01.12.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 04.12.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 04.12.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 04.12.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 04.12.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 04.12.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 04.12.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 04.12.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 04.12.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 03.12.23
 DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 01.12.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 03.12.23

</xml_diff>

<commit_message>
Updated on 05.12.23 12:03
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="25" t="inlineStr">
         <is>
-          <t>Date - 04.12.2023</t>
+          <t>Date - 05.12.2023</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 01.12.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 04.12.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 02.12.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 02.12.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 02.12.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 02.12.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 02.12.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 02.12.23
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 02.12.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 02.12.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 02.12.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 02.12.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 02.12.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 05.12.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 05.12.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 05.12.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 05.12.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 05.12.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 05.12.23
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 05.12.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 05.12.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 05.12.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 05.12.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 05.12.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1109,13 +1109,13 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 01.12.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 03.12.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 01.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 02.12.23
-DIT.E35KT6.WI.ZIP : last exported on 01.12.23
-DEL.K2PKT6.WI.ZIP : last exported on 03.12.23
-DEL.R7AKT6.WI.ZIP : last exported on 02.12.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 04.12.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 04.12.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 04.12.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 04.12.23
+DIT.E35KT6.WI.ZIP : last exported on 04.12.23
+DEL.K2PKT6.WI.ZIP : last exported on 04.12.23
+DEL.R7AKT6.WI.ZIP : last exported on 05.12.23
 DEL.N5FKT6.WI.ZIP : last exported on 01.12.23</t>
         </is>
       </c>
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 28.11.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 04.12.23
-DGV.N3LKT6.EPELS.??????.ZIP : last exported on 27.11.23</t>
+DEL.N3LKT6.HST.??????.ZIP : last exported on 05.12.23
+DGV.N3LKT6.EPELS.??????.ZIP : last exported on 04.12.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 03.12.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 03.12.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 03.12.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 03.12.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 03.12.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 03.12.23
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 03.12.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 03.12.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 03.12.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 03.12.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 03.12.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 03.12.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 03.12.23
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 01.10.23
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 01.10.23
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 01.10.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 03.12.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 04.12.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 04.12.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 04.12.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 04.12.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 04.12.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 04.12.23
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 04.12.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 04.12.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 04.12.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 04.12.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 04.12.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 04.12.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 04.12.23
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 04.12.23
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 04.12.23
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 04.12.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 04.12.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 02.12.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 04.12.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1324,7 +1324,7 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 01.12.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 04.12.23</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
@@ -1359,7 +1359,7 @@
         <is>
           <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 01.12.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
-DLV.I5XKT6.AU.A.ZIP : last exported on 05.07.23
+DLV.I5XKT6.AU.A.ZIP : last exported on 04.12.23
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
         </is>
       </c>
@@ -1367,7 +1367,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 02.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 02.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 02.12.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 04.12.23
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 02.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 02.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 02.12.23
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 03.12.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 03.12.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 04.12.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 04.12.23</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 03.12.23
-DHP.KUDKT6.ORGUNITS : last exported on 04.12.23
-DHS.R11KT6.HSB02ALL : last exported on 01.12.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 04.12.23
+DHP.KUDKT6.ORGUNITS : last exported on 05.12.23
+DHS.R11KT6.HSB02ALL : last exported on 04.12.23</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 01.12.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 01.12.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 03.12.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 01.12.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 01.12.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 01.12.23
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 01.12.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 01.12.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 01.12.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 01.12.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 04.12.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 04.12.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 04.12.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 04.12.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 04.12.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 04.12.23
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 04.12.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 04.12.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 04.12.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 04.12.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1603,38 +1603,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 02.12.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 04.12.23</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 02.12.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 02.12.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 03.12.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 02.12.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 02.12.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 02.12.23
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 02.12.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 02.12.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 02.12.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 02.12.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 02.12.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 02.12.23
-DEL.N1LKT6.MT.??????.G : last exported on 02.12.23
-DEL.N1LKT6.MT.??????.U : last exported on 02.12.23
-DEL.N1LKT6.MT.??????.AS : last exported on 02.12.23
-DVL.N1LN5X.VLM.DSP : last exported on 02.12.23
-DVL.N1LN5X.VLM.WT : last exported on 02.12.23
-DDS.N1LR11.DSP : last exported on 02.12.23
-DDS.N1LR11.WT : last exported on 02.12.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 02.12.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 02.12.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 02.12.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 02.12.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 02.12.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 02.12.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 02.12.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 02.12.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 04.12.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 04.12.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 04.12.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 04.12.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 04.12.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 04.12.23
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 04.12.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 04.12.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 04.12.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 04.12.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 04.12.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 04.12.23
+DEL.N1LKT6.MT.??????.G : last exported on 04.12.23
+DEL.N1LKT6.MT.??????.U : last exported on 04.12.23
+DEL.N1LKT6.MT.??????.AS : last exported on 04.12.23
+DVL.N1LN5X.VLM.DSP : last exported on 04.12.23
+DVL.N1LN5X.VLM.WT : last exported on 04.12.23
+DDS.N1LR11.DSP : last exported on 04.12.23
+DDS.N1LR11.WT : last exported on 04.12.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 04.12.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 04.12.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 04.12.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 04.12.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 04.12.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 04.12.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 04.12.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 04.12.23</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,55 +1662,55 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 04.12.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 04.12.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 04.12.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 04.12.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 04.12.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 04.12.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 04.12.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 04.12.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 05.12.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 05.12.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 05.12.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 05.12.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 05.12.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 05.12.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 05.12.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 05.12.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 03.12.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 01.12.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 04.12.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 03.12.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 03.12.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 03.12.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 03.12.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 03.12.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 03.12.23
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 04.12.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 04.12.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 04.12.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 04.12.23
 DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 03.12.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 03.12.23
-DEL.N1LKT6.EC.??????.G : last exported on 03.12.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 03.12.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 03.12.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 03.12.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 03.12.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 04.12.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 04.12.23
+DEL.N1LKT6.EC.??????.G : last exported on 04.12.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 04.12.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 04.12.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 04.12.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 04.12.23
 DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 03.12.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 03.12.23
-DEL.N1LKT6.EC.??????.U : last exported on 03.12.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 03.12.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 03.12.23
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 03.12.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 03.12.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 03.12.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 04.12.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 04.12.23
+DEL.N1LKT6.EC.??????.U : last exported on 04.12.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 04.12.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 04.12.23
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 04.12.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 04.12.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 04.12.23
 DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 03.12.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 03.12.23
-DEL.N1LKT6.EC.??????.AS : last exported on 03.12.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 03.12.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 03.12.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 03.12.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 03.12.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 03.12.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 03.12.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 03.12.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 03.12.23</t>
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 04.12.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 04.12.23
+DEL.N1LKT6.EC.??????.AS : last exported on 04.12.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 04.12.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 04.12.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 04.12.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 04.12.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 04.12.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 04.12.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 04.12.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 04.12.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 06.12.23 12:11
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="25" t="inlineStr">
         <is>
-          <t>Date - 05.12.2023</t>
+          <t>Date - 06.12.2023</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 04.12.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 05.12.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 05.12.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 05.12.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 05.12.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 05.12.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 05.12.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 05.12.23
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 05.12.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 05.12.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 05.12.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 05.12.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 05.12.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 06.12.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 06.12.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 06.12.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 06.12.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 06.12.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 06.12.23
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 06.12.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 06.12.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 06.12.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 06.12.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 06.12.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1110,28 +1110,28 @@
       <c r="C7" s="10" t="inlineStr">
         <is>
           <t>DLV.R31KT6.WI.C.ZIP : last exported on 04.12.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 04.12.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 05.12.23
 DLV.RPKKT6.WI.S.ZIP : last exported on 04.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 04.12.23
-DIT.E35KT6.WI.ZIP : last exported on 04.12.23
-DEL.K2PKT6.WI.ZIP : last exported on 04.12.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 05.12.23
+DIT.E35KT6.WI.ZIP : last exported on 05.12.23
+DEL.K2PKT6.WI.ZIP : last exported on 05.12.23
 DEL.R7AKT6.WI.ZIP : last exported on 05.12.23
 DEL.N5FKT6.WI.ZIP : last exported on 01.12.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 04.12.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 04.12.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 04.12.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 04.12.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 04.12.23
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 04.12.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 04.12.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 04.12.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 04.12.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 04.12.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 04.12.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 05.12.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 05.12.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 05.12.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 05.12.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 05.12.23
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 05.12.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 05.12.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 05.12.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 05.12.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 05.12.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 05.12.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1234,30 +1234,30 @@
       </c>
       <c r="C10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 28.11.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 05.12.23
+          <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 05.12.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 06.12.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 04.12.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 04.12.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 04.12.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 04.12.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 04.12.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 04.12.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 04.12.23
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 04.12.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 04.12.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 04.12.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 04.12.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 04.12.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 04.12.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 04.12.23
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 04.12.23
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 04.12.23
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 04.12.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 04.12.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 05.12.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 05.12.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 05.12.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 05.12.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 05.12.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 05.12.23
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 05.12.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 05.12.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 05.12.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 05.12.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 05.12.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 05.12.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 05.12.23
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 05.12.23
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 05.12.23
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 05.12.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 05.12.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 04.12.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 05.12.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1324,12 +1324,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 04.12.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 05.12.23</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 02.12.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 05.12.23</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1357,21 +1357,21 @@
       </c>
       <c r="C13" s="10" t="inlineStr">
         <is>
-          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 01.12.23
+          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 05.12.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
-DLV.I5XKT6.AU.A.ZIP : last exported on 04.12.23
+DLV.I5XKT6.AU.A.ZIP : last exported on 05.12.23
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
         </is>
       </c>
       <c r="D13" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 02.12.23
-DEL.N1LN3L.AU.D.GPL.DMP : last exported on 02.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 04.12.23
-DEL.N1LN0R.AU.D.CPD.DMP : last exported on 02.12.23
-DEL.N1LN0R.AU.D.CPL.DMP : last exported on 02.12.23
-DEL.KT6E35.AU.GGO.ZIP : last exported on 02.12.23
-DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 02.12.23</t>
+          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 05.12.23
+DEL.N1LN3L.AU.D.GPL.DMP : last exported on 05.12.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 05.12.23
+DEL.N1LN0R.AU.D.CPD.DMP : last exported on 05.12.23
+DEL.N1LN0R.AU.D.CPL.DMP : last exported on 05.12.23
+DEL.KT6E35.AU.GGO.ZIP : last exported on 05.12.23
+DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 05.12.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 04.12.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 04.12.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 05.12.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 05.12.23</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 04.12.23
-DHP.KUDKT6.ORGUNITS : last exported on 05.12.23
-DHS.R11KT6.HSB02ALL : last exported on 04.12.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 05.12.23
+DHP.KUDKT6.ORGUNITS : last exported on 06.12.23
+DHS.R11KT6.HSB02ALL : last exported on 05.12.23</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 04.12.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 04.12.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 04.12.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 04.12.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 04.12.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 04.12.23
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 04.12.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 04.12.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 04.12.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 04.12.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 05.12.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 05.12.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 05.12.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 05.12.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 05.12.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 05.12.23
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 05.12.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 05.12.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 05.12.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 05.12.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1603,38 +1603,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 04.12.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 05.12.23</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 04.12.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 04.12.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 04.12.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 04.12.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 04.12.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 04.12.23
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 04.12.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 04.12.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 04.12.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 04.12.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 04.12.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 04.12.23
-DEL.N1LKT6.MT.??????.G : last exported on 04.12.23
-DEL.N1LKT6.MT.??????.U : last exported on 04.12.23
-DEL.N1LKT6.MT.??????.AS : last exported on 04.12.23
-DVL.N1LN5X.VLM.DSP : last exported on 04.12.23
-DVL.N1LN5X.VLM.WT : last exported on 04.12.23
-DDS.N1LR11.DSP : last exported on 04.12.23
-DDS.N1LR11.WT : last exported on 04.12.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 04.12.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 04.12.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 04.12.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 04.12.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 04.12.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 04.12.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 04.12.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 04.12.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 05.12.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 05.12.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 05.12.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 05.12.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 05.12.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 05.12.23
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 05.12.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 05.12.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 05.12.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 05.12.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 05.12.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 05.12.23
+DEL.N1LKT6.MT.??????.G : last exported on 05.12.23
+DEL.N1LKT6.MT.??????.U : last exported on 05.12.23
+DEL.N1LKT6.MT.??????.AS : last exported on 05.12.23
+DVL.N1LN5X.VLM.DSP : last exported on 05.12.23
+DVL.N1LN5X.VLM.WT : last exported on 05.12.23
+DDS.N1LR11.DSP : last exported on 05.12.23
+DDS.N1LR11.WT : last exported on 05.12.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 05.12.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 05.12.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 05.12.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 05.12.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 05.12.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 05.12.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 05.12.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 05.12.23</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,55 +1662,55 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 05.12.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 05.12.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 05.12.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 05.12.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 05.12.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 05.12.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 05.12.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 05.12.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 06.12.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 06.12.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 06.12.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 06.12.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 06.12.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 06.12.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 06.12.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 06.12.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 03.12.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 04.12.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 05.12.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 03.12.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 03.12.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 04.12.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 04.12.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 04.12.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 04.12.23
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 05.12.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 05.12.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 05.12.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 05.12.23
 DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 04.12.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 04.12.23
-DEL.N1LKT6.EC.??????.G : last exported on 04.12.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 04.12.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 04.12.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 04.12.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 04.12.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 05.12.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 05.12.23
+DEL.N1LKT6.EC.??????.G : last exported on 05.12.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 05.12.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 05.12.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 05.12.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 05.12.23
 DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 04.12.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 04.12.23
-DEL.N1LKT6.EC.??????.U : last exported on 04.12.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 04.12.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 04.12.23
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 04.12.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 04.12.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 04.12.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 05.12.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 05.12.23
+DEL.N1LKT6.EC.??????.U : last exported on 05.12.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 05.12.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 05.12.23
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 05.12.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 05.12.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 05.12.23
 DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 04.12.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 04.12.23
-DEL.N1LKT6.EC.??????.AS : last exported on 04.12.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 04.12.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 04.12.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 04.12.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 04.12.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 04.12.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 04.12.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 04.12.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 04.12.23</t>
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 05.12.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 05.12.23
+DEL.N1LKT6.EC.??????.AS : last exported on 05.12.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 05.12.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 05.12.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 05.12.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 05.12.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 05.12.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 05.12.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 05.12.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 05.12.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 07.12.23 13:58
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="25" t="inlineStr">
         <is>
-          <t>Date - 06.12.2023</t>
+          <t>Date - 07.12.2023</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 05.12.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 06.12.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 06.12.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 06.12.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 06.12.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 06.12.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 06.12.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 06.12.23
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 06.12.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 06.12.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 06.12.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 06.12.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 06.12.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 07.12.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 07.12.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 07.12.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 07.12.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 07.12.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 07.12.23
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 07.12.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 07.12.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 07.12.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 07.12.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 07.12.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1112,26 +1112,26 @@
           <t>DLV.R31KT6.WI.C.ZIP : last exported on 04.12.23
 DLV.KZ6KT6.WI.V.ZIP : last exported on 05.12.23
 DLV.RPKKT6.WI.S.ZIP : last exported on 04.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 05.12.23
-DIT.E35KT6.WI.ZIP : last exported on 05.12.23
-DEL.K2PKT6.WI.ZIP : last exported on 05.12.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 06.12.23
+DIT.E35KT6.WI.ZIP : last exported on 06.12.23
+DEL.K2PKT6.WI.ZIP : last exported on 06.12.23
 DEL.R7AKT6.WI.ZIP : last exported on 05.12.23
 DEL.N5FKT6.WI.ZIP : last exported on 01.12.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 05.12.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 05.12.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 05.12.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 05.12.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 05.12.23
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 05.12.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 05.12.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 05.12.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 05.12.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 05.12.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 05.12.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 07.12.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 07.12.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 06.12.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 06.12.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 06.12.23
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 07.12.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 07.12.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 06.12.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 06.12.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 06.12.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 06.12.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 05.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 06.12.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 07.12.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 04.12.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 05.12.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 05.12.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 05.12.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 05.12.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 05.12.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 05.12.23
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 05.12.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 05.12.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 05.12.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 05.12.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 05.12.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 05.12.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 05.12.23
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 05.12.23
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 05.12.23
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 05.12.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 05.12.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 06.12.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 06.12.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 06.12.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 06.12.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 06.12.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 06.12.23
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 06.12.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 06.12.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 06.12.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 06.12.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 06.12.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 06.12.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 06.12.23
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 06.12.23
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 06.12.23
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 06.12.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 06.12.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 05.12.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 06.12.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1324,12 +1324,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 05.12.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 06.12.23</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 05.12.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 06.12.23</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1359,19 +1359,19 @@
         <is>
           <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 05.12.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
-DLV.I5XKT6.AU.A.ZIP : last exported on 05.12.23
+DLV.I5XKT6.AU.A.ZIP : last exported on 06.12.23
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
         </is>
       </c>
       <c r="D13" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 05.12.23
-DEL.N1LN3L.AU.D.GPL.DMP : last exported on 05.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 05.12.23
-DEL.N1LN0R.AU.D.CPD.DMP : last exported on 05.12.23
-DEL.N1LN0R.AU.D.CPL.DMP : last exported on 05.12.23
-DEL.KT6E35.AU.GGO.ZIP : last exported on 05.12.23
-DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 05.12.23</t>
+          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 06.12.23
+DEL.N1LN3L.AU.D.GPL.DMP : last exported on 06.12.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 06.12.23
+DEL.N1LN0R.AU.D.CPD.DMP : last exported on 06.12.23
+DEL.N1LN0R.AU.D.CPL.DMP : last exported on 06.12.23
+DEL.KT6E35.AU.GGO.ZIP : last exported on 06.12.23
+DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 06.12.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1399,35 +1399,35 @@
       </c>
       <c r="C14" s="10" t="inlineStr">
         <is>
-          <t>DGQ.R11KT6.BSIVM.TXT : last exported on 06.09.23
-DGQ.R11KT6.BSIVM.C.TXT : last exported on 06.09.23
-DGQ.R11KT6.BSIVM.US2.TXT : last exported on 06.09.23
-DGQ.R11KT6.PKAT.TXT : last exported on 06.09.23
-DGQ.R11KT6.PKAT.C.TXT : last exported on 06.09.23
-DGQ.R11KT6.PKAT.US2.TXT : last exported on 06.09.23
-DGQ.R11KT6.BSITK.TXT : last exported on 06.09.23
-DGQ.R11KT6.BSITX.TXT : last exported on 06.09.23
+          <t>DGQ.R11KT6.BSIVM.TXT : last exported on 06.12.23
+DGQ.R11KT6.BSIVM.C.TXT : last exported on 06.12.23
+DGQ.R11KT6.BSIVM.US2.TXT : last exported on 06.12.23
+DGQ.R11KT6.PKAT.TXT : last exported on 06.12.23
+DGQ.R11KT6.PKAT.C.TXT : last exported on 06.12.23
+DGQ.R11KT6.PKAT.US2.TXT : last exported on 06.12.23
+DGQ.R11KT6.BSITK.TXT : last exported on 06.12.23
+DGQ.R11KT6.BSITX.TXT : last exported on 06.12.23
 DGQ.R31KT6.BSIVMC.TXT : last exported on 12.09.23
 DGQ.R31KT6.PKATC.TXT : last exported on 12.09.23
-DEL.KMPKT6.APOS.DATA.ZIP : last exported on 29.11.23</t>
+DEL.KMPKT6.APOS.DATA.ZIP : last exported on 06.12.23</t>
         </is>
       </c>
       <c r="D14" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 29.11.23
-DEL.N1LN3L.AP.F.GPL.DMP : last exported on 29.11.23
-DEL.N1LN3L.AP.F.GTR.DMP : last exported on 29.11.23
-DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 29.11.23
-DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 29.11.23
-DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 29.11.23
-DEL.N1LN0R.AP.F.CPD.DMP : last exported on 29.11.23
-DEL.N1LN0R.AP.F.CPL.DMP : last exported on 29.11.23
-DEL.N1LR31.AP.F.PPS.DMP : last exported on 29.11.23
-DEL.KT6E35.AP.F.DB.ZIP : last exported on 29.11.23
-DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 29.11.23
-DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 29.11.23
-DVL.KT6N5X.VLM.AP.ZIP : last exported on 29.11.23
-DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 29.11.23</t>
+          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 06.12.23
+DEL.N1LN3L.AP.F.GPL.DMP : last exported on 06.12.23
+DEL.N1LN3L.AP.F.GTR.DMP : last exported on 06.12.23
+DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 06.12.23
+DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 06.12.23
+DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 06.12.23
+DEL.N1LN0R.AP.F.CPD.DMP : last exported on 06.12.23
+DEL.N1LN0R.AP.F.CPL.DMP : last exported on 06.12.23
+DEL.N1LR31.AP.F.PPS.DMP : last exported on 06.12.23
+DEL.KT6E35.AP.F.DB.ZIP : last exported on 06.12.23
+DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 06.12.23
+DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 06.12.23
+DVL.KT6N5X.VLM.AP.ZIP : last exported on 06.12.23
+DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 06.12.23</t>
         </is>
       </c>
       <c r="E14" s="11" t="inlineStr">
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 05.12.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 05.12.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 06.12.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 06.12.23</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 05.12.23
-DHP.KUDKT6.ORGUNITS : last exported on 06.12.23
-DHS.R11KT6.HSB02ALL : last exported on 05.12.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 06.12.23
+DHP.KUDKT6.ORGUNITS : last exported on 07.12.23
+DHS.R11KT6.HSB02ALL : last exported on 06.12.23</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 05.12.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 05.12.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 05.12.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 05.12.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 05.12.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 05.12.23
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 05.12.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 05.12.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 05.12.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 05.12.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 06.12.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 06.12.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 06.12.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 06.12.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 06.12.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 06.12.23
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 06.12.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 06.12.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 06.12.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 06.12.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1603,38 +1603,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 05.12.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 06.12.23</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 05.12.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 05.12.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 05.12.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 05.12.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 05.12.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 05.12.23
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 05.12.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 05.12.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 05.12.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 05.12.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 05.12.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 05.12.23
-DEL.N1LKT6.MT.??????.G : last exported on 05.12.23
-DEL.N1LKT6.MT.??????.U : last exported on 05.12.23
-DEL.N1LKT6.MT.??????.AS : last exported on 05.12.23
-DVL.N1LN5X.VLM.DSP : last exported on 05.12.23
-DVL.N1LN5X.VLM.WT : last exported on 05.12.23
-DDS.N1LR11.DSP : last exported on 05.12.23
-DDS.N1LR11.WT : last exported on 05.12.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 05.12.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 05.12.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 05.12.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 05.12.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 05.12.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 05.12.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 05.12.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 05.12.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 06.12.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 06.12.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 06.12.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 06.12.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 06.12.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 06.12.23
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 06.12.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 06.12.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 06.12.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 06.12.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 06.12.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 06.12.23
+DEL.N1LKT6.MT.??????.G : last exported on 06.12.23
+DEL.N1LKT6.MT.??????.U : last exported on 06.12.23
+DEL.N1LKT6.MT.??????.AS : last exported on 06.12.23
+DVL.N1LN5X.VLM.DSP : last exported on 06.12.23
+DVL.N1LN5X.VLM.WT : last exported on 06.12.23
+DDS.N1LR11.DSP : last exported on 06.12.23
+DDS.N1LR11.WT : last exported on 06.12.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 06.12.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 06.12.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 06.12.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 06.12.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 06.12.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 06.12.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 06.12.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 06.12.23</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,55 +1662,55 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 06.12.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 06.12.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 06.12.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 06.12.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 06.12.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 06.12.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 06.12.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 06.12.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 07.12.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 07.12.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 07.12.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 07.12.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 07.12.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 07.12.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 07.12.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 07.12.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 03.12.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 05.12.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 06.12.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 03.12.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 03.12.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 05.12.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 05.12.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 05.12.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 05.12.23
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 06.12.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 06.12.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 06.12.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 06.12.23
 DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 05.12.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 05.12.23
-DEL.N1LKT6.EC.??????.G : last exported on 05.12.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 05.12.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 05.12.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 05.12.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 05.12.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 06.12.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 06.12.23
+DEL.N1LKT6.EC.??????.G : last exported on 06.12.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 06.12.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 06.12.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 06.12.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 06.12.23
 DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 05.12.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 05.12.23
-DEL.N1LKT6.EC.??????.U : last exported on 05.12.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 05.12.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 05.12.23
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 05.12.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 05.12.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 05.12.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 06.12.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 06.12.23
+DEL.N1LKT6.EC.??????.U : last exported on 06.12.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 06.12.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 06.12.23
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 06.12.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 06.12.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 06.12.23
 DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 05.12.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 05.12.23
-DEL.N1LKT6.EC.??????.AS : last exported on 05.12.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 05.12.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 05.12.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 05.12.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 05.12.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 05.12.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 05.12.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 05.12.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 05.12.23</t>
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 06.12.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 06.12.23
+DEL.N1LKT6.EC.??????.AS : last exported on 06.12.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 06.12.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 06.12.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 06.12.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 06.12.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 06.12.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 06.12.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 06.12.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 06.12.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 08.12.23 11:48
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="25" t="inlineStr">
         <is>
-          <t>Date - 07.12.2023</t>
+          <t>Date - 08.12.2023</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -994,14 +994,14 @@
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 07.12.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 07.12.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 07.12.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 07.12.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 07.12.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 07.12.23
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 07.12.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 07.12.23
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 08.12.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 08.12.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 08.12.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 08.12.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 08.12.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 08.12.23
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 08.12.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 08.12.23
 DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 07.12.23
 DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 07.12.23
 DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 07.12.23</t>
@@ -1123,9 +1123,9 @@
         <is>
           <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 07.12.23
 DEL.N1LN3L.WI.D.GPL.DMP : last exported on 07.12.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 06.12.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 06.12.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 06.12.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 07.12.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 07.12.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 07.12.23
 DEL.N1LN0R.WI.D.CPD.DMP : last exported on 07.12.23
 DEL.N1LN0R.WI.D.CPL.DMP : last exported on 07.12.23
 DEL.KT6E35.WI.GGO.ZIP : last exported on 06.12.23
@@ -1241,14 +1241,14 @@
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 06.12.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 06.12.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 06.12.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 06.12.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 06.12.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 06.12.23
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 06.12.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 06.12.23
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 07.12.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 07.12.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 07.12.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 07.12.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 07.12.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 07.12.23
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 07.12.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 07.12.23
 DEL.KT6E35.TP.D.GGO.ZIP : last exported on 06.12.23
 DEL.KT6E35.TP.D.UGO.ZIP : last exported on 06.12.23
 DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 06.12.23
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 06.12.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 07.12.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1365,11 +1365,11 @@
       </c>
       <c r="D13" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 06.12.23
-DEL.N1LN3L.AU.D.GPL.DMP : last exported on 06.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 06.12.23
-DEL.N1LN0R.AU.D.CPD.DMP : last exported on 06.12.23
-DEL.N1LN0R.AU.D.CPL.DMP : last exported on 06.12.23
+          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 07.12.23
+DEL.N1LN3L.AU.D.GPL.DMP : last exported on 07.12.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 07.12.23
+DEL.N1LN0R.AU.D.CPD.DMP : last exported on 07.12.23
+DEL.N1LN0R.AU.D.CPL.DMP : last exported on 07.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 06.12.23
 DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 06.12.23</t>
         </is>
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 06.12.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 06.12.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 07.12.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 07.12.23</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1496,16 +1496,16 @@
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 06.12.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 06.12.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 06.12.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 06.12.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 06.12.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 06.12.23
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 06.12.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 06.12.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 06.12.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 06.12.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 07.12.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 07.12.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 07.12.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 07.12.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 07.12.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 07.12.23
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 07.12.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 07.12.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 07.12.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 07.12.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1608,25 +1608,25 @@
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 06.12.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 06.12.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 06.12.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 06.12.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 06.12.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 06.12.23
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 06.12.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 06.12.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 06.12.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 06.12.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 06.12.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 06.12.23
-DEL.N1LKT6.MT.??????.G : last exported on 06.12.23
-DEL.N1LKT6.MT.??????.U : last exported on 06.12.23
-DEL.N1LKT6.MT.??????.AS : last exported on 06.12.23
-DVL.N1LN5X.VLM.DSP : last exported on 06.12.23
-DVL.N1LN5X.VLM.WT : last exported on 06.12.23
-DDS.N1LR11.DSP : last exported on 06.12.23
-DDS.N1LR11.WT : last exported on 06.12.23
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 07.12.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 07.12.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 07.12.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 07.12.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 07.12.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 07.12.23
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 07.12.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 07.12.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 07.12.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 07.12.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 07.12.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 07.12.23
+DEL.N1LKT6.MT.??????.G : last exported on 07.12.23
+DEL.N1LKT6.MT.??????.U : last exported on 07.12.23
+DEL.N1LKT6.MT.??????.AS : last exported on 07.12.23
+DVL.N1LN5X.VLM.DSP : last exported on 07.12.23
+DVL.N1LN5X.VLM.WT : last exported on 07.12.23
+DDS.N1LR11.DSP : last exported on 07.12.23
+DDS.N1LR11.WT : last exported on 07.12.23
 DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 06.12.23
 DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 06.12.23
 DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 06.12.23
@@ -1678,38 +1678,38 @@
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 06.12.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 06.12.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 06.12.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 06.12.23
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 07.12.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 07.12.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 07.12.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 07.12.23
 DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 06.12.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 06.12.23
-DEL.N1LKT6.EC.??????.G : last exported on 06.12.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 06.12.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 06.12.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 06.12.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 06.12.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 07.12.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 07.12.23
+DEL.N1LKT6.EC.??????.G : last exported on 07.12.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 07.12.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 07.12.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 07.12.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 07.12.23
 DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 06.12.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 06.12.23
-DEL.N1LKT6.EC.??????.U : last exported on 06.12.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 06.12.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 06.12.23
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 06.12.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 06.12.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 06.12.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 07.12.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 07.12.23
+DEL.N1LKT6.EC.??????.U : last exported on 07.12.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 07.12.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 07.12.23
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 07.12.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 07.12.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 07.12.23
 DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 06.12.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 06.12.23
-DEL.N1LKT6.EC.??????.AS : last exported on 06.12.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 06.12.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 06.12.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 06.12.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 06.12.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 06.12.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 06.12.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 06.12.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 07.12.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 07.12.23
+DEL.N1LKT6.EC.??????.AS : last exported on 07.12.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 07.12.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 07.12.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 07.12.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 07.12.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 07.12.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 07.12.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 07.12.23
 DEL.KT6N5X.EL.F.AU.ZIP : last exported on 06.12.23</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Updated on 11.12.23 11:52
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="25" t="inlineStr">
         <is>
-          <t>Date - 08.12.2023</t>
+          <t>Date - 11.12.2023</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,21 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 06.12.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 07.12.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 08.12.23
 DEL.N1LN3L.WD.D.GPL.DMP : last exported on 08.12.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 08.12.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 10.12.23
 DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 08.12.23
 DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 08.12.23
 DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 08.12.23
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 08.12.23
 DEL.N1LN0R.WD.D.CPL.DMP : last exported on 08.12.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 07.12.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 07.12.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 07.12.23</t>
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 08.12.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 08.12.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 08.12.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1066,22 +1065,21 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 04.12.23
-DEH.N3LKT6.AP.COMPL.SNK : last exported on 04.12.23</t>
+          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 11.12.23
+DEH.N3LKT6.AP.COMPL.SNK : last exported on 11.12.23</t>
         </is>
       </c>
       <c r="D6" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 04.12.23
-DEL.N1LN3L.DN.F.GPL.DMP : last exported on 04.12.23
-DEL.N1LN3L.DN.F.GTR.DMP : last exported on 04.12.23
-DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 04.12.23
-DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 04.12.23
-DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 04.12.23
-DEL.N1LN0R.DN.F.CPD.DMP : last exported on 04.12.23
-DEL.N1LN0R.DN.F.CPL.DMP : last exported on 04.12.23
-DEL.KT6E35.SN.F.GGO.ZIP : last exported on 04.12.23
-DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 04.12.23</t>
+          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 11.12.23
+DEL.N1LN3L.DN.F.GPL.DMP : last exported on 11.12.23
+DEL.N1LN3L.DN.F.GTR.DMP : last exported on 11.12.23
+DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 11.12.23
+DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 11.12.23
+DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 11.12.23
+DEL.N1LN0R.DN.F.CPL.DMP : last exported on 11.12.23
+DEL.KT6E35.SN.F.GGO.ZIP : last exported on 11.12.23
+DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 11.12.23</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
@@ -1109,29 +1107,28 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 04.12.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 05.12.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 07.12.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 10.12.23
 DLV.RPKKT6.WI.S.ZIP : last exported on 04.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 06.12.23
-DIT.E35KT6.WI.ZIP : last exported on 06.12.23
-DEL.K2PKT6.WI.ZIP : last exported on 06.12.23
-DEL.R7AKT6.WI.ZIP : last exported on 05.12.23
-DEL.N5FKT6.WI.ZIP : last exported on 01.12.23</t>
+DLV.I5XKT6.WI.A.ZIP : last exported on 10.12.23
+DIT.E35KT6.WI.ZIP : last exported on 08.12.23
+DEL.K2PKT6.WI.ZIP : last exported on 09.12.23
+DEL.R7AKT6.WI.ZIP : last exported on 08.12.23
+DEL.N5FKT6.WI.ZIP : last exported on 08.12.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 07.12.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 07.12.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 07.12.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 07.12.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 07.12.23
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 07.12.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 07.12.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 06.12.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 06.12.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 06.12.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 06.12.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 11.12.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 11.12.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 10.12.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 10.12.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 10.12.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 11.12.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 10.12.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 10.12.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 10.12.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 10.12.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1205,7 +1202,6 @@
 DEL.N1LKQQ.TRANS.F.UPD.DMP : last exported on 25.02.23
 DEL.N1LN3L.TRANS.F.ASPD.DMP : last exported on 25.02.23
 DEL.N1LN3L.TRANS.F.ASPL.DMP : last exported on 25.02.23
-DEL.N1LN0R.TRANS.D.CPD.DMP : last exported on 25.02.23
 DEL.N1LN0R.TRANS.D.CPL.DMP : last exported on 25.02.23</t>
         </is>
       </c>
@@ -1234,30 +1230,26 @@
       </c>
       <c r="C10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 05.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 07.12.23
+          <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 11.12.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 04.12.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 07.12.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 07.12.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 07.12.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 07.12.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 07.12.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 07.12.23
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 07.12.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 07.12.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 06.12.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 06.12.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 06.12.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 06.12.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 06.12.23
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 06.12.23
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 06.12.23
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 06.12.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 06.12.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 10.12.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 10.12.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 10.12.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 10.12.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 10.12.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 10.12.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 10.12.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 10.12.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 10.12.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 10.12.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 10.12.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 10.12.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 11.12.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1283,55 +1275,47 @@
 Daily</t>
         </is>
       </c>
-      <c r="C11" s="10" t="inlineStr">
+      <c r="C11" s="10" t="inlineStr"/>
+      <c r="D11" s="10" t="inlineStr"/>
+      <c r="E11" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F11" s="12" t="inlineStr">
+        <is>
+          <t>Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="31.7" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A12" s="30" t="inlineStr">
+        <is>
+          <t>TT</t>
+        </is>
+      </c>
+      <c r="B12" s="9" t="inlineStr">
+        <is>
+          <t>17:30
+Daily</t>
+        </is>
+      </c>
+      <c r="C12" s="15" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.MANDANTN.TXT : last exported on 30.11.23</t>
         </is>
       </c>
-      <c r="D11" s="10" t="inlineStr">
+      <c r="D12" s="15" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 07.12.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 10.12.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
 DGI.KT6R11.MANDANT.TXT : last exported on 30.11.23</t>
         </is>
       </c>
-      <c r="E11" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F11" s="12" t="inlineStr">
-        <is>
-          <t>Successful</t>
-        </is>
-      </c>
-    </row>
-    <row r="12" ht="31.7" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A12" s="30" t="inlineStr">
-        <is>
-          <t>TT</t>
-        </is>
-      </c>
-      <c r="B12" s="9" t="inlineStr">
-        <is>
-          <t>17:30
-Daily</t>
-        </is>
-      </c>
-      <c r="C12" s="15" t="inlineStr">
-        <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 06.12.23</t>
-        </is>
-      </c>
-      <c r="D12" s="15" t="inlineStr">
-        <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 06.12.23</t>
-        </is>
-      </c>
       <c r="E12" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
@@ -1357,47 +1341,78 @@
       </c>
       <c r="C13" s="10" t="inlineStr">
         <is>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 08.12.23</t>
+        </is>
+      </c>
+      <c r="D13" s="10" t="inlineStr">
+        <is>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 09.12.23</t>
+        </is>
+      </c>
+      <c r="E13" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F13" s="12" t="inlineStr">
+        <is>
+          <t>Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="182.25" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A14" s="30" t="inlineStr">
+        <is>
+          <t>APOS</t>
+        </is>
+      </c>
+      <c r="B14" s="9" t="inlineStr">
+        <is>
+          <t>18:00
+Wednesday</t>
+        </is>
+      </c>
+      <c r="C14" s="10" t="inlineStr">
+        <is>
           <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 05.12.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
-DLV.I5XKT6.AU.A.ZIP : last exported on 06.12.23
+DLV.I5XKT6.AU.A.ZIP : last exported on 08.12.23
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
         </is>
       </c>
-      <c r="D13" s="10" t="inlineStr">
-        <is>
-          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 07.12.23
-DEL.N1LN3L.AU.D.GPL.DMP : last exported on 07.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 07.12.23
-DEL.N1LN0R.AU.D.CPD.DMP : last exported on 07.12.23
-DEL.N1LN0R.AU.D.CPL.DMP : last exported on 07.12.23
-DEL.KT6E35.AU.GGO.ZIP : last exported on 06.12.23
-DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 06.12.23</t>
-        </is>
-      </c>
-      <c r="E13" s="11" t="inlineStr">
+      <c r="D14" s="10" t="inlineStr">
+        <is>
+          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 09.12.23
+DEL.N1LN3L.AU.D.GPL.DMP : last exported on 09.12.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 10.12.23
+DEL.KT6E35.AU.GGO.ZIP : last exported on 09.12.23
+DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 09.12.23</t>
+        </is>
+      </c>
+      <c r="E14" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
         </is>
       </c>
-      <c r="F13" s="12" t="inlineStr">
+      <c r="F14" s="12" t="inlineStr">
         <is>
           <t>Successful</t>
         </is>
       </c>
     </row>
-    <row r="14" ht="182.25" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A14" s="30" t="inlineStr">
-        <is>
-          <t>APOS</t>
-        </is>
-      </c>
-      <c r="B14" s="9" t="inlineStr">
-        <is>
-          <t>18:00
-Wednesday</t>
-        </is>
-      </c>
-      <c r="C14" s="10" t="inlineStr">
+    <row r="15" ht="37.5" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A15" s="30" t="inlineStr">
+        <is>
+          <t>COK</t>
+        </is>
+      </c>
+      <c r="B15" s="9" t="inlineStr">
+        <is>
+          <t>18:05
+Daily</t>
+        </is>
+      </c>
+      <c r="C15" s="16" t="inlineStr">
         <is>
           <t>DGQ.R11KT6.BSIVM.TXT : last exported on 06.12.23
 DGQ.R11KT6.BSIVM.C.TXT : last exported on 06.12.23
@@ -1412,7 +1427,7 @@
 DEL.KMPKT6.APOS.DATA.ZIP : last exported on 06.12.23</t>
         </is>
       </c>
-      <c r="D14" s="10" t="inlineStr">
+      <c r="D15" s="16" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 06.12.23
 DEL.N1LN3L.AP.F.GPL.DMP : last exported on 06.12.23
@@ -1420,48 +1435,12 @@
 DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 06.12.23
 DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 06.12.23
 DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 06.12.23
-DEL.N1LN0R.AP.F.CPD.DMP : last exported on 06.12.23
 DEL.N1LN0R.AP.F.CPL.DMP : last exported on 06.12.23
 DEL.N1LR31.AP.F.PPS.DMP : last exported on 06.12.23
 DEL.KT6E35.AP.F.DB.ZIP : last exported on 06.12.23
 DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 06.12.23
 DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 06.12.23
-DVL.KT6N5X.VLM.AP.ZIP : last exported on 06.12.23
-DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 06.12.23</t>
-        </is>
-      </c>
-      <c r="E14" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F14" s="12" t="inlineStr">
-        <is>
-          <t>Successful</t>
-        </is>
-      </c>
-    </row>
-    <row r="15" ht="37.5" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A15" s="30" t="inlineStr">
-        <is>
-          <t>COK</t>
-        </is>
-      </c>
-      <c r="B15" s="9" t="inlineStr">
-        <is>
-          <t>18:05
-Daily</t>
-        </is>
-      </c>
-      <c r="C15" s="16" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="D15" s="16" t="inlineStr">
-        <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 07.12.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 07.12.23</t>
+DVL.KT6N5X.VLM.AP.ZIP : last exported on 06.12.23</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1468,13 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 06.12.23
-DHP.KUDKT6.ORGUNITS : last exported on 07.12.23
-DHS.R11KT6.HSB02ALL : last exported on 06.12.23</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 07.12.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 07.12.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 07.12.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 07.12.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 07.12.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 07.12.23
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 07.12.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 07.12.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 07.12.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 07.12.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 10.12.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 10.12.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1533,49 +1502,57 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 10.12.23
+DHP.KUDKT6.ORGUNITS : last exported on 11.12.23
+DHS.R11KT6.HSB02ALL : last exported on 08.12.23</t>
+        </is>
+      </c>
+      <c r="D17" s="10" t="inlineStr">
+        <is>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 08.12.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 08.12.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 10.12.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 08.12.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 08.12.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 08.12.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 08.12.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 08.12.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 08.12.23</t>
+        </is>
+      </c>
+      <c r="E17" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F17" s="13" t="inlineStr">
+        <is>
+          <t>DryRun</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="36.75" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A18" s="30" t="inlineStr">
+        <is>
+          <t>Translations</t>
+        </is>
+      </c>
+      <c r="B18" s="9" t="inlineStr">
+        <is>
+          <t>19:00
+Sunday</t>
+        </is>
+      </c>
+      <c r="C18" s="15" t="inlineStr">
+        <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="D17" s="10" t="inlineStr">
+      <c r="D18" s="15" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.EUTRM.F.GPD.DMP : last exported on 20.05.22
 DEL.N1LN3L.EUTRM.F.GPL.DMP : last exported on 20.05.22
-DEL.N1LN3L.EUTRM.F.GTR.DMP : last exported on 20.05.22
-DEL.N1LN3L.EUTRM.F.CPD.DMP : last exported on 20.05.22
-DEL.N1LN3L.EUTRM.F.CPL.DMP : last exported on 20.05.22</t>
-        </is>
-      </c>
-      <c r="E17" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F17" s="13" t="inlineStr">
-        <is>
-          <t>DryRun</t>
-        </is>
-      </c>
-    </row>
-    <row r="18" ht="36.75" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A18" s="30" t="inlineStr">
-        <is>
-          <t>Translations</t>
-        </is>
-      </c>
-      <c r="B18" s="9" t="inlineStr">
-        <is>
-          <t>19:00
-Sunday</t>
-        </is>
-      </c>
-      <c r="C18" s="15" t="inlineStr">
-        <is>
-          <t>DIT.E35KT6.TRANS.ZIP : last exported on 09.01.23</t>
-        </is>
-      </c>
-      <c r="D18" s="15" t="inlineStr">
-        <is>
-          <t>DEL.N1LE35.TRANS.ZIP : last exported on 03.12.23</t>
+DEL.N1LN3L.EUTRM.F.GTR.DMP : last exported on 20.05.22</t>
         </is>
       </c>
       <c r="E18" s="11" t="inlineStr">
@@ -1603,38 +1580,12 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 06.12.23</t>
+          <t>DIT.E35KT6.TRANS.ZIP : last exported on 09.01.23</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 07.12.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 07.12.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 07.12.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 07.12.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 07.12.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 07.12.23
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 07.12.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 07.12.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 07.12.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 07.12.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 07.12.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 07.12.23
-DEL.N1LKT6.MT.??????.G : last exported on 07.12.23
-DEL.N1LKT6.MT.??????.U : last exported on 07.12.23
-DEL.N1LKT6.MT.??????.AS : last exported on 07.12.23
-DVL.N1LN5X.VLM.DSP : last exported on 07.12.23
-DVL.N1LN5X.VLM.WT : last exported on 07.12.23
-DDS.N1LR11.DSP : last exported on 07.12.23
-DDS.N1LR11.WT : last exported on 07.12.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 06.12.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 06.12.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 06.12.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 06.12.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 06.12.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 06.12.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 06.12.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 06.12.23</t>
+          <t>DEL.N1LE35.TRANS.ZIP : last exported on 10.12.23</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,55 +1613,37 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 07.12.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 07.12.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 07.12.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 07.12.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 07.12.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 07.12.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 07.12.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 07.12.23
-DDC.R11KT6.ELFI.MD.TXT : last exported on 03.12.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 06.12.23
-DDC.R11KT6.ELFI.PK.TXT : last exported on 03.12.23
-DDC.R11KT6.ELFI.PR.TXT : last exported on 03.12.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 09.12.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 07.12.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 07.12.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 07.12.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 07.12.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 07.12.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 07.12.23
-DEL.N1LKT6.EC.??????.G : last exported on 07.12.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 07.12.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 07.12.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 07.12.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 07.12.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 07.12.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 07.12.23
-DEL.N1LKT6.EC.??????.U : last exported on 07.12.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 07.12.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 07.12.23
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 07.12.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 07.12.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 07.12.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 07.12.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 07.12.23
-DEL.N1LKT6.EC.??????.AS : last exported on 07.12.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 07.12.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 07.12.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 07.12.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 07.12.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 07.12.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 07.12.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 07.12.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 06.12.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 09.12.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 09.12.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 10.12.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 09.12.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 09.12.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 09.12.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 09.12.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 09.12.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 09.12.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 09.12.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 09.12.23
+DEL.N1LKT6.MT.??????.G : last exported on 09.12.23
+DEL.N1LKT6.MT.??????.U : last exported on 09.12.23
+DEL.N1LKT6.MT.??????.AS : last exported on 09.12.23
+DVL.N1LN5X.VLM.DSP : last exported on 09.12.23
+DVL.N1LN5X.VLM.WT : last exported on 09.12.23
+DDS.N1LR11.DSP : last exported on 09.12.23
+DDS.N1LR11.WT : last exported on 09.12.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 09.12.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 09.12.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 09.12.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 09.12.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 09.12.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 09.12.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 09.12.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 09.12.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1727,8 +1660,13 @@
     <row r="21" ht="16.5" customHeight="1" thickBot="1" thickTop="1">
       <c r="A21" s="5" t="n"/>
       <c r="B21" s="6" t="n"/>
-      <c r="C21" s="4" t="n"/>
-      <c r="D21" s="4" t="n"/>
+      <c r="C21" s="4" t="inlineStr">
+        <is>
+          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 11.12.23
+DHP.KUDKT6.DPO.EMAILS : last exported on 11.12.23</t>
+        </is>
+      </c>
+      <c r="D21" s="4" t="inlineStr"/>
       <c r="E21" s="2" t="n"/>
       <c r="F21" s="3" t="n"/>
     </row>
@@ -1741,10 +1679,56 @@
       <c r="B22" s="27" t="n"/>
       <c r="C22" s="14" t="inlineStr">
         <is>
-          <t>Utilization of space in Database Server is 24% (free 76%)</t>
-        </is>
-      </c>
-      <c r="D22" s="5" t="n"/>
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 11.12.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 11.12.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 11.12.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 11.12.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 11.12.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 11.12.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 11.12.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 11.12.23
+DDC.R11KT6.ELFI.MD.TXT : last exported on 10.12.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 08.12.23
+DDC.R11KT6.ELFI.PK.TXT : last exported on 10.12.23
+DDC.R11KT6.ELFI.PR.TXT : last exported on 10.12.23</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="inlineStr">
+        <is>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 10.12.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 10.12.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 10.12.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 10.12.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 28.11.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 10.12.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 10.12.23
+DEL.N1LKT6.EC.??????.G : last exported on 10.12.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 10.12.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 10.12.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 10.12.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 10.12.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 28.11.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 10.12.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 10.12.23
+DEL.N1LKT6.EC.??????.U : last exported on 10.12.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 10.12.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 10.12.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 10.12.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 10.12.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 28.11.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 10.12.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 10.12.23
+DEL.N1LKT6.EC.??????.AS : last exported on 10.12.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 10.12.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 10.12.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 10.12.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 10.12.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 10.12.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 10.12.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 10.12.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 10.12.23</t>
+        </is>
+      </c>
       <c r="F22" s="3" t="n"/>
     </row>
     <row r="23" ht="15" customHeight="1" thickBot="1" thickTop="1">

</xml_diff>

<commit_message>
Updated on 11.12.23 12:15
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -1000,6 +1000,7 @@
 DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 08.12.23
 DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 08.12.23
 DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 08.12.23
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 08.12.23
 DEL.N1LN0R.WD.D.CPL.DMP : last exported on 08.12.23
 DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 08.12.23
 DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 08.12.23
@@ -1077,6 +1078,7 @@
 DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 11.12.23
 DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 11.12.23
 DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 11.12.23
+DEL.N1LN0R.DN.F.CPD.DMP : last exported on 11.12.23
 DEL.N1LN0R.DN.F.CPL.DMP : last exported on 11.12.23
 DEL.KT6E35.SN.F.GGO.ZIP : last exported on 11.12.23
 DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 11.12.23</t>
@@ -1124,6 +1126,7 @@
 DEL.N1LN3L.WI.D.GTR.DMP : last exported on 10.12.23
 DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 10.12.23
 DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 10.12.23
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 11.12.23
 DEL.N1LN0R.WI.D.CPL.DMP : last exported on 11.12.23
 DEL.KT6E35.WI.GGO.ZIP : last exported on 10.12.23
 DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 10.12.23
@@ -1202,6 +1205,7 @@
 DEL.N1LKQQ.TRANS.F.UPD.DMP : last exported on 25.02.23
 DEL.N1LN3L.TRANS.F.ASPD.DMP : last exported on 25.02.23
 DEL.N1LN3L.TRANS.F.ASPL.DMP : last exported on 25.02.23
+DEL.N1LN0R.TRANS.D.CPD.DMP : last exported on 25.02.23
 DEL.N1LN0R.TRANS.D.CPL.DMP : last exported on 25.02.23</t>
         </is>
       </c>
@@ -1243,12 +1247,16 @@
 DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 10.12.23
 DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 10.12.23
 DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 10.12.23
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 10.12.23
 DEL.N1LN0R.TP.D.CPL.DMP : last exported on 10.12.23
 DEL.KT6E35.TP.D.GGO.ZIP : last exported on 10.12.23
 DEL.KT6E35.TP.D.UGO.ZIP : last exported on 10.12.23
 DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 10.12.23
 DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 10.12.23
 DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 10.12.23
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 11.12.23
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 11.12.23
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 10.12.23
 DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 11.12.23</t>
         </is>
       </c>
@@ -1275,37 +1283,12 @@
 Daily</t>
         </is>
       </c>
-      <c r="C11" s="10" t="inlineStr"/>
-      <c r="D11" s="10" t="inlineStr"/>
-      <c r="E11" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F11" s="12" t="inlineStr">
-        <is>
-          <t>Successful</t>
-        </is>
-      </c>
-    </row>
-    <row r="12" ht="31.7" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A12" s="30" t="inlineStr">
-        <is>
-          <t>TT</t>
-        </is>
-      </c>
-      <c r="B12" s="9" t="inlineStr">
-        <is>
-          <t>17:30
-Daily</t>
-        </is>
-      </c>
-      <c r="C12" s="15" t="inlineStr">
+      <c r="C11" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.MANDANTN.TXT : last exported on 30.11.23</t>
         </is>
       </c>
-      <c r="D12" s="15" t="inlineStr">
+      <c r="D11" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
@@ -1316,6 +1299,39 @@
 DGI.KT6R11.MANDANT.TXT : last exported on 30.11.23</t>
         </is>
       </c>
+      <c r="E11" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F11" s="12" t="inlineStr">
+        <is>
+          <t>Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="31.7" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A12" s="30" t="inlineStr">
+        <is>
+          <t>TT</t>
+        </is>
+      </c>
+      <c r="B12" s="9" t="inlineStr">
+        <is>
+          <t>17:30
+Daily</t>
+        </is>
+      </c>
+      <c r="C12" s="15" t="inlineStr">
+        <is>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 08.12.23</t>
+        </is>
+      </c>
+      <c r="D12" s="15" t="inlineStr">
+        <is>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 09.12.23</t>
+        </is>
+      </c>
       <c r="E12" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
@@ -1340,39 +1356,6 @@
         </is>
       </c>
       <c r="C13" s="10" t="inlineStr">
-        <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 08.12.23</t>
-        </is>
-      </c>
-      <c r="D13" s="10" t="inlineStr">
-        <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 09.12.23</t>
-        </is>
-      </c>
-      <c r="E13" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F13" s="12" t="inlineStr">
-        <is>
-          <t>Successful</t>
-        </is>
-      </c>
-    </row>
-    <row r="14" ht="182.25" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A14" s="30" t="inlineStr">
-        <is>
-          <t>APOS</t>
-        </is>
-      </c>
-      <c r="B14" s="9" t="inlineStr">
-        <is>
-          <t>18:00
-Wednesday</t>
-        </is>
-      </c>
-      <c r="C14" s="10" t="inlineStr">
         <is>
           <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 05.12.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
@@ -1380,39 +1363,41 @@
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
         </is>
       </c>
-      <c r="D14" s="10" t="inlineStr">
+      <c r="D13" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 09.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 09.12.23
 DEL.N1LN3L.AU.D.GTR.DMP : last exported on 10.12.23
+DEL.N1LN0R.AU.D.CPD.DMP : last exported on 09.12.23
+DEL.N1LN0R.AU.D.CPL.DMP : last exported on 09.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 09.12.23
 DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 09.12.23</t>
         </is>
       </c>
-      <c r="E14" s="11" t="inlineStr">
+      <c r="E13" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
         </is>
       </c>
-      <c r="F14" s="12" t="inlineStr">
+      <c r="F13" s="12" t="inlineStr">
         <is>
           <t>Successful</t>
         </is>
       </c>
     </row>
-    <row r="15" ht="37.5" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A15" s="30" t="inlineStr">
-        <is>
-          <t>COK</t>
-        </is>
-      </c>
-      <c r="B15" s="9" t="inlineStr">
-        <is>
-          <t>18:05
-Daily</t>
-        </is>
-      </c>
-      <c r="C15" s="16" t="inlineStr">
+    <row r="14" ht="182.25" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A14" s="30" t="inlineStr">
+        <is>
+          <t>APOS</t>
+        </is>
+      </c>
+      <c r="B14" s="9" t="inlineStr">
+        <is>
+          <t>18:00
+Wednesday</t>
+        </is>
+      </c>
+      <c r="C14" s="10" t="inlineStr">
         <is>
           <t>DGQ.R11KT6.BSIVM.TXT : last exported on 06.12.23
 DGQ.R11KT6.BSIVM.C.TXT : last exported on 06.12.23
@@ -1427,7 +1412,7 @@
 DEL.KMPKT6.APOS.DATA.ZIP : last exported on 06.12.23</t>
         </is>
       </c>
-      <c r="D15" s="16" t="inlineStr">
+      <c r="D14" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 06.12.23
 DEL.N1LN3L.AP.F.GPL.DMP : last exported on 06.12.23
@@ -1435,12 +1420,48 @@
 DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 06.12.23
 DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 06.12.23
 DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 06.12.23
+DEL.N1LN0R.AP.F.CPD.DMP : last exported on 06.12.23
 DEL.N1LN0R.AP.F.CPL.DMP : last exported on 06.12.23
 DEL.N1LR31.AP.F.PPS.DMP : last exported on 06.12.23
 DEL.KT6E35.AP.F.DB.ZIP : last exported on 06.12.23
 DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 06.12.23
 DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 06.12.23
-DVL.KT6N5X.VLM.AP.ZIP : last exported on 06.12.23</t>
+DVL.KT6N5X.VLM.AP.ZIP : last exported on 06.12.23
+DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 06.12.23</t>
+        </is>
+      </c>
+      <c r="E14" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F14" s="12" t="inlineStr">
+        <is>
+          <t>Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="37.5" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A15" s="30" t="inlineStr">
+        <is>
+          <t>COK</t>
+        </is>
+      </c>
+      <c r="B15" s="9" t="inlineStr">
+        <is>
+          <t>18:05
+Daily</t>
+        </is>
+      </c>
+      <c r="C15" s="16" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="D15" s="16" t="inlineStr">
+        <is>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 10.12.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 10.12.23</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1467,47 +1488,13 @@
         </is>
       </c>
       <c r="C16" s="10" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="D16" s="10" t="inlineStr">
-        <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 10.12.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 10.12.23</t>
-        </is>
-      </c>
-      <c r="E16" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F16" s="12" t="inlineStr">
-        <is>
-          <t>Successful</t>
-        </is>
-      </c>
-    </row>
-    <row r="17" ht="48.2" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A17" s="30" t="inlineStr">
-        <is>
-          <t>EUTERM</t>
-        </is>
-      </c>
-      <c r="B17" s="9" t="inlineStr">
-        <is>
-          <t>18:15
-Daily</t>
-        </is>
-      </c>
-      <c r="C17" s="10" t="inlineStr">
         <is>
           <t>DHP.KUDKT6.KVPSIMPORT : last exported on 10.12.23
 DHP.KUDKT6.ORGUNITS : last exported on 11.12.23
 DHS.R11KT6.HSB02ALL : last exported on 08.12.23</t>
         </is>
       </c>
-      <c r="D17" s="10" t="inlineStr">
+      <c r="D16" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 08.12.23
 DEL.N1LN3L.DP.F.GPL.DMP : last exported on 08.12.23
@@ -1515,11 +1502,49 @@
 DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 08.12.23
 DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 08.12.23
 DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 08.12.23
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 08.12.23
 DEL.N1LN0R.DP.F.CPL.DMP : last exported on 08.12.23
 DEL.N1LN3L.DISSORG.ZIP : last exported on 08.12.23
 DEL.N1LN3L.DISSAORG.ZIP : last exported on 08.12.23</t>
         </is>
       </c>
+      <c r="E16" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F16" s="12" t="inlineStr">
+        <is>
+          <t>Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" ht="48.2" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A17" s="30" t="inlineStr">
+        <is>
+          <t>EUTERM</t>
+        </is>
+      </c>
+      <c r="B17" s="9" t="inlineStr">
+        <is>
+          <t>18:15
+Daily</t>
+        </is>
+      </c>
+      <c r="C17" s="10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="D17" s="10" t="inlineStr">
+        <is>
+          <t>DEL.N1LN3L.EUTRM.F.GPD.DMP : last exported on 20.05.22
+DEL.N1LN3L.EUTRM.F.GPL.DMP : last exported on 20.05.22
+DEL.N1LN3L.EUTRM.F.GTR.DMP : last exported on 20.05.22
+DEL.N1LN3L.EUTRM.F.CPD.DMP : last exported on 20.05.22
+DEL.N1LN3L.EUTRM.F.CPL.DMP : last exported on 20.05.22</t>
+        </is>
+      </c>
       <c r="E17" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
@@ -1545,14 +1570,12 @@
       </c>
       <c r="C18" s="15" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>DIT.E35KT6.TRANS.ZIP : last exported on 09.01.23</t>
         </is>
       </c>
       <c r="D18" s="15" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EUTRM.F.GPD.DMP : last exported on 20.05.22
-DEL.N1LN3L.EUTRM.F.GPL.DMP : last exported on 20.05.22
-DEL.N1LN3L.EUTRM.F.GTR.DMP : last exported on 20.05.22</t>
+          <t>DEL.N1LE35.TRANS.ZIP : last exported on 10.12.23</t>
         </is>
       </c>
       <c r="E18" s="11" t="inlineStr">
@@ -1580,43 +1603,10 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.TRANS.ZIP : last exported on 09.01.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 09.12.23</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
-        <is>
-          <t>DEL.N1LE35.TRANS.ZIP : last exported on 10.12.23</t>
-        </is>
-      </c>
-      <c r="E19" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F19" s="12" t="inlineStr">
-        <is>
-          <t>Successful</t>
-        </is>
-      </c>
-    </row>
-    <row r="20" ht="409.6" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A20" s="30" t="inlineStr">
-        <is>
-          <t>ELFI</t>
-        </is>
-      </c>
-      <c r="B20" s="9" t="inlineStr">
-        <is>
-          <t>20:25
-Daily</t>
-        </is>
-      </c>
-      <c r="C20" s="10" t="inlineStr">
-        <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 09.12.23</t>
-        </is>
-      </c>
-      <c r="D20" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 09.12.23
 DEL.N1LN3L.MT.F.GPL.DMP : last exported on 09.12.23
@@ -1624,6 +1614,7 @@
 DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 09.12.23
 DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 09.12.23
 DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 09.12.23
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 09.12.23
 DEL.N1LN0R.MT.F.CPL.DMP : last exported on 09.12.23
 DEL.N1LR31.MT.F.GPD.DMP : last exported on 09.12.23
 DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 09.12.23
@@ -1644,6 +1635,82 @@
 DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 09.12.23
 DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 09.12.23
 DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 09.12.23</t>
+        </is>
+      </c>
+      <c r="E19" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F19" s="12" t="inlineStr">
+        <is>
+          <t>Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" ht="409.6" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A20" s="30" t="inlineStr">
+        <is>
+          <t>ELFI</t>
+        </is>
+      </c>
+      <c r="B20" s="9" t="inlineStr">
+        <is>
+          <t>20:25
+Daily</t>
+        </is>
+      </c>
+      <c r="C20" s="10" t="inlineStr">
+        <is>
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 11.12.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 11.12.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 11.12.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 11.12.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 11.12.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 11.12.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 11.12.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 11.12.23
+DDC.R11KT6.ELFI.MD.TXT : last exported on 10.12.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 08.12.23
+DDC.R11KT6.ELFI.PK.TXT : last exported on 10.12.23
+DDC.R11KT6.ELFI.PR.TXT : last exported on 10.12.23</t>
+        </is>
+      </c>
+      <c r="D20" s="10" t="inlineStr">
+        <is>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 10.12.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 10.12.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 10.12.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 10.12.23
+DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 28.11.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 10.12.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 10.12.23
+DEL.N1LKT6.EC.??????.G : last exported on 10.12.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 10.12.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 10.12.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 10.12.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 10.12.23
+DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 28.11.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 10.12.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 10.12.23
+DEL.N1LKT6.EC.??????.U : last exported on 10.12.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 10.12.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 10.12.23
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 10.12.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 10.12.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 10.12.23
+DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 28.11.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 10.12.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 10.12.23
+DEL.N1LKT6.EC.??????.AS : last exported on 10.12.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 10.12.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 10.12.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 10.12.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 10.12.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 10.12.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 10.12.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 10.12.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 10.12.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 12.12.23 12:29
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="25" t="inlineStr">
         <is>
-          <t>Date - 11.12.2023</t>
+          <t>Date - 12.12.2023</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 07.12.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 11.12.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 08.12.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 08.12.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 10.12.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 08.12.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 08.12.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 08.12.23
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 08.12.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 08.12.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 08.12.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 08.12.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 08.12.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 12.12.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 12.12.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 12.12.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 12.12.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 12.12.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 12.12.23
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 12.12.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 12.12.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 12.12.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 12.12.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 12.12.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1110,11 +1110,11 @@
       <c r="C7" s="10" t="inlineStr">
         <is>
           <t>DLV.R31KT6.WI.C.ZIP : last exported on 07.12.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 10.12.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 04.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 10.12.23
-DIT.E35KT6.WI.ZIP : last exported on 08.12.23
-DEL.K2PKT6.WI.ZIP : last exported on 09.12.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 11.12.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 11.12.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 11.12.23
+DIT.E35KT6.WI.ZIP : last exported on 11.12.23
+DEL.K2PKT6.WI.ZIP : last exported on 11.12.23
 DEL.R7AKT6.WI.ZIP : last exported on 08.12.23
 DEL.N5FKT6.WI.ZIP : last exported on 08.12.23</t>
         </is>
@@ -1123,15 +1123,15 @@
         <is>
           <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 11.12.23
 DEL.N1LN3L.WI.D.GPL.DMP : last exported on 11.12.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 10.12.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 10.12.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 10.12.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 11.12.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 11.12.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 11.12.23
 DEL.N1LN0R.WI.D.CPD.DMP : last exported on 11.12.23
 DEL.N1LN0R.WI.D.CPL.DMP : last exported on 11.12.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 10.12.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 10.12.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 10.12.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 10.12.23</t>
+DEL.KT6E35.WI.GGO.ZIP : last exported on 11.12.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 11.12.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 11.12.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 11.12.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,28 +1235,28 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 11.12.23
-DGV.N3LKT6.EPELS.??????.ZIP : last exported on 04.12.23</t>
+DEL.N3LKT6.HST.??????.ZIP : last exported on 12.12.23
+DGV.N3LKT6.EPELS.??????.ZIP : last exported on 11.12.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 10.12.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 10.12.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 10.12.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 10.12.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 10.12.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 10.12.23
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 10.12.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 10.12.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 10.12.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 10.12.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 10.12.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 10.12.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 10.12.23
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 11.12.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 11.12.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 11.12.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 11.12.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 11.12.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 11.12.23
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 11.12.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 11.12.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 11.12.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 11.12.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 11.12.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 11.12.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 11.12.23
 DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 11.12.23
 DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 11.12.23
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 10.12.23
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 11.12.23
 DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 11.12.23</t>
         </is>
       </c>
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 10.12.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 11.12.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1324,7 +1324,7 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 08.12.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 11.12.23</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
@@ -1359,7 +1359,7 @@
         <is>
           <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 05.12.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
-DLV.I5XKT6.AU.A.ZIP : last exported on 08.12.23
+DLV.I5XKT6.AU.A.ZIP : last exported on 11.12.23
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
         </is>
       </c>
@@ -1367,7 +1367,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 09.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 09.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 10.12.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 11.12.23
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 09.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 09.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 09.12.23
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 10.12.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 10.12.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 11.12.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 11.12.23</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 10.12.23
-DHP.KUDKT6.ORGUNITS : last exported on 11.12.23
-DHS.R11KT6.HSB02ALL : last exported on 08.12.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 11.12.23
+DHP.KUDKT6.ORGUNITS : last exported on 12.12.23
+DHS.R11KT6.HSB02ALL : last exported on 11.12.23</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 08.12.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 08.12.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 10.12.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 08.12.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 08.12.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 08.12.23
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 08.12.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 08.12.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 08.12.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 08.12.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 11.12.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 11.12.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 11.12.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 11.12.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 11.12.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 11.12.23
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 11.12.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 11.12.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 11.12.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 11.12.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1603,38 +1603,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 09.12.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 11.12.23</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 09.12.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 09.12.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 10.12.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 09.12.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 09.12.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 09.12.23
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 09.12.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 09.12.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 09.12.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 09.12.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 09.12.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 09.12.23
-DEL.N1LKT6.MT.??????.G : last exported on 09.12.23
-DEL.N1LKT6.MT.??????.U : last exported on 09.12.23
-DEL.N1LKT6.MT.??????.AS : last exported on 09.12.23
-DVL.N1LN5X.VLM.DSP : last exported on 09.12.23
-DVL.N1LN5X.VLM.WT : last exported on 09.12.23
-DDS.N1LR11.DSP : last exported on 09.12.23
-DDS.N1LR11.WT : last exported on 09.12.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 09.12.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 09.12.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 09.12.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 09.12.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 09.12.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 09.12.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 09.12.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 09.12.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 11.12.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 11.12.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 11.12.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 11.12.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 11.12.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 11.12.23
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 11.12.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 11.12.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 11.12.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 11.12.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 11.12.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 11.12.23
+DEL.N1LKT6.MT.??????.G : last exported on 11.12.23
+DEL.N1LKT6.MT.??????.U : last exported on 11.12.23
+DEL.N1LKT6.MT.??????.AS : last exported on 11.12.23
+DVL.N1LN5X.VLM.DSP : last exported on 11.12.23
+DVL.N1LN5X.VLM.WT : last exported on 11.12.23
+DDS.N1LR11.DSP : last exported on 11.12.23
+DDS.N1LR11.WT : last exported on 11.12.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 11.12.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 11.12.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 11.12.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 11.12.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 11.12.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 11.12.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 11.12.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 11.12.23</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,55 +1662,55 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 11.12.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 11.12.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 11.12.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 11.12.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 11.12.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 11.12.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 11.12.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 11.12.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 12.12.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 12.12.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 12.12.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 12.12.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 12.12.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 12.12.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 12.12.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 12.12.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 10.12.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 08.12.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 11.12.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 10.12.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 10.12.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 10.12.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 10.12.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 10.12.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 10.12.23
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 11.12.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 11.12.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 11.12.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 11.12.23
 DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 10.12.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 10.12.23
-DEL.N1LKT6.EC.??????.G : last exported on 10.12.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 10.12.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 10.12.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 10.12.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 10.12.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 11.12.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 11.12.23
+DEL.N1LKT6.EC.??????.G : last exported on 11.12.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 11.12.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 11.12.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 11.12.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 11.12.23
 DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 10.12.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 10.12.23
-DEL.N1LKT6.EC.??????.U : last exported on 10.12.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 10.12.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 10.12.23
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 10.12.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 10.12.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 10.12.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 11.12.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 11.12.23
+DEL.N1LKT6.EC.??????.U : last exported on 11.12.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 11.12.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 11.12.23
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 11.12.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 11.12.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 11.12.23
 DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 10.12.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 10.12.23
-DEL.N1LKT6.EC.??????.AS : last exported on 10.12.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 10.12.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 10.12.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 10.12.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 10.12.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 10.12.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 10.12.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 10.12.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 10.12.23</t>
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 11.12.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 11.12.23
+DEL.N1LKT6.EC.??????.AS : last exported on 11.12.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 11.12.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 11.12.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 11.12.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 11.12.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 11.12.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 11.12.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 11.12.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 11.12.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 13.12.23 12:35
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="25" t="inlineStr">
         <is>
-          <t>Date - 12.12.2023</t>
+          <t>Date - 13.12.2023</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 11.12.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 12.12.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 12.12.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 12.12.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 12.12.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 12.12.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 12.12.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 12.12.23
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 12.12.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 12.12.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 12.12.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 12.12.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 12.12.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 13.12.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 13.12.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 13.12.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 13.12.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 13.12.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 13.12.23
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 13.12.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 13.12.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 13.12.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 13.12.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 13.12.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1109,29 +1109,29 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 07.12.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 11.12.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 11.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 11.12.23
-DIT.E35KT6.WI.ZIP : last exported on 11.12.23
-DEL.K2PKT6.WI.ZIP : last exported on 11.12.23
-DEL.R7AKT6.WI.ZIP : last exported on 08.12.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 12.12.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 12.12.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 12.12.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 12.12.23
+DIT.E35KT6.WI.ZIP : last exported on 12.12.23
+DEL.K2PKT6.WI.ZIP : last exported on 12.12.23
+DEL.R7AKT6.WI.ZIP : last exported on 13.12.23
 DEL.N5FKT6.WI.ZIP : last exported on 08.12.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 11.12.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 11.12.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 11.12.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 11.12.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 11.12.23
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 11.12.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 11.12.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 11.12.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 11.12.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 11.12.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 11.12.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 12.12.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 12.12.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 12.12.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 12.12.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 12.12.23
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 12.12.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 12.12.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 12.12.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 12.12.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 12.12.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 12.12.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 12.12.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 13.12.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 11.12.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 11.12.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 11.12.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 11.12.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 11.12.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 11.12.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 11.12.23
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 11.12.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 11.12.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 11.12.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 11.12.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 11.12.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 11.12.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 11.12.23
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 11.12.23
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 11.12.23
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 11.12.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 11.12.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 12.12.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 12.12.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 12.12.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 12.12.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 12.12.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 12.12.23
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 12.12.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 12.12.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 12.12.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 12.12.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 12.12.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 12.12.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 12.12.23
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 12.12.23
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 12.12.23
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 12.12.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 12.12.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 11.12.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 12.12.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1324,12 +1324,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 11.12.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 12.12.23</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 09.12.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 12.12.23</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1367,7 +1367,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 09.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 09.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 11.12.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 12.12.23
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 09.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 09.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 09.12.23
@@ -1407,8 +1407,8 @@
 DGQ.R11KT6.PKAT.US2.TXT : last exported on 06.12.23
 DGQ.R11KT6.BSITK.TXT : last exported on 06.12.23
 DGQ.R11KT6.BSITX.TXT : last exported on 06.12.23
-DGQ.R31KT6.BSIVMC.TXT : last exported on 12.09.23
-DGQ.R31KT6.PKATC.TXT : last exported on 12.09.23
+DGQ.R31KT6.BSIVMC.TXT : last exported on 12.12.23
+DGQ.R31KT6.PKATC.TXT : last exported on 12.12.23
 DEL.KMPKT6.APOS.DATA.ZIP : last exported on 06.12.23</t>
         </is>
       </c>
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 11.12.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 11.12.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 12.12.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 12.12.23</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 11.12.23
-DHP.KUDKT6.ORGUNITS : last exported on 12.12.23
-DHS.R11KT6.HSB02ALL : last exported on 11.12.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 12.12.23
+DHP.KUDKT6.ORGUNITS : last exported on 13.12.23
+DHS.R11KT6.HSB02ALL : last exported on 12.12.23</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 11.12.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 11.12.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 11.12.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 11.12.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 11.12.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 11.12.23
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 11.12.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 11.12.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 11.12.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 11.12.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 12.12.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 12.12.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 12.12.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 12.12.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 12.12.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 12.12.23
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 12.12.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 12.12.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 12.12.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 12.12.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1603,38 +1603,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 11.12.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 12.12.23</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 11.12.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 11.12.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 11.12.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 11.12.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 11.12.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 11.12.23
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 11.12.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 11.12.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 11.12.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 11.12.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 11.12.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 11.12.23
-DEL.N1LKT6.MT.??????.G : last exported on 11.12.23
-DEL.N1LKT6.MT.??????.U : last exported on 11.12.23
-DEL.N1LKT6.MT.??????.AS : last exported on 11.12.23
-DVL.N1LN5X.VLM.DSP : last exported on 11.12.23
-DVL.N1LN5X.VLM.WT : last exported on 11.12.23
-DDS.N1LR11.DSP : last exported on 11.12.23
-DDS.N1LR11.WT : last exported on 11.12.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 11.12.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 11.12.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 11.12.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 11.12.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 11.12.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 11.12.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 11.12.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 11.12.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 12.12.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 12.12.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 12.12.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 12.12.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 12.12.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 12.12.23
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 12.12.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 12.12.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 12.12.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 12.12.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 12.12.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 12.12.23
+DEL.N1LKT6.MT.??????.G : last exported on 12.12.23
+DEL.N1LKT6.MT.??????.U : last exported on 12.12.23
+DEL.N1LKT6.MT.??????.AS : last exported on 12.12.23
+DVL.N1LN5X.VLM.DSP : last exported on 12.12.23
+DVL.N1LN5X.VLM.WT : last exported on 12.12.23
+DDS.N1LR11.DSP : last exported on 12.12.23
+DDS.N1LR11.WT : last exported on 12.12.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 12.12.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 12.12.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 12.12.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 12.12.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 12.12.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 12.12.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 12.12.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 12.12.23</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,55 +1662,55 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 12.12.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 12.12.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 12.12.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 12.12.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 12.12.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 12.12.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 12.12.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 12.12.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 13.12.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 13.12.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 13.12.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 13.12.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 13.12.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 13.12.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 13.12.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 13.12.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 10.12.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 11.12.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 12.12.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 10.12.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 10.12.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 11.12.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 11.12.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 11.12.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 11.12.23
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 12.12.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 12.12.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 12.12.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 12.12.23
 DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 11.12.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 11.12.23
-DEL.N1LKT6.EC.??????.G : last exported on 11.12.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 11.12.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 11.12.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 11.12.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 11.12.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 12.12.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 12.12.23
+DEL.N1LKT6.EC.??????.G : last exported on 12.12.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 12.12.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 12.12.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 12.12.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 12.12.23
 DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 11.12.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 11.12.23
-DEL.N1LKT6.EC.??????.U : last exported on 11.12.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 11.12.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 11.12.23
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 11.12.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 11.12.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 11.12.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 12.12.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 12.12.23
+DEL.N1LKT6.EC.??????.U : last exported on 12.12.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 12.12.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 12.12.23
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 12.12.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 12.12.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 12.12.23
 DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 11.12.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 11.12.23
-DEL.N1LKT6.EC.??????.AS : last exported on 11.12.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 11.12.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 11.12.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 11.12.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 11.12.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 11.12.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 11.12.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 11.12.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 11.12.23</t>
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 12.12.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 12.12.23
+DEL.N1LKT6.EC.??????.AS : last exported on 12.12.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 12.12.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 12.12.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 12.12.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 12.12.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 12.12.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 12.12.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 12.12.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 12.12.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 14.12.23 12:19
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="25" t="inlineStr">
         <is>
-          <t>Date - 13.12.2023</t>
+          <t>Date - 14.12.2023</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 12.12.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 13.12.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 13.12.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 13.12.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 13.12.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 13.12.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 13.12.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 13.12.23
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 13.12.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 13.12.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 13.12.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 13.12.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 13.12.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 14.12.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 14.12.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 14.12.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 14.12.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 14.12.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 14.12.23
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 14.12.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 14.12.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 14.12.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 14.12.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 14.12.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1109,29 +1109,29 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 12.12.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 12.12.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 12.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 12.12.23
-DIT.E35KT6.WI.ZIP : last exported on 12.12.23
-DEL.K2PKT6.WI.ZIP : last exported on 12.12.23
-DEL.R7AKT6.WI.ZIP : last exported on 13.12.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 13.12.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 13.12.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 13.12.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 13.12.23
+DIT.E35KT6.WI.ZIP : last exported on 13.12.23
+DEL.K2PKT6.WI.ZIP : last exported on 13.12.23
+DEL.R7AKT6.WI.ZIP : last exported on 14.12.23
 DEL.N5FKT6.WI.ZIP : last exported on 08.12.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 12.12.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 12.12.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 12.12.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 12.12.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 12.12.23
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 12.12.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 12.12.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 12.12.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 12.12.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 12.12.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 12.12.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 13.12.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 13.12.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 13.12.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 13.12.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 13.12.23
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 13.12.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 13.12.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 13.12.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 13.12.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 13.12.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 13.12.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 13.12.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 14.12.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 11.12.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 12.12.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 12.12.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 12.12.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 12.12.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 12.12.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 12.12.23
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 12.12.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 12.12.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 12.12.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 12.12.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 12.12.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 12.12.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 12.12.23
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 12.12.23
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 12.12.23
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 12.12.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 12.12.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 13.12.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 13.12.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 13.12.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 13.12.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 13.12.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 13.12.23
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 13.12.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 13.12.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 13.12.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 13.12.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 13.12.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 13.12.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 13.12.23
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 13.12.23
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 13.12.23
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 13.12.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 13.12.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 12.12.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 13.12.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1324,12 +1324,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 12.12.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 13.12.23</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 12.12.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 13.12.23</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1359,7 +1359,7 @@
         <is>
           <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 05.12.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
-DLV.I5XKT6.AU.A.ZIP : last exported on 11.12.23
+DLV.I5XKT6.AU.A.ZIP : last exported on 13.12.23
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
         </is>
       </c>
@@ -1367,7 +1367,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 09.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 09.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 12.12.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 13.12.23
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 09.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 09.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 09.12.23
@@ -1409,25 +1409,25 @@
 DGQ.R11KT6.BSITX.TXT : last exported on 06.12.23
 DGQ.R31KT6.BSIVMC.TXT : last exported on 12.12.23
 DGQ.R31KT6.PKATC.TXT : last exported on 12.12.23
-DEL.KMPKT6.APOS.DATA.ZIP : last exported on 06.12.23</t>
+DEL.KMPKT6.APOS.DATA.ZIP : last exported on 13.12.23</t>
         </is>
       </c>
       <c r="D14" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 06.12.23
-DEL.N1LN3L.AP.F.GPL.DMP : last exported on 06.12.23
-DEL.N1LN3L.AP.F.GTR.DMP : last exported on 06.12.23
-DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 06.12.23
-DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 06.12.23
-DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 06.12.23
-DEL.N1LN0R.AP.F.CPD.DMP : last exported on 06.12.23
-DEL.N1LN0R.AP.F.CPL.DMP : last exported on 06.12.23
-DEL.N1LR31.AP.F.PPS.DMP : last exported on 06.12.23
-DEL.KT6E35.AP.F.DB.ZIP : last exported on 06.12.23
-DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 06.12.23
-DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 06.12.23
-DVL.KT6N5X.VLM.AP.ZIP : last exported on 06.12.23
-DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 06.12.23</t>
+          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 13.12.23
+DEL.N1LN3L.AP.F.GPL.DMP : last exported on 13.12.23
+DEL.N1LN3L.AP.F.GTR.DMP : last exported on 13.12.23
+DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 13.12.23
+DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 13.12.23
+DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 13.12.23
+DEL.N1LN0R.AP.F.CPD.DMP : last exported on 13.12.23
+DEL.N1LN0R.AP.F.CPL.DMP : last exported on 13.12.23
+DEL.N1LR31.AP.F.PPS.DMP : last exported on 13.12.23
+DEL.KT6E35.AP.F.DB.ZIP : last exported on 13.12.23
+DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 13.12.23
+DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 13.12.23
+DVL.KT6N5X.VLM.AP.ZIP : last exported on 13.12.23
+DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 13.12.23</t>
         </is>
       </c>
       <c r="E14" s="11" t="inlineStr">
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 12.12.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 12.12.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 13.12.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 13.12.23</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 12.12.23
-DHP.KUDKT6.ORGUNITS : last exported on 13.12.23
-DHS.R11KT6.HSB02ALL : last exported on 12.12.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 13.12.23
+DHP.KUDKT6.ORGUNITS : last exported on 14.12.23
+DHS.R11KT6.HSB02ALL : last exported on 13.12.23</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 12.12.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 12.12.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 12.12.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 12.12.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 12.12.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 12.12.23
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 12.12.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 12.12.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 12.12.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 12.12.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 13.12.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 13.12.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 13.12.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 13.12.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 13.12.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 13.12.23
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 13.12.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 13.12.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 13.12.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 13.12.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1603,38 +1603,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 12.12.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 13.12.23</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 12.12.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 12.12.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 12.12.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 12.12.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 12.12.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 12.12.23
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 12.12.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 12.12.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 12.12.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 12.12.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 12.12.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 12.12.23
-DEL.N1LKT6.MT.??????.G : last exported on 12.12.23
-DEL.N1LKT6.MT.??????.U : last exported on 12.12.23
-DEL.N1LKT6.MT.??????.AS : last exported on 12.12.23
-DVL.N1LN5X.VLM.DSP : last exported on 12.12.23
-DVL.N1LN5X.VLM.WT : last exported on 12.12.23
-DDS.N1LR11.DSP : last exported on 12.12.23
-DDS.N1LR11.WT : last exported on 12.12.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 12.12.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 12.12.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 12.12.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 12.12.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 12.12.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 12.12.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 12.12.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 12.12.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 13.12.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 13.12.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 13.12.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 13.12.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 13.12.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 13.12.23
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 13.12.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 13.12.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 13.12.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 13.12.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 13.12.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 13.12.23
+DEL.N1LKT6.MT.??????.G : last exported on 13.12.23
+DEL.N1LKT6.MT.??????.U : last exported on 13.12.23
+DEL.N1LKT6.MT.??????.AS : last exported on 13.12.23
+DVL.N1LN5X.VLM.DSP : last exported on 13.12.23
+DVL.N1LN5X.VLM.WT : last exported on 13.12.23
+DDS.N1LR11.DSP : last exported on 13.12.23
+DDS.N1LR11.WT : last exported on 13.12.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 13.12.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 13.12.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 13.12.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 13.12.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 13.12.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 13.12.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 13.12.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 13.12.23</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,55 +1662,52 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 13.12.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 13.12.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 13.12.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 13.12.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 13.12.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 13.12.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 13.12.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 13.12.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 14.12.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 14.12.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 14.12.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 14.12.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 14.12.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 14.12.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 14.12.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 14.12.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 10.12.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 12.12.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 13.12.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 10.12.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 10.12.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 12.12.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 12.12.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 12.12.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 12.12.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 12.12.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 12.12.23
-DEL.N1LKT6.EC.??????.G : last exported on 12.12.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 12.12.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 12.12.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 12.12.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 12.12.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 12.12.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 12.12.23
-DEL.N1LKT6.EC.??????.U : last exported on 12.12.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 12.12.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 12.12.23
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 12.12.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 12.12.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 12.12.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 12.12.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 12.12.23
-DEL.N1LKT6.EC.??????.AS : last exported on 12.12.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 12.12.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 12.12.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 12.12.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 12.12.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 12.12.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 12.12.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 12.12.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 12.12.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 13.12.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 13.12.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 13.12.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 13.12.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 13.12.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 13.12.23
+DEL.N1LKT6.EC.??????.G : last exported on 13.12.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 13.12.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 13.12.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 13.12.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 13.12.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 13.12.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 13.12.23
+DEL.N1LKT6.EC.??????.U : last exported on 13.12.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 13.12.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 13.12.23
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 13.12.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 13.12.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 13.12.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 13.12.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 13.12.23
+DEL.N1LKT6.EC.??????.AS : last exported on 13.12.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 13.12.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 13.12.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 13.12.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 13.12.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 13.12.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 13.12.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 13.12.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 13.12.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 15.12.23 12:06
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="25" t="inlineStr">
         <is>
-          <t>Date - 14.12.2023</t>
+          <t>Date - 15.12.2023</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 13.12.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 14.12.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 14.12.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 14.12.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 14.12.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 14.12.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 14.12.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 14.12.23
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 14.12.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 14.12.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 14.12.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 14.12.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 14.12.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 15.12.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 15.12.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 15.12.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 15.12.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 15.12.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 15.12.23
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 15.12.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 15.12.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 15.12.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 15.12.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 15.12.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1109,29 +1109,29 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 13.12.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 13.12.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 14.12.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 14.12.23
 DLV.RPKKT6.WI.S.ZIP : last exported on 13.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 13.12.23
-DIT.E35KT6.WI.ZIP : last exported on 13.12.23
-DEL.K2PKT6.WI.ZIP : last exported on 13.12.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 14.12.23
+DIT.E35KT6.WI.ZIP : last exported on 14.12.23
+DEL.K2PKT6.WI.ZIP : last exported on 14.12.23
 DEL.R7AKT6.WI.ZIP : last exported on 14.12.23
 DEL.N5FKT6.WI.ZIP : last exported on 08.12.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 13.12.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 13.12.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 13.12.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 13.12.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 13.12.23
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 13.12.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 13.12.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 13.12.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 13.12.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 13.12.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 13.12.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 14.12.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 14.12.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 14.12.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 14.12.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 14.12.23
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 14.12.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 14.12.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 14.12.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 14.12.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 14.12.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 14.12.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 14.12.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 15.12.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 11.12.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 13.12.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 13.12.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 13.12.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 13.12.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 13.12.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 13.12.23
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 13.12.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 13.12.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 13.12.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 13.12.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 13.12.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 13.12.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 13.12.23
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 13.12.23
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 13.12.23
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 13.12.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 13.12.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 14.12.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 14.12.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 14.12.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 14.12.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 14.12.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 14.12.23
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 14.12.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 14.12.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 14.12.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 14.12.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 14.12.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 14.12.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 14.12.23
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 14.12.23
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 14.12.23
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 14.12.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 14.12.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1283,55 +1283,47 @@
 Daily</t>
         </is>
       </c>
-      <c r="C11" s="10" t="inlineStr">
+      <c r="C11" s="10" t="inlineStr"/>
+      <c r="D11" s="10" t="inlineStr"/>
+      <c r="E11" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F11" s="12" t="inlineStr">
+        <is>
+          <t>Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="31.7" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A12" s="30" t="inlineStr">
+        <is>
+          <t>TT</t>
+        </is>
+      </c>
+      <c r="B12" s="9" t="inlineStr">
+        <is>
+          <t>17:30
+Daily</t>
+        </is>
+      </c>
+      <c r="C12" s="15" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.MANDANTN.TXT : last exported on 30.11.23</t>
         </is>
       </c>
-      <c r="D11" s="10" t="inlineStr">
+      <c r="D12" s="15" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 13.12.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 14.12.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
 DGI.KT6R11.MANDANT.TXT : last exported on 30.11.23</t>
         </is>
       </c>
-      <c r="E11" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F11" s="12" t="inlineStr">
-        <is>
-          <t>Successful</t>
-        </is>
-      </c>
-    </row>
-    <row r="12" ht="31.7" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A12" s="30" t="inlineStr">
-        <is>
-          <t>TT</t>
-        </is>
-      </c>
-      <c r="B12" s="9" t="inlineStr">
-        <is>
-          <t>17:30
-Daily</t>
-        </is>
-      </c>
-      <c r="C12" s="15" t="inlineStr">
-        <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 13.12.23</t>
-        </is>
-      </c>
-      <c r="D12" s="15" t="inlineStr">
-        <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 13.12.23</t>
-        </is>
-      </c>
       <c r="E12" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
@@ -1356,6 +1348,39 @@
         </is>
       </c>
       <c r="C13" s="10" t="inlineStr">
+        <is>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 14.12.23</t>
+        </is>
+      </c>
+      <c r="D13" s="10" t="inlineStr">
+        <is>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 14.12.23</t>
+        </is>
+      </c>
+      <c r="E13" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F13" s="12" t="inlineStr">
+        <is>
+          <t>Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="182.25" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A14" s="30" t="inlineStr">
+        <is>
+          <t>APOS</t>
+        </is>
+      </c>
+      <c r="B14" s="9" t="inlineStr">
+        <is>
+          <t>18:00
+Wednesday</t>
+        </is>
+      </c>
+      <c r="C14" s="10" t="inlineStr">
         <is>
           <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 05.12.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
@@ -1363,41 +1388,41 @@
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
         </is>
       </c>
-      <c r="D13" s="10" t="inlineStr">
-        <is>
-          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 09.12.23
-DEL.N1LN3L.AU.D.GPL.DMP : last exported on 09.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 13.12.23
-DEL.N1LN0R.AU.D.CPD.DMP : last exported on 09.12.23
-DEL.N1LN0R.AU.D.CPL.DMP : last exported on 09.12.23
-DEL.KT6E35.AU.GGO.ZIP : last exported on 09.12.23
-DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 09.12.23</t>
-        </is>
-      </c>
-      <c r="E13" s="11" t="inlineStr">
+      <c r="D14" s="10" t="inlineStr">
+        <is>
+          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 14.12.23
+DEL.N1LN3L.AU.D.GPL.DMP : last exported on 14.12.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 14.12.23
+DEL.N1LN0R.AU.D.CPD.DMP : last exported on 14.12.23
+DEL.N1LN0R.AU.D.CPL.DMP : last exported on 14.12.23
+DEL.KT6E35.AU.GGO.ZIP : last exported on 14.12.23
+DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 14.12.23</t>
+        </is>
+      </c>
+      <c r="E14" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
         </is>
       </c>
-      <c r="F13" s="12" t="inlineStr">
+      <c r="F14" s="12" t="inlineStr">
         <is>
           <t>Successful</t>
         </is>
       </c>
     </row>
-    <row r="14" ht="182.25" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A14" s="30" t="inlineStr">
-        <is>
-          <t>APOS</t>
-        </is>
-      </c>
-      <c r="B14" s="9" t="inlineStr">
-        <is>
-          <t>18:00
-Wednesday</t>
-        </is>
-      </c>
-      <c r="C14" s="10" t="inlineStr">
+    <row r="15" ht="37.5" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A15" s="30" t="inlineStr">
+        <is>
+          <t>COK</t>
+        </is>
+      </c>
+      <c r="B15" s="9" t="inlineStr">
+        <is>
+          <t>18:05
+Daily</t>
+        </is>
+      </c>
+      <c r="C15" s="16" t="inlineStr">
         <is>
           <t>DGQ.R11KT6.BSIVM.TXT : last exported on 06.12.23
 DGQ.R11KT6.BSIVM.C.TXT : last exported on 06.12.23
@@ -1412,7 +1437,7 @@
 DEL.KMPKT6.APOS.DATA.ZIP : last exported on 13.12.23</t>
         </is>
       </c>
-      <c r="D14" s="10" t="inlineStr">
+      <c r="D15" s="16" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 13.12.23
 DEL.N1LN3L.AP.F.GPL.DMP : last exported on 13.12.23
@@ -1430,40 +1455,6 @@
 DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 13.12.23</t>
         </is>
       </c>
-      <c r="E14" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F14" s="12" t="inlineStr">
-        <is>
-          <t>Successful</t>
-        </is>
-      </c>
-    </row>
-    <row r="15" ht="37.5" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A15" s="30" t="inlineStr">
-        <is>
-          <t>COK</t>
-        </is>
-      </c>
-      <c r="B15" s="9" t="inlineStr">
-        <is>
-          <t>18:05
-Daily</t>
-        </is>
-      </c>
-      <c r="C15" s="16" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="D15" s="16" t="inlineStr">
-        <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 13.12.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 13.12.23</t>
-        </is>
-      </c>
       <c r="E15" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
@@ -1489,23 +1480,13 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 13.12.23
-DHP.KUDKT6.ORGUNITS : last exported on 14.12.23
-DHS.R11KT6.HSB02ALL : last exported on 13.12.23</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 13.12.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 13.12.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 13.12.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 13.12.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 13.12.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 13.12.23
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 13.12.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 13.12.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 13.12.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 13.12.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 14.12.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 14.12.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1533,10 +1514,54 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 14.12.23
+DHP.KUDKT6.ORGUNITS : last exported on 15.12.23
+DHS.R11KT6.HSB02ALL : last exported on 14.12.23</t>
+        </is>
+      </c>
+      <c r="D17" s="10" t="inlineStr">
+        <is>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 14.12.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 14.12.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 14.12.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 14.12.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 14.12.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 14.12.23
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 14.12.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 14.12.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 14.12.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 14.12.23</t>
+        </is>
+      </c>
+      <c r="E17" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F17" s="13" t="inlineStr">
+        <is>
+          <t>DryRun</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="36.75" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A18" s="30" t="inlineStr">
+        <is>
+          <t>Translations</t>
+        </is>
+      </c>
+      <c r="B18" s="9" t="inlineStr">
+        <is>
+          <t>19:00
+Sunday</t>
+        </is>
+      </c>
+      <c r="C18" s="15" t="inlineStr">
+        <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="D17" s="10" t="inlineStr">
+      <c r="D18" s="15" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.EUTRM.F.GPD.DMP : last exported on 20.05.22
 DEL.N1LN3L.EUTRM.F.GPL.DMP : last exported on 20.05.22
@@ -1545,39 +1570,6 @@
 DEL.N1LN3L.EUTRM.F.CPL.DMP : last exported on 20.05.22</t>
         </is>
       </c>
-      <c r="E17" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F17" s="13" t="inlineStr">
-        <is>
-          <t>DryRun</t>
-        </is>
-      </c>
-    </row>
-    <row r="18" ht="36.75" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A18" s="30" t="inlineStr">
-        <is>
-          <t>Translations</t>
-        </is>
-      </c>
-      <c r="B18" s="9" t="inlineStr">
-        <is>
-          <t>19:00
-Sunday</t>
-        </is>
-      </c>
-      <c r="C18" s="15" t="inlineStr">
-        <is>
-          <t>DIT.E35KT6.TRANS.ZIP : last exported on 09.01.23</t>
-        </is>
-      </c>
-      <c r="D18" s="15" t="inlineStr">
-        <is>
-          <t>DEL.N1LE35.TRANS.ZIP : last exported on 10.12.23</t>
-        </is>
-      </c>
       <c r="E18" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
@@ -1603,38 +1595,12 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 13.12.23</t>
+          <t>DIT.E35KT6.TRANS.ZIP : last exported on 09.01.23</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 13.12.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 13.12.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 13.12.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 13.12.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 13.12.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 13.12.23
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 13.12.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 13.12.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 13.12.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 13.12.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 13.12.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 13.12.23
-DEL.N1LKT6.MT.??????.G : last exported on 13.12.23
-DEL.N1LKT6.MT.??????.U : last exported on 13.12.23
-DEL.N1LKT6.MT.??????.AS : last exported on 13.12.23
-DVL.N1LN5X.VLM.DSP : last exported on 13.12.23
-DVL.N1LN5X.VLM.WT : last exported on 13.12.23
-DDS.N1LR11.DSP : last exported on 13.12.23
-DDS.N1LR11.WT : last exported on 13.12.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 13.12.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 13.12.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 13.12.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 13.12.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 13.12.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 13.12.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 13.12.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 13.12.23</t>
+          <t>DEL.N1LE35.TRANS.ZIP : last exported on 10.12.23</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,52 +1628,38 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 14.12.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 14.12.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 14.12.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 14.12.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 14.12.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 14.12.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 14.12.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 14.12.23
-DDC.R11KT6.ELFI.MD.TXT : last exported on 10.12.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 13.12.23
-DDC.R11KT6.ELFI.PK.TXT : last exported on 10.12.23
-DDC.R11KT6.ELFI.PR.TXT : last exported on 10.12.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 14.12.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 13.12.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 13.12.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 13.12.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 13.12.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 13.12.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 13.12.23
-DEL.N1LKT6.EC.??????.G : last exported on 13.12.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 13.12.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 13.12.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 13.12.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 13.12.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 13.12.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 13.12.23
-DEL.N1LKT6.EC.??????.U : last exported on 13.12.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 13.12.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 13.12.23
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 13.12.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 13.12.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 13.12.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 13.12.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 13.12.23
-DEL.N1LKT6.EC.??????.AS : last exported on 13.12.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 13.12.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 13.12.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 13.12.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 13.12.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 13.12.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 13.12.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 13.12.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 13.12.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 14.12.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 14.12.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 14.12.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 14.12.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 14.12.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 14.12.23
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 14.12.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 14.12.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 14.12.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 14.12.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 14.12.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 14.12.23
+DEL.N1LKT6.MT.??????.G : last exported on 14.12.23
+DEL.N1LKT6.MT.??????.U : last exported on 14.12.23
+DEL.N1LKT6.MT.??????.AS : last exported on 14.12.23
+DVL.N1LN5X.VLM.DSP : last exported on 14.12.23
+DVL.N1LN5X.VLM.WT : last exported on 14.12.23
+DDS.N1LR11.DSP : last exported on 14.12.23
+DDS.N1LR11.WT : last exported on 14.12.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 14.12.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 14.12.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 14.12.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 14.12.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 14.12.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 14.12.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 14.12.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 14.12.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1724,12 +1676,7 @@
     <row r="21" ht="16.5" customHeight="1" thickBot="1" thickTop="1">
       <c r="A21" s="5" t="n"/>
       <c r="B21" s="6" t="n"/>
-      <c r="C21" s="4" t="inlineStr">
-        <is>
-          <t>DHP.KUDKT6.EXEMN.ZIP : last exported on 11.12.23
-DHP.KUDKT6.DPO.EMAILS : last exported on 11.12.23</t>
-        </is>
-      </c>
+      <c r="C21" s="4" t="inlineStr"/>
       <c r="D21" s="4" t="inlineStr"/>
       <c r="E21" s="2" t="n"/>
       <c r="F21" s="3" t="n"/>
@@ -1743,54 +1690,52 @@
       <c r="B22" s="27" t="n"/>
       <c r="C22" s="14" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 11.12.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 11.12.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 11.12.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 11.12.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 11.12.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 11.12.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 11.12.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 11.12.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 15.12.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 15.12.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 15.12.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 15.12.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 15.12.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 15.12.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 15.12.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 15.12.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 10.12.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 08.12.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 14.12.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 10.12.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 10.12.23</t>
         </is>
       </c>
       <c r="D22" s="5" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 10.12.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 10.12.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 10.12.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 10.12.23
-DEL.N1LKTZ.EL.F.GGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 10.12.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 10.12.23
-DEL.N1LKT6.EC.??????.G : last exported on 10.12.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 10.12.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 10.12.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 10.12.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 10.12.23
-DEL.N1LKTZ.EL.F.UGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 10.12.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 10.12.23
-DEL.N1LKT6.EC.??????.U : last exported on 10.12.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 10.12.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 10.12.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 10.12.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 10.12.23
-DEL.N1LKTZ.EL.F.ASGO.ZIP : last exported on 28.11.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 10.12.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 10.12.23
-DEL.N1LKT6.EC.??????.AS : last exported on 10.12.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 10.12.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 10.12.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 10.12.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 10.12.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 10.12.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 10.12.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 10.12.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 10.12.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 14.12.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 14.12.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 14.12.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 14.12.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 14.12.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 14.12.23
+DEL.N1LKT6.EC.??????.G : last exported on 14.12.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 14.12.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 14.12.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 14.12.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 14.12.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 14.12.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 14.12.23
+DEL.N1LKT6.EC.??????.U : last exported on 14.12.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 14.12.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 14.12.23
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 14.12.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 14.12.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 14.12.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 14.12.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 14.12.23
+DEL.N1LKT6.EC.??????.AS : last exported on 14.12.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 14.12.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 14.12.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 14.12.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 14.12.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 14.12.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 14.12.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 14.12.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 14.12.23</t>
         </is>
       </c>
       <c r="F22" s="3" t="n"/>

</xml_diff>

<commit_message>
Updated on 15.12.23 13:26
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -1283,37 +1283,12 @@
 Daily</t>
         </is>
       </c>
-      <c r="C11" s="10" t="inlineStr"/>
-      <c r="D11" s="10" t="inlineStr"/>
-      <c r="E11" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F11" s="12" t="inlineStr">
-        <is>
-          <t>Successful</t>
-        </is>
-      </c>
-    </row>
-    <row r="12" ht="31.7" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A12" s="30" t="inlineStr">
-        <is>
-          <t>TT</t>
-        </is>
-      </c>
-      <c r="B12" s="9" t="inlineStr">
-        <is>
-          <t>17:30
-Daily</t>
-        </is>
-      </c>
-      <c r="C12" s="15" t="inlineStr">
+      <c r="C11" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.MANDANTN.TXT : last exported on 30.11.23</t>
         </is>
       </c>
-      <c r="D12" s="15" t="inlineStr">
+      <c r="D11" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
@@ -1324,6 +1299,39 @@
 DGI.KT6R11.MANDANT.TXT : last exported on 30.11.23</t>
         </is>
       </c>
+      <c r="E11" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F11" s="12" t="inlineStr">
+        <is>
+          <t>Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="31.7" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A12" s="30" t="inlineStr">
+        <is>
+          <t>TT</t>
+        </is>
+      </c>
+      <c r="B12" s="9" t="inlineStr">
+        <is>
+          <t>17:30
+Daily</t>
+        </is>
+      </c>
+      <c r="C12" s="15" t="inlineStr">
+        <is>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 14.12.23</t>
+        </is>
+      </c>
+      <c r="D12" s="15" t="inlineStr">
+        <is>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 14.12.23</t>
+        </is>
+      </c>
       <c r="E12" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
@@ -1348,39 +1356,6 @@
         </is>
       </c>
       <c r="C13" s="10" t="inlineStr">
-        <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 14.12.23</t>
-        </is>
-      </c>
-      <c r="D13" s="10" t="inlineStr">
-        <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 14.12.23</t>
-        </is>
-      </c>
-      <c r="E13" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F13" s="12" t="inlineStr">
-        <is>
-          <t>Successful</t>
-        </is>
-      </c>
-    </row>
-    <row r="14" ht="182.25" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A14" s="30" t="inlineStr">
-        <is>
-          <t>APOS</t>
-        </is>
-      </c>
-      <c r="B14" s="9" t="inlineStr">
-        <is>
-          <t>18:00
-Wednesday</t>
-        </is>
-      </c>
-      <c r="C14" s="10" t="inlineStr">
         <is>
           <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 05.12.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
@@ -1388,7 +1363,7 @@
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
         </is>
       </c>
-      <c r="D14" s="10" t="inlineStr">
+      <c r="D13" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 14.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 14.12.23
@@ -1399,30 +1374,30 @@
 DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 14.12.23</t>
         </is>
       </c>
-      <c r="E14" s="11" t="inlineStr">
+      <c r="E13" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
         </is>
       </c>
-      <c r="F14" s="12" t="inlineStr">
+      <c r="F13" s="12" t="inlineStr">
         <is>
           <t>Successful</t>
         </is>
       </c>
     </row>
-    <row r="15" ht="37.5" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A15" s="30" t="inlineStr">
-        <is>
-          <t>COK</t>
-        </is>
-      </c>
-      <c r="B15" s="9" t="inlineStr">
-        <is>
-          <t>18:05
-Daily</t>
-        </is>
-      </c>
-      <c r="C15" s="16" t="inlineStr">
+    <row r="14" ht="182.25" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A14" s="30" t="inlineStr">
+        <is>
+          <t>APOS</t>
+        </is>
+      </c>
+      <c r="B14" s="9" t="inlineStr">
+        <is>
+          <t>18:00
+Wednesday</t>
+        </is>
+      </c>
+      <c r="C14" s="10" t="inlineStr">
         <is>
           <t>DGQ.R11KT6.BSIVM.TXT : last exported on 06.12.23
 DGQ.R11KT6.BSIVM.C.TXT : last exported on 06.12.23
@@ -1437,7 +1412,7 @@
 DEL.KMPKT6.APOS.DATA.ZIP : last exported on 13.12.23</t>
         </is>
       </c>
-      <c r="D15" s="16" t="inlineStr">
+      <c r="D14" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 13.12.23
 DEL.N1LN3L.AP.F.GPL.DMP : last exported on 13.12.23
@@ -1455,6 +1430,40 @@
 DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 13.12.23</t>
         </is>
       </c>
+      <c r="E14" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F14" s="12" t="inlineStr">
+        <is>
+          <t>Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="37.5" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A15" s="30" t="inlineStr">
+        <is>
+          <t>COK</t>
+        </is>
+      </c>
+      <c r="B15" s="9" t="inlineStr">
+        <is>
+          <t>18:05
+Daily</t>
+        </is>
+      </c>
+      <c r="C15" s="16" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="D15" s="16" t="inlineStr">
+        <is>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 14.12.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 14.12.23</t>
+        </is>
+      </c>
       <c r="E15" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
@@ -1479,47 +1488,13 @@
         </is>
       </c>
       <c r="C16" s="10" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="D16" s="10" t="inlineStr">
-        <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 14.12.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 14.12.23</t>
-        </is>
-      </c>
-      <c r="E16" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F16" s="12" t="inlineStr">
-        <is>
-          <t>Successful</t>
-        </is>
-      </c>
-    </row>
-    <row r="17" ht="48.2" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A17" s="30" t="inlineStr">
-        <is>
-          <t>EUTERM</t>
-        </is>
-      </c>
-      <c r="B17" s="9" t="inlineStr">
-        <is>
-          <t>18:15
-Daily</t>
-        </is>
-      </c>
-      <c r="C17" s="10" t="inlineStr">
         <is>
           <t>DHP.KUDKT6.KVPSIMPORT : last exported on 14.12.23
 DHP.KUDKT6.ORGUNITS : last exported on 15.12.23
 DHS.R11KT6.HSB02ALL : last exported on 14.12.23</t>
         </is>
       </c>
-      <c r="D17" s="10" t="inlineStr">
+      <c r="D16" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 14.12.23
 DEL.N1LN3L.DP.F.GPL.DMP : last exported on 14.12.23
@@ -1533,35 +1508,35 @@
 DEL.N1LN3L.DISSAORG.ZIP : last exported on 14.12.23</t>
         </is>
       </c>
-      <c r="E17" s="11" t="inlineStr">
+      <c r="E16" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
         </is>
       </c>
-      <c r="F17" s="13" t="inlineStr">
-        <is>
-          <t>DryRun</t>
-        </is>
-      </c>
-    </row>
-    <row r="18" ht="36.75" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A18" s="30" t="inlineStr">
-        <is>
-          <t>Translations</t>
-        </is>
-      </c>
-      <c r="B18" s="9" t="inlineStr">
-        <is>
-          <t>19:00
-Sunday</t>
-        </is>
-      </c>
-      <c r="C18" s="15" t="inlineStr">
+      <c r="F16" s="12" t="inlineStr">
+        <is>
+          <t>Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" ht="48.2" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A17" s="30" t="inlineStr">
+        <is>
+          <t>EUTERM</t>
+        </is>
+      </c>
+      <c r="B17" s="9" t="inlineStr">
+        <is>
+          <t>18:15
+Daily</t>
+        </is>
+      </c>
+      <c r="C17" s="10" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="D18" s="15" t="inlineStr">
+      <c r="D17" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.EUTRM.F.GPD.DMP : last exported on 20.05.22
 DEL.N1LN3L.EUTRM.F.GPL.DMP : last exported on 20.05.22
@@ -1570,6 +1545,39 @@
 DEL.N1LN3L.EUTRM.F.CPL.DMP : last exported on 20.05.22</t>
         </is>
       </c>
+      <c r="E17" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F17" s="13" t="inlineStr">
+        <is>
+          <t>DryRun</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="36.75" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A18" s="30" t="inlineStr">
+        <is>
+          <t>Translations</t>
+        </is>
+      </c>
+      <c r="B18" s="9" t="inlineStr">
+        <is>
+          <t>19:00
+Sunday</t>
+        </is>
+      </c>
+      <c r="C18" s="15" t="inlineStr">
+        <is>
+          <t>DIT.E35KT6.TRANS.ZIP : last exported on 09.01.23</t>
+        </is>
+      </c>
+      <c r="D18" s="15" t="inlineStr">
+        <is>
+          <t>DEL.N1LE35.TRANS.ZIP : last exported on 10.12.23</t>
+        </is>
+      </c>
       <c r="E18" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
@@ -1595,43 +1603,10 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.TRANS.ZIP : last exported on 09.01.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 14.12.23</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
-        <is>
-          <t>DEL.N1LE35.TRANS.ZIP : last exported on 10.12.23</t>
-        </is>
-      </c>
-      <c r="E19" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F19" s="12" t="inlineStr">
-        <is>
-          <t>Successful</t>
-        </is>
-      </c>
-    </row>
-    <row r="20" ht="409.6" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A20" s="30" t="inlineStr">
-        <is>
-          <t>ELFI</t>
-        </is>
-      </c>
-      <c r="B20" s="9" t="inlineStr">
-        <is>
-          <t>20:25
-Daily</t>
-        </is>
-      </c>
-      <c r="C20" s="10" t="inlineStr">
-        <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 14.12.23</t>
-        </is>
-      </c>
-      <c r="D20" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 14.12.23
 DEL.N1LN3L.MT.F.GPL.DMP : last exported on 14.12.23
@@ -1662,33 +1637,30 @@
 DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 14.12.23</t>
         </is>
       </c>
-      <c r="E20" s="11" t="inlineStr">
+      <c r="E19" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
         </is>
       </c>
-      <c r="F20" s="12" t="inlineStr">
+      <c r="F19" s="12" t="inlineStr">
         <is>
           <t>Successful</t>
         </is>
       </c>
     </row>
-    <row r="21" ht="16.5" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A21" s="5" t="n"/>
-      <c r="B21" s="6" t="n"/>
-      <c r="C21" s="4" t="inlineStr"/>
-      <c r="D21" s="4" t="inlineStr"/>
-      <c r="E21" s="2" t="n"/>
-      <c r="F21" s="3" t="n"/>
-    </row>
-    <row r="22" ht="19.5" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A22" s="30" t="inlineStr">
-        <is>
-          <t>DB server Disk Space Monitoring</t>
-        </is>
-      </c>
-      <c r="B22" s="27" t="n"/>
-      <c r="C22" s="14" t="inlineStr">
+    <row r="20" ht="409.6" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A20" s="30" t="inlineStr">
+        <is>
+          <t>ELFI</t>
+        </is>
+      </c>
+      <c r="B20" s="9" t="inlineStr">
+        <is>
+          <t>20:25
+Daily</t>
+        </is>
+      </c>
+      <c r="C20" s="10" t="inlineStr">
         <is>
           <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 15.12.23
 DKG.R11KT6.L520.P.EDCP.LEI : last exported on 15.12.23
@@ -1704,7 +1676,7 @@
 DDC.R11KT6.ELFI.PR.TXT : last exported on 10.12.23</t>
         </is>
       </c>
-      <c r="D22" s="5" t="inlineStr">
+      <c r="D20" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 14.12.23
 DEL.N1LN3L.EL.F.GPL.DMP : last exported on 14.12.23
@@ -1738,6 +1710,82 @@
 DEL.KT6N5X.EL.F.AU.ZIP : last exported on 14.12.23</t>
         </is>
       </c>
+      <c r="E20" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F20" s="12" t="inlineStr">
+        <is>
+          <t>Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="21" ht="16.5" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A21" s="5" t="n"/>
+      <c r="B21" s="6" t="n"/>
+      <c r="C21" s="4" t="inlineStr"/>
+      <c r="D21" s="4" t="inlineStr"/>
+      <c r="E21" s="2" t="n"/>
+      <c r="F21" s="3" t="n"/>
+    </row>
+    <row r="22" ht="19.5" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A22" s="30" t="inlineStr">
+        <is>
+          <t>DB server Disk Space Monitoring</t>
+        </is>
+      </c>
+      <c r="B22" s="27" t="n"/>
+      <c r="C22" s="14" t="inlineStr">
+        <is>
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 15.12.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 15.12.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 15.12.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 15.12.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 15.12.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 15.12.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 15.12.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 15.12.23
+DDC.R11KT6.ELFI.MD.TXT : last exported on 10.12.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 14.12.23
+DDC.R11KT6.ELFI.PK.TXT : last exported on 10.12.23
+DDC.R11KT6.ELFI.PR.TXT : last exported on 10.12.23</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="inlineStr">
+        <is>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 14.12.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 14.12.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 14.12.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 14.12.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 14.12.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 14.12.23
+DEL.N1LKT6.EC.??????.G : last exported on 14.12.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 14.12.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 14.12.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 14.12.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 14.12.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 14.12.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 14.12.23
+DEL.N1LKT6.EC.??????.U : last exported on 14.12.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 14.12.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 14.12.23
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 14.12.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 14.12.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 14.12.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 14.12.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 14.12.23
+DEL.N1LKT6.EC.??????.AS : last exported on 14.12.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 14.12.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 14.12.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 14.12.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 14.12.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 14.12.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 14.12.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 14.12.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 14.12.23</t>
+        </is>
+      </c>
       <c r="F22" s="3" t="n"/>
     </row>
     <row r="23" ht="15" customHeight="1" thickBot="1" thickTop="1">

</xml_diff>

<commit_message>
Updated on 18.12.23 14:27
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="25" t="inlineStr">
         <is>
-          <t>Date - 15.12.2023</t>
+          <t>Date - 18.12.2023</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 14.12.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 15.12.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 15.12.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 15.12.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 15.12.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 15.12.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 15.12.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 15.12.23
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 15.12.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 15.12.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 15.12.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 15.12.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 15.12.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 16.12.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 16.12.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 17.12.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 16.12.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 16.12.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 16.12.23
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 16.12.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 16.12.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 16.12.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 16.12.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 16.12.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1066,22 +1066,22 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 11.12.23
-DEH.N3LKT6.AP.COMPL.SNK : last exported on 11.12.23</t>
+          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 18.12.23
+DEH.N3LKT6.AP.COMPL.SNK : last exported on 18.12.23</t>
         </is>
       </c>
       <c r="D6" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 11.12.23
-DEL.N1LN3L.DN.F.GPL.DMP : last exported on 11.12.23
-DEL.N1LN3L.DN.F.GTR.DMP : last exported on 11.12.23
-DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 11.12.23
-DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 11.12.23
-DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 11.12.23
-DEL.N1LN0R.DN.F.CPD.DMP : last exported on 11.12.23
-DEL.N1LN0R.DN.F.CPL.DMP : last exported on 11.12.23
-DEL.KT6E35.SN.F.GGO.ZIP : last exported on 11.12.23
-DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 11.12.23</t>
+          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 18.12.23
+DEL.N1LN3L.DN.F.GPL.DMP : last exported on 18.12.23
+DEL.N1LN3L.DN.F.GTR.DMP : last exported on 18.12.23
+DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 18.12.23
+DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 18.12.23
+DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 18.12.23
+DEL.N1LN0R.DN.F.CPD.DMP : last exported on 18.12.23
+DEL.N1LN0R.DN.F.CPL.DMP : last exported on 18.12.23
+DEL.KT6E35.SN.F.GGO.ZIP : last exported on 18.12.23
+DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 18.12.23</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
@@ -1109,29 +1109,29 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 14.12.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 14.12.23
-DLV.RPKKT6.WI.S.ZIP : last exported on 13.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 14.12.23
-DIT.E35KT6.WI.ZIP : last exported on 14.12.23
-DEL.K2PKT6.WI.ZIP : last exported on 14.12.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 15.12.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 17.12.23
+DLV.RPKKT6.WI.S.ZIP : last exported on 15.12.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 16.12.23
+DIT.E35KT6.WI.ZIP : last exported on 15.12.23
+DEL.K2PKT6.WI.ZIP : last exported on 17.12.23
 DEL.R7AKT6.WI.ZIP : last exported on 14.12.23
 DEL.N5FKT6.WI.ZIP : last exported on 08.12.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 14.12.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 14.12.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 14.12.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 14.12.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 14.12.23
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 14.12.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 14.12.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 14.12.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 14.12.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 14.12.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 14.12.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 18.12.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 18.12.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 18.12.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 18.12.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 18.12.23
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 18.12.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 18.12.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 18.12.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 18.12.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 18.12.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 18.12.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 15.12.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 18.12.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 11.12.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 14.12.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 14.12.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 14.12.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 14.12.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 14.12.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 14.12.23
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 14.12.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 14.12.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 14.12.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 14.12.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 14.12.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 14.12.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 14.12.23
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 14.12.23
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 14.12.23
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 14.12.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 14.12.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 17.12.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 17.12.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 17.12.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 17.12.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 17.12.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 17.12.23
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 17.12.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 17.12.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 17.12.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 17.12.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 17.12.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 17.12.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 17.12.23
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 17.12.23
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 17.12.23
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 17.12.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 17.12.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1283,55 +1283,47 @@
 Daily</t>
         </is>
       </c>
-      <c r="C11" s="10" t="inlineStr">
+      <c r="C11" s="10" t="inlineStr"/>
+      <c r="D11" s="10" t="inlineStr"/>
+      <c r="E11" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F11" s="12" t="inlineStr">
+        <is>
+          <t>Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="31.7" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A12" s="30" t="inlineStr">
+        <is>
+          <t>TT</t>
+        </is>
+      </c>
+      <c r="B12" s="9" t="inlineStr">
+        <is>
+          <t>17:30
+Daily</t>
+        </is>
+      </c>
+      <c r="C12" s="15" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.MANDANTN.TXT : last exported on 30.11.23</t>
         </is>
       </c>
-      <c r="D11" s="10" t="inlineStr">
+      <c r="D12" s="15" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 14.12.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 17.12.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
 DGI.KT6R11.MANDANT.TXT : last exported on 30.11.23</t>
         </is>
       </c>
-      <c r="E11" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F11" s="12" t="inlineStr">
-        <is>
-          <t>Successful</t>
-        </is>
-      </c>
-    </row>
-    <row r="12" ht="31.7" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A12" s="30" t="inlineStr">
-        <is>
-          <t>TT</t>
-        </is>
-      </c>
-      <c r="B12" s="9" t="inlineStr">
-        <is>
-          <t>17:30
-Daily</t>
-        </is>
-      </c>
-      <c r="C12" s="15" t="inlineStr">
-        <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 14.12.23</t>
-        </is>
-      </c>
-      <c r="D12" s="15" t="inlineStr">
-        <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 14.12.23</t>
-        </is>
-      </c>
       <c r="E12" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
@@ -1356,6 +1348,39 @@
         </is>
       </c>
       <c r="C13" s="10" t="inlineStr">
+        <is>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 15.12.23</t>
+        </is>
+      </c>
+      <c r="D13" s="10" t="inlineStr">
+        <is>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 16.12.23</t>
+        </is>
+      </c>
+      <c r="E13" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F13" s="12" t="inlineStr">
+        <is>
+          <t>Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="182.25" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A14" s="30" t="inlineStr">
+        <is>
+          <t>APOS</t>
+        </is>
+      </c>
+      <c r="B14" s="9" t="inlineStr">
+        <is>
+          <t>18:00
+Wednesday</t>
+        </is>
+      </c>
+      <c r="C14" s="10" t="inlineStr">
         <is>
           <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 05.12.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
@@ -1363,41 +1388,41 @@
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
         </is>
       </c>
-      <c r="D13" s="10" t="inlineStr">
+      <c r="D14" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 14.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 14.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 14.12.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 17.12.23
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 14.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 14.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 14.12.23
 DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 14.12.23</t>
         </is>
       </c>
-      <c r="E13" s="11" t="inlineStr">
+      <c r="E14" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
         </is>
       </c>
-      <c r="F13" s="12" t="inlineStr">
+      <c r="F14" s="12" t="inlineStr">
         <is>
           <t>Successful</t>
         </is>
       </c>
     </row>
-    <row r="14" ht="182.25" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A14" s="30" t="inlineStr">
-        <is>
-          <t>APOS</t>
-        </is>
-      </c>
-      <c r="B14" s="9" t="inlineStr">
-        <is>
-          <t>18:00
-Wednesday</t>
-        </is>
-      </c>
-      <c r="C14" s="10" t="inlineStr">
+    <row r="15" ht="37.5" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A15" s="30" t="inlineStr">
+        <is>
+          <t>COK</t>
+        </is>
+      </c>
+      <c r="B15" s="9" t="inlineStr">
+        <is>
+          <t>18:05
+Daily</t>
+        </is>
+      </c>
+      <c r="C15" s="16" t="inlineStr">
         <is>
           <t>DGQ.R11KT6.BSIVM.TXT : last exported on 06.12.23
 DGQ.R11KT6.BSIVM.C.TXT : last exported on 06.12.23
@@ -1412,7 +1437,7 @@
 DEL.KMPKT6.APOS.DATA.ZIP : last exported on 13.12.23</t>
         </is>
       </c>
-      <c r="D14" s="10" t="inlineStr">
+      <c r="D15" s="16" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 13.12.23
 DEL.N1LN3L.AP.F.GPL.DMP : last exported on 13.12.23
@@ -1430,40 +1455,6 @@
 DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 13.12.23</t>
         </is>
       </c>
-      <c r="E14" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F14" s="12" t="inlineStr">
-        <is>
-          <t>Successful</t>
-        </is>
-      </c>
-    </row>
-    <row r="15" ht="37.5" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A15" s="30" t="inlineStr">
-        <is>
-          <t>COK</t>
-        </is>
-      </c>
-      <c r="B15" s="9" t="inlineStr">
-        <is>
-          <t>18:05
-Daily</t>
-        </is>
-      </c>
-      <c r="C15" s="16" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="D15" s="16" t="inlineStr">
-        <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 14.12.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 14.12.23</t>
-        </is>
-      </c>
       <c r="E15" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
@@ -1489,23 +1480,13 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 14.12.23
-DHP.KUDKT6.ORGUNITS : last exported on 15.12.23
-DHS.R11KT6.HSB02ALL : last exported on 14.12.23</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 14.12.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 14.12.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 14.12.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 14.12.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 14.12.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 14.12.23
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 14.12.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 14.12.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 14.12.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 14.12.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 17.12.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 17.12.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1533,10 +1514,54 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 17.12.23
+DHP.KUDKT6.ORGUNITS : last exported on 18.12.23
+DHS.R11KT6.HSB02ALL : last exported on 15.12.23</t>
+        </is>
+      </c>
+      <c r="D17" s="10" t="inlineStr">
+        <is>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 15.12.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 15.12.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 17.12.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 15.12.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 15.12.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 15.12.23
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 15.12.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 15.12.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 15.12.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 15.12.23</t>
+        </is>
+      </c>
+      <c r="E17" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F17" s="13" t="inlineStr">
+        <is>
+          <t>DryRun</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="36.75" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A18" s="30" t="inlineStr">
+        <is>
+          <t>Translations</t>
+        </is>
+      </c>
+      <c r="B18" s="9" t="inlineStr">
+        <is>
+          <t>19:00
+Sunday</t>
+        </is>
+      </c>
+      <c r="C18" s="15" t="inlineStr">
+        <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="D17" s="10" t="inlineStr">
+      <c r="D18" s="15" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.EUTRM.F.GPD.DMP : last exported on 20.05.22
 DEL.N1LN3L.EUTRM.F.GPL.DMP : last exported on 20.05.22
@@ -1545,39 +1570,6 @@
 DEL.N1LN3L.EUTRM.F.CPL.DMP : last exported on 20.05.22</t>
         </is>
       </c>
-      <c r="E17" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F17" s="13" t="inlineStr">
-        <is>
-          <t>DryRun</t>
-        </is>
-      </c>
-    </row>
-    <row r="18" ht="36.75" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A18" s="30" t="inlineStr">
-        <is>
-          <t>Translations</t>
-        </is>
-      </c>
-      <c r="B18" s="9" t="inlineStr">
-        <is>
-          <t>19:00
-Sunday</t>
-        </is>
-      </c>
-      <c r="C18" s="15" t="inlineStr">
-        <is>
-          <t>DIT.E35KT6.TRANS.ZIP : last exported on 09.01.23</t>
-        </is>
-      </c>
-      <c r="D18" s="15" t="inlineStr">
-        <is>
-          <t>DEL.N1LE35.TRANS.ZIP : last exported on 10.12.23</t>
-        </is>
-      </c>
       <c r="E18" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
@@ -1603,38 +1595,12 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 14.12.23</t>
+          <t>DIT.E35KT6.TRANS.ZIP : last exported on 09.01.23</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 14.12.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 14.12.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 14.12.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 14.12.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 14.12.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 14.12.23
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 14.12.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 14.12.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 14.12.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 14.12.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 14.12.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 14.12.23
-DEL.N1LKT6.MT.??????.G : last exported on 14.12.23
-DEL.N1LKT6.MT.??????.U : last exported on 14.12.23
-DEL.N1LKT6.MT.??????.AS : last exported on 14.12.23
-DVL.N1LN5X.VLM.DSP : last exported on 14.12.23
-DVL.N1LN5X.VLM.WT : last exported on 14.12.23
-DDS.N1LR11.DSP : last exported on 14.12.23
-DDS.N1LR11.WT : last exported on 14.12.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 14.12.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 14.12.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 14.12.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 14.12.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 14.12.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 14.12.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 14.12.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 14.12.23</t>
+          <t>DEL.N1LE35.TRANS.ZIP : last exported on 17.12.23</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,52 +1628,38 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 15.12.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 15.12.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 15.12.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 15.12.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 15.12.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 15.12.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 15.12.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 15.12.23
-DDC.R11KT6.ELFI.MD.TXT : last exported on 10.12.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 14.12.23
-DDC.R11KT6.ELFI.PK.TXT : last exported on 10.12.23
-DDC.R11KT6.ELFI.PR.TXT : last exported on 10.12.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 16.12.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 14.12.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 14.12.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 14.12.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 14.12.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 14.12.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 14.12.23
-DEL.N1LKT6.EC.??????.G : last exported on 14.12.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 14.12.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 14.12.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 14.12.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 14.12.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 14.12.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 14.12.23
-DEL.N1LKT6.EC.??????.U : last exported on 14.12.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 14.12.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 14.12.23
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 14.12.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 14.12.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 14.12.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 14.12.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 14.12.23
-DEL.N1LKT6.EC.??????.AS : last exported on 14.12.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 14.12.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 14.12.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 14.12.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 14.12.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 14.12.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 14.12.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 14.12.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 14.12.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 16.12.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 16.12.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 17.12.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 16.12.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 16.12.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 16.12.23
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 16.12.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 16.12.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 16.12.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 16.12.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 16.12.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 16.12.23
+DEL.N1LKT6.MT.??????.G : last exported on 16.12.23
+DEL.N1LKT6.MT.??????.U : last exported on 16.12.23
+DEL.N1LKT6.MT.??????.AS : last exported on 16.12.23
+DVL.N1LN5X.VLM.DSP : last exported on 16.12.23
+DVL.N1LN5X.VLM.WT : last exported on 16.12.23
+DDS.N1LR11.DSP : last exported on 16.12.23
+DDS.N1LR11.WT : last exported on 16.12.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 16.12.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 16.12.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 16.12.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 16.12.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 16.12.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 16.12.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 16.12.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 16.12.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1738,52 +1690,52 @@
       <c r="B22" s="27" t="n"/>
       <c r="C22" s="14" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 15.12.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 15.12.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 15.12.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 15.12.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 15.12.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 15.12.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 15.12.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 15.12.23
-DDC.R11KT6.ELFI.MD.TXT : last exported on 10.12.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 14.12.23
-DDC.R11KT6.ELFI.PK.TXT : last exported on 10.12.23
-DDC.R11KT6.ELFI.PR.TXT : last exported on 10.12.23</t>
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 18.12.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 18.12.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 18.12.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 18.12.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 18.12.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 18.12.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 18.12.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 18.12.23
+DDC.R11KT6.ELFI.MD.TXT : last exported on 17.12.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 15.12.23
+DDC.R11KT6.ELFI.PK.TXT : last exported on 17.12.23
+DDC.R11KT6.ELFI.PR.TXT : last exported on 17.12.23</t>
         </is>
       </c>
       <c r="D22" s="5" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 14.12.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 14.12.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 14.12.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 14.12.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 14.12.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 14.12.23
-DEL.N1LKT6.EC.??????.G : last exported on 14.12.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 14.12.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 14.12.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 14.12.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 14.12.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 14.12.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 14.12.23
-DEL.N1LKT6.EC.??????.U : last exported on 14.12.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 14.12.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 14.12.23
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 14.12.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 14.12.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 14.12.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 14.12.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 14.12.23
-DEL.N1LKT6.EC.??????.AS : last exported on 14.12.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 14.12.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 14.12.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 14.12.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 14.12.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 14.12.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 14.12.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 14.12.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 14.12.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 17.12.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 17.12.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 17.12.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 17.12.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 17.12.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 17.12.23
+DEL.N1LKT6.EC.??????.G : last exported on 17.12.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 17.12.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 17.12.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 17.12.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 17.12.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 17.12.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 17.12.23
+DEL.N1LKT6.EC.??????.U : last exported on 17.12.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 17.12.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 17.12.23
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 17.12.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 17.12.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 17.12.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 17.12.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 17.12.23
+DEL.N1LKT6.EC.??????.AS : last exported on 17.12.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 17.12.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 17.12.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 17.12.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 17.12.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 17.12.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 17.12.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 17.12.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 17.12.23</t>
         </is>
       </c>
       <c r="F22" s="3" t="n"/>

</xml_diff>

<commit_message>
Updated on 18.12.23 15:40
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -1283,37 +1283,12 @@
 Daily</t>
         </is>
       </c>
-      <c r="C11" s="10" t="inlineStr"/>
-      <c r="D11" s="10" t="inlineStr"/>
-      <c r="E11" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F11" s="12" t="inlineStr">
-        <is>
-          <t>Successful</t>
-        </is>
-      </c>
-    </row>
-    <row r="12" ht="31.7" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A12" s="30" t="inlineStr">
-        <is>
-          <t>TT</t>
-        </is>
-      </c>
-      <c r="B12" s="9" t="inlineStr">
-        <is>
-          <t>17:30
-Daily</t>
-        </is>
-      </c>
-      <c r="C12" s="15" t="inlineStr">
+      <c r="C11" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.MANDANTN.TXT : last exported on 30.11.23</t>
         </is>
       </c>
-      <c r="D12" s="15" t="inlineStr">
+      <c r="D11" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
@@ -1324,6 +1299,39 @@
 DGI.KT6R11.MANDANT.TXT : last exported on 30.11.23</t>
         </is>
       </c>
+      <c r="E11" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F11" s="12" t="inlineStr">
+        <is>
+          <t>Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="31.7" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A12" s="30" t="inlineStr">
+        <is>
+          <t>TT</t>
+        </is>
+      </c>
+      <c r="B12" s="9" t="inlineStr">
+        <is>
+          <t>17:30
+Daily</t>
+        </is>
+      </c>
+      <c r="C12" s="15" t="inlineStr">
+        <is>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 15.12.23</t>
+        </is>
+      </c>
+      <c r="D12" s="15" t="inlineStr">
+        <is>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 16.12.23</t>
+        </is>
+      </c>
       <c r="E12" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
@@ -1348,39 +1356,6 @@
         </is>
       </c>
       <c r="C13" s="10" t="inlineStr">
-        <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 15.12.23</t>
-        </is>
-      </c>
-      <c r="D13" s="10" t="inlineStr">
-        <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 16.12.23</t>
-        </is>
-      </c>
-      <c r="E13" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F13" s="12" t="inlineStr">
-        <is>
-          <t>Successful</t>
-        </is>
-      </c>
-    </row>
-    <row r="14" ht="182.25" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A14" s="30" t="inlineStr">
-        <is>
-          <t>APOS</t>
-        </is>
-      </c>
-      <c r="B14" s="9" t="inlineStr">
-        <is>
-          <t>18:00
-Wednesday</t>
-        </is>
-      </c>
-      <c r="C14" s="10" t="inlineStr">
         <is>
           <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 05.12.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
@@ -1388,7 +1363,7 @@
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
         </is>
       </c>
-      <c r="D14" s="10" t="inlineStr">
+      <c r="D13" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 14.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 14.12.23
@@ -1399,30 +1374,30 @@
 DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 14.12.23</t>
         </is>
       </c>
-      <c r="E14" s="11" t="inlineStr">
+      <c r="E13" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
         </is>
       </c>
-      <c r="F14" s="12" t="inlineStr">
+      <c r="F13" s="12" t="inlineStr">
         <is>
           <t>Successful</t>
         </is>
       </c>
     </row>
-    <row r="15" ht="37.5" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A15" s="30" t="inlineStr">
-        <is>
-          <t>COK</t>
-        </is>
-      </c>
-      <c r="B15" s="9" t="inlineStr">
-        <is>
-          <t>18:05
-Daily</t>
-        </is>
-      </c>
-      <c r="C15" s="16" t="inlineStr">
+    <row r="14" ht="182.25" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A14" s="30" t="inlineStr">
+        <is>
+          <t>APOS</t>
+        </is>
+      </c>
+      <c r="B14" s="9" t="inlineStr">
+        <is>
+          <t>18:00
+Wednesday</t>
+        </is>
+      </c>
+      <c r="C14" s="10" t="inlineStr">
         <is>
           <t>DGQ.R11KT6.BSIVM.TXT : last exported on 06.12.23
 DGQ.R11KT6.BSIVM.C.TXT : last exported on 06.12.23
@@ -1437,7 +1412,7 @@
 DEL.KMPKT6.APOS.DATA.ZIP : last exported on 13.12.23</t>
         </is>
       </c>
-      <c r="D15" s="16" t="inlineStr">
+      <c r="D14" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 13.12.23
 DEL.N1LN3L.AP.F.GPL.DMP : last exported on 13.12.23
@@ -1455,6 +1430,40 @@
 DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 13.12.23</t>
         </is>
       </c>
+      <c r="E14" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F14" s="12" t="inlineStr">
+        <is>
+          <t>Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="37.5" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A15" s="30" t="inlineStr">
+        <is>
+          <t>COK</t>
+        </is>
+      </c>
+      <c r="B15" s="9" t="inlineStr">
+        <is>
+          <t>18:05
+Daily</t>
+        </is>
+      </c>
+      <c r="C15" s="16" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="D15" s="16" t="inlineStr">
+        <is>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 17.12.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 17.12.23</t>
+        </is>
+      </c>
       <c r="E15" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
@@ -1479,47 +1488,13 @@
         </is>
       </c>
       <c r="C16" s="10" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="D16" s="10" t="inlineStr">
-        <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 17.12.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 17.12.23</t>
-        </is>
-      </c>
-      <c r="E16" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F16" s="12" t="inlineStr">
-        <is>
-          <t>Successful</t>
-        </is>
-      </c>
-    </row>
-    <row r="17" ht="48.2" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A17" s="30" t="inlineStr">
-        <is>
-          <t>EUTERM</t>
-        </is>
-      </c>
-      <c r="B17" s="9" t="inlineStr">
-        <is>
-          <t>18:15
-Daily</t>
-        </is>
-      </c>
-      <c r="C17" s="10" t="inlineStr">
         <is>
           <t>DHP.KUDKT6.KVPSIMPORT : last exported on 17.12.23
 DHP.KUDKT6.ORGUNITS : last exported on 18.12.23
 DHS.R11KT6.HSB02ALL : last exported on 15.12.23</t>
         </is>
       </c>
-      <c r="D17" s="10" t="inlineStr">
+      <c r="D16" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 15.12.23
 DEL.N1LN3L.DP.F.GPL.DMP : last exported on 15.12.23
@@ -1533,35 +1508,35 @@
 DEL.N1LN3L.DISSAORG.ZIP : last exported on 15.12.23</t>
         </is>
       </c>
-      <c r="E17" s="11" t="inlineStr">
+      <c r="E16" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
         </is>
       </c>
-      <c r="F17" s="13" t="inlineStr">
-        <is>
-          <t>DryRun</t>
-        </is>
-      </c>
-    </row>
-    <row r="18" ht="36.75" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A18" s="30" t="inlineStr">
-        <is>
-          <t>Translations</t>
-        </is>
-      </c>
-      <c r="B18" s="9" t="inlineStr">
-        <is>
-          <t>19:00
-Sunday</t>
-        </is>
-      </c>
-      <c r="C18" s="15" t="inlineStr">
+      <c r="F16" s="12" t="inlineStr">
+        <is>
+          <t>Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" ht="48.2" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A17" s="30" t="inlineStr">
+        <is>
+          <t>EUTERM</t>
+        </is>
+      </c>
+      <c r="B17" s="9" t="inlineStr">
+        <is>
+          <t>18:15
+Daily</t>
+        </is>
+      </c>
+      <c r="C17" s="10" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="D18" s="15" t="inlineStr">
+      <c r="D17" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.EUTRM.F.GPD.DMP : last exported on 20.05.22
 DEL.N1LN3L.EUTRM.F.GPL.DMP : last exported on 20.05.22
@@ -1570,6 +1545,39 @@
 DEL.N1LN3L.EUTRM.F.CPL.DMP : last exported on 20.05.22</t>
         </is>
       </c>
+      <c r="E17" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F17" s="13" t="inlineStr">
+        <is>
+          <t>DryRun</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="36.75" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A18" s="30" t="inlineStr">
+        <is>
+          <t>Translations</t>
+        </is>
+      </c>
+      <c r="B18" s="9" t="inlineStr">
+        <is>
+          <t>19:00
+Sunday</t>
+        </is>
+      </c>
+      <c r="C18" s="15" t="inlineStr">
+        <is>
+          <t>DIT.E35KT6.TRANS.ZIP : last exported on 09.01.23</t>
+        </is>
+      </c>
+      <c r="D18" s="15" t="inlineStr">
+        <is>
+          <t>DEL.N1LE35.TRANS.ZIP : last exported on 17.12.23</t>
+        </is>
+      </c>
       <c r="E18" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
@@ -1595,43 +1603,10 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.TRANS.ZIP : last exported on 09.01.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 16.12.23</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
-        <is>
-          <t>DEL.N1LE35.TRANS.ZIP : last exported on 17.12.23</t>
-        </is>
-      </c>
-      <c r="E19" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F19" s="12" t="inlineStr">
-        <is>
-          <t>Successful</t>
-        </is>
-      </c>
-    </row>
-    <row r="20" ht="409.6" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A20" s="30" t="inlineStr">
-        <is>
-          <t>ELFI</t>
-        </is>
-      </c>
-      <c r="B20" s="9" t="inlineStr">
-        <is>
-          <t>20:25
-Daily</t>
-        </is>
-      </c>
-      <c r="C20" s="10" t="inlineStr">
-        <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 16.12.23</t>
-        </is>
-      </c>
-      <c r="D20" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 16.12.23
 DEL.N1LN3L.MT.F.GPL.DMP : last exported on 16.12.23
@@ -1662,33 +1637,30 @@
 DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 16.12.23</t>
         </is>
       </c>
-      <c r="E20" s="11" t="inlineStr">
+      <c r="E19" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
         </is>
       </c>
-      <c r="F20" s="12" t="inlineStr">
+      <c r="F19" s="12" t="inlineStr">
         <is>
           <t>Successful</t>
         </is>
       </c>
     </row>
-    <row r="21" ht="16.5" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A21" s="5" t="n"/>
-      <c r="B21" s="6" t="n"/>
-      <c r="C21" s="4" t="inlineStr"/>
-      <c r="D21" s="4" t="inlineStr"/>
-      <c r="E21" s="2" t="n"/>
-      <c r="F21" s="3" t="n"/>
-    </row>
-    <row r="22" ht="19.5" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A22" s="30" t="inlineStr">
-        <is>
-          <t>DB server Disk Space Monitoring</t>
-        </is>
-      </c>
-      <c r="B22" s="27" t="n"/>
-      <c r="C22" s="14" t="inlineStr">
+    <row r="20" ht="409.6" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A20" s="30" t="inlineStr">
+        <is>
+          <t>ELFI</t>
+        </is>
+      </c>
+      <c r="B20" s="9" t="inlineStr">
+        <is>
+          <t>20:25
+Daily</t>
+        </is>
+      </c>
+      <c r="C20" s="10" t="inlineStr">
         <is>
           <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 18.12.23
 DKG.R11KT6.L520.P.EDCP.LEI : last exported on 18.12.23
@@ -1704,7 +1676,7 @@
 DDC.R11KT6.ELFI.PR.TXT : last exported on 17.12.23</t>
         </is>
       </c>
-      <c r="D22" s="5" t="inlineStr">
+      <c r="D20" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 17.12.23
 DEL.N1LN3L.EL.F.GPL.DMP : last exported on 17.12.23
@@ -1738,6 +1710,82 @@
 DEL.KT6N5X.EL.F.AU.ZIP : last exported on 17.12.23</t>
         </is>
       </c>
+      <c r="E20" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F20" s="12" t="inlineStr">
+        <is>
+          <t>Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="21" ht="16.5" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A21" s="5" t="n"/>
+      <c r="B21" s="6" t="n"/>
+      <c r="C21" s="4" t="inlineStr"/>
+      <c r="D21" s="4" t="inlineStr"/>
+      <c r="E21" s="2" t="n"/>
+      <c r="F21" s="3" t="n"/>
+    </row>
+    <row r="22" ht="19.5" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A22" s="30" t="inlineStr">
+        <is>
+          <t>DB server Disk Space Monitoring</t>
+        </is>
+      </c>
+      <c r="B22" s="27" t="n"/>
+      <c r="C22" s="14" t="inlineStr">
+        <is>
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 18.12.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 18.12.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 18.12.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 18.12.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 18.12.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 18.12.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 18.12.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 18.12.23
+DDC.R11KT6.ELFI.MD.TXT : last exported on 17.12.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 15.12.23
+DDC.R11KT6.ELFI.PK.TXT : last exported on 17.12.23
+DDC.R11KT6.ELFI.PR.TXT : last exported on 17.12.23</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="inlineStr">
+        <is>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 17.12.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 17.12.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 17.12.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 17.12.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 17.12.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 17.12.23
+DEL.N1LKT6.EC.??????.G : last exported on 17.12.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 17.12.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 17.12.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 17.12.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 17.12.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 17.12.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 17.12.23
+DEL.N1LKT6.EC.??????.U : last exported on 17.12.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 17.12.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 17.12.23
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 17.12.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 17.12.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 17.12.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 17.12.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 17.12.23
+DEL.N1LKT6.EC.??????.AS : last exported on 17.12.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 17.12.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 17.12.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 17.12.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 17.12.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 17.12.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 17.12.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 17.12.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 17.12.23</t>
+        </is>
+      </c>
       <c r="F22" s="3" t="n"/>
     </row>
     <row r="23" ht="15" customHeight="1" thickBot="1" thickTop="1">

</xml_diff>

<commit_message>
Updated on 20.12.23 13:03
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 18.12.2023</t>
+          <t>Date - 20.12.2023</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 15.12.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 19.12.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 16.12.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 16.12.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 17.12.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 16.12.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 16.12.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 16.12.23
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 16.12.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 16.12.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 16.12.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 16.12.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 16.12.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 20.12.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 20.12.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 20.12.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 20.12.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 20.12.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 20.12.23
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 20.12.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 20.12.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 20.12.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 20.12.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 20.12.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1109,29 +1109,29 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 15.12.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 17.12.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 19.12.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 19.12.23
 DLV.RPKKT6.WI.S.ZIP : last exported on 15.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 16.12.23
-DIT.E35KT6.WI.ZIP : last exported on 15.12.23
-DEL.K2PKT6.WI.ZIP : last exported on 17.12.23
-DEL.R7AKT6.WI.ZIP : last exported on 14.12.23
-DEL.N5FKT6.WI.ZIP : last exported on 08.12.23</t>
+DLV.I5XKT6.WI.A.ZIP : last exported on 19.12.23
+DIT.E35KT6.WI.ZIP : last exported on 19.12.23
+DEL.K2PKT6.WI.ZIP : last exported on 19.12.23
+DEL.R7AKT6.WI.ZIP : last exported on 20.12.23
+DEL.N5FKT6.WI.ZIP : last exported on 19.12.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 18.12.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 18.12.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 18.12.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 18.12.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 18.12.23
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 18.12.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 18.12.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 18.12.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 18.12.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 18.12.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 18.12.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 19.12.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 19.12.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 19.12.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 19.12.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 19.12.23
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 19.12.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 19.12.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 19.12.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 19.12.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 19.12.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 19.12.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 18.12.23
-DGV.N3LKT6.EPELS.??????.ZIP : last exported on 11.12.23</t>
+DEL.N3LKT6.HST.??????.ZIP : last exported on 20.12.23
+DGV.N3LKT6.EPELS.??????.ZIP : last exported on 18.12.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 17.12.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 17.12.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 17.12.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 17.12.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 17.12.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 17.12.23
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 17.12.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 17.12.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 17.12.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 17.12.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 17.12.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 17.12.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 17.12.23
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 17.12.23
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 17.12.23
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 17.12.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 17.12.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 19.12.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 19.12.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 19.12.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 19.12.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 19.12.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 19.12.23
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 19.12.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 19.12.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 19.12.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 19.12.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 19.12.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 19.12.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 19.12.23
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 19.12.23
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 19.12.23
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 19.12.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 19.12.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 17.12.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 19.12.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1324,12 +1324,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 15.12.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 19.12.23</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 16.12.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 19.12.23</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1367,7 +1367,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 14.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 14.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 17.12.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 19.12.23
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 14.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 14.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 14.12.23
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 17.12.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 17.12.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 19.12.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 19.12.23</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 17.12.23
-DHP.KUDKT6.ORGUNITS : last exported on 18.12.23
-DHS.R11KT6.HSB02ALL : last exported on 15.12.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 19.12.23
+DHP.KUDKT6.ORGUNITS : last exported on 20.12.23
+DHS.R11KT6.HSB02ALL : last exported on 19.12.23</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 15.12.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 15.12.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 17.12.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 15.12.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 15.12.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 15.12.23
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 15.12.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 15.12.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 15.12.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 15.12.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 19.12.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 19.12.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 19.12.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 19.12.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 19.12.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 19.12.23
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 19.12.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 19.12.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 19.12.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 19.12.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1603,38 +1603,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 16.12.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 18.12.23</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 16.12.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 16.12.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 17.12.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 16.12.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 16.12.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 16.12.23
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 16.12.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 16.12.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 16.12.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 16.12.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 16.12.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 16.12.23
-DEL.N1LKT6.MT.??????.G : last exported on 16.12.23
-DEL.N1LKT6.MT.??????.U : last exported on 16.12.23
-DEL.N1LKT6.MT.??????.AS : last exported on 16.12.23
-DVL.N1LN5X.VLM.DSP : last exported on 16.12.23
-DVL.N1LN5X.VLM.WT : last exported on 16.12.23
-DDS.N1LR11.DSP : last exported on 16.12.23
-DDS.N1LR11.WT : last exported on 16.12.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 16.12.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 16.12.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 16.12.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 16.12.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 16.12.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 16.12.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 16.12.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 16.12.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 18.12.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 18.12.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 19.12.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 18.12.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 18.12.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 18.12.23
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 18.12.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 18.12.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 18.12.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 18.12.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 18.12.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 18.12.23
+DEL.N1LKT6.MT.??????.G : last exported on 18.12.23
+DEL.N1LKT6.MT.??????.U : last exported on 18.12.23
+DEL.N1LKT6.MT.??????.AS : last exported on 18.12.23
+DVL.N1LN5X.VLM.DSP : last exported on 18.12.23
+DVL.N1LN5X.VLM.WT : last exported on 18.12.23
+DDS.N1LR11.DSP : last exported on 18.12.23
+DDS.N1LR11.WT : last exported on 18.12.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 18.12.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 18.12.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 18.12.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 18.12.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 18.12.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 18.12.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 18.12.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 18.12.23</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,52 +1662,52 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 18.12.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 18.12.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 18.12.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 18.12.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 18.12.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 18.12.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 18.12.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 18.12.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 20.12.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 20.12.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 20.12.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 20.12.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 20.12.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 20.12.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 20.12.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 20.12.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 17.12.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 15.12.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 19.12.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 17.12.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 17.12.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 17.12.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 17.12.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 17.12.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 17.12.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 17.12.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 17.12.23
-DEL.N1LKT6.EC.??????.G : last exported on 17.12.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 17.12.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 17.12.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 17.12.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 17.12.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 17.12.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 17.12.23
-DEL.N1LKT6.EC.??????.U : last exported on 17.12.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 17.12.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 17.12.23
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 17.12.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 17.12.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 17.12.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 17.12.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 17.12.23
-DEL.N1LKT6.EC.??????.AS : last exported on 17.12.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 17.12.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 17.12.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 17.12.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 17.12.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 17.12.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 17.12.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 17.12.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 17.12.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 19.12.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 19.12.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 19.12.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 19.12.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 19.12.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 19.12.23
+DEL.N1LKT6.EC.??????.G : last exported on 19.12.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 19.12.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 19.12.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 19.12.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 19.12.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 19.12.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 19.12.23
+DEL.N1LKT6.EC.??????.U : last exported on 19.12.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 19.12.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 19.12.23
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 19.12.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 19.12.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 19.12.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 19.12.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 19.12.23
+DEL.N1LKT6.EC.??????.AS : last exported on 19.12.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 19.12.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 19.12.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 19.12.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 19.12.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 19.12.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 19.12.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 19.12.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 19.12.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 21.12.23 13:13
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 20.12.2023</t>
+          <t>Date - 21.12.2023</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 19.12.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 20.12.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 20.12.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 20.12.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 20.12.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 20.12.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 20.12.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 20.12.23
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 20.12.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 20.12.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 20.12.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 20.12.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 20.12.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 21.12.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 21.12.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 21.12.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 21.12.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 21.12.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 21.12.23
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 21.12.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 21.12.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 21.12.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 21.12.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 21.12.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1112,26 +1112,26 @@
           <t>DLV.R31KT6.WI.C.ZIP : last exported on 19.12.23
 DLV.KZ6KT6.WI.V.ZIP : last exported on 19.12.23
 DLV.RPKKT6.WI.S.ZIP : last exported on 15.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 19.12.23
-DIT.E35KT6.WI.ZIP : last exported on 19.12.23
-DEL.K2PKT6.WI.ZIP : last exported on 19.12.23
-DEL.R7AKT6.WI.ZIP : last exported on 20.12.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 20.12.23
+DIT.E35KT6.WI.ZIP : last exported on 20.12.23
+DEL.K2PKT6.WI.ZIP : last exported on 20.12.23
+DEL.R7AKT6.WI.ZIP : last exported on 21.12.23
 DEL.N5FKT6.WI.ZIP : last exported on 19.12.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 19.12.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 19.12.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 19.12.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 19.12.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 19.12.23
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 19.12.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 19.12.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 19.12.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 19.12.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 19.12.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 19.12.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 21.12.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 21.12.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 21.12.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 21.12.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 21.12.23
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 21.12.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 21.12.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 21.12.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 21.12.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 21.12.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 21.12.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 20.12.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 21.12.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 18.12.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 19.12.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 19.12.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 19.12.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 19.12.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 19.12.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 19.12.23
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 19.12.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 19.12.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 19.12.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 19.12.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 19.12.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 19.12.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 19.12.23
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 19.12.23
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 19.12.23
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 19.12.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 19.12.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 20.12.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 20.12.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 20.12.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 20.12.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 20.12.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 20.12.23
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 20.12.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 20.12.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 20.12.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 20.12.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 20.12.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 20.12.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 20.12.23
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 20.12.23
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 20.12.23
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 20.12.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 20.12.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 19.12.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 20.12.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1324,12 +1324,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 19.12.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 20.12.23</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 19.12.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 20.12.23</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="C13" s="10" t="inlineStr">
         <is>
-          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 05.12.23
+          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 20.12.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
 DLV.I5XKT6.AU.A.ZIP : last exported on 13.12.23
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
@@ -1367,7 +1367,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 14.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 14.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 19.12.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 20.12.23
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 14.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 14.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 14.12.23
@@ -1409,25 +1409,25 @@
 DGQ.R11KT6.BSITX.TXT : last exported on 06.12.23
 DGQ.R31KT6.BSIVMC.TXT : last exported on 12.12.23
 DGQ.R31KT6.PKATC.TXT : last exported on 12.12.23
-DEL.KMPKT6.APOS.DATA.ZIP : last exported on 13.12.23</t>
+DEL.KMPKT6.APOS.DATA.ZIP : last exported on 20.12.23</t>
         </is>
       </c>
       <c r="D14" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 13.12.23
-DEL.N1LN3L.AP.F.GPL.DMP : last exported on 13.12.23
-DEL.N1LN3L.AP.F.GTR.DMP : last exported on 13.12.23
-DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 13.12.23
-DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 13.12.23
-DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 13.12.23
-DEL.N1LN0R.AP.F.CPD.DMP : last exported on 13.12.23
-DEL.N1LN0R.AP.F.CPL.DMP : last exported on 13.12.23
-DEL.N1LR31.AP.F.PPS.DMP : last exported on 13.12.23
-DEL.KT6E35.AP.F.DB.ZIP : last exported on 13.12.23
-DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 13.12.23
-DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 13.12.23
-DVL.KT6N5X.VLM.AP.ZIP : last exported on 13.12.23
-DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 13.12.23</t>
+          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 20.12.23
+DEL.N1LN3L.AP.F.GPL.DMP : last exported on 20.12.23
+DEL.N1LN3L.AP.F.GTR.DMP : last exported on 20.12.23
+DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 20.12.23
+DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 20.12.23
+DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 20.12.23
+DEL.N1LN0R.AP.F.CPD.DMP : last exported on 20.12.23
+DEL.N1LN0R.AP.F.CPL.DMP : last exported on 20.12.23
+DEL.N1LR31.AP.F.PPS.DMP : last exported on 20.12.23
+DEL.KT6E35.AP.F.DB.ZIP : last exported on 20.12.23
+DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 20.12.23
+DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 20.12.23
+DVL.KT6N5X.VLM.AP.ZIP : last exported on 20.12.23
+DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 20.12.23</t>
         </is>
       </c>
       <c r="E14" s="11" t="inlineStr">
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 19.12.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 19.12.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 20.12.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 20.12.23</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 19.12.23
-DHP.KUDKT6.ORGUNITS : last exported on 20.12.23
-DHS.R11KT6.HSB02ALL : last exported on 19.12.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 20.12.23
+DHP.KUDKT6.ORGUNITS : last exported on 21.12.23
+DHS.R11KT6.HSB02ALL : last exported on 20.12.23</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 19.12.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 19.12.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 19.12.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 19.12.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 19.12.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 19.12.23
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 19.12.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 19.12.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 19.12.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 19.12.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 20.12.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 20.12.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 20.12.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 20.12.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 20.12.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 20.12.23
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 20.12.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 20.12.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 20.12.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 20.12.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1610,7 +1610,7 @@
         <is>
           <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 18.12.23
 DEL.N1LN3L.MT.F.GPL.DMP : last exported on 18.12.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 19.12.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 20.12.23
 DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 18.12.23
 DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 18.12.23
 DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 18.12.23
@@ -1662,52 +1662,52 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 20.12.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 20.12.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 20.12.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 20.12.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 20.12.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 20.12.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 20.12.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 20.12.23
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 21.12.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 21.12.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 21.12.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 21.12.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 21.12.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 21.12.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 21.12.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 21.12.23
 DDC.R11KT6.ELFI.MD.TXT : last exported on 17.12.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 19.12.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 20.12.23
 DDC.R11KT6.ELFI.PK.TXT : last exported on 17.12.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 17.12.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 19.12.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 19.12.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 19.12.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 19.12.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 19.12.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 19.12.23
-DEL.N1LKT6.EC.??????.G : last exported on 19.12.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 19.12.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 19.12.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 19.12.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 19.12.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 19.12.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 19.12.23
-DEL.N1LKT6.EC.??????.U : last exported on 19.12.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 19.12.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 19.12.23
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 19.12.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 19.12.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 19.12.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 19.12.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 19.12.23
-DEL.N1LKT6.EC.??????.AS : last exported on 19.12.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 19.12.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 19.12.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 19.12.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 19.12.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 19.12.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 19.12.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 19.12.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 19.12.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 20.12.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 20.12.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 20.12.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 20.12.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 20.12.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 20.12.23
+DEL.N1LKT6.EC.??????.G : last exported on 20.12.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 20.12.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 20.12.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 20.12.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 20.12.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 20.12.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 20.12.23
+DEL.N1LKT6.EC.??????.U : last exported on 20.12.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 20.12.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 20.12.23
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 20.12.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 20.12.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 20.12.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 20.12.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 20.12.23
+DEL.N1LKT6.EC.??????.AS : last exported on 20.12.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 20.12.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 20.12.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 20.12.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 20.12.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 20.12.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 20.12.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 20.12.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 20.12.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 25.12.23 13:29
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 21.12.2023</t>
+          <t>Date - 25.12.2023</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 20.12.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 22.12.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 21.12.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 21.12.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 21.12.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 21.12.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 21.12.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 21.12.23
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 21.12.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 21.12.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 21.12.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 21.12.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 21.12.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 23.12.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 23.12.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 24.12.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 23.12.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 23.12.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 23.12.23
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 23.12.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 23.12.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 23.12.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 23.12.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 23.12.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1066,22 +1066,22 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 18.12.23
-DEH.N3LKT6.AP.COMPL.SNK : last exported on 18.12.23</t>
+          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 25.12.23
+DEH.N3LKT6.AP.COMPL.SNK : last exported on 25.12.23</t>
         </is>
       </c>
       <c r="D6" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 18.12.23
-DEL.N1LN3L.DN.F.GPL.DMP : last exported on 18.12.23
-DEL.N1LN3L.DN.F.GTR.DMP : last exported on 18.12.23
-DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 18.12.23
-DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 18.12.23
-DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 18.12.23
-DEL.N1LN0R.DN.F.CPD.DMP : last exported on 18.12.23
-DEL.N1LN0R.DN.F.CPL.DMP : last exported on 18.12.23
-DEL.KT6E35.SN.F.GGO.ZIP : last exported on 18.12.23
-DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 18.12.23</t>
+          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 25.12.23
+DEL.N1LN3L.DN.F.GPL.DMP : last exported on 25.12.23
+DEL.N1LN3L.DN.F.GTR.DMP : last exported on 25.12.23
+DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 25.12.23
+DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 25.12.23
+DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 25.12.23
+DEL.N1LN0R.DN.F.CPD.DMP : last exported on 25.12.23
+DEL.N1LN0R.DN.F.CPL.DMP : last exported on 25.12.23
+DEL.KT6E35.SN.F.GGO.ZIP : last exported on 25.12.23
+DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 25.12.23</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
@@ -1110,28 +1110,28 @@
       <c r="C7" s="10" t="inlineStr">
         <is>
           <t>DLV.R31KT6.WI.C.ZIP : last exported on 19.12.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 19.12.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 24.12.23
 DLV.RPKKT6.WI.S.ZIP : last exported on 15.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 20.12.23
-DIT.E35KT6.WI.ZIP : last exported on 20.12.23
-DEL.K2PKT6.WI.ZIP : last exported on 20.12.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 24.12.23
+DIT.E35KT6.WI.ZIP : last exported on 22.12.23
+DEL.K2PKT6.WI.ZIP : last exported on 24.12.23
 DEL.R7AKT6.WI.ZIP : last exported on 21.12.23
-DEL.N5FKT6.WI.ZIP : last exported on 19.12.23</t>
+DEL.N5FKT6.WI.ZIP : last exported on 22.12.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 21.12.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 21.12.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 21.12.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 21.12.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 21.12.23
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 21.12.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 21.12.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 21.12.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 21.12.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 21.12.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 21.12.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 25.12.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 25.12.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 25.12.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 25.12.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 25.12.23
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 25.12.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 25.12.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 25.12.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 25.12.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 25.12.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 25.12.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 21.12.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 25.12.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 18.12.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 20.12.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 20.12.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 20.12.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 20.12.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 20.12.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 20.12.23
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 20.12.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 20.12.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 20.12.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 20.12.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 20.12.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 20.12.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 20.12.23
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 20.12.23
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 20.12.23
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 20.12.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 20.12.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 24.12.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 24.12.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 24.12.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 24.12.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 24.12.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 24.12.23
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 24.12.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 24.12.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 24.12.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 24.12.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 24.12.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 24.12.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 24.12.23
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 24.12.23
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 24.12.23
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 24.12.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 24.12.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 20.12.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 24.12.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1324,12 +1324,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 20.12.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 22.12.23</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 20.12.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 23.12.23</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="C13" s="10" t="inlineStr">
         <is>
-          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 20.12.23
+          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 23.12.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
 DLV.I5XKT6.AU.A.ZIP : last exported on 13.12.23
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
@@ -1365,13 +1365,13 @@
       </c>
       <c r="D13" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 14.12.23
-DEL.N1LN3L.AU.D.GPL.DMP : last exported on 14.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 20.12.23
-DEL.N1LN0R.AU.D.CPD.DMP : last exported on 14.12.23
-DEL.N1LN0R.AU.D.CPL.DMP : last exported on 14.12.23
-DEL.KT6E35.AU.GGO.ZIP : last exported on 14.12.23
-DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 14.12.23</t>
+          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
+DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 24.12.23
+DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
+DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
+DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
+DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 23.12.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 20.12.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 20.12.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 24.12.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 24.12.23</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 20.12.23
-DHP.KUDKT6.ORGUNITS : last exported on 21.12.23
-DHS.R11KT6.HSB02ALL : last exported on 20.12.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 24.12.23
+DHP.KUDKT6.ORGUNITS : last exported on 25.12.23
+DHS.R11KT6.HSB02ALL : last exported on 22.12.23</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 20.12.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 20.12.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 20.12.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 20.12.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 20.12.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 20.12.23
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 20.12.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 20.12.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 20.12.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 20.12.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 22.12.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 22.12.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 24.12.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 22.12.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 22.12.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 22.12.23
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 22.12.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 22.12.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 22.12.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 22.12.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1575,7 +1575,7 @@
       </c>
       <c r="D18" s="15" t="inlineStr">
         <is>
-          <t>DEL.N1LE35.TRANS.ZIP : last exported on 17.12.23</t>
+          <t>DEL.N1LE35.TRANS.ZIP : last exported on 24.12.23</t>
         </is>
       </c>
       <c r="E18" s="11" t="inlineStr">
@@ -1603,38 +1603,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 18.12.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 23.12.23</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 18.12.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 18.12.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 20.12.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 18.12.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 18.12.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 18.12.23
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 18.12.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 18.12.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 18.12.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 18.12.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 18.12.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 18.12.23
-DEL.N1LKT6.MT.??????.G : last exported on 18.12.23
-DEL.N1LKT6.MT.??????.U : last exported on 18.12.23
-DEL.N1LKT6.MT.??????.AS : last exported on 18.12.23
-DVL.N1LN5X.VLM.DSP : last exported on 18.12.23
-DVL.N1LN5X.VLM.WT : last exported on 18.12.23
-DDS.N1LR11.DSP : last exported on 18.12.23
-DDS.N1LR11.WT : last exported on 18.12.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 18.12.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 18.12.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 18.12.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 18.12.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 18.12.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 18.12.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 18.12.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 18.12.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 23.12.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 23.12.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 24.12.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 23.12.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 23.12.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 23.12.23
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 23.12.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 23.12.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 23.12.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 23.12.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 23.12.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 23.12.23
+DEL.N1LKT6.MT.??????.G : last exported on 23.12.23
+DEL.N1LKT6.MT.??????.U : last exported on 23.12.23
+DEL.N1LKT6.MT.??????.AS : last exported on 23.12.23
+DVL.N1LN5X.VLM.DSP : last exported on 23.12.23
+DVL.N1LN5X.VLM.WT : last exported on 23.12.23
+DDS.N1LR11.DSP : last exported on 23.12.23
+DDS.N1LR11.WT : last exported on 23.12.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 23.12.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 23.12.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 23.12.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 23.12.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 23.12.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 23.12.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 23.12.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 23.12.23</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,52 +1662,52 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 21.12.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 21.12.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 21.12.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 21.12.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 21.12.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 21.12.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 21.12.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 21.12.23
-DDC.R11KT6.ELFI.MD.TXT : last exported on 17.12.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 20.12.23
-DDC.R11KT6.ELFI.PK.TXT : last exported on 17.12.23
-DDC.R11KT6.ELFI.PR.TXT : last exported on 17.12.23</t>
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 22.12.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 22.12.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 22.12.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 22.12.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 22.12.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 22.12.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 22.12.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 22.12.23
+DDC.R11KT6.ELFI.MD.TXT : last exported on 24.12.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 22.12.23
+DDC.R11KT6.ELFI.PK.TXT : last exported on 24.12.23
+DDC.R11KT6.ELFI.PR.TXT : last exported on 24.12.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 20.12.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 20.12.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 20.12.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 20.12.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 20.12.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 20.12.23
-DEL.N1LKT6.EC.??????.G : last exported on 20.12.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 20.12.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 20.12.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 20.12.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 20.12.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 20.12.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 20.12.23
-DEL.N1LKT6.EC.??????.U : last exported on 20.12.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 20.12.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 20.12.23
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 20.12.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 20.12.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 20.12.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 20.12.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 20.12.23
-DEL.N1LKT6.EC.??????.AS : last exported on 20.12.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 20.12.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 20.12.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 20.12.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 20.12.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 20.12.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 20.12.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 20.12.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 20.12.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 24.12.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 24.12.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 24.12.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 24.12.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 24.12.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 24.12.23
+DEL.N1LKT6.EC.??????.G : last exported on 24.12.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 24.12.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 24.12.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 24.12.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 24.12.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 24.12.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 24.12.23
+DEL.N1LKT6.EC.??????.U : last exported on 24.12.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 24.12.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 24.12.23
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 24.12.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 24.12.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 24.12.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 24.12.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 24.12.23
+DEL.N1LKT6.EC.??????.AS : last exported on 24.12.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 24.12.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 24.12.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 24.12.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 24.12.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 24.12.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 24.12.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 24.12.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 24.12.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 26.12.23 12:32
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 25.12.2023</t>
+          <t>Date - 26.12.2023</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -996,7 +996,7 @@
         <is>
           <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 23.12.23
 DEL.N1LN3L.WD.D.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 24.12.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 26.12.23
 DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 23.12.23
 DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 23.12.23
 DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 23.12.23
@@ -1121,13 +1121,13 @@
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 25.12.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 25.12.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 25.12.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 25.12.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 25.12.23
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 25.12.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 25.12.23
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 26.12.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 26.12.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 26.12.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 26.12.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 26.12.23
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 26.12.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 26.12.23
 DEL.KT6E35.WI.GGO.ZIP : last exported on 25.12.23
 DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 25.12.23
 DEL.KT6N5M.WI.GGO.ZIP : last exported on 25.12.23
@@ -1241,14 +1241,14 @@
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 24.12.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 24.12.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 24.12.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 24.12.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 24.12.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 24.12.23
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 24.12.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 24.12.23
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 25.12.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 25.12.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 25.12.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 25.12.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 25.12.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 25.12.23
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 25.12.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 25.12.23
 DEL.KT6E35.TP.D.GGO.ZIP : last exported on 24.12.23
 DEL.KT6E35.TP.D.UGO.ZIP : last exported on 24.12.23
 DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 24.12.23
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 24.12.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 25.12.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1367,7 +1367,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 24.12.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 25.12.23
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 24.12.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 24.12.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 25.12.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 25.12.23</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1496,16 +1496,16 @@
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 22.12.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 22.12.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 24.12.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 22.12.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 22.12.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 22.12.23
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 22.12.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 22.12.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 22.12.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 22.12.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 25.12.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 25.12.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 25.12.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 25.12.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 25.12.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 25.12.23
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 25.12.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 25.12.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 25.12.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 25.12.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1608,25 +1608,25 @@
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 23.12.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 24.12.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 23.12.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 23.12.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 23.12.23
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 23.12.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 23.12.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 23.12.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 23.12.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 23.12.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 23.12.23
-DEL.N1LKT6.MT.??????.G : last exported on 23.12.23
-DEL.N1LKT6.MT.??????.U : last exported on 23.12.23
-DEL.N1LKT6.MT.??????.AS : last exported on 23.12.23
-DVL.N1LN5X.VLM.DSP : last exported on 23.12.23
-DVL.N1LN5X.VLM.WT : last exported on 23.12.23
-DDS.N1LR11.DSP : last exported on 23.12.23
-DDS.N1LR11.WT : last exported on 23.12.23
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 25.12.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 25.12.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 25.12.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 25.12.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 25.12.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 25.12.23
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 25.12.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 25.12.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 25.12.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 25.12.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 25.12.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 25.12.23
+DEL.N1LKT6.MT.??????.G : last exported on 25.12.23
+DEL.N1LKT6.MT.??????.U : last exported on 25.12.23
+DEL.N1LKT6.MT.??????.AS : last exported on 25.12.23
+DVL.N1LN5X.VLM.DSP : last exported on 25.12.23
+DVL.N1LN5X.VLM.WT : last exported on 25.12.23
+DDS.N1LR11.DSP : last exported on 25.12.23
+DDS.N1LR11.WT : last exported on 25.12.23
 DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 23.12.23
 DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 23.12.23
 DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 23.12.23
@@ -1678,35 +1678,35 @@
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 24.12.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 24.12.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 24.12.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 24.12.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 24.12.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 24.12.23
-DEL.N1LKT6.EC.??????.G : last exported on 24.12.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 24.12.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 24.12.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 24.12.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 24.12.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 24.12.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 24.12.23
-DEL.N1LKT6.EC.??????.U : last exported on 24.12.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 24.12.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 24.12.23
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 24.12.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 24.12.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 24.12.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 24.12.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 24.12.23
-DEL.N1LKT6.EC.??????.AS : last exported on 24.12.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 24.12.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 24.12.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 24.12.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 24.12.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 24.12.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 24.12.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 24.12.23
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 25.12.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 25.12.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 25.12.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 25.12.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 25.12.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 25.12.23
+DEL.N1LKT6.EC.??????.G : last exported on 25.12.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 25.12.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 25.12.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 25.12.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 25.12.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 25.12.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 25.12.23
+DEL.N1LKT6.EC.??????.U : last exported on 25.12.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 25.12.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 25.12.23
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 25.12.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 25.12.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 25.12.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 25.12.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 25.12.23
+DEL.N1LKT6.EC.??????.AS : last exported on 25.12.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 25.12.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 25.12.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 25.12.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 25.12.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 25.12.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 25.12.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 25.12.23
 DEL.KT6N5X.EL.F.AU.ZIP : last exported on 24.12.23</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Updated on 28.12.23 14:54
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 26.12.2023</t>
+          <t>Date - 28.12.2023</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 22.12.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 15.12.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 23.12.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 26.12.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 23.12.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 23.12.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 23.12.23
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 23.12.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 23.12.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 23.12.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 23.12.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 23.12.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 16.12.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 16.12.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 17.12.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 16.12.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 16.12.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 16.12.23
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 16.12.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 16.12.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 16.12.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 16.12.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 16.12.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1066,22 +1066,22 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 25.12.23
-DEH.N3LKT6.AP.COMPL.SNK : last exported on 25.12.23</t>
+          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 18.12.23
+DEH.N3LKT6.AP.COMPL.SNK : last exported on 18.12.23</t>
         </is>
       </c>
       <c r="D6" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 25.12.23
-DEL.N1LN3L.DN.F.GPL.DMP : last exported on 25.12.23
-DEL.N1LN3L.DN.F.GTR.DMP : last exported on 25.12.23
-DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 25.12.23
-DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 25.12.23
-DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 25.12.23
-DEL.N1LN0R.DN.F.CPD.DMP : last exported on 25.12.23
-DEL.N1LN0R.DN.F.CPL.DMP : last exported on 25.12.23
-DEL.KT6E35.SN.F.GGO.ZIP : last exported on 25.12.23
-DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 25.12.23</t>
+          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 18.12.23
+DEL.N1LN3L.DN.F.GPL.DMP : last exported on 18.12.23
+DEL.N1LN3L.DN.F.GTR.DMP : last exported on 18.12.23
+DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 18.12.23
+DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 18.12.23
+DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 18.12.23
+DEL.N1LN0R.DN.F.CPD.DMP : last exported on 18.12.23
+DEL.N1LN0R.DN.F.CPL.DMP : last exported on 18.12.23
+DEL.KT6E35.SN.F.GGO.ZIP : last exported on 18.12.23
+DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 18.12.23</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
@@ -1109,29 +1109,29 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 19.12.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 24.12.23
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 15.12.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 17.12.23
 DLV.RPKKT6.WI.S.ZIP : last exported on 15.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 24.12.23
-DIT.E35KT6.WI.ZIP : last exported on 22.12.23
-DEL.K2PKT6.WI.ZIP : last exported on 24.12.23
-DEL.R7AKT6.WI.ZIP : last exported on 21.12.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 16.12.23
+DIT.E35KT6.WI.ZIP : last exported on 15.12.23
+DEL.K2PKT6.WI.ZIP : last exported on 17.12.23
+DEL.R7AKT6.WI.ZIP : last exported on 14.12.23
 DEL.N5FKT6.WI.ZIP : last exported on 22.12.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 26.12.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 26.12.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 26.12.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 26.12.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 26.12.23
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 26.12.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 26.12.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 25.12.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 25.12.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 25.12.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 25.12.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 18.12.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 18.12.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 18.12.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 18.12.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 18.12.23
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 18.12.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 18.12.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 18.12.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 18.12.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 18.12.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 18.12.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 25.12.23
-DGV.N3LKT6.EPELS.??????.ZIP : last exported on 18.12.23</t>
+DEL.N3LKT6.HST.??????.ZIP : last exported on 18.12.23
+DGV.N3LKT6.EPELS.??????.ZIP : last exported on 11.12.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 25.12.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 25.12.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 25.12.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 25.12.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 25.12.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 25.12.23
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 25.12.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 25.12.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 24.12.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 24.12.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 24.12.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 24.12.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 24.12.23
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 24.12.23
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 24.12.23
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 24.12.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 24.12.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 17.12.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 17.12.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 17.12.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 17.12.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 17.12.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 17.12.23
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 17.12.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 17.12.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 17.12.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 17.12.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 17.12.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 17.12.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 17.12.23
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 17.12.23
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 17.12.23
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 17.12.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 17.12.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 25.12.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 17.12.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1324,12 +1324,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 22.12.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 15.12.23</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 23.12.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 16.12.23</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1365,13 +1365,13 @@
       </c>
       <c r="D13" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
-DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 25.12.23
-DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
-DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
-DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
-DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 23.12.23</t>
+          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 14.12.23
+DEL.N1LN3L.AU.D.GPL.DMP : last exported on 14.12.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 17.12.23
+DEL.N1LN0R.AU.D.CPD.DMP : last exported on 14.12.23
+DEL.N1LN0R.AU.D.CPL.DMP : last exported on 14.12.23
+DEL.KT6E35.AU.GGO.ZIP : last exported on 14.12.23
+DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 14.12.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1409,25 +1409,25 @@
 DGQ.R11KT6.BSITX.TXT : last exported on 06.12.23
 DGQ.R31KT6.BSIVMC.TXT : last exported on 12.12.23
 DGQ.R31KT6.PKATC.TXT : last exported on 12.12.23
-DEL.KMPKT6.APOS.DATA.ZIP : last exported on 20.12.23</t>
+DEL.KMPKT6.APOS.DATA.ZIP : last exported on 13.12.23</t>
         </is>
       </c>
       <c r="D14" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 20.12.23
-DEL.N1LN3L.AP.F.GPL.DMP : last exported on 20.12.23
-DEL.N1LN3L.AP.F.GTR.DMP : last exported on 20.12.23
-DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 20.12.23
-DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 20.12.23
-DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 20.12.23
-DEL.N1LN0R.AP.F.CPD.DMP : last exported on 20.12.23
-DEL.N1LN0R.AP.F.CPL.DMP : last exported on 20.12.23
-DEL.N1LR31.AP.F.PPS.DMP : last exported on 20.12.23
-DEL.KT6E35.AP.F.DB.ZIP : last exported on 20.12.23
-DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 20.12.23
-DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 20.12.23
-DVL.KT6N5X.VLM.AP.ZIP : last exported on 20.12.23
-DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 20.12.23</t>
+          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 13.12.23
+DEL.N1LN3L.AP.F.GPL.DMP : last exported on 13.12.23
+DEL.N1LN3L.AP.F.GTR.DMP : last exported on 13.12.23
+DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 13.12.23
+DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 13.12.23
+DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 13.12.23
+DEL.N1LN0R.AP.F.CPD.DMP : last exported on 13.12.23
+DEL.N1LN0R.AP.F.CPL.DMP : last exported on 13.12.23
+DEL.N1LR31.AP.F.PPS.DMP : last exported on 13.12.23
+DEL.KT6E35.AP.F.DB.ZIP : last exported on 13.12.23
+DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 13.12.23
+DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 13.12.23
+DVL.KT6N5X.VLM.AP.ZIP : last exported on 13.12.23
+DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 13.12.23</t>
         </is>
       </c>
       <c r="E14" s="11" t="inlineStr">
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 25.12.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 25.12.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 17.12.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 17.12.23</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 24.12.23
-DHP.KUDKT6.ORGUNITS : last exported on 25.12.23
-DHS.R11KT6.HSB02ALL : last exported on 22.12.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 17.12.23
+DHP.KUDKT6.ORGUNITS : last exported on 18.12.23
+DHS.R11KT6.HSB02ALL : last exported on 15.12.23</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 25.12.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 25.12.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 25.12.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 25.12.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 25.12.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 25.12.23
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 25.12.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 25.12.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 25.12.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 25.12.23</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 15.12.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 15.12.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 17.12.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 15.12.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 15.12.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 15.12.23
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 15.12.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 15.12.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 15.12.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 15.12.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1575,7 +1575,7 @@
       </c>
       <c r="D18" s="15" t="inlineStr">
         <is>
-          <t>DEL.N1LE35.TRANS.ZIP : last exported on 24.12.23</t>
+          <t>DEL.N1LE35.TRANS.ZIP : last exported on 17.12.23</t>
         </is>
       </c>
       <c r="E18" s="11" t="inlineStr">
@@ -1603,38 +1603,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 23.12.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 16.12.23</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 25.12.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 25.12.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 25.12.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 25.12.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 25.12.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 25.12.23
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 25.12.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 25.12.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 25.12.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 25.12.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 25.12.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 25.12.23
-DEL.N1LKT6.MT.??????.G : last exported on 25.12.23
-DEL.N1LKT6.MT.??????.U : last exported on 25.12.23
-DEL.N1LKT6.MT.??????.AS : last exported on 25.12.23
-DVL.N1LN5X.VLM.DSP : last exported on 25.12.23
-DVL.N1LN5X.VLM.WT : last exported on 25.12.23
-DDS.N1LR11.DSP : last exported on 25.12.23
-DDS.N1LR11.WT : last exported on 25.12.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 23.12.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 23.12.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 23.12.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 23.12.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 23.12.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 23.12.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 23.12.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 23.12.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 16.12.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 16.12.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 17.12.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 16.12.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 16.12.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 16.12.23
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 16.12.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 16.12.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 16.12.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 16.12.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 16.12.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 16.12.23
+DEL.N1LKT6.MT.??????.G : last exported on 16.12.23
+DEL.N1LKT6.MT.??????.U : last exported on 16.12.23
+DEL.N1LKT6.MT.??????.AS : last exported on 16.12.23
+DVL.N1LN5X.VLM.DSP : last exported on 16.12.23
+DVL.N1LN5X.VLM.WT : last exported on 16.12.23
+DDS.N1LR11.DSP : last exported on 16.12.23
+DDS.N1LR11.WT : last exported on 16.12.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 16.12.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 16.12.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 16.12.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 16.12.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 16.12.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 16.12.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 16.12.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 16.12.23</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,52 +1662,52 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 22.12.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 22.12.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 22.12.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 22.12.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 22.12.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 22.12.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 22.12.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 22.12.23
-DDC.R11KT6.ELFI.MD.TXT : last exported on 24.12.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 22.12.23
-DDC.R11KT6.ELFI.PK.TXT : last exported on 24.12.23
-DDC.R11KT6.ELFI.PR.TXT : last exported on 24.12.23</t>
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 18.12.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 18.12.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 18.12.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 18.12.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 18.12.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 18.12.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 18.12.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 18.12.23
+DDC.R11KT6.ELFI.MD.TXT : last exported on 17.12.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 15.12.23
+DDC.R11KT6.ELFI.PK.TXT : last exported on 17.12.23
+DDC.R11KT6.ELFI.PR.TXT : last exported on 17.12.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 25.12.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 25.12.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 25.12.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 25.12.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 25.12.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 25.12.23
-DEL.N1LKT6.EC.??????.G : last exported on 25.12.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 25.12.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 25.12.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 25.12.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 25.12.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 25.12.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 25.12.23
-DEL.N1LKT6.EC.??????.U : last exported on 25.12.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 25.12.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 25.12.23
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 25.12.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 25.12.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 25.12.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 25.12.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 25.12.23
-DEL.N1LKT6.EC.??????.AS : last exported on 25.12.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 25.12.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 25.12.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 25.12.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 25.12.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 25.12.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 25.12.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 25.12.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 24.12.23</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 17.12.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 17.12.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 17.12.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 17.12.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 17.12.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 17.12.23
+DEL.N1LKT6.EC.??????.G : last exported on 17.12.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 17.12.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 17.12.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 17.12.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 17.12.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 17.12.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 17.12.23
+DEL.N1LKT6.EC.??????.U : last exported on 17.12.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 17.12.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 17.12.23
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 17.12.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 17.12.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 17.12.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 17.12.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 17.12.23
+DEL.N1LKT6.EC.??????.AS : last exported on 17.12.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 17.12.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 17.12.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 17.12.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 17.12.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 17.12.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 17.12.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 17.12.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 17.12.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 29.12.23 12:55
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 28.12.2023</t>
+          <t>Date - 29.12.2023</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 15.12.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 28.12.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 16.12.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 16.12.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 17.12.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 16.12.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 16.12.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 16.12.23
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 16.12.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 16.12.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 16.12.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 16.12.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 16.12.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 29.12.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 29.12.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 29.12.23
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 29.12.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 29.12.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 29.12.23
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 29.12.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 29.12.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 29.12.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 29.12.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 29.12.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1066,22 +1066,22 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 18.12.23
-DEH.N3LKT6.AP.COMPL.SNK : last exported on 18.12.23</t>
+          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 25.12.23
+DEH.N3LKT6.AP.COMPL.SNK : last exported on 25.12.23</t>
         </is>
       </c>
       <c r="D6" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 18.12.23
-DEL.N1LN3L.DN.F.GPL.DMP : last exported on 18.12.23
-DEL.N1LN3L.DN.F.GTR.DMP : last exported on 18.12.23
-DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 18.12.23
-DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 18.12.23
-DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 18.12.23
-DEL.N1LN0R.DN.F.CPD.DMP : last exported on 18.12.23
-DEL.N1LN0R.DN.F.CPL.DMP : last exported on 18.12.23
-DEL.KT6E35.SN.F.GGO.ZIP : last exported on 18.12.23
-DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 18.12.23</t>
+          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 25.12.23
+DEL.N1LN3L.DN.F.GPL.DMP : last exported on 25.12.23
+DEL.N1LN3L.DN.F.GTR.DMP : last exported on 25.12.23
+DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 25.12.23
+DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 25.12.23
+DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 25.12.23
+DEL.N1LN0R.DN.F.CPD.DMP : last exported on 25.12.23
+DEL.N1LN0R.DN.F.CPL.DMP : last exported on 25.12.23
+DEL.KT6E35.SN.F.GGO.ZIP : last exported on 25.12.23
+DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 25.12.23</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
@@ -1110,28 +1110,28 @@
       <c r="C7" s="10" t="inlineStr">
         <is>
           <t>DLV.R31KT6.WI.C.ZIP : last exported on 15.12.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 17.12.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 27.12.23
 DLV.RPKKT6.WI.S.ZIP : last exported on 15.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 16.12.23
-DIT.E35KT6.WI.ZIP : last exported on 15.12.23
-DEL.K2PKT6.WI.ZIP : last exported on 17.12.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 28.12.23
+DIT.E35KT6.WI.ZIP : last exported on 28.12.23
+DEL.K2PKT6.WI.ZIP : last exported on 28.12.23
 DEL.R7AKT6.WI.ZIP : last exported on 14.12.23
-DEL.N5FKT6.WI.ZIP : last exported on 22.12.23</t>
+DEL.N5FKT6.WI.ZIP : last exported on 25.12.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 18.12.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 18.12.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 18.12.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 18.12.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 18.12.23
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 18.12.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 18.12.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 18.12.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 18.12.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 18.12.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 18.12.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 29.12.23
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 29.12.23
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 29.12.23
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 29.12.23
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 29.12.23
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 29.12.23
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 29.12.23
+DEL.KT6E35.WI.GGO.ZIP : last exported on 29.12.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 29.12.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 29.12.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 29.12.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 18.12.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 29.12.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 11.12.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 17.12.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 17.12.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 17.12.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 17.12.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 17.12.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 17.12.23
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 17.12.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 17.12.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 17.12.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 17.12.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 17.12.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 17.12.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 17.12.23
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 17.12.23
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 17.12.23
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 17.12.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 17.12.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 28.12.23
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 28.12.23
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 28.12.23
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 28.12.23
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 28.12.23
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 28.12.23
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 28.12.23
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 28.12.23
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 28.12.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 28.12.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 28.12.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 28.12.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 28.12.23
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 28.12.23
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 28.12.23
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 28.12.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 28.12.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1283,55 +1283,47 @@
 Daily</t>
         </is>
       </c>
-      <c r="C11" s="10" t="inlineStr">
+      <c r="C11" s="10" t="inlineStr"/>
+      <c r="D11" s="10" t="inlineStr"/>
+      <c r="E11" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F11" s="12" t="inlineStr">
+        <is>
+          <t>Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="31.7" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A12" s="32" t="inlineStr">
+        <is>
+          <t>TT</t>
+        </is>
+      </c>
+      <c r="B12" s="9" t="inlineStr">
+        <is>
+          <t>17:30
+Daily</t>
+        </is>
+      </c>
+      <c r="C12" s="15" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.MANDANTN.TXT : last exported on 30.11.23</t>
         </is>
       </c>
-      <c r="D11" s="10" t="inlineStr">
+      <c r="D12" s="15" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 17.12.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 28.12.23
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
 DGI.KT6R11.MANDANT.TXT : last exported on 30.11.23</t>
         </is>
       </c>
-      <c r="E11" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F11" s="12" t="inlineStr">
-        <is>
-          <t>Successful</t>
-        </is>
-      </c>
-    </row>
-    <row r="12" ht="31.7" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A12" s="32" t="inlineStr">
-        <is>
-          <t>TT</t>
-        </is>
-      </c>
-      <c r="B12" s="9" t="inlineStr">
-        <is>
-          <t>17:30
-Daily</t>
-        </is>
-      </c>
-      <c r="C12" s="15" t="inlineStr">
-        <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 15.12.23</t>
-        </is>
-      </c>
-      <c r="D12" s="15" t="inlineStr">
-        <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 16.12.23</t>
-        </is>
-      </c>
       <c r="E12" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
@@ -1356,6 +1348,39 @@
         </is>
       </c>
       <c r="C13" s="10" t="inlineStr">
+        <is>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 28.12.23</t>
+        </is>
+      </c>
+      <c r="D13" s="10" t="inlineStr">
+        <is>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 28.12.23</t>
+        </is>
+      </c>
+      <c r="E13" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F13" s="12" t="inlineStr">
+        <is>
+          <t>Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="182.25" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A14" s="32" t="inlineStr">
+        <is>
+          <t>APOS</t>
+        </is>
+      </c>
+      <c r="B14" s="9" t="inlineStr">
+        <is>
+          <t>18:00
+Wednesday</t>
+        </is>
+      </c>
+      <c r="C14" s="10" t="inlineStr">
         <is>
           <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 23.12.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
@@ -1363,41 +1388,41 @@
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
         </is>
       </c>
-      <c r="D13" s="10" t="inlineStr">
-        <is>
-          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 14.12.23
-DEL.N1LN3L.AU.D.GPL.DMP : last exported on 14.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 17.12.23
-DEL.N1LN0R.AU.D.CPD.DMP : last exported on 14.12.23
-DEL.N1LN0R.AU.D.CPL.DMP : last exported on 14.12.23
-DEL.KT6E35.AU.GGO.ZIP : last exported on 14.12.23
-DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 14.12.23</t>
-        </is>
-      </c>
-      <c r="E13" s="11" t="inlineStr">
+      <c r="D14" s="10" t="inlineStr">
+        <is>
+          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
+DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 28.12.23
+DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
+DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
+DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
+DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 23.12.23</t>
+        </is>
+      </c>
+      <c r="E14" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
         </is>
       </c>
-      <c r="F13" s="12" t="inlineStr">
+      <c r="F14" s="12" t="inlineStr">
         <is>
           <t>Successful</t>
         </is>
       </c>
     </row>
-    <row r="14" ht="182.25" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A14" s="32" t="inlineStr">
-        <is>
-          <t>APOS</t>
-        </is>
-      </c>
-      <c r="B14" s="9" t="inlineStr">
-        <is>
-          <t>18:00
-Wednesday</t>
-        </is>
-      </c>
-      <c r="C14" s="10" t="inlineStr">
+    <row r="15" ht="37.5" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A15" s="32" t="inlineStr">
+        <is>
+          <t>COK</t>
+        </is>
+      </c>
+      <c r="B15" s="9" t="inlineStr">
+        <is>
+          <t>18:05
+Daily</t>
+        </is>
+      </c>
+      <c r="C15" s="16" t="inlineStr">
         <is>
           <t>DGQ.R11KT6.BSIVM.TXT : last exported on 06.12.23
 DGQ.R11KT6.BSIVM.C.TXT : last exported on 06.12.23
@@ -1409,59 +1434,25 @@
 DGQ.R11KT6.BSITX.TXT : last exported on 06.12.23
 DGQ.R31KT6.BSIVMC.TXT : last exported on 12.12.23
 DGQ.R31KT6.PKATC.TXT : last exported on 12.12.23
-DEL.KMPKT6.APOS.DATA.ZIP : last exported on 13.12.23</t>
-        </is>
-      </c>
-      <c r="D14" s="10" t="inlineStr">
-        <is>
-          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 13.12.23
-DEL.N1LN3L.AP.F.GPL.DMP : last exported on 13.12.23
-DEL.N1LN3L.AP.F.GTR.DMP : last exported on 13.12.23
-DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 13.12.23
-DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 13.12.23
-DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 13.12.23
-DEL.N1LN0R.AP.F.CPD.DMP : last exported on 13.12.23
-DEL.N1LN0R.AP.F.CPL.DMP : last exported on 13.12.23
-DEL.N1LR31.AP.F.PPS.DMP : last exported on 13.12.23
-DEL.KT6E35.AP.F.DB.ZIP : last exported on 13.12.23
-DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 13.12.23
-DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 13.12.23
-DVL.KT6N5X.VLM.AP.ZIP : last exported on 13.12.23
-DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 13.12.23</t>
-        </is>
-      </c>
-      <c r="E14" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F14" s="12" t="inlineStr">
-        <is>
-          <t>Successful</t>
-        </is>
-      </c>
-    </row>
-    <row r="15" ht="37.5" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A15" s="32" t="inlineStr">
-        <is>
-          <t>COK</t>
-        </is>
-      </c>
-      <c r="B15" s="9" t="inlineStr">
-        <is>
-          <t>18:05
-Daily</t>
-        </is>
-      </c>
-      <c r="C15" s="16" t="inlineStr">
-        <is>
-          <t>NA</t>
+DEL.KMPKT6.APOS.DATA.ZIP : last exported on 27.12.23</t>
         </is>
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 17.12.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 17.12.23</t>
+          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 27.12.23
+DEL.N1LN3L.AP.F.GPL.DMP : last exported on 27.12.23
+DEL.N1LN3L.AP.F.GTR.DMP : last exported on 27.12.23
+DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 27.12.23
+DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 27.12.23
+DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 27.12.23
+DEL.N1LN0R.AP.F.CPD.DMP : last exported on 27.12.23
+DEL.N1LN0R.AP.F.CPL.DMP : last exported on 27.12.23
+DEL.N1LR31.AP.F.PPS.DMP : last exported on 27.12.23
+DEL.KT6E35.AP.F.DB.ZIP : last exported on 27.12.23
+DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 27.12.23
+DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 27.12.23
+DVL.KT6N5X.VLM.AP.ZIP : last exported on 27.12.23
+DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 27.12.23</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1480,13 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 17.12.23
-DHP.KUDKT6.ORGUNITS : last exported on 18.12.23
-DHS.R11KT6.HSB02ALL : last exported on 15.12.23</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 15.12.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 15.12.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 17.12.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 15.12.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 15.12.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 15.12.23
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 15.12.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 15.12.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 15.12.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 15.12.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 28.12.23
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 28.12.23</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1533,10 +1514,54 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 28.12.23
+DHP.KUDKT6.ORGUNITS : last exported on 29.12.23
+DHS.R11KT6.HSB02ALL : last exported on 28.12.23</t>
+        </is>
+      </c>
+      <c r="D17" s="10" t="inlineStr">
+        <is>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 28.12.23
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 28.12.23
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 28.12.23
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 28.12.23
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 28.12.23
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 28.12.23
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 28.12.23
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 28.12.23
+DEL.N1LN3L.DISSORG.ZIP : last exported on 28.12.23
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 28.12.23</t>
+        </is>
+      </c>
+      <c r="E17" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F17" s="13" t="inlineStr">
+        <is>
+          <t>DryRun</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="36.75" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A18" s="32" t="inlineStr">
+        <is>
+          <t>Translations</t>
+        </is>
+      </c>
+      <c r="B18" s="9" t="inlineStr">
+        <is>
+          <t>19:00
+Sunday</t>
+        </is>
+      </c>
+      <c r="C18" s="15" t="inlineStr">
+        <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="D17" s="10" t="inlineStr">
+      <c r="D18" s="15" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.EUTRM.F.GPD.DMP : last exported on 20.05.22
 DEL.N1LN3L.EUTRM.F.GPL.DMP : last exported on 20.05.22
@@ -1545,39 +1570,6 @@
 DEL.N1LN3L.EUTRM.F.CPL.DMP : last exported on 20.05.22</t>
         </is>
       </c>
-      <c r="E17" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F17" s="13" t="inlineStr">
-        <is>
-          <t>DryRun</t>
-        </is>
-      </c>
-    </row>
-    <row r="18" ht="36.75" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A18" s="32" t="inlineStr">
-        <is>
-          <t>Translations</t>
-        </is>
-      </c>
-      <c r="B18" s="9" t="inlineStr">
-        <is>
-          <t>19:00
-Sunday</t>
-        </is>
-      </c>
-      <c r="C18" s="15" t="inlineStr">
-        <is>
-          <t>DIT.E35KT6.TRANS.ZIP : last exported on 09.01.23</t>
-        </is>
-      </c>
-      <c r="D18" s="15" t="inlineStr">
-        <is>
-          <t>DEL.N1LE35.TRANS.ZIP : last exported on 17.12.23</t>
-        </is>
-      </c>
       <c r="E18" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
@@ -1603,38 +1595,12 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 16.12.23</t>
+          <t>DIT.E35KT6.TRANS.ZIP : last exported on 09.01.23</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 16.12.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 16.12.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 17.12.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 16.12.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 16.12.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 16.12.23
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 16.12.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 16.12.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 16.12.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 16.12.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 16.12.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 16.12.23
-DEL.N1LKT6.MT.??????.G : last exported on 16.12.23
-DEL.N1LKT6.MT.??????.U : last exported on 16.12.23
-DEL.N1LKT6.MT.??????.AS : last exported on 16.12.23
-DVL.N1LN5X.VLM.DSP : last exported on 16.12.23
-DVL.N1LN5X.VLM.WT : last exported on 16.12.23
-DDS.N1LR11.DSP : last exported on 16.12.23
-DDS.N1LR11.WT : last exported on 16.12.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 16.12.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 16.12.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 16.12.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 16.12.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 16.12.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 16.12.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 16.12.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 16.12.23</t>
+          <t>DEL.N1LE35.TRANS.ZIP : last exported on 24.12.23</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,52 +1628,38 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 18.12.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 18.12.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 18.12.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 18.12.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 18.12.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 18.12.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 18.12.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 18.12.23
-DDC.R11KT6.ELFI.MD.TXT : last exported on 17.12.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 15.12.23
-DDC.R11KT6.ELFI.PK.TXT : last exported on 17.12.23
-DDC.R11KT6.ELFI.PR.TXT : last exported on 17.12.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 28.12.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 17.12.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 17.12.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 17.12.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 17.12.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 17.12.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 17.12.23
-DEL.N1LKT6.EC.??????.G : last exported on 17.12.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 17.12.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 17.12.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 17.12.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 17.12.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 17.12.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 17.12.23
-DEL.N1LKT6.EC.??????.U : last exported on 17.12.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 17.12.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 17.12.23
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 17.12.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 17.12.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 17.12.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 17.12.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 17.12.23
-DEL.N1LKT6.EC.??????.AS : last exported on 17.12.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 17.12.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 17.12.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 17.12.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 17.12.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 17.12.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 17.12.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 17.12.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 17.12.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 28.12.23
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 28.12.23
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 28.12.23
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 28.12.23
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 28.12.23
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 28.12.23
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 28.12.23
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 28.12.23
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 28.12.23
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 28.12.23
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 28.12.23
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 28.12.23
+DEL.N1LKT6.MT.??????.G : last exported on 28.12.23
+DEL.N1LKT6.MT.??????.U : last exported on 28.12.23
+DEL.N1LKT6.MT.??????.AS : last exported on 28.12.23
+DVL.N1LN5X.VLM.DSP : last exported on 28.12.23
+DVL.N1LN5X.VLM.WT : last exported on 28.12.23
+DDS.N1LR11.DSP : last exported on 28.12.23
+DDS.N1LR11.WT : last exported on 28.12.23
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 28.12.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 28.12.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 28.12.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 28.12.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 28.12.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 28.12.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 28.12.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 28.12.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1724,8 +1676,8 @@
     <row r="21" ht="16.5" customHeight="1" thickBot="1" thickTop="1">
       <c r="A21" s="5" t="n"/>
       <c r="B21" s="6" t="n"/>
-      <c r="C21" s="4" t="n"/>
-      <c r="D21" s="4" t="n"/>
+      <c r="C21" s="4" t="inlineStr"/>
+      <c r="D21" s="4" t="inlineStr"/>
       <c r="E21" s="2" t="n"/>
       <c r="F21" s="3" t="n"/>
     </row>
@@ -1738,10 +1690,54 @@
       <c r="B22" s="27" t="n"/>
       <c r="C22" s="14" t="inlineStr">
         <is>
-          <t>Utilization of space in Database Server is 29% (free 71%)</t>
-        </is>
-      </c>
-      <c r="D22" s="4" t="n"/>
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 29.12.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 29.12.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 29.12.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 29.12.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 29.12.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 29.12.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 29.12.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 29.12.23
+DDC.R11KT6.ELFI.MD.TXT : last exported on 24.12.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 28.12.23
+DDC.R11KT6.ELFI.PK.TXT : last exported on 24.12.23
+DDC.R11KT6.ELFI.PR.TXT : last exported on 24.12.23</t>
+        </is>
+      </c>
+      <c r="D22" s="4" t="inlineStr">
+        <is>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 28.12.23
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 28.12.23
+DEL.N1LE35.ELFI.G.DATA : last exported on 28.12.23
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 28.12.23
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 28.12.23
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 28.12.23
+DEL.N1LKT6.EC.??????.G : last exported on 28.12.23
+DWT.N1LN3L.WT.??????.ZIP : last exported on 28.12.23
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 28.12.23
+DEL.N1LE35.ELFI.U.DATA : last exported on 28.12.23
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 28.12.23
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 28.12.23
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 28.12.23
+DEL.N1LKT6.EC.??????.U : last exported on 28.12.23
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 28.12.23
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 28.12.23
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 28.12.23
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 28.12.23
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 28.12.23
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 28.12.23
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 28.12.23
+DEL.N1LKT6.EC.??????.AS : last exported on 28.12.23
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 28.12.23
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 28.12.23
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 28.12.23
+DGV.N1LCEN.EL.F.ZIP : last exported on 28.12.23
+DGV.N1LN7K.EL.F.ZIP : last exported on 28.12.23
+DGV.N1LN5X.EL.F.ZIP : last exported on 28.12.23
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 28.12.23
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 28.12.23</t>
+        </is>
+      </c>
       <c r="F22" s="3" t="n"/>
     </row>
     <row r="23" ht="15" customHeight="1" thickBot="1" thickTop="1">

</xml_diff>

<commit_message>
Updated on 02.01.24 14:34
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 18.12.2023</t>
+          <t>Date - 02.01.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 15.12.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 28.12.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 16.12.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 16.12.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 17.12.23
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 16.12.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 16.12.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 16.12.23
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 16.12.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 16.12.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 16.12.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 16.12.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 16.12.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 30.12.23
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 30.12.23
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 02.01.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 30.12.23
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 30.12.23
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 30.12.23
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 30.12.23
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 30.12.23
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 29.12.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 29.12.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 29.12.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1066,22 +1066,22 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 18.12.23
-DEH.N3LKT6.AP.COMPL.SNK : last exported on 18.12.23</t>
+          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 25.12.23
+DEH.N3LKT6.AP.COMPL.SNK : last exported on 25.12.23</t>
         </is>
       </c>
       <c r="D6" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 18.12.23
-DEL.N1LN3L.DN.F.GPL.DMP : last exported on 18.12.23
-DEL.N1LN3L.DN.F.GTR.DMP : last exported on 18.12.23
-DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 18.12.23
-DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 18.12.23
-DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 18.12.23
-DEL.N1LN0R.DN.F.CPD.DMP : last exported on 18.12.23
-DEL.N1LN0R.DN.F.CPL.DMP : last exported on 18.12.23
-DEL.KT6E35.SN.F.GGO.ZIP : last exported on 18.12.23
-DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 18.12.23</t>
+          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 01.01.24
+DEL.N1LN3L.DN.F.GPL.DMP : last exported on 01.01.24
+DEL.N1LN3L.DN.F.GTR.DMP : last exported on 01.01.24
+DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 01.01.24
+DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 01.01.24
+DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 01.01.24
+DEL.N1LN0R.DN.F.CPD.DMP : last exported on 01.01.24
+DEL.N1LN0R.DN.F.CPL.DMP : last exported on 01.01.24
+DEL.KT6E35.SN.F.GGO.ZIP : last exported on 25.12.23
+DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 25.12.23</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
@@ -1110,28 +1110,28 @@
       <c r="C7" s="10" t="inlineStr">
         <is>
           <t>DLV.R31KT6.WI.C.ZIP : last exported on 15.12.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 17.12.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 27.12.23
 DLV.RPKKT6.WI.S.ZIP : last exported on 15.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 16.12.23
-DIT.E35KT6.WI.ZIP : last exported on 15.12.23
-DEL.K2PKT6.WI.ZIP : last exported on 17.12.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 28.12.23
+DIT.E35KT6.WI.ZIP : last exported on 28.12.23
+DEL.K2PKT6.WI.ZIP : last exported on 28.12.23
 DEL.R7AKT6.WI.ZIP : last exported on 14.12.23
-DEL.N5FKT6.WI.ZIP : last exported on 08.12.23</t>
+DEL.N5FKT6.WI.ZIP : last exported on 25.12.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 18.12.23
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 18.12.23
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 18.12.23
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 18.12.23
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 18.12.23
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 18.12.23
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 18.12.23
-DEL.KT6E35.WI.GGO.ZIP : last exported on 18.12.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 18.12.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 18.12.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 18.12.23</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 02.01.24
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 02.01.24
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 02.01.24
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 02.01.24
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 02.01.24
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 02.01.24
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 02.01.24
+DEL.KT6E35.WI.GGO.ZIP : last exported on 29.12.23
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 29.12.23
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 29.12.23
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 29.12.23</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 18.12.23
+DEL.N3LKT6.HST.??????.ZIP : last exported on 29.12.23
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 11.12.23</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 17.12.23
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 17.12.23
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 17.12.23
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 17.12.23
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 17.12.23
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 17.12.23
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 17.12.23
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 17.12.23
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 17.12.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 17.12.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 17.12.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 17.12.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 17.12.23
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 17.12.23
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 17.12.23
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 17.12.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 17.12.23</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 01.01.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 01.01.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 01.01.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 01.01.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 01.01.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 01.01.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 01.01.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 01.01.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 28.12.23
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 28.12.23
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 28.12.23
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 28.12.23
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 28.12.23
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 28.12.23
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 28.12.23
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 28.12.23
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 28.12.23</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1283,55 +1283,47 @@
 Daily</t>
         </is>
       </c>
-      <c r="C11" s="10" t="inlineStr">
+      <c r="C11" s="10" t="inlineStr"/>
+      <c r="D11" s="10" t="inlineStr"/>
+      <c r="E11" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F11" s="12" t="inlineStr">
+        <is>
+          <t>Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="31.7" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A12" s="32" t="inlineStr">
+        <is>
+          <t>TT</t>
+        </is>
+      </c>
+      <c r="B12" s="9" t="inlineStr">
+        <is>
+          <t>17:30
+Daily</t>
+        </is>
+      </c>
+      <c r="C12" s="15" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.MANDANTN.TXT : last exported on 30.11.23</t>
         </is>
       </c>
-      <c r="D11" s="10" t="inlineStr">
+      <c r="D12" s="15" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 17.12.23
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 01.01.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
 DGI.KT6R11.MANDANT.TXT : last exported on 30.11.23</t>
         </is>
       </c>
-      <c r="E11" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F11" s="12" t="inlineStr">
-        <is>
-          <t>Successful</t>
-        </is>
-      </c>
-    </row>
-    <row r="12" ht="31.7" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A12" s="32" t="inlineStr">
-        <is>
-          <t>TT</t>
-        </is>
-      </c>
-      <c r="B12" s="9" t="inlineStr">
-        <is>
-          <t>17:30
-Daily</t>
-        </is>
-      </c>
-      <c r="C12" s="15" t="inlineStr">
-        <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 15.12.23</t>
-        </is>
-      </c>
-      <c r="D12" s="15" t="inlineStr">
-        <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 16.12.23</t>
-        </is>
-      </c>
       <c r="E12" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
@@ -1357,47 +1349,80 @@
       </c>
       <c r="C13" s="10" t="inlineStr">
         <is>
-          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 05.12.23
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 28.12.23</t>
+        </is>
+      </c>
+      <c r="D13" s="10" t="inlineStr">
+        <is>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 28.12.23</t>
+        </is>
+      </c>
+      <c r="E13" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F13" s="12" t="inlineStr">
+        <is>
+          <t>Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="182.25" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A14" s="32" t="inlineStr">
+        <is>
+          <t>APOS</t>
+        </is>
+      </c>
+      <c r="B14" s="9" t="inlineStr">
+        <is>
+          <t>18:00
+Wednesday</t>
+        </is>
+      </c>
+      <c r="C14" s="10" t="inlineStr">
+        <is>
+          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 23.12.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
 DLV.I5XKT6.AU.A.ZIP : last exported on 13.12.23
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
         </is>
       </c>
-      <c r="D13" s="10" t="inlineStr">
-        <is>
-          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 14.12.23
-DEL.N1LN3L.AU.D.GPL.DMP : last exported on 14.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 17.12.23
-DEL.N1LN0R.AU.D.CPD.DMP : last exported on 14.12.23
-DEL.N1LN0R.AU.D.CPL.DMP : last exported on 14.12.23
-DEL.KT6E35.AU.GGO.ZIP : last exported on 14.12.23
-DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 14.12.23</t>
-        </is>
-      </c>
-      <c r="E13" s="11" t="inlineStr">
+      <c r="D14" s="10" t="inlineStr">
+        <is>
+          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
+DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 01.01.24
+DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
+DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
+DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
+DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 23.12.23</t>
+        </is>
+      </c>
+      <c r="E14" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
         </is>
       </c>
-      <c r="F13" s="12" t="inlineStr">
+      <c r="F14" s="12" t="inlineStr">
         <is>
           <t>Successful</t>
         </is>
       </c>
     </row>
-    <row r="14" ht="182.25" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A14" s="32" t="inlineStr">
-        <is>
-          <t>APOS</t>
-        </is>
-      </c>
-      <c r="B14" s="9" t="inlineStr">
-        <is>
-          <t>18:00
-Wednesday</t>
-        </is>
-      </c>
-      <c r="C14" s="10" t="inlineStr">
+    <row r="15" ht="37.5" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A15" s="32" t="inlineStr">
+        <is>
+          <t>COK</t>
+        </is>
+      </c>
+      <c r="B15" s="9" t="inlineStr">
+        <is>
+          <t>18:05
+Daily</t>
+        </is>
+      </c>
+      <c r="C15" s="16" t="inlineStr">
         <is>
           <t>DGQ.R11KT6.BSIVM.TXT : last exported on 06.12.23
 DGQ.R11KT6.BSIVM.C.TXT : last exported on 06.12.23
@@ -1409,59 +1434,25 @@
 DGQ.R11KT6.BSITX.TXT : last exported on 06.12.23
 DGQ.R31KT6.BSIVMC.TXT : last exported on 12.12.23
 DGQ.R31KT6.PKATC.TXT : last exported on 12.12.23
-DEL.KMPKT6.APOS.DATA.ZIP : last exported on 13.12.23</t>
-        </is>
-      </c>
-      <c r="D14" s="10" t="inlineStr">
-        <is>
-          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 13.12.23
-DEL.N1LN3L.AP.F.GPL.DMP : last exported on 13.12.23
-DEL.N1LN3L.AP.F.GTR.DMP : last exported on 13.12.23
-DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 13.12.23
-DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 13.12.23
-DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 13.12.23
-DEL.N1LN0R.AP.F.CPD.DMP : last exported on 13.12.23
-DEL.N1LN0R.AP.F.CPL.DMP : last exported on 13.12.23
-DEL.N1LR31.AP.F.PPS.DMP : last exported on 13.12.23
-DEL.KT6E35.AP.F.DB.ZIP : last exported on 13.12.23
-DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 13.12.23
-DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 13.12.23
-DVL.KT6N5X.VLM.AP.ZIP : last exported on 13.12.23
-DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 13.12.23</t>
-        </is>
-      </c>
-      <c r="E14" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F14" s="12" t="inlineStr">
-        <is>
-          <t>Successful</t>
-        </is>
-      </c>
-    </row>
-    <row r="15" ht="37.5" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A15" s="32" t="inlineStr">
-        <is>
-          <t>COK</t>
-        </is>
-      </c>
-      <c r="B15" s="9" t="inlineStr">
-        <is>
-          <t>18:05
-Daily</t>
-        </is>
-      </c>
-      <c r="C15" s="16" t="inlineStr">
-        <is>
-          <t>NA</t>
+DEL.KMPKT6.APOS.DATA.ZIP : last exported on 27.12.23</t>
         </is>
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 17.12.23
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 17.12.23</t>
+          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 27.12.23
+DEL.N1LN3L.AP.F.GPL.DMP : last exported on 27.12.23
+DEL.N1LN3L.AP.F.GTR.DMP : last exported on 27.12.23
+DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 27.12.23
+DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 27.12.23
+DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 27.12.23
+DEL.N1LN0R.AP.F.CPD.DMP : last exported on 27.12.23
+DEL.N1LN0R.AP.F.CPL.DMP : last exported on 27.12.23
+DEL.N1LR31.AP.F.PPS.DMP : last exported on 27.12.23
+DEL.KT6E35.AP.F.DB.ZIP : last exported on 27.12.23
+DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 27.12.23
+DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 27.12.23
+DVL.KT6N5X.VLM.AP.ZIP : last exported on 27.12.23
+DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 27.12.23</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1480,13 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 17.12.23
-DHP.KUDKT6.ORGUNITS : last exported on 18.12.23
-DHS.R11KT6.HSB02ALL : last exported on 15.12.23</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 15.12.23
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 15.12.23
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 17.12.23
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 15.12.23
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 15.12.23
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 15.12.23
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 15.12.23
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 15.12.23
-DEL.N1LN3L.DISSORG.ZIP : last exported on 15.12.23
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 15.12.23</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 01.01.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 01.01.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1533,10 +1514,54 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 28.12.23
+DHP.KUDKT6.ORGUNITS : last exported on 29.12.23
+DHS.R11KT6.HSB02ALL : last exported on 28.12.23</t>
+        </is>
+      </c>
+      <c r="D17" s="10" t="inlineStr">
+        <is>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 01.01.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 01.01.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 01.01.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 01.01.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 01.01.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 01.01.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 01.01.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 01.01.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 01.01.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 01.01.24</t>
+        </is>
+      </c>
+      <c r="E17" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F17" s="13" t="inlineStr">
+        <is>
+          <t>DryRun</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="36.75" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A18" s="32" t="inlineStr">
+        <is>
+          <t>Translations</t>
+        </is>
+      </c>
+      <c r="B18" s="9" t="inlineStr">
+        <is>
+          <t>19:00
+Sunday</t>
+        </is>
+      </c>
+      <c r="C18" s="15" t="inlineStr">
+        <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="D17" s="10" t="inlineStr">
+      <c r="D18" s="15" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.EUTRM.F.GPD.DMP : last exported on 20.05.22
 DEL.N1LN3L.EUTRM.F.GPL.DMP : last exported on 20.05.22
@@ -1545,39 +1570,6 @@
 DEL.N1LN3L.EUTRM.F.CPL.DMP : last exported on 20.05.22</t>
         </is>
       </c>
-      <c r="E17" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F17" s="13" t="inlineStr">
-        <is>
-          <t>DryRun</t>
-        </is>
-      </c>
-    </row>
-    <row r="18" ht="36.75" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A18" s="32" t="inlineStr">
-        <is>
-          <t>Translations</t>
-        </is>
-      </c>
-      <c r="B18" s="9" t="inlineStr">
-        <is>
-          <t>19:00
-Sunday</t>
-        </is>
-      </c>
-      <c r="C18" s="15" t="inlineStr">
-        <is>
-          <t>DIT.E35KT6.TRANS.ZIP : last exported on 09.01.23</t>
-        </is>
-      </c>
-      <c r="D18" s="15" t="inlineStr">
-        <is>
-          <t>DEL.N1LE35.TRANS.ZIP : last exported on 17.12.23</t>
-        </is>
-      </c>
       <c r="E18" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
@@ -1603,38 +1595,12 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 16.12.23</t>
+          <t>DIT.E35KT6.TRANS.ZIP : last exported on 09.01.23</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 16.12.23
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 16.12.23
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 17.12.23
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 16.12.23
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 16.12.23
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 16.12.23
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 16.12.23
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 16.12.23
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 16.12.23
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 16.12.23
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 16.12.23
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 16.12.23
-DEL.N1LKT6.MT.??????.G : last exported on 16.12.23
-DEL.N1LKT6.MT.??????.U : last exported on 16.12.23
-DEL.N1LKT6.MT.??????.AS : last exported on 16.12.23
-DVL.N1LN5X.VLM.DSP : last exported on 16.12.23
-DVL.N1LN5X.VLM.WT : last exported on 16.12.23
-DDS.N1LR11.DSP : last exported on 16.12.23
-DDS.N1LR11.WT : last exported on 16.12.23
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 16.12.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 16.12.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 16.12.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 16.12.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 16.12.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 16.12.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 16.12.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 16.12.23</t>
+          <t>DEL.N1LE35.TRANS.ZIP : last exported on 31.12.23</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,52 +1628,38 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 18.12.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 18.12.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 18.12.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 18.12.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 18.12.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 18.12.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 18.12.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 18.12.23
-DDC.R11KT6.ELFI.MD.TXT : last exported on 17.12.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 15.12.23
-DDC.R11KT6.ELFI.PK.TXT : last exported on 17.12.23
-DDC.R11KT6.ELFI.PR.TXT : last exported on 17.12.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 28.12.23</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 17.12.23
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 17.12.23
-DEL.N1LE35.ELFI.G.DATA : last exported on 17.12.23
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 17.12.23
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 17.12.23
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 17.12.23
-DEL.N1LKT6.EC.??????.G : last exported on 17.12.23
-DWT.N1LN3L.WT.??????.ZIP : last exported on 17.12.23
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 17.12.23
-DEL.N1LE35.ELFI.U.DATA : last exported on 17.12.23
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 17.12.23
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 17.12.23
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 17.12.23
-DEL.N1LKT6.EC.??????.U : last exported on 17.12.23
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 17.12.23
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 17.12.23
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 17.12.23
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 17.12.23
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 17.12.23
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 17.12.23
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 17.12.23
-DEL.N1LKT6.EC.??????.AS : last exported on 17.12.23
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 17.12.23
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 17.12.23
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 17.12.23
-DGV.N1LCEN.EL.F.ZIP : last exported on 17.12.23
-DGV.N1LN7K.EL.F.ZIP : last exported on 17.12.23
-DGV.N1LN5X.EL.F.ZIP : last exported on 17.12.23
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 17.12.23
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 17.12.23</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 01.01.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 01.01.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 01.01.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 01.01.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 01.01.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 01.01.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 01.01.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 01.01.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 01.01.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 01.01.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 01.01.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 01.01.24
+DEL.N1LKT6.MT.??????.G : last exported on 01.01.24
+DEL.N1LKT6.MT.??????.U : last exported on 01.01.24
+DEL.N1LKT6.MT.??????.AS : last exported on 01.01.24
+DVL.N1LN5X.VLM.DSP : last exported on 01.01.24
+DVL.N1LN5X.VLM.WT : last exported on 01.01.24
+DDS.N1LR11.DSP : last exported on 01.01.24
+DDS.N1LR11.WT : last exported on 01.01.24
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 28.12.23
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 28.12.23
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 28.12.23
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 28.12.23
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 28.12.23
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 28.12.23
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 28.12.23
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 28.12.23</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1724,8 +1676,8 @@
     <row r="21" ht="16.5" customHeight="1" thickBot="1" thickTop="1">
       <c r="A21" s="5" t="n"/>
       <c r="B21" s="6" t="n"/>
-      <c r="C21" s="4" t="n"/>
-      <c r="D21" s="4" t="n"/>
+      <c r="C21" s="4" t="inlineStr"/>
+      <c r="D21" s="4" t="inlineStr"/>
       <c r="E21" s="2" t="n"/>
       <c r="F21" s="3" t="n"/>
     </row>
@@ -1738,10 +1690,54 @@
       <c r="B22" s="27" t="n"/>
       <c r="C22" s="14" t="inlineStr">
         <is>
-          <t>Utilization of space in Database Server is 29% (free 71%)</t>
-        </is>
-      </c>
-      <c r="D22" s="4" t="n"/>
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 29.12.23
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 29.12.23
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 29.12.23
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 29.12.23
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 29.12.23
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 29.12.23
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 29.12.23
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 29.12.23
+DDC.R11KT6.ELFI.MD.TXT : last exported on 24.12.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 28.12.23
+DDC.R11KT6.ELFI.PK.TXT : last exported on 24.12.23
+DDC.R11KT6.ELFI.PR.TXT : last exported on 24.12.23</t>
+        </is>
+      </c>
+      <c r="D22" s="4" t="inlineStr">
+        <is>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 01.01.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 01.01.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 01.01.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 01.01.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 01.01.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 01.01.24
+DEL.N1LKT6.EC.??????.G : last exported on 01.01.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 01.01.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 01.01.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 01.01.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 01.01.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 01.01.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 01.01.24
+DEL.N1LKT6.EC.??????.U : last exported on 01.01.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 01.01.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 01.01.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 01.01.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 01.01.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 01.01.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 01.01.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 01.01.24
+DEL.N1LKT6.EC.??????.AS : last exported on 01.01.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 01.01.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 01.01.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 01.01.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 01.01.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 01.01.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 01.01.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 01.01.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 28.12.23</t>
+        </is>
+      </c>
       <c r="F22" s="3" t="n"/>
     </row>
     <row r="23" ht="15" customHeight="1" thickBot="1" thickTop="1">

</xml_diff>

<commit_message>
Updated on 02.01.24 14:59
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -989,7 +989,7 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 28.12.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 29.12.23</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
@@ -1002,9 +1002,9 @@
 DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 30.12.23
 DEL.N1LN0R.WD.D.CPD.DMP : last exported on 30.12.23
 DEL.N1LN0R.WD.D.CPL.DMP : last exported on 30.12.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 29.12.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 29.12.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 29.12.23</t>
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 30.12.23
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 30.12.23
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 30.12.23</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1066,8 +1066,8 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 25.12.23
-DEH.N3LKT6.AP.COMPL.SNK : last exported on 25.12.23</t>
+          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 01.01.24
+DEH.N3LKT6.AP.COMPL.SNK : last exported on 01.01.24</t>
         </is>
       </c>
       <c r="D6" s="10" t="inlineStr">
@@ -1080,8 +1080,8 @@
 DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 01.01.24
 DEL.N1LN0R.DN.F.CPD.DMP : last exported on 01.01.24
 DEL.N1LN0R.DN.F.CPL.DMP : last exported on 01.01.24
-DEL.KT6E35.SN.F.GGO.ZIP : last exported on 25.12.23
-DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 25.12.23</t>
+DEL.KT6E35.SN.F.GGO.ZIP : last exported on 01.01.24
+DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 01.01.24</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
@@ -1110,13 +1110,13 @@
       <c r="C7" s="10" t="inlineStr">
         <is>
           <t>DLV.R31KT6.WI.C.ZIP : last exported on 15.12.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 27.12.23
+DLV.KZ6KT6.WI.V.ZIP : last exported on 01.01.24
 DLV.RPKKT6.WI.S.ZIP : last exported on 15.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 28.12.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 01.01.24
 DIT.E35KT6.WI.ZIP : last exported on 28.12.23
-DEL.K2PKT6.WI.ZIP : last exported on 28.12.23
+DEL.K2PKT6.WI.ZIP : last exported on 01.01.24
 DEL.R7AKT6.WI.ZIP : last exported on 14.12.23
-DEL.N5FKT6.WI.ZIP : last exported on 25.12.23</t>
+DEL.N5FKT6.WI.ZIP : last exported on 29.12.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
@@ -1128,10 +1128,10 @@
 DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 02.01.24
 DEL.N1LN0R.WI.D.CPD.DMP : last exported on 02.01.24
 DEL.N1LN0R.WI.D.CPL.DMP : last exported on 02.01.24
-DEL.KT6E35.WI.GGO.ZIP : last exported on 29.12.23
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 29.12.23
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 29.12.23
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 29.12.23</t>
+DEL.KT6E35.WI.GGO.ZIP : last exported on 02.01.24
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 02.01.24
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 02.01.24
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 02.01.24</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,8 +1235,8 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 29.12.23
-DGV.N3LKT6.EPELS.??????.ZIP : last exported on 11.12.23</t>
+DEL.N3LKT6.HST.??????.ZIP : last exported on 02.01.24
+DGV.N3LKT6.EPELS.??????.ZIP : last exported on 01.01.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
@@ -1249,15 +1249,15 @@
 DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 01.01.24
 DEL.N1LN0R.TP.D.CPD.DMP : last exported on 01.01.24
 DEL.N1LN0R.TP.D.CPL.DMP : last exported on 01.01.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 28.12.23
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 28.12.23
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 28.12.23
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 28.12.23
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 28.12.23
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 28.12.23
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 28.12.23
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 28.12.23
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 28.12.23</t>
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 01.01.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 01.01.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 01.01.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 01.01.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 01.01.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 01.01.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 01.01.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 01.01.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 01.01.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1349,12 +1349,12 @@
       </c>
       <c r="C13" s="10" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 28.12.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 29.12.23</t>
         </is>
       </c>
       <c r="D13" s="10" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 28.12.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 30.12.23</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1382,7 +1382,7 @@
       </c>
       <c r="C14" s="10" t="inlineStr">
         <is>
-          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 23.12.23
+          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 30.12.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
 DLV.I5XKT6.AU.A.ZIP : last exported on 13.12.23
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
@@ -1514,9 +1514,9 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 28.12.23
-DHP.KUDKT6.ORGUNITS : last exported on 29.12.23
-DHS.R11KT6.HSB02ALL : last exported on 28.12.23</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 01.01.24
+DHP.KUDKT6.ORGUNITS : last exported on 02.01.24
+DHS.R11KT6.HSB02ALL : last exported on 01.01.24</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
@@ -1628,7 +1628,7 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 28.12.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 01.01.24</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
@@ -1652,14 +1652,14 @@
 DVL.N1LN5X.VLM.WT : last exported on 01.01.24
 DDS.N1LR11.DSP : last exported on 01.01.24
 DDS.N1LR11.WT : last exported on 01.01.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 28.12.23
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 28.12.23
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 28.12.23
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 28.12.23
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 28.12.23
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 28.12.23
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 28.12.23
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 28.12.23</t>
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 01.01.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 01.01.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 01.01.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 01.01.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 01.01.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 01.01.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 01.01.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 01.01.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1690,18 +1690,18 @@
       <c r="B22" s="27" t="n"/>
       <c r="C22" s="14" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 29.12.23
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 29.12.23
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 29.12.23
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 29.12.23
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 29.12.23
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 29.12.23
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 29.12.23
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 29.12.23
-DDC.R11KT6.ELFI.MD.TXT : last exported on 24.12.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 28.12.23
-DDC.R11KT6.ELFI.PK.TXT : last exported on 24.12.23
-DDC.R11KT6.ELFI.PR.TXT : last exported on 24.12.23</t>
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 02.01.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 02.01.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 02.01.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 02.01.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 02.01.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 02.01.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 02.01.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 02.01.24
+DDC.R11KT6.ELFI.MD.TXT : last exported on 31.12.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 29.12.23
+DDC.R11KT6.ELFI.PK.TXT : last exported on 31.12.23
+DDC.R11KT6.ELFI.PR.TXT : last exported on 31.12.23</t>
         </is>
       </c>
       <c r="D22" s="4" t="inlineStr">
@@ -1735,7 +1735,7 @@
 DGV.N1LN7K.EL.F.ZIP : last exported on 01.01.24
 DGV.N1LN5X.EL.F.ZIP : last exported on 01.01.24
 DEL.KT6KT6.EL.F.DRE.CSV : last exported on 01.01.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 28.12.23</t>
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 01.01.24</t>
         </is>
       </c>
       <c r="F22" s="3" t="n"/>

</xml_diff>

<commit_message>
Updated on 03.01.24 14:01
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 02.01.2024</t>
+          <t>Date - 03.01.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 29.12.23</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 02.01.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 30.12.23
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 30.12.23
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 02.01.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 30.12.23
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 30.12.23
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 30.12.23
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 30.12.23
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 30.12.23
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 30.12.23
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 30.12.23
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 30.12.23</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 03.01.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 03.01.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 03.01.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 03.01.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 03.01.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 03.01.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 03.01.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 03.01.24
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 03.01.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 03.01.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 03.01.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1110,28 +1110,28 @@
       <c r="C7" s="10" t="inlineStr">
         <is>
           <t>DLV.R31KT6.WI.C.ZIP : last exported on 15.12.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 01.01.24
+DLV.KZ6KT6.WI.V.ZIP : last exported on 02.01.24
 DLV.RPKKT6.WI.S.ZIP : last exported on 15.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 01.01.24
-DIT.E35KT6.WI.ZIP : last exported on 28.12.23
-DEL.K2PKT6.WI.ZIP : last exported on 01.01.24
+DLV.I5XKT6.WI.A.ZIP : last exported on 02.01.24
+DIT.E35KT6.WI.ZIP : last exported on 02.01.24
+DEL.K2PKT6.WI.ZIP : last exported on 02.01.24
 DEL.R7AKT6.WI.ZIP : last exported on 14.12.23
 DEL.N5FKT6.WI.ZIP : last exported on 29.12.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 02.01.24
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 02.01.24
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 02.01.24
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 02.01.24
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 02.01.24
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 02.01.24
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 02.01.24
-DEL.KT6E35.WI.GGO.ZIP : last exported on 02.01.24
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 02.01.24
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 02.01.24
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 02.01.24</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 03.01.24
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 03.01.24
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 03.01.24
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 03.01.24
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 03.01.24
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 03.01.24
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 03.01.24
+DEL.KT6E35.WI.GGO.ZIP : last exported on 03.01.24
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 03.01.24
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 03.01.24
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 03.01.24</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 02.01.24
+DEL.N3LKT6.HST.??????.ZIP : last exported on 03.01.24
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 01.01.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 01.01.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 01.01.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 01.01.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 01.01.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 01.01.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 01.01.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 01.01.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 01.01.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 01.01.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 01.01.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 01.01.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 01.01.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 01.01.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 01.01.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 01.01.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 01.01.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 01.01.24</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 02.01.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 02.01.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 02.01.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 02.01.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 02.01.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 02.01.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 02.01.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 02.01.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 02.01.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 02.01.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 02.01.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 02.01.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 02.01.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 02.01.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 02.01.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 02.01.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 02.01.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1317,7 +1317,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 01.01.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 02.01.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1349,7 +1349,7 @@
       </c>
       <c r="C13" s="10" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 29.12.23</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 02.01.24</t>
         </is>
       </c>
       <c r="D13" s="10" t="inlineStr">
@@ -1392,7 +1392,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 01.01.24
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 02.01.24
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
@@ -1485,8 +1485,8 @@
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 01.01.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 01.01.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 02.01.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 02.01.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1514,23 +1514,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 01.01.24
-DHP.KUDKT6.ORGUNITS : last exported on 02.01.24
-DHS.R11KT6.HSB02ALL : last exported on 01.01.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 02.01.24
+DHP.KUDKT6.ORGUNITS : last exported on 03.01.24
+DHS.R11KT6.HSB02ALL : last exported on 02.01.24</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 01.01.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 01.01.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 01.01.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 01.01.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 01.01.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 01.01.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 01.01.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 01.01.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 01.01.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 01.01.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 02.01.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 02.01.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 02.01.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 02.01.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 02.01.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 02.01.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 02.01.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 02.01.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 02.01.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 02.01.24</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1628,38 +1628,38 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 01.01.24</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 02.01.24</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 01.01.24
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 01.01.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 01.01.24
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 01.01.24
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 01.01.24
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 01.01.24
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 01.01.24
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 01.01.24
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 01.01.24
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 01.01.24
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 01.01.24
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 01.01.24
-DEL.N1LKT6.MT.??????.G : last exported on 01.01.24
-DEL.N1LKT6.MT.??????.U : last exported on 01.01.24
-DEL.N1LKT6.MT.??????.AS : last exported on 01.01.24
-DVL.N1LN5X.VLM.DSP : last exported on 01.01.24
-DVL.N1LN5X.VLM.WT : last exported on 01.01.24
-DDS.N1LR11.DSP : last exported on 01.01.24
-DDS.N1LR11.WT : last exported on 01.01.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 01.01.24
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 01.01.24
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 01.01.24
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 01.01.24
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 01.01.24
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 01.01.24
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 01.01.24
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 01.01.24</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 02.01.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 02.01.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 02.01.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 02.01.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 02.01.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 02.01.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 02.01.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 02.01.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 02.01.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 02.01.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 02.01.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 02.01.24
+DEL.N1LKT6.MT.??????.G : last exported on 02.01.24
+DEL.N1LKT6.MT.??????.U : last exported on 02.01.24
+DEL.N1LKT6.MT.??????.AS : last exported on 02.01.24
+DVL.N1LN5X.VLM.DSP : last exported on 02.01.24
+DVL.N1LN5X.VLM.WT : last exported on 02.01.24
+DDS.N1LR11.DSP : last exported on 02.01.24
+DDS.N1LR11.WT : last exported on 02.01.24
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 02.01.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 02.01.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 02.01.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 02.01.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 02.01.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 02.01.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 02.01.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 02.01.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1690,52 +1690,52 @@
       <c r="B22" s="27" t="n"/>
       <c r="C22" s="14" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 02.01.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 02.01.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 02.01.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 02.01.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 02.01.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 02.01.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 02.01.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 02.01.24
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 03.01.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 03.01.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 03.01.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 03.01.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 03.01.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 03.01.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 03.01.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 03.01.24
 DDC.R11KT6.ELFI.MD.TXT : last exported on 31.12.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 29.12.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 02.01.24
 DDC.R11KT6.ELFI.PK.TXT : last exported on 31.12.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 31.12.23</t>
         </is>
       </c>
       <c r="D22" s="4" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 01.01.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 01.01.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 01.01.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 01.01.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 01.01.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 01.01.24
-DEL.N1LKT6.EC.??????.G : last exported on 01.01.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 01.01.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 01.01.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 01.01.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 01.01.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 01.01.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 01.01.24
-DEL.N1LKT6.EC.??????.U : last exported on 01.01.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 01.01.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 01.01.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 01.01.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 01.01.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 01.01.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 01.01.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 01.01.24
-DEL.N1LKT6.EC.??????.AS : last exported on 01.01.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 01.01.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 01.01.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 01.01.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 01.01.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 01.01.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 01.01.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 01.01.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 01.01.24</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 02.01.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 02.01.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 02.01.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 02.01.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 02.01.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 02.01.24
+DEL.N1LKT6.EC.??????.G : last exported on 02.01.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 02.01.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 02.01.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 02.01.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 02.01.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 02.01.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 02.01.24
+DEL.N1LKT6.EC.??????.U : last exported on 02.01.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 02.01.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 02.01.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 02.01.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 02.01.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 02.01.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 02.01.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 02.01.24
+DEL.N1LKT6.EC.??????.AS : last exported on 02.01.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 02.01.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 02.01.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 02.01.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 02.01.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 02.01.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 02.01.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 02.01.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 02.01.24</t>
         </is>
       </c>
       <c r="F22" s="3" t="n"/>

</xml_diff>

<commit_message>
Updated on 04.01.24 13:25
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 03.01.2024</t>
+          <t>Date - 04.01.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 02.01.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 03.01.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 03.01.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 03.01.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 03.01.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 03.01.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 03.01.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 03.01.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 03.01.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 03.01.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 03.01.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 03.01.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 03.01.24</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 04.01.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 04.01.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 04.01.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 04.01.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 04.01.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 04.01.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 04.01.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 04.01.24
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 04.01.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 04.01.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 04.01.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1109,29 +1109,29 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 15.12.23
-DLV.KZ6KT6.WI.V.ZIP : last exported on 02.01.24
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 03.01.24
+DLV.KZ6KT6.WI.V.ZIP : last exported on 03.01.24
 DLV.RPKKT6.WI.S.ZIP : last exported on 15.12.23
 DLV.I5XKT6.WI.A.ZIP : last exported on 02.01.24
-DIT.E35KT6.WI.ZIP : last exported on 02.01.24
-DEL.K2PKT6.WI.ZIP : last exported on 02.01.24
+DIT.E35KT6.WI.ZIP : last exported on 03.01.24
+DEL.K2PKT6.WI.ZIP : last exported on 03.01.24
 DEL.R7AKT6.WI.ZIP : last exported on 14.12.23
 DEL.N5FKT6.WI.ZIP : last exported on 29.12.23</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 03.01.24
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 03.01.24
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 03.01.24
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 03.01.24
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 03.01.24
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 03.01.24
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 03.01.24
-DEL.KT6E35.WI.GGO.ZIP : last exported on 03.01.24
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 03.01.24
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 03.01.24
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 03.01.24</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 04.01.24
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 04.01.24
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 04.01.24
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 04.01.24
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 04.01.24
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 04.01.24
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 04.01.24
+DEL.KT6E35.WI.GGO.ZIP : last exported on 04.01.24
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 04.01.24
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 04.01.24
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 04.01.24</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 03.01.24
+DEL.N3LKT6.HST.??????.ZIP : last exported on 04.01.24
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 01.01.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 02.01.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 02.01.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 02.01.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 02.01.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 02.01.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 02.01.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 02.01.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 02.01.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 02.01.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 02.01.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 02.01.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 02.01.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 02.01.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 02.01.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 02.01.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 02.01.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 02.01.24</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 03.01.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 03.01.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 03.01.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 03.01.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 03.01.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 03.01.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 03.01.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 03.01.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 03.01.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 03.01.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 03.01.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 03.01.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 03.01.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 03.01.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 03.01.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 03.01.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 03.01.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1317,7 +1317,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 02.01.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 03.01.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1349,12 +1349,12 @@
       </c>
       <c r="C13" s="10" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 02.01.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 03.01.24</t>
         </is>
       </c>
       <c r="D13" s="10" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 30.12.23</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 03.01.24</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1392,7 +1392,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 02.01.24
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 03.01.24
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
@@ -1434,25 +1434,25 @@
 DGQ.R11KT6.BSITX.TXT : last exported on 06.12.23
 DGQ.R31KT6.BSIVMC.TXT : last exported on 12.12.23
 DGQ.R31KT6.PKATC.TXT : last exported on 12.12.23
-DEL.KMPKT6.APOS.DATA.ZIP : last exported on 27.12.23</t>
+DEL.KMPKT6.APOS.DATA.ZIP : last exported on 03.01.24</t>
         </is>
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 27.12.23
-DEL.N1LN3L.AP.F.GPL.DMP : last exported on 27.12.23
-DEL.N1LN3L.AP.F.GTR.DMP : last exported on 27.12.23
-DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 27.12.23
-DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 27.12.23
-DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 27.12.23
-DEL.N1LN0R.AP.F.CPD.DMP : last exported on 27.12.23
-DEL.N1LN0R.AP.F.CPL.DMP : last exported on 27.12.23
-DEL.N1LR31.AP.F.PPS.DMP : last exported on 27.12.23
-DEL.KT6E35.AP.F.DB.ZIP : last exported on 27.12.23
-DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 27.12.23
-DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 27.12.23
-DVL.KT6N5X.VLM.AP.ZIP : last exported on 27.12.23
-DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 27.12.23</t>
+          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 03.01.24
+DEL.N1LN3L.AP.F.GPL.DMP : last exported on 03.01.24
+DEL.N1LN3L.AP.F.GTR.DMP : last exported on 03.01.24
+DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 03.01.24
+DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 03.01.24
+DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 03.01.24
+DEL.N1LN0R.AP.F.CPD.DMP : last exported on 03.01.24
+DEL.N1LN0R.AP.F.CPL.DMP : last exported on 03.01.24
+DEL.N1LR31.AP.F.PPS.DMP : last exported on 03.01.24
+DEL.KT6E35.AP.F.DB.ZIP : last exported on 03.01.24
+DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 03.01.24
+DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 03.01.24
+DVL.KT6N5X.VLM.AP.ZIP : last exported on 03.01.24
+DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 03.01.24</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1485,8 +1485,8 @@
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 02.01.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 02.01.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 03.01.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 03.01.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1514,23 +1514,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 02.01.24
-DHP.KUDKT6.ORGUNITS : last exported on 03.01.24
-DHS.R11KT6.HSB02ALL : last exported on 02.01.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 03.01.24
+DHP.KUDKT6.ORGUNITS : last exported on 04.01.24
+DHS.R11KT6.HSB02ALL : last exported on 03.01.24</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 02.01.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 02.01.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 02.01.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 02.01.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 02.01.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 02.01.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 02.01.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 02.01.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 02.01.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 02.01.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 03.01.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 03.01.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 03.01.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 03.01.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 03.01.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 03.01.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 03.01.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 03.01.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 03.01.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 03.01.24</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1628,38 +1628,38 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 02.01.24</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 03.01.24</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 02.01.24
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 02.01.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 02.01.24
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 02.01.24
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 02.01.24
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 02.01.24
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 02.01.24
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 02.01.24
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 02.01.24
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 02.01.24
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 02.01.24
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 02.01.24
-DEL.N1LKT6.MT.??????.G : last exported on 02.01.24
-DEL.N1LKT6.MT.??????.U : last exported on 02.01.24
-DEL.N1LKT6.MT.??????.AS : last exported on 02.01.24
-DVL.N1LN5X.VLM.DSP : last exported on 02.01.24
-DVL.N1LN5X.VLM.WT : last exported on 02.01.24
-DDS.N1LR11.DSP : last exported on 02.01.24
-DDS.N1LR11.WT : last exported on 02.01.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 02.01.24
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 02.01.24
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 02.01.24
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 02.01.24
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 02.01.24
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 02.01.24
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 02.01.24
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 02.01.24</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 03.01.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 03.01.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 03.01.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 03.01.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 03.01.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 03.01.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 03.01.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 03.01.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 03.01.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 03.01.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 03.01.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 03.01.24
+DEL.N1LKT6.MT.??????.G : last exported on 03.01.24
+DEL.N1LKT6.MT.??????.U : last exported on 03.01.24
+DEL.N1LKT6.MT.??????.AS : last exported on 03.01.24
+DVL.N1LN5X.VLM.DSP : last exported on 03.01.24
+DVL.N1LN5X.VLM.WT : last exported on 03.01.24
+DDS.N1LR11.DSP : last exported on 03.01.24
+DDS.N1LR11.WT : last exported on 03.01.24
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 03.01.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 03.01.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 03.01.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 03.01.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 03.01.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 03.01.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 03.01.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 03.01.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1690,52 +1690,52 @@
       <c r="B22" s="27" t="n"/>
       <c r="C22" s="14" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 03.01.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 03.01.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 03.01.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 03.01.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 03.01.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 03.01.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 03.01.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 03.01.24
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 04.01.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 04.01.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 04.01.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 04.01.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 04.01.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 04.01.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 04.01.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 04.01.24
 DDC.R11KT6.ELFI.MD.TXT : last exported on 31.12.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 02.01.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 03.01.24
 DDC.R11KT6.ELFI.PK.TXT : last exported on 31.12.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 31.12.23</t>
         </is>
       </c>
       <c r="D22" s="4" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 02.01.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 02.01.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 02.01.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 02.01.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 02.01.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 02.01.24
-DEL.N1LKT6.EC.??????.G : last exported on 02.01.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 02.01.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 02.01.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 02.01.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 02.01.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 02.01.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 02.01.24
-DEL.N1LKT6.EC.??????.U : last exported on 02.01.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 02.01.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 02.01.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 02.01.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 02.01.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 02.01.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 02.01.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 02.01.24
-DEL.N1LKT6.EC.??????.AS : last exported on 02.01.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 02.01.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 02.01.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 02.01.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 02.01.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 02.01.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 02.01.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 02.01.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 02.01.24</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 03.01.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 03.01.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 03.01.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 03.01.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 03.01.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 03.01.24
+DEL.N1LKT6.EC.??????.G : last exported on 03.01.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 03.01.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 03.01.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 03.01.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 03.01.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 03.01.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 03.01.24
+DEL.N1LKT6.EC.??????.U : last exported on 03.01.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 03.01.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 03.01.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 03.01.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 03.01.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 03.01.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 03.01.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 03.01.24
+DEL.N1LKT6.EC.??????.AS : last exported on 03.01.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 03.01.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 03.01.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 03.01.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 03.01.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 03.01.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 03.01.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 03.01.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 03.01.24</t>
         </is>
       </c>
       <c r="F22" s="3" t="n"/>

</xml_diff>

<commit_message>
Updated on 05.01.24 14:30
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 04.01.2024</t>
+          <t>Date - 05.01.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 03.01.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 04.01.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 04.01.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 04.01.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 04.01.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 04.01.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 04.01.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 04.01.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 04.01.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 04.01.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 04.01.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 04.01.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 04.01.24</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 05.01.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 05.01.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 05.01.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 05.01.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 05.01.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 05.01.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 05.01.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 05.01.24
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 05.01.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 05.01.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 05.01.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1112,26 +1112,26 @@
           <t>DLV.R31KT6.WI.C.ZIP : last exported on 03.01.24
 DLV.KZ6KT6.WI.V.ZIP : last exported on 03.01.24
 DLV.RPKKT6.WI.S.ZIP : last exported on 15.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 02.01.24
-DIT.E35KT6.WI.ZIP : last exported on 03.01.24
-DEL.K2PKT6.WI.ZIP : last exported on 03.01.24
+DLV.I5XKT6.WI.A.ZIP : last exported on 04.01.24
+DIT.E35KT6.WI.ZIP : last exported on 04.01.24
+DEL.K2PKT6.WI.ZIP : last exported on 04.01.24
 DEL.R7AKT6.WI.ZIP : last exported on 14.12.23
-DEL.N5FKT6.WI.ZIP : last exported on 29.12.23</t>
+DEL.N5FKT6.WI.ZIP : last exported on 04.01.24</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 04.01.24
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 04.01.24
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 04.01.24
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 04.01.24
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 04.01.24
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 04.01.24
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 04.01.24
-DEL.KT6E35.WI.GGO.ZIP : last exported on 04.01.24
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 04.01.24
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 04.01.24
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 04.01.24</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 05.01.24
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 05.01.24
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 05.01.24
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 05.01.24
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 05.01.24
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 05.01.24
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 05.01.24
+DEL.KT6E35.WI.GGO.ZIP : last exported on 05.01.24
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 05.01.24
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 05.01.24
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 05.01.24</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 04.01.24
+DEL.N3LKT6.HST.??????.ZIP : last exported on 05.01.24
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 01.01.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 03.01.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 03.01.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 03.01.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 03.01.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 03.01.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 03.01.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 03.01.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 03.01.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 03.01.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 03.01.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 03.01.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 03.01.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 03.01.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 03.01.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 03.01.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 03.01.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 03.01.24</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 04.01.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 04.01.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 04.01.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 04.01.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 04.01.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 04.01.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 04.01.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 04.01.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 04.01.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 04.01.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 04.01.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 04.01.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 04.01.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 04.01.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 04.01.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 04.01.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 04.01.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1317,7 +1317,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 03.01.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 04.01.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1349,12 +1349,12 @@
       </c>
       <c r="C13" s="10" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 03.01.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 04.01.24</t>
         </is>
       </c>
       <c r="D13" s="10" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 03.01.24</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 04.01.24</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1392,7 +1392,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 03.01.24
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 04.01.24
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
@@ -1485,8 +1485,8 @@
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 03.01.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 03.01.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 04.01.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 04.01.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1514,23 +1514,23 @@
       </c>
       <c r="C17" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 03.01.24
-DHP.KUDKT6.ORGUNITS : last exported on 04.01.24
-DHS.R11KT6.HSB02ALL : last exported on 03.01.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 04.01.24
+DHP.KUDKT6.ORGUNITS : last exported on 05.01.24
+DHS.R11KT6.HSB02ALL : last exported on 04.01.24</t>
         </is>
       </c>
       <c r="D17" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 03.01.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 03.01.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 03.01.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 03.01.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 03.01.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 03.01.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 03.01.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 03.01.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 03.01.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 03.01.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 04.01.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 04.01.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 04.01.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 04.01.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 04.01.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 04.01.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 04.01.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 04.01.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 04.01.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 04.01.24</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -1628,38 +1628,38 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 03.01.24</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 04.01.24</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 03.01.24
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 03.01.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 03.01.24
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 03.01.24
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 03.01.24
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 03.01.24
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 03.01.24
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 03.01.24
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 03.01.24
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 03.01.24
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 03.01.24
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 03.01.24
-DEL.N1LKT6.MT.??????.G : last exported on 03.01.24
-DEL.N1LKT6.MT.??????.U : last exported on 03.01.24
-DEL.N1LKT6.MT.??????.AS : last exported on 03.01.24
-DVL.N1LN5X.VLM.DSP : last exported on 03.01.24
-DVL.N1LN5X.VLM.WT : last exported on 03.01.24
-DDS.N1LR11.DSP : last exported on 03.01.24
-DDS.N1LR11.WT : last exported on 03.01.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 03.01.24
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 03.01.24
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 03.01.24
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 03.01.24
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 03.01.24
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 03.01.24
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 03.01.24
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 03.01.24</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 04.01.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 04.01.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 04.01.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 04.01.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 04.01.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 04.01.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 04.01.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 04.01.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 04.01.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 04.01.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 04.01.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 04.01.24
+DEL.N1LKT6.MT.??????.G : last exported on 04.01.24
+DEL.N1LKT6.MT.??????.U : last exported on 04.01.24
+DEL.N1LKT6.MT.??????.AS : last exported on 04.01.24
+DVL.N1LN5X.VLM.DSP : last exported on 04.01.24
+DVL.N1LN5X.VLM.WT : last exported on 04.01.24
+DDS.N1LR11.DSP : last exported on 04.01.24
+DDS.N1LR11.WT : last exported on 04.01.24
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 04.01.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 04.01.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 04.01.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 04.01.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 04.01.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 04.01.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 04.01.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 04.01.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">
@@ -1690,52 +1690,52 @@
       <c r="B22" s="27" t="n"/>
       <c r="C22" s="14" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 04.01.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 04.01.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 04.01.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 04.01.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 04.01.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 04.01.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 04.01.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 04.01.24
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 05.01.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 05.01.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 05.01.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 05.01.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 05.01.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 05.01.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 05.01.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 05.01.24
 DDC.R11KT6.ELFI.MD.TXT : last exported on 31.12.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 03.01.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 04.01.24
 DDC.R11KT6.ELFI.PK.TXT : last exported on 31.12.23
 DDC.R11KT6.ELFI.PR.TXT : last exported on 31.12.23</t>
         </is>
       </c>
       <c r="D22" s="4" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 03.01.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 03.01.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 03.01.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 03.01.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 03.01.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 03.01.24
-DEL.N1LKT6.EC.??????.G : last exported on 03.01.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 03.01.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 03.01.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 03.01.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 03.01.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 03.01.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 03.01.24
-DEL.N1LKT6.EC.??????.U : last exported on 03.01.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 03.01.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 03.01.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 03.01.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 03.01.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 03.01.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 03.01.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 03.01.24
-DEL.N1LKT6.EC.??????.AS : last exported on 03.01.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 03.01.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 03.01.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 03.01.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 03.01.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 03.01.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 03.01.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 03.01.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 03.01.24</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 04.01.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 04.01.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 04.01.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 04.01.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 04.01.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 04.01.24
+DEL.N1LKT6.EC.??????.G : last exported on 04.01.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 04.01.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 04.01.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 04.01.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 04.01.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 04.01.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 04.01.24
+DEL.N1LKT6.EC.??????.U : last exported on 04.01.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 04.01.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 04.01.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 04.01.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 04.01.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 04.01.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 04.01.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 04.01.24
+DEL.N1LKT6.EC.??????.AS : last exported on 04.01.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 04.01.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 04.01.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 04.01.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 04.01.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 04.01.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 04.01.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 04.01.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 04.01.24</t>
         </is>
       </c>
       <c r="F22" s="3" t="n"/>

</xml_diff>

<commit_message>
Updated on 05.01.24 14:36
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -1283,37 +1283,12 @@
 Daily</t>
         </is>
       </c>
-      <c r="C11" s="10" t="inlineStr"/>
-      <c r="D11" s="10" t="inlineStr"/>
-      <c r="E11" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F11" s="12" t="inlineStr">
-        <is>
-          <t>Successful</t>
-        </is>
-      </c>
-    </row>
-    <row r="12" ht="31.7" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A12" s="32" t="inlineStr">
-        <is>
-          <t>TT</t>
-        </is>
-      </c>
-      <c r="B12" s="9" t="inlineStr">
-        <is>
-          <t>17:30
-Daily</t>
-        </is>
-      </c>
-      <c r="C12" s="15" t="inlineStr">
+      <c r="C11" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.MANDANTN.TXT : last exported on 30.11.23</t>
         </is>
       </c>
-      <c r="D12" s="15" t="inlineStr">
+      <c r="D11" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
@@ -1324,6 +1299,39 @@
 DGI.KT6R11.MANDANT.TXT : last exported on 30.11.23</t>
         </is>
       </c>
+      <c r="E11" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F11" s="12" t="inlineStr">
+        <is>
+          <t>Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="31.7" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A12" s="32" t="inlineStr">
+        <is>
+          <t>TT</t>
+        </is>
+      </c>
+      <c r="B12" s="9" t="inlineStr">
+        <is>
+          <t>17:30
+Daily</t>
+        </is>
+      </c>
+      <c r="C12" s="15" t="inlineStr">
+        <is>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 04.01.24</t>
+        </is>
+      </c>
+      <c r="D12" s="15" t="inlineStr">
+        <is>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 04.01.24</t>
+        </is>
+      </c>
       <c r="E12" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
@@ -1348,39 +1356,6 @@
         </is>
       </c>
       <c r="C13" s="10" t="inlineStr">
-        <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 04.01.24</t>
-        </is>
-      </c>
-      <c r="D13" s="10" t="inlineStr">
-        <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 04.01.24</t>
-        </is>
-      </c>
-      <c r="E13" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F13" s="12" t="inlineStr">
-        <is>
-          <t>Successful</t>
-        </is>
-      </c>
-    </row>
-    <row r="14" ht="182.25" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A14" s="32" t="inlineStr">
-        <is>
-          <t>APOS</t>
-        </is>
-      </c>
-      <c r="B14" s="9" t="inlineStr">
-        <is>
-          <t>18:00
-Wednesday</t>
-        </is>
-      </c>
-      <c r="C14" s="10" t="inlineStr">
         <is>
           <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 30.12.23
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
@@ -1388,7 +1363,7 @@
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
         </is>
       </c>
-      <c r="D14" s="10" t="inlineStr">
+      <c r="D13" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
@@ -1399,30 +1374,30 @@
 DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 23.12.23</t>
         </is>
       </c>
-      <c r="E14" s="11" t="inlineStr">
+      <c r="E13" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
         </is>
       </c>
-      <c r="F14" s="12" t="inlineStr">
+      <c r="F13" s="12" t="inlineStr">
         <is>
           <t>Successful</t>
         </is>
       </c>
     </row>
-    <row r="15" ht="37.5" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A15" s="32" t="inlineStr">
-        <is>
-          <t>COK</t>
-        </is>
-      </c>
-      <c r="B15" s="9" t="inlineStr">
-        <is>
-          <t>18:05
-Daily</t>
-        </is>
-      </c>
-      <c r="C15" s="16" t="inlineStr">
+    <row r="14" ht="182.25" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A14" s="32" t="inlineStr">
+        <is>
+          <t>APOS</t>
+        </is>
+      </c>
+      <c r="B14" s="9" t="inlineStr">
+        <is>
+          <t>18:00
+Wednesday</t>
+        </is>
+      </c>
+      <c r="C14" s="10" t="inlineStr">
         <is>
           <t>DGQ.R11KT6.BSIVM.TXT : last exported on 06.12.23
 DGQ.R11KT6.BSIVM.C.TXT : last exported on 06.12.23
@@ -1437,7 +1412,7 @@
 DEL.KMPKT6.APOS.DATA.ZIP : last exported on 03.01.24</t>
         </is>
       </c>
-      <c r="D15" s="16" t="inlineStr">
+      <c r="D14" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 03.01.24
 DEL.N1LN3L.AP.F.GPL.DMP : last exported on 03.01.24
@@ -1455,6 +1430,40 @@
 DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 03.01.24</t>
         </is>
       </c>
+      <c r="E14" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F14" s="12" t="inlineStr">
+        <is>
+          <t>Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="37.5" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A15" s="32" t="inlineStr">
+        <is>
+          <t>COK</t>
+        </is>
+      </c>
+      <c r="B15" s="9" t="inlineStr">
+        <is>
+          <t>18:05
+Daily</t>
+        </is>
+      </c>
+      <c r="C15" s="16" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="D15" s="16" t="inlineStr">
+        <is>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 04.01.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 04.01.24</t>
+        </is>
+      </c>
       <c r="E15" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
@@ -1479,47 +1488,13 @@
         </is>
       </c>
       <c r="C16" s="10" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="D16" s="10" t="inlineStr">
-        <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 04.01.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 04.01.24</t>
-        </is>
-      </c>
-      <c r="E16" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F16" s="12" t="inlineStr">
-        <is>
-          <t>Successful</t>
-        </is>
-      </c>
-    </row>
-    <row r="17" ht="48.2" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A17" s="32" t="inlineStr">
-        <is>
-          <t>EUTERM</t>
-        </is>
-      </c>
-      <c r="B17" s="9" t="inlineStr">
-        <is>
-          <t>18:15
-Daily</t>
-        </is>
-      </c>
-      <c r="C17" s="10" t="inlineStr">
         <is>
           <t>DHP.KUDKT6.KVPSIMPORT : last exported on 04.01.24
 DHP.KUDKT6.ORGUNITS : last exported on 05.01.24
 DHS.R11KT6.HSB02ALL : last exported on 04.01.24</t>
         </is>
       </c>
-      <c r="D17" s="10" t="inlineStr">
+      <c r="D16" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 04.01.24
 DEL.N1LN3L.DP.F.GPL.DMP : last exported on 04.01.24
@@ -1533,35 +1508,35 @@
 DEL.N1LN3L.DISSAORG.ZIP : last exported on 04.01.24</t>
         </is>
       </c>
-      <c r="E17" s="11" t="inlineStr">
+      <c r="E16" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
         </is>
       </c>
-      <c r="F17" s="13" t="inlineStr">
-        <is>
-          <t>DryRun</t>
-        </is>
-      </c>
-    </row>
-    <row r="18" ht="36.75" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A18" s="32" t="inlineStr">
-        <is>
-          <t>Translations</t>
-        </is>
-      </c>
-      <c r="B18" s="9" t="inlineStr">
-        <is>
-          <t>19:00
-Sunday</t>
-        </is>
-      </c>
-      <c r="C18" s="15" t="inlineStr">
+      <c r="F16" s="12" t="inlineStr">
+        <is>
+          <t>Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" ht="48.2" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A17" s="32" t="inlineStr">
+        <is>
+          <t>EUTERM</t>
+        </is>
+      </c>
+      <c r="B17" s="9" t="inlineStr">
+        <is>
+          <t>18:15
+Daily</t>
+        </is>
+      </c>
+      <c r="C17" s="10" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
-      <c r="D18" s="15" t="inlineStr">
+      <c r="D17" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.EUTRM.F.GPD.DMP : last exported on 20.05.22
 DEL.N1LN3L.EUTRM.F.GPL.DMP : last exported on 20.05.22
@@ -1570,6 +1545,39 @@
 DEL.N1LN3L.EUTRM.F.CPL.DMP : last exported on 20.05.22</t>
         </is>
       </c>
+      <c r="E17" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F17" s="13" t="inlineStr">
+        <is>
+          <t>DryRun</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="36.75" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A18" s="32" t="inlineStr">
+        <is>
+          <t>Translations</t>
+        </is>
+      </c>
+      <c r="B18" s="9" t="inlineStr">
+        <is>
+          <t>19:00
+Sunday</t>
+        </is>
+      </c>
+      <c r="C18" s="15" t="inlineStr">
+        <is>
+          <t>DIT.E35KT6.TRANS.ZIP : last exported on 09.01.23</t>
+        </is>
+      </c>
+      <c r="D18" s="15" t="inlineStr">
+        <is>
+          <t>DEL.N1LE35.TRANS.ZIP : last exported on 31.12.23</t>
+        </is>
+      </c>
       <c r="E18" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
@@ -1595,43 +1603,10 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.TRANS.ZIP : last exported on 09.01.23</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 04.01.24</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
-        <is>
-          <t>DEL.N1LE35.TRANS.ZIP : last exported on 31.12.23</t>
-        </is>
-      </c>
-      <c r="E19" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F19" s="12" t="inlineStr">
-        <is>
-          <t>Successful</t>
-        </is>
-      </c>
-    </row>
-    <row r="20" ht="409.6" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A20" s="32" t="inlineStr">
-        <is>
-          <t>ELFI</t>
-        </is>
-      </c>
-      <c r="B20" s="9" t="inlineStr">
-        <is>
-          <t>20:25
-Daily</t>
-        </is>
-      </c>
-      <c r="C20" s="10" t="inlineStr">
-        <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 04.01.24</t>
-        </is>
-      </c>
-      <c r="D20" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 04.01.24
 DEL.N1LN3L.MT.F.GPL.DMP : last exported on 04.01.24
@@ -1662,33 +1637,30 @@
 DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 04.01.24</t>
         </is>
       </c>
-      <c r="E20" s="11" t="inlineStr">
+      <c r="E19" s="11" t="inlineStr">
         <is>
           <t>Ok</t>
         </is>
       </c>
-      <c r="F20" s="12" t="inlineStr">
+      <c r="F19" s="12" t="inlineStr">
         <is>
           <t>Successful</t>
         </is>
       </c>
     </row>
-    <row r="21" ht="16.5" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A21" s="5" t="n"/>
-      <c r="B21" s="6" t="n"/>
-      <c r="C21" s="4" t="inlineStr"/>
-      <c r="D21" s="4" t="inlineStr"/>
-      <c r="E21" s="2" t="n"/>
-      <c r="F21" s="3" t="n"/>
-    </row>
-    <row r="22" ht="19.5" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A22" s="32" t="inlineStr">
-        <is>
-          <t>DB server Disk Space Monitoring</t>
-        </is>
-      </c>
-      <c r="B22" s="27" t="n"/>
-      <c r="C22" s="14" t="inlineStr">
+    <row r="20" ht="409.6" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A20" s="32" t="inlineStr">
+        <is>
+          <t>ELFI</t>
+        </is>
+      </c>
+      <c r="B20" s="9" t="inlineStr">
+        <is>
+          <t>20:25
+Daily</t>
+        </is>
+      </c>
+      <c r="C20" s="10" t="inlineStr">
         <is>
           <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 05.01.24
 DKG.R11KT6.L520.P.EDCP.LEI : last exported on 05.01.24
@@ -1704,7 +1676,7 @@
 DDC.R11KT6.ELFI.PR.TXT : last exported on 31.12.23</t>
         </is>
       </c>
-      <c r="D22" s="4" t="inlineStr">
+      <c r="D20" s="10" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 04.01.24
 DEL.N1LN3L.EL.F.GPL.DMP : last exported on 04.01.24
@@ -1738,6 +1710,82 @@
 DEL.KT6N5X.EL.F.AU.ZIP : last exported on 04.01.24</t>
         </is>
       </c>
+      <c r="E20" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F20" s="12" t="inlineStr">
+        <is>
+          <t>Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="21" ht="16.5" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A21" s="5" t="n"/>
+      <c r="B21" s="6" t="n"/>
+      <c r="C21" s="4" t="inlineStr"/>
+      <c r="D21" s="4" t="inlineStr"/>
+      <c r="E21" s="2" t="n"/>
+      <c r="F21" s="3" t="n"/>
+    </row>
+    <row r="22" ht="19.5" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A22" s="32" t="inlineStr">
+        <is>
+          <t>DB server Disk Space Monitoring</t>
+        </is>
+      </c>
+      <c r="B22" s="27" t="n"/>
+      <c r="C22" s="14" t="inlineStr">
+        <is>
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 05.01.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 05.01.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 05.01.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 05.01.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 05.01.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 05.01.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 05.01.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 05.01.24
+DDC.R11KT6.ELFI.MD.TXT : last exported on 31.12.23
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 04.01.24
+DDC.R11KT6.ELFI.PK.TXT : last exported on 31.12.23
+DDC.R11KT6.ELFI.PR.TXT : last exported on 31.12.23</t>
+        </is>
+      </c>
+      <c r="D22" s="4" t="inlineStr">
+        <is>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 04.01.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 04.01.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 04.01.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 04.01.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 04.01.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 04.01.24
+DEL.N1LKT6.EC.??????.G : last exported on 04.01.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 04.01.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 04.01.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 04.01.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 04.01.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 04.01.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 04.01.24
+DEL.N1LKT6.EC.??????.U : last exported on 04.01.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 04.01.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 04.01.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 04.01.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 04.01.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 04.01.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 04.01.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 04.01.24
+DEL.N1LKT6.EC.??????.AS : last exported on 04.01.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 04.01.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 04.01.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 04.01.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 04.01.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 04.01.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 04.01.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 04.01.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 04.01.24</t>
+        </is>
+      </c>
       <c r="F22" s="3" t="n"/>
     </row>
     <row r="23" ht="15" customHeight="1" thickBot="1" thickTop="1">

</xml_diff>

<commit_message>
Updated on 08.01.24 12:44
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 05.01.2024</t>
+          <t>Date - 08.01.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 04.01.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 05.01.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 05.01.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 05.01.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 05.01.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 05.01.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 05.01.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 05.01.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 05.01.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 05.01.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 05.01.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 05.01.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 05.01.24</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 06.01.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 06.01.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 07.01.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 06.01.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 06.01.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 06.01.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 06.01.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 06.01.24
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 06.01.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 06.01.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 06.01.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1032,13 +1032,13 @@
       </c>
       <c r="C5" s="10" t="inlineStr">
         <is>
-          <t>DGQ.R11KT6.KDNR.TXT : last exported on 01.12.23</t>
+          <t>DGQ.R11KT6.KDNR.TXT : last exported on 05.01.24</t>
         </is>
       </c>
       <c r="D5" s="10" t="inlineStr">
         <is>
-          <t>DDS.N1LR11.KDNRTXT : last exported on 04.12.23
-DVL.N1LN5X.VLM.KDNRTXT : last exported on 04.12.23</t>
+          <t>DDS.N1LR11.KDNRTXT : last exported on 08.01.24
+DVL.N1LN5X.VLM.KDNRTXT : last exported on 08.01.24</t>
         </is>
       </c>
       <c r="E5" s="11" t="inlineStr">
@@ -1066,22 +1066,22 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 01.01.24
-DEH.N3LKT6.AP.COMPL.SNK : last exported on 01.01.24</t>
+          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 08.01.24
+DEH.N3LKT6.AP.COMPL.SNK : last exported on 08.01.24</t>
         </is>
       </c>
       <c r="D6" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 01.01.24
-DEL.N1LN3L.DN.F.GPL.DMP : last exported on 01.01.24
-DEL.N1LN3L.DN.F.GTR.DMP : last exported on 01.01.24
-DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 01.01.24
-DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 01.01.24
-DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 01.01.24
-DEL.N1LN0R.DN.F.CPD.DMP : last exported on 01.01.24
-DEL.N1LN0R.DN.F.CPL.DMP : last exported on 01.01.24
-DEL.KT6E35.SN.F.GGO.ZIP : last exported on 01.01.24
-DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 01.01.24</t>
+          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 08.01.24
+DEL.N1LN3L.DN.F.GPL.DMP : last exported on 08.01.24
+DEL.N1LN3L.DN.F.GTR.DMP : last exported on 08.01.24
+DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 08.01.24
+DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 08.01.24
+DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 08.01.24
+DEL.N1LN0R.DN.F.CPD.DMP : last exported on 08.01.24
+DEL.N1LN0R.DN.F.CPL.DMP : last exported on 08.01.24
+DEL.KT6E35.SN.F.GGO.ZIP : last exported on 08.01.24
+DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 08.01.24</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
@@ -1109,29 +1109,29 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 03.01.24
-DLV.KZ6KT6.WI.V.ZIP : last exported on 03.01.24
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 05.01.24
+DLV.KZ6KT6.WI.V.ZIP : last exported on 07.01.24
 DLV.RPKKT6.WI.S.ZIP : last exported on 15.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 04.01.24
+DLV.I5XKT6.WI.A.ZIP : last exported on 05.01.24
 DIT.E35KT6.WI.ZIP : last exported on 04.01.24
-DEL.K2PKT6.WI.ZIP : last exported on 04.01.24
+DEL.K2PKT6.WI.ZIP : last exported on 07.01.24
 DEL.R7AKT6.WI.ZIP : last exported on 14.12.23
-DEL.N5FKT6.WI.ZIP : last exported on 04.01.24</t>
+DEL.N5FKT6.WI.ZIP : last exported on 05.01.24</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 05.01.24
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 05.01.24
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 05.01.24
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 05.01.24
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 05.01.24
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 05.01.24
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 05.01.24
-DEL.KT6E35.WI.GGO.ZIP : last exported on 05.01.24
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 05.01.24
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 05.01.24
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 05.01.24</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 08.01.24
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 08.01.24
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 08.01.24
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 08.01.24
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 08.01.24
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 08.01.24
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 08.01.24
+DEL.KT6E35.WI.GGO.ZIP : last exported on 08.01.24
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 08.01.24
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 08.01.24
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 08.01.24</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 05.01.24
+DEL.N3LKT6.HST.??????.ZIP : last exported on 08.01.24
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 01.01.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 04.01.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 04.01.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 04.01.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 04.01.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 04.01.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 04.01.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 04.01.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 04.01.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 04.01.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 04.01.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 04.01.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 04.01.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 04.01.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 04.01.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 04.01.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 04.01.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 04.01.24</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 07.01.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 07.01.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 07.01.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 07.01.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 07.01.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 07.01.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 07.01.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 07.01.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 07.01.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 07.01.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 07.01.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 07.01.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 07.01.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 07.01.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 07.01.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 07.01.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 07.01.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 04.01.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 07.01.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1324,12 +1324,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 04.01.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 05.01.24</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 04.01.24</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 06.01.24</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="C13" s="10" t="inlineStr">
         <is>
-          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 30.12.23
+          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 06.01.24
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
 DLV.I5XKT6.AU.A.ZIP : last exported on 13.12.23
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
@@ -1367,7 +1367,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 04.01.24
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 07.01.24
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 04.01.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 04.01.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 07.01.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 07.01.24</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 04.01.24
-DHP.KUDKT6.ORGUNITS : last exported on 05.01.24
-DHS.R11KT6.HSB02ALL : last exported on 04.01.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 07.01.24
+DHP.KUDKT6.ORGUNITS : last exported on 08.01.24
+DHS.R11KT6.HSB02ALL : last exported on 05.01.24</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 04.01.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 04.01.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 04.01.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 04.01.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 04.01.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 04.01.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 04.01.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 04.01.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 04.01.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 04.01.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 05.01.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 05.01.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 07.01.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 05.01.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 05.01.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 05.01.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 05.01.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 05.01.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 05.01.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 05.01.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1575,7 +1575,7 @@
       </c>
       <c r="D18" s="15" t="inlineStr">
         <is>
-          <t>DEL.N1LE35.TRANS.ZIP : last exported on 31.12.23</t>
+          <t>DEL.N1LE35.TRANS.ZIP : last exported on 07.01.24</t>
         </is>
       </c>
       <c r="E18" s="11" t="inlineStr">
@@ -1603,38 +1603,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 04.01.24</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 06.01.24</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 04.01.24
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 04.01.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 04.01.24
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 04.01.24
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 04.01.24
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 04.01.24
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 04.01.24
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 04.01.24
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 04.01.24
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 04.01.24
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 04.01.24
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 04.01.24
-DEL.N1LKT6.MT.??????.G : last exported on 04.01.24
-DEL.N1LKT6.MT.??????.U : last exported on 04.01.24
-DEL.N1LKT6.MT.??????.AS : last exported on 04.01.24
-DVL.N1LN5X.VLM.DSP : last exported on 04.01.24
-DVL.N1LN5X.VLM.WT : last exported on 04.01.24
-DDS.N1LR11.DSP : last exported on 04.01.24
-DDS.N1LR11.WT : last exported on 04.01.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 04.01.24
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 04.01.24
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 04.01.24
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 04.01.24
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 04.01.24
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 04.01.24
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 04.01.24
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 04.01.24</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 06.01.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 06.01.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 07.01.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 06.01.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 06.01.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 06.01.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 06.01.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 06.01.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 06.01.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 06.01.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 06.01.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 06.01.24
+DEL.N1LKT6.MT.??????.G : last exported on 06.01.24
+DEL.N1LKT6.MT.??????.U : last exported on 06.01.24
+DEL.N1LKT6.MT.??????.AS : last exported on 06.01.24
+DVL.N1LN5X.VLM.DSP : last exported on 06.01.24
+DVL.N1LN5X.VLM.WT : last exported on 06.01.24
+DDS.N1LR11.DSP : last exported on 06.01.24
+DDS.N1LR11.WT : last exported on 06.01.24
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 06.01.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 06.01.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 06.01.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 06.01.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 06.01.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 06.01.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 06.01.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 06.01.24</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1661,6 +1661,82 @@
         </is>
       </c>
       <c r="C20" s="10" t="inlineStr">
+        <is>
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 08.01.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 08.01.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 08.01.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 08.01.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 08.01.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 08.01.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 08.01.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 08.01.24
+DDC.R11KT6.ELFI.MD.TXT : last exported on 07.01.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 05.01.24
+DDC.R11KT6.ELFI.PK.TXT : last exported on 07.01.24
+DDC.R11KT6.ELFI.PR.TXT : last exported on 07.01.24</t>
+        </is>
+      </c>
+      <c r="D20" s="10" t="inlineStr">
+        <is>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 07.01.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 07.01.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 07.01.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 07.01.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 07.01.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 07.01.24
+DEL.N1LKT6.EC.??????.G : last exported on 07.01.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 07.01.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 07.01.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 07.01.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 07.01.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 07.01.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 07.01.24
+DEL.N1LKT6.EC.??????.U : last exported on 07.01.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 07.01.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 07.01.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 07.01.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 07.01.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 07.01.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 07.01.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 07.01.24
+DEL.N1LKT6.EC.??????.AS : last exported on 07.01.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 07.01.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 07.01.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 07.01.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 07.01.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 07.01.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 07.01.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 07.01.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 07.01.24</t>
+        </is>
+      </c>
+      <c r="E20" s="11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="F20" s="12" t="inlineStr">
+        <is>
+          <t>Successful</t>
+        </is>
+      </c>
+    </row>
+    <row r="21" ht="16.5" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A21" s="5" t="n"/>
+      <c r="B21" s="6" t="n"/>
+      <c r="C21" s="4" t="inlineStr"/>
+      <c r="D21" s="4" t="inlineStr"/>
+      <c r="E21" s="2" t="n"/>
+      <c r="F21" s="3" t="n"/>
+    </row>
+    <row r="22" ht="19.5" customHeight="1" thickBot="1" thickTop="1">
+      <c r="A22" s="32" t="inlineStr">
+        <is>
+          <t>DB server Disk Space Monitoring</t>
+        </is>
+      </c>
+      <c r="B22" s="27" t="n"/>
+      <c r="C22" s="14" t="inlineStr">
         <is>
           <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 05.01.24
 DKG.R11KT6.L520.P.EDCP.LEI : last exported on 05.01.24
@@ -1676,7 +1752,7 @@
 DDC.R11KT6.ELFI.PR.TXT : last exported on 31.12.23</t>
         </is>
       </c>
-      <c r="D20" s="10" t="inlineStr">
+      <c r="D22" s="4" t="inlineStr">
         <is>
           <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 04.01.24
 DEL.N1LN3L.EL.F.GPL.DMP : last exported on 04.01.24
@@ -1710,82 +1786,6 @@
 DEL.KT6N5X.EL.F.AU.ZIP : last exported on 04.01.24</t>
         </is>
       </c>
-      <c r="E20" s="11" t="inlineStr">
-        <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="F20" s="12" t="inlineStr">
-        <is>
-          <t>Successful</t>
-        </is>
-      </c>
-    </row>
-    <row r="21" ht="16.5" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A21" s="5" t="n"/>
-      <c r="B21" s="6" t="n"/>
-      <c r="C21" s="4" t="inlineStr"/>
-      <c r="D21" s="4" t="inlineStr"/>
-      <c r="E21" s="2" t="n"/>
-      <c r="F21" s="3" t="n"/>
-    </row>
-    <row r="22" ht="19.5" customHeight="1" thickBot="1" thickTop="1">
-      <c r="A22" s="32" t="inlineStr">
-        <is>
-          <t>DB server Disk Space Monitoring</t>
-        </is>
-      </c>
-      <c r="B22" s="27" t="n"/>
-      <c r="C22" s="14" t="inlineStr">
-        <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 05.01.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 05.01.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 05.01.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 05.01.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 05.01.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 05.01.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 05.01.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 05.01.24
-DDC.R11KT6.ELFI.MD.TXT : last exported on 31.12.23
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 04.01.24
-DDC.R11KT6.ELFI.PK.TXT : last exported on 31.12.23
-DDC.R11KT6.ELFI.PR.TXT : last exported on 31.12.23</t>
-        </is>
-      </c>
-      <c r="D22" s="4" t="inlineStr">
-        <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 04.01.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 04.01.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 04.01.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 04.01.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 04.01.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 04.01.24
-DEL.N1LKT6.EC.??????.G : last exported on 04.01.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 04.01.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 04.01.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 04.01.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 04.01.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 04.01.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 04.01.24
-DEL.N1LKT6.EC.??????.U : last exported on 04.01.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 04.01.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 04.01.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 04.01.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 04.01.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 04.01.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 04.01.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 04.01.24
-DEL.N1LKT6.EC.??????.AS : last exported on 04.01.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 04.01.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 04.01.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 04.01.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 04.01.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 04.01.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 04.01.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 04.01.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 04.01.24</t>
-        </is>
-      </c>
       <c r="F22" s="3" t="n"/>
     </row>
     <row r="23" ht="15" customHeight="1" thickBot="1" thickTop="1">

</xml_diff>

<commit_message>
Updated on 09.01.24 13:22
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 08.01.2024</t>
+          <t>Date - 09.01.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 05.01.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 08.01.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 06.01.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 06.01.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 07.01.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 06.01.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 06.01.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 06.01.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 06.01.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 06.01.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 06.01.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 06.01.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 06.01.24</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 09.01.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 09.01.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 09.01.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 09.01.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 09.01.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 09.01.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 09.01.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 09.01.24
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 09.01.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 09.01.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 09.01.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1109,29 +1109,29 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 05.01.24
-DLV.KZ6KT6.WI.V.ZIP : last exported on 07.01.24
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 08.01.24
+DLV.KZ6KT6.WI.V.ZIP : last exported on 08.01.24
 DLV.RPKKT6.WI.S.ZIP : last exported on 15.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 05.01.24
-DIT.E35KT6.WI.ZIP : last exported on 04.01.24
-DEL.K2PKT6.WI.ZIP : last exported on 07.01.24
+DLV.I5XKT6.WI.A.ZIP : last exported on 08.01.24
+DIT.E35KT6.WI.ZIP : last exported on 08.01.24
+DEL.K2PKT6.WI.ZIP : last exported on 08.01.24
 DEL.R7AKT6.WI.ZIP : last exported on 14.12.23
 DEL.N5FKT6.WI.ZIP : last exported on 05.01.24</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 08.01.24
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 08.01.24
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 08.01.24
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 08.01.24
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 08.01.24
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 08.01.24
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 08.01.24
-DEL.KT6E35.WI.GGO.ZIP : last exported on 08.01.24
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 08.01.24
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 08.01.24
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 08.01.24</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 09.01.24
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 09.01.24
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 09.01.24
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 09.01.24
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 09.01.24
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 09.01.24
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 09.01.24
+DEL.KT6E35.WI.GGO.ZIP : last exported on 09.01.24
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 09.01.24
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 09.01.24
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 09.01.24</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 08.01.24
-DGV.N3LKT6.EPELS.??????.ZIP : last exported on 01.01.24</t>
+DEL.N3LKT6.HST.??????.ZIP : last exported on 09.01.24
+DGV.N3LKT6.EPELS.??????.ZIP : last exported on 08.01.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 07.01.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 07.01.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 07.01.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 07.01.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 07.01.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 07.01.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 07.01.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 07.01.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 07.01.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 07.01.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 07.01.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 07.01.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 07.01.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 07.01.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 07.01.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 07.01.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 07.01.24</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 08.01.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 08.01.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 08.01.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 08.01.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 08.01.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 08.01.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 08.01.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 08.01.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 08.01.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 08.01.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 08.01.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 08.01.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 08.01.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 08.01.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 08.01.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 08.01.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 08.01.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 07.01.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 08.01.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1324,7 +1324,7 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 05.01.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 08.01.24</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
@@ -1367,7 +1367,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 07.01.24
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 08.01.24
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 07.01.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 07.01.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 08.01.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 08.01.24</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 07.01.24
-DHP.KUDKT6.ORGUNITS : last exported on 08.01.24
-DHS.R11KT6.HSB02ALL : last exported on 05.01.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 08.01.24
+DHP.KUDKT6.ORGUNITS : last exported on 09.01.24
+DHS.R11KT6.HSB02ALL : last exported on 08.01.24</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 05.01.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 05.01.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 07.01.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 05.01.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 05.01.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 05.01.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 05.01.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 05.01.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 05.01.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 05.01.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 08.01.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 08.01.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 08.01.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 08.01.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 08.01.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 08.01.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 08.01.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 08.01.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 08.01.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 08.01.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1610,7 +1610,7 @@
         <is>
           <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 06.01.24
 DEL.N1LN3L.MT.F.GPL.DMP : last exported on 06.01.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 07.01.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 08.01.24
 DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 06.01.24
 DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 06.01.24
 DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 06.01.24
@@ -1662,52 +1662,52 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 08.01.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 08.01.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 08.01.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 08.01.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 08.01.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 08.01.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 08.01.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 08.01.24
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 09.01.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 09.01.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 09.01.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 09.01.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 09.01.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 09.01.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 09.01.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 09.01.24
 DDC.R11KT6.ELFI.MD.TXT : last exported on 07.01.24
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 05.01.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 08.01.24
 DDC.R11KT6.ELFI.PK.TXT : last exported on 07.01.24
 DDC.R11KT6.ELFI.PR.TXT : last exported on 07.01.24</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 07.01.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 07.01.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 07.01.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 07.01.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 07.01.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 07.01.24
-DEL.N1LKT6.EC.??????.G : last exported on 07.01.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 07.01.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 07.01.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 07.01.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 07.01.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 07.01.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 07.01.24
-DEL.N1LKT6.EC.??????.U : last exported on 07.01.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 07.01.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 07.01.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 07.01.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 07.01.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 07.01.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 07.01.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 07.01.24
-DEL.N1LKT6.EC.??????.AS : last exported on 07.01.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 07.01.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 07.01.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 07.01.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 07.01.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 07.01.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 07.01.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 07.01.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 07.01.24</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 08.01.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 08.01.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 08.01.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 08.01.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 08.01.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 08.01.24
+DEL.N1LKT6.EC.??????.G : last exported on 08.01.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 08.01.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 08.01.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 08.01.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 08.01.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 08.01.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 08.01.24
+DEL.N1LKT6.EC.??????.U : last exported on 08.01.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 08.01.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 08.01.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 08.01.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 08.01.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 08.01.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 08.01.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 08.01.24
+DEL.N1LKT6.EC.??????.AS : last exported on 08.01.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 08.01.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 08.01.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 08.01.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 08.01.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 08.01.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 08.01.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 08.01.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 08.01.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 10.01.24 13:56
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 09.01.2024</t>
+          <t>Date - 10.01.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 08.01.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 09.01.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 09.01.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 09.01.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 09.01.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 09.01.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 09.01.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 09.01.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 09.01.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 09.01.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 09.01.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 09.01.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 09.01.24</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 10.01.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 10.01.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 10.01.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 10.01.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 10.01.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 10.01.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 10.01.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 10.01.24
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 10.01.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 10.01.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 10.01.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1109,12 +1109,12 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 08.01.24
-DLV.KZ6KT6.WI.V.ZIP : last exported on 08.01.24
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 09.01.24
+DLV.KZ6KT6.WI.V.ZIP : last exported on 09.01.24
 DLV.RPKKT6.WI.S.ZIP : last exported on 15.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 08.01.24
-DIT.E35KT6.WI.ZIP : last exported on 08.01.24
-DEL.K2PKT6.WI.ZIP : last exported on 08.01.24
+DLV.I5XKT6.WI.A.ZIP : last exported on 09.01.24
+DIT.E35KT6.WI.ZIP : last exported on 09.01.24
+DEL.K2PKT6.WI.ZIP : last exported on 09.01.24
 DEL.R7AKT6.WI.ZIP : last exported on 14.12.23
 DEL.N5FKT6.WI.ZIP : last exported on 05.01.24</t>
         </is>
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 09.01.24
+DEL.N3LKT6.HST.??????.ZIP : last exported on 10.01.24
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 08.01.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 08.01.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 08.01.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 08.01.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 08.01.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 08.01.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 08.01.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 08.01.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 08.01.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 08.01.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 08.01.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 08.01.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 08.01.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 08.01.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 08.01.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 08.01.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 08.01.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 08.01.24</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 09.01.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 09.01.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 09.01.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 09.01.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 09.01.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 09.01.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 09.01.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 09.01.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 09.01.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 09.01.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 09.01.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 09.01.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 09.01.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 09.01.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 09.01.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 09.01.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 09.01.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 08.01.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 09.01.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1324,12 +1324,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 08.01.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 09.01.24</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 06.01.24</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 09.01.24</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="C13" s="10" t="inlineStr">
         <is>
-          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 06.01.24
+          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 09.01.24
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
 DLV.I5XKT6.AU.A.ZIP : last exported on 13.12.23
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
@@ -1367,7 +1367,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 08.01.24
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 09.01.24
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 08.01.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 08.01.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 09.01.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 09.01.24</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 08.01.24
-DHP.KUDKT6.ORGUNITS : last exported on 09.01.24
-DHS.R11KT6.HSB02ALL : last exported on 08.01.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 09.01.24
+DHP.KUDKT6.ORGUNITS : last exported on 10.01.24
+DHS.R11KT6.HSB02ALL : last exported on 09.01.24</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 08.01.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 08.01.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 08.01.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 08.01.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 08.01.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 08.01.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 08.01.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 08.01.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 08.01.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 08.01.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 09.01.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 09.01.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 09.01.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 09.01.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 09.01.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 09.01.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 09.01.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 09.01.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 09.01.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 09.01.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1603,38 +1603,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 06.01.24</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 09.01.24</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 06.01.24
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 06.01.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 08.01.24
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 06.01.24
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 06.01.24
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 06.01.24
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 06.01.24
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 06.01.24
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 06.01.24
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 06.01.24
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 06.01.24
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 06.01.24
-DEL.N1LKT6.MT.??????.G : last exported on 06.01.24
-DEL.N1LKT6.MT.??????.U : last exported on 06.01.24
-DEL.N1LKT6.MT.??????.AS : last exported on 06.01.24
-DVL.N1LN5X.VLM.DSP : last exported on 06.01.24
-DVL.N1LN5X.VLM.WT : last exported on 06.01.24
-DDS.N1LR11.DSP : last exported on 06.01.24
-DDS.N1LR11.WT : last exported on 06.01.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 06.01.24
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 06.01.24
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 06.01.24
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 06.01.24
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 06.01.24
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 06.01.24
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 06.01.24
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 06.01.24</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 09.01.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 09.01.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 09.01.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 09.01.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 09.01.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 09.01.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 09.01.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 09.01.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 09.01.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 09.01.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 09.01.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 09.01.24
+DEL.N1LKT6.MT.??????.G : last exported on 09.01.24
+DEL.N1LKT6.MT.??????.U : last exported on 09.01.24
+DEL.N1LKT6.MT.??????.AS : last exported on 09.01.24
+DVL.N1LN5X.VLM.DSP : last exported on 09.01.24
+DVL.N1LN5X.VLM.WT : last exported on 09.01.24
+DDS.N1LR11.DSP : last exported on 09.01.24
+DDS.N1LR11.WT : last exported on 09.01.24
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 09.01.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 09.01.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 09.01.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 09.01.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 09.01.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 09.01.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 09.01.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 09.01.24</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,52 +1662,52 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 09.01.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 09.01.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 09.01.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 09.01.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 09.01.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 09.01.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 09.01.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 09.01.24
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 10.01.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 10.01.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 10.01.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 10.01.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 10.01.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 10.01.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 10.01.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 10.01.24
 DDC.R11KT6.ELFI.MD.TXT : last exported on 07.01.24
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 08.01.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 09.01.24
 DDC.R11KT6.ELFI.PK.TXT : last exported on 07.01.24
 DDC.R11KT6.ELFI.PR.TXT : last exported on 07.01.24</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 08.01.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 08.01.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 08.01.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 08.01.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 08.01.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 08.01.24
-DEL.N1LKT6.EC.??????.G : last exported on 08.01.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 08.01.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 08.01.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 08.01.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 08.01.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 08.01.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 08.01.24
-DEL.N1LKT6.EC.??????.U : last exported on 08.01.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 08.01.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 08.01.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 08.01.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 08.01.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 08.01.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 08.01.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 08.01.24
-DEL.N1LKT6.EC.??????.AS : last exported on 08.01.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 08.01.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 08.01.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 08.01.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 08.01.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 08.01.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 08.01.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 08.01.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 08.01.24</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 09.01.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 09.01.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 09.01.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 09.01.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 09.01.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 09.01.24
+DEL.N1LKT6.EC.??????.G : last exported on 09.01.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 09.01.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 09.01.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 09.01.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 09.01.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 09.01.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 09.01.24
+DEL.N1LKT6.EC.??????.U : last exported on 09.01.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 09.01.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 09.01.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 09.01.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 09.01.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 09.01.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 09.01.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 09.01.24
+DEL.N1LKT6.EC.??????.AS : last exported on 09.01.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 09.01.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 09.01.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 09.01.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 09.01.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 09.01.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 09.01.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 09.01.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 09.01.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 11.01.24 15:26
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 10.01.2024</t>
+          <t>Date - 11.01.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 09.01.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 10.01.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 10.01.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 10.01.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 10.01.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 10.01.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 10.01.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 10.01.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 10.01.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 10.01.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 10.01.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 10.01.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 10.01.24</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 11.01.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 11.01.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 11.01.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 11.01.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 11.01.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 11.01.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 11.01.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 11.01.24
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 11.01.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 11.01.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 11.01.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1109,29 +1109,29 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 09.01.24
-DLV.KZ6KT6.WI.V.ZIP : last exported on 09.01.24
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 10.01.24
+DLV.KZ6KT6.WI.V.ZIP : last exported on 10.01.24
 DLV.RPKKT6.WI.S.ZIP : last exported on 15.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 09.01.24
-DIT.E35KT6.WI.ZIP : last exported on 09.01.24
-DEL.K2PKT6.WI.ZIP : last exported on 09.01.24
+DLV.I5XKT6.WI.A.ZIP : last exported on 10.01.24
+DIT.E35KT6.WI.ZIP : last exported on 10.01.24
+DEL.K2PKT6.WI.ZIP : last exported on 10.01.24
 DEL.R7AKT6.WI.ZIP : last exported on 14.12.23
 DEL.N5FKT6.WI.ZIP : last exported on 05.01.24</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 09.01.24
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 09.01.24
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 09.01.24
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 09.01.24
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 09.01.24
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 09.01.24
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 09.01.24
-DEL.KT6E35.WI.GGO.ZIP : last exported on 09.01.24
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 09.01.24
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 09.01.24
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 09.01.24</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 10.01.24
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 10.01.24
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 10.01.24
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 10.01.24
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 10.01.24
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 10.01.24
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 10.01.24
+DEL.KT6E35.WI.GGO.ZIP : last exported on 10.01.24
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 10.01.24
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 10.01.24
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 10.01.24</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 10.01.24
+DEL.N3LKT6.HST.??????.ZIP : last exported on 11.01.24
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 08.01.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 09.01.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 09.01.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 09.01.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 09.01.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 09.01.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 09.01.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 09.01.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 09.01.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 09.01.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 09.01.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 09.01.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 09.01.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 09.01.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 09.01.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 09.01.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 09.01.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 09.01.24</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 10.01.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 10.01.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 10.01.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 10.01.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 10.01.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 10.01.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 10.01.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 10.01.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 10.01.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 10.01.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 10.01.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 10.01.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 10.01.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 10.01.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 10.01.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 10.01.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 10.01.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 09.01.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 10.01.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1324,12 +1324,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 09.01.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 10.01.24</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 09.01.24</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 10.01.24</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="C13" s="10" t="inlineStr">
         <is>
-          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 09.01.24
+          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 10.01.24
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
 DLV.I5XKT6.AU.A.ZIP : last exported on 13.12.23
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
@@ -1367,7 +1367,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 09.01.24
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 10.01.24
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
@@ -1409,25 +1409,25 @@
 DGQ.R11KT6.BSITX.TXT : last exported on 06.12.23
 DGQ.R31KT6.BSIVMC.TXT : last exported on 12.12.23
 DGQ.R31KT6.PKATC.TXT : last exported on 12.12.23
-DEL.KMPKT6.APOS.DATA.ZIP : last exported on 03.01.24</t>
+DEL.KMPKT6.APOS.DATA.ZIP : last exported on 10.01.24</t>
         </is>
       </c>
       <c r="D14" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 03.01.24
-DEL.N1LN3L.AP.F.GPL.DMP : last exported on 03.01.24
-DEL.N1LN3L.AP.F.GTR.DMP : last exported on 03.01.24
-DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 03.01.24
-DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 03.01.24
-DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 03.01.24
-DEL.N1LN0R.AP.F.CPD.DMP : last exported on 03.01.24
-DEL.N1LN0R.AP.F.CPL.DMP : last exported on 03.01.24
-DEL.N1LR31.AP.F.PPS.DMP : last exported on 03.01.24
-DEL.KT6E35.AP.F.DB.ZIP : last exported on 03.01.24
-DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 03.01.24
-DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 03.01.24
-DVL.KT6N5X.VLM.AP.ZIP : last exported on 03.01.24
-DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 03.01.24</t>
+          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 10.01.24
+DEL.N1LN3L.AP.F.GPL.DMP : last exported on 10.01.24
+DEL.N1LN3L.AP.F.GTR.DMP : last exported on 10.01.24
+DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 10.01.24
+DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 10.01.24
+DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 10.01.24
+DEL.N1LN0R.AP.F.CPD.DMP : last exported on 10.01.24
+DEL.N1LN0R.AP.F.CPL.DMP : last exported on 10.01.24
+DEL.N1LR31.AP.F.PPS.DMP : last exported on 10.01.24
+DEL.KT6E35.AP.F.DB.ZIP : last exported on 10.01.24
+DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 10.01.24
+DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 10.01.24
+DVL.KT6N5X.VLM.AP.ZIP : last exported on 10.01.24
+DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 10.01.24</t>
         </is>
       </c>
       <c r="E14" s="11" t="inlineStr">
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 09.01.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 09.01.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 10.01.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 10.01.24</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 09.01.24
-DHP.KUDKT6.ORGUNITS : last exported on 10.01.24
-DHS.R11KT6.HSB02ALL : last exported on 09.01.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 10.01.24
+DHP.KUDKT6.ORGUNITS : last exported on 11.01.24
+DHS.R11KT6.HSB02ALL : last exported on 10.01.24</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 09.01.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 09.01.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 09.01.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 09.01.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 09.01.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 09.01.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 09.01.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 09.01.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 09.01.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 09.01.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 10.01.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 10.01.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 10.01.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 10.01.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 10.01.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 10.01.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 10.01.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 10.01.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 10.01.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 10.01.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1610,7 +1610,7 @@
         <is>
           <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 09.01.24
 DEL.N1LN3L.MT.F.GPL.DMP : last exported on 09.01.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 09.01.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 10.01.24
 DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 09.01.24
 DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 09.01.24
 DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 09.01.24
@@ -1662,52 +1662,52 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 10.01.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 10.01.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 10.01.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 10.01.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 10.01.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 10.01.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 10.01.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 10.01.24
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 11.01.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 11.01.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 11.01.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 11.01.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 11.01.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 11.01.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 11.01.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 11.01.24
 DDC.R11KT6.ELFI.MD.TXT : last exported on 07.01.24
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 09.01.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 10.01.24
 DDC.R11KT6.ELFI.PK.TXT : last exported on 07.01.24
 DDC.R11KT6.ELFI.PR.TXT : last exported on 07.01.24</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 09.01.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 09.01.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 09.01.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 09.01.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 09.01.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 09.01.24
-DEL.N1LKT6.EC.??????.G : last exported on 09.01.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 09.01.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 09.01.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 09.01.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 09.01.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 09.01.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 09.01.24
-DEL.N1LKT6.EC.??????.U : last exported on 09.01.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 09.01.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 09.01.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 09.01.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 09.01.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 09.01.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 09.01.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 09.01.24
-DEL.N1LKT6.EC.??????.AS : last exported on 09.01.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 09.01.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 09.01.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 09.01.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 09.01.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 09.01.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 09.01.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 09.01.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 09.01.24</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 10.01.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 10.01.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 10.01.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 10.01.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 10.01.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 10.01.24
+DEL.N1LKT6.EC.??????.G : last exported on 10.01.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 10.01.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 10.01.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 10.01.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 10.01.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 10.01.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 10.01.24
+DEL.N1LKT6.EC.??????.U : last exported on 10.01.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 10.01.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 10.01.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 10.01.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 10.01.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 10.01.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 10.01.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 10.01.24
+DEL.N1LKT6.EC.??????.AS : last exported on 10.01.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 10.01.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 10.01.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 10.01.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 10.01.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 10.01.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 10.01.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 10.01.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 10.01.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 12.01.24 12:57
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 11.01.2024</t>
+          <t>Date - 12.01.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 10.01.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 11.01.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 11.01.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 11.01.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 11.01.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 11.01.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 11.01.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 11.01.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 11.01.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 11.01.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 11.01.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 11.01.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 11.01.24</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 12.01.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 12.01.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 12.01.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 12.01.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 12.01.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 12.01.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 12.01.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 12.01.24
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 12.01.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 12.01.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 12.01.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1109,29 +1109,29 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 10.01.24
-DLV.KZ6KT6.WI.V.ZIP : last exported on 10.01.24
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 11.01.24
+DLV.KZ6KT6.WI.V.ZIP : last exported on 11.01.24
 DLV.RPKKT6.WI.S.ZIP : last exported on 15.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 10.01.24
-DIT.E35KT6.WI.ZIP : last exported on 10.01.24
-DEL.K2PKT6.WI.ZIP : last exported on 10.01.24
+DLV.I5XKT6.WI.A.ZIP : last exported on 11.01.24
+DIT.E35KT6.WI.ZIP : last exported on 11.01.24
+DEL.K2PKT6.WI.ZIP : last exported on 11.01.24
 DEL.R7AKT6.WI.ZIP : last exported on 14.12.23
-DEL.N5FKT6.WI.ZIP : last exported on 05.01.24</t>
+DEL.N5FKT6.WI.ZIP : last exported on 11.01.24</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 10.01.24
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 10.01.24
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 10.01.24
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 10.01.24
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 10.01.24
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 10.01.24
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 10.01.24
-DEL.KT6E35.WI.GGO.ZIP : last exported on 10.01.24
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 10.01.24
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 10.01.24
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 10.01.24</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 11.01.24
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 11.01.24
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 11.01.24
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 11.01.24
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 11.01.24
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 11.01.24
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 11.01.24
+DEL.KT6E35.WI.GGO.ZIP : last exported on 11.01.24
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 11.01.24
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 11.01.24
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 11.01.24</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 11.01.24
+DEL.N3LKT6.HST.??????.ZIP : last exported on 12.01.24
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 08.01.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 10.01.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 10.01.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 10.01.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 10.01.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 10.01.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 10.01.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 10.01.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 10.01.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 10.01.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 10.01.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 10.01.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 10.01.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 10.01.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 10.01.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 10.01.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 10.01.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 10.01.24</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 11.01.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 11.01.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 11.01.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 11.01.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 11.01.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 11.01.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 11.01.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 11.01.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 11.01.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 11.01.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 11.01.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 11.01.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 11.01.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 11.01.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 11.01.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 11.01.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 11.01.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 10.01.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 11.01.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1324,12 +1324,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 10.01.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 11.01.24</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 10.01.24</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 11.01.24</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="C13" s="10" t="inlineStr">
         <is>
-          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 10.01.24
+          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 11.01.24
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
 DLV.I5XKT6.AU.A.ZIP : last exported on 13.12.23
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
@@ -1367,7 +1367,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 10.01.24
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 11.01.24
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 10.01.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 10.01.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 11.01.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 11.01.24</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 10.01.24
-DHP.KUDKT6.ORGUNITS : last exported on 11.01.24
-DHS.R11KT6.HSB02ALL : last exported on 10.01.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 11.01.24
+DHP.KUDKT6.ORGUNITS : last exported on 12.01.24
+DHS.R11KT6.HSB02ALL : last exported on 11.01.24</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 10.01.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 10.01.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 10.01.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 10.01.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 10.01.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 10.01.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 10.01.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 10.01.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 10.01.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 10.01.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 11.01.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 11.01.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 11.01.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 11.01.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 11.01.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 11.01.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 11.01.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 11.01.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 11.01.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 11.01.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1603,38 +1603,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 09.01.24</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 11.01.24</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 09.01.24
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 09.01.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 10.01.24
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 09.01.24
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 09.01.24
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 09.01.24
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 09.01.24
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 09.01.24
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 09.01.24
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 09.01.24
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 09.01.24
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 09.01.24
-DEL.N1LKT6.MT.??????.G : last exported on 09.01.24
-DEL.N1LKT6.MT.??????.U : last exported on 09.01.24
-DEL.N1LKT6.MT.??????.AS : last exported on 09.01.24
-DVL.N1LN5X.VLM.DSP : last exported on 09.01.24
-DVL.N1LN5X.VLM.WT : last exported on 09.01.24
-DDS.N1LR11.DSP : last exported on 09.01.24
-DDS.N1LR11.WT : last exported on 09.01.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 09.01.24
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 09.01.24
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 09.01.24
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 09.01.24
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 09.01.24
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 09.01.24
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 09.01.24
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 09.01.24</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 11.01.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 11.01.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 11.01.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 11.01.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 11.01.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 11.01.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 11.01.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 11.01.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 11.01.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 11.01.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 11.01.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 11.01.24
+DEL.N1LKT6.MT.??????.G : last exported on 11.01.24
+DEL.N1LKT6.MT.??????.U : last exported on 11.01.24
+DEL.N1LKT6.MT.??????.AS : last exported on 11.01.24
+DVL.N1LN5X.VLM.DSP : last exported on 11.01.24
+DVL.N1LN5X.VLM.WT : last exported on 11.01.24
+DDS.N1LR11.DSP : last exported on 11.01.24
+DDS.N1LR11.WT : last exported on 11.01.24
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 11.01.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 11.01.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 11.01.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 11.01.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 11.01.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 11.01.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 11.01.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 11.01.24</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,52 +1662,52 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 11.01.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 11.01.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 11.01.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 11.01.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 11.01.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 11.01.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 11.01.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 11.01.24
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 12.01.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 12.01.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 12.01.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 12.01.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 12.01.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 12.01.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 12.01.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 12.01.24
 DDC.R11KT6.ELFI.MD.TXT : last exported on 07.01.24
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 10.01.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 11.01.24
 DDC.R11KT6.ELFI.PK.TXT : last exported on 07.01.24
 DDC.R11KT6.ELFI.PR.TXT : last exported on 07.01.24</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 10.01.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 10.01.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 10.01.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 10.01.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 10.01.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 10.01.24
-DEL.N1LKT6.EC.??????.G : last exported on 10.01.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 10.01.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 10.01.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 10.01.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 10.01.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 10.01.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 10.01.24
-DEL.N1LKT6.EC.??????.U : last exported on 10.01.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 10.01.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 10.01.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 10.01.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 10.01.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 10.01.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 10.01.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 10.01.24
-DEL.N1LKT6.EC.??????.AS : last exported on 10.01.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 10.01.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 10.01.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 10.01.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 10.01.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 10.01.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 10.01.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 10.01.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 10.01.24</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 11.01.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 11.01.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 11.01.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 11.01.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 11.01.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 11.01.24
+DEL.N1LKT6.EC.??????.G : last exported on 11.01.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 11.01.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 11.01.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 11.01.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 11.01.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 11.01.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 11.01.24
+DEL.N1LKT6.EC.??????.U : last exported on 11.01.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 11.01.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 11.01.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 11.01.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 11.01.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 11.01.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 11.01.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 11.01.24
+DEL.N1LKT6.EC.??????.AS : last exported on 11.01.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 11.01.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 11.01.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 11.01.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 11.01.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 11.01.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 11.01.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 11.01.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 11.01.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 15.01.24 13:39
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 12.01.2024</t>
+          <t>Date - 15.01.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 11.01.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 12.01.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 12.01.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 12.01.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 12.01.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 12.01.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 12.01.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 12.01.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 12.01.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 12.01.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 12.01.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 12.01.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 12.01.24</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 13.01.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 13.01.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 14.01.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 13.01.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 13.01.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 13.01.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 13.01.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 13.01.24
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 13.01.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 13.01.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 13.01.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1066,22 +1066,22 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 08.01.24
-DEH.N3LKT6.AP.COMPL.SNK : last exported on 08.01.24</t>
+          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 15.01.24
+DEH.N3LKT6.AP.COMPL.SNK : last exported on 15.01.24</t>
         </is>
       </c>
       <c r="D6" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 08.01.24
-DEL.N1LN3L.DN.F.GPL.DMP : last exported on 08.01.24
-DEL.N1LN3L.DN.F.GTR.DMP : last exported on 08.01.24
-DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 08.01.24
-DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 08.01.24
-DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 08.01.24
-DEL.N1LN0R.DN.F.CPD.DMP : last exported on 08.01.24
-DEL.N1LN0R.DN.F.CPL.DMP : last exported on 08.01.24
-DEL.KT6E35.SN.F.GGO.ZIP : last exported on 08.01.24
-DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 08.01.24</t>
+          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 15.01.24
+DEL.N1LN3L.DN.F.GPL.DMP : last exported on 15.01.24
+DEL.N1LN3L.DN.F.GTR.DMP : last exported on 15.01.24
+DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 15.01.24
+DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 15.01.24
+DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 15.01.24
+DEL.N1LN0R.DN.F.CPD.DMP : last exported on 15.01.24
+DEL.N1LN0R.DN.F.CPL.DMP : last exported on 15.01.24
+DEL.KT6E35.SN.F.GGO.ZIP : last exported on 15.01.24
+DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 15.01.24</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
@@ -1110,28 +1110,28 @@
       <c r="C7" s="10" t="inlineStr">
         <is>
           <t>DLV.R31KT6.WI.C.ZIP : last exported on 11.01.24
-DLV.KZ6KT6.WI.V.ZIP : last exported on 11.01.24
+DLV.KZ6KT6.WI.V.ZIP : last exported on 14.01.24
 DLV.RPKKT6.WI.S.ZIP : last exported on 15.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 11.01.24
-DIT.E35KT6.WI.ZIP : last exported on 11.01.24
-DEL.K2PKT6.WI.ZIP : last exported on 11.01.24
+DLV.I5XKT6.WI.A.ZIP : last exported on 14.01.24
+DIT.E35KT6.WI.ZIP : last exported on 12.01.24
+DEL.K2PKT6.WI.ZIP : last exported on 14.01.24
 DEL.R7AKT6.WI.ZIP : last exported on 14.12.23
-DEL.N5FKT6.WI.ZIP : last exported on 11.01.24</t>
+DEL.N5FKT6.WI.ZIP : last exported on 12.01.24</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 11.01.24
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 11.01.24
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 11.01.24
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 11.01.24
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 11.01.24
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 11.01.24
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 11.01.24
-DEL.KT6E35.WI.GGO.ZIP : last exported on 11.01.24
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 11.01.24
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 11.01.24
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 11.01.24</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 15.01.24
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 15.01.24
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 15.01.24
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 15.01.24
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 15.01.24
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 15.01.24
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 15.01.24
+DEL.KT6E35.WI.GGO.ZIP : last exported on 15.01.24
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 15.01.24
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 15.01.24
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 15.01.24</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 12.01.24
+DEL.N3LKT6.HST.??????.ZIP : last exported on 15.01.24
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 08.01.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 11.01.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 11.01.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 11.01.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 11.01.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 11.01.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 11.01.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 11.01.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 11.01.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 11.01.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 11.01.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 11.01.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 11.01.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 11.01.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 11.01.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 11.01.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 11.01.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 11.01.24</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 14.01.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 14.01.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 14.01.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 14.01.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 14.01.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 14.01.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 14.01.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 14.01.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 14.01.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 14.01.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 14.01.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 14.01.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 14.01.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 14.01.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 14.01.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 14.01.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 14.01.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 11.01.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 14.01.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1324,12 +1324,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 11.01.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 12.01.24</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 11.01.24</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 13.01.24</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1357,9 +1357,9 @@
       </c>
       <c r="C13" s="10" t="inlineStr">
         <is>
-          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 11.01.24
+          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 13.01.24
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
-DLV.I5XKT6.AU.A.ZIP : last exported on 13.12.23
+DLV.I5XKT6.AU.A.ZIP : last exported on 12.01.24
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
         </is>
       </c>
@@ -1367,7 +1367,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 11.01.24
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 14.01.24
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 11.01.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 11.01.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 14.01.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 14.01.24</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 11.01.24
-DHP.KUDKT6.ORGUNITS : last exported on 12.01.24
-DHS.R11KT6.HSB02ALL : last exported on 11.01.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 14.01.24
+DHP.KUDKT6.ORGUNITS : last exported on 15.01.24
+DHS.R11KT6.HSB02ALL : last exported on 12.01.24</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 11.01.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 11.01.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 11.01.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 11.01.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 11.01.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 11.01.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 11.01.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 11.01.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 11.01.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 11.01.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 12.01.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 12.01.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 14.01.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 12.01.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 12.01.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 12.01.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 12.01.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 12.01.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 12.01.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 12.01.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1570,12 +1570,12 @@
       </c>
       <c r="C18" s="15" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.TRANS.ZIP : last exported on 09.01.23</t>
+          <t>DIT.E35KT6.TRANS.ZIP : last exported on 12.01.24</t>
         </is>
       </c>
       <c r="D18" s="15" t="inlineStr">
         <is>
-          <t>DEL.N1LE35.TRANS.ZIP : last exported on 07.01.24</t>
+          <t>DEL.N1LE35.TRANS.ZIP : last exported on 14.01.24</t>
         </is>
       </c>
       <c r="E18" s="11" t="inlineStr">
@@ -1603,38 +1603,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 11.01.24</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 13.01.24</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 11.01.24
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 11.01.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 11.01.24
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 11.01.24
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 11.01.24
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 11.01.24
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 11.01.24
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 11.01.24
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 11.01.24
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 11.01.24
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 11.01.24
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 11.01.24
-DEL.N1LKT6.MT.??????.G : last exported on 11.01.24
-DEL.N1LKT6.MT.??????.U : last exported on 11.01.24
-DEL.N1LKT6.MT.??????.AS : last exported on 11.01.24
-DVL.N1LN5X.VLM.DSP : last exported on 11.01.24
-DVL.N1LN5X.VLM.WT : last exported on 11.01.24
-DDS.N1LR11.DSP : last exported on 11.01.24
-DDS.N1LR11.WT : last exported on 11.01.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 11.01.24
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 11.01.24
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 11.01.24
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 11.01.24
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 11.01.24
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 11.01.24
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 11.01.24
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 11.01.24</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 13.01.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 13.01.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 14.01.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 13.01.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 13.01.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 13.01.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 13.01.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 13.01.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 13.01.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 13.01.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 13.01.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 13.01.24
+DEL.N1LKT6.MT.??????.G : last exported on 13.01.24
+DEL.N1LKT6.MT.??????.U : last exported on 13.01.24
+DEL.N1LKT6.MT.??????.AS : last exported on 13.01.24
+DVL.N1LN5X.VLM.DSP : last exported on 13.01.24
+DVL.N1LN5X.VLM.WT : last exported on 13.01.24
+DDS.N1LR11.DSP : last exported on 13.01.24
+DDS.N1LR11.WT : last exported on 13.01.24
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 13.01.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 13.01.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 13.01.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 13.01.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 13.01.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 13.01.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 13.01.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 13.01.24</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,52 +1662,52 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 12.01.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 12.01.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 12.01.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 12.01.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 12.01.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 12.01.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 12.01.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 12.01.24
-DDC.R11KT6.ELFI.MD.TXT : last exported on 07.01.24
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 11.01.24
-DDC.R11KT6.ELFI.PK.TXT : last exported on 07.01.24
-DDC.R11KT6.ELFI.PR.TXT : last exported on 07.01.24</t>
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 15.01.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 15.01.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 15.01.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 15.01.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 15.01.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 15.01.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 15.01.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 15.01.24
+DDC.R11KT6.ELFI.MD.TXT : last exported on 14.01.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 12.01.24
+DDC.R11KT6.ELFI.PK.TXT : last exported on 14.01.24
+DDC.R11KT6.ELFI.PR.TXT : last exported on 14.01.24</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 11.01.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 11.01.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 11.01.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 11.01.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 11.01.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 11.01.24
-DEL.N1LKT6.EC.??????.G : last exported on 11.01.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 11.01.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 11.01.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 11.01.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 11.01.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 11.01.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 11.01.24
-DEL.N1LKT6.EC.??????.U : last exported on 11.01.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 11.01.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 11.01.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 11.01.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 11.01.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 11.01.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 11.01.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 11.01.24
-DEL.N1LKT6.EC.??????.AS : last exported on 11.01.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 11.01.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 11.01.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 11.01.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 11.01.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 11.01.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 11.01.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 11.01.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 11.01.24</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 14.01.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 14.01.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 14.01.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 14.01.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 14.01.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 14.01.24
+DEL.N1LKT6.EC.??????.G : last exported on 14.01.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 14.01.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 14.01.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 14.01.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 14.01.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 14.01.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 14.01.24
+DEL.N1LKT6.EC.??????.U : last exported on 14.01.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 14.01.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 14.01.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 14.01.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 14.01.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 14.01.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 14.01.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 14.01.24
+DEL.N1LKT6.EC.??????.AS : last exported on 14.01.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 14.01.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 14.01.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 14.01.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 14.01.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 14.01.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 14.01.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 14.01.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 14.01.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 16.01.24 12:05
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 15.01.2024</t>
+          <t>Date - 16.01.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 12.01.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 15.01.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 13.01.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 13.01.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 14.01.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 13.01.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 13.01.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 13.01.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 13.01.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 13.01.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 13.01.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 13.01.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 13.01.24</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 16.01.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 16.01.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 16.01.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 16.01.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 16.01.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 16.01.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 16.01.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 16.01.24
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 16.01.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 16.01.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 16.01.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1110,11 +1110,11 @@
       <c r="C7" s="10" t="inlineStr">
         <is>
           <t>DLV.R31KT6.WI.C.ZIP : last exported on 11.01.24
-DLV.KZ6KT6.WI.V.ZIP : last exported on 14.01.24
+DLV.KZ6KT6.WI.V.ZIP : last exported on 15.01.24
 DLV.RPKKT6.WI.S.ZIP : last exported on 15.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 14.01.24
-DIT.E35KT6.WI.ZIP : last exported on 12.01.24
-DEL.K2PKT6.WI.ZIP : last exported on 14.01.24
+DLV.I5XKT6.WI.A.ZIP : last exported on 15.01.24
+DIT.E35KT6.WI.ZIP : last exported on 15.01.24
+DEL.K2PKT6.WI.ZIP : last exported on 15.01.24
 DEL.R7AKT6.WI.ZIP : last exported on 14.12.23
 DEL.N5FKT6.WI.ZIP : last exported on 12.01.24</t>
         </is>
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 15.01.24
-DGV.N3LKT6.EPELS.??????.ZIP : last exported on 08.01.24</t>
+DEL.N3LKT6.HST.??????.ZIP : last exported on 16.01.24
+DGV.N3LKT6.EPELS.??????.ZIP : last exported on 15.01.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 14.01.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 14.01.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 14.01.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 14.01.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 14.01.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 14.01.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 14.01.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 14.01.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 14.01.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 14.01.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 14.01.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 14.01.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 14.01.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 14.01.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 14.01.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 14.01.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 14.01.24</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 15.01.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 15.01.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 15.01.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 15.01.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 15.01.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 15.01.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 15.01.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 15.01.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 15.01.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 15.01.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 15.01.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 15.01.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 15.01.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 15.01.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 15.01.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 15.01.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 15.01.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 14.01.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 15.01.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1324,7 +1324,7 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 12.01.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 15.01.24</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
@@ -1367,7 +1367,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 14.01.24
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 15.01.24
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 14.01.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 14.01.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 15.01.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 15.01.24</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 14.01.24
-DHP.KUDKT6.ORGUNITS : last exported on 15.01.24
-DHS.R11KT6.HSB02ALL : last exported on 12.01.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 15.01.24
+DHP.KUDKT6.ORGUNITS : last exported on 16.01.24
+DHS.R11KT6.HSB02ALL : last exported on 15.01.24</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 12.01.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 12.01.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 14.01.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 12.01.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 12.01.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 12.01.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 12.01.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 12.01.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 12.01.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 12.01.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 15.01.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 15.01.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 15.01.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 15.01.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 15.01.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 15.01.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 15.01.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 15.01.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 15.01.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 15.01.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1603,38 +1603,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 13.01.24</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 15.01.24</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 13.01.24
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 13.01.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 14.01.24
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 13.01.24
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 13.01.24
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 13.01.24
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 13.01.24
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 13.01.24
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 13.01.24
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 13.01.24
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 13.01.24
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 13.01.24
-DEL.N1LKT6.MT.??????.G : last exported on 13.01.24
-DEL.N1LKT6.MT.??????.U : last exported on 13.01.24
-DEL.N1LKT6.MT.??????.AS : last exported on 13.01.24
-DVL.N1LN5X.VLM.DSP : last exported on 13.01.24
-DVL.N1LN5X.VLM.WT : last exported on 13.01.24
-DDS.N1LR11.DSP : last exported on 13.01.24
-DDS.N1LR11.WT : last exported on 13.01.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 13.01.24
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 13.01.24
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 13.01.24
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 13.01.24
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 13.01.24
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 13.01.24
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 13.01.24
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 13.01.24</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 15.01.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 15.01.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 15.01.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 15.01.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 15.01.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 15.01.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 15.01.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 15.01.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 15.01.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 15.01.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 15.01.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 15.01.24
+DEL.N1LKT6.MT.??????.G : last exported on 15.01.24
+DEL.N1LKT6.MT.??????.U : last exported on 15.01.24
+DEL.N1LKT6.MT.??????.AS : last exported on 15.01.24
+DVL.N1LN5X.VLM.DSP : last exported on 15.01.24
+DVL.N1LN5X.VLM.WT : last exported on 15.01.24
+DDS.N1LR11.DSP : last exported on 15.01.24
+DDS.N1LR11.WT : last exported on 15.01.24
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 15.01.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 15.01.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 15.01.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 15.01.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 15.01.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 15.01.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 15.01.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 15.01.24</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,52 +1662,52 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 15.01.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 15.01.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 15.01.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 15.01.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 15.01.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 15.01.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 15.01.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 15.01.24
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 16.01.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 16.01.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 16.01.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 16.01.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 16.01.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 16.01.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 16.01.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 16.01.24
 DDC.R11KT6.ELFI.MD.TXT : last exported on 14.01.24
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 12.01.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 15.01.24
 DDC.R11KT6.ELFI.PK.TXT : last exported on 14.01.24
 DDC.R11KT6.ELFI.PR.TXT : last exported on 14.01.24</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 14.01.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 14.01.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 14.01.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 14.01.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 14.01.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 14.01.24
-DEL.N1LKT6.EC.??????.G : last exported on 14.01.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 14.01.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 14.01.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 14.01.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 14.01.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 14.01.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 14.01.24
-DEL.N1LKT6.EC.??????.U : last exported on 14.01.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 14.01.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 14.01.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 14.01.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 14.01.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 14.01.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 14.01.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 14.01.24
-DEL.N1LKT6.EC.??????.AS : last exported on 14.01.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 14.01.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 14.01.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 14.01.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 14.01.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 14.01.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 14.01.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 14.01.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 14.01.24</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 15.01.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 15.01.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 15.01.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 15.01.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 15.01.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 15.01.24
+DEL.N1LKT6.EC.??????.G : last exported on 15.01.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 15.01.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 15.01.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 15.01.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 15.01.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 15.01.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 15.01.24
+DEL.N1LKT6.EC.??????.U : last exported on 15.01.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 15.01.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 15.01.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 15.01.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 15.01.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 15.01.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 15.01.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 15.01.24
+DEL.N1LKT6.EC.??????.AS : last exported on 15.01.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 15.01.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 15.01.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 15.01.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 15.01.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 15.01.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 15.01.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 15.01.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 15.01.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 17.01.24 11:55
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 16.01.2024</t>
+          <t>Date - 17.01.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 15.01.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 16.01.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 16.01.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 16.01.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 16.01.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 16.01.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 16.01.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 16.01.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 16.01.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 16.01.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 16.01.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 16.01.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 16.01.24</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 17.01.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 17.01.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 17.01.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 17.01.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 17.01.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 17.01.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 17.01.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 17.01.24
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 17.01.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 17.01.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 17.01.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1110,28 +1110,28 @@
       <c r="C7" s="10" t="inlineStr">
         <is>
           <t>DLV.R31KT6.WI.C.ZIP : last exported on 11.01.24
-DLV.KZ6KT6.WI.V.ZIP : last exported on 15.01.24
+DLV.KZ6KT6.WI.V.ZIP : last exported on 16.01.24
 DLV.RPKKT6.WI.S.ZIP : last exported on 15.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 15.01.24
+DLV.I5XKT6.WI.A.ZIP : last exported on 16.01.24
 DIT.E35KT6.WI.ZIP : last exported on 15.01.24
-DEL.K2PKT6.WI.ZIP : last exported on 15.01.24
+DEL.K2PKT6.WI.ZIP : last exported on 16.01.24
 DEL.R7AKT6.WI.ZIP : last exported on 14.12.23
 DEL.N5FKT6.WI.ZIP : last exported on 12.01.24</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 15.01.24
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 15.01.24
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 15.01.24
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 15.01.24
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 15.01.24
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 15.01.24
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 15.01.24
-DEL.KT6E35.WI.GGO.ZIP : last exported on 15.01.24
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 15.01.24
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 15.01.24
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 15.01.24</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 16.01.24
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 16.01.24
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 16.01.24
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 16.01.24
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 16.01.24
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 16.01.24
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 16.01.24
+DEL.KT6E35.WI.GGO.ZIP : last exported on 16.01.24
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 16.01.24
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 16.01.24
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 16.01.24</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 16.01.24
+DEL.N3LKT6.HST.??????.ZIP : last exported on 17.01.24
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 15.01.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 15.01.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 15.01.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 15.01.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 15.01.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 15.01.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 15.01.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 15.01.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 15.01.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 15.01.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 15.01.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 15.01.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 15.01.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 15.01.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 15.01.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 15.01.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 15.01.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 15.01.24</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 16.01.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 16.01.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 16.01.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 16.01.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 16.01.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 16.01.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 16.01.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 16.01.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 16.01.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 16.01.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 16.01.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 16.01.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 16.01.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 16.01.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 16.01.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 16.01.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 16.01.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 15.01.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 16.01.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1324,12 +1324,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 15.01.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 16.01.24</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 13.01.24</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 16.01.24</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="C13" s="10" t="inlineStr">
         <is>
-          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 13.01.24
+          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 16.01.24
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
 DLV.I5XKT6.AU.A.ZIP : last exported on 12.01.24
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
@@ -1367,7 +1367,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 15.01.24
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 16.01.24
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 15.01.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 15.01.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 16.01.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 16.01.24</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 15.01.24
-DHP.KUDKT6.ORGUNITS : last exported on 16.01.24
-DHS.R11KT6.HSB02ALL : last exported on 15.01.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 16.01.24
+DHP.KUDKT6.ORGUNITS : last exported on 17.01.24
+DHS.R11KT6.HSB02ALL : last exported on 16.01.24</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 15.01.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 15.01.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 15.01.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 15.01.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 15.01.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 15.01.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 15.01.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 15.01.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 15.01.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 15.01.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 16.01.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 16.01.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 16.01.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 16.01.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 16.01.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 16.01.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 16.01.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 16.01.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 16.01.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 16.01.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1603,38 +1603,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 15.01.24</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 16.01.24</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 15.01.24
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 15.01.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 15.01.24
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 15.01.24
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 15.01.24
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 15.01.24
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 15.01.24
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 15.01.24
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 15.01.24
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 15.01.24
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 15.01.24
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 15.01.24
-DEL.N1LKT6.MT.??????.G : last exported on 15.01.24
-DEL.N1LKT6.MT.??????.U : last exported on 15.01.24
-DEL.N1LKT6.MT.??????.AS : last exported on 15.01.24
-DVL.N1LN5X.VLM.DSP : last exported on 15.01.24
-DVL.N1LN5X.VLM.WT : last exported on 15.01.24
-DDS.N1LR11.DSP : last exported on 15.01.24
-DDS.N1LR11.WT : last exported on 15.01.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 15.01.24
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 15.01.24
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 15.01.24
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 15.01.24
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 15.01.24
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 15.01.24
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 15.01.24
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 15.01.24</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 16.01.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 16.01.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 16.01.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 16.01.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 16.01.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 16.01.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 16.01.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 16.01.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 16.01.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 16.01.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 16.01.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 16.01.24
+DEL.N1LKT6.MT.??????.G : last exported on 16.01.24
+DEL.N1LKT6.MT.??????.U : last exported on 16.01.24
+DEL.N1LKT6.MT.??????.AS : last exported on 16.01.24
+DVL.N1LN5X.VLM.DSP : last exported on 16.01.24
+DVL.N1LN5X.VLM.WT : last exported on 16.01.24
+DDS.N1LR11.DSP : last exported on 16.01.24
+DDS.N1LR11.WT : last exported on 16.01.24
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 16.01.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 16.01.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 16.01.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 16.01.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 16.01.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 16.01.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 16.01.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 16.01.24</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,16 +1662,16 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 16.01.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 16.01.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 16.01.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 16.01.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 16.01.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 16.01.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 16.01.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 16.01.24
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 17.01.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 17.01.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 17.01.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 17.01.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 17.01.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 17.01.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 17.01.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 17.01.24
 DDC.R11KT6.ELFI.MD.TXT : last exported on 14.01.24
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 15.01.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 16.01.24
 DDC.R11KT6.ELFI.PK.TXT : last exported on 14.01.24
 DDC.R11KT6.ELFI.PR.TXT : last exported on 14.01.24</t>
         </is>
@@ -1700,14 +1700,14 @@
 DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 15.01.24
 DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 15.01.24
 DEL.N1LKT6.EC.??????.AS : last exported on 15.01.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 15.01.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 15.01.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 15.01.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 15.01.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 15.01.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 15.01.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 17.01.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 17.01.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 17.01.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 17.01.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 17.01.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 17.01.24
 DEL.KT6KT6.EL.F.DRE.CSV : last exported on 15.01.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 15.01.24</t>
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 17.01.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 18.01.24 11:45
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 17.01.2024</t>
+          <t>Date - 18.01.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -994,14 +994,14 @@
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 17.01.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 17.01.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 17.01.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 17.01.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 17.01.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 17.01.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 17.01.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 17.01.24
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 18.01.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 18.01.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 18.01.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 18.01.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 18.01.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 18.01.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 18.01.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 18.01.24
 DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 17.01.24
 DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 17.01.24
 DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 17.01.24</t>
@@ -1121,13 +1121,13 @@
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 16.01.24
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 16.01.24
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 16.01.24
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 16.01.24
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 16.01.24
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 16.01.24
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 16.01.24
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 17.01.24
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 17.01.24
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 17.01.24
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 17.01.24
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 17.01.24
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 17.01.24
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 17.01.24
 DEL.KT6E35.WI.GGO.ZIP : last exported on 16.01.24
 DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 16.01.24
 DEL.KT6N5M.WI.GGO.ZIP : last exported on 16.01.24
@@ -1241,14 +1241,14 @@
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 16.01.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 16.01.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 16.01.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 16.01.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 16.01.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 16.01.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 16.01.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 16.01.24
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 17.01.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 17.01.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 17.01.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 17.01.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 17.01.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 17.01.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 17.01.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 17.01.24
 DEL.KT6E35.TP.D.GGO.ZIP : last exported on 16.01.24
 DEL.KT6E35.TP.D.UGO.ZIP : last exported on 16.01.24
 DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 16.01.24
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 16.01.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 17.01.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1367,7 +1367,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 16.01.24
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 17.01.24
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
@@ -1409,20 +1409,20 @@
 DGQ.R11KT6.BSITX.TXT : last exported on 06.12.23
 DGQ.R31KT6.BSIVMC.TXT : last exported on 12.12.23
 DGQ.R31KT6.PKATC.TXT : last exported on 12.12.23
-DEL.KMPKT6.APOS.DATA.ZIP : last exported on 10.01.24</t>
+DEL.KMPKT6.APOS.DATA.ZIP : last exported on 17.01.24</t>
         </is>
       </c>
       <c r="D14" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 10.01.24
-DEL.N1LN3L.AP.F.GPL.DMP : last exported on 10.01.24
-DEL.N1LN3L.AP.F.GTR.DMP : last exported on 10.01.24
-DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 10.01.24
-DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 10.01.24
-DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 10.01.24
-DEL.N1LN0R.AP.F.CPD.DMP : last exported on 10.01.24
-DEL.N1LN0R.AP.F.CPL.DMP : last exported on 10.01.24
-DEL.N1LR31.AP.F.PPS.DMP : last exported on 10.01.24
+          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 17.01.24
+DEL.N1LN3L.AP.F.GPL.DMP : last exported on 17.01.24
+DEL.N1LN3L.AP.F.GTR.DMP : last exported on 17.01.24
+DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 17.01.24
+DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 17.01.24
+DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 17.01.24
+DEL.N1LN0R.AP.F.CPD.DMP : last exported on 17.01.24
+DEL.N1LN0R.AP.F.CPL.DMP : last exported on 17.01.24
+DEL.N1LR31.AP.F.PPS.DMP : last exported on 17.01.24
 DEL.KT6E35.AP.F.DB.ZIP : last exported on 10.01.24
 DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 10.01.24
 DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 10.01.24
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 16.01.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 16.01.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 17.01.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 17.01.24</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1496,16 +1496,16 @@
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 16.01.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 16.01.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 16.01.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 16.01.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 16.01.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 16.01.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 16.01.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 16.01.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 16.01.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 16.01.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 17.01.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 17.01.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 17.01.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 17.01.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 17.01.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 17.01.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 17.01.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 17.01.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 17.01.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 17.01.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1608,25 +1608,25 @@
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 16.01.24
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 16.01.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 16.01.24
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 16.01.24
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 16.01.24
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 16.01.24
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 16.01.24
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 16.01.24
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 16.01.24
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 16.01.24
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 16.01.24
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 16.01.24
-DEL.N1LKT6.MT.??????.G : last exported on 16.01.24
-DEL.N1LKT6.MT.??????.U : last exported on 16.01.24
-DEL.N1LKT6.MT.??????.AS : last exported on 16.01.24
-DVL.N1LN5X.VLM.DSP : last exported on 16.01.24
-DVL.N1LN5X.VLM.WT : last exported on 16.01.24
-DDS.N1LR11.DSP : last exported on 16.01.24
-DDS.N1LR11.WT : last exported on 16.01.24
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 17.01.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 17.01.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 17.01.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 17.01.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 17.01.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 17.01.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 17.01.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 17.01.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 17.01.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 17.01.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 17.01.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 17.01.24
+DEL.N1LKT6.MT.??????.G : last exported on 17.01.24
+DEL.N1LKT6.MT.??????.U : last exported on 17.01.24
+DEL.N1LKT6.MT.??????.AS : last exported on 17.01.24
+DVL.N1LN5X.VLM.DSP : last exported on 17.01.24
+DVL.N1LN5X.VLM.WT : last exported on 17.01.24
+DDS.N1LR11.DSP : last exported on 17.01.24
+DDS.N1LR11.WT : last exported on 17.01.24
 DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 16.01.24
 DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 16.01.24
 DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 16.01.24
@@ -1678,35 +1678,35 @@
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 15.01.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 15.01.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 15.01.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 15.01.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 15.01.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 15.01.24
-DEL.N1LKT6.EC.??????.G : last exported on 15.01.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 15.01.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 15.01.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 15.01.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 15.01.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 15.01.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 15.01.24
-DEL.N1LKT6.EC.??????.U : last exported on 15.01.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 15.01.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 15.01.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 15.01.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 15.01.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 15.01.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 15.01.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 15.01.24
-DEL.N1LKT6.EC.??????.AS : last exported on 15.01.24
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 17.01.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 17.01.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 17.01.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 17.01.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 17.01.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 17.01.24
+DEL.N1LKT6.EC.??????.G : last exported on 17.01.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 17.01.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 17.01.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 17.01.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 17.01.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 17.01.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 17.01.24
+DEL.N1LKT6.EC.??????.U : last exported on 17.01.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 17.01.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 17.01.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 17.01.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 17.01.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 17.01.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 17.01.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 17.01.24
+DEL.N1LKT6.EC.??????.AS : last exported on 17.01.24
 DEL.N1LN3L.EL.F.GTR.DMP : last exported on 17.01.24
 DGV.N1LR31.EL.F.HST.ZIP : last exported on 17.01.24
 DGV.N1LN3L.EL.F.HST.ZIP : last exported on 17.01.24
 DGV.N1LCEN.EL.F.ZIP : last exported on 17.01.24
 DGV.N1LN7K.EL.F.ZIP : last exported on 17.01.24
 DGV.N1LN5X.EL.F.ZIP : last exported on 17.01.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 15.01.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 17.01.24
 DEL.KT6N5X.EL.F.AU.ZIP : last exported on 17.01.24</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Updated on 18.01.24 13:12
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -1121,13 +1121,13 @@
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 17.01.24
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 17.01.24
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 17.01.24
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 17.01.24
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 17.01.24
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 17.01.24
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 17.01.24
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 18.01.24
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 18.01.24
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 18.01.24
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 18.01.24
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 18.01.24
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 18.01.24
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 18.01.24
 DEL.KT6E35.WI.GGO.ZIP : last exported on 16.01.24
 DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 16.01.24
 DEL.KT6N5M.WI.GGO.ZIP : last exported on 16.01.24

</xml_diff>

<commit_message>
Updated on 19.01.24 11:56
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 18.01.2024</t>
+          <t>Date - 19.01.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 16.01.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 18.01.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 18.01.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 18.01.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 18.01.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 18.01.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 18.01.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 18.01.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 18.01.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 18.01.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 17.01.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 17.01.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 17.01.24</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 19.01.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 19.01.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 19.01.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 19.01.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 19.01.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 19.01.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 19.01.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 19.01.24
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 19.01.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 19.01.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 19.01.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1109,12 +1109,12 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 11.01.24
-DLV.KZ6KT6.WI.V.ZIP : last exported on 16.01.24
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 18.01.24
+DLV.KZ6KT6.WI.V.ZIP : last exported on 18.01.24
 DLV.RPKKT6.WI.S.ZIP : last exported on 15.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 16.01.24
-DIT.E35KT6.WI.ZIP : last exported on 15.01.24
-DEL.K2PKT6.WI.ZIP : last exported on 16.01.24
+DLV.I5XKT6.WI.A.ZIP : last exported on 18.01.24
+DIT.E35KT6.WI.ZIP : last exported on 18.01.24
+DEL.K2PKT6.WI.ZIP : last exported on 18.01.24
 DEL.R7AKT6.WI.ZIP : last exported on 14.12.23
 DEL.N5FKT6.WI.ZIP : last exported on 12.01.24</t>
         </is>
@@ -1128,10 +1128,10 @@
 DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 18.01.24
 DEL.N1LN0R.WI.D.CPD.DMP : last exported on 18.01.24
 DEL.N1LN0R.WI.D.CPL.DMP : last exported on 18.01.24
-DEL.KT6E35.WI.GGO.ZIP : last exported on 16.01.24
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 16.01.24
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 16.01.24
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 16.01.24</t>
+DEL.KT6E35.WI.GGO.ZIP : last exported on 18.01.24
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 18.01.24
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 18.01.24
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 18.01.24</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 17.01.24
+DEL.N3LKT6.HST.??????.ZIP : last exported on 19.01.24
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 15.01.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 17.01.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 17.01.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 17.01.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 17.01.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 17.01.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 17.01.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 17.01.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 17.01.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 16.01.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 16.01.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 16.01.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 16.01.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 16.01.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 16.01.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 16.01.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 16.01.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 16.01.24</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 18.01.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 18.01.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 18.01.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 18.01.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 18.01.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 18.01.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 18.01.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 18.01.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 18.01.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 18.01.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 18.01.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 18.01.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 18.01.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 18.01.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 18.01.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 18.01.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 18.01.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 17.01.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 18.01.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1324,12 +1324,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 16.01.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 18.01.24</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 16.01.24</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 18.01.24</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="C13" s="10" t="inlineStr">
         <is>
-          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 16.01.24
+          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 18.01.24
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
 DLV.I5XKT6.AU.A.ZIP : last exported on 12.01.24
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
@@ -1367,7 +1367,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 17.01.24
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 18.01.24
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
@@ -1423,11 +1423,11 @@
 DEL.N1LN0R.AP.F.CPD.DMP : last exported on 17.01.24
 DEL.N1LN0R.AP.F.CPL.DMP : last exported on 17.01.24
 DEL.N1LR31.AP.F.PPS.DMP : last exported on 17.01.24
-DEL.KT6E35.AP.F.DB.ZIP : last exported on 10.01.24
-DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 10.01.24
-DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 10.01.24
-DVL.KT6N5X.VLM.AP.ZIP : last exported on 10.01.24
-DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 10.01.24</t>
+DEL.KT6E35.AP.F.DB.ZIP : last exported on 17.01.24
+DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 17.01.24
+DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 17.01.24
+DVL.KT6N5X.VLM.AP.ZIP : last exported on 17.01.24
+DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 17.01.24</t>
         </is>
       </c>
       <c r="E14" s="11" t="inlineStr">
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 17.01.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 17.01.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 18.01.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 18.01.24</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 16.01.24
-DHP.KUDKT6.ORGUNITS : last exported on 17.01.24
-DHS.R11KT6.HSB02ALL : last exported on 16.01.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 18.01.24
+DHP.KUDKT6.ORGUNITS : last exported on 19.01.24
+DHS.R11KT6.HSB02ALL : last exported on 18.01.24</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 17.01.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 17.01.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 17.01.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 17.01.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 17.01.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 17.01.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 17.01.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 17.01.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 17.01.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 17.01.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 18.01.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 18.01.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 18.01.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 18.01.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 18.01.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 18.01.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 18.01.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 18.01.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 18.01.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 18.01.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1603,38 +1603,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 16.01.24</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 18.01.24</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 17.01.24
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 17.01.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 17.01.24
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 17.01.24
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 17.01.24
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 17.01.24
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 17.01.24
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 17.01.24
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 17.01.24
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 17.01.24
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 17.01.24
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 17.01.24
-DEL.N1LKT6.MT.??????.G : last exported on 17.01.24
-DEL.N1LKT6.MT.??????.U : last exported on 17.01.24
-DEL.N1LKT6.MT.??????.AS : last exported on 17.01.24
-DVL.N1LN5X.VLM.DSP : last exported on 17.01.24
-DVL.N1LN5X.VLM.WT : last exported on 17.01.24
-DDS.N1LR11.DSP : last exported on 17.01.24
-DDS.N1LR11.WT : last exported on 17.01.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 16.01.24
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 16.01.24
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 16.01.24
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 16.01.24
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 16.01.24
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 16.01.24
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 16.01.24
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 16.01.24</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 18.01.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 18.01.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 18.01.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 18.01.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 18.01.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 18.01.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 18.01.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 18.01.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 18.01.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 18.01.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 18.01.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 18.01.24
+DEL.N1LKT6.MT.??????.G : last exported on 18.01.24
+DEL.N1LKT6.MT.??????.U : last exported on 18.01.24
+DEL.N1LKT6.MT.??????.AS : last exported on 18.01.24
+DVL.N1LN5X.VLM.DSP : last exported on 18.01.24
+DVL.N1LN5X.VLM.WT : last exported on 18.01.24
+DDS.N1LR11.DSP : last exported on 18.01.24
+DDS.N1LR11.WT : last exported on 18.01.24
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 18.01.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 18.01.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 18.01.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 18.01.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 18.01.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 18.01.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 18.01.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 18.01.24</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,52 +1662,52 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 17.01.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 17.01.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 17.01.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 17.01.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 17.01.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 17.01.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 17.01.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 17.01.24
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 19.01.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 19.01.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 19.01.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 19.01.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 19.01.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 19.01.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 19.01.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 19.01.24
 DDC.R11KT6.ELFI.MD.TXT : last exported on 14.01.24
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 16.01.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 18.01.24
 DDC.R11KT6.ELFI.PK.TXT : last exported on 14.01.24
 DDC.R11KT6.ELFI.PR.TXT : last exported on 14.01.24</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 17.01.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 17.01.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 17.01.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 17.01.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 17.01.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 17.01.24
-DEL.N1LKT6.EC.??????.G : last exported on 17.01.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 17.01.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 17.01.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 17.01.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 17.01.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 17.01.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 17.01.24
-DEL.N1LKT6.EC.??????.U : last exported on 17.01.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 17.01.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 17.01.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 17.01.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 17.01.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 17.01.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 17.01.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 17.01.24
-DEL.N1LKT6.EC.??????.AS : last exported on 17.01.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 17.01.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 17.01.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 17.01.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 17.01.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 17.01.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 17.01.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 17.01.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 17.01.24</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 18.01.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 18.01.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 18.01.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 18.01.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 18.01.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 18.01.24
+DEL.N1LKT6.EC.??????.G : last exported on 18.01.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 18.01.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 18.01.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 18.01.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 18.01.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 18.01.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 18.01.24
+DEL.N1LKT6.EC.??????.U : last exported on 18.01.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 18.01.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 18.01.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 18.01.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 18.01.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 18.01.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 18.01.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 18.01.24
+DEL.N1LKT6.EC.??????.AS : last exported on 18.01.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 18.01.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 18.01.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 18.01.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 18.01.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 18.01.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 18.01.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 18.01.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 18.01.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 22.01.24 12:09
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 19.01.2024</t>
+          <t>Date - 22.01.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -994,14 +994,14 @@
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 19.01.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 19.01.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 19.01.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 19.01.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 19.01.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 19.01.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 19.01.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 19.01.24
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 20.01.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 20.01.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 21.01.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 20.01.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 20.01.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 20.01.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 20.01.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 20.01.24
 DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 19.01.24
 DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 19.01.24
 DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 19.01.24</t>
@@ -1072,14 +1072,14 @@
       </c>
       <c r="D6" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 15.01.24
-DEL.N1LN3L.DN.F.GPL.DMP : last exported on 15.01.24
-DEL.N1LN3L.DN.F.GTR.DMP : last exported on 15.01.24
-DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 15.01.24
-DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 15.01.24
-DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 15.01.24
-DEL.N1LN0R.DN.F.CPD.DMP : last exported on 15.01.24
-DEL.N1LN0R.DN.F.CPL.DMP : last exported on 15.01.24
+          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 22.01.24
+DEL.N1LN3L.DN.F.GPL.DMP : last exported on 22.01.24
+DEL.N1LN3L.DN.F.GTR.DMP : last exported on 22.01.24
+DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 22.01.24
+DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 22.01.24
+DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 22.01.24
+DEL.N1LN0R.DN.F.CPD.DMP : last exported on 22.01.24
+DEL.N1LN0R.DN.F.CPL.DMP : last exported on 22.01.24
 DEL.KT6E35.SN.F.GGO.ZIP : last exported on 15.01.24
 DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 15.01.24</t>
         </is>
@@ -1121,13 +1121,13 @@
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 18.01.24
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 18.01.24
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 18.01.24
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 18.01.24
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 18.01.24
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 18.01.24
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 18.01.24
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 22.01.24
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 22.01.24
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 22.01.24
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 22.01.24
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 22.01.24
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 22.01.24
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 22.01.24
 DEL.KT6E35.WI.GGO.ZIP : last exported on 18.01.24
 DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 18.01.24
 DEL.KT6N5M.WI.GGO.ZIP : last exported on 18.01.24
@@ -1241,14 +1241,14 @@
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 18.01.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 18.01.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 18.01.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 18.01.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 18.01.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 18.01.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 18.01.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 18.01.24
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 21.01.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 21.01.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 21.01.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 21.01.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 21.01.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 21.01.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 21.01.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 21.01.24
 DEL.KT6E35.TP.D.GGO.ZIP : last exported on 18.01.24
 DEL.KT6E35.TP.D.UGO.ZIP : last exported on 18.01.24
 DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 18.01.24
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 18.01.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 21.01.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1367,7 +1367,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 18.01.24
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 21.01.24
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 18.01.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 18.01.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 21.01.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 21.01.24</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1496,16 +1496,16 @@
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 18.01.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 18.01.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 18.01.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 18.01.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 18.01.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 18.01.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 18.01.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 18.01.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 18.01.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 18.01.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 19.01.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 19.01.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 21.01.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 19.01.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 19.01.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 19.01.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 19.01.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 19.01.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 19.01.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 19.01.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1575,7 +1575,7 @@
       </c>
       <c r="D18" s="15" t="inlineStr">
         <is>
-          <t>DEL.N1LE35.TRANS.ZIP : last exported on 14.01.24</t>
+          <t>DEL.N1LE35.TRANS.ZIP : last exported on 21.01.24</t>
         </is>
       </c>
       <c r="E18" s="11" t="inlineStr">
@@ -1608,25 +1608,25 @@
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 18.01.24
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 18.01.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 18.01.24
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 18.01.24
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 18.01.24
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 18.01.24
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 18.01.24
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 18.01.24
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 18.01.24
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 18.01.24
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 18.01.24
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 18.01.24
-DEL.N1LKT6.MT.??????.G : last exported on 18.01.24
-DEL.N1LKT6.MT.??????.U : last exported on 18.01.24
-DEL.N1LKT6.MT.??????.AS : last exported on 18.01.24
-DVL.N1LN5X.VLM.DSP : last exported on 18.01.24
-DVL.N1LN5X.VLM.WT : last exported on 18.01.24
-DDS.N1LR11.DSP : last exported on 18.01.24
-DDS.N1LR11.WT : last exported on 18.01.24
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 20.01.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 20.01.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 21.01.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 20.01.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 20.01.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 20.01.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 20.01.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 20.01.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 20.01.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 20.01.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 20.01.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 20.01.24
+DEL.N1LKT6.MT.??????.G : last exported on 20.01.24
+DEL.N1LKT6.MT.??????.U : last exported on 20.01.24
+DEL.N1LKT6.MT.??????.AS : last exported on 20.01.24
+DVL.N1LN5X.VLM.DSP : last exported on 20.01.24
+DVL.N1LN5X.VLM.WT : last exported on 20.01.24
+DDS.N1LR11.DSP : last exported on 20.01.24
+DDS.N1LR11.WT : last exported on 20.01.24
 DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 18.01.24
 DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 18.01.24
 DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 18.01.24
@@ -1678,35 +1678,35 @@
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 18.01.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 18.01.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 18.01.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 18.01.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 18.01.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 18.01.24
-DEL.N1LKT6.EC.??????.G : last exported on 18.01.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 18.01.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 18.01.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 18.01.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 18.01.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 18.01.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 18.01.24
-DEL.N1LKT6.EC.??????.U : last exported on 18.01.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 18.01.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 18.01.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 18.01.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 18.01.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 18.01.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 18.01.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 18.01.24
-DEL.N1LKT6.EC.??????.AS : last exported on 18.01.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 18.01.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 18.01.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 18.01.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 18.01.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 18.01.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 18.01.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 18.01.24
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 21.01.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 21.01.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 21.01.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 21.01.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 21.01.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 21.01.24
+DEL.N1LKT6.EC.??????.G : last exported on 21.01.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 21.01.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 21.01.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 21.01.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 21.01.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 21.01.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 21.01.24
+DEL.N1LKT6.EC.??????.U : last exported on 21.01.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 21.01.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 21.01.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 21.01.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 21.01.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 21.01.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 21.01.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 21.01.24
+DEL.N1LKT6.EC.??????.AS : last exported on 21.01.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 21.01.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 21.01.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 21.01.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 21.01.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 21.01.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 21.01.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 21.01.24
 DEL.KT6N5X.EL.F.AU.ZIP : last exported on 18.01.24</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Updated on 22.01.24 12:42
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -989,7 +989,7 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 18.01.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 19.01.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
@@ -1002,9 +1002,9 @@
 DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 20.01.24
 DEL.N1LN0R.WD.D.CPD.DMP : last exported on 20.01.24
 DEL.N1LN0R.WD.D.CPL.DMP : last exported on 20.01.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 19.01.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 19.01.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 19.01.24</t>
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 20.01.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 20.01.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 20.01.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1066,8 +1066,8 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 15.01.24
-DEH.N3LKT6.AP.COMPL.SNK : last exported on 15.01.24</t>
+          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 22.01.24
+DEH.N3LKT6.AP.COMPL.SNK : last exported on 22.01.24</t>
         </is>
       </c>
       <c r="D6" s="10" t="inlineStr">
@@ -1080,8 +1080,8 @@
 DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 22.01.24
 DEL.N1LN0R.DN.F.CPD.DMP : last exported on 22.01.24
 DEL.N1LN0R.DN.F.CPL.DMP : last exported on 22.01.24
-DEL.KT6E35.SN.F.GGO.ZIP : last exported on 15.01.24
-DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 15.01.24</t>
+DEL.KT6E35.SN.F.GGO.ZIP : last exported on 22.01.24
+DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 22.01.24</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
@@ -1109,13 +1109,13 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 18.01.24
-DLV.KZ6KT6.WI.V.ZIP : last exported on 18.01.24
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 19.01.24
+DLV.KZ6KT6.WI.V.ZIP : last exported on 21.01.24
 DLV.RPKKT6.WI.S.ZIP : last exported on 15.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 18.01.24
-DIT.E35KT6.WI.ZIP : last exported on 18.01.24
-DEL.K2PKT6.WI.ZIP : last exported on 18.01.24
-DEL.R7AKT6.WI.ZIP : last exported on 14.12.23
+DLV.I5XKT6.WI.A.ZIP : last exported on 20.01.24
+DIT.E35KT6.WI.ZIP : last exported on 19.01.24
+DEL.K2PKT6.WI.ZIP : last exported on 21.01.24
+DEL.R7AKT6.WI.ZIP : last exported on 22.01.24
 DEL.N5FKT6.WI.ZIP : last exported on 12.01.24</t>
         </is>
       </c>
@@ -1128,10 +1128,10 @@
 DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 22.01.24
 DEL.N1LN0R.WI.D.CPD.DMP : last exported on 22.01.24
 DEL.N1LN0R.WI.D.CPL.DMP : last exported on 22.01.24
-DEL.KT6E35.WI.GGO.ZIP : last exported on 18.01.24
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 18.01.24
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 18.01.24
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 18.01.24</t>
+DEL.KT6E35.WI.GGO.ZIP : last exported on 22.01.24
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 22.01.24
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 22.01.24
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 22.01.24</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,7 +1235,7 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 19.01.24
+DEL.N3LKT6.HST.??????.ZIP : last exported on 22.01.24
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 15.01.24</t>
         </is>
       </c>
@@ -1249,15 +1249,15 @@
 DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 21.01.24
 DEL.N1LN0R.TP.D.CPD.DMP : last exported on 21.01.24
 DEL.N1LN0R.TP.D.CPL.DMP : last exported on 21.01.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 18.01.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 18.01.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 18.01.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 18.01.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 18.01.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 18.01.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 18.01.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 18.01.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 18.01.24</t>
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 21.01.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 21.01.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 21.01.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 21.01.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 21.01.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 21.01.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 21.01.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 21.01.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 21.01.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1324,12 +1324,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 18.01.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 19.01.24</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 18.01.24</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 20.01.24</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="C13" s="10" t="inlineStr">
         <is>
-          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 18.01.24
+          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 19.01.24
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
 DLV.I5XKT6.AU.A.ZIP : last exported on 12.01.24
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
@@ -1489,9 +1489,9 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 18.01.24
-DHP.KUDKT6.ORGUNITS : last exported on 19.01.24
-DHS.R11KT6.HSB02ALL : last exported on 18.01.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 21.01.24
+DHP.KUDKT6.ORGUNITS : last exported on 22.01.24
+DHS.R11KT6.HSB02ALL : last exported on 19.01.24</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
@@ -1603,7 +1603,7 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 18.01.24</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 20.01.24</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
@@ -1627,14 +1627,14 @@
 DVL.N1LN5X.VLM.WT : last exported on 20.01.24
 DDS.N1LR11.DSP : last exported on 20.01.24
 DDS.N1LR11.WT : last exported on 20.01.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 18.01.24
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 18.01.24
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 18.01.24
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 18.01.24
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 18.01.24
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 18.01.24
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 18.01.24
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 18.01.24</t>
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 20.01.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 20.01.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 20.01.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 20.01.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 20.01.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 20.01.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 20.01.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 20.01.24</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,18 +1662,18 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 19.01.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 19.01.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 19.01.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 19.01.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 19.01.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 19.01.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 19.01.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 19.01.24
-DDC.R11KT6.ELFI.MD.TXT : last exported on 14.01.24
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 18.01.24
-DDC.R11KT6.ELFI.PK.TXT : last exported on 14.01.24
-DDC.R11KT6.ELFI.PR.TXT : last exported on 14.01.24</t>
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 22.01.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 22.01.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 22.01.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 22.01.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 22.01.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 22.01.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 22.01.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 22.01.24
+DDC.R11KT6.ELFI.MD.TXT : last exported on 21.01.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 19.01.24
+DDC.R11KT6.ELFI.PK.TXT : last exported on 21.01.24
+DDC.R11KT6.ELFI.PR.TXT : last exported on 21.01.24</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
@@ -1707,7 +1707,7 @@
 DGV.N1LN7K.EL.F.ZIP : last exported on 21.01.24
 DGV.N1LN5X.EL.F.ZIP : last exported on 21.01.24
 DEL.KT6KT6.EL.F.DRE.CSV : last exported on 21.01.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 18.01.24</t>
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 21.01.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 25.01.24 13:56
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 22.01.2024</t>
+          <t>Date - 25.01.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 19.01.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 23.01.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 20.01.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 20.01.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 21.01.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 20.01.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 20.01.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 20.01.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 20.01.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 20.01.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 20.01.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 20.01.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 20.01.24</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 25.01.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 25.01.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 25.01.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 25.01.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 25.01.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 25.01.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 25.01.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 25.01.24
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 24.01.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 24.01.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 24.01.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1109,29 +1109,29 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 19.01.24
-DLV.KZ6KT6.WI.V.ZIP : last exported on 21.01.24
-DLV.RPKKT6.WI.S.ZIP : last exported on 15.12.23
-DLV.I5XKT6.WI.A.ZIP : last exported on 20.01.24
-DIT.E35KT6.WI.ZIP : last exported on 19.01.24
-DEL.K2PKT6.WI.ZIP : last exported on 21.01.24
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 23.01.24
+DLV.KZ6KT6.WI.V.ZIP : last exported on 23.01.24
+DLV.RPKKT6.WI.S.ZIP : last exported on 22.01.24
+DLV.I5XKT6.WI.A.ZIP : last exported on 23.01.24
+DIT.E35KT6.WI.ZIP : last exported on 23.01.24
+DEL.K2PKT6.WI.ZIP : last exported on 23.01.24
 DEL.R7AKT6.WI.ZIP : last exported on 22.01.24
 DEL.N5FKT6.WI.ZIP : last exported on 12.01.24</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 22.01.24
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 22.01.24
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 22.01.24
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 22.01.24
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 22.01.24
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 22.01.24
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 22.01.24
-DEL.KT6E35.WI.GGO.ZIP : last exported on 22.01.24
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 22.01.24
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 22.01.24
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 22.01.24</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 25.01.24
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 25.01.24
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 25.01.24
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 25.01.24
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 25.01.24
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 25.01.24
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 25.01.24
+DEL.KT6E35.WI.GGO.ZIP : last exported on 23.01.24
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 23.01.24
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 23.01.24
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 23.01.24</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 22.01.24
-DGV.N3LKT6.EPELS.??????.ZIP : last exported on 15.01.24</t>
+DEL.N3LKT6.HST.??????.ZIP : last exported on 24.01.24
+DGV.N3LKT6.EPELS.??????.ZIP : last exported on 22.01.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 21.01.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 21.01.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 21.01.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 21.01.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 21.01.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 21.01.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 21.01.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 21.01.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 21.01.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 21.01.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 21.01.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 21.01.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 21.01.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 21.01.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 21.01.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 21.01.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 21.01.24</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 24.01.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 24.01.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 24.01.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 24.01.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 24.01.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 24.01.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 24.01.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 24.01.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 23.01.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 23.01.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 23.01.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 23.01.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 23.01.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 23.01.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 23.01.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 23.01.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 23.01.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 21.01.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 24.01.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1324,12 +1324,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 19.01.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 23.01.24</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 20.01.24</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 23.01.24</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="C13" s="10" t="inlineStr">
         <is>
-          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 19.01.24
+          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 23.01.24
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
 DLV.I5XKT6.AU.A.ZIP : last exported on 12.01.24
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
@@ -1367,7 +1367,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 21.01.24
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 24.01.24
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
@@ -1409,20 +1409,20 @@
 DGQ.R11KT6.BSITX.TXT : last exported on 06.12.23
 DGQ.R31KT6.BSIVMC.TXT : last exported on 12.12.23
 DGQ.R31KT6.PKATC.TXT : last exported on 12.12.23
-DEL.KMPKT6.APOS.DATA.ZIP : last exported on 17.01.24</t>
+DEL.KMPKT6.APOS.DATA.ZIP : last exported on 24.01.24</t>
         </is>
       </c>
       <c r="D14" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 17.01.24
-DEL.N1LN3L.AP.F.GPL.DMP : last exported on 17.01.24
-DEL.N1LN3L.AP.F.GTR.DMP : last exported on 17.01.24
-DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 17.01.24
-DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 17.01.24
-DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 17.01.24
-DEL.N1LN0R.AP.F.CPD.DMP : last exported on 17.01.24
-DEL.N1LN0R.AP.F.CPL.DMP : last exported on 17.01.24
-DEL.N1LR31.AP.F.PPS.DMP : last exported on 17.01.24
+          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 24.01.24
+DEL.N1LN3L.AP.F.GPL.DMP : last exported on 24.01.24
+DEL.N1LN3L.AP.F.GTR.DMP : last exported on 24.01.24
+DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 24.01.24
+DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 24.01.24
+DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 24.01.24
+DEL.N1LN0R.AP.F.CPD.DMP : last exported on 24.01.24
+DEL.N1LN0R.AP.F.CPL.DMP : last exported on 24.01.24
+DEL.N1LR31.AP.F.PPS.DMP : last exported on 24.01.24
 DEL.KT6E35.AP.F.DB.ZIP : last exported on 17.01.24
 DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 17.01.24
 DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 17.01.24
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 21.01.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 21.01.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 24.01.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 24.01.24</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 21.01.24
-DHP.KUDKT6.ORGUNITS : last exported on 22.01.24
-DHS.R11KT6.HSB02ALL : last exported on 19.01.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 23.01.24
+DHP.KUDKT6.ORGUNITS : last exported on 24.01.24
+DHS.R11KT6.HSB02ALL : last exported on 23.01.24</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 19.01.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 19.01.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 21.01.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 19.01.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 19.01.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 19.01.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 19.01.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 19.01.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 19.01.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 19.01.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 24.01.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 24.01.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 24.01.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 24.01.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 24.01.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 24.01.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 24.01.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 24.01.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 24.01.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 24.01.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1603,38 +1603,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 20.01.24</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 23.01.24</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 20.01.24
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 20.01.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 21.01.24
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 20.01.24
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 20.01.24
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 20.01.24
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 20.01.24
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 20.01.24
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 20.01.24
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 20.01.24
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 20.01.24
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 20.01.24
-DEL.N1LKT6.MT.??????.G : last exported on 20.01.24
-DEL.N1LKT6.MT.??????.U : last exported on 20.01.24
-DEL.N1LKT6.MT.??????.AS : last exported on 20.01.24
-DVL.N1LN5X.VLM.DSP : last exported on 20.01.24
-DVL.N1LN5X.VLM.WT : last exported on 20.01.24
-DDS.N1LR11.DSP : last exported on 20.01.24
-DDS.N1LR11.WT : last exported on 20.01.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 20.01.24
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 20.01.24
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 20.01.24
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 20.01.24
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 20.01.24
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 20.01.24
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 20.01.24
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 20.01.24</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 24.01.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 24.01.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 24.01.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 24.01.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 24.01.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 24.01.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 24.01.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 24.01.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 24.01.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 24.01.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 24.01.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 24.01.24
+DEL.N1LKT6.MT.??????.G : last exported on 24.01.24
+DEL.N1LKT6.MT.??????.U : last exported on 24.01.24
+DEL.N1LKT6.MT.??????.AS : last exported on 24.01.24
+DVL.N1LN5X.VLM.DSP : last exported on 24.01.24
+DVL.N1LN5X.VLM.WT : last exported on 24.01.24
+DDS.N1LR11.DSP : last exported on 24.01.24
+DDS.N1LR11.WT : last exported on 24.01.24
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 23.01.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 23.01.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 23.01.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 23.01.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 23.01.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 23.01.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 23.01.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 23.01.24</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,52 +1662,52 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 22.01.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 22.01.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 22.01.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 22.01.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 22.01.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 22.01.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 22.01.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 22.01.24
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 24.01.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 24.01.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 24.01.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 24.01.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 24.01.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 24.01.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 24.01.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 24.01.24
 DDC.R11KT6.ELFI.MD.TXT : last exported on 21.01.24
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 19.01.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 23.01.24
 DDC.R11KT6.ELFI.PK.TXT : last exported on 21.01.24
 DDC.R11KT6.ELFI.PR.TXT : last exported on 21.01.24</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 21.01.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 21.01.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 21.01.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 21.01.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 21.01.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 21.01.24
-DEL.N1LKT6.EC.??????.G : last exported on 21.01.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 21.01.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 21.01.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 21.01.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 21.01.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 21.01.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 21.01.24
-DEL.N1LKT6.EC.??????.U : last exported on 21.01.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 21.01.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 21.01.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 21.01.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 21.01.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 21.01.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 21.01.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 21.01.24
-DEL.N1LKT6.EC.??????.AS : last exported on 21.01.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 21.01.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 21.01.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 21.01.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 21.01.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 21.01.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 21.01.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 21.01.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 21.01.24</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 24.01.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 24.01.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 24.01.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 24.01.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 24.01.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 24.01.24
+DEL.N1LKT6.EC.??????.G : last exported on 24.01.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 24.01.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 24.01.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 24.01.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 24.01.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 24.01.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 24.01.24
+DEL.N1LKT6.EC.??????.U : last exported on 24.01.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 24.01.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 24.01.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 24.01.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 24.01.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 24.01.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 24.01.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 24.01.24
+DEL.N1LKT6.EC.??????.AS : last exported on 24.01.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 24.01.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 24.01.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 24.01.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 24.01.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 24.01.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 24.01.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 24.01.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 23.01.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 25.01.24 14:02
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -989,7 +989,7 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 23.01.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 24.01.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
@@ -1002,9 +1002,9 @@
 DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 25.01.24
 DEL.N1LN0R.WD.D.CPD.DMP : last exported on 25.01.24
 DEL.N1LN0R.WD.D.CPL.DMP : last exported on 25.01.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 24.01.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 24.01.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 24.01.24</t>
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 25.01.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 25.01.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 25.01.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1109,13 +1109,13 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 23.01.24
-DLV.KZ6KT6.WI.V.ZIP : last exported on 23.01.24
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 24.01.24
+DLV.KZ6KT6.WI.V.ZIP : last exported on 24.01.24
 DLV.RPKKT6.WI.S.ZIP : last exported on 22.01.24
 DLV.I5XKT6.WI.A.ZIP : last exported on 23.01.24
-DIT.E35KT6.WI.ZIP : last exported on 23.01.24
-DEL.K2PKT6.WI.ZIP : last exported on 23.01.24
-DEL.R7AKT6.WI.ZIP : last exported on 22.01.24
+DIT.E35KT6.WI.ZIP : last exported on 24.01.24
+DEL.K2PKT6.WI.ZIP : last exported on 24.01.24
+DEL.R7AKT6.WI.ZIP : last exported on 25.01.24
 DEL.N5FKT6.WI.ZIP : last exported on 12.01.24</t>
         </is>
       </c>
@@ -1128,10 +1128,10 @@
 DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 25.01.24
 DEL.N1LN0R.WI.D.CPD.DMP : last exported on 25.01.24
 DEL.N1LN0R.WI.D.CPL.DMP : last exported on 25.01.24
-DEL.KT6E35.WI.GGO.ZIP : last exported on 23.01.24
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 23.01.24
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 23.01.24
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 23.01.24</t>
+DEL.KT6E35.WI.GGO.ZIP : last exported on 25.01.24
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 25.01.24
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 25.01.24
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 25.01.24</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,7 +1235,7 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 24.01.24
+DEL.N3LKT6.HST.??????.ZIP : last exported on 25.01.24
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 22.01.24</t>
         </is>
       </c>
@@ -1249,15 +1249,15 @@
 DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 24.01.24
 DEL.N1LN0R.TP.D.CPD.DMP : last exported on 24.01.24
 DEL.N1LN0R.TP.D.CPL.DMP : last exported on 24.01.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 23.01.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 23.01.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 23.01.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 23.01.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 23.01.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 23.01.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 23.01.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 23.01.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 23.01.24</t>
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 24.01.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 24.01.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 24.01.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 24.01.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 24.01.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 24.01.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 24.01.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 24.01.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 24.01.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1324,12 +1324,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 23.01.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 24.01.24</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 23.01.24</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 24.01.24</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="C13" s="10" t="inlineStr">
         <is>
-          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 23.01.24
+          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 24.01.24
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
 DLV.I5XKT6.AU.A.ZIP : last exported on 12.01.24
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
@@ -1423,11 +1423,11 @@
 DEL.N1LN0R.AP.F.CPD.DMP : last exported on 24.01.24
 DEL.N1LN0R.AP.F.CPL.DMP : last exported on 24.01.24
 DEL.N1LR31.AP.F.PPS.DMP : last exported on 24.01.24
-DEL.KT6E35.AP.F.DB.ZIP : last exported on 17.01.24
-DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 17.01.24
-DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 17.01.24
-DVL.KT6N5X.VLM.AP.ZIP : last exported on 17.01.24
-DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 17.01.24</t>
+DEL.KT6E35.AP.F.DB.ZIP : last exported on 24.01.24
+DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 24.01.24
+DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 24.01.24
+DVL.KT6N5X.VLM.AP.ZIP : last exported on 24.01.24
+DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 24.01.24</t>
         </is>
       </c>
       <c r="E14" s="11" t="inlineStr">
@@ -1489,9 +1489,9 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 23.01.24
-DHP.KUDKT6.ORGUNITS : last exported on 24.01.24
-DHS.R11KT6.HSB02ALL : last exported on 23.01.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 24.01.24
+DHP.KUDKT6.ORGUNITS : last exported on 25.01.24
+DHS.R11KT6.HSB02ALL : last exported on 24.01.24</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
@@ -1603,7 +1603,7 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 23.01.24</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 24.01.24</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
@@ -1627,14 +1627,14 @@
 DVL.N1LN5X.VLM.WT : last exported on 24.01.24
 DDS.N1LR11.DSP : last exported on 24.01.24
 DDS.N1LR11.WT : last exported on 24.01.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 23.01.24
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 23.01.24
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 23.01.24
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 23.01.24
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 23.01.24
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 23.01.24
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 23.01.24
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 23.01.24</t>
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 24.01.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 24.01.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 24.01.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 24.01.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 24.01.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 24.01.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 24.01.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 24.01.24</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,16 +1662,16 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 24.01.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 24.01.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 24.01.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 24.01.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 24.01.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 24.01.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 24.01.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 24.01.24
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 25.01.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 25.01.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 25.01.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 25.01.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 25.01.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 25.01.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 25.01.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 25.01.24
 DDC.R11KT6.ELFI.MD.TXT : last exported on 21.01.24
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 23.01.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 24.01.24
 DDC.R11KT6.ELFI.PK.TXT : last exported on 21.01.24
 DDC.R11KT6.ELFI.PR.TXT : last exported on 21.01.24</t>
         </is>
@@ -1707,7 +1707,7 @@
 DGV.N1LN7K.EL.F.ZIP : last exported on 24.01.24
 DGV.N1LN5X.EL.F.ZIP : last exported on 24.01.24
 DEL.KT6KT6.EL.F.DRE.CSV : last exported on 24.01.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 23.01.24</t>
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 24.01.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 29.01.24 14:42
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 25.01.2024</t>
+          <t>Date - 29.01.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 24.01.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 26.01.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 25.01.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 25.01.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 25.01.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 25.01.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 25.01.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 25.01.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 25.01.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 25.01.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 25.01.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 25.01.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 25.01.24</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 27.01.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 27.01.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 28.01.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 27.01.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 27.01.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 27.01.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 27.01.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 27.01.24
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 27.01.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 27.01.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 27.01.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1066,22 +1066,22 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 22.01.24
-DEH.N3LKT6.AP.COMPL.SNK : last exported on 22.01.24</t>
+          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 29.01.24
+DEH.N3LKT6.AP.COMPL.SNK : last exported on 29.01.24</t>
         </is>
       </c>
       <c r="D6" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 22.01.24
-DEL.N1LN3L.DN.F.GPL.DMP : last exported on 22.01.24
-DEL.N1LN3L.DN.F.GTR.DMP : last exported on 22.01.24
-DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 22.01.24
-DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 22.01.24
-DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 22.01.24
-DEL.N1LN0R.DN.F.CPD.DMP : last exported on 22.01.24
-DEL.N1LN0R.DN.F.CPL.DMP : last exported on 22.01.24
-DEL.KT6E35.SN.F.GGO.ZIP : last exported on 22.01.24
-DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 22.01.24</t>
+          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 29.01.24
+DEL.N1LN3L.DN.F.GPL.DMP : last exported on 29.01.24
+DEL.N1LN3L.DN.F.GTR.DMP : last exported on 29.01.24
+DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 29.01.24
+DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 29.01.24
+DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 29.01.24
+DEL.N1LN0R.DN.F.CPD.DMP : last exported on 29.01.24
+DEL.N1LN0R.DN.F.CPL.DMP : last exported on 29.01.24
+DEL.KT6E35.SN.F.GGO.ZIP : last exported on 29.01.24
+DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 29.01.24</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
@@ -1109,29 +1109,29 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 24.01.24
-DLV.KZ6KT6.WI.V.ZIP : last exported on 24.01.24
-DLV.RPKKT6.WI.S.ZIP : last exported on 22.01.24
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 26.01.24
+DLV.KZ6KT6.WI.V.ZIP : last exported on 28.01.24
+DLV.RPKKT6.WI.S.ZIP : last exported on 26.01.24
 DLV.I5XKT6.WI.A.ZIP : last exported on 23.01.24
-DIT.E35KT6.WI.ZIP : last exported on 24.01.24
-DEL.K2PKT6.WI.ZIP : last exported on 24.01.24
+DIT.E35KT6.WI.ZIP : last exported on 26.01.24
+DEL.K2PKT6.WI.ZIP : last exported on 27.01.24
 DEL.R7AKT6.WI.ZIP : last exported on 25.01.24
-DEL.N5FKT6.WI.ZIP : last exported on 12.01.24</t>
+DEL.N5FKT6.WI.ZIP : last exported on 26.01.24</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 25.01.24
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 25.01.24
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 25.01.24
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 25.01.24
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 25.01.24
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 25.01.24
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 25.01.24
-DEL.KT6E35.WI.GGO.ZIP : last exported on 25.01.24
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 25.01.24
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 25.01.24
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 25.01.24</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 29.01.24
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 29.01.24
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 29.01.24
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 29.01.24
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 29.01.24
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 29.01.24
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 29.01.24
+DEL.KT6E35.WI.GGO.ZIP : last exported on 29.01.24
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 29.01.24
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 29.01.24
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 29.01.24</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 25.01.24
+DEL.N3LKT6.HST.??????.ZIP : last exported on 29.01.24
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 22.01.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 24.01.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 24.01.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 24.01.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 24.01.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 24.01.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 24.01.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 24.01.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 24.01.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 24.01.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 24.01.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 24.01.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 24.01.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 24.01.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 24.01.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 24.01.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 24.01.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 24.01.24</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 28.01.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 28.01.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 28.01.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 28.01.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 28.01.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 28.01.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 28.01.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 28.01.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 28.01.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 28.01.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 28.01.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 28.01.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 28.01.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 28.01.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 28.01.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 28.01.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 28.01.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 24.01.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 28.01.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1324,12 +1324,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 24.01.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 26.01.24</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 24.01.24</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 27.01.24</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="C13" s="10" t="inlineStr">
         <is>
-          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 24.01.24
+          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 26.01.24
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
 DLV.I5XKT6.AU.A.ZIP : last exported on 12.01.24
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
@@ -1367,7 +1367,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 24.01.24
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 28.01.24
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 24.01.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 24.01.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 28.01.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 28.01.24</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 24.01.24
-DHP.KUDKT6.ORGUNITS : last exported on 25.01.24
-DHS.R11KT6.HSB02ALL : last exported on 24.01.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 28.01.24
+DHP.KUDKT6.ORGUNITS : last exported on 29.01.24
+DHS.R11KT6.HSB02ALL : last exported on 26.01.24</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 24.01.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 24.01.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 24.01.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 24.01.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 24.01.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 24.01.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 24.01.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 24.01.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 24.01.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 24.01.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 26.01.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 26.01.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 28.01.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 26.01.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 26.01.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 26.01.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 26.01.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 26.01.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 26.01.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 26.01.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1575,7 +1575,7 @@
       </c>
       <c r="D18" s="15" t="inlineStr">
         <is>
-          <t>DEL.N1LE35.TRANS.ZIP : last exported on 21.01.24</t>
+          <t>DEL.N1LE35.TRANS.ZIP : last exported on 28.01.24</t>
         </is>
       </c>
       <c r="E18" s="11" t="inlineStr">
@@ -1603,38 +1603,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 24.01.24</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 27.01.24</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 24.01.24
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 24.01.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 24.01.24
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 24.01.24
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 24.01.24
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 24.01.24
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 24.01.24
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 24.01.24
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 24.01.24
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 24.01.24
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 24.01.24
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 24.01.24
-DEL.N1LKT6.MT.??????.G : last exported on 24.01.24
-DEL.N1LKT6.MT.??????.U : last exported on 24.01.24
-DEL.N1LKT6.MT.??????.AS : last exported on 24.01.24
-DVL.N1LN5X.VLM.DSP : last exported on 24.01.24
-DVL.N1LN5X.VLM.WT : last exported on 24.01.24
-DDS.N1LR11.DSP : last exported on 24.01.24
-DDS.N1LR11.WT : last exported on 24.01.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 24.01.24
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 24.01.24
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 24.01.24
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 24.01.24
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 24.01.24
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 24.01.24
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 24.01.24
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 24.01.24</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 27.01.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 27.01.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 28.01.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 27.01.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 27.01.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 27.01.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 27.01.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 27.01.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 27.01.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 27.01.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 27.01.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 27.01.24
+DEL.N1LKT6.MT.??????.G : last exported on 27.01.24
+DEL.N1LKT6.MT.??????.U : last exported on 27.01.24
+DEL.N1LKT6.MT.??????.AS : last exported on 27.01.24
+DVL.N1LN5X.VLM.DSP : last exported on 27.01.24
+DVL.N1LN5X.VLM.WT : last exported on 27.01.24
+DDS.N1LR11.DSP : last exported on 27.01.24
+DDS.N1LR11.WT : last exported on 27.01.24
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 27.01.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 27.01.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 27.01.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 27.01.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 27.01.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 27.01.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 27.01.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 27.01.24</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,52 +1662,52 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 25.01.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 25.01.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 25.01.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 25.01.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 25.01.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 25.01.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 25.01.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 25.01.24
-DDC.R11KT6.ELFI.MD.TXT : last exported on 21.01.24
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 24.01.24
-DDC.R11KT6.ELFI.PK.TXT : last exported on 21.01.24
-DDC.R11KT6.ELFI.PR.TXT : last exported on 21.01.24</t>
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 29.01.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 29.01.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 29.01.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 29.01.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 29.01.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 29.01.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 29.01.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 29.01.24
+DDC.R11KT6.ELFI.MD.TXT : last exported on 28.01.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 26.01.24
+DDC.R11KT6.ELFI.PK.TXT : last exported on 28.01.24
+DDC.R11KT6.ELFI.PR.TXT : last exported on 28.01.24</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 24.01.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 24.01.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 24.01.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 24.01.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 24.01.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 24.01.24
-DEL.N1LKT6.EC.??????.G : last exported on 24.01.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 24.01.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 24.01.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 24.01.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 24.01.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 24.01.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 24.01.24
-DEL.N1LKT6.EC.??????.U : last exported on 24.01.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 24.01.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 24.01.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 24.01.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 24.01.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 24.01.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 24.01.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 24.01.24
-DEL.N1LKT6.EC.??????.AS : last exported on 24.01.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 24.01.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 24.01.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 24.01.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 24.01.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 24.01.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 24.01.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 24.01.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 24.01.24</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 28.01.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 28.01.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 28.01.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 28.01.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 28.01.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 28.01.24
+DEL.N1LKT6.EC.??????.G : last exported on 28.01.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 28.01.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 28.01.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 28.01.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 28.01.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 28.01.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 28.01.24
+DEL.N1LKT6.EC.??????.U : last exported on 28.01.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 28.01.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 28.01.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 28.01.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 28.01.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 28.01.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 28.01.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 28.01.24
+DEL.N1LKT6.EC.??????.AS : last exported on 28.01.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 28.01.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 28.01.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 28.01.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 28.01.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 28.01.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 28.01.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 28.01.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 28.01.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 30.01.24 13:30
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 29.01.2024</t>
+          <t>Date - 30.01.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 26.01.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 29.01.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 27.01.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 27.01.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 28.01.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 27.01.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 27.01.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 27.01.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 27.01.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 27.01.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 27.01.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 27.01.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 27.01.24</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 30.01.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 30.01.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 30.01.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 30.01.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 30.01.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 30.01.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 30.01.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 30.01.24
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 30.01.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 30.01.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 30.01.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1109,12 +1109,12 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 26.01.24
-DLV.KZ6KT6.WI.V.ZIP : last exported on 28.01.24
-DLV.RPKKT6.WI.S.ZIP : last exported on 26.01.24
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 29.01.24
+DLV.KZ6KT6.WI.V.ZIP : last exported on 29.01.24
+DLV.RPKKT6.WI.S.ZIP : last exported on 29.01.24
 DLV.I5XKT6.WI.A.ZIP : last exported on 23.01.24
-DIT.E35KT6.WI.ZIP : last exported on 26.01.24
-DEL.K2PKT6.WI.ZIP : last exported on 27.01.24
+DIT.E35KT6.WI.ZIP : last exported on 29.01.24
+DEL.K2PKT6.WI.ZIP : last exported on 29.01.24
 DEL.R7AKT6.WI.ZIP : last exported on 25.01.24
 DEL.N5FKT6.WI.ZIP : last exported on 26.01.24</t>
         </is>
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 29.01.24
-DGV.N3LKT6.EPELS.??????.ZIP : last exported on 22.01.24</t>
+DEL.N3LKT6.HST.??????.ZIP : last exported on 30.01.24
+DGV.N3LKT6.EPELS.??????.ZIP : last exported on 29.01.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 28.01.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 28.01.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 28.01.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 28.01.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 28.01.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 28.01.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 28.01.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 28.01.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 28.01.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 28.01.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 28.01.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 28.01.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 28.01.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 28.01.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 28.01.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 28.01.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 28.01.24</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 29.01.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 29.01.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 29.01.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 29.01.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 29.01.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 29.01.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 29.01.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 29.01.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 29.01.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 29.01.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 29.01.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 29.01.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 29.01.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 29.01.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 29.01.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 29.01.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 29.01.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 28.01.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 29.01.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1324,7 +1324,7 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 26.01.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 29.01.24</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
@@ -1367,7 +1367,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 28.01.24
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 29.01.24
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 28.01.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 28.01.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 29.01.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 29.01.24</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 28.01.24
-DHP.KUDKT6.ORGUNITS : last exported on 29.01.24
-DHS.R11KT6.HSB02ALL : last exported on 26.01.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 29.01.24
+DHP.KUDKT6.ORGUNITS : last exported on 30.01.24
+DHS.R11KT6.HSB02ALL : last exported on 29.01.24</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 26.01.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 26.01.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 28.01.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 26.01.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 26.01.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 26.01.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 26.01.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 26.01.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 26.01.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 26.01.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 29.01.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 29.01.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 29.01.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 29.01.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 29.01.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 29.01.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 29.01.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 29.01.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 29.01.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 29.01.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1603,38 +1603,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 27.01.24</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 29.01.24</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 27.01.24
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 27.01.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 28.01.24
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 27.01.24
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 27.01.24
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 27.01.24
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 27.01.24
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 27.01.24
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 27.01.24
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 27.01.24
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 27.01.24
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 27.01.24
-DEL.N1LKT6.MT.??????.G : last exported on 27.01.24
-DEL.N1LKT6.MT.??????.U : last exported on 27.01.24
-DEL.N1LKT6.MT.??????.AS : last exported on 27.01.24
-DVL.N1LN5X.VLM.DSP : last exported on 27.01.24
-DVL.N1LN5X.VLM.WT : last exported on 27.01.24
-DDS.N1LR11.DSP : last exported on 27.01.24
-DDS.N1LR11.WT : last exported on 27.01.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 27.01.24
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 27.01.24
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 27.01.24
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 27.01.24
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 27.01.24
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 27.01.24
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 27.01.24
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 27.01.24</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 29.01.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 29.01.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 29.01.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 29.01.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 29.01.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 29.01.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 29.01.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 29.01.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 29.01.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 29.01.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 29.01.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 29.01.24
+DEL.N1LKT6.MT.??????.G : last exported on 29.01.24
+DEL.N1LKT6.MT.??????.U : last exported on 29.01.24
+DEL.N1LKT6.MT.??????.AS : last exported on 29.01.24
+DVL.N1LN5X.VLM.DSP : last exported on 29.01.24
+DVL.N1LN5X.VLM.WT : last exported on 29.01.24
+DDS.N1LR11.DSP : last exported on 29.01.24
+DDS.N1LR11.WT : last exported on 29.01.24
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 29.01.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 29.01.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 29.01.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 29.01.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 29.01.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 29.01.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 29.01.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 29.01.24</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,52 +1662,52 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 29.01.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 29.01.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 29.01.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 29.01.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 29.01.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 29.01.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 29.01.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 29.01.24
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 30.01.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 30.01.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 30.01.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 30.01.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 30.01.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 30.01.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 30.01.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 30.01.24
 DDC.R11KT6.ELFI.MD.TXT : last exported on 28.01.24
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 26.01.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 29.01.24
 DDC.R11KT6.ELFI.PK.TXT : last exported on 28.01.24
 DDC.R11KT6.ELFI.PR.TXT : last exported on 28.01.24</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 28.01.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 28.01.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 28.01.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 28.01.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 28.01.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 28.01.24
-DEL.N1LKT6.EC.??????.G : last exported on 28.01.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 28.01.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 28.01.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 28.01.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 28.01.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 28.01.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 28.01.24
-DEL.N1LKT6.EC.??????.U : last exported on 28.01.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 28.01.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 28.01.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 28.01.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 28.01.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 28.01.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 28.01.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 28.01.24
-DEL.N1LKT6.EC.??????.AS : last exported on 28.01.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 28.01.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 28.01.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 28.01.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 28.01.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 28.01.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 28.01.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 28.01.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 28.01.24</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 29.01.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 29.01.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 29.01.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 29.01.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 29.01.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 29.01.24
+DEL.N1LKT6.EC.??????.G : last exported on 29.01.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 29.01.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 29.01.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 29.01.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 29.01.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 29.01.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 29.01.24
+DEL.N1LKT6.EC.??????.U : last exported on 29.01.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 29.01.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 29.01.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 29.01.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 29.01.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 29.01.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 29.01.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 29.01.24
+DEL.N1LKT6.EC.??????.AS : last exported on 29.01.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 29.01.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 29.01.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 29.01.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 29.01.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 29.01.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 29.01.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 29.01.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 29.01.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 31.01.24 14:44
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 30.01.2024</t>
+          <t>Date - 31.01.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 29.01.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 30.01.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 30.01.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 30.01.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 30.01.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 30.01.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 30.01.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 30.01.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 30.01.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 30.01.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 30.01.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 30.01.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 30.01.24</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 31.01.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 31.01.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 31.01.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 31.01.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 31.01.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 31.01.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 31.01.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 31.01.24
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 31.01.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 31.01.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 31.01.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1109,29 +1109,29 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 29.01.24
-DLV.KZ6KT6.WI.V.ZIP : last exported on 29.01.24
-DLV.RPKKT6.WI.S.ZIP : last exported on 29.01.24
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 30.01.24
+DLV.KZ6KT6.WI.V.ZIP : last exported on 30.01.24
+DLV.RPKKT6.WI.S.ZIP : last exported on 30.01.24
 DLV.I5XKT6.WI.A.ZIP : last exported on 23.01.24
-DIT.E35KT6.WI.ZIP : last exported on 29.01.24
-DEL.K2PKT6.WI.ZIP : last exported on 29.01.24
+DIT.E35KT6.WI.ZIP : last exported on 30.01.24
+DEL.K2PKT6.WI.ZIP : last exported on 30.01.24
 DEL.R7AKT6.WI.ZIP : last exported on 25.01.24
 DEL.N5FKT6.WI.ZIP : last exported on 26.01.24</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 29.01.24
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 29.01.24
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 29.01.24
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 29.01.24
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 29.01.24
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 29.01.24
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 29.01.24
-DEL.KT6E35.WI.GGO.ZIP : last exported on 29.01.24
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 29.01.24
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 29.01.24
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 29.01.24</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 31.01.24
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 31.01.24
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 31.01.24
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 31.01.24
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 31.01.24
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 31.01.24
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 31.01.24
+DEL.KT6E35.WI.GGO.ZIP : last exported on 31.01.24
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 31.01.24
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 31.01.24
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 31.01.24</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 30.01.24
+DEL.N3LKT6.HST.??????.ZIP : last exported on 31.01.24
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 29.01.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 29.01.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 29.01.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 29.01.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 29.01.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 29.01.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 29.01.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 29.01.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 29.01.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 29.01.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 29.01.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 29.01.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 29.01.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 29.01.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 29.01.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 29.01.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 29.01.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 29.01.24</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 30.01.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 30.01.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 30.01.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 30.01.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 30.01.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 30.01.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 30.01.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 30.01.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 30.01.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 30.01.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 30.01.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 30.01.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 30.01.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 30.01.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 30.01.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 30.01.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 30.01.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 29.01.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 30.01.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1324,12 +1324,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 29.01.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 30.01.24</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 27.01.24</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 30.01.24</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1367,7 +1367,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 29.01.24
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 30.01.24
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 29.01.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 29.01.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 30.01.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 30.01.24</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 29.01.24
-DHP.KUDKT6.ORGUNITS : last exported on 30.01.24
-DHS.R11KT6.HSB02ALL : last exported on 29.01.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 30.01.24
+DHP.KUDKT6.ORGUNITS : last exported on 31.01.24
+DHS.R11KT6.HSB02ALL : last exported on 30.01.24</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 29.01.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 29.01.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 29.01.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 29.01.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 29.01.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 29.01.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 29.01.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 29.01.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 29.01.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 29.01.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 30.01.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 30.01.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 30.01.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 30.01.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 30.01.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 30.01.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 30.01.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 30.01.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 30.01.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 30.01.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1603,38 +1603,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 29.01.24</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 30.01.24</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 29.01.24
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 29.01.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 29.01.24
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 29.01.24
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 29.01.24
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 29.01.24
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 29.01.24
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 29.01.24
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 29.01.24
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 29.01.24
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 29.01.24
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 29.01.24
-DEL.N1LKT6.MT.??????.G : last exported on 29.01.24
-DEL.N1LKT6.MT.??????.U : last exported on 29.01.24
-DEL.N1LKT6.MT.??????.AS : last exported on 29.01.24
-DVL.N1LN5X.VLM.DSP : last exported on 29.01.24
-DVL.N1LN5X.VLM.WT : last exported on 29.01.24
-DDS.N1LR11.DSP : last exported on 29.01.24
-DDS.N1LR11.WT : last exported on 29.01.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 29.01.24
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 29.01.24
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 29.01.24
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 29.01.24
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 29.01.24
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 29.01.24
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 29.01.24
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 29.01.24</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 30.01.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 30.01.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 30.01.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 30.01.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 30.01.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 30.01.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 30.01.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 30.01.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 30.01.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 30.01.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 30.01.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 30.01.24
+DEL.N1LKT6.MT.??????.G : last exported on 30.01.24
+DEL.N1LKT6.MT.??????.U : last exported on 30.01.24
+DEL.N1LKT6.MT.??????.AS : last exported on 30.01.24
+DVL.N1LN5X.VLM.DSP : last exported on 30.01.24
+DVL.N1LN5X.VLM.WT : last exported on 30.01.24
+DDS.N1LR11.DSP : last exported on 30.01.24
+DDS.N1LR11.WT : last exported on 30.01.24
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 30.01.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 30.01.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 30.01.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 30.01.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 30.01.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 30.01.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 30.01.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 30.01.24</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,52 +1662,52 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 30.01.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 30.01.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 30.01.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 30.01.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 30.01.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 30.01.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 30.01.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 30.01.24
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 31.01.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 31.01.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 31.01.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 31.01.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 31.01.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 31.01.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 31.01.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 31.01.24
 DDC.R11KT6.ELFI.MD.TXT : last exported on 28.01.24
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 29.01.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 30.01.24
 DDC.R11KT6.ELFI.PK.TXT : last exported on 28.01.24
 DDC.R11KT6.ELFI.PR.TXT : last exported on 28.01.24</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 29.01.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 29.01.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 29.01.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 29.01.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 29.01.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 29.01.24
-DEL.N1LKT6.EC.??????.G : last exported on 29.01.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 29.01.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 29.01.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 29.01.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 29.01.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 29.01.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 29.01.24
-DEL.N1LKT6.EC.??????.U : last exported on 29.01.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 29.01.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 29.01.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 29.01.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 29.01.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 29.01.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 29.01.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 29.01.24
-DEL.N1LKT6.EC.??????.AS : last exported on 29.01.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 29.01.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 29.01.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 29.01.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 29.01.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 29.01.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 29.01.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 29.01.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 29.01.24</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 30.01.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 30.01.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 30.01.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 30.01.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 30.01.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 30.01.24
+DEL.N1LKT6.EC.??????.G : last exported on 30.01.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 30.01.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 30.01.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 30.01.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 30.01.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 30.01.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 30.01.24
+DEL.N1LKT6.EC.??????.U : last exported on 30.01.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 30.01.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 30.01.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 30.01.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 30.01.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 30.01.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 30.01.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 30.01.24
+DEL.N1LKT6.EC.??????.AS : last exported on 30.01.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 30.01.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 30.01.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 30.01.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 30.01.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 30.01.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 30.01.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 30.01.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 30.01.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 01.02.24 14:43
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 31.01.2024</t>
+          <t>Date - 01.02.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 30.01.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 31.01.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 31.01.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 31.01.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 31.01.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 31.01.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 31.01.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 31.01.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 31.01.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 31.01.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 31.01.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 31.01.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 31.01.24</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 01.02.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 01.02.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 01.02.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 01.02.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 01.02.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 01.02.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 01.02.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 01.02.24
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 01.02.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 01.02.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 01.02.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1109,29 +1109,29 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 30.01.24
-DLV.KZ6KT6.WI.V.ZIP : last exported on 30.01.24
-DLV.RPKKT6.WI.S.ZIP : last exported on 30.01.24
-DLV.I5XKT6.WI.A.ZIP : last exported on 23.01.24
-DIT.E35KT6.WI.ZIP : last exported on 30.01.24
-DEL.K2PKT6.WI.ZIP : last exported on 30.01.24
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 31.01.24
+DLV.KZ6KT6.WI.V.ZIP : last exported on 31.01.24
+DLV.RPKKT6.WI.S.ZIP : last exported on 31.01.24
+DLV.I5XKT6.WI.A.ZIP : last exported on 31.01.24
+DIT.E35KT6.WI.ZIP : last exported on 31.01.24
+DEL.K2PKT6.WI.ZIP : last exported on 31.01.24
 DEL.R7AKT6.WI.ZIP : last exported on 25.01.24
 DEL.N5FKT6.WI.ZIP : last exported on 26.01.24</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 31.01.24
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 31.01.24
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 31.01.24
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 31.01.24
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 31.01.24
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 31.01.24
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 31.01.24
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 01.02.24
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 01.02.24
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 01.02.24
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 01.02.24
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 01.02.24
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 01.02.24
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 01.02.24
 DEL.KT6E35.WI.GGO.ZIP : last exported on 31.01.24
 DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 31.01.24
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 31.01.24
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 31.01.24</t>
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 01.02.24
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 01.02.24</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 31.01.24
+DEL.N3LKT6.HST.??????.ZIP : last exported on 01.02.24
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 29.01.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 30.01.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 30.01.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 30.01.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 30.01.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 30.01.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 30.01.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 30.01.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 30.01.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 30.01.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 30.01.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 30.01.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 30.01.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 30.01.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 30.01.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 30.01.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 30.01.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 30.01.24</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 31.01.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 31.01.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 31.01.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 31.01.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 31.01.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 31.01.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 31.01.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 31.01.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 31.01.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 31.01.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 31.01.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 31.01.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 31.01.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 31.01.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 31.01.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 31.01.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 31.01.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 30.01.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 31.01.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
@@ -1324,12 +1324,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 30.01.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 31.01.24</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 30.01.24</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 31.01.24</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1367,7 +1367,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 30.01.24
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 31.01.24
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
@@ -1399,35 +1399,35 @@
       </c>
       <c r="C14" s="10" t="inlineStr">
         <is>
-          <t>DGQ.R11KT6.BSIVM.TXT : last exported on 06.12.23
-DGQ.R11KT6.BSIVM.C.TXT : last exported on 06.12.23
-DGQ.R11KT6.BSIVM.US2.TXT : last exported on 06.12.23
-DGQ.R11KT6.PKAT.TXT : last exported on 06.12.23
-DGQ.R11KT6.PKAT.C.TXT : last exported on 06.12.23
-DGQ.R11KT6.PKAT.US2.TXT : last exported on 06.12.23
-DGQ.R11KT6.BSITK.TXT : last exported on 06.12.23
-DGQ.R11KT6.BSITX.TXT : last exported on 06.12.23
+          <t>DGQ.R11KT6.BSIVM.TXT : last exported on 31.01.24
+DGQ.R11KT6.BSIVM.C.TXT : last exported on 31.01.24
+DGQ.R11KT6.BSIVM.US2.TXT : last exported on 31.01.24
+DGQ.R11KT6.PKAT.TXT : last exported on 31.01.24
+DGQ.R11KT6.PKAT.C.TXT : last exported on 31.01.24
+DGQ.R11KT6.PKAT.US2.TXT : last exported on 31.01.24
+DGQ.R11KT6.BSITK.TXT : last exported on 31.01.24
+DGQ.R11KT6.BSITX.TXT : last exported on 31.01.24
 DGQ.R31KT6.BSIVMC.TXT : last exported on 12.12.23
 DGQ.R31KT6.PKATC.TXT : last exported on 12.12.23
-DEL.KMPKT6.APOS.DATA.ZIP : last exported on 24.01.24</t>
+DEL.KMPKT6.APOS.DATA.ZIP : last exported on 31.01.24</t>
         </is>
       </c>
       <c r="D14" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 24.01.24
-DEL.N1LN3L.AP.F.GPL.DMP : last exported on 24.01.24
-DEL.N1LN3L.AP.F.GTR.DMP : last exported on 24.01.24
-DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 24.01.24
-DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 24.01.24
-DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 24.01.24
-DEL.N1LN0R.AP.F.CPD.DMP : last exported on 24.01.24
-DEL.N1LN0R.AP.F.CPL.DMP : last exported on 24.01.24
-DEL.N1LR31.AP.F.PPS.DMP : last exported on 24.01.24
-DEL.KT6E35.AP.F.DB.ZIP : last exported on 24.01.24
-DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 24.01.24
-DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 24.01.24
-DVL.KT6N5X.VLM.AP.ZIP : last exported on 24.01.24
-DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 24.01.24</t>
+          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 31.01.24
+DEL.N1LN3L.AP.F.GPL.DMP : last exported on 31.01.24
+DEL.N1LN3L.AP.F.GTR.DMP : last exported on 31.01.24
+DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 31.01.24
+DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 31.01.24
+DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 31.01.24
+DEL.N1LN0R.AP.F.CPD.DMP : last exported on 31.01.24
+DEL.N1LN0R.AP.F.CPL.DMP : last exported on 31.01.24
+DEL.N1LR31.AP.F.PPS.DMP : last exported on 31.01.24
+DEL.KT6E35.AP.F.DB.ZIP : last exported on 31.01.24
+DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 31.01.24
+DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 31.01.24
+DVL.KT6N5X.VLM.AP.ZIP : last exported on 31.01.24
+DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 31.01.24</t>
         </is>
       </c>
       <c r="E14" s="11" t="inlineStr">
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 30.01.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 30.01.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 31.01.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 31.01.24</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 30.01.24
-DHP.KUDKT6.ORGUNITS : last exported on 31.01.24
-DHS.R11KT6.HSB02ALL : last exported on 30.01.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 31.01.24
+DHP.KUDKT6.ORGUNITS : last exported on 01.02.24
+DHS.R11KT6.HSB02ALL : last exported on 31.01.24</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 30.01.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 30.01.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 30.01.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 30.01.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 30.01.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 30.01.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 30.01.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 30.01.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 30.01.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 30.01.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 31.01.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 31.01.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 31.01.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 31.01.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 31.01.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 31.01.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 31.01.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 31.01.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 31.01.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 31.01.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1603,38 +1603,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 30.01.24</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 31.01.24</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 30.01.24
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 30.01.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 30.01.24
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 30.01.24
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 30.01.24
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 30.01.24
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 30.01.24
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 30.01.24
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 30.01.24
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 30.01.24
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 30.01.24
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 30.01.24
-DEL.N1LKT6.MT.??????.G : last exported on 30.01.24
-DEL.N1LKT6.MT.??????.U : last exported on 30.01.24
-DEL.N1LKT6.MT.??????.AS : last exported on 30.01.24
-DVL.N1LN5X.VLM.DSP : last exported on 30.01.24
-DVL.N1LN5X.VLM.WT : last exported on 30.01.24
-DDS.N1LR11.DSP : last exported on 30.01.24
-DDS.N1LR11.WT : last exported on 30.01.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 30.01.24
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 30.01.24
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 30.01.24
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 30.01.24
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 30.01.24
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 30.01.24
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 30.01.24
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 30.01.24</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 31.01.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 31.01.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 31.01.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 31.01.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 31.01.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 31.01.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 31.01.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 31.01.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 31.01.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 31.01.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 31.01.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 31.01.24
+DEL.N1LKT6.MT.??????.G : last exported on 31.01.24
+DEL.N1LKT6.MT.??????.U : last exported on 31.01.24
+DEL.N1LKT6.MT.??????.AS : last exported on 31.01.24
+DVL.N1LN5X.VLM.DSP : last exported on 31.01.24
+DVL.N1LN5X.VLM.WT : last exported on 31.01.24
+DDS.N1LR11.DSP : last exported on 31.01.24
+DDS.N1LR11.WT : last exported on 31.01.24
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 31.01.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 31.01.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 31.01.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 31.01.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 31.01.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 31.01.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 31.01.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 31.01.24</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,52 +1662,52 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 31.01.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 31.01.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 31.01.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 31.01.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 31.01.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 31.01.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 31.01.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 31.01.24
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 01.02.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 01.02.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 01.02.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 01.02.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 01.02.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 01.02.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 01.02.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 01.02.24
 DDC.R11KT6.ELFI.MD.TXT : last exported on 28.01.24
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 30.01.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 31.01.24
 DDC.R11KT6.ELFI.PK.TXT : last exported on 28.01.24
 DDC.R11KT6.ELFI.PR.TXT : last exported on 28.01.24</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 30.01.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 30.01.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 30.01.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 30.01.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 30.01.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 30.01.24
-DEL.N1LKT6.EC.??????.G : last exported on 30.01.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 30.01.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 30.01.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 30.01.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 30.01.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 30.01.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 30.01.24
-DEL.N1LKT6.EC.??????.U : last exported on 30.01.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 30.01.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 30.01.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 30.01.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 30.01.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 30.01.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 30.01.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 30.01.24
-DEL.N1LKT6.EC.??????.AS : last exported on 30.01.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 30.01.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 30.01.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 30.01.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 30.01.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 30.01.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 30.01.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 30.01.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 30.01.24</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 31.01.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 31.01.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 31.01.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 31.01.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 31.01.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 31.01.24
+DEL.N1LKT6.EC.??????.G : last exported on 31.01.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 31.01.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 31.01.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 31.01.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 31.01.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 31.01.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 31.01.24
+DEL.N1LKT6.EC.??????.U : last exported on 31.01.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 31.01.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 31.01.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 31.01.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 31.01.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 31.01.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 31.01.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 31.01.24
+DEL.N1LKT6.EC.??????.AS : last exported on 31.01.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 31.01.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 31.01.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 31.01.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 31.01.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 31.01.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 31.01.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 31.01.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 31.01.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 02.02.24 14:24
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 01.02.2024</t>
+          <t>Date - 02.02.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 31.01.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 01.02.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 01.02.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 01.02.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 01.02.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 01.02.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 01.02.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 01.02.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 01.02.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 01.02.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 01.02.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 01.02.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 01.02.24</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 02.02.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 02.02.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 02.02.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 02.02.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 02.02.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 02.02.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 02.02.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 02.02.24
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 02.02.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 02.02.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 02.02.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1109,12 +1109,12 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 31.01.24
-DLV.KZ6KT6.WI.V.ZIP : last exported on 31.01.24
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 01.02.24
+DLV.KZ6KT6.WI.V.ZIP : last exported on 01.02.24
 DLV.RPKKT6.WI.S.ZIP : last exported on 31.01.24
-DLV.I5XKT6.WI.A.ZIP : last exported on 31.01.24
-DIT.E35KT6.WI.ZIP : last exported on 31.01.24
-DEL.K2PKT6.WI.ZIP : last exported on 31.01.24
+DLV.I5XKT6.WI.A.ZIP : last exported on 01.02.24
+DIT.E35KT6.WI.ZIP : last exported on 01.02.24
+DEL.K2PKT6.WI.ZIP : last exported on 01.02.24
 DEL.R7AKT6.WI.ZIP : last exported on 25.01.24
 DEL.N5FKT6.WI.ZIP : last exported on 26.01.24</t>
         </is>
@@ -1128,8 +1128,8 @@
 DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 01.02.24
 DEL.N1LN0R.WI.D.CPD.DMP : last exported on 01.02.24
 DEL.N1LN0R.WI.D.CPL.DMP : last exported on 01.02.24
-DEL.KT6E35.WI.GGO.ZIP : last exported on 31.01.24
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 31.01.24
+DEL.KT6E35.WI.GGO.ZIP : last exported on 01.02.24
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 01.02.24
 DEL.KT6N5M.WI.GGO.ZIP : last exported on 01.02.24
 DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 01.02.24</t>
         </is>
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 01.02.24
+DEL.N3LKT6.HST.??????.ZIP : last exported on 02.02.24
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 29.01.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 31.01.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 31.01.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 31.01.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 31.01.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 31.01.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 31.01.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 31.01.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 31.01.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 31.01.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 31.01.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 31.01.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 31.01.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 31.01.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 31.01.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 31.01.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 31.01.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 31.01.24</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 01.02.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 01.02.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 01.02.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 01.02.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 01.02.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 01.02.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 01.02.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 01.02.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 01.02.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 01.02.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 01.02.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 01.02.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 01.02.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 01.02.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 01.02.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 01.02.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 01.02.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1285,18 +1285,18 @@
       </c>
       <c r="C11" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.MANDANTN.TXT : last exported on 30.11.23</t>
+          <t>DEL.N3LKT6.MANDANTN.TXT : last exported on 01.02.24</t>
         </is>
       </c>
       <c r="D11" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GPL.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 31.01.24
-DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 30.11.23
-DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 30.11.23
-DGI.KT6R11.MANDANT.TXT : last exported on 30.11.23</t>
+          <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 01.02.24
+DEL.N1LN3L.MC.F.GPL.DMP : last exported on 01.02.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 01.02.24
+DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 01.02.24
+DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 01.02.24
+DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 01.02.24
+DGI.KT6R11.MANDANT.TXT : last exported on 01.02.24</t>
         </is>
       </c>
       <c r="E11" s="11" t="inlineStr">
@@ -1324,12 +1324,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 31.01.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 01.02.24</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 31.01.24</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 01.02.24</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="C13" s="10" t="inlineStr">
         <is>
-          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 26.01.24
+          <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 01.02.24
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
 DLV.I5XKT6.AU.A.ZIP : last exported on 12.01.24
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
@@ -1367,7 +1367,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 31.01.24
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 01.02.24
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 31.01.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 31.01.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 01.02.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 01.02.24</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 31.01.24
-DHP.KUDKT6.ORGUNITS : last exported on 01.02.24
-DHS.R11KT6.HSB02ALL : last exported on 31.01.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 01.02.24
+DHP.KUDKT6.ORGUNITS : last exported on 02.02.24
+DHS.R11KT6.HSB02ALL : last exported on 01.02.24</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 31.01.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 31.01.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 31.01.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 31.01.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 31.01.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 31.01.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 31.01.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 31.01.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 31.01.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 31.01.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 01.02.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 01.02.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 01.02.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 01.02.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 01.02.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 01.02.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 01.02.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 01.02.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 01.02.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 01.02.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1603,38 +1603,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 31.01.24</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 01.02.24</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 31.01.24
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 31.01.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 31.01.24
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 31.01.24
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 31.01.24
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 31.01.24
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 31.01.24
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 31.01.24
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 31.01.24
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 31.01.24
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 31.01.24
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 31.01.24
-DEL.N1LKT6.MT.??????.G : last exported on 31.01.24
-DEL.N1LKT6.MT.??????.U : last exported on 31.01.24
-DEL.N1LKT6.MT.??????.AS : last exported on 31.01.24
-DVL.N1LN5X.VLM.DSP : last exported on 31.01.24
-DVL.N1LN5X.VLM.WT : last exported on 31.01.24
-DDS.N1LR11.DSP : last exported on 31.01.24
-DDS.N1LR11.WT : last exported on 31.01.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 31.01.24
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 31.01.24
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 31.01.24
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 31.01.24
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 31.01.24
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 31.01.24
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 31.01.24
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 31.01.24</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 01.02.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 01.02.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 01.02.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 01.02.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 01.02.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 01.02.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 01.02.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 01.02.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 01.02.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 01.02.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 01.02.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 01.02.24
+DEL.N1LKT6.MT.??????.G : last exported on 01.02.24
+DEL.N1LKT6.MT.??????.U : last exported on 01.02.24
+DEL.N1LKT6.MT.??????.AS : last exported on 01.02.24
+DVL.N1LN5X.VLM.DSP : last exported on 01.02.24
+DVL.N1LN5X.VLM.WT : last exported on 01.02.24
+DDS.N1LR11.DSP : last exported on 01.02.24
+DDS.N1LR11.WT : last exported on 01.02.24
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 01.02.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 01.02.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 01.02.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 01.02.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 01.02.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 01.02.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 01.02.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 01.02.24</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,52 +1662,52 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 01.02.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 01.02.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 01.02.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 01.02.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 01.02.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 01.02.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 01.02.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 01.02.24
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 02.02.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 02.02.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 02.02.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 02.02.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 02.02.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 02.02.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 02.02.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 02.02.24
 DDC.R11KT6.ELFI.MD.TXT : last exported on 28.01.24
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 31.01.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 01.02.24
 DDC.R11KT6.ELFI.PK.TXT : last exported on 28.01.24
 DDC.R11KT6.ELFI.PR.TXT : last exported on 28.01.24</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 31.01.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 31.01.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 31.01.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 31.01.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 31.01.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 31.01.24
-DEL.N1LKT6.EC.??????.G : last exported on 31.01.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 31.01.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 31.01.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 31.01.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 31.01.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 31.01.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 31.01.24
-DEL.N1LKT6.EC.??????.U : last exported on 31.01.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 31.01.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 31.01.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 31.01.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 31.01.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 31.01.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 31.01.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 31.01.24
-DEL.N1LKT6.EC.??????.AS : last exported on 31.01.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 31.01.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 31.01.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 31.01.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 31.01.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 31.01.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 31.01.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 31.01.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 31.01.24</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 01.02.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 01.02.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 01.02.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 01.02.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 01.02.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 01.02.24
+DEL.N1LKT6.EC.??????.G : last exported on 01.02.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 01.02.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 01.02.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 01.02.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 01.02.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 01.02.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 01.02.24
+DEL.N1LKT6.EC.??????.U : last exported on 01.02.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 01.02.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 01.02.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 01.02.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 01.02.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 01.02.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 01.02.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 01.02.24
+DEL.N1LKT6.EC.??????.AS : last exported on 01.02.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 01.02.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 01.02.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 01.02.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 01.02.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 01.02.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 01.02.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 01.02.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 01.02.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 07.02.24 15:55
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 02.02.2024</t>
+          <t>Date - 07.02.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 01.02.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 05.02.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 02.02.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 02.02.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 02.02.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 02.02.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 02.02.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 02.02.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 02.02.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 02.02.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 02.02.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 02.02.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 02.02.24</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 07.02.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 07.02.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 07.02.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 07.02.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 07.02.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 07.02.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 07.02.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 07.02.24
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 06.02.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 06.02.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 06.02.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1032,13 +1032,13 @@
       </c>
       <c r="C5" s="10" t="inlineStr">
         <is>
-          <t>DGQ.R11KT6.KDNR.TXT : last exported on 05.01.24</t>
+          <t>DGQ.R11KT6.KDNR.TXT : last exported on 02.02.24</t>
         </is>
       </c>
       <c r="D5" s="10" t="inlineStr">
         <is>
-          <t>DDS.N1LR11.KDNRTXT : last exported on 08.01.24
-DVL.N1LN5X.VLM.KDNRTXT : last exported on 08.01.24</t>
+          <t>DDS.N1LR11.KDNRTXT : last exported on 05.02.24
+DVL.N1LN5X.VLM.KDNRTXT : last exported on 05.02.24</t>
         </is>
       </c>
       <c r="E5" s="11" t="inlineStr">
@@ -1066,22 +1066,22 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 29.01.24
-DEH.N3LKT6.AP.COMPL.SNK : last exported on 29.01.24</t>
+          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 05.02.24
+DEH.N3LKT6.AP.COMPL.SNK : last exported on 05.02.24</t>
         </is>
       </c>
       <c r="D6" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 29.01.24
-DEL.N1LN3L.DN.F.GPL.DMP : last exported on 29.01.24
-DEL.N1LN3L.DN.F.GTR.DMP : last exported on 29.01.24
-DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 29.01.24
-DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 29.01.24
-DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 29.01.24
-DEL.N1LN0R.DN.F.CPD.DMP : last exported on 29.01.24
-DEL.N1LN0R.DN.F.CPL.DMP : last exported on 29.01.24
-DEL.KT6E35.SN.F.GGO.ZIP : last exported on 29.01.24
-DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 29.01.24</t>
+          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 05.02.24
+DEL.N1LN3L.DN.F.GPL.DMP : last exported on 05.02.24
+DEL.N1LN3L.DN.F.GTR.DMP : last exported on 05.02.24
+DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 05.02.24
+DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 05.02.24
+DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 05.02.24
+DEL.N1LN0R.DN.F.CPD.DMP : last exported on 05.02.24
+DEL.N1LN0R.DN.F.CPL.DMP : last exported on 05.02.24
+DEL.KT6E35.SN.F.GGO.ZIP : last exported on 05.02.24
+DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 05.02.24</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
@@ -1109,29 +1109,29 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 01.02.24
-DLV.KZ6KT6.WI.V.ZIP : last exported on 01.02.24
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 05.02.24
+DLV.KZ6KT6.WI.V.ZIP : last exported on 05.02.24
 DLV.RPKKT6.WI.S.ZIP : last exported on 31.01.24
-DLV.I5XKT6.WI.A.ZIP : last exported on 01.02.24
-DIT.E35KT6.WI.ZIP : last exported on 01.02.24
-DEL.K2PKT6.WI.ZIP : last exported on 01.02.24
+DLV.I5XKT6.WI.A.ZIP : last exported on 05.02.24
+DIT.E35KT6.WI.ZIP : last exported on 05.02.24
+DEL.K2PKT6.WI.ZIP : last exported on 05.02.24
 DEL.R7AKT6.WI.ZIP : last exported on 25.01.24
 DEL.N5FKT6.WI.ZIP : last exported on 26.01.24</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 01.02.24
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 01.02.24
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 01.02.24
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 01.02.24
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 01.02.24
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 01.02.24
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 01.02.24
-DEL.KT6E35.WI.GGO.ZIP : last exported on 01.02.24
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 01.02.24
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 01.02.24
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 01.02.24</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 07.02.24
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 07.02.24
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 07.02.24
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 07.02.24
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 07.02.24
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 07.02.24
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 07.02.24
+DEL.KT6E35.WI.GGO.ZIP : last exported on 06.02.24
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 06.02.24
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 06.02.24
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 06.02.24</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1194,15 +1194,15 @@
       </c>
       <c r="C9" s="10" t="inlineStr">
         <is>
-          <t>ElsaPro-GUI_&lt;language&gt;.xml : last exported on 25.02.23</t>
+          <t>ElsaPro-GUI_&lt;language&gt;.xml : last exported on 06.02.24</t>
         </is>
       </c>
       <c r="D9" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TRANS.F.GPD.DMP : last exported on 25.02.23
-DEL.N1LN3L.TRANS.F.GPL.DMP : last exported on 25.02.23
+          <t>DEL.N1LN3L.TRANS.F.GPD.DMP : last exported on 06.02.24
+DEL.N1LN3L.TRANS.F.GPL.DMP : last exported on 06.02.24
 DEL.N1LN3L.TRANS.F.GTR.DMP : last exported on 25.02.23
-DEL.N1LKQQ.TRANS.F.UPD.DMP : last exported on 25.02.23
+DEL.N1LKQQ.TRANS.F.UPD.DMP : last exported on 06.02.24
 DEL.N1LN3L.TRANS.F.ASPD.DMP : last exported on 25.02.23
 DEL.N1LN3L.TRANS.F.ASPL.DMP : last exported on 25.02.23
 DEL.N1LN0R.TRANS.D.CPD.DMP : last exported on 25.02.23
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 02.02.24
-DGV.N3LKT6.EPELS.??????.ZIP : last exported on 29.01.24</t>
+DEL.N3LKT6.HST.??????.ZIP : last exported on 06.02.24
+DGV.N3LKT6.EPELS.??????.ZIP : last exported on 05.02.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 01.02.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 01.02.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 01.02.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 01.02.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 01.02.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 01.02.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 01.02.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 01.02.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 01.02.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 01.02.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 01.02.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 01.02.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 01.02.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 01.02.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 01.02.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 01.02.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 01.02.24</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 06.02.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 06.02.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 06.02.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 06.02.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 06.02.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 06.02.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 06.02.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 06.02.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 05.02.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 05.02.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 05.02.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 05.02.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 05.02.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 05.02.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 05.02.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 05.02.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 05.02.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 01.02.24
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 01.02.24
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 01.02.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 06.02.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 01.02.24
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 01.02.24
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 01.02.24
@@ -1324,12 +1324,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 01.02.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 05.02.24</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 01.02.24</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 03.02.24</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1367,7 +1367,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 01.02.24
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 06.02.24
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 01.02.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 01.02.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 06.02.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 06.02.24</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 01.02.24
-DHP.KUDKT6.ORGUNITS : last exported on 02.02.24
-DHS.R11KT6.HSB02ALL : last exported on 01.02.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 05.02.24
+DHP.KUDKT6.ORGUNITS : last exported on 06.02.24
+DHS.R11KT6.HSB02ALL : last exported on 05.02.24</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 01.02.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 01.02.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 01.02.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 01.02.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 01.02.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 01.02.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 01.02.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 01.02.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 01.02.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 01.02.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 06.02.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 06.02.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 06.02.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 06.02.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 06.02.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 06.02.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 06.02.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 06.02.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 06.02.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 06.02.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1575,7 +1575,7 @@
       </c>
       <c r="D18" s="15" t="inlineStr">
         <is>
-          <t>DEL.N1LE35.TRANS.ZIP : last exported on 28.01.24</t>
+          <t>DEL.N1LE35.TRANS.ZIP : last exported on 04.02.24</t>
         </is>
       </c>
       <c r="E18" s="11" t="inlineStr">
@@ -1603,38 +1603,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 01.02.24</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 05.02.24</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 01.02.24
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 01.02.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 01.02.24
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 01.02.24
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 01.02.24
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 01.02.24
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 01.02.24
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 01.02.24
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 01.02.24
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 01.02.24
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 01.02.24
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 01.02.24
-DEL.N1LKT6.MT.??????.G : last exported on 01.02.24
-DEL.N1LKT6.MT.??????.U : last exported on 01.02.24
-DEL.N1LKT6.MT.??????.AS : last exported on 01.02.24
-DVL.N1LN5X.VLM.DSP : last exported on 01.02.24
-DVL.N1LN5X.VLM.WT : last exported on 01.02.24
-DDS.N1LR11.DSP : last exported on 01.02.24
-DDS.N1LR11.WT : last exported on 01.02.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 01.02.24
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 01.02.24
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 01.02.24
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 01.02.24
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 01.02.24
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 01.02.24
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 01.02.24
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 01.02.24</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 06.02.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 06.02.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 06.02.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 06.02.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 06.02.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 06.02.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 06.02.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 06.02.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 06.02.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 06.02.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 06.02.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 06.02.24
+DEL.N1LKT6.MT.??????.G : last exported on 06.02.24
+DEL.N1LKT6.MT.??????.U : last exported on 06.02.24
+DEL.N1LKT6.MT.??????.AS : last exported on 06.02.24
+DVL.N1LN5X.VLM.DSP : last exported on 06.02.24
+DVL.N1LN5X.VLM.WT : last exported on 06.02.24
+DDS.N1LR11.DSP : last exported on 06.02.24
+DDS.N1LR11.WT : last exported on 06.02.24
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 05.02.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 05.02.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 05.02.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 05.02.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 05.02.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 05.02.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 05.02.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 05.02.24</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,52 +1662,52 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 02.02.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 02.02.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 02.02.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 02.02.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 02.02.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 02.02.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 02.02.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 02.02.24
-DDC.R11KT6.ELFI.MD.TXT : last exported on 28.01.24
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 01.02.24
-DDC.R11KT6.ELFI.PK.TXT : last exported on 28.01.24
-DDC.R11KT6.ELFI.PR.TXT : last exported on 28.01.24</t>
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 06.02.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 06.02.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 06.02.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 06.02.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 06.02.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 06.02.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 06.02.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 06.02.24
+DDC.R11KT6.ELFI.MD.TXT : last exported on 04.02.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 05.02.24
+DDC.R11KT6.ELFI.PK.TXT : last exported on 04.02.24
+DDC.R11KT6.ELFI.PR.TXT : last exported on 04.02.24</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 01.02.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 01.02.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 01.02.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 01.02.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 01.02.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 01.02.24
-DEL.N1LKT6.EC.??????.G : last exported on 01.02.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 01.02.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 01.02.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 01.02.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 01.02.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 01.02.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 01.02.24
-DEL.N1LKT6.EC.??????.U : last exported on 01.02.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 01.02.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 01.02.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 01.02.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 01.02.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 01.02.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 01.02.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 01.02.24
-DEL.N1LKT6.EC.??????.AS : last exported on 01.02.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 01.02.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 01.02.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 01.02.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 01.02.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 01.02.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 01.02.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 01.02.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 01.02.24</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 06.02.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 06.02.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 06.02.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 06.02.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 06.02.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 06.02.24
+DEL.N1LKT6.EC.??????.G : last exported on 06.02.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 06.02.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 06.02.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 06.02.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 06.02.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 06.02.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 06.02.24
+DEL.N1LKT6.EC.??????.U : last exported on 06.02.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 06.02.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 06.02.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 06.02.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 06.02.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 06.02.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 06.02.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 06.02.24
+DEL.N1LKT6.EC.??????.AS : last exported on 06.02.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 06.02.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 06.02.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 06.02.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 06.02.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 06.02.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 06.02.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 06.02.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 05.02.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 09.02.24 14:39
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 07.02.2024</t>
+          <t>Date - 09.02.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 05.02.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 08.02.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 07.02.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 07.02.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 07.02.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 07.02.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 07.02.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 07.02.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 07.02.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 07.02.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 06.02.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 06.02.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 06.02.24</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 09.02.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 09.02.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 09.02.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 09.02.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 09.02.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 09.02.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 09.02.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 09.02.24
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 09.02.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 09.02.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 09.02.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1109,29 +1109,29 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 05.02.24
-DLV.KZ6KT6.WI.V.ZIP : last exported on 05.02.24
-DLV.RPKKT6.WI.S.ZIP : last exported on 31.01.24
-DLV.I5XKT6.WI.A.ZIP : last exported on 05.02.24
-DIT.E35KT6.WI.ZIP : last exported on 05.02.24
-DEL.K2PKT6.WI.ZIP : last exported on 05.02.24
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 08.02.24
+DLV.KZ6KT6.WI.V.ZIP : last exported on 08.02.24
+DLV.RPKKT6.WI.S.ZIP : last exported on 08.02.24
+DLV.I5XKT6.WI.A.ZIP : last exported on 08.02.24
+DIT.E35KT6.WI.ZIP : last exported on 08.02.24
+DEL.K2PKT6.WI.ZIP : last exported on 08.02.24
 DEL.R7AKT6.WI.ZIP : last exported on 25.01.24
-DEL.N5FKT6.WI.ZIP : last exported on 26.01.24</t>
+DEL.N5FKT6.WI.ZIP : last exported on 06.02.24</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 07.02.24
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 07.02.24
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 07.02.24
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 07.02.24
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 07.02.24
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 07.02.24
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 07.02.24
-DEL.KT6E35.WI.GGO.ZIP : last exported on 06.02.24
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 06.02.24
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 06.02.24
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 06.02.24</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 08.02.24
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 08.02.24
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 08.02.24
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 08.02.24
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 08.02.24
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 08.02.24
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 08.02.24
+DEL.KT6E35.WI.GGO.ZIP : last exported on 08.02.24
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 08.02.24
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 08.02.24
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 08.02.24</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 06.02.24
+DEL.N3LKT6.HST.??????.ZIP : last exported on 09.02.24
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 05.02.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 06.02.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 06.02.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 06.02.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 06.02.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 06.02.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 06.02.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 06.02.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 06.02.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 05.02.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 05.02.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 05.02.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 05.02.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 05.02.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 05.02.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 05.02.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 05.02.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 05.02.24</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 08.02.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 08.02.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 08.02.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 08.02.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 08.02.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 08.02.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 08.02.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 08.02.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 08.02.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 08.02.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 08.02.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 08.02.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 08.02.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 08.02.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 08.02.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 08.02.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 08.02.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 01.02.24
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 01.02.24
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 06.02.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 08.02.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 01.02.24
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 01.02.24
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 01.02.24
@@ -1324,12 +1324,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 05.02.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 08.02.24</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 03.02.24</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 08.02.24</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1367,7 +1367,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 06.02.24
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 07.02.24
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
 DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
@@ -1407,27 +1407,27 @@
 DGQ.R11KT6.PKAT.US2.TXT : last exported on 31.01.24
 DGQ.R11KT6.BSITK.TXT : last exported on 31.01.24
 DGQ.R11KT6.BSITX.TXT : last exported on 31.01.24
-DGQ.R31KT6.BSIVMC.TXT : last exported on 12.12.23
-DGQ.R31KT6.PKATC.TXT : last exported on 12.12.23
-DEL.KMPKT6.APOS.DATA.ZIP : last exported on 31.01.24</t>
+DGQ.R31KT6.BSIVMC.TXT : last exported on 06.02.24
+DGQ.R31KT6.PKATC.TXT : last exported on 06.02.24
+DEL.KMPKT6.APOS.DATA.ZIP : last exported on 07.02.24</t>
         </is>
       </c>
       <c r="D14" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 31.01.24
-DEL.N1LN3L.AP.F.GPL.DMP : last exported on 31.01.24
-DEL.N1LN3L.AP.F.GTR.DMP : last exported on 31.01.24
-DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 31.01.24
-DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 31.01.24
-DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 31.01.24
-DEL.N1LN0R.AP.F.CPD.DMP : last exported on 31.01.24
-DEL.N1LN0R.AP.F.CPL.DMP : last exported on 31.01.24
-DEL.N1LR31.AP.F.PPS.DMP : last exported on 31.01.24
-DEL.KT6E35.AP.F.DB.ZIP : last exported on 31.01.24
-DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 31.01.24
-DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 31.01.24
-DVL.KT6N5X.VLM.AP.ZIP : last exported on 31.01.24
-DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 31.01.24</t>
+          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 07.02.24
+DEL.N1LN3L.AP.F.GPL.DMP : last exported on 07.02.24
+DEL.N1LN3L.AP.F.GTR.DMP : last exported on 07.02.24
+DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 07.02.24
+DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 07.02.24
+DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 07.02.24
+DEL.N1LN0R.AP.F.CPD.DMP : last exported on 07.02.24
+DEL.N1LN0R.AP.F.CPL.DMP : last exported on 07.02.24
+DEL.N1LR31.AP.F.PPS.DMP : last exported on 07.02.24
+DEL.KT6E35.AP.F.DB.ZIP : last exported on 07.02.24
+DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 07.02.24
+DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 07.02.24
+DVL.KT6N5X.VLM.AP.ZIP : last exported on 07.02.24
+DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 07.02.24</t>
         </is>
       </c>
       <c r="E14" s="11" t="inlineStr">
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 06.02.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 06.02.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 08.02.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 08.02.24</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 05.02.24
-DHP.KUDKT6.ORGUNITS : last exported on 06.02.24
-DHS.R11KT6.HSB02ALL : last exported on 05.02.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 08.02.24
+DHP.KUDKT6.ORGUNITS : last exported on 09.02.24
+DHS.R11KT6.HSB02ALL : last exported on 08.02.24</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 06.02.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 06.02.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 06.02.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 06.02.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 06.02.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 06.02.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 06.02.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 06.02.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 06.02.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 06.02.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 08.02.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 08.02.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 08.02.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 08.02.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 08.02.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 08.02.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 08.02.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 08.02.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 08.02.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 08.02.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1603,38 +1603,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 05.02.24</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 08.02.24</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 06.02.24
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 06.02.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 06.02.24
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 06.02.24
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 06.02.24
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 06.02.24
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 06.02.24
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 06.02.24
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 06.02.24
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 06.02.24
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 06.02.24
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 06.02.24
-DEL.N1LKT6.MT.??????.G : last exported on 06.02.24
-DEL.N1LKT6.MT.??????.U : last exported on 06.02.24
-DEL.N1LKT6.MT.??????.AS : last exported on 06.02.24
-DVL.N1LN5X.VLM.DSP : last exported on 06.02.24
-DVL.N1LN5X.VLM.WT : last exported on 06.02.24
-DDS.N1LR11.DSP : last exported on 06.02.24
-DDS.N1LR11.WT : last exported on 06.02.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 05.02.24
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 05.02.24
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 05.02.24
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 05.02.24
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 05.02.24
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 05.02.24
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 05.02.24
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 05.02.24</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 08.02.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 08.02.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 08.02.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 08.02.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 08.02.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 08.02.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 08.02.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 08.02.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 08.02.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 08.02.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 08.02.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 08.02.24
+DEL.N1LKT6.MT.??????.G : last exported on 08.02.24
+DEL.N1LKT6.MT.??????.U : last exported on 08.02.24
+DEL.N1LKT6.MT.??????.AS : last exported on 08.02.24
+DVL.N1LN5X.VLM.DSP : last exported on 08.02.24
+DVL.N1LN5X.VLM.WT : last exported on 08.02.24
+DDS.N1LR11.DSP : last exported on 08.02.24
+DDS.N1LR11.WT : last exported on 08.02.24
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 08.02.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 08.02.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 08.02.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 08.02.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 08.02.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 08.02.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 08.02.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 08.02.24</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,52 +1662,52 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 06.02.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 06.02.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 06.02.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 06.02.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 06.02.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 06.02.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 06.02.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 06.02.24
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 09.02.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 09.02.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 09.02.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 09.02.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 09.02.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 09.02.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 09.02.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 09.02.24
 DDC.R11KT6.ELFI.MD.TXT : last exported on 04.02.24
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 05.02.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 08.02.24
 DDC.R11KT6.ELFI.PK.TXT : last exported on 04.02.24
 DDC.R11KT6.ELFI.PR.TXT : last exported on 04.02.24</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 06.02.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 06.02.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 06.02.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 06.02.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 06.02.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 06.02.24
-DEL.N1LKT6.EC.??????.G : last exported on 06.02.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 06.02.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 06.02.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 06.02.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 06.02.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 06.02.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 06.02.24
-DEL.N1LKT6.EC.??????.U : last exported on 06.02.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 06.02.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 06.02.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 06.02.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 06.02.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 06.02.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 06.02.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 06.02.24
-DEL.N1LKT6.EC.??????.AS : last exported on 06.02.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 06.02.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 06.02.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 06.02.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 06.02.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 06.02.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 06.02.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 06.02.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 05.02.24</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 08.02.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 08.02.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 08.02.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 08.02.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 08.02.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 08.02.24
+DEL.N1LKT6.EC.??????.G : last exported on 08.02.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 08.02.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 08.02.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 08.02.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 08.02.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 08.02.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 08.02.24
+DEL.N1LKT6.EC.??????.U : last exported on 08.02.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 08.02.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 08.02.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 08.02.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 08.02.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 08.02.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 08.02.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 08.02.24
+DEL.N1LKT6.EC.??????.AS : last exported on 08.02.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 08.02.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 08.02.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 08.02.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 08.02.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 08.02.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 08.02.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 08.02.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 08.02.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 12.02.24 13:03
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 09.02.2024</t>
+          <t>Date - 12.02.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 08.02.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 09.02.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 09.02.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 09.02.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 09.02.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 09.02.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 09.02.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 09.02.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 09.02.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 09.02.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 09.02.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 09.02.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 09.02.24</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 10.02.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 10.02.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 11.02.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 10.02.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 10.02.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 10.02.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 10.02.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 10.02.24
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 10.02.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 10.02.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 10.02.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1066,22 +1066,22 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 05.02.24
-DEH.N3LKT6.AP.COMPL.SNK : last exported on 05.02.24</t>
+          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 12.02.24
+DEH.N3LKT6.AP.COMPL.SNK : last exported on 12.02.24</t>
         </is>
       </c>
       <c r="D6" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 05.02.24
-DEL.N1LN3L.DN.F.GPL.DMP : last exported on 05.02.24
-DEL.N1LN3L.DN.F.GTR.DMP : last exported on 05.02.24
-DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 05.02.24
-DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 05.02.24
-DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 05.02.24
-DEL.N1LN0R.DN.F.CPD.DMP : last exported on 05.02.24
-DEL.N1LN0R.DN.F.CPL.DMP : last exported on 05.02.24
-DEL.KT6E35.SN.F.GGO.ZIP : last exported on 05.02.24
-DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 05.02.24</t>
+          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 12.02.24
+DEL.N1LN3L.DN.F.GPL.DMP : last exported on 12.02.24
+DEL.N1LN3L.DN.F.GTR.DMP : last exported on 12.02.24
+DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 12.02.24
+DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 12.02.24
+DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 12.02.24
+DEL.N1LN0R.DN.F.CPD.DMP : last exported on 12.02.24
+DEL.N1LN0R.DN.F.CPL.DMP : last exported on 12.02.24
+DEL.KT6E35.SN.F.GGO.ZIP : last exported on 12.02.24
+DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 12.02.24</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
@@ -1109,29 +1109,29 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 08.02.24
-DLV.KZ6KT6.WI.V.ZIP : last exported on 08.02.24
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 09.02.24
+DLV.KZ6KT6.WI.V.ZIP : last exported on 11.02.24
 DLV.RPKKT6.WI.S.ZIP : last exported on 08.02.24
-DLV.I5XKT6.WI.A.ZIP : last exported on 08.02.24
-DIT.E35KT6.WI.ZIP : last exported on 08.02.24
-DEL.K2PKT6.WI.ZIP : last exported on 08.02.24
+DLV.I5XKT6.WI.A.ZIP : last exported on 11.02.24
+DIT.E35KT6.WI.ZIP : last exported on 09.02.24
+DEL.K2PKT6.WI.ZIP : last exported on 11.02.24
 DEL.R7AKT6.WI.ZIP : last exported on 25.01.24
 DEL.N5FKT6.WI.ZIP : last exported on 06.02.24</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 08.02.24
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 08.02.24
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 08.02.24
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 08.02.24
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 08.02.24
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 08.02.24
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 08.02.24
-DEL.KT6E35.WI.GGO.ZIP : last exported on 08.02.24
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 08.02.24
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 08.02.24
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 08.02.24</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 12.02.24
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 12.02.24
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 12.02.24
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 12.02.24
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 12.02.24
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 12.02.24
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 12.02.24
+DEL.KT6E35.WI.GGO.ZIP : last exported on 12.02.24
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 12.02.24
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 12.02.24
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 12.02.24</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 09.02.24
+DEL.N3LKT6.HST.??????.ZIP : last exported on 12.02.24
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 05.02.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 08.02.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 08.02.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 08.02.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 08.02.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 08.02.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 08.02.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 08.02.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 08.02.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 08.02.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 08.02.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 08.02.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 08.02.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 08.02.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 08.02.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 08.02.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 08.02.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 08.02.24</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 11.02.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 11.02.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 11.02.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 11.02.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 11.02.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 11.02.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 11.02.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 11.02.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 11.02.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 11.02.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 11.02.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 11.02.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 11.02.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 11.02.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 11.02.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 11.02.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 11.02.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 01.02.24
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 01.02.24
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 08.02.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 11.02.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 01.02.24
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 01.02.24
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 01.02.24
@@ -1324,12 +1324,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 08.02.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 09.02.24</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 08.02.24</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 10.02.24</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 08.02.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 08.02.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 11.02.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 11.02.24</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 08.02.24
-DHP.KUDKT6.ORGUNITS : last exported on 09.02.24
-DHS.R11KT6.HSB02ALL : last exported on 08.02.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 11.02.24
+DHP.KUDKT6.ORGUNITS : last exported on 12.02.24
+DHS.R11KT6.HSB02ALL : last exported on 09.02.24</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 08.02.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 08.02.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 08.02.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 08.02.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 08.02.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 08.02.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 08.02.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 08.02.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 08.02.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 08.02.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 09.02.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 09.02.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 11.02.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 09.02.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 09.02.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 09.02.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 09.02.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 09.02.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 09.02.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 09.02.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1575,7 +1575,7 @@
       </c>
       <c r="D18" s="15" t="inlineStr">
         <is>
-          <t>DEL.N1LE35.TRANS.ZIP : last exported on 04.02.24</t>
+          <t>DEL.N1LE35.TRANS.ZIP : last exported on 11.02.24</t>
         </is>
       </c>
       <c r="E18" s="11" t="inlineStr">
@@ -1603,38 +1603,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 08.02.24</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 10.02.24</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 08.02.24
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 08.02.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 08.02.24
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 08.02.24
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 08.02.24
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 08.02.24
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 08.02.24
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 08.02.24
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 08.02.24
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 08.02.24
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 08.02.24
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 08.02.24
-DEL.N1LKT6.MT.??????.G : last exported on 08.02.24
-DEL.N1LKT6.MT.??????.U : last exported on 08.02.24
-DEL.N1LKT6.MT.??????.AS : last exported on 08.02.24
-DVL.N1LN5X.VLM.DSP : last exported on 08.02.24
-DVL.N1LN5X.VLM.WT : last exported on 08.02.24
-DDS.N1LR11.DSP : last exported on 08.02.24
-DDS.N1LR11.WT : last exported on 08.02.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 08.02.24
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 08.02.24
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 08.02.24
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 08.02.24
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 08.02.24
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 08.02.24
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 08.02.24
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 08.02.24</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 10.02.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 10.02.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 11.02.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 10.02.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 10.02.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 10.02.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 10.02.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 10.02.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 10.02.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 10.02.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 10.02.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 10.02.24
+DEL.N1LKT6.MT.??????.G : last exported on 10.02.24
+DEL.N1LKT6.MT.??????.U : last exported on 10.02.24
+DEL.N1LKT6.MT.??????.AS : last exported on 10.02.24
+DVL.N1LN5X.VLM.DSP : last exported on 10.02.24
+DVL.N1LN5X.VLM.WT : last exported on 10.02.24
+DDS.N1LR11.DSP : last exported on 10.02.24
+DDS.N1LR11.WT : last exported on 10.02.24
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 10.02.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 10.02.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 10.02.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 10.02.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 10.02.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 10.02.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 10.02.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 10.02.24</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,52 +1662,52 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 09.02.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 09.02.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 09.02.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 09.02.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 09.02.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 09.02.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 09.02.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 09.02.24
-DDC.R11KT6.ELFI.MD.TXT : last exported on 04.02.24
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 08.02.24
-DDC.R11KT6.ELFI.PK.TXT : last exported on 04.02.24
-DDC.R11KT6.ELFI.PR.TXT : last exported on 04.02.24</t>
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 12.02.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 12.02.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 12.02.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 12.02.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 12.02.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 12.02.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 12.02.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 12.02.24
+DDC.R11KT6.ELFI.MD.TXT : last exported on 11.02.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 09.02.24
+DDC.R11KT6.ELFI.PK.TXT : last exported on 11.02.24
+DDC.R11KT6.ELFI.PR.TXT : last exported on 11.02.24</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 08.02.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 08.02.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 08.02.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 08.02.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 08.02.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 08.02.24
-DEL.N1LKT6.EC.??????.G : last exported on 08.02.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 08.02.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 08.02.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 08.02.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 08.02.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 08.02.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 08.02.24
-DEL.N1LKT6.EC.??????.U : last exported on 08.02.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 08.02.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 08.02.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 08.02.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 08.02.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 08.02.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 08.02.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 08.02.24
-DEL.N1LKT6.EC.??????.AS : last exported on 08.02.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 08.02.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 08.02.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 08.02.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 08.02.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 08.02.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 08.02.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 08.02.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 08.02.24</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 11.02.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 11.02.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 11.02.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 11.02.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 11.02.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 11.02.24
+DEL.N1LKT6.EC.??????.G : last exported on 11.02.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 11.02.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 11.02.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 11.02.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 11.02.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 11.02.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 11.02.24
+DEL.N1LKT6.EC.??????.U : last exported on 11.02.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 11.02.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 11.02.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 11.02.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 11.02.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 11.02.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 11.02.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 11.02.24
+DEL.N1LKT6.EC.??????.AS : last exported on 11.02.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 11.02.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 11.02.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 11.02.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 11.02.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 11.02.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 11.02.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 11.02.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 11.02.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 15.02.24 13:26
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 12.02.2024</t>
+          <t>Date - 15.02.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 09.02.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 14.02.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 10.02.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 10.02.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 11.02.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 10.02.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 10.02.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 10.02.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 10.02.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 10.02.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 10.02.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 10.02.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 10.02.24</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 15.02.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 15.02.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 15.02.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 15.02.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 15.02.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 15.02.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 15.02.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 15.02.24
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 15.02.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 15.02.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 15.02.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1109,29 +1109,29 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 09.02.24
-DLV.KZ6KT6.WI.V.ZIP : last exported on 11.02.24
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 13.02.24
+DLV.KZ6KT6.WI.V.ZIP : last exported on 14.02.24
 DLV.RPKKT6.WI.S.ZIP : last exported on 08.02.24
-DLV.I5XKT6.WI.A.ZIP : last exported on 11.02.24
-DIT.E35KT6.WI.ZIP : last exported on 09.02.24
-DEL.K2PKT6.WI.ZIP : last exported on 11.02.24
+DLV.I5XKT6.WI.A.ZIP : last exported on 14.02.24
+DIT.E35KT6.WI.ZIP : last exported on 14.02.24
+DEL.K2PKT6.WI.ZIP : last exported on 14.02.24
 DEL.R7AKT6.WI.ZIP : last exported on 25.01.24
 DEL.N5FKT6.WI.ZIP : last exported on 06.02.24</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 12.02.24
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 12.02.24
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 12.02.24
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 12.02.24
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 12.02.24
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 12.02.24
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 12.02.24
-DEL.KT6E35.WI.GGO.ZIP : last exported on 12.02.24
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 12.02.24
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 12.02.24
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 12.02.24</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 15.02.24
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 15.02.24
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 15.02.24
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 15.02.24
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 15.02.24
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 15.02.24
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 15.02.24
+DEL.KT6E35.WI.GGO.ZIP : last exported on 15.02.24
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 15.02.24
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 15.02.24
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 15.02.24</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1235,29 +1235,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 12.02.24
-DGV.N3LKT6.EPELS.??????.ZIP : last exported on 05.02.24</t>
+DEL.N3LKT6.HST.??????.ZIP : last exported on 15.02.24
+DGV.N3LKT6.EPELS.??????.ZIP : last exported on 12.02.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 11.02.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 11.02.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 11.02.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 11.02.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 11.02.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 11.02.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 11.02.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 11.02.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 11.02.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 11.02.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 11.02.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 11.02.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 11.02.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 11.02.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 11.02.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 11.02.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 11.02.24</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 14.02.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 14.02.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 14.02.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 14.02.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 14.02.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 14.02.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 14.02.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 14.02.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 14.02.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 14.02.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 14.02.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 14.02.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 14.02.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 14.02.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 14.02.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 14.02.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 14.02.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 01.02.24
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 01.02.24
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 11.02.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 14.02.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 01.02.24
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 01.02.24
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 01.02.24
@@ -1324,12 +1324,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 09.02.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 14.02.24</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 10.02.24</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 14.02.24</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1409,25 +1409,25 @@
 DGQ.R11KT6.BSITX.TXT : last exported on 31.01.24
 DGQ.R31KT6.BSIVMC.TXT : last exported on 06.02.24
 DGQ.R31KT6.PKATC.TXT : last exported on 06.02.24
-DEL.KMPKT6.APOS.DATA.ZIP : last exported on 07.02.24</t>
+DEL.KMPKT6.APOS.DATA.ZIP : last exported on 14.02.24</t>
         </is>
       </c>
       <c r="D14" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 07.02.24
-DEL.N1LN3L.AP.F.GPL.DMP : last exported on 07.02.24
-DEL.N1LN3L.AP.F.GTR.DMP : last exported on 07.02.24
-DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 07.02.24
-DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 07.02.24
-DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 07.02.24
-DEL.N1LN0R.AP.F.CPD.DMP : last exported on 07.02.24
-DEL.N1LN0R.AP.F.CPL.DMP : last exported on 07.02.24
-DEL.N1LR31.AP.F.PPS.DMP : last exported on 07.02.24
-DEL.KT6E35.AP.F.DB.ZIP : last exported on 07.02.24
-DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 07.02.24
-DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 07.02.24
-DVL.KT6N5X.VLM.AP.ZIP : last exported on 07.02.24
-DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 07.02.24</t>
+          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 14.02.24
+DEL.N1LN3L.AP.F.GPL.DMP : last exported on 14.02.24
+DEL.N1LN3L.AP.F.GTR.DMP : last exported on 14.02.24
+DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 14.02.24
+DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 14.02.24
+DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 14.02.24
+DEL.N1LN0R.AP.F.CPD.DMP : last exported on 14.02.24
+DEL.N1LN0R.AP.F.CPL.DMP : last exported on 14.02.24
+DEL.N1LR31.AP.F.PPS.DMP : last exported on 14.02.24
+DEL.KT6E35.AP.F.DB.ZIP : last exported on 14.02.24
+DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 14.02.24
+DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 14.02.24
+DVL.KT6N5X.VLM.AP.ZIP : last exported on 14.02.24
+DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 14.02.24</t>
         </is>
       </c>
       <c r="E14" s="11" t="inlineStr">
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 11.02.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 11.02.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 14.02.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 14.02.24</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 11.02.24
-DHP.KUDKT6.ORGUNITS : last exported on 12.02.24
-DHS.R11KT6.HSB02ALL : last exported on 09.02.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 14.02.24
+DHP.KUDKT6.ORGUNITS : last exported on 15.02.24
+DHS.R11KT6.HSB02ALL : last exported on 14.02.24</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 09.02.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 09.02.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 11.02.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 09.02.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 09.02.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 09.02.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 09.02.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 09.02.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 09.02.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 09.02.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 14.02.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 14.02.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 14.02.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 14.02.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 14.02.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 14.02.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 14.02.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 14.02.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 14.02.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 14.02.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1603,38 +1603,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 10.02.24</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 14.02.24</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 10.02.24
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 10.02.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 11.02.24
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 10.02.24
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 10.02.24
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 10.02.24
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 10.02.24
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 10.02.24
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 10.02.24
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 10.02.24
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 10.02.24
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 10.02.24
-DEL.N1LKT6.MT.??????.G : last exported on 10.02.24
-DEL.N1LKT6.MT.??????.U : last exported on 10.02.24
-DEL.N1LKT6.MT.??????.AS : last exported on 10.02.24
-DVL.N1LN5X.VLM.DSP : last exported on 10.02.24
-DVL.N1LN5X.VLM.WT : last exported on 10.02.24
-DDS.N1LR11.DSP : last exported on 10.02.24
-DDS.N1LR11.WT : last exported on 10.02.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 10.02.24
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 10.02.24
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 10.02.24
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 10.02.24
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 10.02.24
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 10.02.24
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 10.02.24
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 10.02.24</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 14.02.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 14.02.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 14.02.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 14.02.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 14.02.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 14.02.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 14.02.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 14.02.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 14.02.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 14.02.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 14.02.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 14.02.24
+DEL.N1LKT6.MT.??????.G : last exported on 14.02.24
+DEL.N1LKT6.MT.??????.U : last exported on 14.02.24
+DEL.N1LKT6.MT.??????.AS : last exported on 14.02.24
+DVL.N1LN5X.VLM.DSP : last exported on 14.02.24
+DVL.N1LN5X.VLM.WT : last exported on 14.02.24
+DDS.N1LR11.DSP : last exported on 14.02.24
+DDS.N1LR11.WT : last exported on 14.02.24
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 14.02.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 14.02.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 14.02.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 14.02.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 14.02.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 14.02.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 14.02.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 14.02.24</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,52 +1662,52 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 12.02.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 12.02.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 12.02.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 12.02.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 12.02.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 12.02.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 12.02.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 12.02.24
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 15.02.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 15.02.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 15.02.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 15.02.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 15.02.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 15.02.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 15.02.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 15.02.24
 DDC.R11KT6.ELFI.MD.TXT : last exported on 11.02.24
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 09.02.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 14.02.24
 DDC.R11KT6.ELFI.PK.TXT : last exported on 11.02.24
 DDC.R11KT6.ELFI.PR.TXT : last exported on 11.02.24</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 11.02.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 11.02.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 11.02.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 11.02.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 11.02.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 11.02.24
-DEL.N1LKT6.EC.??????.G : last exported on 11.02.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 11.02.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 11.02.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 11.02.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 11.02.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 11.02.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 11.02.24
-DEL.N1LKT6.EC.??????.U : last exported on 11.02.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 11.02.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 11.02.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 11.02.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 11.02.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 11.02.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 11.02.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 11.02.24
-DEL.N1LKT6.EC.??????.AS : last exported on 11.02.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 11.02.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 11.02.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 11.02.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 11.02.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 11.02.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 11.02.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 11.02.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 11.02.24</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 14.02.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 14.02.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 14.02.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 14.02.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 14.02.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 14.02.24
+DEL.N1LKT6.EC.??????.G : last exported on 14.02.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 14.02.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 14.02.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 14.02.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 14.02.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 14.02.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 14.02.24
+DEL.N1LKT6.EC.??????.U : last exported on 14.02.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 14.02.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 14.02.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 14.02.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 14.02.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 14.02.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 14.02.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 14.02.24
+DEL.N1LKT6.EC.??????.AS : last exported on 14.02.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 14.02.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 14.02.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 14.02.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 14.02.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 14.02.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 14.02.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 14.02.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 14.02.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 20.02.24 13:26
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 15.02.2024</t>
+          <t>Date - 20.02.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 14.02.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 19.02.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 15.02.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 15.02.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 15.02.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 15.02.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 15.02.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 15.02.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 15.02.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 15.02.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 15.02.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 15.02.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 15.02.24</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 20.02.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 20.02.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 20.02.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 20.02.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 20.02.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 20.02.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 20.02.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 20.02.24
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 20.02.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 20.02.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 20.02.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1066,22 +1066,22 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 12.02.24
-DEH.N3LKT6.AP.COMPL.SNK : last exported on 12.02.24</t>
+          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 19.02.24
+DEH.N3LKT6.AP.COMPL.SNK : last exported on 19.02.24</t>
         </is>
       </c>
       <c r="D6" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 12.02.24
-DEL.N1LN3L.DN.F.GPL.DMP : last exported on 12.02.24
-DEL.N1LN3L.DN.F.GTR.DMP : last exported on 12.02.24
-DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 12.02.24
-DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 12.02.24
-DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 12.02.24
-DEL.N1LN0R.DN.F.CPD.DMP : last exported on 12.02.24
-DEL.N1LN0R.DN.F.CPL.DMP : last exported on 12.02.24
-DEL.KT6E35.SN.F.GGO.ZIP : last exported on 12.02.24
-DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 12.02.24</t>
+          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 19.02.24
+DEL.N1LN3L.DN.F.GPL.DMP : last exported on 19.02.24
+DEL.N1LN3L.DN.F.GTR.DMP : last exported on 19.02.24
+DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 19.02.24
+DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 19.02.24
+DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 19.02.24
+DEL.N1LN0R.DN.F.CPD.DMP : last exported on 19.02.24
+DEL.N1LN0R.DN.F.CPL.DMP : last exported on 19.02.24
+DEL.KT6E35.SN.F.GGO.ZIP : last exported on 19.02.24
+DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 19.02.24</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
@@ -1109,29 +1109,29 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 13.02.24
-DLV.KZ6KT6.WI.V.ZIP : last exported on 14.02.24
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 16.02.24
+DLV.KZ6KT6.WI.V.ZIP : last exported on 19.02.24
 DLV.RPKKT6.WI.S.ZIP : last exported on 08.02.24
-DLV.I5XKT6.WI.A.ZIP : last exported on 14.02.24
-DIT.E35KT6.WI.ZIP : last exported on 14.02.24
-DEL.K2PKT6.WI.ZIP : last exported on 14.02.24
+DLV.I5XKT6.WI.A.ZIP : last exported on 19.02.24
+DIT.E35KT6.WI.ZIP : last exported on 19.02.24
+DEL.K2PKT6.WI.ZIP : last exported on 19.02.24
 DEL.R7AKT6.WI.ZIP : last exported on 25.01.24
 DEL.N5FKT6.WI.ZIP : last exported on 06.02.24</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 15.02.24
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 15.02.24
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 15.02.24
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 15.02.24
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 15.02.24
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 15.02.24
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 15.02.24
-DEL.KT6E35.WI.GGO.ZIP : last exported on 15.02.24
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 15.02.24
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 15.02.24
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 15.02.24</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 20.02.24
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 20.02.24
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 20.02.24
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 20.02.24
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 20.02.24
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 20.02.24
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 20.02.24
+DEL.KT6E35.WI.GGO.ZIP : last exported on 20.02.24
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 20.02.24
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 20.02.24
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 20.02.24</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1234,30 +1234,30 @@
       </c>
       <c r="C10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 07.12.23
-DEL.N3LKT6.HST.??????.ZIP : last exported on 15.02.24
-DGV.N3LKT6.EPELS.??????.ZIP : last exported on 12.02.24</t>
+          <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 16.02.24
+DEL.N3LKT6.HST.??????.ZIP : last exported on 20.02.24
+DGV.N3LKT6.EPELS.??????.ZIP : last exported on 19.02.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 14.02.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 14.02.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 14.02.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 14.02.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 14.02.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 14.02.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 14.02.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 14.02.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 14.02.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 14.02.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 14.02.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 14.02.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 14.02.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 14.02.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 14.02.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 14.02.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 14.02.24</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 19.02.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 19.02.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 19.02.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 19.02.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 19.02.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 19.02.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 19.02.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 19.02.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 19.02.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 19.02.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 19.02.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 19.02.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 19.02.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 19.02.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 19.02.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 19.02.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 19.02.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1292,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 01.02.24
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 01.02.24
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 14.02.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 19.02.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 01.02.24
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 01.02.24
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 01.02.24
@@ -1324,12 +1324,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 14.02.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 19.02.24</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 14.02.24</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 17.02.24</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1359,19 +1359,19 @@
         <is>
           <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 01.02.24
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
-DLV.I5XKT6.AU.A.ZIP : last exported on 12.01.24
+DLV.I5XKT6.AU.A.ZIP : last exported on 16.02.24
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
         </is>
       </c>
       <c r="D13" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 23.12.23
-DEL.N1LN3L.AU.D.GPL.DMP : last exported on 23.12.23
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 07.02.24
-DEL.N1LN0R.AU.D.CPD.DMP : last exported on 23.12.23
-DEL.N1LN0R.AU.D.CPL.DMP : last exported on 23.12.23
-DEL.KT6E35.AU.GGO.ZIP : last exported on 23.12.23
-DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 23.12.23</t>
+          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 17.02.24
+DEL.N1LN3L.AU.D.GPL.DMP : last exported on 17.02.24
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 19.02.24
+DEL.N1LN0R.AU.D.CPD.DMP : last exported on 17.02.24
+DEL.N1LN0R.AU.D.CPL.DMP : last exported on 17.02.24
+DEL.KT6E35.AU.GGO.ZIP : last exported on 17.02.24
+DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 17.02.24</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1460,8 +1460,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 14.02.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 14.02.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 19.02.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 19.02.24</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1489,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 14.02.24
-DHP.KUDKT6.ORGUNITS : last exported on 15.02.24
-DHS.R11KT6.HSB02ALL : last exported on 14.02.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 19.02.24
+DHP.KUDKT6.ORGUNITS : last exported on 20.02.24
+DHS.R11KT6.HSB02ALL : last exported on 19.02.24</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 14.02.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 14.02.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 14.02.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 14.02.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 14.02.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 14.02.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 14.02.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 14.02.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 14.02.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 14.02.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 19.02.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 19.02.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 19.02.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 19.02.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 19.02.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 19.02.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 19.02.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 19.02.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 19.02.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 19.02.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1575,7 +1575,7 @@
       </c>
       <c r="D18" s="15" t="inlineStr">
         <is>
-          <t>DEL.N1LE35.TRANS.ZIP : last exported on 11.02.24</t>
+          <t>DEL.N1LE35.TRANS.ZIP : last exported on 18.02.24</t>
         </is>
       </c>
       <c r="E18" s="11" t="inlineStr">
@@ -1603,38 +1603,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 14.02.24</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 19.02.24</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 14.02.24
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 14.02.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 14.02.24
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 14.02.24
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 14.02.24
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 14.02.24
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 14.02.24
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 14.02.24
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 14.02.24
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 14.02.24
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 14.02.24
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 14.02.24
-DEL.N1LKT6.MT.??????.G : last exported on 14.02.24
-DEL.N1LKT6.MT.??????.U : last exported on 14.02.24
-DEL.N1LKT6.MT.??????.AS : last exported on 14.02.24
-DVL.N1LN5X.VLM.DSP : last exported on 14.02.24
-DVL.N1LN5X.VLM.WT : last exported on 14.02.24
-DDS.N1LR11.DSP : last exported on 14.02.24
-DDS.N1LR11.WT : last exported on 14.02.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 14.02.24
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 14.02.24
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 14.02.24
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 14.02.24
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 14.02.24
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 14.02.24
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 14.02.24
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 14.02.24</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 19.02.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 19.02.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 19.02.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 19.02.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 19.02.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 19.02.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 19.02.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 19.02.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 19.02.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 19.02.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 19.02.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 19.02.24
+DEL.N1LKT6.MT.??????.G : last exported on 19.02.24
+DEL.N1LKT6.MT.??????.U : last exported on 19.02.24
+DEL.N1LKT6.MT.??????.AS : last exported on 19.02.24
+DVL.N1LN5X.VLM.DSP : last exported on 19.02.24
+DVL.N1LN5X.VLM.WT : last exported on 19.02.24
+DDS.N1LR11.DSP : last exported on 19.02.24
+DDS.N1LR11.WT : last exported on 19.02.24
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 19.02.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 19.02.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 19.02.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 19.02.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 19.02.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 19.02.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 19.02.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 19.02.24</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,52 +1662,52 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 15.02.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 15.02.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 15.02.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 15.02.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 15.02.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 15.02.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 15.02.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 15.02.24
-DDC.R11KT6.ELFI.MD.TXT : last exported on 11.02.24
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 14.02.24
-DDC.R11KT6.ELFI.PK.TXT : last exported on 11.02.24
-DDC.R11KT6.ELFI.PR.TXT : last exported on 11.02.24</t>
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 20.02.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 20.02.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 20.02.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 20.02.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 20.02.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 20.02.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 20.02.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 20.02.24
+DDC.R11KT6.ELFI.MD.TXT : last exported on 18.02.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 19.02.24
+DDC.R11KT6.ELFI.PK.TXT : last exported on 18.02.24
+DDC.R11KT6.ELFI.PR.TXT : last exported on 18.02.24</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 14.02.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 14.02.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 14.02.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 14.02.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 14.02.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 14.02.24
-DEL.N1LKT6.EC.??????.G : last exported on 14.02.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 14.02.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 14.02.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 14.02.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 14.02.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 14.02.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 14.02.24
-DEL.N1LKT6.EC.??????.U : last exported on 14.02.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 14.02.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 14.02.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 14.02.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 14.02.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 14.02.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 14.02.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 14.02.24
-DEL.N1LKT6.EC.??????.AS : last exported on 14.02.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 14.02.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 14.02.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 14.02.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 14.02.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 14.02.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 14.02.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 14.02.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 14.02.24</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 19.02.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 19.02.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 19.02.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 19.02.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 19.02.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 19.02.24
+DEL.N1LKT6.EC.??????.G : last exported on 19.02.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 19.02.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 19.02.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 19.02.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 19.02.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 19.02.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 19.02.24
+DEL.N1LKT6.EC.??????.U : last exported on 19.02.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 19.02.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 19.02.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 19.02.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 19.02.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 19.02.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 19.02.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 19.02.24
+DEL.N1LKT6.EC.??????.AS : last exported on 19.02.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 19.02.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 19.02.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 19.02.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 19.02.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 19.02.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 19.02.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 19.02.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 19.02.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 22.02.24 11:57
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 20.02.2024</t>
+          <t>Date - 22.02.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 19.02.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 21.02.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 20.02.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 20.02.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 20.02.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 20.02.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 20.02.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 20.02.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 20.02.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 20.02.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 20.02.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 20.02.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 20.02.24</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 22.02.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 22.02.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 22.02.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 22.02.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 22.02.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 22.02.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 22.02.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 22.02.24
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 22.02.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 22.02.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 22.02.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1109,29 +1109,29 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 16.02.24
-DLV.KZ6KT6.WI.V.ZIP : last exported on 19.02.24
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 21.02.24
+DLV.KZ6KT6.WI.V.ZIP : last exported on 21.02.24
 DLV.RPKKT6.WI.S.ZIP : last exported on 08.02.24
-DLV.I5XKT6.WI.A.ZIP : last exported on 19.02.24
-DIT.E35KT6.WI.ZIP : last exported on 19.02.24
-DEL.K2PKT6.WI.ZIP : last exported on 19.02.24
-DEL.R7AKT6.WI.ZIP : last exported on 25.01.24
+DLV.I5XKT6.WI.A.ZIP : last exported on 21.02.24
+DIT.E35KT6.WI.ZIP : last exported on 21.02.24
+DEL.K2PKT6.WI.ZIP : last exported on 21.02.24
+DEL.R7AKT6.WI.ZIP : last exported on 22.02.24
 DEL.N5FKT6.WI.ZIP : last exported on 06.02.24</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 20.02.24
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 20.02.24
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 20.02.24
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 20.02.24
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 20.02.24
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 20.02.24
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 20.02.24
-DEL.KT6E35.WI.GGO.ZIP : last exported on 20.02.24
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 20.02.24
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 20.02.24
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 20.02.24</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 21.02.24
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 21.02.24
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 21.02.24
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 21.02.24
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 21.02.24
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 21.02.24
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 21.02.24
+DEL.KT6E35.WI.GGO.ZIP : last exported on 21.02.24
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 21.02.24
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 21.02.24
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 21.02.24</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1201,12 +1201,10 @@
         <is>
           <t>DEL.N1LN3L.TRANS.F.GPD.DMP : last exported on 06.02.24
 DEL.N1LN3L.TRANS.F.GPL.DMP : last exported on 06.02.24
-DEL.N1LN3L.TRANS.F.GTR.DMP : last exported on 25.02.23
+DEL.N1LN3L.TRANS.F.GTR.DMP : last exported on 06.02.24
 DEL.N1LKQQ.TRANS.F.UPD.DMP : last exported on 06.02.24
-DEL.N1LN3L.TRANS.F.ASPD.DMP : last exported on 25.02.23
-DEL.N1LN3L.TRANS.F.ASPL.DMP : last exported on 25.02.23
-DEL.N1LN0R.TRANS.D.CPD.DMP : last exported on 25.02.23
-DEL.N1LN0R.TRANS.D.CPL.DMP : last exported on 25.02.23</t>
+DEL.N1LN0R.TRANS.D.CPD.DMP : last exported on 06.02.24
+DEL.N1LN0R.TRANS.D.CPL.DMP : last exported on 06.02.24</t>
         </is>
       </c>
       <c r="E9" s="11" t="inlineStr">
@@ -1235,29 +1233,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 16.02.24
-DEL.N3LKT6.HST.??????.ZIP : last exported on 20.02.24
+DEL.N3LKT6.HST.??????.ZIP : last exported on 22.02.24
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 19.02.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 19.02.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 19.02.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 19.02.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 19.02.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 19.02.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 19.02.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 19.02.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 19.02.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 19.02.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 19.02.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 19.02.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 19.02.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 19.02.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 19.02.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 19.02.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 19.02.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 19.02.24</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 21.02.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 21.02.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 21.02.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 21.02.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 21.02.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 21.02.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 21.02.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 21.02.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 21.02.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 21.02.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 21.02.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 21.02.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 21.02.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 21.02.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 21.02.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 21.02.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 21.02.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1292,7 +1290,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 01.02.24
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 01.02.24
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 19.02.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 21.02.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 01.02.24
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 01.02.24
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 01.02.24
@@ -1324,12 +1322,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 19.02.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 21.02.24</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 17.02.24</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 21.02.24</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1367,7 +1365,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 17.02.24
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 17.02.24
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 19.02.24
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 21.02.24
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 17.02.24
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 17.02.24
 DEL.KT6E35.AU.GGO.ZIP : last exported on 17.02.24
@@ -1409,25 +1407,25 @@
 DGQ.R11KT6.BSITX.TXT : last exported on 31.01.24
 DGQ.R31KT6.BSIVMC.TXT : last exported on 06.02.24
 DGQ.R31KT6.PKATC.TXT : last exported on 06.02.24
-DEL.KMPKT6.APOS.DATA.ZIP : last exported on 14.02.24</t>
+DEL.KMPKT6.APOS.DATA.ZIP : last exported on 21.02.24</t>
         </is>
       </c>
       <c r="D14" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 14.02.24
-DEL.N1LN3L.AP.F.GPL.DMP : last exported on 14.02.24
-DEL.N1LN3L.AP.F.GTR.DMP : last exported on 14.02.24
-DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 14.02.24
-DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 14.02.24
-DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 14.02.24
-DEL.N1LN0R.AP.F.CPD.DMP : last exported on 14.02.24
-DEL.N1LN0R.AP.F.CPL.DMP : last exported on 14.02.24
-DEL.N1LR31.AP.F.PPS.DMP : last exported on 14.02.24
-DEL.KT6E35.AP.F.DB.ZIP : last exported on 14.02.24
-DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 14.02.24
-DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 14.02.24
-DVL.KT6N5X.VLM.AP.ZIP : last exported on 14.02.24
-DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 14.02.24</t>
+          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 21.02.24
+DEL.N1LN3L.AP.F.GPL.DMP : last exported on 21.02.24
+DEL.N1LN3L.AP.F.GTR.DMP : last exported on 21.02.24
+DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 21.02.24
+DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 21.02.24
+DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 21.02.24
+DEL.N1LN0R.AP.F.CPD.DMP : last exported on 21.02.24
+DEL.N1LN0R.AP.F.CPL.DMP : last exported on 21.02.24
+DEL.N1LR31.AP.F.PPS.DMP : last exported on 21.02.24
+DEL.KT6E35.AP.F.DB.ZIP : last exported on 21.02.24
+DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 21.02.24
+DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 21.02.24
+DVL.KT6N5X.VLM.AP.ZIP : last exported on 21.02.24
+DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 21.02.24</t>
         </is>
       </c>
       <c r="E14" s="11" t="inlineStr">
@@ -1460,8 +1458,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 19.02.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 19.02.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 21.02.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 21.02.24</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1489,23 +1487,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 19.02.24
-DHP.KUDKT6.ORGUNITS : last exported on 20.02.24
-DHS.R11KT6.HSB02ALL : last exported on 19.02.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 21.02.24
+DHP.KUDKT6.ORGUNITS : last exported on 22.02.24
+DHS.R11KT6.HSB02ALL : last exported on 21.02.24</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 19.02.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 19.02.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 19.02.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 19.02.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 19.02.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 19.02.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 19.02.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 19.02.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 19.02.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 19.02.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 21.02.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 21.02.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 21.02.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 21.02.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 21.02.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 21.02.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 21.02.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 21.02.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 21.02.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 21.02.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1603,38 +1601,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 19.02.24</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 21.02.24</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 19.02.24
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 19.02.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 19.02.24
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 19.02.24
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 19.02.24
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 19.02.24
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 19.02.24
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 19.02.24
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 19.02.24
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 19.02.24
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 19.02.24
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 19.02.24
-DEL.N1LKT6.MT.??????.G : last exported on 19.02.24
-DEL.N1LKT6.MT.??????.U : last exported on 19.02.24
-DEL.N1LKT6.MT.??????.AS : last exported on 19.02.24
-DVL.N1LN5X.VLM.DSP : last exported on 19.02.24
-DVL.N1LN5X.VLM.WT : last exported on 19.02.24
-DDS.N1LR11.DSP : last exported on 19.02.24
-DDS.N1LR11.WT : last exported on 19.02.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 19.02.24
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 19.02.24
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 19.02.24
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 19.02.24
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 19.02.24
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 19.02.24
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 19.02.24
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 19.02.24</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 21.02.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 21.02.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 21.02.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 21.02.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 21.02.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 21.02.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 21.02.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 21.02.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 21.02.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 21.02.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 21.02.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 21.02.24
+DEL.N1LKT6.MT.??????.G : last exported on 21.02.24
+DEL.N1LKT6.MT.??????.U : last exported on 21.02.24
+DEL.N1LKT6.MT.??????.AS : last exported on 21.02.24
+DVL.N1LN5X.VLM.DSP : last exported on 21.02.24
+DVL.N1LN5X.VLM.WT : last exported on 21.02.24
+DDS.N1LR11.DSP : last exported on 21.02.24
+DDS.N1LR11.WT : last exported on 21.02.24
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 21.02.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 21.02.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 21.02.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 21.02.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 21.02.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 21.02.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 21.02.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 21.02.24</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1662,52 +1660,52 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 20.02.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 20.02.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 20.02.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 20.02.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 20.02.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 20.02.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 20.02.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 20.02.24
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 22.02.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 22.02.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 22.02.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 22.02.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 22.02.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 22.02.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 22.02.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 22.02.24
 DDC.R11KT6.ELFI.MD.TXT : last exported on 18.02.24
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 19.02.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 21.02.24
 DDC.R11KT6.ELFI.PK.TXT : last exported on 18.02.24
 DDC.R11KT6.ELFI.PR.TXT : last exported on 18.02.24</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 19.02.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 19.02.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 19.02.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 19.02.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 19.02.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 19.02.24
-DEL.N1LKT6.EC.??????.G : last exported on 19.02.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 19.02.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 19.02.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 19.02.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 19.02.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 19.02.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 19.02.24
-DEL.N1LKT6.EC.??????.U : last exported on 19.02.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 19.02.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 19.02.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 19.02.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 19.02.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 19.02.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 19.02.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 19.02.24
-DEL.N1LKT6.EC.??????.AS : last exported on 19.02.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 19.02.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 19.02.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 19.02.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 19.02.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 19.02.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 19.02.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 19.02.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 19.02.24</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 21.02.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 21.02.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 21.02.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 21.02.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 21.02.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 21.02.24
+DEL.N1LKT6.EC.??????.G : last exported on 21.02.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 21.02.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 21.02.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 21.02.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 21.02.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 21.02.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 21.02.24
+DEL.N1LKT6.EC.??????.U : last exported on 21.02.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 21.02.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 21.02.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 21.02.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 21.02.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 21.02.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 21.02.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 21.02.24
+DEL.N1LKT6.EC.??????.AS : last exported on 21.02.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 21.02.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 21.02.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 21.02.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 21.02.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 21.02.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 21.02.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 21.02.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 21.02.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 26.02.24 15:01
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 22.02.2024</t>
+          <t>Date - 26.02.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 21.02.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 23.02.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 22.02.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 22.02.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 22.02.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 22.02.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 22.02.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 22.02.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 22.02.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 22.02.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 22.02.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 22.02.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 22.02.24</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 24.02.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 24.02.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 25.02.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 24.02.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 24.02.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 24.02.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 24.02.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 24.02.24
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 24.02.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 24.02.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 24.02.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1066,22 +1066,22 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 19.02.24
-DEH.N3LKT6.AP.COMPL.SNK : last exported on 19.02.24</t>
+          <t>DEH.N3LKT6.AP.COMPLETE.SNK : last exported on 26.02.24
+DEH.N3LKT6.AP.COMPL.SNK : last exported on 26.02.24</t>
         </is>
       </c>
       <c r="D6" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 19.02.24
-DEL.N1LN3L.DN.F.GPL.DMP : last exported on 19.02.24
-DEL.N1LN3L.DN.F.GTR.DMP : last exported on 19.02.24
-DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 19.02.24
-DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 19.02.24
-DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 19.02.24
-DEL.N1LN0R.DN.F.CPD.DMP : last exported on 19.02.24
-DEL.N1LN0R.DN.F.CPL.DMP : last exported on 19.02.24
-DEL.KT6E35.SN.F.GGO.ZIP : last exported on 19.02.24
-DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 19.02.24</t>
+          <t>DEL.N1LN3L.DN.F.GPD.DMP : last exported on 26.02.24
+DEL.N1LN3L.DN.F.GPL.DMP : last exported on 26.02.24
+DEL.N1LN3L.DN.F.GTR.DMP : last exported on 26.02.24
+DEL.N1LKQQ.DN.F.UPD.DMP : last exported on 26.02.24
+DEL.N1LN3L.DN.F.ASPD.DMP : last exported on 26.02.24
+DEL.N1LN3L.DN.F.ASPL.DMP : last exported on 26.02.24
+DEL.N1LN0R.DN.F.CPD.DMP : last exported on 26.02.24
+DEL.N1LN0R.DN.F.CPL.DMP : last exported on 26.02.24
+DEL.KT6E35.SN.F.GGO.ZIP : last exported on 26.02.24
+DEL.KT6N5M.SN.F.GGO.ZIP : last exported on 26.02.24</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
@@ -1109,29 +1109,29 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 21.02.24
-DLV.KZ6KT6.WI.V.ZIP : last exported on 21.02.24
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 23.02.24
+DLV.KZ6KT6.WI.V.ZIP : last exported on 24.02.24
 DLV.RPKKT6.WI.S.ZIP : last exported on 08.02.24
-DLV.I5XKT6.WI.A.ZIP : last exported on 21.02.24
-DIT.E35KT6.WI.ZIP : last exported on 21.02.24
-DEL.K2PKT6.WI.ZIP : last exported on 21.02.24
+DLV.I5XKT6.WI.A.ZIP : last exported on 24.02.24
+DIT.E35KT6.WI.ZIP : last exported on 23.02.24
+DEL.K2PKT6.WI.ZIP : last exported on 24.02.24
 DEL.R7AKT6.WI.ZIP : last exported on 22.02.24
-DEL.N5FKT6.WI.ZIP : last exported on 06.02.24</t>
+DEL.N5FKT6.WI.ZIP : last exported on 23.02.24</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 21.02.24
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 21.02.24
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 21.02.24
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 21.02.24
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 21.02.24
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 21.02.24
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 21.02.24
-DEL.KT6E35.WI.GGO.ZIP : last exported on 21.02.24
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 21.02.24
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 21.02.24
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 21.02.24</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 25.02.24
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 25.02.24
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 26.02.24
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 25.02.24
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 25.02.24
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 25.02.24
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 25.02.24
+DEL.KT6E35.WI.GGO.ZIP : last exported on 25.02.24
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 25.02.24
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 25.02.24
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 25.02.24</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1233,29 +1233,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 16.02.24
-DEL.N3LKT6.HST.??????.ZIP : last exported on 22.02.24
+DEL.N3LKT6.HST.??????.ZIP : last exported on 26.02.24
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 19.02.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 21.02.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 21.02.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 21.02.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 21.02.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 21.02.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 21.02.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 21.02.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 21.02.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 21.02.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 21.02.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 21.02.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 21.02.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 21.02.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 21.02.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 21.02.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 21.02.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 21.02.24</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 25.02.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 25.02.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 25.02.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 25.02.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 25.02.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 25.02.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 25.02.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 25.02.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 25.02.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 25.02.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 25.02.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 25.02.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 25.02.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 25.02.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 25.02.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 25.02.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 25.02.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1290,7 +1290,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 01.02.24
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 01.02.24
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 21.02.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 25.02.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 01.02.24
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 01.02.24
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 01.02.24
@@ -1322,12 +1322,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 21.02.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 23.02.24</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 21.02.24</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 24.02.24</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1357,19 +1357,19 @@
         <is>
           <t>DLV.KZ6KT6.AU.V.ZIP : last exported on 01.02.24
 DLV.RPKKT6.AU.S.ZIP : last exported on 01.08.23
-DLV.I5XKT6.AU.A.ZIP : last exported on 16.02.24
+DLV.I5XKT6.AU.A.ZIP : last exported on 23.02.24
 DLV.R31KT6.AU.C.ZIP : last exported on 26.09.23</t>
         </is>
       </c>
       <c r="D13" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 17.02.24
-DEL.N1LN3L.AU.D.GPL.DMP : last exported on 17.02.24
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 21.02.24
-DEL.N1LN0R.AU.D.CPD.DMP : last exported on 17.02.24
-DEL.N1LN0R.AU.D.CPL.DMP : last exported on 17.02.24
-DEL.KT6E35.AU.GGO.ZIP : last exported on 17.02.24
-DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 17.02.24</t>
+          <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 24.02.24
+DEL.N1LN3L.AU.D.GPL.DMP : last exported on 24.02.24
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 25.02.24
+DEL.N1LN0R.AU.D.CPD.DMP : last exported on 24.02.24
+DEL.N1LN0R.AU.D.CPL.DMP : last exported on 24.02.24
+DEL.KT6E35.AU.GGO.ZIP : last exported on 24.02.24
+DEL.KT6E35.AU.IMG.GGO.ZIP : last exported on 24.02.24</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -1458,8 +1458,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 21.02.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 21.02.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 25.02.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 25.02.24</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1487,23 +1487,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 21.02.24
-DHP.KUDKT6.ORGUNITS : last exported on 22.02.24
-DHS.R11KT6.HSB02ALL : last exported on 21.02.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 25.02.24
+DHP.KUDKT6.ORGUNITS : last exported on 26.02.24
+DHS.R11KT6.HSB02ALL : last exported on 23.02.24</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 21.02.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 21.02.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 21.02.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 21.02.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 21.02.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 21.02.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 21.02.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 21.02.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 21.02.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 21.02.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 23.02.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 23.02.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 25.02.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 23.02.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 23.02.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 23.02.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 23.02.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 23.02.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 23.02.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 23.02.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1573,7 +1573,7 @@
       </c>
       <c r="D18" s="15" t="inlineStr">
         <is>
-          <t>DEL.N1LE35.TRANS.ZIP : last exported on 18.02.24</t>
+          <t>DEL.N1LE35.TRANS.ZIP : last exported on 25.02.24</t>
         </is>
       </c>
       <c r="E18" s="11" t="inlineStr">
@@ -1601,38 +1601,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 21.02.24</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 24.02.24</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 21.02.24
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 21.02.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 21.02.24
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 21.02.24
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 21.02.24
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 21.02.24
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 21.02.24
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 21.02.24
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 21.02.24
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 21.02.24
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 21.02.24
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 21.02.24
-DEL.N1LKT6.MT.??????.G : last exported on 21.02.24
-DEL.N1LKT6.MT.??????.U : last exported on 21.02.24
-DEL.N1LKT6.MT.??????.AS : last exported on 21.02.24
-DVL.N1LN5X.VLM.DSP : last exported on 21.02.24
-DVL.N1LN5X.VLM.WT : last exported on 21.02.24
-DDS.N1LR11.DSP : last exported on 21.02.24
-DDS.N1LR11.WT : last exported on 21.02.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 21.02.24
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 21.02.24
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 21.02.24
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 21.02.24
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 21.02.24
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 21.02.24
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 21.02.24
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 21.02.24</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 24.02.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 24.02.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 25.02.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 24.02.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 24.02.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 24.02.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 24.02.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 24.02.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 24.02.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 24.02.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 24.02.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 24.02.24
+DEL.N1LKT6.MT.??????.G : last exported on 24.02.24
+DEL.N1LKT6.MT.??????.U : last exported on 24.02.24
+DEL.N1LKT6.MT.??????.AS : last exported on 24.02.24
+DVL.N1LN5X.VLM.DSP : last exported on 24.02.24
+DVL.N1LN5X.VLM.WT : last exported on 24.02.24
+DDS.N1LR11.DSP : last exported on 24.02.24
+DDS.N1LR11.WT : last exported on 24.02.24
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 24.02.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 24.02.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 24.02.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 24.02.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 24.02.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 24.02.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 24.02.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 24.02.24</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1660,52 +1660,52 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 22.02.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 22.02.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 22.02.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 22.02.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 22.02.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 22.02.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 22.02.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 22.02.24
-DDC.R11KT6.ELFI.MD.TXT : last exported on 18.02.24
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 21.02.24
-DDC.R11KT6.ELFI.PK.TXT : last exported on 18.02.24
-DDC.R11KT6.ELFI.PR.TXT : last exported on 18.02.24</t>
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 26.02.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 26.02.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 26.02.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 26.02.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 26.02.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 26.02.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 26.02.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 26.02.24
+DDC.R11KT6.ELFI.MD.TXT : last exported on 25.02.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 23.02.24
+DDC.R11KT6.ELFI.PK.TXT : last exported on 25.02.24
+DDC.R11KT6.ELFI.PR.TXT : last exported on 25.02.24</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 21.02.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 21.02.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 21.02.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 21.02.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 21.02.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 21.02.24
-DEL.N1LKT6.EC.??????.G : last exported on 21.02.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 21.02.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 21.02.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 21.02.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 21.02.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 21.02.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 21.02.24
-DEL.N1LKT6.EC.??????.U : last exported on 21.02.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 21.02.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 21.02.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 21.02.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 21.02.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 21.02.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 21.02.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 21.02.24
-DEL.N1LKT6.EC.??????.AS : last exported on 21.02.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 21.02.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 21.02.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 21.02.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 21.02.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 21.02.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 21.02.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 21.02.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 21.02.24</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 25.02.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 25.02.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 25.02.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 25.02.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 25.02.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 25.02.24
+DEL.N1LKT6.EC.??????.G : last exported on 25.02.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 25.02.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 25.02.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 25.02.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 25.02.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 25.02.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 25.02.24
+DEL.N1LKT6.EC.??????.U : last exported on 25.02.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 25.02.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 25.02.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 25.02.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 25.02.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 25.02.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 25.02.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 25.02.24
+DEL.N1LKT6.EC.??????.AS : last exported on 25.02.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 25.02.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 25.02.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 25.02.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 25.02.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 25.02.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 25.02.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 25.02.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 25.02.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 27.02.24 13:00
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 26.02.2024</t>
+          <t>Date - 27.02.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 23.02.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 26.02.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 24.02.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 24.02.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 25.02.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 24.02.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 24.02.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 24.02.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 24.02.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 24.02.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 24.02.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 24.02.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 24.02.24</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 27.02.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 27.02.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 27.02.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 27.02.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 27.02.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 27.02.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 27.02.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 27.02.24
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 27.02.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 27.02.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 27.02.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1037,8 +1037,8 @@
       </c>
       <c r="D5" s="10" t="inlineStr">
         <is>
-          <t>DDS.N1LR11.KDNRTXT : last exported on 05.02.24
-DVL.N1LN5X.VLM.KDNRTXT : last exported on 05.02.24</t>
+          <t>DDS.N1LR11.KDNRTXT : last exported on 26.02.24
+DVL.N1LN5X.VLM.KDNRTXT : last exported on 26.02.24</t>
         </is>
       </c>
       <c r="E5" s="11" t="inlineStr">
@@ -1111,27 +1111,27 @@
         <is>
           <t>DLV.R31KT6.WI.C.ZIP : last exported on 23.02.24
 DLV.KZ6KT6.WI.V.ZIP : last exported on 24.02.24
-DLV.RPKKT6.WI.S.ZIP : last exported on 08.02.24
+DLV.RPKKT6.WI.S.ZIP : last exported on 26.02.24
 DLV.I5XKT6.WI.A.ZIP : last exported on 24.02.24
-DIT.E35KT6.WI.ZIP : last exported on 23.02.24
-DEL.K2PKT6.WI.ZIP : last exported on 24.02.24
+DIT.E35KT6.WI.ZIP : last exported on 26.02.24
+DEL.K2PKT6.WI.ZIP : last exported on 26.02.24
 DEL.R7AKT6.WI.ZIP : last exported on 22.02.24
 DEL.N5FKT6.WI.ZIP : last exported on 23.02.24</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 25.02.24
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 25.02.24
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 26.02.24
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 25.02.24
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 25.02.24
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 25.02.24
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 25.02.24
-DEL.KT6E35.WI.GGO.ZIP : last exported on 25.02.24
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 25.02.24
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 25.02.24
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 25.02.24</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 27.02.24
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 27.02.24
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 27.02.24
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 27.02.24
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 27.02.24
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 27.02.24
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 27.02.24
+DEL.KT6E35.WI.GGO.ZIP : last exported on 27.02.24
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 27.02.24
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 27.02.24
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 27.02.24</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1233,29 +1233,29 @@
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 16.02.24
-DEL.N3LKT6.HST.??????.ZIP : last exported on 26.02.24
-DGV.N3LKT6.EPELS.??????.ZIP : last exported on 19.02.24</t>
+DEL.N3LKT6.HST.??????.ZIP : last exported on 27.02.24
+DGV.N3LKT6.EPELS.??????.ZIP : last exported on 26.02.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 25.02.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 25.02.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 25.02.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 25.02.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 25.02.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 25.02.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 25.02.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 25.02.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 25.02.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 25.02.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 25.02.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 25.02.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 25.02.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 25.02.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 25.02.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 25.02.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 25.02.24</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 26.02.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 26.02.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 26.02.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 26.02.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 26.02.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 26.02.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 26.02.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 26.02.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 26.02.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 26.02.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 26.02.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 26.02.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 26.02.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 26.02.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 26.02.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 26.02.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 26.02.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1290,7 +1290,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 01.02.24
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 01.02.24
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 25.02.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 26.02.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 01.02.24
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 01.02.24
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 01.02.24
@@ -1322,7 +1322,7 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 23.02.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 26.02.24</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
@@ -1365,7 +1365,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 24.02.24
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 24.02.24
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 25.02.24
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 26.02.24
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 24.02.24
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 24.02.24
 DEL.KT6E35.AU.GGO.ZIP : last exported on 24.02.24
@@ -1458,8 +1458,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 25.02.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 25.02.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 26.02.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 26.02.24</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1487,23 +1487,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 25.02.24
-DHP.KUDKT6.ORGUNITS : last exported on 26.02.24
-DHS.R11KT6.HSB02ALL : last exported on 23.02.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 26.02.24
+DHP.KUDKT6.ORGUNITS : last exported on 27.02.24
+DHS.R11KT6.HSB02ALL : last exported on 26.02.24</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 23.02.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 23.02.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 25.02.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 23.02.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 23.02.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 23.02.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 23.02.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 23.02.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 23.02.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 23.02.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 26.02.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 26.02.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 26.02.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 26.02.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 26.02.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 26.02.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 26.02.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 26.02.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 26.02.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 26.02.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1601,38 +1601,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 24.02.24</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 26.02.24</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 24.02.24
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 24.02.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 25.02.24
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 24.02.24
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 24.02.24
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 24.02.24
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 24.02.24
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 24.02.24
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 24.02.24
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 24.02.24
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 24.02.24
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 24.02.24
-DEL.N1LKT6.MT.??????.G : last exported on 24.02.24
-DEL.N1LKT6.MT.??????.U : last exported on 24.02.24
-DEL.N1LKT6.MT.??????.AS : last exported on 24.02.24
-DVL.N1LN5X.VLM.DSP : last exported on 24.02.24
-DVL.N1LN5X.VLM.WT : last exported on 24.02.24
-DDS.N1LR11.DSP : last exported on 24.02.24
-DDS.N1LR11.WT : last exported on 24.02.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 24.02.24
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 24.02.24
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 24.02.24
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 24.02.24
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 24.02.24
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 24.02.24
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 24.02.24
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 24.02.24</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 26.02.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 26.02.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 26.02.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 26.02.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 26.02.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 26.02.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 26.02.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 26.02.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 26.02.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 26.02.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 26.02.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 26.02.24
+DEL.N1LKT6.MT.??????.G : last exported on 26.02.24
+DEL.N1LKT6.MT.??????.U : last exported on 26.02.24
+DEL.N1LKT6.MT.??????.AS : last exported on 26.02.24
+DVL.N1LN5X.VLM.DSP : last exported on 26.02.24
+DVL.N1LN5X.VLM.WT : last exported on 26.02.24
+DDS.N1LR11.DSP : last exported on 26.02.24
+DDS.N1LR11.WT : last exported on 26.02.24
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 26.02.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 26.02.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 26.02.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 26.02.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 26.02.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 26.02.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 26.02.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 26.02.24</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1660,52 +1660,52 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 26.02.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 26.02.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 26.02.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 26.02.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 26.02.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 26.02.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 26.02.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 26.02.24
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 27.02.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 27.02.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 27.02.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 27.02.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 27.02.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 27.02.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 27.02.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 27.02.24
 DDC.R11KT6.ELFI.MD.TXT : last exported on 25.02.24
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 23.02.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 26.02.24
 DDC.R11KT6.ELFI.PK.TXT : last exported on 25.02.24
 DDC.R11KT6.ELFI.PR.TXT : last exported on 25.02.24</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 25.02.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 25.02.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 25.02.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 25.02.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 25.02.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 25.02.24
-DEL.N1LKT6.EC.??????.G : last exported on 25.02.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 25.02.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 25.02.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 25.02.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 25.02.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 25.02.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 25.02.24
-DEL.N1LKT6.EC.??????.U : last exported on 25.02.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 25.02.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 25.02.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 25.02.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 25.02.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 25.02.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 25.02.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 25.02.24
-DEL.N1LKT6.EC.??????.AS : last exported on 25.02.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 25.02.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 25.02.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 25.02.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 25.02.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 25.02.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 25.02.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 25.02.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 25.02.24</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 26.02.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 26.02.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 26.02.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 26.02.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 26.02.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 26.02.24
+DEL.N1LKT6.EC.??????.G : last exported on 26.02.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 26.02.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 26.02.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 26.02.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 26.02.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 26.02.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 26.02.24
+DEL.N1LKT6.EC.??????.U : last exported on 26.02.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 26.02.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 26.02.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 26.02.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 26.02.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 26.02.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 26.02.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 26.02.24
+DEL.N1LKT6.EC.??????.AS : last exported on 26.02.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 26.02.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 26.02.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 26.02.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 26.02.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 26.02.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 26.02.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 26.02.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 26.02.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Updated on 01.03.24 14:27
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -934,7 +934,7 @@
     <row r="2" ht="15.75" customHeight="1" thickBot="1" thickTop="1">
       <c r="A2" s="33" t="inlineStr">
         <is>
-          <t>Date - 27.02.2024</t>
+          <t>Date - 01.03.2024</t>
         </is>
       </c>
       <c r="B2" s="26" t="n"/>
@@ -1397,14 +1397,14 @@
       </c>
       <c r="C14" s="10" t="inlineStr">
         <is>
-          <t>DGQ.R11KT6.BSIVM.TXT : last exported on 31.01.24
-DGQ.R11KT6.BSIVM.C.TXT : last exported on 31.01.24
-DGQ.R11KT6.BSIVM.US2.TXT : last exported on 31.01.24
-DGQ.R11KT6.PKAT.TXT : last exported on 31.01.24
-DGQ.R11KT6.PKAT.C.TXT : last exported on 31.01.24
-DGQ.R11KT6.PKAT.US2.TXT : last exported on 31.01.24
-DGQ.R11KT6.BSITK.TXT : last exported on 31.01.24
-DGQ.R11KT6.BSITX.TXT : last exported on 31.01.24
+          <t>DGQ.R11KT6.BSIVM.TXT : last exported on 28.02.24
+DGQ.R11KT6.BSIVM.C.TXT : last exported on 28.02.24
+DGQ.R11KT6.BSIVM.US2.TXT : last exported on 28.02.24
+DGQ.R11KT6.PKAT.TXT : last exported on 28.02.24
+DGQ.R11KT6.PKAT.C.TXT : last exported on 28.02.24
+DGQ.R11KT6.PKAT.US2.TXT : last exported on 28.02.24
+DGQ.R11KT6.BSITK.TXT : last exported on 28.02.24
+DGQ.R11KT6.BSITX.TXT : last exported on 28.02.24
 DGQ.R31KT6.BSIVMC.TXT : last exported on 06.02.24
 DGQ.R31KT6.PKATC.TXT : last exported on 06.02.24
 DEL.KMPKT6.APOS.DATA.ZIP : last exported on 21.02.24</t>

</xml_diff>

<commit_message>
Updated on 01.03.24 14:42
</commit_message>
<xml_diff>
--- a/Daily_Job_Checklist_ELSADCP.xlsx
+++ b/Daily_Job_Checklist_ELSADCP.xlsx
@@ -989,22 +989,22 @@
       </c>
       <c r="C4" s="10" t="inlineStr">
         <is>
-          <t>DIT.E35KT6.SLP3.ZIP : last exported on 26.02.24</t>
+          <t>DIT.E35KT6.SLP3.ZIP : last exported on 29.02.24</t>
         </is>
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 27.02.24
-DEL.N1LN3L.WD.D.GPL.DMP : last exported on 27.02.24
-DEL.N1LN3L.WD.D.GTR.DMP : last exported on 27.02.24
-DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 27.02.24
-DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 27.02.24
-DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 27.02.24
-DEL.N1LN0R.WD.D.CPD.DMP : last exported on 27.02.24
-DEL.N1LN0R.WD.D.CPL.DMP : last exported on 27.02.24
-DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 27.02.24
-DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 27.02.24
-DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 27.02.24</t>
+          <t>DEL.N1LN3L.WD.D.GPD.DMP : last exported on 01.03.24
+DEL.N1LN3L.WD.D.GPL.DMP : last exported on 01.03.24
+DEL.N1LN3L.WD.D.GTR.DMP : last exported on 01.03.24
+DEL.N1LKQQ.WD.D.UPD.DMP : last exported on 01.03.24
+DEL.N1LN3L.WD.D.ASPD.DMP : last exported on 01.03.24
+DEL.N1LN3L.WD.D.ASPL.DMP : last exported on 01.03.24
+DEL.N1LN0R.WD.D.CPD.DMP : last exported on 01.03.24
+DEL.N1LN0R.WD.D.CPL.DMP : last exported on 01.03.24
+DEL.KT6N5M.SL.D.GGO.ZIP : last exported on 01.03.24
+DEL.KT6N5M.SL.D.UGO.ZIP : last exported on 01.03.24
+DEL.KT6N5M.SL.D.ASGO.ZIP : last exported on 01.03.24</t>
         </is>
       </c>
       <c r="E4" s="11" t="inlineStr">
@@ -1109,29 +1109,29 @@
       </c>
       <c r="C7" s="10" t="inlineStr">
         <is>
-          <t>DLV.R31KT6.WI.C.ZIP : last exported on 23.02.24
+          <t>DLV.R31KT6.WI.C.ZIP : last exported on 29.02.24
 DLV.KZ6KT6.WI.V.ZIP : last exported on 24.02.24
 DLV.RPKKT6.WI.S.ZIP : last exported on 26.02.24
-DLV.I5XKT6.WI.A.ZIP : last exported on 24.02.24
-DIT.E35KT6.WI.ZIP : last exported on 26.02.24
-DEL.K2PKT6.WI.ZIP : last exported on 26.02.24
-DEL.R7AKT6.WI.ZIP : last exported on 22.02.24
-DEL.N5FKT6.WI.ZIP : last exported on 23.02.24</t>
+DLV.I5XKT6.WI.A.ZIP : last exported on 29.02.24
+DIT.E35KT6.WI.ZIP : last exported on 29.02.24
+DEL.K2PKT6.WI.ZIP : last exported on 29.02.24
+DEL.R7AKT6.WI.ZIP : last exported on 01.03.24
+DEL.N5FKT6.WI.ZIP : last exported on 01.03.24</t>
         </is>
       </c>
       <c r="D7" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 27.02.24
-DEL.N1LN3L.WI.D.GPL.DMP : last exported on 27.02.24
-DEL.N1LN3L.WI.D.GTR.DMP : last exported on 27.02.24
-DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 27.02.24
-DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 27.02.24
-DEL.N1LN0R.WI.D.CPD.DMP : last exported on 27.02.24
-DEL.N1LN0R.WI.D.CPL.DMP : last exported on 27.02.24
-DEL.KT6E35.WI.GGO.ZIP : last exported on 27.02.24
-DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 27.02.24
-DEL.KT6N5M.WI.GGO.ZIP : last exported on 27.02.24
-DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 27.02.24</t>
+          <t>DEL.N1LN3L.WI.D.GPD.DMP : last exported on 01.03.24
+DEL.N1LN3L.WI.D.GPL.DMP : last exported on 01.03.24
+DEL.N1LN3L.WI.D.GTR.DMP : last exported on 01.03.24
+DEL.N1LN3L.WI.D.ASPD.DMP : last exported on 01.03.24
+DEL.N1LN3L.WI.D.ASPL.DMP : last exported on 01.03.24
+DEL.N1LN0R.WI.D.CPD.DMP : last exported on 01.03.24
+DEL.N1LN0R.WI.D.CPL.DMP : last exported on 01.03.24
+DEL.KT6E35.WI.GGO.ZIP : last exported on 01.03.24
+DEL.KT6E35.WI.IMG.GGO.ZIP : last exported on 01.03.24
+DEL.KT6N5M.WI.GGO.ZIP : last exported on 01.03.24
+DEL.KT6N5M.WI.IMG.GGO.ZIP : last exported on 01.03.24</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1232,30 +1232,30 @@
       </c>
       <c r="C10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 16.02.24
-DEL.N3LKT6.HST.??????.ZIP : last exported on 27.02.24
+          <t>DEL.N3LKT6.HST.MASTER.ZIP : last exported on 29.02.24
+DEL.N3LKT6.HST.??????.ZIP : last exported on 01.03.24
 DGV.N3LKT6.EPELS.??????.ZIP : last exported on 26.02.24</t>
         </is>
       </c>
       <c r="D10" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 26.02.24
-DEL.N1LN3L.TP.D.GPL.DMP : last exported on 26.02.24
-DEL.N1LN3L.TP.D.GTR.DMP : last exported on 26.02.24
-DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 26.02.24
-DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 26.02.24
-DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 26.02.24
-DEL.N1LN0R.TP.D.CPD.DMP : last exported on 26.02.24
-DEL.N1LN0R.TP.D.CPL.DMP : last exported on 26.02.24
-DEL.KT6E35.TP.D.GGO.ZIP : last exported on 26.02.24
-DEL.KT6E35.TP.D.UGO.ZIP : last exported on 26.02.24
-DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 26.02.24
-DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 26.02.24
-DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 26.02.24
-DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 26.02.24
-DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 26.02.24
-DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 26.02.24
-DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 26.02.24</t>
+          <t>DEL.N1LN3L.TP.D.GPD.DMP : last exported on 29.02.24
+DEL.N1LN3L.TP.D.GPL.DMP : last exported on 29.02.24
+DEL.N1LN3L.TP.D.GTR.DMP : last exported on 29.02.24
+DEL.N1LKQQ.TP.D.UPD.DMP : last exported on 29.02.24
+DEL.N1LN3L.TP.D.ASPD.DMP : last exported on 29.02.24
+DEL.N1LN3L.TP.D.ASPL.DMP : last exported on 29.02.24
+DEL.N1LN0R.TP.D.CPD.DMP : last exported on 29.02.24
+DEL.N1LN0R.TP.D.CPL.DMP : last exported on 29.02.24
+DEL.KT6E35.TP.D.GGO.ZIP : last exported on 29.02.24
+DEL.KT6E35.TP.D.UGO.ZIP : last exported on 29.02.24
+DEL.KT6N5M.TP.D.GGO.ZIP : last exported on 29.02.24
+DEL.KT6N5M.TP.D.UGO.ZIP : last exported on 29.02.24
+DEL.KT6N5M.TP.D.ASGO.ZIP : last exported on 29.02.24
+DEL.KT6N5M.TP.D.UOC.ZIP : last exported on 29.02.24
+DEL.KT6N5M.TP.D.ASOC.ZIP : last exported on 29.02.24
+DEL.KT6N5M.TP.D.GOC.ZIP : last exported on 29.02.24
+DED.KT6I1M.HST2.D.GGO.ZIP : last exported on 29.02.24</t>
         </is>
       </c>
       <c r="E10" s="11" t="inlineStr">
@@ -1290,7 +1290,7 @@
         <is>
           <t>DEL.N1LN3L.MC.F.GPD.DMP : last exported on 01.02.24
 DEL.N1LN3L.MC.F.GPL.DMP : last exported on 01.02.24
-DEL.N1LN3L.MC.F.GTR.DMP : last exported on 26.02.24
+DEL.N1LN3L.MC.F.GTR.DMP : last exported on 29.02.24
 DEL.N1LKQQ.MC.F.UPD.DMP : last exported on 01.02.24
 DEL.N1LN3L.MC.F.ASPD.DMP : last exported on 01.02.24
 DEL.N1LN3L.MC.F.ASPL.DMP : last exported on 01.02.24
@@ -1322,12 +1322,12 @@
       </c>
       <c r="C12" s="15" t="inlineStr">
         <is>
-          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 26.02.24</t>
+          <t>DDC.R11KT6.ELFI.TT.TXT : last exported on 29.02.24</t>
         </is>
       </c>
       <c r="D12" s="15" t="inlineStr">
         <is>
-          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 24.02.24</t>
+          <t>DKG.KT6R11.ELFI.TT.TXT : last exported on 29.02.24</t>
         </is>
       </c>
       <c r="E12" s="11" t="inlineStr">
@@ -1365,7 +1365,7 @@
         <is>
           <t>DEL.N1LN3L.AU.D.GPD.DMP : last exported on 24.02.24
 DEL.N1LN3L.AU.D.GPL.DMP : last exported on 24.02.24
-DEL.N1LN3L.AU.D.GTR.DMP : last exported on 26.02.24
+DEL.N1LN3L.AU.D.GTR.DMP : last exported on 29.02.24
 DEL.N1LN0R.AU.D.CPD.DMP : last exported on 24.02.24
 DEL.N1LN0R.AU.D.CPL.DMP : last exported on 24.02.24
 DEL.KT6E35.AU.GGO.ZIP : last exported on 24.02.24
@@ -1407,25 +1407,25 @@
 DGQ.R11KT6.BSITX.TXT : last exported on 28.02.24
 DGQ.R31KT6.BSIVMC.TXT : last exported on 06.02.24
 DGQ.R31KT6.PKATC.TXT : last exported on 06.02.24
-DEL.KMPKT6.APOS.DATA.ZIP : last exported on 21.02.24</t>
+DEL.KMPKT6.APOS.DATA.ZIP : last exported on 28.02.24</t>
         </is>
       </c>
       <c r="D14" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 21.02.24
-DEL.N1LN3L.AP.F.GPL.DMP : last exported on 21.02.24
-DEL.N1LN3L.AP.F.GTR.DMP : last exported on 21.02.24
-DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 21.02.24
-DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 21.02.24
-DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 21.02.24
-DEL.N1LN0R.AP.F.CPD.DMP : last exported on 21.02.24
-DEL.N1LN0R.AP.F.CPL.DMP : last exported on 21.02.24
-DEL.N1LR31.AP.F.PPS.DMP : last exported on 21.02.24
-DEL.KT6E35.AP.F.DB.ZIP : last exported on 21.02.24
-DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 21.02.24
-DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 21.02.24
-DVL.KT6N5X.VLM.AP.ZIP : last exported on 21.02.24
-DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 21.02.24</t>
+          <t>DEL.N1LN3L.AP.F.GPD.DMP : last exported on 28.02.24
+DEL.N1LN3L.AP.F.GPL.DMP : last exported on 28.02.24
+DEL.N1LN3L.AP.F.GTR.DMP : last exported on 28.02.24
+DEL.N1LKQQ.AP.F.UPD.DMP : last exported on 28.02.24
+DEL.N1LN3L.AP.F.ASPD.DMP : last exported on 28.02.24
+DEL.N1LN3L.AP.F.ASPL.DMP : last exported on 28.02.24
+DEL.N1LN0R.AP.F.CPD.DMP : last exported on 28.02.24
+DEL.N1LN0R.AP.F.CPL.DMP : last exported on 28.02.24
+DEL.N1LR31.AP.F.PPS.DMP : last exported on 28.02.24
+DEL.KT6E35.AP.F.DB.ZIP : last exported on 28.02.24
+DEL.KT6KGZ.AP.F.DWH.ZIP : last exported on 28.02.24
+DEL.KT6UGV.AP.F.CEB.ZIP : last exported on 28.02.24
+DVL.KT6N5X.VLM.AP.ZIP : last exported on 28.02.24
+DEL.KT6N5M.AP.F.GGO.ZIP : last exported on 28.02.24</t>
         </is>
       </c>
       <c r="E14" s="11" t="inlineStr">
@@ -1458,8 +1458,8 @@
       </c>
       <c r="D15" s="16" t="inlineStr">
         <is>
-          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 26.02.24
-DGI.N1LR11.FB.IMPTR.CSV : last exported on 26.02.24</t>
+          <t>DGI.N1LR11.FB.ORGUNIT.CSV : last exported on 29.02.24
+DGI.N1LR11.FB.IMPTR.CSV : last exported on 29.02.24</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -1487,23 +1487,23 @@
       </c>
       <c r="C16" s="10" t="inlineStr">
         <is>
-          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 26.02.24
-DHP.KUDKT6.ORGUNITS : last exported on 27.02.24
-DHS.R11KT6.HSB02ALL : last exported on 26.02.24</t>
+          <t>DHP.KUDKT6.KVPSIMPORT : last exported on 29.02.24
+DHP.KUDKT6.ORGUNITS : last exported on 01.03.24
+DHS.R11KT6.HSB02ALL : last exported on 29.02.24</t>
         </is>
       </c>
       <c r="D16" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 26.02.24
-DEL.N1LN3L.DP.F.GPL.DMP : last exported on 26.02.24
-DEL.N1LN3L.DP.F.GTR.DMP : last exported on 26.02.24
-DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 26.02.24
-DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 26.02.24
-DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 26.02.24
-DEL.N1LN0R.DP.F.CPD.DMP : last exported on 26.02.24
-DEL.N1LN0R.DP.F.CPL.DMP : last exported on 26.02.24
-DEL.N1LN3L.DISSORG.ZIP : last exported on 26.02.24
-DEL.N1LN3L.DISSAORG.ZIP : last exported on 26.02.24</t>
+          <t>DEL.N1LN3L.DP.F.GPD.DMP : last exported on 29.02.24
+DEL.N1LN3L.DP.F.GPL.DMP : last exported on 29.02.24
+DEL.N1LN3L.DP.F.GTR.DMP : last exported on 29.02.24
+DEL.N1LKQQ.DP.F.UPD.DMP : last exported on 29.02.24
+DEL.N1LN3L.DP.F.ASPD.DMP : last exported on 29.02.24
+DEL.N1LN3L.DP.F.ASPL.DMP : last exported on 29.02.24
+DEL.N1LN0R.DP.F.CPD.DMP : last exported on 29.02.24
+DEL.N1LN0R.DP.F.CPL.DMP : last exported on 29.02.24
+DEL.N1LN3L.DISSORG.ZIP : last exported on 29.02.24
+DEL.N1LN3L.DISSAORG.ZIP : last exported on 29.02.24</t>
         </is>
       </c>
       <c r="E16" s="11" t="inlineStr">
@@ -1601,38 +1601,38 @@
       </c>
       <c r="C19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 26.02.24</t>
+          <t>DEL.N3LKT6.WT.??????.ZIP : last exported on 29.02.24</t>
         </is>
       </c>
       <c r="D19" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 26.02.24
-DEL.N1LN3L.MT.F.GPL.DMP : last exported on 26.02.24
-DEL.N1LN3L.MT.F.GTR.DMP : last exported on 26.02.24
-DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 26.02.24
-DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 26.02.24
-DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 26.02.24
-DEL.N1LN0R.MT.F.CPD.DMP : last exported on 26.02.24
-DEL.N1LN0R.MT.F.CPL.DMP : last exported on 26.02.24
-DEL.N1LR31.MT.F.GPD.DMP : last exported on 26.02.24
-DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 26.02.24
-DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 26.02.24
-DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 26.02.24
-DEL.N1LKT6.MT.??????.G : last exported on 26.02.24
-DEL.N1LKT6.MT.??????.U : last exported on 26.02.24
-DEL.N1LKT6.MT.??????.AS : last exported on 26.02.24
-DVL.N1LN5X.VLM.DSP : last exported on 26.02.24
-DVL.N1LN5X.VLM.WT : last exported on 26.02.24
-DDS.N1LR11.DSP : last exported on 26.02.24
-DDS.N1LR11.WT : last exported on 26.02.24
-DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 26.02.24
-DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 26.02.24
-DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 26.02.24
-DEL.KT6E35.MT.F.GGO.ZIP : last exported on 26.02.24
-DEL.KT6E35.MT.F.UGO.ZIP : last exported on 26.02.24
-DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 26.02.24
-DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 26.02.24
-DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 26.02.24</t>
+          <t>DEL.N1LN3L.MT.F.GPD.DMP : last exported on 29.02.24
+DEL.N1LN3L.MT.F.GPL.DMP : last exported on 29.02.24
+DEL.N1LN3L.MT.F.GTR.DMP : last exported on 29.02.24
+DEL.N1LKQQ.MT.F.UPD.DMP : last exported on 29.02.24
+DEL.N1LN3L.MT.F.ASPD.DMP : last exported on 29.02.24
+DEL.N1LN3L.MT.F.ASPL.DMP : last exported on 29.02.24
+DEL.N1LN0R.MT.F.CPD.DMP : last exported on 29.02.24
+DEL.N1LN0R.MT.F.CPL.DMP : last exported on 29.02.24
+DEL.N1LR31.MT.F.GPD.DMP : last exported on 29.02.24
+DEL.N1LI4X.MT.F.GPD.ZIP : last exported on 29.02.24
+DEL.N1LI4Y.MT.F.GPL.ZIP : last exported on 29.02.24
+DEL.N1LGN1.NL.F.GPD.ZIP : last exported on 29.02.24
+DEL.N1LKT6.MT.??????.G : last exported on 29.02.24
+DEL.N1LKT6.MT.??????.U : last exported on 29.02.24
+DEL.N1LKT6.MT.??????.AS : last exported on 29.02.24
+DVL.N1LN5X.VLM.DSP : last exported on 29.02.24
+DVL.N1LN5X.VLM.WT : last exported on 29.02.24
+DDS.N1LR11.DSP : last exported on 29.02.24
+DDS.N1LR11.WT : last exported on 29.02.24
+DEL.KT6N5M.MT.F.GGO.ZIP : last exported on 29.02.24
+DEL.KT6N5M.MT.F.UGO.ZIP : last exported on 29.02.24
+DEL.KT6N5M.MT.F.ASGO.ZIP : last exported on 29.02.24
+DEL.KT6E35.MT.F.GGO.ZIP : last exported on 29.02.24
+DEL.KT6E35.MT.F.UGO.ZIP : last exported on 29.02.24
+DEL.KT6N5X.MT.F.GGO.ZIP : last exported on 29.02.24
+DEL.KT6N5X.MT.F.UGO.ZIP : last exported on 29.02.24
+DEL.KT6N5X.MT.F.ASGO.ZIP : last exported on 29.02.24</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -1660,52 +1660,52 @@
       </c>
       <c r="C20" s="10" t="inlineStr">
         <is>
-          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 27.02.24
-DKG.R11KT6.L520.P.EDCP.LEI : last exported on 27.02.24
-DKG.R11KT6.L520.P.EDCP.SGE : last exported on 27.02.24
-DKG.R11KT6.L520.P.EDCP.SMO : last exported on 27.02.24
-DKG.R11KT6.L520.P.EDCP.STR : last exported on 27.02.24
-DKG.R11KT6.L520.P.EDCP.TEC : last exported on 27.02.24
-DKG.R11KT6.L520.P.EDCP.TGE : last exported on 27.02.24
-DKG.R11KT6.L520.P.EDCP.TMO : last exported on 27.02.24
+          <t>DKG.R11KT6.L520.P.EDCP.HVB : last exported on 01.03.24
+DKG.R11KT6.L520.P.EDCP.LEI : last exported on 01.03.24
+DKG.R11KT6.L520.P.EDCP.SGE : last exported on 01.03.24
+DKG.R11KT6.L520.P.EDCP.SMO : last exported on 01.03.24
+DKG.R11KT6.L520.P.EDCP.STR : last exported on 01.03.24
+DKG.R11KT6.L520.P.EDCP.TEC : last exported on 01.03.24
+DKG.R11KT6.L520.P.EDCP.TGE : last exported on 01.03.24
+DKG.R11KT6.L520.P.EDCP.TMO : last exported on 01.03.24
 DDC.R11KT6.ELFI.MD.TXT : last exported on 25.02.24
-DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 26.02.24
+DDC.R11KT6.ELFI.TT.EXT.TXT : last exported on 29.02.24
 DDC.R11KT6.ELFI.PK.TXT : last exported on 25.02.24
 DDC.R11KT6.ELFI.PR.TXT : last exported on 25.02.24</t>
         </is>
       </c>
       <c r="D20" s="10" t="inlineStr">
         <is>
-          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 26.02.24
-DEL.N1LN3L.EL.F.GPL.DMP : last exported on 26.02.24
-DEL.N1LE35.ELFI.G.DATA : last exported on 26.02.24
-DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 26.02.24
-DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 26.02.24
-DEL.N1LE35.EL.F.GGO.ZIP : last exported on 26.02.24
-DEL.N1LKT6.EC.??????.G : last exported on 26.02.24
-DWT.N1LN3L.WT.??????.ZIP : last exported on 26.02.24
-DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 26.02.24
-DEL.N1LE35.ELFI.U.DATA : last exported on 26.02.24
-DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 26.02.24
-DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 26.02.24
-DEL.N1LE35.EL.F.UGO.ZIP : last exported on 26.02.24
-DEL.N1LKT6.EC.??????.U : last exported on 26.02.24
-DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 26.02.24
-DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 26.02.24
-DEL.N1LN0R.EL.F.CPD.DMP : last exported on 26.02.24
-DEL.N1LN0R.EL.F.CPL.DMP : last exported on 26.02.24
-DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 26.02.24
-DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 26.02.24
-DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 26.02.24
-DEL.N1LKT6.EC.??????.AS : last exported on 26.02.24
-DEL.N1LN3L.EL.F.GTR.DMP : last exported on 26.02.24
-DGV.N1LR31.EL.F.HST.ZIP : last exported on 26.02.24
-DGV.N1LN3L.EL.F.HST.ZIP : last exported on 26.02.24
-DGV.N1LCEN.EL.F.ZIP : last exported on 26.02.24
-DGV.N1LN7K.EL.F.ZIP : last exported on 26.02.24
-DGV.N1LN5X.EL.F.ZIP : last exported on 26.02.24
-DEL.KT6KT6.EL.F.DRE.CSV : last exported on 26.02.24
-DEL.KT6N5X.EL.F.AU.ZIP : last exported on 26.02.24</t>
+          <t>DEL.N1LN3L.EL.F.GPD.DMP : last exported on 29.02.24
+DEL.N1LN3L.EL.F.GPL.DMP : last exported on 29.02.24
+DEL.N1LE35.ELFI.G.DATA : last exported on 29.02.24
+DEL.N1LN5M.EL.F.GGO.ZIP : last exported on 29.02.24
+DEL.N1LN5X.EL.F.GGO.ZIP : last exported on 29.02.24
+DEL.N1LE35.EL.F.GGO.ZIP : last exported on 29.02.24
+DEL.N1LKT6.EC.??????.G : last exported on 29.02.24
+DWT.N1LN3L.WT.??????.ZIP : last exported on 29.02.24
+DEL.N1LKQQ.EL.F.UPD.DMP : last exported on 29.02.24
+DEL.N1LE35.ELFI.U.DATA : last exported on 29.02.24
+DEL.N1LN5M.EL.F.UGO.ZIP : last exported on 29.02.24
+DEL.N1LN5X.EL.F.UGO.ZIP : last exported on 29.02.24
+DEL.N1LE35.EL.F.UGO.ZIP : last exported on 29.02.24
+DEL.N1LKT6.EC.??????.U : last exported on 29.02.24
+DEL.N1LN3L.EL.F.ASPD.DMP : last exported on 29.02.24
+DEL.N1LN3L.EL.F.ASPL.DMP : last exported on 29.02.24
+DEL.N1LN0R.EL.F.CPD.DMP : last exported on 29.02.24
+DEL.N1LN0R.EL.F.CPL.DMP : last exported on 29.02.24
+DEL.N1LN5M.EL.F.ASGO.ZIP : last exported on 29.02.24
+DEL.N1LN5X.EL.F.ASGO.ZIP : last exported on 29.02.24
+DEL.N1LE35.EL.F.ASGO.ZIP : last exported on 29.02.24
+DEL.N1LKT6.EC.??????.AS : last exported on 29.02.24
+DEL.N1LN3L.EL.F.GTR.DMP : last exported on 29.02.24
+DGV.N1LR31.EL.F.HST.ZIP : last exported on 29.02.24
+DGV.N1LN3L.EL.F.HST.ZIP : last exported on 29.02.24
+DGV.N1LCEN.EL.F.ZIP : last exported on 29.02.24
+DGV.N1LN7K.EL.F.ZIP : last exported on 29.02.24
+DGV.N1LN5X.EL.F.ZIP : last exported on 29.02.24
+DEL.KT6KT6.EL.F.DRE.CSV : last exported on 29.02.24
+DEL.KT6N5X.EL.F.AU.ZIP : last exported on 29.02.24</t>
         </is>
       </c>
       <c r="E20" s="11" t="inlineStr">

</xml_diff>